<commit_message>
selenium sheet changed runner
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="105">
   <si>
     <t>Places</t>
   </si>
@@ -216,49 +216,128 @@
     <t>50.8030° N, 6.4811° E</t>
   </si>
   <si>
-    <t>dusseldorf</t>
-  </si>
-  <si>
-    <t>14.98.</t>
-  </si>
-  <si>
-    <t>15.12.</t>
-  </si>
-  <si>
-    <t>16.02.</t>
-  </si>
-  <si>
-    <t>15.7.</t>
-  </si>
-  <si>
-    <t>14.92.</t>
-  </si>
-  <si>
-    <t>15.42.</t>
-  </si>
-  <si>
-    <t>Hamm,DE</t>
-  </si>
-  <si>
-    <t>barrow,US</t>
-  </si>
-  <si>
-    <t>London,GB</t>
-  </si>
-  <si>
-    <t>London,US</t>
-  </si>
-  <si>
-    <t>London,AU</t>
-  </si>
-  <si>
-    <t>durban</t>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>jammu</t>
+  </si>
+  <si>
+    <t>moga</t>
+  </si>
+  <si>
+    <t>hisar</t>
+  </si>
+  <si>
+    <t>palwal</t>
+  </si>
+  <si>
+    <t>agra</t>
+  </si>
+  <si>
+    <t>udaipur</t>
+  </si>
+  <si>
+    <t>ajmer</t>
+  </si>
+  <si>
+    <t>surat</t>
+  </si>
+  <si>
+    <t>chiplun</t>
+  </si>
+  <si>
+    <t>karwar</t>
+  </si>
+  <si>
+    <t>kannur</t>
+  </si>
+  <si>
+    <t>kozhikode</t>
+  </si>
+  <si>
+    <t>33.9.</t>
+  </si>
+  <si>
+    <t>33.02.</t>
+  </si>
+  <si>
+    <t>35.99.</t>
+  </si>
+  <si>
+    <t>31.2.</t>
+  </si>
+  <si>
+    <t>34.15.</t>
+  </si>
+  <si>
+    <t>25.5.</t>
+  </si>
+  <si>
+    <t>23.42.</t>
+  </si>
+  <si>
+    <t>29.99.</t>
+  </si>
+  <si>
+    <t>28.22.</t>
+  </si>
+  <si>
+    <t>27.11.</t>
+  </si>
+  <si>
+    <t>Temperature1</t>
+  </si>
+  <si>
+    <t>Temperature2</t>
+  </si>
+  <si>
+    <t>kasaragod</t>
+  </si>
+  <si>
+    <t>28.17.</t>
+  </si>
+  <si>
+    <t>29.84.</t>
+  </si>
+  <si>
+    <t>29.88.</t>
+  </si>
+  <si>
+    <t>30.32.</t>
+  </si>
+  <si>
+    <t>28.89.</t>
+  </si>
+  <si>
+    <t>22.56.</t>
+  </si>
+  <si>
+    <t>23.9.</t>
+  </si>
+  <si>
+    <t>27.02.</t>
+  </si>
+  <si>
+    <t>24.99.</t>
+  </si>
+  <si>
+    <t>25.75.</t>
+  </si>
+  <si>
+    <t>26.59.</t>
+  </si>
+  <si>
+    <t>25.37.</t>
+  </si>
+  <si>
+    <t>24.65.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,81 +677,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
+      <c r="C14" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -690,9 +854,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Multiple runner with delay
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Places</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>21.54.</t>
+  </si>
+  <si>
+    <t>25.48.</t>
+  </si>
+  <si>
+    <t>21.09.</t>
+  </si>
+  <si>
+    <t>17.52.</t>
   </si>
 </sst>
 </file>
@@ -689,10 +698,10 @@
         <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -715,7 +724,7 @@
         <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -738,7 +747,7 @@
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
little adventure improvemnte went wrong
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>Places</t>
   </si>
@@ -216,9 +216,6 @@
     <t>50.8030° N, 6.4811° E</t>
   </si>
   <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>35.99.</t>
   </si>
   <si>
@@ -231,24 +228,9 @@
     <t>28.17.</t>
   </si>
   <si>
-    <t>29.84.</t>
-  </si>
-  <si>
-    <t>29.88.</t>
-  </si>
-  <si>
     <t>29.44.</t>
   </si>
   <si>
-    <t>srinagar</t>
-  </si>
-  <si>
-    <t>17.71.</t>
-  </si>
-  <si>
-    <t>skardu</t>
-  </si>
-  <si>
     <t>Temperature3</t>
   </si>
   <si>
@@ -267,22 +249,85 @@
     <t>Temperature8</t>
   </si>
   <si>
-    <t>gilgit</t>
-  </si>
-  <si>
-    <t>25.55.</t>
-  </si>
-  <si>
-    <t>21.54.</t>
-  </si>
-  <si>
-    <t>25.48.</t>
-  </si>
-  <si>
-    <t>21.09.</t>
-  </si>
-  <si>
-    <t>17.52.</t>
+    <t>dusseldorf</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>Monte Carlo</t>
+  </si>
+  <si>
+    <t>Temperature9</t>
+  </si>
+  <si>
+    <t>Temperature10</t>
+  </si>
+  <si>
+    <t>Temperature11</t>
+  </si>
+  <si>
+    <t>Temperature12</t>
+  </si>
+  <si>
+    <t>Temperature13</t>
+  </si>
+  <si>
+    <t>Temperature14</t>
+  </si>
+  <si>
+    <t>Temperature15</t>
+  </si>
+  <si>
+    <t>Temperature16</t>
+  </si>
+  <si>
+    <t>Temperature17</t>
+  </si>
+  <si>
+    <t>Temperature18</t>
+  </si>
+  <si>
+    <t>13.37.</t>
+  </si>
+  <si>
+    <t>13.42.</t>
+  </si>
+  <si>
+    <t>19.35.</t>
+  </si>
+  <si>
+    <t>21.89.</t>
+  </si>
+  <si>
+    <t>13.28.</t>
+  </si>
+  <si>
+    <t>21.81.</t>
+  </si>
+  <si>
+    <t>13.3.</t>
+  </si>
+  <si>
+    <t>19.12.</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>16.04.$[[ChromeDriver: chrome on XP (70d13a5d04fcbe4353588bb598b793d3)] -&gt; id: xPat]</t>
+  </si>
+  <si>
+    <t>13.58.$[[ChromeDriver: chrome on XP (6467ec0d74fea02c0a3ac09ad57bcefb)] -&gt; id: xPat]</t>
+  </si>
+  <si>
+    <t>20.36.$[[ChromeDriver: chrome on XP (d2699a01bbe2d02d9fdb2c4a0859a00f)] -&gt; id: xPat]</t>
+  </si>
+  <si>
+    <t>21.96.$[[ChromeDriver: chrome on XP (52ab270f72e9e43db6022c5f290b4b9d)] -&gt; id: xPat]</t>
   </si>
 </sst>
 </file>
@@ -629,125 +674,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="83.03125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="83.03125" collapsed="true"/>
+    <col min="4" max="11" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="12" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" t="s">
+        <v>98</v>
+      </c>
+      <c r="S4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>88</v>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5" t="s">
+        <v>96</v>
+      </c>
+      <c r="S5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
little adventure improvemnt corrected
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>Places</t>
   </si>
@@ -328,6 +328,30 @@
   </si>
   <si>
     <t>21.96.$[[ChromeDriver: chrome on XP (52ab270f72e9e43db6022c5f290b4b9d)] -&gt; id: xPat]</t>
+  </si>
+  <si>
+    <t>51.2217,6.7762</t>
+  </si>
+  <si>
+    <t>15.82.</t>
+  </si>
+  <si>
+    <t>44,7.25</t>
+  </si>
+  <si>
+    <t>13.34.</t>
+  </si>
+  <si>
+    <t>43.3333,5.5</t>
+  </si>
+  <si>
+    <t>20.24.</t>
+  </si>
+  <si>
+    <t>43.7496,7.437</t>
+  </si>
+  <si>
+    <t>21.83.</t>
   </si>
 </sst>
 </file>
@@ -683,8 +707,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="83.03125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="83.03125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="82.52734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="82.52734375" collapsed="true"/>
     <col min="4" max="11" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="12" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
@@ -756,10 +780,10 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R2" t="s">
         <v>97</v>
@@ -773,10 +797,10 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="R3" t="s">
         <v>95</v>
@@ -790,10 +814,10 @@
         <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="R4" t="s">
         <v>98</v>
@@ -807,10 +831,10 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="R5" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
ten places from europa conference league
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="126">
   <si>
     <t>Places</t>
   </si>
@@ -216,21 +216,12 @@
     <t>50.8030° N, 6.4811° E</t>
   </si>
   <si>
-    <t>35.99.</t>
-  </si>
-  <si>
     <t>Temperature1</t>
   </si>
   <si>
     <t>Temperature2</t>
   </si>
   <si>
-    <t>28.17.</t>
-  </si>
-  <si>
-    <t>29.44.</t>
-  </si>
-  <si>
     <t>Temperature3</t>
   </si>
   <si>
@@ -252,15 +243,6 @@
     <t>dusseldorf</t>
   </si>
   <si>
-    <t>Nice</t>
-  </si>
-  <si>
-    <t>Marseille</t>
-  </si>
-  <si>
-    <t>Monte Carlo</t>
-  </si>
-  <si>
     <t>Temperature9</t>
   </si>
   <si>
@@ -291,18 +273,6 @@
     <t>Temperature18</t>
   </si>
   <si>
-    <t>13.37.</t>
-  </si>
-  <si>
-    <t>13.42.</t>
-  </si>
-  <si>
-    <t>19.35.</t>
-  </si>
-  <si>
-    <t>21.89.</t>
-  </si>
-  <si>
     <t>13.28.</t>
   </si>
   <si>
@@ -318,18 +288,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>16.04.$[[ChromeDriver: chrome on XP (70d13a5d04fcbe4353588bb598b793d3)] -&gt; id: xPat]</t>
-  </si>
-  <si>
-    <t>13.58.$[[ChromeDriver: chrome on XP (6467ec0d74fea02c0a3ac09ad57bcefb)] -&gt; id: xPat]</t>
-  </si>
-  <si>
-    <t>20.36.$[[ChromeDriver: chrome on XP (d2699a01bbe2d02d9fdb2c4a0859a00f)] -&gt; id: xPat]</t>
-  </si>
-  <si>
-    <t>21.96.$[[ChromeDriver: chrome on XP (52ab270f72e9e43db6022c5f290b4b9d)] -&gt; id: xPat]</t>
-  </si>
-  <si>
     <t>51.2217,6.7762</t>
   </si>
   <si>
@@ -352,6 +310,90 @@
   </si>
   <si>
     <t>21.83.</t>
+  </si>
+  <si>
+    <t>Yerevan</t>
+  </si>
+  <si>
+    <t>oral</t>
+  </si>
+  <si>
+    <t>windhoek</t>
+  </si>
+  <si>
+    <t>Aire-sur-l'Adour</t>
+  </si>
+  <si>
+    <t>Foz do Iguaçu</t>
+  </si>
+  <si>
+    <t>São João de Ver</t>
+  </si>
+  <si>
+    <t>Łódź</t>
+  </si>
+  <si>
+    <t>Tournai</t>
+  </si>
+  <si>
+    <t>Bratislava</t>
+  </si>
+  <si>
+    <t>17.77.</t>
+  </si>
+  <si>
+    <t>40.1811,44.5136</t>
+  </si>
+  <si>
+    <t>26.09.</t>
+  </si>
+  <si>
+    <t>51.2333,51.3667</t>
+  </si>
+  <si>
+    <t>21.99.</t>
+  </si>
+  <si>
+    <t>-22.5594,17.0832</t>
+  </si>
+  <si>
+    <t>10.06.</t>
+  </si>
+  <si>
+    <t>48.1482,17.1067</t>
+  </si>
+  <si>
+    <t>15.75.</t>
+  </si>
+  <si>
+    <t>50.6072,3.3893</t>
+  </si>
+  <si>
+    <t>18.14.</t>
+  </si>
+  <si>
+    <t>51.5,19.5</t>
+  </si>
+  <si>
+    <t>14.73.</t>
+  </si>
+  <si>
+    <t>40.9553,-8.5512</t>
+  </si>
+  <si>
+    <t>18.36.</t>
+  </si>
+  <si>
+    <t>-25.5478,-54.5881</t>
+  </si>
+  <si>
+    <t>21.49.</t>
+  </si>
+  <si>
+    <t>43.7018,-0.2645</t>
+  </si>
+  <si>
+    <t>19.48.</t>
   </si>
 </sst>
 </file>
@@ -359,13 +401,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -394,9 +442,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,17 +747,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="82.52734375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="82.52734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.90234375" collapsed="true"/>
     <col min="4" max="11" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="12" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
@@ -718,133 +767,200 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="R2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="S2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
+      <c r="A3" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="S3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="S4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="S5" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
FPL with Se real committ
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="122">
   <si>
     <t>Places</t>
   </si>
@@ -368,6 +368,21 @@
   </si>
   <si>
     <t>23.92.</t>
+  </si>
+  <si>
+    <t>Zibin</t>
+  </si>
+  <si>
+    <t>440807</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>420</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1329,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,24 +1353,32 @@
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="6">
-        <v>1288683</v>
+      <c r="B2" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="6">
-        <v>143864</v>
+      <c r="B3" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="6">
-        <v>25825</v>
+      <c r="B4" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the \n issue
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="286">
   <si>
     <t>Places</t>
   </si>
@@ -330,12 +330,6 @@
     <t>AF</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
     <t>wellington,AU</t>
   </si>
   <si>
@@ -675,45 +669,6 @@
     <t>Manager_iD</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>Hogwarts</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>Tekirdag</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>rwterte</t>
-  </si>
-  <si>
     <t>24.81.</t>
   </si>
   <si>
@@ -855,9 +810,6 @@
     <t>27.99.</t>
   </si>
   <si>
-    <t>26.01.</t>
-  </si>
-  <si>
     <t>13.0878,80.2785</t>
   </si>
   <si>
@@ -873,21 +825,9 @@
     <t>DE</t>
   </si>
   <si>
-    <t>16.22.</t>
-  </si>
-  <si>
     <t>51.5085,-0.1257</t>
   </si>
   <si>
-    <t>16.59.</t>
-  </si>
-  <si>
-    <t>16.88.</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>28.69.</t>
   </si>
   <si>
@@ -901,6 +841,46 @@
   </si>
   <si>
     <t>16.65.</t>
+  </si>
+  <si>
+    <t>38
+Reload</t>
+  </si>
+  <si>
+    <t>Points
+Reload</t>
+  </si>
+  <si>
+    <t>50
+Reload</t>
+  </si>
+  <si>
+    <t>18
+Reload</t>
+  </si>
+  <si>
+    <t>5123456</t>
+  </si>
+  <si>
+    <t>4408073</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Mogrem97</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>PINE</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>jones</t>
   </si>
 </sst>
 </file>
@@ -908,7 +888,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -928,6 +908,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1A1AA6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -956,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -965,6 +951,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,81 +1370,81 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" t="s">
         <v>210</v>
       </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E2" t="s">
-        <v>212</v>
-      </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="O2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="S2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="U2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1848,10 +1836,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1862,87 +1850,65 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>103</v>
+        <v>281</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>104</v>
+        <v>283</v>
+      </c>
+      <c r="B3" s="9">
+        <v>158870</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>226</v>
+      <c r="A4" t="s">
+        <v>285</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>222</v>
+        <v>278</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" t="s">
-        <v>229</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2068,13 +2034,13 @@
         <v>100</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -2111,13 +2077,13 @@
         <v>102</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2154,13 +2120,13 @@
         <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2188,22 +2154,22 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2231,22 +2197,22 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2274,22 +2240,22 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2317,22 +2283,22 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2360,22 +2326,22 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2403,22 +2369,22 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2446,22 +2412,22 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2492,19 +2458,19 @@
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2535,19 +2501,19 @@
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2575,22 +2541,22 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2618,22 +2584,22 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2661,22 +2627,22 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2704,22 +2670,22 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2747,22 +2713,22 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2790,22 +2756,22 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2833,22 +2799,22 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2879,19 +2845,19 @@
         <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2919,22 +2885,22 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2965,19 +2931,19 @@
         <v>29</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -3008,19 +2974,19 @@
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3048,22 +3014,22 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3091,22 +3057,22 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -3134,22 +3100,22 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -3177,22 +3143,22 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -3220,22 +3186,22 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3263,22 +3229,22 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -3313,18 +3279,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.078125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.609375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.609375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.609375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3352,203 +3316,203 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="E3" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E4" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F4" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="E5" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="F5" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E6" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F6" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="E7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="F7" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E8" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F8" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="E9" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="F9" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="C10" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="E10" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="F10" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="E11" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="F11" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3556,19 +3520,19 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kuch kaam ka ni hai isme
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="667">
   <si>
     <t>Places</t>
   </si>
@@ -1947,37 +1947,82 @@
     <t>madrid</t>
   </si>
   <si>
-    <t>22.22.</t>
-  </si>
-  <si>
     <t>40.4165,-3.7026</t>
   </si>
   <si>
     <t>ES</t>
   </si>
   <si>
-    <t>20.16.</t>
-  </si>
-  <si>
-    <t>13.84.</t>
-  </si>
-  <si>
-    <t>22.39.</t>
-  </si>
-  <si>
     <t>barcelona</t>
   </si>
   <si>
-    <t>12.86.</t>
-  </si>
-  <si>
-    <t>22.2.</t>
-  </si>
-  <si>
     <t>41.3888,2.159</t>
   </si>
   <si>
-    <t>24.64.</t>
+    <t>vitoria</t>
+  </si>
+  <si>
+    <t>vigo</t>
+  </si>
+  <si>
+    <t>san sebastian</t>
+  </si>
+  <si>
+    <t>21.75.</t>
+  </si>
+  <si>
+    <t>21.42.</t>
+  </si>
+  <si>
+    <t>19.86.</t>
+  </si>
+  <si>
+    <t>22.48.</t>
+  </si>
+  <si>
+    <t>-20.3194,-40.3378</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>25.75.</t>
+  </si>
+  <si>
+    <t>42.2328,-8.7226</t>
+  </si>
+  <si>
+    <t>18.72.</t>
+  </si>
+  <si>
+    <t>43.3128,-1.975</t>
+  </si>
+  <si>
+    <t>19.05.</t>
+  </si>
+  <si>
+    <t>43.2627,-2.9253</t>
+  </si>
+  <si>
+    <t>20.39.</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>319</t>
+  </si>
+  <si>
+    <t>361</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>336</t>
   </si>
 </sst>
 </file>
@@ -2450,21 +2495,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="16.078125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="6.609375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="6.609375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="6.609375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="6.609375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
     <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
     <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
     <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
@@ -2576,16 +2618,16 @@
         <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>210</v>
@@ -2641,16 +2683,16 @@
         <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="G3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -2658,33 +2700,33 @@
         <v>640</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>643</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E4" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F4" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="G4" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B5" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="C5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D5" t="s">
         <v>651</v>
@@ -2697,6 +2739,98 @@
       </c>
       <c r="G5" t="s">
         <v>651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C6" t="s">
+        <v>653</v>
+      </c>
+      <c r="D6" t="s">
+        <v>654</v>
+      </c>
+      <c r="E6" t="s">
+        <v>654</v>
+      </c>
+      <c r="F6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G6" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="B7" t="s">
+        <v>655</v>
+      </c>
+      <c r="C7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D7" t="s">
+        <v>656</v>
+      </c>
+      <c r="E7" t="s">
+        <v>656</v>
+      </c>
+      <c r="F7" t="s">
+        <v>656</v>
+      </c>
+      <c r="G7" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B8" t="s">
+        <v>657</v>
+      </c>
+      <c r="C8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D8" t="s">
+        <v>658</v>
+      </c>
+      <c r="E8" t="s">
+        <v>658</v>
+      </c>
+      <c r="F8" t="s">
+        <v>658</v>
+      </c>
+      <c r="G8" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>659</v>
+      </c>
+      <c r="C9" t="s">
+        <v>642</v>
+      </c>
+      <c r="D9" t="s">
+        <v>660</v>
+      </c>
+      <c r="E9" t="s">
+        <v>660</v>
+      </c>
+      <c r="F9" t="s">
+        <v>660</v>
+      </c>
+      <c r="G9" t="s">
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -3105,7 +3239,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="A2" sqref="A2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5123,7 +5257,7 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7901,19 +8035,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7944,10 +8078,10 @@
         <v>318</v>
       </c>
       <c r="D2" t="s">
-        <v>606</v>
+        <v>662</v>
       </c>
       <c r="E2" t="s">
-        <v>606</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7961,10 +8095,10 @@
         <v>270</v>
       </c>
       <c r="D3" t="s">
-        <v>607</v>
+        <v>663</v>
       </c>
       <c r="E3" t="s">
-        <v>607</v>
+        <v>663</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7978,10 +8112,10 @@
         <v>608</v>
       </c>
       <c r="D4" t="s">
-        <v>609</v>
+        <v>664</v>
       </c>
       <c r="E4" t="s">
-        <v>609</v>
+        <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -7995,10 +8129,27 @@
         <v>276</v>
       </c>
       <c r="D5" t="s">
-        <v>610</v>
+        <v>665</v>
       </c>
       <c r="E5" t="s">
-        <v>610</v>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="B6">
+        <v>269580</v>
+      </c>
+      <c r="C6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" t="s">
+        <v>666</v>
+      </c>
+      <c r="E6" t="s">
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
findelements by classname for spieler Name
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="730">
   <si>
     <t>Places</t>
   </si>
@@ -1923,12 +1923,6 @@
     <t>17.35.</t>
   </si>
   <si>
-    <t>madrid</t>
-  </si>
-  <si>
-    <t>40.4165,-3.7026</t>
-  </si>
-  <si>
     <t>ES</t>
   </si>
   <si>
@@ -1965,156 +1959,30 @@
     <t>19.05.</t>
   </si>
   <si>
-    <t>43.2627,-2.9253</t>
-  </si>
-  <si>
     <t>20.39.</t>
   </si>
   <si>
     <t>venlo</t>
   </si>
   <si>
-    <t>venlo,us</t>
-  </si>
-  <si>
-    <t>girona</t>
-  </si>
-  <si>
     <t>castille</t>
   </si>
   <si>
     <t>51.3667,6.1667</t>
   </si>
   <si>
-    <t>17.29.</t>
-  </si>
-  <si>
-    <t>41.9831,2.8249</t>
-  </si>
-  <si>
-    <t>20.99.</t>
-  </si>
-  <si>
-    <t>19.39.</t>
-  </si>
-  <si>
-    <t>22.82.</t>
-  </si>
-  <si>
-    <t>46.4864,-97.4462</t>
-  </si>
-  <si>
-    <t>23.12.</t>
-  </si>
-  <si>
     <t>44.0401,0.209</t>
   </si>
   <si>
     <t>FR</t>
   </si>
   <si>
-    <t>19.38.</t>
-  </si>
-  <si>
-    <t>26.78.</t>
-  </si>
-  <si>
-    <t>26.34.</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>341</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>474</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>438</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>380</t>
-  </si>
-  <si>
     <t>playerName</t>
   </si>
   <si>
-    <t>Football fc</t>
-  </si>
-  <si>
-    <t>Maisie Rogers</t>
-  </si>
-  <si>
-    <t>3,427,444</t>
-  </si>
-  <si>
-    <t>FC SZTEJTI 10</t>
-  </si>
-  <si>
-    <t>Adam Sztejter</t>
-  </si>
-  <si>
-    <t>16,963</t>
-  </si>
-  <si>
-    <t>Holy hamburgers</t>
-  </si>
-  <si>
-    <t>Leri Jiso</t>
-  </si>
-  <si>
-    <t>226,285</t>
-  </si>
-  <si>
-    <t>Mohammed 94</t>
-  </si>
-  <si>
-    <t>Mohammed Mzory</t>
-  </si>
-  <si>
-    <t>1,646,257</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t>MrTrias500</t>
-  </si>
-  <si>
-    <t>Eni Shtini</t>
-  </si>
-  <si>
-    <t>317,891</t>
-  </si>
-  <si>
-    <t>431</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Traitorzero</t>
-  </si>
-  <si>
-    <t>Kamil Nainggolan</t>
-  </si>
-  <si>
-    <t>7,720</t>
-  </si>
-  <si>
-    <t>481</t>
-  </si>
-  <si>
     <t>gwXfr</t>
   </si>
   <si>
@@ -2212,6 +2080,138 @@
   </si>
   <si>
     <t>437</t>
+  </si>
+  <si>
+    <t>SpielerName</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>tacoma</t>
+  </si>
+  <si>
+    <t>akron</t>
+  </si>
+  <si>
+    <t>reus</t>
+  </si>
+  <si>
+    <t>11.87.</t>
+  </si>
+  <si>
+    <t>47.6062,-122.3321</t>
+  </si>
+  <si>
+    <t>13.64.</t>
+  </si>
+  <si>
+    <t>47.2529,-122.4443</t>
+  </si>
+  <si>
+    <t>13.53.</t>
+  </si>
+  <si>
+    <t>17.31.</t>
+  </si>
+  <si>
+    <t>41.0814,-81.519</t>
+  </si>
+  <si>
+    <t>20.02.</t>
+  </si>
+  <si>
+    <t>13.71.</t>
+  </si>
+  <si>
+    <t>12.17.</t>
+  </si>
+  <si>
+    <t>41.1561,1.1069</t>
+  </si>
+  <si>
+    <t>14.89.</t>
+  </si>
+  <si>
+    <t>dfk</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>AleTypiara</t>
+  </si>
+  <si>
+    <t>Koralina Jones</t>
+  </si>
+  <si>
+    <t>1,285,839</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Joe Rodon Experience</t>
+  </si>
+  <si>
+    <t>Ivar Mehl Olsen</t>
+  </si>
+  <si>
+    <t>409,075</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>begalviai</t>
+  </si>
+  <si>
+    <t>Martynas Džiugas</t>
+  </si>
+  <si>
+    <t>44,679</t>
+  </si>
+  <si>
+    <t>484</t>
+  </si>
+  <si>
+    <t>Gilmour Girls</t>
+  </si>
+  <si>
+    <t>Jath V</t>
+  </si>
+  <si>
+    <t>390,758</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>(C) Scarlett</t>
+  </si>
+  <si>
+    <t>Rob Sinclair</t>
+  </si>
+  <si>
+    <t>11,899</t>
+  </si>
+  <si>
+    <t>497</t>
+  </si>
+  <si>
+    <t>Soucek &amp; the BenMees</t>
+  </si>
+  <si>
+    <t>Alastair Cameron</t>
+  </si>
+  <si>
+    <t>13,047</t>
   </si>
 </sst>
 </file>
@@ -2687,13 +2687,13 @@
   <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
     <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
     <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
@@ -2798,25 +2798,25 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>654</v>
+        <v>691</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>654</v>
+        <v>691</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>208</v>
@@ -2863,163 +2863,163 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>651</v>
+        <v>687</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>655</v>
+        <v>692</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>635</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>656</v>
+        <v>693</v>
       </c>
       <c r="E3" t="s">
-        <v>656</v>
+        <v>693</v>
       </c>
       <c r="F3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>633</v>
+        <v>688</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>634</v>
+        <v>694</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>635</v>
+        <v>140</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>657</v>
+        <v>695</v>
       </c>
       <c r="E4" t="s">
-        <v>657</v>
+        <v>695</v>
       </c>
       <c r="F4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D5" t="s">
-        <v>658</v>
+        <v>696</v>
       </c>
       <c r="E5" t="s">
-        <v>658</v>
+        <v>696</v>
       </c>
       <c r="F5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>650</v>
+        <v>689</v>
       </c>
       <c r="B6" t="s">
-        <v>659</v>
+        <v>697</v>
       </c>
       <c r="C6" t="s">
         <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>660</v>
+        <v>698</v>
       </c>
       <c r="E6" t="s">
-        <v>660</v>
+        <v>698</v>
       </c>
       <c r="F6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="B7" t="s">
-        <v>661</v>
+        <v>649</v>
       </c>
       <c r="C7" t="s">
-        <v>662</v>
+        <v>650</v>
       </c>
       <c r="D7" t="s">
-        <v>663</v>
+        <v>699</v>
       </c>
       <c r="E7" t="s">
-        <v>663</v>
+        <v>699</v>
       </c>
       <c r="F7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="G7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D8" t="s">
-        <v>664</v>
+        <v>700</v>
       </c>
       <c r="E8" t="s">
-        <v>664</v>
+        <v>700</v>
       </c>
       <c r="F8" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G8" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>690</v>
       </c>
       <c r="B9" t="s">
-        <v>647</v>
+        <v>701</v>
       </c>
       <c r="C9" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D9" t="s">
-        <v>665</v>
+        <v>702</v>
       </c>
       <c r="E9" t="s">
-        <v>665</v>
+        <v>702</v>
       </c>
       <c r="F9" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="G9" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -5445,8 +5445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8224,24 +8224,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.93359375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.74609375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.07421875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.87109375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>211</v>
       </c>
@@ -8258,148 +8260,238 @@
         <v>603</v>
       </c>
       <c r="F1" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
       <c r="G1" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+      <c r="H1" t="s">
+        <v>703</v>
+      </c>
+      <c r="I1" t="s">
+        <v>703</v>
+      </c>
+      <c r="J1" t="s">
+        <v>703</v>
+      </c>
+      <c r="K1" t="s">
+        <v>703</v>
+      </c>
+      <c r="L1" t="s">
+        <v>703</v>
+      </c>
+      <c r="M1" t="s">
+        <v>703</v>
+      </c>
+      <c r="N1" t="s">
+        <v>703</v>
+      </c>
+      <c r="O1" t="s">
+        <v>703</v>
+      </c>
+      <c r="P1" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>703</v>
+      </c>
+      <c r="R1" t="s">
+        <v>686</v>
+      </c>
+      <c r="S1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T1" t="s">
+        <v>330</v>
+      </c>
+      <c r="U1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V1" t="s">
+        <v>332</v>
+      </c>
+      <c r="W1" t="s">
+        <v>333</v>
+      </c>
+      <c r="X1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
-        <v>687</v>
+        <v>704</v>
       </c>
       <c r="D2" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="E2" t="s">
-        <v>700</v>
+        <v>707</v>
       </c>
       <c r="F2" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="G2" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="B3">
+        <v>324</v>
+      </c>
+      <c r="C3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D3" t="s">
+        <v>713</v>
+      </c>
+      <c r="E3" t="s">
+        <v>712</v>
+      </c>
+      <c r="F3" t="s">
+        <v>711</v>
+      </c>
+      <c r="G3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B4">
+        <v>325</v>
+      </c>
+      <c r="C4" t="s">
+        <v>709</v>
+      </c>
+      <c r="D4" t="s">
+        <v>717</v>
+      </c>
+      <c r="E4" t="s">
+        <v>716</v>
+      </c>
+      <c r="F4" t="s">
+        <v>715</v>
+      </c>
+      <c r="G4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B5">
+        <v>326</v>
+      </c>
+      <c r="C5" t="s">
         <v>704</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>703</v>
-      </c>
-      <c r="D3" t="s">
-        <v>707</v>
-      </c>
-      <c r="E3" t="s">
-        <v>706</v>
-      </c>
-      <c r="F3" t="s">
-        <v>705</v>
-      </c>
-      <c r="G3" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>709</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>687</v>
-      </c>
-      <c r="D4" t="s">
-        <v>712</v>
-      </c>
-      <c r="E4" t="s">
-        <v>711</v>
-      </c>
-      <c r="F4" t="s">
-        <v>710</v>
-      </c>
-      <c r="G4" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>715</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>714</v>
-      </c>
       <c r="D5" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="E5" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="F5" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="G5" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>327</v>
       </c>
       <c r="C6" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="D6" t="s">
+        <v>726</v>
+      </c>
+      <c r="E6" t="s">
+        <v>725</v>
+      </c>
+      <c r="F6" t="s">
         <v>724</v>
       </c>
-      <c r="E6" t="s">
-        <v>723</v>
-      </c>
-      <c r="F6" t="s">
-        <v>722</v>
-      </c>
       <c r="G6" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B7">
+        <v>328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" t="s">
         <v>726</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>725</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>729</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>728</v>
       </c>
-      <c r="F7" t="s">
-        <v>727</v>
-      </c>
       <c r="G7" t="s">
-        <v>713</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
foundation done for vba replica
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="705">
   <si>
     <t>Places</t>
   </si>
@@ -1986,9 +1986,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>SpielerName</t>
   </si>
   <si>
@@ -2043,42 +2040,9 @@
     <t>dfk</t>
   </si>
   <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>Rubber Digne Rapids</t>
-  </si>
-  <si>
-    <t>Shahzad Yasin</t>
-  </si>
-  <si>
-    <t>269,865</t>
-  </si>
-  <si>
-    <t>458</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>InsertWittyNameHere</t>
-  </si>
-  <si>
-    <t>tom newall</t>
-  </si>
-  <si>
-    <t>98,153</t>
-  </si>
-  <si>
-    <t>474</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
-    <t>Lagomt</t>
-  </si>
-  <si>
     <t>Morris Ku</t>
   </si>
   <si>
@@ -2094,9 +2058,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>Pepe Pig</t>
-  </si>
-  <si>
     <t>Dillon Williams</t>
   </si>
   <si>
@@ -2104,13 +2065,84 @@
   </si>
   <si>
     <t>456</t>
+  </si>
+  <si>
+    <t>Sánchez 6</t>
+  </si>
+  <si>
+    <t>Duffy 6</t>
+  </si>
+  <si>
+    <t>Livramento 4</t>
+  </si>
+  <si>
+    <t>White 7</t>
+  </si>
+  <si>
+    <t>Salah 13</t>
+  </si>
+  <si>
+    <t>Gray 2</t>
+  </si>
+  <si>
+    <t>Raphinha 3</t>
+  </si>
+  <si>
+    <t>Sarr 1</t>
+  </si>
+  <si>
+    <t>Antonio 2</t>
+  </si>
+  <si>
+    <t>Ronaldo 1</t>
+  </si>
+  <si>
+    <t>Lukaku 4</t>
+  </si>
+  <si>
+    <t>S.Longstaff 2</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold 0</t>
+  </si>
+  <si>
+    <t>Amartey 0</t>
+  </si>
+  <si>
+    <t>Ramsdale 6</t>
+  </si>
+  <si>
+    <t>Dias 0</t>
+  </si>
+  <si>
+    <t>Rüdiger 2</t>
+  </si>
+  <si>
+    <t>Cancelo 0</t>
+  </si>
+  <si>
+    <t>Saka 3</t>
+  </si>
+  <si>
+    <t>Gallagher 2</t>
+  </si>
+  <si>
+    <t>Saint-Maximin 2</t>
+  </si>
+  <si>
+    <t>Foster 2</t>
+  </si>
+  <si>
+    <t>Christensen 0</t>
+  </si>
+  <si>
+    <t>Douglas Luiz 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2584,19 +2616,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
-    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
-    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
-    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -2699,10 +2731,10 @@
         <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>637</v>
@@ -2755,19 +2787,19 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F3" t="s">
         <v>638</v>
@@ -2778,19 +2810,19 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F4" t="s">
         <v>639</v>
@@ -2810,10 +2842,10 @@
         <v>633</v>
       </c>
       <c r="D5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F5" t="s">
         <v>640</v>
@@ -2824,19 +2856,19 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C6" t="s">
         <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F6" t="s">
         <v>641</v>
@@ -2856,10 +2888,10 @@
         <v>650</v>
       </c>
       <c r="D7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F7" t="s">
         <v>642</v>
@@ -2879,10 +2911,10 @@
         <v>633</v>
       </c>
       <c r="D8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F8" t="s">
         <v>644</v>
@@ -2893,19 +2925,19 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C9" t="s">
         <v>633</v>
       </c>
       <c r="D9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F9" t="s">
         <v>645</v>
@@ -2931,9 +2963,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3325,10 +3357,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,10 +3746,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -5072,10 +5104,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5337,18 +5369,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -8116,23 +8148,36 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.79296875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.93359375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -8158,37 +8203,37 @@
         <v>652</v>
       </c>
       <c r="H1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="Q1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="R1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="S1" t="s">
         <v>329</v>
@@ -8250,48 +8295,378 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2438499</v>
+      </c>
+      <c r="C2" t="s">
+        <v>672</v>
+      </c>
+      <c r="D2" t="s">
+        <v>675</v>
+      </c>
+      <c r="E2" t="s">
+        <v>674</v>
+      </c>
+      <c r="F2" t="s">
+        <v>673</v>
+      </c>
+      <c r="G2" t="s">
+        <v>676</v>
+      </c>
+      <c r="T2" t="s">
+        <v>681</v>
+      </c>
+      <c r="U2" t="s">
+        <v>682</v>
+      </c>
+      <c r="V2" t="s">
+        <v>683</v>
+      </c>
+      <c r="W2" t="s">
         <v>684</v>
       </c>
-      <c r="B2">
-        <v>100000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="X2" t="s">
+        <v>685</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>686</v>
+      </c>
+      <c r="Z2" t="s">
         <v>687</v>
       </c>
-      <c r="E2" t="s">
-        <v>686</v>
-      </c>
-      <c r="F2" t="s">
-        <v>685</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="AA2" t="s">
         <v>688</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>689</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>690</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>691</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>692</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>693</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>690</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
+        <v>271</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>677</v>
       </c>
       <c r="D3" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="E3" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="F3" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
+      </c>
+      <c r="T3" t="s">
+        <v>695</v>
+      </c>
+      <c r="U3" t="s">
+        <v>696</v>
+      </c>
+      <c r="V3" t="s">
+        <v>697</v>
+      </c>
+      <c r="W3" t="s">
+        <v>698</v>
+      </c>
+      <c r="X3" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>700</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>685</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>687</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>691</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>701</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>689</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>702</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>704</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="8">
+        <v>4115919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2324952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2522621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="8">
+        <v>488734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1069199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1327409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2203632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3998490</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="8">
+        <v>440807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2184142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2795791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15" s="8">
+        <v>228724</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2185186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2317783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18" s="8">
+        <v>364277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1396639</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1339989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="8">
+        <v>474028</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>306</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1229286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2340261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1708392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>310</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2719892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" s="8">
+        <v>122847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>312</v>
+      </c>
+      <c r="B27" s="8">
+        <v>362369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>313</v>
+      </c>
+      <c r="B28" s="8">
+        <v>290784</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>314</v>
+      </c>
+      <c r="B29" s="8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>315</v>
+      </c>
+      <c r="B30" s="8">
+        <v>23487</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B31" s="8">
+        <v>360554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2090014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B33" s="8">
+        <v>158870</v>
       </c>
     </row>
   </sheetData>
@@ -8309,10 +8684,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
gw 26 fpl6 done
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="bluePrint" sheetId="7" r:id="rId7"/>
     <sheet name="turf" sheetId="8" r:id="rId8"/>
     <sheet name="sept" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="909">
   <si>
     <t>Places</t>
   </si>
@@ -1986,9 +1987,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>SpielerName</t>
-  </si>
-  <si>
     <t>Seattle</t>
   </si>
   <si>
@@ -2043,106 +2041,722 @@
     <t>49</t>
   </si>
   <si>
-    <t>Morris Ku</t>
-  </si>
-  <si>
-    <t>207,246</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Sánchez 6</t>
+  </si>
+  <si>
+    <t>Duffy 6</t>
+  </si>
+  <si>
+    <t>Livramento 4</t>
+  </si>
+  <si>
+    <t>White 7</t>
+  </si>
+  <si>
+    <t>Salah 13</t>
+  </si>
+  <si>
+    <t>Gray 2</t>
+  </si>
+  <si>
+    <t>Raphinha 3</t>
+  </si>
+  <si>
+    <t>Sarr 1</t>
+  </si>
+  <si>
+    <t>Antonio 2</t>
+  </si>
+  <si>
+    <t>Ronaldo 1</t>
+  </si>
+  <si>
+    <t>Lukaku 4</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold 0</t>
+  </si>
+  <si>
+    <t>Amartey 0</t>
+  </si>
+  <si>
+    <t>Ramsdale 6</t>
+  </si>
+  <si>
+    <t>Dias 0</t>
+  </si>
+  <si>
+    <t>Rüdiger 2</t>
+  </si>
+  <si>
+    <t>Cancelo 0</t>
+  </si>
+  <si>
+    <t>Saka 3</t>
+  </si>
+  <si>
+    <t>Gallagher 2</t>
+  </si>
+  <si>
+    <t>Saint-Maximin 2</t>
+  </si>
+  <si>
+    <t>Foster 2</t>
+  </si>
+  <si>
+    <t>Christensen 0</t>
+  </si>
+  <si>
+    <t>Douglas Luiz 2</t>
+  </si>
+  <si>
+    <t>Marçal 3</t>
+  </si>
+  <si>
+    <t>Fernandes 5</t>
+  </si>
+  <si>
+    <t>Salah 26</t>
+  </si>
+  <si>
+    <t>Greenwood 1</t>
+  </si>
+  <si>
+    <t>Maupay 1</t>
+  </si>
+  <si>
+    <t>Pukki 2</t>
+  </si>
+  <si>
+    <t>Torres 0</t>
+  </si>
+  <si>
+    <t>Kanté 0</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>2,930,864</t>
+  </si>
+  <si>
+    <t>376</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Alonso 0</t>
+  </si>
+  <si>
+    <t>Klich 3</t>
+  </si>
+  <si>
+    <t>Guaita 2</t>
+  </si>
+  <si>
+    <t>Omobamidele 0</t>
+  </si>
+  <si>
+    <t>Archer 1</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Lucky FC</t>
+  </si>
+  <si>
+    <t>Saurabh Tamang</t>
+  </si>
+  <si>
+    <t>3,705,347</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>Schmeichel 1</t>
+  </si>
+  <si>
+    <t>Shaw 2</t>
+  </si>
+  <si>
+    <t>Dier 3</t>
+  </si>
+  <si>
+    <t>Kovacic 2</t>
+  </si>
+  <si>
+    <t>Smith Rowe 3</t>
+  </si>
+  <si>
+    <t>Immortal FC</t>
+  </si>
+  <si>
+    <t>Pranesh Sharma</t>
+  </si>
+  <si>
+    <t>2,202,109</t>
+  </si>
+  <si>
+    <t>393</t>
+  </si>
+  <si>
+    <t>Mendy 2</t>
+  </si>
+  <si>
+    <t>van Dijk 1</t>
+  </si>
+  <si>
+    <t>Lukaku 2</t>
+  </si>
+  <si>
+    <t>Elyounoussi 1</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>GAROBADHA UNITED</t>
+  </si>
+  <si>
+    <t>957,666</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>Thiago Silva 1</t>
+  </si>
+  <si>
+    <t>Tomiyasu 6</t>
+  </si>
+  <si>
+    <t>Reguilón 2</t>
+  </si>
+  <si>
+    <t>James 3</t>
+  </si>
+  <si>
+    <t>Benrahma 2</t>
+  </si>
+  <si>
+    <t>Ødegaard 3</t>
+  </si>
+  <si>
+    <t>Vardy 8</t>
+  </si>
+  <si>
+    <t>Antonio 4</t>
+  </si>
+  <si>
+    <t>McCarthy 3</t>
+  </si>
+  <si>
+    <t>Moder 3</t>
+  </si>
+  <si>
+    <t>The Borderland Fc</t>
+  </si>
+  <si>
+    <t>1,642,402</t>
+  </si>
+  <si>
+    <t>407</t>
+  </si>
+  <si>
+    <t>Walker 1</t>
+  </si>
+  <si>
+    <t>Doucouré 5</t>
+  </si>
+  <si>
+    <t>Ward-Prowse 4</t>
+  </si>
+  <si>
+    <t>Dennis 1</t>
+  </si>
+  <si>
+    <t>Tsimikas 0</t>
+  </si>
+  <si>
+    <t>Bissouma 0</t>
+  </si>
+  <si>
+    <t>2,490,505</t>
+  </si>
+  <si>
+    <t>386</t>
+  </si>
+  <si>
+    <t>Veltman 5</t>
+  </si>
+  <si>
+    <t>Pinnock 2</t>
+  </si>
+  <si>
+    <t>Jota 2</t>
+  </si>
+  <si>
+    <t>Ronaldo 2</t>
+  </si>
+  <si>
+    <t>Scarlett 0</t>
+  </si>
+  <si>
+    <t>BUSBY BABIES 2</t>
+  </si>
+  <si>
+    <t>455,744</t>
+  </si>
+  <si>
+    <t>447</t>
+  </si>
+  <si>
+    <t>Manquillo 3</t>
+  </si>
+  <si>
+    <t>Raya 3</t>
+  </si>
+  <si>
+    <t>SYAKREE FC</t>
+  </si>
+  <si>
+    <t>1,562,668</t>
+  </si>
+  <si>
+    <t>409</t>
+  </si>
+  <si>
+    <t>Ward 0</t>
+  </si>
+  <si>
+    <t>Gilmour 0</t>
+  </si>
+  <si>
+    <t>Ashim Lama</t>
+  </si>
+  <si>
+    <t>1,383,981</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>PEPPERBOX83</t>
+  </si>
+  <si>
+    <t>Vivek Pradhan</t>
+  </si>
+  <si>
+    <t>1,210,823</t>
+  </si>
+  <si>
+    <t>419</t>
+  </si>
+  <si>
+    <t>Grealish 2</t>
+  </si>
+  <si>
+    <t>Ederson 1</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>1,080,787</t>
+  </si>
+  <si>
+    <t>423</t>
+  </si>
+  <si>
+    <t>Alisson 1</t>
+  </si>
+  <si>
+    <t>Jansson 5</t>
+  </si>
+  <si>
+    <t>Varane 2</t>
+  </si>
+  <si>
+    <t>Bamford 0</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>1,145,115</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>Meslier 6</t>
+  </si>
+  <si>
+    <t>Söyüncü 1</t>
+  </si>
+  <si>
+    <t>Tierney 6</t>
+  </si>
+  <si>
+    <t>Coady 2</t>
+  </si>
+  <si>
+    <t>Digne 2</t>
+  </si>
+  <si>
+    <t>Maddison 1</t>
+  </si>
+  <si>
+    <t>Aubameyang 2</t>
+  </si>
+  <si>
+    <t>Jiménez 10</t>
+  </si>
+  <si>
+    <t>Kung Fu Pandoos</t>
+  </si>
+  <si>
+    <t>1,014,782</t>
+  </si>
+  <si>
+    <t>425</t>
+  </si>
+  <si>
+    <t>Toney 2</t>
+  </si>
+  <si>
+    <t>PL CG FC</t>
+  </si>
+  <si>
+    <t>Rishi Thulung</t>
+  </si>
+  <si>
+    <t>573,917</t>
+  </si>
+  <si>
+    <t>442</t>
+  </si>
+  <si>
+    <t>Steele 0</t>
+  </si>
+  <si>
+    <t>Allan 2</t>
+  </si>
+  <si>
+    <t>Williams 0</t>
+  </si>
+  <si>
+    <t>475,884</t>
+  </si>
+  <si>
+    <t>446</t>
+  </si>
+  <si>
+    <t>McArthur 1</t>
+  </si>
+  <si>
+    <t>1,279,096</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>Benrahma 4</t>
+  </si>
+  <si>
+    <t>Obafemi 0</t>
+  </si>
+  <si>
+    <t>Gustavous Gunner</t>
+  </si>
+  <si>
+    <t>657,196</t>
+  </si>
+  <si>
+    <t>438</t>
+  </si>
+  <si>
+    <t>Azpilicueta 10</t>
+  </si>
+  <si>
+    <t>Brownhill 2</t>
+  </si>
+  <si>
+    <t>False 9</t>
+  </si>
+  <si>
+    <t>269,865</t>
+  </si>
+  <si>
+    <t>458</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Weightloss Coach</t>
+  </si>
+  <si>
+    <t>386,683</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>Coufal 1</t>
+  </si>
+  <si>
+    <t>334,845</t>
+  </si>
+  <si>
+    <t>454</t>
+  </si>
+  <si>
+    <t>Richardson 0</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Gooner for Life 037</t>
+  </si>
+  <si>
+    <t>541,562</t>
+  </si>
+  <si>
+    <t>443</t>
+  </si>
+  <si>
+    <t>Sá 2</t>
+  </si>
+  <si>
+    <t>Matip 1</t>
+  </si>
+  <si>
+    <t>RAJIYUNG Sun</t>
+  </si>
+  <si>
+    <t>423,397</t>
+  </si>
+  <si>
+    <t>449</t>
+  </si>
+  <si>
+    <t>Krul 9</t>
+  </si>
+  <si>
+    <t>Tielemans 1</t>
+  </si>
+  <si>
+    <t>Almirón 2</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>404,624</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>Jiménez 20</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>prabin kumar</t>
+  </si>
+  <si>
+    <t>1,978,926</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>Semedo 2</t>
+  </si>
+  <si>
+    <t>Marijuana Fields FC</t>
+  </si>
+  <si>
+    <t>693,096</t>
+  </si>
+  <si>
+    <t>437</t>
+  </si>
+  <si>
+    <t>Mbeumo 8</t>
+  </si>
+  <si>
+    <t>abcde FC</t>
+  </si>
+  <si>
+    <t>Prayash Thapa</t>
+  </si>
+  <si>
+    <t>105,628</t>
+  </si>
+  <si>
+    <t>473</t>
+  </si>
+  <si>
+    <t>One Step Beyond 026*</t>
+  </si>
+  <si>
+    <t>Tenzing Ninjey</t>
+  </si>
+  <si>
+    <t>442,587</t>
+  </si>
+  <si>
+    <t>448</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Up the Bees</t>
+  </si>
+  <si>
+    <t>Harsh Raval</t>
+  </si>
+  <si>
+    <t>6,731</t>
+  </si>
+  <si>
+    <t>502</t>
+  </si>
+  <si>
+    <t>PRAYAS BAJGAI</t>
+  </si>
+  <si>
+    <t>152,754</t>
+  </si>
+  <si>
+    <t>468</t>
+  </si>
+  <si>
+    <t>Raphinha 6</t>
+  </si>
+  <si>
+    <t>Roing FC</t>
+  </si>
+  <si>
+    <t>AVIJIT DAS</t>
+  </si>
+  <si>
+    <t>222,646</t>
+  </si>
+  <si>
+    <t>462</t>
+  </si>
+  <si>
+    <t>Wan-Bissaka 2</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>WEIGHTLOSS COACH</t>
+  </si>
+  <si>
+    <t>155,423</t>
+  </si>
+  <si>
+    <t>117,486</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainer_name </t>
+  </si>
+  <si>
+    <t>Pickford 3</t>
+  </si>
+  <si>
+    <t>Rashica 1</t>
+  </si>
+  <si>
+    <t>Son 10</t>
+  </si>
+  <si>
+    <t>Calvert-Lewin 0</t>
+  </si>
+  <si>
+    <t>Begović 0</t>
+  </si>
+  <si>
+    <t>Reid 0</t>
+  </si>
+  <si>
+    <t>Chiellini2020</t>
+  </si>
+  <si>
+    <t>enio minxhozi</t>
+  </si>
+  <si>
+    <t>202,671</t>
   </si>
   <si>
     <t>463</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Dillon Williams</t>
-  </si>
-  <si>
-    <t>302,936</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>Sánchez 6</t>
-  </si>
-  <si>
-    <t>Duffy 6</t>
-  </si>
-  <si>
-    <t>Livramento 4</t>
-  </si>
-  <si>
-    <t>White 7</t>
-  </si>
-  <si>
-    <t>Salah 13</t>
-  </si>
-  <si>
-    <t>Gray 2</t>
-  </si>
-  <si>
-    <t>Raphinha 3</t>
-  </si>
-  <si>
-    <t>Sarr 1</t>
-  </si>
-  <si>
-    <t>Antonio 2</t>
-  </si>
-  <si>
-    <t>Ronaldo 1</t>
-  </si>
-  <si>
-    <t>Lukaku 4</t>
-  </si>
-  <si>
-    <t>S.Longstaff 2</t>
-  </si>
-  <si>
-    <t>Alexander-Arnold 0</t>
-  </si>
-  <si>
-    <t>Amartey 0</t>
-  </si>
-  <si>
-    <t>Ramsdale 6</t>
-  </si>
-  <si>
-    <t>Dias 0</t>
-  </si>
-  <si>
-    <t>Rüdiger 2</t>
-  </si>
-  <si>
-    <t>Cancelo 0</t>
-  </si>
-  <si>
-    <t>Saka 3</t>
-  </si>
-  <si>
-    <t>Gallagher 2</t>
-  </si>
-  <si>
-    <t>Saint-Maximin 2</t>
-  </si>
-  <si>
-    <t>Foster 2</t>
-  </si>
-  <si>
-    <t>Christensen 0</t>
-  </si>
-  <si>
-    <t>Douglas Luiz 2</t>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Not sure yet</t>
+  </si>
+  <si>
+    <t>Sunit Patel</t>
+  </si>
+  <si>
+    <t>20,082</t>
+  </si>
+  <si>
+    <t>493</t>
+  </si>
+  <si>
+    <t>Supercampeones</t>
+  </si>
+  <si>
+    <t>Ronny Nelkenbaum</t>
+  </si>
+  <si>
+    <t>338,771</t>
+  </si>
+  <si>
+    <t>11 spaghetti</t>
+  </si>
+  <si>
+    <t>teo teo</t>
+  </si>
+  <si>
+    <t>240,712</t>
+  </si>
+  <si>
+    <t>460</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2616,19 +3230,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
+    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -2731,10 +3345,10 @@
         <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>637</v>
@@ -2787,19 +3401,19 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F3" t="s">
         <v>638</v>
@@ -2810,19 +3424,19 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F4" t="s">
         <v>639</v>
@@ -2842,10 +3456,10 @@
         <v>633</v>
       </c>
       <c r="D5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F5" t="s">
         <v>640</v>
@@ -2856,19 +3470,19 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C6" t="s">
         <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F6" t="s">
         <v>641</v>
@@ -2888,10 +3502,10 @@
         <v>650</v>
       </c>
       <c r="D7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F7" t="s">
         <v>642</v>
@@ -2911,10 +3525,10 @@
         <v>633</v>
       </c>
       <c r="D8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F8" t="s">
         <v>644</v>
@@ -2925,25 +3539,534 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C9" t="s">
         <v>633</v>
       </c>
       <c r="D9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F9" t="s">
         <v>645</v>
       </c>
       <c r="G9" t="s">
         <v>645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.484375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.32421875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.45703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="9.72265625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.3671875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.8984375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.94140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.91796875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.265625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="E1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F1" t="s">
+        <v>651</v>
+      </c>
+      <c r="G1" t="s">
+        <v>652</v>
+      </c>
+      <c r="H1" t="s">
+        <v>670</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>670</v>
+      </c>
+      <c r="K1" t="s">
+        <v>670</v>
+      </c>
+      <c r="L1" t="s">
+        <v>670</v>
+      </c>
+      <c r="M1" t="s">
+        <v>670</v>
+      </c>
+      <c r="N1" t="s">
+        <v>670</v>
+      </c>
+      <c r="O1" t="s">
+        <v>670</v>
+      </c>
+      <c r="P1" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>670</v>
+      </c>
+      <c r="R1" t="s">
+        <v>328</v>
+      </c>
+      <c r="S1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T1" t="s">
+        <v>330</v>
+      </c>
+      <c r="U1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V1" t="s">
+        <v>332</v>
+      </c>
+      <c r="W1" t="s">
+        <v>333</v>
+      </c>
+      <c r="X1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B2">
+        <v>5695560</v>
+      </c>
+      <c r="C2" t="s">
+        <v>671</v>
+      </c>
+      <c r="D2" t="s">
+        <v>896</v>
+      </c>
+      <c r="E2" t="s">
+        <v>895</v>
+      </c>
+      <c r="G2" t="s">
+        <v>672</v>
+      </c>
+      <c r="R2" t="s">
+        <v>894</v>
+      </c>
+      <c r="S2" t="s">
+        <v>893</v>
+      </c>
+      <c r="T2" t="s">
+        <v>887</v>
+      </c>
+      <c r="U2" t="s">
+        <v>738</v>
+      </c>
+      <c r="V2" t="s">
+        <v>736</v>
+      </c>
+      <c r="W2" t="s">
+        <v>688</v>
+      </c>
+      <c r="X2" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>888</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>889</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>890</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>891</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>753</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>754</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>899</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1153704</v>
+      </c>
+      <c r="C3" t="s">
+        <v>897</v>
+      </c>
+      <c r="D3" t="s">
+        <v>901</v>
+      </c>
+      <c r="E3" t="s">
+        <v>900</v>
+      </c>
+      <c r="G3" t="s">
+        <v>672</v>
+      </c>
+      <c r="R3" t="s">
+        <v>899</v>
+      </c>
+      <c r="S3" t="s">
+        <v>898</v>
+      </c>
+      <c r="T3" t="s">
+        <v>674</v>
+      </c>
+      <c r="U3" t="s">
+        <v>689</v>
+      </c>
+      <c r="V3" t="s">
+        <v>821</v>
+      </c>
+      <c r="W3" t="s">
+        <v>677</v>
+      </c>
+      <c r="X3" t="s">
+        <v>759</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>760</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>799</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>822</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B4">
+        <v>440807</v>
+      </c>
+      <c r="C4" t="s">
+        <v>782</v>
+      </c>
+      <c r="D4" t="s">
+        <v>784</v>
+      </c>
+      <c r="E4" t="s">
+        <v>783</v>
+      </c>
+      <c r="G4" t="s">
+        <v>653</v>
+      </c>
+      <c r="R4" t="s">
+        <v>418</v>
+      </c>
+      <c r="S4" t="s">
+        <v>289</v>
+      </c>
+      <c r="T4" t="s">
+        <v>687</v>
+      </c>
+      <c r="U4" t="s">
+        <v>689</v>
+      </c>
+      <c r="V4" t="s">
+        <v>677</v>
+      </c>
+      <c r="W4" t="s">
+        <v>688</v>
+      </c>
+      <c r="X4" t="s">
+        <v>780</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>723</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>684</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>693</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>781</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>903</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4642646</v>
+      </c>
+      <c r="C5" t="s">
+        <v>732</v>
+      </c>
+      <c r="D5" t="s">
+        <v>832</v>
+      </c>
+      <c r="E5" t="s">
+        <v>904</v>
+      </c>
+      <c r="G5" t="s">
+        <v>653</v>
+      </c>
+      <c r="R5" t="s">
+        <v>903</v>
+      </c>
+      <c r="S5" t="s">
+        <v>902</v>
+      </c>
+      <c r="T5" t="s">
+        <v>674</v>
+      </c>
+      <c r="U5" t="s">
+        <v>677</v>
+      </c>
+      <c r="V5" t="s">
+        <v>697</v>
+      </c>
+      <c r="W5" t="s">
+        <v>690</v>
+      </c>
+      <c r="X5" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>722</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>799</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>730</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>906</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1364835</v>
+      </c>
+      <c r="C6" t="s">
+        <v>850</v>
+      </c>
+      <c r="D6" t="s">
+        <v>908</v>
+      </c>
+      <c r="E6" t="s">
+        <v>907</v>
+      </c>
+      <c r="G6" t="s">
+        <v>708</v>
+      </c>
+      <c r="R6" t="s">
+        <v>906</v>
+      </c>
+      <c r="S6" t="s">
+        <v>905</v>
+      </c>
+      <c r="T6" t="s">
+        <v>728</v>
+      </c>
+      <c r="U6" t="s">
+        <v>738</v>
+      </c>
+      <c r="V6" t="s">
+        <v>675</v>
+      </c>
+      <c r="W6" t="s">
+        <v>688</v>
+      </c>
+      <c r="X6" t="s">
+        <v>690</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>786</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>722</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>752</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>766</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>809</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>754</v>
       </c>
     </row>
   </sheetData>
@@ -2963,9 +4086,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3357,10 +4480,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,10 +4869,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -5104,10 +6227,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5370,17 +6493,17 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:AK1"/>
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -8150,39 +9273,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="26" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>886</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>212</v>
@@ -8203,37 +9323,37 @@
         <v>652</v>
       </c>
       <c r="H1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="P1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="Q1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="R1" t="s">
-        <v>654</v>
+        <v>328</v>
       </c>
       <c r="S1" t="s">
         <v>329</v>
@@ -8301,180 +9421,588 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>672</v>
+        <v>705</v>
       </c>
       <c r="D2" t="s">
-        <v>675</v>
+        <v>707</v>
       </c>
       <c r="E2" t="s">
+        <v>706</v>
+      </c>
+      <c r="F2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G2" t="s">
+        <v>708</v>
+      </c>
+      <c r="R2" t="s">
+        <v>548</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="T2" t="s">
         <v>674</v>
       </c>
-      <c r="F2" t="s">
-        <v>673</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="U2" t="s">
+        <v>697</v>
+      </c>
+      <c r="V2" t="s">
+        <v>677</v>
+      </c>
+      <c r="W2" t="s">
         <v>676</v>
       </c>
-      <c r="T2" t="s">
-        <v>681</v>
-      </c>
-      <c r="U2" t="s">
-        <v>682</v>
-      </c>
-      <c r="V2" t="s">
-        <v>683</v>
-      </c>
-      <c r="W2" t="s">
-        <v>684</v>
-      </c>
       <c r="X2" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>698</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>700</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>701</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>693</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>702</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>704</v>
+      </c>
+      <c r="AH2" t="s">
         <v>685</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>686</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>687</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>688</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>689</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>690</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>691</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>399</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>692</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>693</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>271</v>
+        <v>715</v>
       </c>
       <c r="B3" s="8">
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>677</v>
+        <v>714</v>
       </c>
       <c r="D3" t="s">
-        <v>680</v>
+        <v>718</v>
       </c>
       <c r="E3" t="s">
-        <v>679</v>
+        <v>717</v>
       </c>
       <c r="F3" t="s">
-        <v>678</v>
+        <v>716</v>
       </c>
       <c r="G3" t="s">
-        <v>653</v>
+        <v>672</v>
+      </c>
+      <c r="R3" t="s">
+        <v>716</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>715</v>
       </c>
       <c r="T3" t="s">
-        <v>695</v>
+        <v>674</v>
       </c>
       <c r="U3" t="s">
-        <v>696</v>
+        <v>676</v>
       </c>
       <c r="V3" t="s">
         <v>697</v>
       </c>
       <c r="W3" t="s">
-        <v>698</v>
+        <v>709</v>
       </c>
       <c r="X3" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="Y3" t="s">
-        <v>700</v>
+        <v>678</v>
       </c>
       <c r="Z3" t="s">
+        <v>692</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>710</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>711</v>
+      </c>
+      <c r="AF3" t="s">
         <v>685</v>
       </c>
-      <c r="AA3" t="s">
-        <v>687</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>691</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>701</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>689</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>702</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>703</v>
-      </c>
       <c r="AG3" t="s">
-        <v>704</v>
+        <v>712</v>
       </c>
       <c r="AH3" t="s">
-        <v>693</v>
+        <v>713</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>724</v>
       </c>
       <c r="B4" s="8">
         <v>4115919</v>
       </c>
+      <c r="C4" t="s">
+        <v>714</v>
+      </c>
+      <c r="D4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E4" t="s">
+        <v>726</v>
+      </c>
+      <c r="F4" t="s">
+        <v>725</v>
+      </c>
+      <c r="G4" t="s">
+        <v>672</v>
+      </c>
+      <c r="R4" t="s">
+        <v>725</v>
+      </c>
+      <c r="S4" t="s">
+        <v>724</v>
+      </c>
+      <c r="T4" t="s">
+        <v>719</v>
+      </c>
+      <c r="U4" t="s">
+        <v>720</v>
+      </c>
+      <c r="V4" t="s">
+        <v>721</v>
+      </c>
+      <c r="W4" t="s">
+        <v>677</v>
+      </c>
+      <c r="X4" t="s">
+        <v>722</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>723</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>702</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>733</v>
       </c>
       <c r="B5" s="8">
         <v>2324952</v>
       </c>
+      <c r="C5" t="s">
+        <v>732</v>
+      </c>
+      <c r="D5" t="s">
+        <v>735</v>
+      </c>
+      <c r="E5" t="s">
+        <v>734</v>
+      </c>
+      <c r="F5" t="s">
+        <v>583</v>
+      </c>
+      <c r="G5" t="s">
+        <v>653</v>
+      </c>
+      <c r="R5" t="s">
+        <v>583</v>
+      </c>
+      <c r="S5" t="s">
+        <v>733</v>
+      </c>
+      <c r="T5" t="s">
+        <v>728</v>
+      </c>
+      <c r="U5" t="s">
+        <v>677</v>
+      </c>
+      <c r="V5" t="s">
+        <v>690</v>
+      </c>
+      <c r="W5" t="s">
+        <v>729</v>
+      </c>
+      <c r="X5" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>692</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>691</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>702</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>731</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>746</v>
       </c>
       <c r="B6" s="8">
         <v>2522621</v>
       </c>
+      <c r="C6" t="s">
+        <v>671</v>
+      </c>
+      <c r="D6" t="s">
+        <v>748</v>
+      </c>
+      <c r="E6" t="s">
+        <v>747</v>
+      </c>
+      <c r="F6" t="s">
+        <v>495</v>
+      </c>
+      <c r="G6" t="s">
+        <v>708</v>
+      </c>
+      <c r="R6" t="s">
+        <v>495</v>
+      </c>
+      <c r="S6" t="s">
+        <v>746</v>
+      </c>
+      <c r="T6" t="s">
+        <v>687</v>
+      </c>
+      <c r="U6" t="s">
+        <v>736</v>
+      </c>
+      <c r="V6" t="s">
+        <v>737</v>
+      </c>
+      <c r="W6" t="s">
+        <v>738</v>
+      </c>
+      <c r="X6" t="s">
+        <v>739</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>741</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>743</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>690</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>435</v>
       </c>
       <c r="B7" s="8">
         <v>488734</v>
       </c>
+      <c r="C7" t="s">
+        <v>714</v>
+      </c>
+      <c r="D7" t="s">
+        <v>756</v>
+      </c>
+      <c r="E7" t="s">
+        <v>755</v>
+      </c>
+      <c r="F7" t="s">
+        <v>432</v>
+      </c>
+      <c r="G7" t="s">
+        <v>708</v>
+      </c>
+      <c r="R7" t="s">
+        <v>432</v>
+      </c>
+      <c r="S7" t="s">
+        <v>435</v>
+      </c>
+      <c r="T7" t="s">
+        <v>728</v>
+      </c>
+      <c r="U7" t="s">
+        <v>395</v>
+      </c>
+      <c r="V7" t="s">
+        <v>749</v>
+      </c>
+      <c r="W7" t="s">
+        <v>675</v>
+      </c>
+      <c r="X7" t="s">
+        <v>750</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>751</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>684</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>752</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>711</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>753</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>762</v>
       </c>
       <c r="B8" s="8">
         <v>1069199</v>
       </c>
+      <c r="C8" t="s">
+        <v>714</v>
+      </c>
+      <c r="D8" t="s">
+        <v>764</v>
+      </c>
+      <c r="E8" t="s">
+        <v>763</v>
+      </c>
+      <c r="F8" t="s">
+        <v>573</v>
+      </c>
+      <c r="G8" t="s">
+        <v>708</v>
+      </c>
+      <c r="R8" t="s">
+        <v>573</v>
+      </c>
+      <c r="S8" t="s">
+        <v>762</v>
+      </c>
+      <c r="T8" t="s">
+        <v>674</v>
+      </c>
+      <c r="U8" t="s">
+        <v>757</v>
+      </c>
+      <c r="V8" t="s">
+        <v>758</v>
+      </c>
+      <c r="W8" t="s">
+        <v>689</v>
+      </c>
+      <c r="X8" t="s">
+        <v>740</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>759</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>703</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>678</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>685</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>767</v>
       </c>
       <c r="B9" s="8">
         <v>1327409</v>
+      </c>
+      <c r="C9" t="s">
+        <v>714</v>
+      </c>
+      <c r="D9" t="s">
+        <v>769</v>
+      </c>
+      <c r="E9" t="s">
+        <v>768</v>
+      </c>
+      <c r="F9" t="s">
+        <v>566</v>
+      </c>
+      <c r="G9" t="s">
+        <v>653</v>
+      </c>
+      <c r="R9" t="s">
+        <v>566</v>
+      </c>
+      <c r="S9" t="s">
+        <v>767</v>
+      </c>
+      <c r="T9" t="s">
+        <v>674</v>
+      </c>
+      <c r="U9" t="s">
+        <v>765</v>
+      </c>
+      <c r="V9" t="s">
+        <v>688</v>
+      </c>
+      <c r="W9" t="s">
+        <v>697</v>
+      </c>
+      <c r="X9" t="s">
+        <v>703</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>750</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>741</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>683</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>684</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>752</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>766</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>754</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -8484,13 +10012,145 @@
       <c r="B10" s="8">
         <v>2203632</v>
       </c>
+      <c r="C10" t="s">
+        <v>673</v>
+      </c>
+      <c r="D10" t="s">
+        <v>774</v>
+      </c>
+      <c r="E10" t="s">
+        <v>773</v>
+      </c>
+      <c r="F10" t="s">
+        <v>772</v>
+      </c>
+      <c r="G10" t="s">
+        <v>708</v>
+      </c>
+      <c r="R10" t="s">
+        <v>772</v>
+      </c>
+      <c r="S10" t="s">
+        <v>285</v>
+      </c>
+      <c r="T10" t="s">
+        <v>436</v>
+      </c>
+      <c r="U10" t="s">
+        <v>675</v>
+      </c>
+      <c r="V10" t="s">
+        <v>709</v>
+      </c>
+      <c r="W10" t="s">
+        <v>697</v>
+      </c>
+      <c r="X10" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>692</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>684</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>770</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>686</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>771</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>287</v>
+        <v>776</v>
       </c>
       <c r="B11" s="8">
         <v>3998490</v>
+      </c>
+      <c r="C11" t="s">
+        <v>775</v>
+      </c>
+      <c r="D11" t="s">
+        <v>779</v>
+      </c>
+      <c r="E11" t="s">
+        <v>778</v>
+      </c>
+      <c r="F11" t="s">
+        <v>777</v>
+      </c>
+      <c r="G11" t="s">
+        <v>708</v>
+      </c>
+      <c r="R11" t="s">
+        <v>777</v>
+      </c>
+      <c r="S11" t="s">
+        <v>776</v>
+      </c>
+      <c r="T11" t="s">
+        <v>674</v>
+      </c>
+      <c r="U11" t="s">
+        <v>688</v>
+      </c>
+      <c r="V11" t="s">
+        <v>738</v>
+      </c>
+      <c r="W11" t="s">
+        <v>675</v>
+      </c>
+      <c r="X11" t="s">
+        <v>740</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>722</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>679</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>680</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>766</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>758</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -8500,6 +10160,72 @@
       <c r="B12" s="8">
         <v>440807</v>
       </c>
+      <c r="C12" t="s">
+        <v>782</v>
+      </c>
+      <c r="D12" t="s">
+        <v>784</v>
+      </c>
+      <c r="E12" t="s">
+        <v>783</v>
+      </c>
+      <c r="F12" t="s">
+        <v>418</v>
+      </c>
+      <c r="G12" t="s">
+        <v>653</v>
+      </c>
+      <c r="R12" t="s">
+        <v>418</v>
+      </c>
+      <c r="S12" t="s">
+        <v>289</v>
+      </c>
+      <c r="T12" t="s">
+        <v>687</v>
+      </c>
+      <c r="U12" t="s">
+        <v>689</v>
+      </c>
+      <c r="V12" t="s">
+        <v>677</v>
+      </c>
+      <c r="W12" t="s">
+        <v>688</v>
+      </c>
+      <c r="X12" t="s">
+        <v>780</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>723</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>684</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>693</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>781</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -8508,21 +10234,219 @@
       <c r="B13" s="8">
         <v>2184142</v>
       </c>
+      <c r="C13" t="s">
+        <v>789</v>
+      </c>
+      <c r="D13" t="s">
+        <v>791</v>
+      </c>
+      <c r="E13" t="s">
+        <v>790</v>
+      </c>
+      <c r="F13" t="s">
+        <v>512</v>
+      </c>
+      <c r="G13" t="s">
+        <v>672</v>
+      </c>
+      <c r="R13" t="s">
+        <v>512</v>
+      </c>
+      <c r="S13" t="s">
+        <v>291</v>
+      </c>
+      <c r="T13" t="s">
+        <v>785</v>
+      </c>
+      <c r="U13" t="s">
+        <v>786</v>
+      </c>
+      <c r="V13" t="s">
+        <v>787</v>
+      </c>
+      <c r="W13" t="s">
+        <v>675</v>
+      </c>
+      <c r="X13" t="s">
+        <v>709</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>722</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>743</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>754</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>293</v>
+        <v>800</v>
       </c>
       <c r="B14" s="8">
         <v>2795791</v>
       </c>
+      <c r="C14" t="s">
+        <v>732</v>
+      </c>
+      <c r="D14" t="s">
+        <v>802</v>
+      </c>
+      <c r="E14" t="s">
+        <v>801</v>
+      </c>
+      <c r="F14" t="s">
+        <v>459</v>
+      </c>
+      <c r="G14" t="s">
+        <v>708</v>
+      </c>
+      <c r="R14" t="s">
+        <v>459</v>
+      </c>
+      <c r="S14" t="s">
+        <v>800</v>
+      </c>
+      <c r="T14" t="s">
+        <v>792</v>
+      </c>
+      <c r="U14" t="s">
+        <v>793</v>
+      </c>
+      <c r="V14" t="s">
+        <v>794</v>
+      </c>
+      <c r="W14" t="s">
+        <v>795</v>
+      </c>
+      <c r="X14" t="s">
+        <v>796</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>797</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>798</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>684</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>799</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>754</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>295</v>
+        <v>804</v>
       </c>
       <c r="B15" s="8">
         <v>228724</v>
+      </c>
+      <c r="C15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" t="s">
+        <v>807</v>
+      </c>
+      <c r="E15" t="s">
+        <v>806</v>
+      </c>
+      <c r="F15" t="s">
+        <v>805</v>
+      </c>
+      <c r="G15" t="s">
+        <v>708</v>
+      </c>
+      <c r="R15" t="s">
+        <v>805</v>
+      </c>
+      <c r="S15" t="s">
+        <v>804</v>
+      </c>
+      <c r="T15" t="s">
+        <v>674</v>
+      </c>
+      <c r="U15" t="s">
+        <v>677</v>
+      </c>
+      <c r="V15" t="s">
+        <v>720</v>
+      </c>
+      <c r="W15" t="s">
+        <v>675</v>
+      </c>
+      <c r="X15" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>803</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>686</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -8532,141 +10456,1329 @@
       <c r="B16" s="8">
         <v>2185186</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>775</v>
+      </c>
+      <c r="D16" t="s">
+        <v>812</v>
+      </c>
+      <c r="E16" t="s">
+        <v>811</v>
+      </c>
+      <c r="F16" t="s">
+        <v>406</v>
+      </c>
+      <c r="G16" t="s">
+        <v>653</v>
+      </c>
+      <c r="R16" t="s">
+        <v>406</v>
+      </c>
+      <c r="S16" t="s">
+        <v>296</v>
+      </c>
+      <c r="T16" t="s">
+        <v>674</v>
+      </c>
+      <c r="U16" t="s">
+        <v>720</v>
+      </c>
+      <c r="V16" t="s">
+        <v>686</v>
+      </c>
+      <c r="W16" t="s">
+        <v>695</v>
+      </c>
+      <c r="X16" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>759</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>799</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>808</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>685</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>809</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>298</v>
       </c>
       <c r="B17" s="8">
         <v>2317783</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>714</v>
+      </c>
+      <c r="D17" t="s">
+        <v>815</v>
+      </c>
+      <c r="E17" t="s">
+        <v>814</v>
+      </c>
+      <c r="F17" t="s">
+        <v>348</v>
+      </c>
+      <c r="G17" t="s">
+        <v>708</v>
+      </c>
+      <c r="R17" t="s">
+        <v>348</v>
+      </c>
+      <c r="S17" t="s">
+        <v>298</v>
+      </c>
+      <c r="T17" t="s">
+        <v>674</v>
+      </c>
+      <c r="U17" t="s">
+        <v>675</v>
+      </c>
+      <c r="V17" t="s">
+        <v>689</v>
+      </c>
+      <c r="W17" t="s">
+        <v>690</v>
+      </c>
+      <c r="X17" t="s">
+        <v>679</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>813</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>683</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>809</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>300</v>
+        <v>818</v>
       </c>
       <c r="B18" s="8">
         <v>364277</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>782</v>
+      </c>
+      <c r="D18" t="s">
+        <v>820</v>
+      </c>
+      <c r="E18" t="s">
+        <v>819</v>
+      </c>
+      <c r="F18" t="s">
+        <v>527</v>
+      </c>
+      <c r="G18" t="s">
+        <v>672</v>
+      </c>
+      <c r="R18" t="s">
+        <v>527</v>
+      </c>
+      <c r="S18" t="s">
+        <v>818</v>
+      </c>
+      <c r="T18" t="s">
+        <v>719</v>
+      </c>
+      <c r="U18" t="s">
+        <v>677</v>
+      </c>
+      <c r="V18" t="s">
+        <v>675</v>
+      </c>
+      <c r="W18" t="s">
+        <v>690</v>
+      </c>
+      <c r="X18" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>816</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>692</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>678</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>798</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>302</v>
+        <v>823</v>
       </c>
       <c r="B19" s="8">
         <v>1396639</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>294</v>
+      </c>
+      <c r="D19" t="s">
+        <v>825</v>
+      </c>
+      <c r="E19" t="s">
+        <v>824</v>
+      </c>
+      <c r="F19" t="s">
+        <v>373</v>
+      </c>
+      <c r="G19" t="s">
+        <v>653</v>
+      </c>
+      <c r="R19" t="s">
+        <v>373</v>
+      </c>
+      <c r="S19" t="s">
+        <v>823</v>
+      </c>
+      <c r="T19" t="s">
+        <v>687</v>
+      </c>
+      <c r="U19" t="s">
+        <v>821</v>
+      </c>
+      <c r="V19" t="s">
+        <v>689</v>
+      </c>
+      <c r="W19" t="s">
+        <v>737</v>
+      </c>
+      <c r="X19" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>680</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>684</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>766</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>690</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>822</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>303</v>
+        <v>827</v>
       </c>
       <c r="B20" s="8">
         <v>1339989</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>826</v>
+      </c>
+      <c r="D20" t="s">
+        <v>829</v>
+      </c>
+      <c r="E20" t="s">
+        <v>828</v>
+      </c>
+      <c r="F20" t="s">
+        <v>542</v>
+      </c>
+      <c r="G20" t="s">
+        <v>708</v>
+      </c>
+      <c r="R20" t="s">
+        <v>542</v>
+      </c>
+      <c r="S20" t="s">
+        <v>827</v>
+      </c>
+      <c r="T20" t="s">
+        <v>378</v>
+      </c>
+      <c r="U20" t="s">
+        <v>765</v>
+      </c>
+      <c r="V20" t="s">
+        <v>688</v>
+      </c>
+      <c r="W20" t="s">
+        <v>395</v>
+      </c>
+      <c r="X20" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>693</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>753</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>304</v>
       </c>
       <c r="B21" s="8">
         <v>474028</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>782</v>
+      </c>
+      <c r="D21" t="s">
+        <v>832</v>
+      </c>
+      <c r="E21" t="s">
+        <v>831</v>
+      </c>
+      <c r="F21" t="s">
+        <v>401</v>
+      </c>
+      <c r="G21" t="s">
+        <v>653</v>
+      </c>
+      <c r="R21" t="s">
+        <v>401</v>
+      </c>
+      <c r="S21" t="s">
+        <v>304</v>
+      </c>
+      <c r="T21" t="s">
+        <v>674</v>
+      </c>
+      <c r="U21" t="s">
+        <v>677</v>
+      </c>
+      <c r="V21" t="s">
+        <v>697</v>
+      </c>
+      <c r="W21" t="s">
+        <v>830</v>
+      </c>
+      <c r="X21" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>759</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>680</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>760</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>808</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>720</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>835</v>
       </c>
       <c r="B22" s="8">
         <v>1229286</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>834</v>
+      </c>
+      <c r="D22" t="s">
+        <v>837</v>
+      </c>
+      <c r="E22" t="s">
+        <v>836</v>
+      </c>
+      <c r="F22" t="s">
+        <v>599</v>
+      </c>
+      <c r="G22" t="s">
+        <v>653</v>
+      </c>
+      <c r="R22" t="s">
+        <v>599</v>
+      </c>
+      <c r="S22" t="s">
+        <v>835</v>
+      </c>
+      <c r="T22" t="s">
+        <v>694</v>
+      </c>
+      <c r="U22" t="s">
+        <v>675</v>
+      </c>
+      <c r="V22" t="s">
+        <v>737</v>
+      </c>
+      <c r="W22" t="s">
+        <v>689</v>
+      </c>
+      <c r="X22" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>692</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>759</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>743</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>307</v>
       </c>
       <c r="B23" s="8">
         <v>2340261</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>673</v>
+      </c>
+      <c r="D23" t="s">
+        <v>842</v>
+      </c>
+      <c r="E23" t="s">
+        <v>841</v>
+      </c>
+      <c r="F23" t="s">
+        <v>840</v>
+      </c>
+      <c r="G23" t="s">
+        <v>708</v>
+      </c>
+      <c r="R23" t="s">
+        <v>840</v>
+      </c>
+      <c r="S23" t="s">
+        <v>307</v>
+      </c>
+      <c r="T23" t="s">
+        <v>838</v>
+      </c>
+      <c r="U23" t="s">
+        <v>839</v>
+      </c>
+      <c r="V23" t="s">
+        <v>688</v>
+      </c>
+      <c r="W23" t="s">
+        <v>697</v>
+      </c>
+      <c r="X23" t="s">
+        <v>692</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>743</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>675</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>309</v>
       </c>
       <c r="B24" s="8">
         <v>1708392</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>846</v>
+      </c>
+      <c r="D24" t="s">
+        <v>848</v>
+      </c>
+      <c r="E24" t="s">
+        <v>847</v>
+      </c>
+      <c r="F24" t="s">
+        <v>588</v>
+      </c>
+      <c r="G24" t="s">
+        <v>672</v>
+      </c>
+      <c r="R24" t="s">
+        <v>588</v>
+      </c>
+      <c r="S24" t="s">
+        <v>309</v>
+      </c>
+      <c r="T24" t="s">
+        <v>843</v>
+      </c>
+      <c r="U24" t="s">
+        <v>690</v>
+      </c>
+      <c r="V24" t="s">
+        <v>395</v>
+      </c>
+      <c r="W24" t="s">
+        <v>794</v>
+      </c>
+      <c r="X24" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>844</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>845</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>723</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>712</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>487</v>
       </c>
       <c r="B25" s="8">
         <v>2719892</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>850</v>
+      </c>
+      <c r="D25" t="s">
+        <v>853</v>
+      </c>
+      <c r="E25" t="s">
+        <v>852</v>
+      </c>
+      <c r="F25" t="s">
+        <v>851</v>
+      </c>
+      <c r="G25" t="s">
+        <v>672</v>
+      </c>
+      <c r="R25" t="s">
+        <v>851</v>
+      </c>
+      <c r="S25" t="s">
+        <v>487</v>
+      </c>
+      <c r="T25" t="s">
+        <v>728</v>
+      </c>
+      <c r="U25" t="s">
+        <v>720</v>
+      </c>
+      <c r="V25" t="s">
+        <v>688</v>
+      </c>
+      <c r="W25" t="s">
+        <v>689</v>
+      </c>
+      <c r="X25" t="s">
+        <v>759</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>780</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>700</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>849</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>753</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>311</v>
+        <v>855</v>
       </c>
       <c r="B26" s="8">
         <v>122847</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>775</v>
+      </c>
+      <c r="D26" t="s">
+        <v>857</v>
+      </c>
+      <c r="E26" t="s">
+        <v>856</v>
+      </c>
+      <c r="F26" t="s">
+        <v>595</v>
+      </c>
+      <c r="G26" t="s">
+        <v>708</v>
+      </c>
+      <c r="R26" t="s">
+        <v>595</v>
+      </c>
+      <c r="S26" t="s">
+        <v>855</v>
+      </c>
+      <c r="T26" t="s">
+        <v>674</v>
+      </c>
+      <c r="U26" t="s">
+        <v>854</v>
+      </c>
+      <c r="V26" t="s">
+        <v>689</v>
+      </c>
+      <c r="W26" t="s">
+        <v>676</v>
+      </c>
+      <c r="X26" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>759</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>702</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>808</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>685</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>822</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>312</v>
+        <v>859</v>
       </c>
       <c r="B27" s="8">
         <v>362369</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>276</v>
+      </c>
+      <c r="D27" t="s">
+        <v>862</v>
+      </c>
+      <c r="E27" t="s">
+        <v>861</v>
+      </c>
+      <c r="F27" t="s">
+        <v>860</v>
+      </c>
+      <c r="G27" t="s">
+        <v>653</v>
+      </c>
+      <c r="R27" t="s">
+        <v>860</v>
+      </c>
+      <c r="S27" t="s">
+        <v>859</v>
+      </c>
+      <c r="T27" t="s">
+        <v>687</v>
+      </c>
+      <c r="U27" t="s">
+        <v>821</v>
+      </c>
+      <c r="V27" t="s">
+        <v>690</v>
+      </c>
+      <c r="W27" t="s">
+        <v>689</v>
+      </c>
+      <c r="X27" t="s">
+        <v>691</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>858</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>696</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>688</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>313</v>
+        <v>863</v>
       </c>
       <c r="B28" s="8">
         <v>290784</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>714</v>
+      </c>
+      <c r="D28" t="s">
+        <v>866</v>
+      </c>
+      <c r="E28" t="s">
+        <v>865</v>
+      </c>
+      <c r="F28" t="s">
+        <v>864</v>
+      </c>
+      <c r="G28" t="s">
+        <v>867</v>
+      </c>
+      <c r="R28" t="s">
+        <v>864</v>
+      </c>
+      <c r="S28" t="s">
+        <v>863</v>
+      </c>
+      <c r="T28" t="s">
+        <v>674</v>
+      </c>
+      <c r="U28" t="s">
+        <v>676</v>
+      </c>
+      <c r="V28" t="s">
+        <v>689</v>
+      </c>
+      <c r="W28" t="s">
+        <v>697</v>
+      </c>
+      <c r="X28" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>752</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>684</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>810</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>709</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>868</v>
       </c>
       <c r="B29" s="8">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>789</v>
+      </c>
+      <c r="D29" t="s">
+        <v>871</v>
+      </c>
+      <c r="E29" t="s">
+        <v>870</v>
+      </c>
+      <c r="F29" t="s">
+        <v>869</v>
+      </c>
+      <c r="G29" t="s">
+        <v>653</v>
+      </c>
+      <c r="R29" t="s">
+        <v>869</v>
+      </c>
+      <c r="S29" t="s">
+        <v>868</v>
+      </c>
+      <c r="T29" t="s">
+        <v>674</v>
+      </c>
+      <c r="U29" t="s">
+        <v>677</v>
+      </c>
+      <c r="V29" t="s">
+        <v>720</v>
+      </c>
+      <c r="W29" t="s">
+        <v>688</v>
+      </c>
+      <c r="X29" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>692</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>803</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>315</v>
       </c>
       <c r="B30" s="8">
         <v>23487</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>714</v>
+      </c>
+      <c r="D30" t="s">
+        <v>874</v>
+      </c>
+      <c r="E30" t="s">
+        <v>873</v>
+      </c>
+      <c r="F30" t="s">
+        <v>872</v>
+      </c>
+      <c r="G30" t="s">
+        <v>653</v>
+      </c>
+      <c r="R30" t="s">
+        <v>872</v>
+      </c>
+      <c r="S30" t="s">
+        <v>315</v>
+      </c>
+      <c r="T30" t="s">
+        <v>687</v>
+      </c>
+      <c r="U30" t="s">
+        <v>690</v>
+      </c>
+      <c r="V30" t="s">
+        <v>676</v>
+      </c>
+      <c r="W30" t="s">
+        <v>689</v>
+      </c>
+      <c r="X30" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>723</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>822</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>810</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>317</v>
+        <v>876</v>
       </c>
       <c r="B31" s="8">
         <v>360554</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>714</v>
+      </c>
+      <c r="D31" t="s">
+        <v>879</v>
+      </c>
+      <c r="E31" t="s">
+        <v>878</v>
+      </c>
+      <c r="F31" t="s">
+        <v>877</v>
+      </c>
+      <c r="G31" t="s">
+        <v>672</v>
+      </c>
+      <c r="R31" t="s">
+        <v>877</v>
+      </c>
+      <c r="S31" t="s">
+        <v>876</v>
+      </c>
+      <c r="T31" t="s">
+        <v>674</v>
+      </c>
+      <c r="U31" t="s">
+        <v>720</v>
+      </c>
+      <c r="V31" t="s">
+        <v>689</v>
+      </c>
+      <c r="W31" t="s">
+        <v>854</v>
+      </c>
+      <c r="X31" t="s">
+        <v>875</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>803</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>808</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>822</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>686</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>318</v>
+        <v>882</v>
       </c>
       <c r="B32" s="8">
         <v>2090014</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>881</v>
+      </c>
+      <c r="D32" t="s">
+        <v>874</v>
+      </c>
+      <c r="E32" t="s">
+        <v>883</v>
+      </c>
+      <c r="F32" t="s">
+        <v>520</v>
+      </c>
+      <c r="G32" t="s">
+        <v>708</v>
+      </c>
+      <c r="R32" t="s">
+        <v>520</v>
+      </c>
+      <c r="S32" t="s">
+        <v>882</v>
+      </c>
+      <c r="T32" t="s">
+        <v>838</v>
+      </c>
+      <c r="U32" t="s">
+        <v>688</v>
+      </c>
+      <c r="V32" t="s">
+        <v>880</v>
+      </c>
+      <c r="W32" t="s">
+        <v>765</v>
+      </c>
+      <c r="X32" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>680</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>803</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>760</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>753</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>709</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>267</v>
       </c>
       <c r="B33" s="8">
         <v>158870</v>
+      </c>
+      <c r="C33" t="s">
+        <v>846</v>
+      </c>
+      <c r="D33" t="s">
+        <v>885</v>
+      </c>
+      <c r="E33" t="s">
+        <v>884</v>
+      </c>
+      <c r="F33" t="s">
+        <v>444</v>
+      </c>
+      <c r="G33" t="s">
+        <v>708</v>
+      </c>
+      <c r="R33" t="s">
+        <v>444</v>
+      </c>
+      <c r="S33" t="s">
+        <v>267</v>
+      </c>
+      <c r="T33" t="s">
+        <v>674</v>
+      </c>
+      <c r="U33" t="s">
+        <v>821</v>
+      </c>
+      <c r="V33" t="s">
+        <v>720</v>
+      </c>
+      <c r="W33" t="s">
+        <v>854</v>
+      </c>
+      <c r="X33" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>700</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>740</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>822</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>760</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>788</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -8684,10 +11796,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minutes before majaor breakthrough
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,15 @@
     <sheet name="bluePrint" sheetId="7" r:id="rId7"/>
     <sheet name="turf" sheetId="8" r:id="rId8"/>
     <sheet name="sept" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet4" sheetId="10" r:id="rId10"/>
+    <sheet name="RoC" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="921">
   <si>
     <t>Places</t>
   </si>
@@ -2750,6 +2751,42 @@
   </si>
   <si>
     <t>460</t>
+  </si>
+  <si>
+    <t>Laporte 1</t>
+  </si>
+  <si>
+    <t>Maguire 0</t>
+  </si>
+  <si>
+    <t>Canós 4</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Football fc</t>
+  </si>
+  <si>
+    <t>Maisie Rogers</t>
+  </si>
+  <si>
+    <t>3,516,619</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>deval vora</t>
+  </si>
+  <si>
+    <t>1,695,039</t>
+  </si>
+  <si>
+    <t>406</t>
   </si>
 </sst>
 </file>
@@ -3570,35 +3607,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection sqref="A1:AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.484375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.32421875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.45703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="9.72265625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="9.3671875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.8984375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.94140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="9.91796875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.265625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="33" max="34" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4072,6 +4107,229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.37890625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.03515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.14453125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="E1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F1" t="s">
+        <v>651</v>
+      </c>
+      <c r="G1" t="s">
+        <v>652</v>
+      </c>
+      <c r="H1" t="s">
+        <v>670</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>670</v>
+      </c>
+      <c r="K1" t="s">
+        <v>670</v>
+      </c>
+      <c r="L1" t="s">
+        <v>670</v>
+      </c>
+      <c r="M1" t="s">
+        <v>670</v>
+      </c>
+      <c r="N1" t="s">
+        <v>670</v>
+      </c>
+      <c r="O1" t="s">
+        <v>670</v>
+      </c>
+      <c r="P1" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>670</v>
+      </c>
+      <c r="R1" t="s">
+        <v>328</v>
+      </c>
+      <c r="S1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T1" t="s">
+        <v>330</v>
+      </c>
+      <c r="U1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V1" t="s">
+        <v>332</v>
+      </c>
+      <c r="W1" t="s">
+        <v>333</v>
+      </c>
+      <c r="X1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B2">
+        <v>1234567</v>
+      </c>
+      <c r="C2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D2" t="s">
+        <v>920</v>
+      </c>
+      <c r="E2" t="s">
+        <v>919</v>
+      </c>
+      <c r="G2" t="s">
+        <v>653</v>
+      </c>
+      <c r="R2" t="s">
+        <v>918</v>
+      </c>
+      <c r="S2" t="s">
+        <v>917</v>
+      </c>
+      <c r="T2" t="s">
+        <v>687</v>
+      </c>
+      <c r="U2" t="s">
+        <v>690</v>
+      </c>
+      <c r="V2" t="s">
+        <v>676</v>
+      </c>
+      <c r="W2" t="s">
+        <v>810</v>
+      </c>
+      <c r="X2" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>780</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>693</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>822</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
minutes after majaor breakthrough
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="942">
   <si>
     <t>Places</t>
   </si>
@@ -2753,30 +2753,6 @@
     <t>460</t>
   </si>
   <si>
-    <t>Laporte 1</t>
-  </si>
-  <si>
-    <t>Maguire 0</t>
-  </si>
-  <si>
-    <t>Canós 4</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Football fc</t>
-  </si>
-  <si>
-    <t>Maisie Rogers</t>
-  </si>
-  <si>
-    <t>3,516,619</t>
-  </si>
-  <si>
-    <t>363</t>
-  </si>
-  <si>
     <t>D11</t>
   </si>
   <si>
@@ -2787,6 +2763,93 @@
   </si>
   <si>
     <t>406</t>
+  </si>
+  <si>
+    <t>Lukaku 4$ captain</t>
+  </si>
+  <si>
+    <t>ddf</t>
+  </si>
+  <si>
+    <t>Salah 26$ captain</t>
+  </si>
+  <si>
+    <t>Ronaldo 2$ captain</t>
+  </si>
+  <si>
+    <t>Antonio 4$ captain</t>
+  </si>
+  <si>
+    <t>Ings 2</t>
+  </si>
+  <si>
+    <t>Jesus 5</t>
+  </si>
+  <si>
+    <t>Gibbs-White 0</t>
+  </si>
+  <si>
+    <t>Pollock 0</t>
+  </si>
+  <si>
+    <t>Kamilkas United</t>
+  </si>
+  <si>
+    <t>Camilla Nurkhanov</t>
+  </si>
+  <si>
+    <t>1,529,578</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>Dallas 3</t>
+  </si>
+  <si>
+    <t>TheChiellinis</t>
+  </si>
+  <si>
+    <t>Leonardo Lombardi</t>
+  </si>
+  <si>
+    <t>1,923,784</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Cash 1</t>
+  </si>
+  <si>
+    <t>Kane 4$ captain</t>
+  </si>
+  <si>
+    <t>Cucho 0</t>
+  </si>
+  <si>
+    <t>James 0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Pink Lemonade</t>
+  </si>
+  <si>
+    <t>Lorin Minxhozi</t>
+  </si>
+  <si>
+    <t>3,717,085</t>
+  </si>
+  <si>
+    <t>Benrahma 4$ captain</t>
+  </si>
+  <si>
+    <t>Jiménez 20$ captain</t>
+  </si>
+  <si>
+    <t>Raphinha 6$ captain</t>
   </si>
 </sst>
 </file>
@@ -3605,35 +3668,37 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK6"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection sqref="A1:AK2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="33" max="34" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.484375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.32421875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.45703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="9.734375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="17.14453125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.9765625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.265625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.83984375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -3787,7 +3852,7 @@
         <v>688</v>
       </c>
       <c r="X2" t="s">
-        <v>699</v>
+        <v>915</v>
       </c>
       <c r="Y2" t="s">
         <v>888</v>
@@ -3873,7 +3938,7 @@
         <v>682</v>
       </c>
       <c r="AC3" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AD3" t="s">
         <v>799</v>
@@ -3941,7 +4006,7 @@
         <v>681</v>
       </c>
       <c r="AB4" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AC4" t="s">
         <v>693</v>
@@ -4012,7 +4077,7 @@
         <v>722</v>
       </c>
       <c r="AB5" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AC5" t="s">
         <v>799</v>
@@ -4089,7 +4154,7 @@
         <v>683</v>
       </c>
       <c r="AD6" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE6" t="s">
         <v>766</v>
@@ -4102,6 +4167,224 @@
       </c>
       <c r="AH6" t="s">
         <v>754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>923</v>
+      </c>
+      <c r="B7">
+        <v>5306515</v>
+      </c>
+      <c r="C7" t="s">
+        <v>775</v>
+      </c>
+      <c r="D7" t="s">
+        <v>925</v>
+      </c>
+      <c r="E7" t="s">
+        <v>924</v>
+      </c>
+      <c r="G7" t="s">
+        <v>672</v>
+      </c>
+      <c r="R7" t="s">
+        <v>923</v>
+      </c>
+      <c r="S7" t="s">
+        <v>922</v>
+      </c>
+      <c r="T7" t="s">
+        <v>378</v>
+      </c>
+      <c r="U7" t="s">
+        <v>688</v>
+      </c>
+      <c r="V7" t="s">
+        <v>676</v>
+      </c>
+      <c r="W7" t="s">
+        <v>729</v>
+      </c>
+      <c r="X7" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>780</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>680</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>917</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>918</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>919</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>887</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>709</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>920</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>928</v>
+      </c>
+      <c r="B8">
+        <v>2249991</v>
+      </c>
+      <c r="C8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" t="s">
+        <v>930</v>
+      </c>
+      <c r="E8" t="s">
+        <v>929</v>
+      </c>
+      <c r="G8" t="s">
+        <v>653</v>
+      </c>
+      <c r="R8" t="s">
+        <v>928</v>
+      </c>
+      <c r="S8" t="s">
+        <v>927</v>
+      </c>
+      <c r="T8" t="s">
+        <v>887</v>
+      </c>
+      <c r="U8" t="s">
+        <v>720</v>
+      </c>
+      <c r="V8" t="s">
+        <v>688</v>
+      </c>
+      <c r="W8" t="s">
+        <v>721</v>
+      </c>
+      <c r="X8" t="s">
+        <v>926</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>759</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>915</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>918</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>793</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>809</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>937</v>
+      </c>
+      <c r="B9">
+        <v>2056865</v>
+      </c>
+      <c r="C9" t="s">
+        <v>935</v>
+      </c>
+      <c r="D9" t="s">
+        <v>718</v>
+      </c>
+      <c r="E9" t="s">
+        <v>938</v>
+      </c>
+      <c r="G9" t="s">
+        <v>672</v>
+      </c>
+      <c r="R9" t="s">
+        <v>937</v>
+      </c>
+      <c r="S9" t="s">
+        <v>936</v>
+      </c>
+      <c r="T9" t="s">
+        <v>838</v>
+      </c>
+      <c r="U9" t="s">
+        <v>786</v>
+      </c>
+      <c r="V9" t="s">
+        <v>688</v>
+      </c>
+      <c r="W9" t="s">
+        <v>931</v>
+      </c>
+      <c r="X9" t="s">
+        <v>692</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>700</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>679</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>703</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>759</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>932</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>730</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>933</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>914</v>
       </c>
     </row>
   </sheetData>
@@ -4114,34 +4397,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.37890625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.03515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.14453125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="31" max="32" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4259,7 +4541,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="B2">
         <v>1234567</v>
@@ -4268,19 +4550,19 @@
         <v>714</v>
       </c>
       <c r="D2" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="E2" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
       </c>
       <c r="R2" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="S2" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="T2" t="s">
         <v>687</v>
@@ -4310,7 +4592,7 @@
         <v>693</v>
       </c>
       <c r="AC2" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AD2" t="s">
         <v>682</v>
@@ -9532,30 +9814,35 @@
   <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:AK1"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="26" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.01953125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.2109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.08984375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.1484375" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.34375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -9673,7 +9960,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>269</v>
+        <v>548</v>
       </c>
       <c r="B2" s="8">
         <v>2438499</v>
@@ -9718,7 +10005,7 @@
         <v>698</v>
       </c>
       <c r="Z2" t="s">
-        <v>699</v>
+        <v>915</v>
       </c>
       <c r="AA2" t="s">
         <v>700</v>
@@ -9747,7 +10034,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B3" s="8">
         <v>1293900</v>
@@ -9804,7 +10091,7 @@
         <v>683</v>
       </c>
       <c r="AD3" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE3" t="s">
         <v>711</v>
@@ -9821,7 +10108,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B4" s="8">
         <v>4115919</v>
@@ -9878,7 +10165,7 @@
         <v>683</v>
       </c>
       <c r="AD4" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE4" t="s">
         <v>694</v>
@@ -9895,7 +10182,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>733</v>
+        <v>583</v>
       </c>
       <c r="B5" s="8">
         <v>2324952</v>
@@ -9934,7 +10221,7 @@
         <v>729</v>
       </c>
       <c r="X5" t="s">
-        <v>699</v>
+        <v>915</v>
       </c>
       <c r="Y5" t="s">
         <v>692</v>
@@ -9969,7 +10256,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>746</v>
+        <v>495</v>
       </c>
       <c r="B6" s="8">
         <v>2522621</v>
@@ -10023,7 +10310,7 @@
         <v>742</v>
       </c>
       <c r="AC6" t="s">
-        <v>743</v>
+        <v>917</v>
       </c>
       <c r="AD6" t="s">
         <v>683</v>
@@ -10043,7 +10330,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B7" s="8">
         <v>488734</v>
@@ -10094,7 +10381,7 @@
         <v>678</v>
       </c>
       <c r="AB7" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AC7" t="s">
         <v>683</v>
@@ -10117,7 +10404,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>762</v>
+        <v>573</v>
       </c>
       <c r="B8" s="8">
         <v>1069199</v>
@@ -10174,7 +10461,7 @@
         <v>682</v>
       </c>
       <c r="AD8" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE8" t="s">
         <v>399</v>
@@ -10191,7 +10478,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>767</v>
+        <v>566</v>
       </c>
       <c r="B9" s="8">
         <v>1327409</v>
@@ -10245,7 +10532,7 @@
         <v>683</v>
       </c>
       <c r="AC9" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AD9" t="s">
         <v>752</v>
@@ -10265,7 +10552,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>772</v>
       </c>
       <c r="B10" s="8">
         <v>2203632</v>
@@ -10316,7 +10603,7 @@
         <v>679</v>
       </c>
       <c r="AB10" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AC10" t="s">
         <v>683</v>
@@ -10339,7 +10626,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B11" s="8">
         <v>3998490</v>
@@ -10396,7 +10683,7 @@
         <v>682</v>
       </c>
       <c r="AD11" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE11" t="s">
         <v>766</v>
@@ -10413,7 +10700,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>289</v>
+        <v>418</v>
       </c>
       <c r="B12" s="8">
         <v>440807</v>
@@ -10464,7 +10751,7 @@
         <v>681</v>
       </c>
       <c r="AB12" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AC12" t="s">
         <v>693</v>
@@ -10487,7 +10774,7 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>291</v>
+        <v>512</v>
       </c>
       <c r="B13" s="8">
         <v>2184142</v>
@@ -10541,7 +10828,7 @@
         <v>722</v>
       </c>
       <c r="AC13" t="s">
-        <v>743</v>
+        <v>917</v>
       </c>
       <c r="AD13" t="s">
         <v>683</v>
@@ -10561,7 +10848,7 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>800</v>
+        <v>459</v>
       </c>
       <c r="B14" s="8">
         <v>2795791</v>
@@ -10615,7 +10902,7 @@
         <v>798</v>
       </c>
       <c r="AC14" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AD14" t="s">
         <v>799</v>
@@ -10635,7 +10922,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B15" s="8">
         <v>228724</v>
@@ -10692,7 +10979,7 @@
         <v>682</v>
       </c>
       <c r="AD15" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE15" t="s">
         <v>694</v>
@@ -10709,7 +10996,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>296</v>
+        <v>406</v>
       </c>
       <c r="B16" s="8">
         <v>2185186</v>
@@ -10760,7 +11047,7 @@
         <v>759</v>
       </c>
       <c r="AB16" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AC16" t="s">
         <v>799</v>
@@ -10783,7 +11070,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="B17" s="8">
         <v>2317783</v>
@@ -10840,7 +11127,7 @@
         <v>702</v>
       </c>
       <c r="AD17" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE17" t="s">
         <v>694</v>
@@ -10857,7 +11144,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>818</v>
+        <v>527</v>
       </c>
       <c r="B18" s="8">
         <v>364277</v>
@@ -10899,7 +11186,7 @@
         <v>680</v>
       </c>
       <c r="Y18" t="s">
-        <v>816</v>
+        <v>939</v>
       </c>
       <c r="Z18" t="s">
         <v>692</v>
@@ -10931,7 +11218,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>823</v>
+        <v>373</v>
       </c>
       <c r="B19" s="8">
         <v>1396639</v>
@@ -10985,7 +11272,7 @@
         <v>799</v>
       </c>
       <c r="AC19" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AD19" t="s">
         <v>682</v>
@@ -11005,7 +11292,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>827</v>
+        <v>542</v>
       </c>
       <c r="B20" s="8">
         <v>1339989</v>
@@ -11062,7 +11349,7 @@
         <v>682</v>
       </c>
       <c r="AD20" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE20" t="s">
         <v>674</v>
@@ -11079,7 +11366,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>304</v>
+        <v>401</v>
       </c>
       <c r="B21" s="8">
         <v>474028</v>
@@ -11133,7 +11420,7 @@
         <v>680</v>
       </c>
       <c r="AC21" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AD21" t="s">
         <v>682</v>
@@ -11153,7 +11440,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>835</v>
+        <v>599</v>
       </c>
       <c r="B22" s="8">
         <v>1229286</v>
@@ -11207,7 +11494,7 @@
         <v>759</v>
       </c>
       <c r="AC22" t="s">
-        <v>743</v>
+        <v>917</v>
       </c>
       <c r="AD22" t="s">
         <v>683</v>
@@ -11227,7 +11514,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>307</v>
+        <v>840</v>
       </c>
       <c r="B23" s="8">
         <v>2340261</v>
@@ -11281,7 +11568,7 @@
         <v>742</v>
       </c>
       <c r="AC23" t="s">
-        <v>743</v>
+        <v>917</v>
       </c>
       <c r="AD23" t="s">
         <v>683</v>
@@ -11301,7 +11588,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>588</v>
       </c>
       <c r="B24" s="8">
         <v>1708392</v>
@@ -11358,7 +11645,7 @@
         <v>683</v>
       </c>
       <c r="AD24" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE24" t="s">
         <v>694</v>
@@ -11375,7 +11662,7 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>487</v>
+        <v>851</v>
       </c>
       <c r="B25" s="8">
         <v>2719892</v>
@@ -11432,7 +11719,7 @@
         <v>683</v>
       </c>
       <c r="AD25" t="s">
-        <v>849</v>
+        <v>940</v>
       </c>
       <c r="AE25" t="s">
         <v>694</v>
@@ -11449,7 +11736,7 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>855</v>
+        <v>595</v>
       </c>
       <c r="B26" s="8">
         <v>122847</v>
@@ -11500,7 +11787,7 @@
         <v>740</v>
       </c>
       <c r="AB26" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AC26" t="s">
         <v>682</v>
@@ -11523,7 +11810,7 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B27" s="8">
         <v>362369</v>
@@ -11580,7 +11867,7 @@
         <v>682</v>
       </c>
       <c r="AD27" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE27" t="s">
         <v>694</v>
@@ -11597,7 +11884,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B28" s="8">
         <v>290784</v>
@@ -11651,7 +11938,7 @@
         <v>752</v>
       </c>
       <c r="AC28" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AD28" t="s">
         <v>682</v>
@@ -11671,7 +11958,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B29" s="8">
         <v>57</v>
@@ -11728,7 +12015,7 @@
         <v>682</v>
       </c>
       <c r="AD29" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE29" t="s">
         <v>694</v>
@@ -11745,7 +12032,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>315</v>
+        <v>872</v>
       </c>
       <c r="B30" s="8">
         <v>23487</v>
@@ -11802,7 +12089,7 @@
         <v>683</v>
       </c>
       <c r="AD30" t="s">
-        <v>684</v>
+        <v>913</v>
       </c>
       <c r="AE30" t="s">
         <v>694</v>
@@ -11819,7 +12106,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B31" s="8">
         <v>360554</v>
@@ -11858,7 +12145,7 @@
         <v>854</v>
       </c>
       <c r="X31" t="s">
-        <v>875</v>
+        <v>941</v>
       </c>
       <c r="Y31" t="s">
         <v>678</v>
@@ -11893,7 +12180,7 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>882</v>
+        <v>520</v>
       </c>
       <c r="B32" s="8">
         <v>2090014</v>
@@ -11950,7 +12237,7 @@
         <v>682</v>
       </c>
       <c r="AD32" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AE32" t="s">
         <v>694</v>
@@ -11967,7 +12254,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>267</v>
+        <v>444</v>
       </c>
       <c r="B33" s="8">
         <v>158870</v>
@@ -12021,7 +12308,7 @@
         <v>822</v>
       </c>
       <c r="AC33" t="s">
-        <v>760</v>
+        <v>916</v>
       </c>
       <c r="AD33" t="s">
         <v>682</v>

</xml_diff>

<commit_message>
40 percent faster by commenting unwanted lines
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="937">
   <si>
     <t>Places</t>
   </si>
@@ -2841,6 +2841,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3321,19 +3322,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
+    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -3667,28 +3668,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4452,24 +4453,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="34" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.55859375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.83984375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.14453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.171875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4743,9 +4748,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5137,10 +5142,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5526,10 +5531,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -6884,10 +6889,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7155,12 +7160,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -9936,27 +9941,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="34" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -12455,10 +12460,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RoC folder added to GW/RoC
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="sept" sheetId="9" r:id="rId9"/>
     <sheet name="RoC" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet5" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2907" uniqueCount="994">
   <si>
     <t>Places</t>
   </si>
@@ -2835,6 +2836,177 @@
   </si>
   <si>
     <t>420</t>
+  </si>
+  <si>
+    <t>Skipp 1</t>
+  </si>
+  <si>
+    <t>Zaha 2</t>
+  </si>
+  <si>
+    <t>Maguire 0</t>
+  </si>
+  <si>
+    <t>Broja 0</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>xcure 500</t>
+  </si>
+  <si>
+    <t>Florian Toslluku</t>
+  </si>
+  <si>
+    <t>5,092,640</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>MrTrias500</t>
+  </si>
+  <si>
+    <t>Eni Shtini</t>
+  </si>
+  <si>
+    <t>329,299</t>
+  </si>
+  <si>
+    <t>de Gea 2</t>
+  </si>
+  <si>
+    <t>Keane 2</t>
+  </si>
+  <si>
+    <t>McGovern 0</t>
+  </si>
+  <si>
+    <t>Bermondsey FC</t>
+  </si>
+  <si>
+    <t>Rui Mendes</t>
+  </si>
+  <si>
+    <t>2,551,641</t>
+  </si>
+  <si>
+    <t>385</t>
+  </si>
+  <si>
+    <t>Lingard 0</t>
+  </si>
+  <si>
+    <t>Winks 0</t>
+  </si>
+  <si>
+    <t>Street 0</t>
+  </si>
+  <si>
+    <t>Sound of the Lloris</t>
+  </si>
+  <si>
+    <t>Glenn Drawbridge</t>
+  </si>
+  <si>
+    <t>2,916,968</t>
+  </si>
+  <si>
+    <t>Gunn 0</t>
+  </si>
+  <si>
+    <t>Romeu 1</t>
+  </si>
+  <si>
+    <t>N.Williams 0</t>
+  </si>
+  <si>
+    <t>Dinamo</t>
+  </si>
+  <si>
+    <t>Erald Haxhiu</t>
+  </si>
+  <si>
+    <t>3,184,240</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>Kilman 2</t>
+  </si>
+  <si>
+    <t>Mount 1</t>
+  </si>
+  <si>
+    <t>Vardy 16$ captain</t>
+  </si>
+  <si>
+    <t>Aarons 5</t>
+  </si>
+  <si>
+    <t>MDEX</t>
+  </si>
+  <si>
+    <t>magi muco</t>
+  </si>
+  <si>
+    <t>4,187,276</t>
+  </si>
+  <si>
+    <t>347</t>
+  </si>
+  <si>
+    <t>Pogba 1</t>
+  </si>
+  <si>
+    <t>Mahrez 0</t>
+  </si>
+  <si>
+    <t>Rodrigo 2</t>
+  </si>
+  <si>
+    <t>Kenny 0</t>
+  </si>
+  <si>
+    <t>Xhaka 0</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Boris the greatest</t>
+  </si>
+  <si>
+    <t>Bardhyl Minxhozi</t>
+  </si>
+  <si>
+    <t>5,855,514</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>Bednarek 1</t>
+  </si>
+  <si>
+    <t>Gabriel 6</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Bella Ciao</t>
+  </si>
+  <si>
+    <t>Geri Muho</t>
+  </si>
+  <si>
+    <t>7,846,916</t>
+  </si>
+  <si>
+    <t>156</t>
   </si>
 </sst>
 </file>
@@ -3668,28 +3840,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.01953125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -3875,6 +4049,9 @@
       <c r="AH2" t="s">
         <v>885</v>
       </c>
+      <c r="AI2" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3893,7 +4070,7 @@
         <v>893</v>
       </c>
       <c r="G3" t="s">
-        <v>672</v>
+        <v>452</v>
       </c>
       <c r="R3" t="s">
         <v>892</v>
@@ -3945,6 +4122,9 @@
       </c>
       <c r="AH3" t="s">
         <v>676</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -4017,6 +4197,9 @@
       <c r="AH4" t="s">
         <v>761</v>
       </c>
+      <c r="AI4" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4088,6 +4271,9 @@
       <c r="AH5" t="s">
         <v>676</v>
       </c>
+      <c r="AI5" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4159,6 +4345,9 @@
       <c r="AH6" t="s">
         <v>751</v>
       </c>
+      <c r="AI6" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4230,6 +4419,9 @@
       <c r="AH7" t="s">
         <v>910</v>
       </c>
+      <c r="AI7" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -4301,6 +4493,9 @@
       <c r="AH8" t="s">
         <v>412</v>
       </c>
+      <c r="AI8" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4372,69 +4567,600 @@
       <c r="AH9" t="s">
         <v>923</v>
       </c>
+      <c r="AI9" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>903</v>
+        <v>943</v>
       </c>
       <c r="B10" s="29">
         <v>5142355</v>
       </c>
+      <c r="C10" t="s">
+        <v>941</v>
+      </c>
+      <c r="D10" t="s">
+        <v>945</v>
+      </c>
+      <c r="E10" t="s">
+        <v>944</v>
+      </c>
+      <c r="G10" t="s">
+        <v>706</v>
+      </c>
+      <c r="R10" t="s">
+        <v>943</v>
+      </c>
+      <c r="S10" t="s">
+        <v>942</v>
+      </c>
+      <c r="T10" t="s">
+        <v>781</v>
+      </c>
+      <c r="U10" t="s">
+        <v>873</v>
+      </c>
+      <c r="V10" t="s">
+        <v>719</v>
+      </c>
+      <c r="W10" t="s">
+        <v>791</v>
+      </c>
+      <c r="X10" t="s">
+        <v>937</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>805</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>938</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>747</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>728</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>939</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>940</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>806</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>903</v>
+        <v>947</v>
       </c>
       <c r="B11" s="29">
         <v>1628438</v>
       </c>
+      <c r="C11" t="s">
+        <v>771</v>
+      </c>
+      <c r="D11" t="s">
+        <v>827</v>
+      </c>
+      <c r="E11" t="s">
+        <v>948</v>
+      </c>
+      <c r="G11" t="s">
+        <v>706</v>
+      </c>
+      <c r="R11" t="s">
+        <v>947</v>
+      </c>
+      <c r="S11" t="s">
+        <v>946</v>
+      </c>
+      <c r="T11" t="s">
+        <v>674</v>
+      </c>
+      <c r="U11" t="s">
+        <v>688</v>
+      </c>
+      <c r="V11" t="s">
+        <v>675</v>
+      </c>
+      <c r="W11" t="s">
+        <v>791</v>
+      </c>
+      <c r="X11" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>739</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>749</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>905</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>804</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>756</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>676</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>903</v>
+        <v>953</v>
       </c>
       <c r="B12" s="29">
         <v>1427447</v>
       </c>
+      <c r="C12" t="s">
+        <v>874</v>
+      </c>
+      <c r="D12" t="s">
+        <v>955</v>
+      </c>
+      <c r="E12" t="s">
+        <v>954</v>
+      </c>
+      <c r="G12" t="s">
+        <v>706</v>
+      </c>
+      <c r="R12" t="s">
+        <v>953</v>
+      </c>
+      <c r="S12" t="s">
+        <v>952</v>
+      </c>
+      <c r="T12" t="s">
+        <v>949</v>
+      </c>
+      <c r="U12" t="s">
+        <v>677</v>
+      </c>
+      <c r="V12" t="s">
+        <v>950</v>
+      </c>
+      <c r="W12" t="s">
+        <v>688</v>
+      </c>
+      <c r="X12" t="s">
+        <v>687</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>915</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>697</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>776</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>720</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>908</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>951</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>684</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>922</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>721</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>903</v>
+        <v>960</v>
       </c>
       <c r="B13" s="29">
         <v>5648774</v>
       </c>
+      <c r="C13" t="s">
+        <v>941</v>
+      </c>
+      <c r="D13" t="s">
+        <v>705</v>
+      </c>
+      <c r="E13" t="s">
+        <v>961</v>
+      </c>
+      <c r="G13" t="s">
+        <v>653</v>
+      </c>
+      <c r="R13" t="s">
+        <v>960</v>
+      </c>
+      <c r="S13" t="s">
+        <v>959</v>
+      </c>
+      <c r="T13" t="s">
+        <v>741</v>
+      </c>
+      <c r="U13" t="s">
+        <v>675</v>
+      </c>
+      <c r="V13" t="s">
+        <v>718</v>
+      </c>
+      <c r="W13" t="s">
+        <v>755</v>
+      </c>
+      <c r="X13" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>956</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>776</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>728</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>806</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>957</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>958</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>903</v>
+        <v>966</v>
       </c>
       <c r="B14" s="29">
         <v>3452385</v>
       </c>
+      <c r="C14" t="s">
+        <v>771</v>
+      </c>
+      <c r="D14" t="s">
+        <v>968</v>
+      </c>
+      <c r="E14" t="s">
+        <v>967</v>
+      </c>
+      <c r="G14" t="s">
+        <v>653</v>
+      </c>
+      <c r="R14" t="s">
+        <v>966</v>
+      </c>
+      <c r="S14" t="s">
+        <v>965</v>
+      </c>
+      <c r="T14" t="s">
+        <v>717</v>
+      </c>
+      <c r="U14" t="s">
+        <v>923</v>
+      </c>
+      <c r="V14" t="s">
+        <v>736</v>
+      </c>
+      <c r="W14" t="s">
+        <v>395</v>
+      </c>
+      <c r="X14" t="s">
+        <v>738</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>904</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>691</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>728</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>962</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>963</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>964</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>903</v>
+        <v>974</v>
       </c>
       <c r="B15" s="29">
         <v>2297330</v>
       </c>
+      <c r="C15" t="s">
+        <v>290</v>
+      </c>
+      <c r="D15" t="s">
+        <v>976</v>
+      </c>
+      <c r="E15" t="s">
+        <v>975</v>
+      </c>
+      <c r="G15" t="s">
+        <v>706</v>
+      </c>
+      <c r="R15" t="s">
+        <v>974</v>
+      </c>
+      <c r="S15" t="s">
+        <v>973</v>
+      </c>
+      <c r="T15" t="s">
+        <v>717</v>
+      </c>
+      <c r="U15" t="s">
+        <v>718</v>
+      </c>
+      <c r="V15" t="s">
+        <v>677</v>
+      </c>
+      <c r="W15" t="s">
+        <v>969</v>
+      </c>
+      <c r="X15" t="s">
+        <v>938</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>882</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>970</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>690</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>971</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>795</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>794</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>884</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>805</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>972</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>400</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>903</v>
+        <v>984</v>
       </c>
       <c r="B16" s="29">
         <v>5361878</v>
       </c>
+      <c r="C16" t="s">
+        <v>982</v>
+      </c>
+      <c r="D16" t="s">
+        <v>986</v>
+      </c>
+      <c r="E16" t="s">
+        <v>985</v>
+      </c>
+      <c r="G16" t="s">
+        <v>653</v>
+      </c>
+      <c r="R16" t="s">
+        <v>984</v>
+      </c>
+      <c r="S16" t="s">
+        <v>983</v>
+      </c>
+      <c r="T16" t="s">
+        <v>781</v>
+      </c>
+      <c r="U16" t="s">
+        <v>923</v>
+      </c>
+      <c r="V16" t="s">
+        <v>718</v>
+      </c>
+      <c r="W16" t="s">
+        <v>939</v>
+      </c>
+      <c r="X16" t="s">
+        <v>915</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>776</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>977</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>978</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>908</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>979</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>717</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>980</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>981</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>903</v>
+        <v>991</v>
       </c>
       <c r="B17" s="29">
         <v>5344757</v>
+      </c>
+      <c r="C17" t="s">
+        <v>989</v>
+      </c>
+      <c r="D17" t="s">
+        <v>993</v>
+      </c>
+      <c r="E17" t="s">
+        <v>992</v>
+      </c>
+      <c r="G17" t="s">
+        <v>653</v>
+      </c>
+      <c r="R17" t="s">
+        <v>991</v>
+      </c>
+      <c r="S17" t="s">
+        <v>990</v>
+      </c>
+      <c r="T17" t="s">
+        <v>949</v>
+      </c>
+      <c r="U17" t="s">
+        <v>412</v>
+      </c>
+      <c r="V17" t="s">
+        <v>920</v>
+      </c>
+      <c r="W17" t="s">
+        <v>734</v>
+      </c>
+      <c r="X17" t="s">
+        <v>739</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>970</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>776</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>691</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>698</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>987</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>988</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>749</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>989</v>
       </c>
     </row>
   </sheetData>
@@ -4447,34 +5173,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="9.55859375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="8.83984375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="17.14453125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.171875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="23" max="25" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4730,6 +5454,33 @@
       </c>
       <c r="AH3" t="s">
         <v>817</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
writing the league fetcher
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2907" uniqueCount="994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2657" uniqueCount="993">
   <si>
     <t>Places</t>
   </si>
@@ -2734,9 +2734,6 @@
   </si>
   <si>
     <t>Lukaku 4$ captain</t>
-  </si>
-  <si>
-    <t>ddf</t>
   </si>
   <si>
     <t>Salah 26$ captain</t>
@@ -3013,7 +3010,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3494,19 +3490,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
-    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
-    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
-    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -3840,30 +3836,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="14.01953125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.08203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -4017,7 +4009,7 @@
         <v>687</v>
       </c>
       <c r="X2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Y2" t="s">
         <v>881</v>
@@ -4106,7 +4098,7 @@
         <v>682</v>
       </c>
       <c r="AC3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD3" t="s">
         <v>795</v>
@@ -4251,7 +4243,7 @@
         <v>720</v>
       </c>
       <c r="AB5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AC5" t="s">
         <v>795</v>
@@ -4351,7 +4343,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B7">
         <v>5306515</v>
@@ -4360,19 +4352,19 @@
         <v>771</v>
       </c>
       <c r="D7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G7" t="s">
         <v>672</v>
       </c>
       <c r="R7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="S7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="T7" t="s">
         <v>378</v>
@@ -4399,13 +4391,13 @@
         <v>680</v>
       </c>
       <c r="AB7" t="s">
+        <v>905</v>
+      </c>
+      <c r="AC7" t="s">
         <v>906</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>907</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>908</v>
       </c>
       <c r="AE7" t="s">
         <v>880</v>
@@ -4414,10 +4406,10 @@
         <v>707</v>
       </c>
       <c r="AG7" t="s">
+        <v>908</v>
+      </c>
+      <c r="AH7" t="s">
         <v>909</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>910</v>
       </c>
       <c r="AI7" t="s">
         <v>771</v>
@@ -4425,7 +4417,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B8">
         <v>2249991</v>
@@ -4434,19 +4426,19 @@
         <v>268</v>
       </c>
       <c r="D8" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E8" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G8" t="s">
         <v>653</v>
       </c>
       <c r="R8" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="S8" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="T8" t="s">
         <v>880</v>
@@ -4461,7 +4453,7 @@
         <v>719</v>
       </c>
       <c r="X8" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Y8" t="s">
         <v>756</v>
@@ -4470,7 +4462,7 @@
         <v>691</v>
       </c>
       <c r="AA8" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="AB8" t="s">
         <v>682</v>
@@ -4479,7 +4471,7 @@
         <v>683</v>
       </c>
       <c r="AD8" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="AE8" t="s">
         <v>674</v>
@@ -4499,28 +4491,28 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B9">
         <v>2056865</v>
       </c>
       <c r="C9" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D9" t="s">
         <v>716</v>
       </c>
       <c r="E9" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G9" t="s">
         <v>672</v>
       </c>
       <c r="R9" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="S9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T9" t="s">
         <v>833</v>
@@ -4532,7 +4524,7 @@
         <v>687</v>
       </c>
       <c r="W9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="X9" t="s">
         <v>691</v>
@@ -4550,7 +4542,7 @@
         <v>756</v>
       </c>
       <c r="AC9" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="AD9" t="s">
         <v>728</v>
@@ -4559,42 +4551,42 @@
         <v>693</v>
       </c>
       <c r="AF9" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AG9" t="s">
         <v>684</v>
       </c>
       <c r="AH9" t="s">
+        <v>922</v>
+      </c>
+      <c r="AI9" t="s">
         <v>923</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B10" s="29">
         <v>5142355</v>
       </c>
       <c r="C10" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D10" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="E10" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G10" t="s">
         <v>706</v>
       </c>
       <c r="R10" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="S10" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="T10" t="s">
         <v>781</v>
@@ -4609,13 +4601,13 @@
         <v>791</v>
       </c>
       <c r="X10" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="Y10" t="s">
         <v>805</v>
       </c>
       <c r="Z10" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AA10" t="s">
         <v>678</v>
@@ -4624,7 +4616,7 @@
         <v>747</v>
       </c>
       <c r="AC10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD10" t="s">
         <v>728</v>
@@ -4633,21 +4625,21 @@
         <v>709</v>
       </c>
       <c r="AF10" t="s">
+        <v>938</v>
+      </c>
+      <c r="AG10" t="s">
         <v>939</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>940</v>
       </c>
       <c r="AH10" t="s">
         <v>806</v>
       </c>
       <c r="AI10" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B11" s="29">
         <v>1628438</v>
@@ -4659,16 +4651,16 @@
         <v>827</v>
       </c>
       <c r="E11" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="G11" t="s">
         <v>706</v>
       </c>
       <c r="R11" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="S11" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="T11" t="s">
         <v>674</v>
@@ -4701,7 +4693,7 @@
         <v>682</v>
       </c>
       <c r="AD11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE11" t="s">
         <v>804</v>
@@ -4721,7 +4713,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B12" s="29">
         <v>1427447</v>
@@ -4730,28 +4722,28 @@
         <v>874</v>
       </c>
       <c r="D12" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E12" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G12" t="s">
         <v>706</v>
       </c>
       <c r="R12" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="S12" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="T12" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="U12" t="s">
         <v>677</v>
       </c>
       <c r="V12" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="W12" t="s">
         <v>688</v>
@@ -4760,7 +4752,7 @@
         <v>687</v>
       </c>
       <c r="Y12" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Z12" t="s">
         <v>697</v>
@@ -4772,19 +4764,19 @@
         <v>720</v>
       </c>
       <c r="AC12" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD12" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AE12" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="AF12" t="s">
         <v>684</v>
       </c>
       <c r="AG12" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AH12" t="s">
         <v>721</v>
@@ -4795,28 +4787,28 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B13" s="29">
         <v>5648774</v>
       </c>
       <c r="C13" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D13" t="s">
         <v>705</v>
       </c>
       <c r="E13" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G13" t="s">
         <v>653</v>
       </c>
       <c r="R13" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="S13" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="T13" t="s">
         <v>741</v>
@@ -4837,7 +4829,7 @@
         <v>678</v>
       </c>
       <c r="Z13" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AA13" t="s">
         <v>738</v>
@@ -4846,7 +4838,7 @@
         <v>776</v>
       </c>
       <c r="AC13" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD13" t="s">
         <v>728</v>
@@ -4858,18 +4850,18 @@
         <v>806</v>
       </c>
       <c r="AG13" t="s">
+        <v>956</v>
+      </c>
+      <c r="AH13" t="s">
         <v>957</v>
       </c>
-      <c r="AH13" t="s">
-        <v>958</v>
-      </c>
       <c r="AI13" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B14" s="29">
         <v>3452385</v>
@@ -4878,25 +4870,25 @@
         <v>771</v>
       </c>
       <c r="D14" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E14" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
       </c>
       <c r="R14" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="S14" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="T14" t="s">
         <v>717</v>
       </c>
       <c r="U14" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="V14" t="s">
         <v>736</v>
@@ -4908,7 +4900,7 @@
         <v>738</v>
       </c>
       <c r="Y14" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Z14" t="s">
         <v>681</v>
@@ -4926,16 +4918,16 @@
         <v>728</v>
       </c>
       <c r="AE14" t="s">
+        <v>961</v>
+      </c>
+      <c r="AF14" t="s">
         <v>962</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>963</v>
       </c>
       <c r="AG14" t="s">
         <v>685</v>
       </c>
       <c r="AH14" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="AI14" t="s">
         <v>771</v>
@@ -4943,7 +4935,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B15" s="29">
         <v>2297330</v>
@@ -4952,19 +4944,19 @@
         <v>290</v>
       </c>
       <c r="D15" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E15" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G15" t="s">
         <v>706</v>
       </c>
       <c r="R15" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="S15" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="T15" t="s">
         <v>717</v>
@@ -4976,22 +4968,22 @@
         <v>677</v>
       </c>
       <c r="W15" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="X15" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="Y15" t="s">
         <v>882</v>
       </c>
       <c r="Z15" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AA15" t="s">
         <v>690</v>
       </c>
       <c r="AB15" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="AC15" t="s">
         <v>795</v>
@@ -5006,7 +4998,7 @@
         <v>805</v>
       </c>
       <c r="AG15" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="AH15" t="s">
         <v>400</v>
@@ -5017,58 +5009,58 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B16" s="29">
         <v>5361878</v>
       </c>
       <c r="C16" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D16" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E16" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G16" t="s">
         <v>653</v>
       </c>
       <c r="R16" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="S16" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="T16" t="s">
         <v>781</v>
       </c>
       <c r="U16" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="V16" t="s">
         <v>718</v>
       </c>
       <c r="W16" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="X16" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Y16" t="s">
         <v>776</v>
       </c>
       <c r="Z16" t="s">
+        <v>976</v>
+      </c>
+      <c r="AA16" t="s">
         <v>977</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
+        <v>907</v>
+      </c>
+      <c r="AC16" t="s">
         <v>978</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>908</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>979</v>
       </c>
       <c r="AD16" t="s">
         <v>902</v>
@@ -5080,48 +5072,48 @@
         <v>707</v>
       </c>
       <c r="AG16" t="s">
+        <v>979</v>
+      </c>
+      <c r="AH16" t="s">
         <v>980</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AI16" t="s">
         <v>981</v>
       </c>
-      <c r="AI16" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B17" s="29">
         <v>5344757</v>
       </c>
       <c r="C17" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D17" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
       </c>
       <c r="R17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="S17" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="T17" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="U17" t="s">
         <v>412</v>
       </c>
       <c r="V17" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="W17" t="s">
         <v>734</v>
@@ -5130,7 +5122,7 @@
         <v>739</v>
       </c>
       <c r="Y17" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="Z17" t="s">
         <v>776</v>
@@ -5151,16 +5143,16 @@
         <v>693</v>
       </c>
       <c r="AF17" t="s">
+        <v>986</v>
+      </c>
+      <c r="AG17" t="s">
         <v>987</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>988</v>
       </c>
       <c r="AH17" t="s">
         <v>749</v>
       </c>
       <c r="AI17" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -5179,26 +5171,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="23" max="25" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5331,7 +5323,7 @@
         <v>859</v>
       </c>
       <c r="G2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="R2" t="s">
         <v>858</v>
@@ -5387,28 +5379,28 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B3">
         <v>12467</v>
       </c>
       <c r="C3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
       </c>
       <c r="R3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="S3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="T3" t="s">
         <v>693</v>
@@ -5441,7 +5433,7 @@
         <v>728</v>
       </c>
       <c r="AD3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE3" t="s">
         <v>674</v>
@@ -5466,13 +5458,13 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5499,9 +5491,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5893,10 +5885,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6282,10 +6274,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -7640,10 +7632,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7911,12 +7903,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10692,27 +10684,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="34" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10875,7 +10867,7 @@
         <v>697</v>
       </c>
       <c r="Z2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="AA2" t="s">
         <v>698</v>
@@ -11091,7 +11083,7 @@
         <v>727</v>
       </c>
       <c r="X5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Y5" t="s">
         <v>691</v>
@@ -11180,7 +11172,7 @@
         <v>740</v>
       </c>
       <c r="AC6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AD6" t="s">
         <v>683</v>
@@ -11331,7 +11323,7 @@
         <v>682</v>
       </c>
       <c r="AD8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE8" t="s">
         <v>399</v>
@@ -11553,7 +11545,7 @@
         <v>682</v>
       </c>
       <c r="AD11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE11" t="s">
         <v>762</v>
@@ -11698,7 +11690,7 @@
         <v>720</v>
       </c>
       <c r="AC13" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AD13" t="s">
         <v>683</v>
@@ -11849,7 +11841,7 @@
         <v>682</v>
       </c>
       <c r="AD15" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE15" t="s">
         <v>693</v>
@@ -11917,7 +11909,7 @@
         <v>756</v>
       </c>
       <c r="AB16" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AC16" t="s">
         <v>795</v>
@@ -12056,7 +12048,7 @@
         <v>680</v>
       </c>
       <c r="Y18" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Z18" t="s">
         <v>691</v>
@@ -12219,7 +12211,7 @@
         <v>682</v>
       </c>
       <c r="AD20" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE20" t="s">
         <v>674</v>
@@ -12290,7 +12282,7 @@
         <v>680</v>
       </c>
       <c r="AC21" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD21" t="s">
         <v>682</v>
@@ -12364,7 +12356,7 @@
         <v>756</v>
       </c>
       <c r="AC22" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AD22" t="s">
         <v>683</v>
@@ -12438,7 +12430,7 @@
         <v>740</v>
       </c>
       <c r="AC23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AD23" t="s">
         <v>683</v>
@@ -12589,7 +12581,7 @@
         <v>683</v>
       </c>
       <c r="AD25" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AE25" t="s">
         <v>693</v>
@@ -12657,7 +12649,7 @@
         <v>738</v>
       </c>
       <c r="AB26" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AC26" t="s">
         <v>682</v>
@@ -12885,7 +12877,7 @@
         <v>682</v>
       </c>
       <c r="AD29" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE29" t="s">
         <v>693</v>
@@ -13015,7 +13007,7 @@
         <v>848</v>
       </c>
       <c r="X31" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="Y31" t="s">
         <v>678</v>
@@ -13107,7 +13099,7 @@
         <v>682</v>
       </c>
       <c r="AD32" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AE32" t="s">
         <v>693</v>
@@ -13178,7 +13170,7 @@
         <v>817</v>
       </c>
       <c r="AC33" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AD33" t="s">
         <v>682</v>
@@ -13211,10 +13203,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
stupidest mistake expecting something WT writing
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2657" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="1020">
   <si>
     <t>Places</t>
   </si>
@@ -3004,12 +3004,94 @@
   </si>
   <si>
     <t>156</t>
+  </si>
+  <si>
+    <t>Josh's kIngs</t>
+  </si>
+  <si>
+    <t>1000066</t>
+  </si>
+  <si>
+    <t>Game of VAR</t>
+  </si>
+  <si>
+    <t>2023094</t>
+  </si>
+  <si>
+    <t>GSW Champs 21/22</t>
+  </si>
+  <si>
+    <t>352025</t>
+  </si>
+  <si>
+    <t>Phosphenes</t>
+  </si>
+  <si>
+    <t>140849</t>
+  </si>
+  <si>
+    <t>J team</t>
+  </si>
+  <si>
+    <t>2556247</t>
+  </si>
+  <si>
+    <t>JFT97</t>
+  </si>
+  <si>
+    <t>5522451</t>
+  </si>
+  <si>
+    <t>winde</t>
+  </si>
+  <si>
+    <t>2567394</t>
+  </si>
+  <si>
+    <t>ryan_alexandre</t>
+  </si>
+  <si>
+    <t>2071423</t>
+  </si>
+  <si>
+    <t>Kingsman</t>
+  </si>
+  <si>
+    <t>291276</t>
+  </si>
+  <si>
+    <t>Joshua Conceicao</t>
+  </si>
+  <si>
+    <t>shawn yeo</t>
+  </si>
+  <si>
+    <t>Glenn tan</t>
+  </si>
+  <si>
+    <t>Ryan Lee</t>
+  </si>
+  <si>
+    <t>Jethro Ng</t>
+  </si>
+  <si>
+    <t>Jellan Emmanuel</t>
+  </si>
+  <si>
+    <t>Andre De Souza</t>
+  </si>
+  <si>
+    <t>Ryan De Souza</t>
+  </si>
+  <si>
+    <t>JIN WEI LIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3490,19 +3572,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
+    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -3836,26 +3918,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="28" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5171,26 +5253,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.82421875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.55859375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.83984375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.14453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.171875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5376,6 +5462,9 @@
       <c r="AH2" t="s">
         <v>756</v>
       </c>
+      <c r="AI2" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5446,6 +5535,9 @@
       </c>
       <c r="AH3" t="s">
         <v>817</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>931</v>
       </c>
     </row>
   </sheetData>
@@ -5455,16 +5547,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.78515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5473,6 +5565,78 @@
       </c>
       <c r="B1" s="6" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B2" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B3" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1010</v>
       </c>
     </row>
   </sheetData>
@@ -5491,9 +5655,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5885,10 +6049,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6274,10 +6438,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -7632,10 +7796,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7903,12 +8067,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10684,27 +10848,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="34" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -13203,10 +13367,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
wrong gw added gw7
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="11175" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="RoC" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet5" sheetId="12" r:id="rId12"/>
+    <sheet name="FPL6" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="1072">
   <si>
     <t>Places</t>
   </si>
@@ -3067,12 +3068,187 @@
   </si>
   <si>
     <t>523</t>
+  </si>
+  <si>
+    <t>2,215,341</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
+    <t>3,775,793</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>2,518,285</t>
+  </si>
+  <si>
+    <t>774,188</t>
+  </si>
+  <si>
+    <t>489</t>
+  </si>
+  <si>
+    <t>1,772,881</t>
+  </si>
+  <si>
+    <t>457</t>
+  </si>
+  <si>
+    <t>2,249,060</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>959,159</t>
+  </si>
+  <si>
+    <t>482</t>
+  </si>
+  <si>
+    <t>1,666,201</t>
+  </si>
+  <si>
+    <t>1,631,173</t>
+  </si>
+  <si>
+    <t>461</t>
+  </si>
+  <si>
+    <t>1,104,018</t>
+  </si>
+  <si>
+    <t>477</t>
+  </si>
+  <si>
+    <t>1,259,126</t>
+  </si>
+  <si>
+    <t>1,205,384</t>
+  </si>
+  <si>
+    <t>474</t>
+  </si>
+  <si>
+    <t>985,538</t>
+  </si>
+  <si>
+    <t>481</t>
+  </si>
+  <si>
+    <t>412,043</t>
+  </si>
+  <si>
+    <t>506</t>
+  </si>
+  <si>
+    <t>482,481</t>
+  </si>
+  <si>
+    <t>1,294,773</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>561,245</t>
+  </si>
+  <si>
+    <t>498</t>
+  </si>
+  <si>
+    <t>341,378</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>381,471</t>
+  </si>
+  <si>
+    <t>508</t>
+  </si>
+  <si>
+    <t>325,740</t>
+  </si>
+  <si>
+    <t>511</t>
+  </si>
+  <si>
+    <t>463,169</t>
+  </si>
+  <si>
+    <t>503</t>
+  </si>
+  <si>
+    <t>364,608</t>
+  </si>
+  <si>
+    <t>509</t>
+  </si>
+  <si>
+    <t>398,555</t>
+  </si>
+  <si>
+    <t>507</t>
+  </si>
+  <si>
+    <t>2,988,766</t>
+  </si>
+  <si>
+    <t>709,616</t>
+  </si>
+  <si>
+    <t>492</t>
+  </si>
+  <si>
+    <t>142,826</t>
+  </si>
+  <si>
+    <t>526</t>
+  </si>
+  <si>
+    <t>344,983</t>
+  </si>
+  <si>
+    <t>23,328</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>164,749</t>
+  </si>
+  <si>
+    <t>524</t>
+  </si>
+  <si>
+    <t>244,878</t>
+  </si>
+  <si>
+    <t>517</t>
+  </si>
+  <si>
+    <t>155,235</t>
+  </si>
+  <si>
+    <t>525</t>
+  </si>
+  <si>
+    <t>42,901</t>
+  </si>
+  <si>
+    <t>543</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3553,19 +3729,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
+    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -3893,32 +4069,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A17"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="28" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5234,28 +5410,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="23" max="25" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5528,24 +5704,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="30" max="34" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="20" max="28" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="30" max="34" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -5797,6 +5973,2528 @@
       </c>
       <c r="B10" t="s">
         <v>1001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:AK1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.55078125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.01953125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.2109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.08984375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.1484375" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.34375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="E1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F1" t="s">
+        <v>651</v>
+      </c>
+      <c r="G1" t="s">
+        <v>652</v>
+      </c>
+      <c r="H1" t="s">
+        <v>670</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>670</v>
+      </c>
+      <c r="K1" t="s">
+        <v>670</v>
+      </c>
+      <c r="L1" t="s">
+        <v>670</v>
+      </c>
+      <c r="M1" t="s">
+        <v>670</v>
+      </c>
+      <c r="N1" t="s">
+        <v>670</v>
+      </c>
+      <c r="O1" t="s">
+        <v>670</v>
+      </c>
+      <c r="P1" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>670</v>
+      </c>
+      <c r="R1" t="s">
+        <v>328</v>
+      </c>
+      <c r="S1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T1" t="s">
+        <v>330</v>
+      </c>
+      <c r="U1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V1" t="s">
+        <v>332</v>
+      </c>
+      <c r="W1" t="s">
+        <v>333</v>
+      </c>
+      <c r="X1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2438499</v>
+      </c>
+      <c r="C2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G2" t="s">
+        <v>706</v>
+      </c>
+      <c r="R2" t="s">
+        <v>548</v>
+      </c>
+      <c r="S2" t="s">
+        <v>269</v>
+      </c>
+      <c r="T2" t="s">
+        <v>674</v>
+      </c>
+      <c r="U2" t="s">
+        <v>696</v>
+      </c>
+      <c r="V2" t="s">
+        <v>677</v>
+      </c>
+      <c r="W2" t="s">
+        <v>676</v>
+      </c>
+      <c r="X2" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>697</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>698</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>700</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>701</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>702</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1293900</v>
+      </c>
+      <c r="C3" t="s">
+        <v>712</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G3" t="s">
+        <v>672</v>
+      </c>
+      <c r="R3" t="s">
+        <v>714</v>
+      </c>
+      <c r="S3" t="s">
+        <v>713</v>
+      </c>
+      <c r="T3" t="s">
+        <v>674</v>
+      </c>
+      <c r="U3" t="s">
+        <v>676</v>
+      </c>
+      <c r="V3" t="s">
+        <v>696</v>
+      </c>
+      <c r="W3" t="s">
+        <v>707</v>
+      </c>
+      <c r="X3" t="s">
+        <v>679</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>708</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>684</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>710</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>711</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>723</v>
+      </c>
+      <c r="B4" s="8">
+        <v>4115919</v>
+      </c>
+      <c r="C4" t="s">
+        <v>712</v>
+      </c>
+      <c r="D4" t="s">
+        <v>851</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G4" t="s">
+        <v>672</v>
+      </c>
+      <c r="R4" t="s">
+        <v>723</v>
+      </c>
+      <c r="S4" t="s">
+        <v>722</v>
+      </c>
+      <c r="T4" t="s">
+        <v>717</v>
+      </c>
+      <c r="U4" t="s">
+        <v>718</v>
+      </c>
+      <c r="V4" t="s">
+        <v>719</v>
+      </c>
+      <c r="W4" t="s">
+        <v>677</v>
+      </c>
+      <c r="X4" t="s">
+        <v>720</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>721</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>700</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>685</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>583</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2324952</v>
+      </c>
+      <c r="C5" t="s">
+        <v>730</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G5" t="s">
+        <v>653</v>
+      </c>
+      <c r="R5" t="s">
+        <v>583</v>
+      </c>
+      <c r="S5" t="s">
+        <v>731</v>
+      </c>
+      <c r="T5" t="s">
+        <v>726</v>
+      </c>
+      <c r="U5" t="s">
+        <v>677</v>
+      </c>
+      <c r="V5" t="s">
+        <v>689</v>
+      </c>
+      <c r="W5" t="s">
+        <v>727</v>
+      </c>
+      <c r="X5" t="s">
+        <v>903</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>690</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>700</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>728</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>729</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>675</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2522621</v>
+      </c>
+      <c r="C6" t="s">
+        <v>671</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G6" t="s">
+        <v>706</v>
+      </c>
+      <c r="R6" t="s">
+        <v>495</v>
+      </c>
+      <c r="S6" t="s">
+        <v>743</v>
+      </c>
+      <c r="T6" t="s">
+        <v>686</v>
+      </c>
+      <c r="U6" t="s">
+        <v>734</v>
+      </c>
+      <c r="V6" t="s">
+        <v>735</v>
+      </c>
+      <c r="W6" t="s">
+        <v>736</v>
+      </c>
+      <c r="X6" t="s">
+        <v>737</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>739</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>740</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>741</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>689</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>742</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>676</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="8">
+        <v>488734</v>
+      </c>
+      <c r="C7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G7" t="s">
+        <v>706</v>
+      </c>
+      <c r="R7" t="s">
+        <v>432</v>
+      </c>
+      <c r="S7" t="s">
+        <v>435</v>
+      </c>
+      <c r="T7" t="s">
+        <v>726</v>
+      </c>
+      <c r="U7" t="s">
+        <v>395</v>
+      </c>
+      <c r="V7" t="s">
+        <v>746</v>
+      </c>
+      <c r="W7" t="s">
+        <v>675</v>
+      </c>
+      <c r="X7" t="s">
+        <v>747</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>748</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>698</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>902</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>749</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>750</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>573</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1069199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>712</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G8" t="s">
+        <v>706</v>
+      </c>
+      <c r="R8" t="s">
+        <v>573</v>
+      </c>
+      <c r="S8" t="s">
+        <v>758</v>
+      </c>
+      <c r="T8" t="s">
+        <v>674</v>
+      </c>
+      <c r="U8" t="s">
+        <v>754</v>
+      </c>
+      <c r="V8" t="s">
+        <v>755</v>
+      </c>
+      <c r="W8" t="s">
+        <v>688</v>
+      </c>
+      <c r="X8" t="s">
+        <v>738</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>756</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>701</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>678</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>684</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>757</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>566</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1327409</v>
+      </c>
+      <c r="C9" t="s">
+        <v>712</v>
+      </c>
+      <c r="D9" t="s">
+        <v>901</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G9" t="s">
+        <v>653</v>
+      </c>
+      <c r="R9" t="s">
+        <v>566</v>
+      </c>
+      <c r="S9" t="s">
+        <v>763</v>
+      </c>
+      <c r="T9" t="s">
+        <v>674</v>
+      </c>
+      <c r="U9" t="s">
+        <v>761</v>
+      </c>
+      <c r="V9" t="s">
+        <v>687</v>
+      </c>
+      <c r="W9" t="s">
+        <v>696</v>
+      </c>
+      <c r="X9" t="s">
+        <v>701</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>747</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>739</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>683</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>902</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>749</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>762</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>751</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>768</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2203632</v>
+      </c>
+      <c r="C10" t="s">
+        <v>673</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G10" t="s">
+        <v>706</v>
+      </c>
+      <c r="R10" t="s">
+        <v>768</v>
+      </c>
+      <c r="S10" t="s">
+        <v>285</v>
+      </c>
+      <c r="T10" t="s">
+        <v>436</v>
+      </c>
+      <c r="U10" t="s">
+        <v>675</v>
+      </c>
+      <c r="V10" t="s">
+        <v>707</v>
+      </c>
+      <c r="W10" t="s">
+        <v>696</v>
+      </c>
+      <c r="X10" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>902</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>766</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>767</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>400</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>773</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3998490</v>
+      </c>
+      <c r="C11" t="s">
+        <v>771</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G11" t="s">
+        <v>706</v>
+      </c>
+      <c r="R11" t="s">
+        <v>773</v>
+      </c>
+      <c r="S11" t="s">
+        <v>772</v>
+      </c>
+      <c r="T11" t="s">
+        <v>674</v>
+      </c>
+      <c r="U11" t="s">
+        <v>687</v>
+      </c>
+      <c r="V11" t="s">
+        <v>736</v>
+      </c>
+      <c r="W11" t="s">
+        <v>675</v>
+      </c>
+      <c r="X11" t="s">
+        <v>738</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>720</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>679</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>680</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>762</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>755</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>749</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="8">
+        <v>440807</v>
+      </c>
+      <c r="C12" t="s">
+        <v>778</v>
+      </c>
+      <c r="D12" t="s">
+        <v>878</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G12" t="s">
+        <v>653</v>
+      </c>
+      <c r="R12" t="s">
+        <v>418</v>
+      </c>
+      <c r="S12" t="s">
+        <v>289</v>
+      </c>
+      <c r="T12" t="s">
+        <v>686</v>
+      </c>
+      <c r="U12" t="s">
+        <v>688</v>
+      </c>
+      <c r="V12" t="s">
+        <v>677</v>
+      </c>
+      <c r="W12" t="s">
+        <v>687</v>
+      </c>
+      <c r="X12" t="s">
+        <v>776</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>721</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>902</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>777</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>761</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>512</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2184142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>785</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G13" t="s">
+        <v>672</v>
+      </c>
+      <c r="R13" t="s">
+        <v>512</v>
+      </c>
+      <c r="S13" t="s">
+        <v>291</v>
+      </c>
+      <c r="T13" t="s">
+        <v>781</v>
+      </c>
+      <c r="U13" t="s">
+        <v>782</v>
+      </c>
+      <c r="V13" t="s">
+        <v>783</v>
+      </c>
+      <c r="W13" t="s">
+        <v>675</v>
+      </c>
+      <c r="X13" t="s">
+        <v>707</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>720</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>751</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>784</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>459</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2795791</v>
+      </c>
+      <c r="C14" t="s">
+        <v>730</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G14" t="s">
+        <v>706</v>
+      </c>
+      <c r="R14" t="s">
+        <v>459</v>
+      </c>
+      <c r="S14" t="s">
+        <v>796</v>
+      </c>
+      <c r="T14" t="s">
+        <v>788</v>
+      </c>
+      <c r="U14" t="s">
+        <v>789</v>
+      </c>
+      <c r="V14" t="s">
+        <v>790</v>
+      </c>
+      <c r="W14" t="s">
+        <v>791</v>
+      </c>
+      <c r="X14" t="s">
+        <v>792</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>690</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>793</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>794</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>902</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>795</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>751</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>767</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>801</v>
+      </c>
+      <c r="B15" s="8">
+        <v>228724</v>
+      </c>
+      <c r="C15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G15" t="s">
+        <v>706</v>
+      </c>
+      <c r="R15" t="s">
+        <v>801</v>
+      </c>
+      <c r="S15" t="s">
+        <v>800</v>
+      </c>
+      <c r="T15" t="s">
+        <v>674</v>
+      </c>
+      <c r="U15" t="s">
+        <v>677</v>
+      </c>
+      <c r="V15" t="s">
+        <v>718</v>
+      </c>
+      <c r="W15" t="s">
+        <v>675</v>
+      </c>
+      <c r="X15" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>685</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>701</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>406</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2185186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>771</v>
+      </c>
+      <c r="D16" t="s">
+        <v>865</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G16" t="s">
+        <v>653</v>
+      </c>
+      <c r="R16" t="s">
+        <v>406</v>
+      </c>
+      <c r="S16" t="s">
+        <v>296</v>
+      </c>
+      <c r="T16" t="s">
+        <v>674</v>
+      </c>
+      <c r="U16" t="s">
+        <v>718</v>
+      </c>
+      <c r="V16" t="s">
+        <v>685</v>
+      </c>
+      <c r="W16" t="s">
+        <v>694</v>
+      </c>
+      <c r="X16" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>756</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>904</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>795</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>804</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>684</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>805</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>806</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2317783</v>
+      </c>
+      <c r="C17" t="s">
+        <v>712</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G17" t="s">
+        <v>706</v>
+      </c>
+      <c r="R17" t="s">
+        <v>348</v>
+      </c>
+      <c r="S17" t="s">
+        <v>298</v>
+      </c>
+      <c r="T17" t="s">
+        <v>674</v>
+      </c>
+      <c r="U17" t="s">
+        <v>675</v>
+      </c>
+      <c r="V17" t="s">
+        <v>688</v>
+      </c>
+      <c r="W17" t="s">
+        <v>689</v>
+      </c>
+      <c r="X17" t="s">
+        <v>679</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>809</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>683</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>700</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>805</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>400</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>527</v>
+      </c>
+      <c r="B18" s="8">
+        <v>364277</v>
+      </c>
+      <c r="C18" t="s">
+        <v>778</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G18" t="s">
+        <v>672</v>
+      </c>
+      <c r="R18" t="s">
+        <v>527</v>
+      </c>
+      <c r="S18" t="s">
+        <v>813</v>
+      </c>
+      <c r="T18" t="s">
+        <v>717</v>
+      </c>
+      <c r="U18" t="s">
+        <v>677</v>
+      </c>
+      <c r="V18" t="s">
+        <v>675</v>
+      </c>
+      <c r="W18" t="s">
+        <v>689</v>
+      </c>
+      <c r="X18" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>927</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>678</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>728</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>794</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>812</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1396639</v>
+      </c>
+      <c r="C19" t="s">
+        <v>294</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G19" t="s">
+        <v>653</v>
+      </c>
+      <c r="R19" t="s">
+        <v>373</v>
+      </c>
+      <c r="S19" t="s">
+        <v>818</v>
+      </c>
+      <c r="T19" t="s">
+        <v>686</v>
+      </c>
+      <c r="U19" t="s">
+        <v>816</v>
+      </c>
+      <c r="V19" t="s">
+        <v>688</v>
+      </c>
+      <c r="W19" t="s">
+        <v>735</v>
+      </c>
+      <c r="X19" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>680</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>690</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>795</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>902</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>762</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>689</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>817</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>676</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>542</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1339989</v>
+      </c>
+      <c r="C20" t="s">
+        <v>821</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G20" t="s">
+        <v>706</v>
+      </c>
+      <c r="R20" t="s">
+        <v>542</v>
+      </c>
+      <c r="S20" t="s">
+        <v>822</v>
+      </c>
+      <c r="T20" t="s">
+        <v>378</v>
+      </c>
+      <c r="U20" t="s">
+        <v>761</v>
+      </c>
+      <c r="V20" t="s">
+        <v>687</v>
+      </c>
+      <c r="W20" t="s">
+        <v>395</v>
+      </c>
+      <c r="X20" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>692</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>401</v>
+      </c>
+      <c r="B21" s="8">
+        <v>474028</v>
+      </c>
+      <c r="C21" t="s">
+        <v>778</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G21" t="s">
+        <v>653</v>
+      </c>
+      <c r="R21" t="s">
+        <v>401</v>
+      </c>
+      <c r="S21" t="s">
+        <v>304</v>
+      </c>
+      <c r="T21" t="s">
+        <v>674</v>
+      </c>
+      <c r="U21" t="s">
+        <v>677</v>
+      </c>
+      <c r="V21" t="s">
+        <v>696</v>
+      </c>
+      <c r="W21" t="s">
+        <v>825</v>
+      </c>
+      <c r="X21" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>756</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>680</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>904</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>804</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>718</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>757</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>599</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1229286</v>
+      </c>
+      <c r="C22" t="s">
+        <v>829</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G22" t="s">
+        <v>653</v>
+      </c>
+      <c r="R22" t="s">
+        <v>599</v>
+      </c>
+      <c r="S22" t="s">
+        <v>830</v>
+      </c>
+      <c r="T22" t="s">
+        <v>693</v>
+      </c>
+      <c r="U22" t="s">
+        <v>675</v>
+      </c>
+      <c r="V22" t="s">
+        <v>735</v>
+      </c>
+      <c r="W22" t="s">
+        <v>688</v>
+      </c>
+      <c r="X22" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>756</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>828</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>835</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2340261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>673</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G23" t="s">
+        <v>706</v>
+      </c>
+      <c r="R23" t="s">
+        <v>835</v>
+      </c>
+      <c r="S23" t="s">
+        <v>307</v>
+      </c>
+      <c r="T23" t="s">
+        <v>833</v>
+      </c>
+      <c r="U23" t="s">
+        <v>834</v>
+      </c>
+      <c r="V23" t="s">
+        <v>687</v>
+      </c>
+      <c r="W23" t="s">
+        <v>696</v>
+      </c>
+      <c r="X23" t="s">
+        <v>691</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>740</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>683</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>675</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>809</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>588</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1708392</v>
+      </c>
+      <c r="C24" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G24" t="s">
+        <v>672</v>
+      </c>
+      <c r="R24" t="s">
+        <v>588</v>
+      </c>
+      <c r="S24" t="s">
+        <v>309</v>
+      </c>
+      <c r="T24" t="s">
+        <v>838</v>
+      </c>
+      <c r="U24" t="s">
+        <v>689</v>
+      </c>
+      <c r="V24" t="s">
+        <v>395</v>
+      </c>
+      <c r="W24" t="s">
+        <v>790</v>
+      </c>
+      <c r="X24" t="s">
+        <v>696</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>839</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>840</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>721</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>701</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>710</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>757</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>845</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2719892</v>
+      </c>
+      <c r="C25" t="s">
+        <v>844</v>
+      </c>
+      <c r="D25" t="s">
+        <v>798</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G25" t="s">
+        <v>452</v>
+      </c>
+      <c r="R25" t="s">
+        <v>845</v>
+      </c>
+      <c r="S25" t="s">
+        <v>487</v>
+      </c>
+      <c r="T25" t="s">
+        <v>726</v>
+      </c>
+      <c r="U25" t="s">
+        <v>718</v>
+      </c>
+      <c r="V25" t="s">
+        <v>687</v>
+      </c>
+      <c r="W25" t="s">
+        <v>688</v>
+      </c>
+      <c r="X25" t="s">
+        <v>756</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>776</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>698</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>928</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>595</v>
+      </c>
+      <c r="B26" s="8">
+        <v>122847</v>
+      </c>
+      <c r="C26" t="s">
+        <v>771</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G26" t="s">
+        <v>706</v>
+      </c>
+      <c r="R26" t="s">
+        <v>595</v>
+      </c>
+      <c r="S26" t="s">
+        <v>849</v>
+      </c>
+      <c r="T26" t="s">
+        <v>674</v>
+      </c>
+      <c r="U26" t="s">
+        <v>848</v>
+      </c>
+      <c r="V26" t="s">
+        <v>688</v>
+      </c>
+      <c r="W26" t="s">
+        <v>676</v>
+      </c>
+      <c r="X26" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>756</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>904</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>700</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>804</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>684</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>817</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>685</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>854</v>
+      </c>
+      <c r="B27" s="8">
+        <v>362369</v>
+      </c>
+      <c r="C27" t="s">
+        <v>276</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G27" t="s">
+        <v>653</v>
+      </c>
+      <c r="R27" t="s">
+        <v>854</v>
+      </c>
+      <c r="S27" t="s">
+        <v>853</v>
+      </c>
+      <c r="T27" t="s">
+        <v>686</v>
+      </c>
+      <c r="U27" t="s">
+        <v>816</v>
+      </c>
+      <c r="V27" t="s">
+        <v>689</v>
+      </c>
+      <c r="W27" t="s">
+        <v>688</v>
+      </c>
+      <c r="X27" t="s">
+        <v>690</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>852</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>795</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>695</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>687</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>676</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>858</v>
+      </c>
+      <c r="B28" s="8">
+        <v>290784</v>
+      </c>
+      <c r="C28" t="s">
+        <v>712</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G28" t="s">
+        <v>930</v>
+      </c>
+      <c r="R28" t="s">
+        <v>858</v>
+      </c>
+      <c r="S28" t="s">
+        <v>857</v>
+      </c>
+      <c r="T28" t="s">
+        <v>674</v>
+      </c>
+      <c r="U28" t="s">
+        <v>676</v>
+      </c>
+      <c r="V28" t="s">
+        <v>688</v>
+      </c>
+      <c r="W28" t="s">
+        <v>696</v>
+      </c>
+      <c r="X28" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>698</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>749</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>902</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>399</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>806</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>707</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>756</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>863</v>
+      </c>
+      <c r="B29" s="8">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>785</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G29" t="s">
+        <v>653</v>
+      </c>
+      <c r="R29" t="s">
+        <v>863</v>
+      </c>
+      <c r="S29" t="s">
+        <v>862</v>
+      </c>
+      <c r="T29" t="s">
+        <v>674</v>
+      </c>
+      <c r="U29" t="s">
+        <v>677</v>
+      </c>
+      <c r="V29" t="s">
+        <v>718</v>
+      </c>
+      <c r="W29" t="s">
+        <v>687</v>
+      </c>
+      <c r="X29" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>698</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>679</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>684</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>750</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>866</v>
+      </c>
+      <c r="B30" s="8">
+        <v>23487</v>
+      </c>
+      <c r="C30" t="s">
+        <v>712</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G30" t="s">
+        <v>653</v>
+      </c>
+      <c r="R30" t="s">
+        <v>866</v>
+      </c>
+      <c r="S30" t="s">
+        <v>315</v>
+      </c>
+      <c r="T30" t="s">
+        <v>686</v>
+      </c>
+      <c r="U30" t="s">
+        <v>689</v>
+      </c>
+      <c r="V30" t="s">
+        <v>676</v>
+      </c>
+      <c r="W30" t="s">
+        <v>688</v>
+      </c>
+      <c r="X30" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>902</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>817</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>806</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>694</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>870</v>
+      </c>
+      <c r="B31" s="8">
+        <v>360554</v>
+      </c>
+      <c r="C31" t="s">
+        <v>712</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G31" t="s">
+        <v>452</v>
+      </c>
+      <c r="R31" t="s">
+        <v>870</v>
+      </c>
+      <c r="S31" t="s">
+        <v>869</v>
+      </c>
+      <c r="T31" t="s">
+        <v>674</v>
+      </c>
+      <c r="U31" t="s">
+        <v>718</v>
+      </c>
+      <c r="V31" t="s">
+        <v>688</v>
+      </c>
+      <c r="W31" t="s">
+        <v>848</v>
+      </c>
+      <c r="X31" t="s">
+        <v>929</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>804</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>817</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>685</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>684</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>520</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2090014</v>
+      </c>
+      <c r="C32" t="s">
+        <v>874</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G32" t="s">
+        <v>706</v>
+      </c>
+      <c r="R32" t="s">
+        <v>520</v>
+      </c>
+      <c r="S32" t="s">
+        <v>875</v>
+      </c>
+      <c r="T32" t="s">
+        <v>833</v>
+      </c>
+      <c r="U32" t="s">
+        <v>687</v>
+      </c>
+      <c r="V32" t="s">
+        <v>873</v>
+      </c>
+      <c r="W32" t="s">
+        <v>761</v>
+      </c>
+      <c r="X32" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>680</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>799</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>904</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>750</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>707</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>444</v>
+      </c>
+      <c r="B33" s="8">
+        <v>158870</v>
+      </c>
+      <c r="C33" t="s">
+        <v>841</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G33" t="s">
+        <v>706</v>
+      </c>
+      <c r="R33" t="s">
+        <v>444</v>
+      </c>
+      <c r="S33" t="s">
+        <v>267</v>
+      </c>
+      <c r="T33" t="s">
+        <v>674</v>
+      </c>
+      <c r="U33" t="s">
+        <v>816</v>
+      </c>
+      <c r="V33" t="s">
+        <v>718</v>
+      </c>
+      <c r="W33" t="s">
+        <v>848</v>
+      </c>
+      <c r="X33" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>681</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>698</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>817</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>904</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>682</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>693</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>784</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>685</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -5815,9 +8513,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6209,10 +8907,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6598,10 +9296,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -7956,10 +10654,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -8227,12 +10925,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -11003,32 +13701,32 @@
   <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B28" sqref="A28:B28"/>
+      <selection sqref="A1:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="34" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -13527,10 +16225,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
combo not running in conjuction
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3811" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3943" uniqueCount="1369">
   <si>
     <t>Places</t>
   </si>
@@ -4029,148 +4029,112 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Flint Fc</t>
-  </si>
-  <si>
-    <t>1699830</t>
-  </si>
-  <si>
-    <t>NoviceMb</t>
-  </si>
-  <si>
-    <t>351931</t>
-  </si>
-  <si>
-    <t>The Offside Traps</t>
-  </si>
-  <si>
-    <t>3958276</t>
-  </si>
-  <si>
-    <t>Holy Divers</t>
-  </si>
-  <si>
-    <t>124801</t>
-  </si>
-  <si>
-    <t>Quaranteam</t>
-  </si>
-  <si>
-    <t>4354768</t>
-  </si>
-  <si>
-    <t>Ozymendiaz</t>
-  </si>
-  <si>
-    <t>380438</t>
-  </si>
-  <si>
-    <t>frogs</t>
-  </si>
-  <si>
-    <t>5109360</t>
-  </si>
-  <si>
-    <t>Ben D’S 11</t>
-  </si>
-  <si>
-    <t>4193686</t>
-  </si>
-  <si>
-    <t>City Wok First XI</t>
-  </si>
-  <si>
-    <t>3822239</t>
-  </si>
-  <si>
-    <t>denilsonx</t>
-  </si>
-  <si>
-    <t>4374651</t>
-  </si>
-  <si>
-    <t>TOPBOYS</t>
-  </si>
-  <si>
-    <t>6329451</t>
-  </si>
-  <si>
-    <t>Hooligans</t>
-  </si>
-  <si>
-    <t>3741828</t>
-  </si>
-  <si>
-    <t>Kang and Kodos</t>
-  </si>
-  <si>
-    <t>462617</t>
-  </si>
-  <si>
-    <t>Bergkamp</t>
-  </si>
-  <si>
-    <t>4136051</t>
-  </si>
-  <si>
-    <t>NO Madder son</t>
-  </si>
-  <si>
-    <t>2640115</t>
+    <t>Deep</t>
+  </si>
+  <si>
+    <t>Sabuj Sangha</t>
+  </si>
+  <si>
+    <t>The non negotiables</t>
+  </si>
+  <si>
+    <t>Three Cheers</t>
+  </si>
+  <si>
+    <t>pokyong_rong</t>
+  </si>
+  <si>
+    <t>WILDHORN</t>
   </si>
   <si>
     <t>Pp11</t>
   </si>
   <si>
+    <t>In search of Kwan</t>
+  </si>
+  <si>
+    <t>DestyBubu</t>
+  </si>
+  <si>
+    <t>Bachmann 0</t>
+  </si>
+  <si>
+    <t>deep chaudhury</t>
+  </si>
+  <si>
+    <t>Saïss 7</t>
+  </si>
+  <si>
+    <t>Soumya Chowdhury</t>
+  </si>
+  <si>
+    <t>souvik ray</t>
+  </si>
+  <si>
+    <t>Jyotibrata Das</t>
+  </si>
+  <si>
+    <t>Temkup Lepcha</t>
+  </si>
+  <si>
+    <t>Romeu 3</t>
+  </si>
+  <si>
+    <t>Antonio 2$ captain</t>
+  </si>
+  <si>
+    <t>Cavani 0</t>
+  </si>
+  <si>
+    <t>Dabojit Banerjee</t>
+  </si>
+  <si>
+    <t>priyanko pal</t>
+  </si>
+  <si>
+    <t>S.Longstaff 0</t>
+  </si>
+  <si>
+    <t>Sourav Chatterjee</t>
+  </si>
+  <si>
+    <t>Soucek 3</t>
+  </si>
+  <si>
+    <t>Havertz 1</t>
+  </si>
+  <si>
+    <t>Greenwood 0</t>
+  </si>
+  <si>
+    <t>Anirban Sett</t>
+  </si>
+  <si>
+    <t>417137</t>
+  </si>
+  <si>
+    <t>975590</t>
+  </si>
+  <si>
+    <t>8321</t>
+  </si>
+  <si>
+    <t>383984</t>
+  </si>
+  <si>
+    <t>1626153</t>
+  </si>
+  <si>
+    <t>1805393</t>
+  </si>
+  <si>
     <t>2317004</t>
   </si>
   <si>
-    <t>Ondieki Stars</t>
-  </si>
-  <si>
-    <t>4779115</t>
-  </si>
-  <si>
-    <t>Havilah FC</t>
-  </si>
-  <si>
-    <t>3672554</t>
-  </si>
-  <si>
-    <t>China1</t>
-  </si>
-  <si>
-    <t>6205577</t>
-  </si>
-  <si>
-    <t>AbuMazeedah</t>
-  </si>
-  <si>
-    <t>4014921</t>
-  </si>
-  <si>
-    <t>KinsaleGoons</t>
-  </si>
-  <si>
-    <t>4323491</t>
-  </si>
-  <si>
-    <t>Savage United</t>
-  </si>
-  <si>
-    <t>4363088</t>
-  </si>
-  <si>
-    <t>MK FC</t>
-  </si>
-  <si>
-    <t>4761319</t>
-  </si>
-  <si>
-    <t>Athletic Beerbarrel</t>
-  </si>
-  <si>
-    <t>2535693</t>
+    <t>2880295</t>
+  </si>
+  <si>
+    <t>5767407</t>
   </si>
 </sst>
 </file>
@@ -10293,16 +10257,37 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK25"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.18359375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.03515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10418,196 +10403,562 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1333</v>
       </c>
       <c r="B2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="X2" t="s">
+        <v>360</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1077</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>805</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1334</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="T3" t="s">
+        <v>674</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="V3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="W3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>903</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>740</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>809</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1335</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>1362</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1335</v>
+      </c>
+      <c r="T4" t="s">
+        <v>674</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="V4" t="s">
+        <v>360</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>799</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>884</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>767</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1336</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1336</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="V5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>902</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>1077</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>582</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1337</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>1364</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1348</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1337</v>
+      </c>
+      <c r="T6" t="s">
+        <v>674</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="V6" t="s">
+        <v>792</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1117</v>
+      </c>
+      <c r="X6" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>707</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>809</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>1365</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1352</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="T7" t="s">
+        <v>674</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="V7" t="s">
+        <v>792</v>
+      </c>
+      <c r="W7" t="s">
+        <v>1071</v>
+      </c>
+      <c r="X7" t="s">
+        <v>1117</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>678</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>697</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>1349</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>1350</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>784</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>1339</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>1366</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1353</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="T8" t="s">
+        <v>674</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1117</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1055</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1079</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>976</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>1097</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>679</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>1340</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>1367</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1355</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1340</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="V9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="X9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>812</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>1341</v>
       </c>
-      <c r="B6" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1348</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>1349</v>
-      </c>
       <c r="B10" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1352</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1354</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1359</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1341</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1072</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1102</v>
+      </c>
+      <c r="V10" t="s">
+        <v>1117</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1058</v>
+      </c>
+      <c r="X10" t="s">
+        <v>1100</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>976</v>
+      </c>
+      <c r="Z10" t="s">
         <v>1356</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="AA10" t="s">
+        <v>1098</v>
+      </c>
+      <c r="AB10" t="s">
         <v>1357</v>
       </c>
-      <c r="B14" t="s">
+      <c r="AC10" t="s">
+        <v>902</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AG10" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>1361</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1362</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>1367</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>1375</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>1377</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1378</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>1379</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1380</v>
+      <c r="AH10" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FPL6 gw9 md2 bonus inclusion
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7301" uniqueCount="1628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8658" uniqueCount="1702">
   <si>
     <t>Places</t>
   </si>
@@ -4912,6 +4912,228 @@
   </si>
   <si>
     <t>893,732</t>
+  </si>
+  <si>
+    <t>Sánchez 4</t>
+  </si>
+  <si>
+    <t>Livramento 9</t>
+  </si>
+  <si>
+    <t>2,253,626</t>
+  </si>
+  <si>
+    <t>464</t>
+  </si>
+  <si>
+    <t>Gray 5</t>
+  </si>
+  <si>
+    <t>3,681,409</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t>James 13</t>
+  </si>
+  <si>
+    <t>Kovacic 11</t>
+  </si>
+  <si>
+    <t>1,584,650</t>
+  </si>
+  <si>
+    <t>Cancelo 1</t>
+  </si>
+  <si>
+    <t>Hwang 8</t>
+  </si>
+  <si>
+    <t>Duffy 0</t>
+  </si>
+  <si>
+    <t>912,045</t>
+  </si>
+  <si>
+    <t>McCarthy 2</t>
+  </si>
+  <si>
+    <t>Moder 1</t>
+  </si>
+  <si>
+    <t>1,996,141</t>
+  </si>
+  <si>
+    <t>Dennis 12</t>
+  </si>
+  <si>
+    <t>1,855,985</t>
+  </si>
+  <si>
+    <t>475</t>
+  </si>
+  <si>
+    <t>1,123,513</t>
+  </si>
+  <si>
+    <t>Dias 4$ captain</t>
+  </si>
+  <si>
+    <t>Manquillo 2</t>
+  </si>
+  <si>
+    <t>Bernardo 5</t>
+  </si>
+  <si>
+    <t>1,817,832</t>
+  </si>
+  <si>
+    <t>476</t>
+  </si>
+  <si>
+    <t>1,684,357</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>Dias 2</t>
+  </si>
+  <si>
+    <t>1,152,156</t>
+  </si>
+  <si>
+    <t>497</t>
+  </si>
+  <si>
+    <t>Ederson 2</t>
+  </si>
+  <si>
+    <t>812,952</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1,099,835</t>
+  </si>
+  <si>
+    <t>499</t>
+  </si>
+  <si>
+    <t>Digne -1</t>
+  </si>
+  <si>
+    <t>Jiménez 5</t>
+  </si>
+  <si>
+    <t>1,009,957</t>
+  </si>
+  <si>
+    <t>592,894</t>
+  </si>
+  <si>
+    <t>587,373</t>
+  </si>
+  <si>
+    <t>McArthur 5</t>
+  </si>
+  <si>
+    <t>1,334,564</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>569,707</t>
+  </si>
+  <si>
+    <t>Laporte 2</t>
+  </si>
+  <si>
+    <t>364,636</t>
+  </si>
+  <si>
+    <t>533</t>
+  </si>
+  <si>
+    <t>372,527</t>
+  </si>
+  <si>
+    <t>Foden 18</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>296,166</t>
+  </si>
+  <si>
+    <t>579,551</t>
+  </si>
+  <si>
+    <t>Sá 3</t>
+  </si>
+  <si>
+    <t>Jesus 10$ captain</t>
+  </si>
+  <si>
+    <t>301,418</t>
+  </si>
+  <si>
+    <t>Rodrigo 8</t>
+  </si>
+  <si>
+    <t>231,474</t>
+  </si>
+  <si>
+    <t>544</t>
+  </si>
+  <si>
+    <t>2,524,691</t>
+  </si>
+  <si>
+    <t>719,665</t>
+  </si>
+  <si>
+    <t>194,309</t>
+  </si>
+  <si>
+    <t>547</t>
+  </si>
+  <si>
+    <t>240,571</t>
+  </si>
+  <si>
+    <t>2,253,635</t>
+  </si>
+  <si>
+    <t>37,355</t>
+  </si>
+  <si>
+    <t>575</t>
+  </si>
+  <si>
+    <t>277,925</t>
+  </si>
+  <si>
+    <t>540</t>
+  </si>
+  <si>
+    <t>480,096</t>
+  </si>
+  <si>
+    <t>285,781</t>
+  </si>
+  <si>
+    <t>539</t>
+  </si>
+  <si>
+    <t>Mahrez 6</t>
+  </si>
+  <si>
+    <t>38,036</t>
   </si>
 </sst>
 </file>
@@ -8137,13 +8359,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>1614</v>
+        <v>988</v>
       </c>
       <c r="D2" t="s">
-        <v>760</v>
+        <v>1631</v>
       </c>
       <c r="E2" t="s">
-        <v>1615</v>
+        <v>1692</v>
       </c>
       <c r="G2" t="s">
         <v>672</v>
@@ -8155,7 +8377,7 @@
         <v>269</v>
       </c>
       <c r="T2" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U2" t="s">
         <v>1535</v>
@@ -8164,7 +8386,7 @@
         <v>1485</v>
       </c>
       <c r="W2" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="X2" t="s">
         <v>1372</v>
@@ -8182,10 +8404,10 @@
         <v>1376</v>
       </c>
       <c r="AC2" t="s">
-        <v>1537</v>
+        <v>1132</v>
       </c>
       <c r="AD2" t="s">
-        <v>481</v>
+        <v>692</v>
       </c>
       <c r="AE2" t="s">
         <v>1062</v>
@@ -8197,10 +8419,10 @@
         <v>1381</v>
       </c>
       <c r="AH2" t="s">
-        <v>1382</v>
+        <v>699</v>
       </c>
       <c r="AI2" t="s">
-        <v>1614</v>
+        <v>988</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -8211,13 +8433,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>1602</v>
+        <v>1564</v>
       </c>
       <c r="D3" t="s">
-        <v>1000</v>
+        <v>1634</v>
       </c>
       <c r="E3" t="s">
-        <v>1616</v>
+        <v>1633</v>
       </c>
       <c r="G3" t="s">
         <v>672</v>
@@ -8229,10 +8451,10 @@
         <v>713</v>
       </c>
       <c r="T3" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U3" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="V3" t="s">
         <v>1535</v>
@@ -8244,16 +8466,16 @@
         <v>1381</v>
       </c>
       <c r="Y3" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Z3" t="s">
         <v>1385</v>
       </c>
       <c r="AA3" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="AB3" t="s">
-        <v>1541</v>
+        <v>553</v>
       </c>
       <c r="AC3" t="s">
         <v>1388</v>
@@ -8262,10 +8484,10 @@
         <v>1389</v>
       </c>
       <c r="AE3" t="s">
-        <v>1542</v>
+        <v>709</v>
       </c>
       <c r="AF3" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="AG3" t="s">
         <v>710</v>
@@ -8274,7 +8496,7 @@
         <v>1067</v>
       </c>
       <c r="AI3" t="s">
-        <v>1602</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -8285,13 +8507,13 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>829</v>
+        <v>268</v>
       </c>
       <c r="D4" t="s">
-        <v>856</v>
+        <v>1523</v>
       </c>
       <c r="E4" t="s">
-        <v>1617</v>
+        <v>1637</v>
       </c>
       <c r="G4" t="s">
         <v>706</v>
@@ -8306,7 +8528,7 @@
         <v>1393</v>
       </c>
       <c r="U4" t="s">
-        <v>1500</v>
+        <v>1635</v>
       </c>
       <c r="V4" t="s">
         <v>1485</v>
@@ -8315,10 +8537,10 @@
         <v>1381</v>
       </c>
       <c r="X4" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Y4" t="s">
-        <v>1501</v>
+        <v>1636</v>
       </c>
       <c r="Z4" t="s">
         <v>1385</v>
@@ -8327,7 +8549,7 @@
         <v>1502</v>
       </c>
       <c r="AB4" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="AC4" t="s">
         <v>1388</v>
@@ -8348,7 +8570,7 @@
         <v>1398</v>
       </c>
       <c r="AI4" t="s">
-        <v>829</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -8359,13 +8581,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>1553</v>
+        <v>923</v>
       </c>
       <c r="D5" t="s">
-        <v>894</v>
+        <v>1021</v>
       </c>
       <c r="E5" t="s">
-        <v>1618</v>
+        <v>1641</v>
       </c>
       <c r="G5" t="s">
         <v>452</v>
@@ -8383,7 +8605,7 @@
         <v>707</v>
       </c>
       <c r="V5" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W5" t="s">
         <v>1403</v>
@@ -8401,10 +8623,10 @@
         <v>1545</v>
       </c>
       <c r="AB5" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="AC5" t="s">
-        <v>1571</v>
+        <v>1639</v>
       </c>
       <c r="AD5" t="s">
         <v>1408</v>
@@ -8419,10 +8641,10 @@
         <v>700</v>
       </c>
       <c r="AH5" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AI5" t="s">
-        <v>1553</v>
+        <v>923</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -8433,13 +8655,13 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
       <c r="D6" t="s">
-        <v>820</v>
+        <v>1024</v>
       </c>
       <c r="E6" t="s">
-        <v>1619</v>
+        <v>1644</v>
       </c>
       <c r="G6" t="s">
         <v>706</v>
@@ -8451,16 +8673,16 @@
         <v>743</v>
       </c>
       <c r="T6" t="s">
-        <v>1548</v>
+        <v>1642</v>
       </c>
       <c r="U6" t="s">
-        <v>1411</v>
+        <v>746</v>
       </c>
       <c r="V6" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="W6" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="X6" t="s">
         <v>1412</v>
@@ -8493,10 +8715,10 @@
         <v>1490</v>
       </c>
       <c r="AH6" t="s">
-        <v>1418</v>
+        <v>1643</v>
       </c>
       <c r="AI6" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -8507,13 +8729,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>1592</v>
+        <v>931</v>
       </c>
       <c r="D7" t="s">
-        <v>843</v>
+        <v>1647</v>
       </c>
       <c r="E7" t="s">
-        <v>1620</v>
+        <v>1646</v>
       </c>
       <c r="G7" t="s">
         <v>672</v>
@@ -8531,13 +8753,13 @@
         <v>1372</v>
       </c>
       <c r="V7" t="s">
-        <v>1411</v>
+        <v>746</v>
       </c>
       <c r="W7" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="X7" t="s">
-        <v>1537</v>
+        <v>1132</v>
       </c>
       <c r="Y7" t="s">
         <v>1545</v>
@@ -8549,7 +8771,7 @@
         <v>1385</v>
       </c>
       <c r="AB7" t="s">
-        <v>1550</v>
+        <v>1645</v>
       </c>
       <c r="AC7" t="s">
         <v>1389</v>
@@ -8558,19 +8780,19 @@
         <v>1388</v>
       </c>
       <c r="AE7" t="s">
-        <v>1542</v>
+        <v>709</v>
       </c>
       <c r="AF7" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AG7" t="s">
         <v>1420</v>
       </c>
       <c r="AH7" t="s">
-        <v>1421</v>
+        <v>751</v>
       </c>
       <c r="AI7" t="s">
-        <v>1592</v>
+        <v>931</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -8581,13 +8803,13 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>1553</v>
+        <v>981</v>
       </c>
       <c r="D8" t="s">
-        <v>894</v>
+        <v>1026</v>
       </c>
       <c r="E8" t="s">
-        <v>1621</v>
+        <v>1648</v>
       </c>
       <c r="G8" t="s">
         <v>452</v>
@@ -8599,7 +8821,7 @@
         <v>758</v>
       </c>
       <c r="T8" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U8" t="s">
         <v>1552</v>
@@ -8635,7 +8857,7 @@
         <v>399</v>
       </c>
       <c r="AF8" t="s">
-        <v>1426</v>
+        <v>1090</v>
       </c>
       <c r="AG8" t="s">
         <v>400</v>
@@ -8644,7 +8866,7 @@
         <v>1428</v>
       </c>
       <c r="AI8" t="s">
-        <v>1553</v>
+        <v>981</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -8655,13 +8877,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>672</v>
+        <v>1553</v>
       </c>
       <c r="D9" t="s">
-        <v>1012</v>
+        <v>1653</v>
       </c>
       <c r="E9" t="s">
-        <v>1622</v>
+        <v>1652</v>
       </c>
       <c r="G9" t="s">
         <v>653</v>
@@ -8673,22 +8895,22 @@
         <v>763</v>
       </c>
       <c r="T9" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U9" t="s">
         <v>1381</v>
       </c>
       <c r="V9" t="s">
-        <v>1429</v>
+        <v>1649</v>
       </c>
       <c r="W9" t="s">
         <v>1535</v>
       </c>
       <c r="X9" t="s">
-        <v>1555</v>
+        <v>1650</v>
       </c>
       <c r="Y9" t="s">
-        <v>1431</v>
+        <v>1651</v>
       </c>
       <c r="Z9" t="s">
         <v>1385</v>
@@ -8712,13 +8934,13 @@
         <v>1435</v>
       </c>
       <c r="AG9" t="s">
-        <v>1550</v>
+        <v>1645</v>
       </c>
       <c r="AH9" t="s">
         <v>1398</v>
       </c>
       <c r="AI9" t="s">
-        <v>672</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -8729,13 +8951,13 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>1558</v>
+        <v>988</v>
       </c>
       <c r="D10" t="s">
-        <v>856</v>
+        <v>1655</v>
       </c>
       <c r="E10" t="s">
-        <v>1617</v>
+        <v>1654</v>
       </c>
       <c r="G10" t="s">
         <v>706</v>
@@ -8762,13 +8984,13 @@
         <v>1375</v>
       </c>
       <c r="Y10" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="Z10" t="s">
         <v>1373</v>
       </c>
       <c r="AA10" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="AB10" t="s">
         <v>1514</v>
@@ -8786,13 +9008,13 @@
         <v>1398</v>
       </c>
       <c r="AG10" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AH10" t="s">
         <v>767</v>
       </c>
       <c r="AI10" t="s">
-        <v>1558</v>
+        <v>988</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -8803,13 +9025,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>1492</v>
+        <v>981</v>
       </c>
       <c r="D11" t="s">
-        <v>1560</v>
+        <v>1658</v>
       </c>
       <c r="E11" t="s">
-        <v>1623</v>
+        <v>1657</v>
       </c>
       <c r="G11" t="s">
         <v>672</v>
@@ -8824,10 +9046,10 @@
         <v>1434</v>
       </c>
       <c r="U11" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="V11" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W11" t="s">
         <v>1381</v>
@@ -8839,10 +9061,10 @@
         <v>1373</v>
       </c>
       <c r="Z11" t="s">
-        <v>1501</v>
+        <v>1636</v>
       </c>
       <c r="AA11" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="AB11" t="s">
         <v>1375</v>
@@ -8854,7 +9076,7 @@
         <v>1408</v>
       </c>
       <c r="AE11" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="AF11" t="s">
         <v>1423</v>
@@ -8863,10 +9085,10 @@
         <v>1417</v>
       </c>
       <c r="AH11" t="s">
-        <v>1550</v>
+        <v>1645</v>
       </c>
       <c r="AI11" t="s">
-        <v>1492</v>
+        <v>981</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -8877,13 +9099,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>940</v>
+        <v>778</v>
       </c>
       <c r="D12" t="s">
-        <v>1563</v>
+        <v>1028</v>
       </c>
       <c r="E12" t="s">
-        <v>1624</v>
+        <v>1660</v>
       </c>
       <c r="G12" t="s">
         <v>578</v>
@@ -8895,19 +9117,19 @@
         <v>289</v>
       </c>
       <c r="T12" t="s">
-        <v>1442</v>
+        <v>1659</v>
       </c>
       <c r="U12" t="s">
         <v>1485</v>
       </c>
       <c r="V12" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="W12" t="s">
         <v>1552</v>
       </c>
       <c r="X12" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="Y12" t="s">
         <v>1520</v>
@@ -8916,7 +9138,7 @@
         <v>1375</v>
       </c>
       <c r="AA12" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="AB12" t="s">
         <v>1502</v>
@@ -8931,16 +9153,16 @@
         <v>1489</v>
       </c>
       <c r="AF12" t="s">
-        <v>1444</v>
+        <v>492</v>
       </c>
       <c r="AG12" t="s">
-        <v>481</v>
+        <v>692</v>
       </c>
       <c r="AH12" t="s">
-        <v>1555</v>
+        <v>1650</v>
       </c>
       <c r="AI12" t="s">
-        <v>940</v>
+        <v>778</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -8951,13 +9173,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>1564</v>
+        <v>1661</v>
       </c>
       <c r="D13" t="s">
-        <v>1041</v>
+        <v>1663</v>
       </c>
       <c r="E13" t="s">
-        <v>1625</v>
+        <v>1662</v>
       </c>
       <c r="G13" t="s">
         <v>706</v>
@@ -8978,13 +9200,13 @@
         <v>1381</v>
       </c>
       <c r="W13" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="X13" t="s">
         <v>707</v>
       </c>
       <c r="Y13" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Z13" t="s">
         <v>1373</v>
@@ -8993,7 +9215,7 @@
         <v>1385</v>
       </c>
       <c r="AB13" t="s">
-        <v>1501</v>
+        <v>1636</v>
       </c>
       <c r="AC13" t="s">
         <v>1414</v>
@@ -9008,13 +9230,13 @@
         <v>1437</v>
       </c>
       <c r="AG13" t="s">
-        <v>1421</v>
+        <v>751</v>
       </c>
       <c r="AH13" t="s">
         <v>784</v>
       </c>
       <c r="AI13" t="s">
-        <v>1564</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -9025,13 +9247,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>1524</v>
+        <v>923</v>
       </c>
       <c r="D14" t="s">
-        <v>894</v>
+        <v>865</v>
       </c>
       <c r="E14" t="s">
-        <v>1627</v>
+        <v>1666</v>
       </c>
       <c r="G14" t="s">
         <v>672</v>
@@ -9043,16 +9265,16 @@
         <v>796</v>
       </c>
       <c r="T14" t="s">
-        <v>1566</v>
+        <v>1106</v>
       </c>
       <c r="U14" t="s">
-        <v>1626</v>
+        <v>1664</v>
       </c>
       <c r="V14" t="s">
         <v>565</v>
       </c>
       <c r="W14" t="s">
-        <v>1568</v>
+        <v>791</v>
       </c>
       <c r="X14" t="s">
         <v>1497</v>
@@ -9067,7 +9289,7 @@
         <v>1385</v>
       </c>
       <c r="AB14" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AC14" t="s">
         <v>1408</v>
@@ -9082,13 +9304,13 @@
         <v>456</v>
       </c>
       <c r="AG14" t="s">
-        <v>1421</v>
+        <v>751</v>
       </c>
       <c r="AH14" t="s">
         <v>767</v>
       </c>
       <c r="AI14" t="s">
-        <v>1524</v>
+        <v>923</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -9099,13 +9321,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
       <c r="D15" t="s">
-        <v>1028</v>
+        <v>1608</v>
       </c>
       <c r="E15" t="s">
-        <v>1572</v>
+        <v>1667</v>
       </c>
       <c r="G15" t="s">
         <v>706</v>
@@ -9120,13 +9342,13 @@
         <v>1489</v>
       </c>
       <c r="U15" t="s">
-        <v>1411</v>
+        <v>746</v>
       </c>
       <c r="V15" t="s">
         <v>1381</v>
       </c>
       <c r="W15" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="X15" t="s">
         <v>1456</v>
@@ -9141,7 +9363,7 @@
         <v>1457</v>
       </c>
       <c r="AB15" t="s">
-        <v>1571</v>
+        <v>1639</v>
       </c>
       <c r="AC15" t="s">
         <v>1414</v>
@@ -9153,16 +9375,16 @@
         <v>1062</v>
       </c>
       <c r="AF15" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AG15" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AH15" t="s">
         <v>1556</v>
       </c>
       <c r="AI15" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -9173,13 +9395,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>1518</v>
+        <v>1524</v>
       </c>
       <c r="D16" t="s">
-        <v>865</v>
+        <v>1608</v>
       </c>
       <c r="E16" t="s">
-        <v>1575</v>
+        <v>1668</v>
       </c>
       <c r="G16" t="s">
         <v>653</v>
@@ -9191,22 +9413,22 @@
         <v>296</v>
       </c>
       <c r="T16" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U16" t="s">
         <v>1458</v>
       </c>
       <c r="V16" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="W16" t="s">
         <v>694</v>
       </c>
       <c r="X16" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="Y16" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Z16" t="s">
         <v>1375</v>
@@ -9218,13 +9440,13 @@
         <v>1388</v>
       </c>
       <c r="AC16" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AD16" t="s">
         <v>1414</v>
       </c>
       <c r="AE16" t="s">
-        <v>1460</v>
+        <v>804</v>
       </c>
       <c r="AF16" t="s">
         <v>1398</v>
@@ -9236,7 +9458,7 @@
         <v>1574</v>
       </c>
       <c r="AI16" t="s">
-        <v>1518</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -9247,13 +9469,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
       <c r="D17" t="s">
-        <v>1577</v>
+        <v>1671</v>
       </c>
       <c r="E17" t="s">
-        <v>1576</v>
+        <v>1670</v>
       </c>
       <c r="G17" t="s">
         <v>452</v>
@@ -9271,16 +9493,16 @@
         <v>707</v>
       </c>
       <c r="V17" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W17" t="s">
         <v>1516</v>
       </c>
       <c r="X17" t="s">
-        <v>809</v>
+        <v>1669</v>
       </c>
       <c r="Y17" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Z17" t="s">
         <v>1385</v>
@@ -9298,10 +9520,10 @@
         <v>1414</v>
       </c>
       <c r="AE17" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="AF17" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AG17" t="s">
         <v>1573</v>
@@ -9310,7 +9532,7 @@
         <v>400</v>
       </c>
       <c r="AI17" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -9321,13 +9543,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>981</v>
+        <v>1599</v>
       </c>
       <c r="D18" t="s">
-        <v>1532</v>
+        <v>1589</v>
       </c>
       <c r="E18" t="s">
-        <v>1578</v>
+        <v>1672</v>
       </c>
       <c r="G18" t="s">
         <v>672</v>
@@ -9345,13 +9567,13 @@
         <v>1485</v>
       </c>
       <c r="V18" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W18" t="s">
         <v>1381</v>
       </c>
       <c r="X18" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="Y18" t="s">
         <v>1545</v>
@@ -9360,7 +9582,7 @@
         <v>1385</v>
       </c>
       <c r="AA18" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="AB18" t="s">
         <v>1373</v>
@@ -9378,13 +9600,13 @@
         <v>1423</v>
       </c>
       <c r="AG18" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AH18" t="s">
         <v>812</v>
       </c>
       <c r="AI18" t="s">
-        <v>981</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -9395,13 +9617,13 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>1553</v>
+        <v>1599</v>
       </c>
       <c r="D19" t="s">
-        <v>1534</v>
+        <v>1675</v>
       </c>
       <c r="E19" t="s">
-        <v>1580</v>
+        <v>1674</v>
       </c>
       <c r="G19" t="s">
         <v>706</v>
@@ -9419,13 +9641,13 @@
         <v>1497</v>
       </c>
       <c r="V19" t="s">
-        <v>1466</v>
+        <v>1673</v>
       </c>
       <c r="W19" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="X19" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="Y19" t="s">
         <v>1375</v>
@@ -9434,10 +9656,10 @@
         <v>1545</v>
       </c>
       <c r="AA19" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="AB19" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AC19" t="s">
         <v>1408</v>
@@ -9449,7 +9671,7 @@
         <v>1434</v>
       </c>
       <c r="AF19" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AG19" t="s">
         <v>1490</v>
@@ -9458,7 +9680,7 @@
         <v>456</v>
       </c>
       <c r="AI19" t="s">
-        <v>1553</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
@@ -9469,13 +9691,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>1599</v>
+        <v>1561</v>
       </c>
       <c r="D20" t="s">
-        <v>1583</v>
+        <v>1675</v>
       </c>
       <c r="E20" t="s">
-        <v>1582</v>
+        <v>1676</v>
       </c>
       <c r="G20" t="s">
         <v>452</v>
@@ -9490,16 +9712,16 @@
         <v>1581</v>
       </c>
       <c r="U20" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="V20" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="W20" t="s">
         <v>1372</v>
       </c>
       <c r="X20" t="s">
-        <v>1555</v>
+        <v>1650</v>
       </c>
       <c r="Y20" t="s">
         <v>1545</v>
@@ -9514,25 +9736,25 @@
         <v>1414</v>
       </c>
       <c r="AC20" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AD20" t="s">
         <v>1389</v>
       </c>
       <c r="AE20" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="AF20" t="s">
         <v>1373</v>
       </c>
       <c r="AG20" t="s">
-        <v>1421</v>
+        <v>751</v>
       </c>
       <c r="AH20" t="s">
         <v>1420</v>
       </c>
       <c r="AI20" t="s">
-        <v>1599</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -9543,13 +9765,13 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>1455</v>
+        <v>1678</v>
       </c>
       <c r="D21" t="s">
-        <v>1585</v>
+        <v>1598</v>
       </c>
       <c r="E21" t="s">
-        <v>1584</v>
+        <v>1679</v>
       </c>
       <c r="G21" t="s">
         <v>706</v>
@@ -9564,19 +9786,19 @@
         <v>1489</v>
       </c>
       <c r="U21" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="V21" t="s">
         <v>1381</v>
       </c>
       <c r="W21" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="X21" t="s">
         <v>1375</v>
       </c>
       <c r="Y21" t="s">
-        <v>1469</v>
+        <v>1677</v>
       </c>
       <c r="Z21" t="s">
         <v>456</v>
@@ -9597,16 +9819,16 @@
         <v>1062</v>
       </c>
       <c r="AF21" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AG21" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AH21" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AI21" t="s">
-        <v>1455</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -9617,13 +9839,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>981</v>
+        <v>1129</v>
       </c>
       <c r="D22" t="s">
-        <v>1534</v>
+        <v>1589</v>
       </c>
       <c r="E22" t="s">
-        <v>1586</v>
+        <v>1680</v>
       </c>
       <c r="G22" t="s">
         <v>1474</v>
@@ -9644,7 +9866,7 @@
         <v>1381</v>
       </c>
       <c r="W22" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="X22" t="s">
         <v>1545</v>
@@ -9665,22 +9887,22 @@
         <v>1414</v>
       </c>
       <c r="AD22" t="s">
-        <v>1472</v>
+        <v>907</v>
       </c>
       <c r="AE22" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="AF22" t="s">
         <v>1490</v>
       </c>
       <c r="AG22" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AH22" t="s">
         <v>828</v>
       </c>
       <c r="AI22" t="s">
-        <v>981</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -9691,13 +9913,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>1492</v>
+        <v>1561</v>
       </c>
       <c r="D23" t="s">
-        <v>1589</v>
+        <v>1598</v>
       </c>
       <c r="E23" t="s">
-        <v>1588</v>
+        <v>1683</v>
       </c>
       <c r="G23" t="s">
         <v>706</v>
@@ -9709,7 +9931,7 @@
         <v>307</v>
       </c>
       <c r="T23" t="s">
-        <v>1587</v>
+        <v>1681</v>
       </c>
       <c r="U23" t="s">
         <v>1516</v>
@@ -9718,13 +9940,13 @@
         <v>1535</v>
       </c>
       <c r="W23" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="X23" t="s">
         <v>1373</v>
       </c>
       <c r="Y23" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="Z23" t="s">
         <v>1385</v>
@@ -9736,7 +9958,7 @@
         <v>1414</v>
       </c>
       <c r="AC23" t="s">
-        <v>1476</v>
+        <v>1682</v>
       </c>
       <c r="AD23" t="s">
         <v>1408</v>
@@ -9748,13 +9970,13 @@
         <v>1477</v>
       </c>
       <c r="AG23" t="s">
-        <v>1409</v>
+        <v>1640</v>
       </c>
       <c r="AH23" t="s">
-        <v>809</v>
+        <v>1669</v>
       </c>
       <c r="AI23" t="s">
-        <v>1492</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -9765,13 +9987,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>1592</v>
+        <v>829</v>
       </c>
       <c r="D24" t="s">
-        <v>1050</v>
+        <v>1686</v>
       </c>
       <c r="E24" t="s">
-        <v>1593</v>
+        <v>1685</v>
       </c>
       <c r="G24" t="s">
         <v>452</v>
@@ -9786,7 +10008,7 @@
         <v>1590</v>
       </c>
       <c r="U24" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="V24" t="s">
         <v>1372</v>
@@ -9807,10 +10029,10 @@
         <v>1385</v>
       </c>
       <c r="AB24" t="s">
-        <v>1469</v>
+        <v>1677</v>
       </c>
       <c r="AC24" t="s">
-        <v>1591</v>
+        <v>1684</v>
       </c>
       <c r="AD24" t="s">
         <v>1388</v>
@@ -9828,7 +10050,7 @@
         <v>1428</v>
       </c>
       <c r="AI24" t="s">
-        <v>1592</v>
+        <v>829</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -9839,13 +10061,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>874</v>
+        <v>844</v>
       </c>
       <c r="D25" t="s">
-        <v>860</v>
+        <v>1005</v>
       </c>
       <c r="E25" t="s">
-        <v>1594</v>
+        <v>1687</v>
       </c>
       <c r="G25" t="s">
         <v>578</v>
@@ -9866,7 +10088,7 @@
         <v>707</v>
       </c>
       <c r="W25" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="X25" t="s">
         <v>1373</v>
@@ -9875,13 +10097,13 @@
         <v>1376</v>
       </c>
       <c r="Z25" t="s">
-        <v>1537</v>
+        <v>1132</v>
       </c>
       <c r="AA25" t="s">
         <v>1457</v>
       </c>
       <c r="AB25" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AC25" t="s">
         <v>1414</v>
@@ -9899,10 +10121,10 @@
         <v>1420</v>
       </c>
       <c r="AH25" t="s">
-        <v>1421</v>
+        <v>751</v>
       </c>
       <c r="AI25" t="s">
-        <v>874</v>
+        <v>844</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -9913,13 +10135,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>1524</v>
+        <v>1564</v>
       </c>
       <c r="D26" t="s">
-        <v>1596</v>
+        <v>1583</v>
       </c>
       <c r="E26" t="s">
-        <v>1595</v>
+        <v>1688</v>
       </c>
       <c r="G26" t="s">
         <v>653</v>
@@ -9937,7 +10159,7 @@
         <v>1381</v>
       </c>
       <c r="V26" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W26" t="s">
         <v>1516</v>
@@ -9961,22 +10183,22 @@
         <v>1483</v>
       </c>
       <c r="AD26" t="s">
-        <v>1571</v>
+        <v>1639</v>
       </c>
       <c r="AE26" t="s">
         <v>1062</v>
       </c>
       <c r="AF26" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AG26" t="s">
         <v>1485</v>
       </c>
       <c r="AH26" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AI26" t="s">
-        <v>1524</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -9987,13 +10209,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>1558</v>
+        <v>923</v>
       </c>
       <c r="D27" t="s">
-        <v>1598</v>
+        <v>1690</v>
       </c>
       <c r="E27" t="s">
-        <v>1597</v>
+        <v>1689</v>
       </c>
       <c r="G27" t="s">
         <v>672</v>
@@ -10011,10 +10233,10 @@
         <v>1381</v>
       </c>
       <c r="V27" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W27" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="X27" t="s">
         <v>1552</v>
@@ -10029,7 +10251,7 @@
         <v>1545</v>
       </c>
       <c r="AB27" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AC27" t="s">
         <v>1414</v>
@@ -10044,13 +10266,13 @@
         <v>456</v>
       </c>
       <c r="AG27" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AH27" t="s">
         <v>1456</v>
       </c>
       <c r="AI27" t="s">
-        <v>1558</v>
+        <v>923</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -10061,13 +10283,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>1561</v>
+        <v>673</v>
       </c>
       <c r="D28" t="s">
-        <v>1601</v>
+        <v>1054</v>
       </c>
       <c r="E28" t="s">
-        <v>1600</v>
+        <v>1691</v>
       </c>
       <c r="G28" t="s">
         <v>452</v>
@@ -10079,16 +10301,16 @@
         <v>857</v>
       </c>
       <c r="T28" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="U28" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="V28" t="s">
         <v>1516</v>
       </c>
       <c r="W28" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="X28" t="s">
         <v>1552</v>
@@ -10103,7 +10325,7 @@
         <v>1373</v>
       </c>
       <c r="AB28" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="AC28" t="s">
         <v>1414</v>
@@ -10118,13 +10340,13 @@
         <v>1535</v>
       </c>
       <c r="AG28" t="s">
-        <v>1550</v>
+        <v>1645</v>
       </c>
       <c r="AH28" t="s">
         <v>1471</v>
       </c>
       <c r="AI28" t="s">
-        <v>1561</v>
+        <v>673</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -10135,13 +10357,13 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>988</v>
+        <v>1661</v>
       </c>
       <c r="D29" t="s">
-        <v>1604</v>
+        <v>1694</v>
       </c>
       <c r="E29" t="s">
-        <v>1603</v>
+        <v>1693</v>
       </c>
       <c r="G29" t="s">
         <v>706</v>
@@ -10156,19 +10378,19 @@
         <v>1062</v>
       </c>
       <c r="U29" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="V29" t="s">
         <v>1381</v>
       </c>
       <c r="W29" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="X29" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="Y29" t="s">
-        <v>1539</v>
+        <v>1632</v>
       </c>
       <c r="Z29" t="s">
         <v>1385</v>
@@ -10186,10 +10408,10 @@
         <v>1414</v>
       </c>
       <c r="AE29" t="s">
-        <v>1369</v>
+        <v>1628</v>
       </c>
       <c r="AF29" t="s">
-        <v>681</v>
+        <v>1065</v>
       </c>
       <c r="AG29" t="s">
         <v>1485</v>
@@ -10198,7 +10420,7 @@
         <v>1420</v>
       </c>
       <c r="AI29" t="s">
-        <v>988</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -10209,13 +10431,13 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>1564</v>
+        <v>1521</v>
       </c>
       <c r="D30" t="s">
-        <v>1606</v>
+        <v>1696</v>
       </c>
       <c r="E30" t="s">
-        <v>1605</v>
+        <v>1695</v>
       </c>
       <c r="G30" t="s">
         <v>930</v>
@@ -10230,13 +10452,13 @@
         <v>1489</v>
       </c>
       <c r="U30" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="V30" t="s">
         <v>694</v>
       </c>
       <c r="W30" t="s">
-        <v>1500</v>
+        <v>1635</v>
       </c>
       <c r="X30" t="s">
         <v>1545</v>
@@ -10263,16 +10485,16 @@
         <v>1062</v>
       </c>
       <c r="AF30" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AG30" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AH30" t="s">
         <v>1574</v>
       </c>
       <c r="AI30" t="s">
-        <v>1564</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -10283,13 +10505,13 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>1399</v>
+        <v>1518</v>
       </c>
       <c r="D31" t="s">
-        <v>1608</v>
+        <v>1043</v>
       </c>
       <c r="E31" t="s">
-        <v>1607</v>
+        <v>1697</v>
       </c>
       <c r="G31" t="s">
         <v>706</v>
@@ -10304,10 +10526,10 @@
         <v>1489</v>
       </c>
       <c r="U31" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="V31" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="W31" t="s">
         <v>1497</v>
@@ -10322,7 +10544,7 @@
         <v>1375</v>
       </c>
       <c r="AA31" t="s">
-        <v>1537</v>
+        <v>1132</v>
       </c>
       <c r="AB31" t="s">
         <v>1424</v>
@@ -10337,16 +10559,16 @@
         <v>1062</v>
       </c>
       <c r="AF31" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AG31" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AH31" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AI31" t="s">
-        <v>1399</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -10357,13 +10579,13 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
       <c r="D32" t="s">
-        <v>1610</v>
+        <v>1699</v>
       </c>
       <c r="E32" t="s">
-        <v>1609</v>
+        <v>1698</v>
       </c>
       <c r="G32" t="s">
         <v>706</v>
@@ -10381,19 +10603,19 @@
         <v>1381</v>
       </c>
       <c r="V32" t="s">
-        <v>1441</v>
+        <v>1656</v>
       </c>
       <c r="W32" t="s">
         <v>694</v>
       </c>
       <c r="X32" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="Y32" t="s">
         <v>1545</v>
       </c>
       <c r="Z32" t="s">
-        <v>1537</v>
+        <v>1132</v>
       </c>
       <c r="AA32" t="s">
         <v>1385</v>
@@ -10402,7 +10624,7 @@
         <v>1389</v>
       </c>
       <c r="AC32" t="s">
-        <v>1569</v>
+        <v>1665</v>
       </c>
       <c r="AD32" t="s">
         <v>1414</v>
@@ -10411,16 +10633,16 @@
         <v>1062</v>
       </c>
       <c r="AF32" t="s">
-        <v>1555</v>
+        <v>1650</v>
       </c>
       <c r="AG32" t="s">
-        <v>1540</v>
+        <v>691</v>
       </c>
       <c r="AH32" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AI32" t="s">
-        <v>1518</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -10431,13 +10653,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>1129</v>
+        <v>844</v>
       </c>
       <c r="D33" t="s">
-        <v>1612</v>
+        <v>1694</v>
       </c>
       <c r="E33" t="s">
-        <v>1611</v>
+        <v>1701</v>
       </c>
       <c r="G33" t="s">
         <v>452</v>
@@ -10452,7 +10674,7 @@
         <v>1489</v>
       </c>
       <c r="U33" t="s">
-        <v>1402</v>
+        <v>1638</v>
       </c>
       <c r="V33" t="s">
         <v>1516</v>
@@ -10470,13 +10692,13 @@
         <v>1385</v>
       </c>
       <c r="AA33" t="s">
-        <v>1484</v>
+        <v>1700</v>
       </c>
       <c r="AB33" t="s">
         <v>1470</v>
       </c>
       <c r="AC33" t="s">
-        <v>1571</v>
+        <v>1639</v>
       </c>
       <c r="AD33" t="s">
         <v>1414</v>
@@ -10485,16 +10707,16 @@
         <v>1062</v>
       </c>
       <c r="AF33" t="s">
-        <v>1613</v>
+        <v>1629</v>
       </c>
       <c r="AG33" t="s">
         <v>1485</v>
       </c>
       <c r="AH33" t="s">
-        <v>1579</v>
+        <v>817</v>
       </c>
       <c r="AI33" t="s">
-        <v>1129</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FPL6 n RoC gw12 final
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9276" uniqueCount="2260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9805" uniqueCount="2285">
   <si>
     <t>Places</t>
   </si>
@@ -6814,6 +6814,81 @@
   </si>
   <si>
     <t>124,613</t>
+  </si>
+  <si>
+    <t>1,090,368</t>
+  </si>
+  <si>
+    <t>59,274</t>
+  </si>
+  <si>
+    <t>107,662</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>485,877</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>1,054,867</t>
+  </si>
+  <si>
+    <t>714</t>
+  </si>
+  <si>
+    <t>2,390,108</t>
+  </si>
+  <si>
+    <t>2,365,757</t>
+  </si>
+  <si>
+    <t>Salah 16</t>
+  </si>
+  <si>
+    <t>5,249,908</t>
+  </si>
+  <si>
+    <t>549</t>
+  </si>
+  <si>
+    <t>525,763</t>
+  </si>
+  <si>
+    <t>Dallas 4</t>
+  </si>
+  <si>
+    <t>2,249,557</t>
+  </si>
+  <si>
+    <t>664</t>
+  </si>
+  <si>
+    <t>3,381,220</t>
+  </si>
+  <si>
+    <t>1,607,980</t>
+  </si>
+  <si>
+    <t>5,377,966</t>
+  </si>
+  <si>
+    <t>544</t>
+  </si>
+  <si>
+    <t>5,737,708</t>
+  </si>
+  <si>
+    <t>Ronaldo 10</t>
+  </si>
+  <si>
+    <t>7,675,436</t>
+  </si>
+  <si>
+    <t>391</t>
   </si>
 </sst>
 </file>
@@ -7659,16 +7734,16 @@
     <col min="21" max="21" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.8359375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="11.40625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.48828125" collapsed="true"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="12.2734375" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
@@ -7794,13 +7869,13 @@
         <v>5695560</v>
       </c>
       <c r="C2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D2" t="s">
-        <v>1400</v>
+        <v>2060</v>
       </c>
       <c r="E2" t="s">
-        <v>2104</v>
+        <v>2260</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -7815,40 +7890,40 @@
         <v>2101</v>
       </c>
       <c r="U2" t="s">
-        <v>2102</v>
+        <v>2220</v>
       </c>
       <c r="V2" t="s">
         <v>1911</v>
       </c>
       <c r="W2" t="s">
-        <v>687</v>
+        <v>1856</v>
       </c>
       <c r="X2" t="s">
+        <v>2103</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA2" t="s">
         <v>2050</v>
       </c>
-      <c r="Y2" t="s">
-        <v>2103</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>738</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>383</v>
-      </c>
       <c r="AB2" t="s">
+        <v>894</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD2" t="s">
         <v>1496</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>894</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>682</v>
       </c>
       <c r="AE2" t="s">
         <v>880</v>
       </c>
       <c r="AF2" t="s">
-        <v>1856</v>
+        <v>687</v>
       </c>
       <c r="AG2" t="s">
         <v>2056</v>
@@ -7857,7 +7932,7 @@
         <v>881</v>
       </c>
       <c r="AI2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -7868,13 +7943,13 @@
         <v>1153704</v>
       </c>
       <c r="C3" t="s">
-        <v>1571</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s">
-        <v>2108</v>
+        <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>2107</v>
+        <v>2261</v>
       </c>
       <c r="G3" t="s">
         <v>672</v>
@@ -7889,7 +7964,7 @@
         <v>2039</v>
       </c>
       <c r="U3" t="s">
-        <v>2105</v>
+        <v>2214</v>
       </c>
       <c r="V3" t="s">
         <v>2048</v>
@@ -7898,40 +7973,40 @@
         <v>1894</v>
       </c>
       <c r="X3" t="s">
-        <v>687</v>
+        <v>425</v>
       </c>
       <c r="Y3" t="s">
-        <v>1214</v>
+        <v>817</v>
       </c>
       <c r="Z3" t="s">
         <v>1428</v>
       </c>
       <c r="AA3" t="s">
+        <v>2050</v>
+      </c>
+      <c r="AB3" t="s">
         <v>2106</v>
       </c>
-      <c r="AB3" t="s">
-        <v>2050</v>
-      </c>
       <c r="AC3" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD3" t="s">
         <v>1268</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>682</v>
       </c>
       <c r="AE3" t="s">
         <v>2031</v>
       </c>
       <c r="AF3" t="s">
-        <v>425</v>
+        <v>687</v>
       </c>
       <c r="AG3" t="s">
-        <v>817</v>
+        <v>1214</v>
       </c>
       <c r="AH3" t="s">
         <v>532</v>
       </c>
       <c r="AI3" t="s">
-        <v>1571</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -7942,13 +8017,13 @@
         <v>440807</v>
       </c>
       <c r="C4" t="s">
-        <v>1510</v>
+        <v>1571</v>
       </c>
       <c r="D4" t="s">
-        <v>1361</v>
+        <v>1463</v>
       </c>
       <c r="E4" t="s">
-        <v>2111</v>
+        <v>2230</v>
       </c>
       <c r="G4" t="s">
         <v>706</v>
@@ -7963,40 +8038,40 @@
         <v>2109</v>
       </c>
       <c r="U4" t="s">
-        <v>687</v>
+        <v>2065</v>
       </c>
       <c r="V4" t="s">
-        <v>2065</v>
+        <v>2216</v>
       </c>
       <c r="W4" t="s">
+        <v>1859</v>
+      </c>
+      <c r="X4" t="s">
         <v>2036</v>
       </c>
-      <c r="X4" t="s">
-        <v>2110</v>
-      </c>
       <c r="Y4" t="s">
-        <v>1859</v>
+        <v>425</v>
       </c>
       <c r="Z4" t="s">
+        <v>2028</v>
+      </c>
+      <c r="AA4" t="s">
         <v>1220</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>2050</v>
       </c>
-      <c r="AB4" t="s">
-        <v>2028</v>
-      </c>
       <c r="AC4" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD4" t="s">
         <v>1417</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>682</v>
       </c>
       <c r="AE4" t="s">
         <v>2039</v>
       </c>
       <c r="AF4" t="s">
-        <v>425</v>
+        <v>687</v>
       </c>
       <c r="AG4" t="s">
         <v>2106</v>
@@ -8005,7 +8080,7 @@
         <v>1496</v>
       </c>
       <c r="AI4" t="s">
-        <v>1510</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -8016,13 +8091,13 @@
         <v>4642646</v>
       </c>
       <c r="C5" t="s">
-        <v>1810</v>
+        <v>1264</v>
       </c>
       <c r="D5" t="s">
-        <v>1531</v>
+        <v>2263</v>
       </c>
       <c r="E5" t="s">
-        <v>2113</v>
+        <v>2262</v>
       </c>
       <c r="G5" t="s">
         <v>653</v>
@@ -8037,28 +8112,28 @@
         <v>2031</v>
       </c>
       <c r="U5" t="s">
+        <v>2048</v>
+      </c>
+      <c r="V5" t="s">
         <v>2049</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1859</v>
       </c>
-      <c r="W5" t="s">
-        <v>2105</v>
-      </c>
       <c r="X5" t="s">
-        <v>2048</v>
+        <v>2214</v>
       </c>
       <c r="Y5" t="s">
+        <v>2036</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA5" t="s">
         <v>2050</v>
       </c>
-      <c r="Z5" t="s">
-        <v>1408</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>738</v>
-      </c>
       <c r="AB5" t="s">
-        <v>2112</v>
+        <v>425</v>
       </c>
       <c r="AC5" t="s">
         <v>2075</v>
@@ -8073,13 +8148,13 @@
         <v>953</v>
       </c>
       <c r="AG5" t="s">
-        <v>425</v>
+        <v>1408</v>
       </c>
       <c r="AH5" t="s">
-        <v>2036</v>
+        <v>2112</v>
       </c>
       <c r="AI5" t="s">
-        <v>1810</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -8090,13 +8165,13 @@
         <v>1364835</v>
       </c>
       <c r="C6" t="s">
-        <v>653</v>
+        <v>1264</v>
       </c>
       <c r="D6" t="s">
-        <v>2021</v>
+        <v>2265</v>
       </c>
       <c r="E6" t="s">
-        <v>2115</v>
+        <v>2264</v>
       </c>
       <c r="G6" t="s">
         <v>706</v>
@@ -8117,7 +8192,7 @@
         <v>2048</v>
       </c>
       <c r="W6" t="s">
-        <v>2105</v>
+        <v>2214</v>
       </c>
       <c r="X6" t="s">
         <v>1932</v>
@@ -8153,7 +8228,7 @@
         <v>2067</v>
       </c>
       <c r="AI6" t="s">
-        <v>653</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -8164,13 +8239,13 @@
         <v>5306515</v>
       </c>
       <c r="C7" t="s">
-        <v>703</v>
+        <v>1260</v>
       </c>
       <c r="D7" t="s">
-        <v>2012</v>
+        <v>2267</v>
       </c>
       <c r="E7" t="s">
-        <v>2117</v>
+        <v>2266</v>
       </c>
       <c r="G7" t="s">
         <v>706</v>
@@ -8185,49 +8260,49 @@
         <v>2042</v>
       </c>
       <c r="U7" t="s">
+        <v>1859</v>
+      </c>
+      <c r="V7" t="s">
+        <v>2049</v>
+      </c>
+      <c r="W7" t="s">
         <v>950</v>
       </c>
-      <c r="V7" t="s">
-        <v>687</v>
-      </c>
-      <c r="W7" t="s">
-        <v>2049</v>
-      </c>
       <c r="X7" t="s">
-        <v>1859</v>
+        <v>2038</v>
       </c>
       <c r="Y7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="Z7" t="s">
         <v>738</v>
       </c>
-      <c r="Z7" t="s">
-        <v>2116</v>
-      </c>
       <c r="AA7" t="s">
-        <v>953</v>
+        <v>2028</v>
       </c>
       <c r="AB7" t="s">
-        <v>2028</v>
+        <v>817</v>
       </c>
       <c r="AC7" t="s">
+        <v>2051</v>
+      </c>
+      <c r="AD7" t="s">
         <v>682</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>2112</v>
       </c>
       <c r="AE7" t="s">
         <v>2101</v>
       </c>
       <c r="AF7" t="s">
-        <v>2051</v>
+        <v>687</v>
       </c>
       <c r="AG7" t="s">
-        <v>2038</v>
+        <v>953</v>
       </c>
       <c r="AH7" t="s">
-        <v>817</v>
+        <v>2112</v>
       </c>
       <c r="AI7" t="s">
-        <v>703</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -8238,13 +8313,13 @@
         <v>2249991</v>
       </c>
       <c r="C8" t="s">
-        <v>1510</v>
+        <v>703</v>
       </c>
       <c r="D8" t="s">
-        <v>2119</v>
+        <v>1379</v>
       </c>
       <c r="E8" t="s">
-        <v>2118</v>
+        <v>2268</v>
       </c>
       <c r="G8" t="s">
         <v>672</v>
@@ -8256,52 +8331,52 @@
         <v>898</v>
       </c>
       <c r="T8" t="s">
-        <v>1930</v>
+        <v>2101</v>
       </c>
       <c r="U8" t="s">
+        <v>1932</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1894</v>
+      </c>
+      <c r="W8" t="s">
         <v>1859</v>
       </c>
-      <c r="V8" t="s">
-        <v>1932</v>
-      </c>
-      <c r="W8" t="s">
-        <v>1894</v>
-      </c>
       <c r="X8" t="s">
-        <v>687</v>
+        <v>805</v>
       </c>
       <c r="Y8" t="s">
+        <v>1860</v>
+      </c>
+      <c r="Z8" t="s">
         <v>977</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>1860</v>
       </c>
       <c r="AA8" t="s">
         <v>2050</v>
       </c>
       <c r="AB8" t="s">
+        <v>2030</v>
+      </c>
+      <c r="AC8" t="s">
         <v>682</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>2030</v>
       </c>
       <c r="AD8" t="s">
         <v>2051</v>
       </c>
       <c r="AE8" t="s">
-        <v>2101</v>
+        <v>1930</v>
       </c>
       <c r="AF8" t="s">
-        <v>805</v>
+        <v>687</v>
       </c>
       <c r="AG8" t="s">
-        <v>2110</v>
+        <v>2216</v>
       </c>
       <c r="AH8" t="s">
         <v>2028</v>
       </c>
       <c r="AI8" t="s">
-        <v>1510</v>
+        <v>703</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -8312,13 +8387,13 @@
         <v>2056865</v>
       </c>
       <c r="C9" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="D9" t="s">
-        <v>2123</v>
+        <v>1366</v>
       </c>
       <c r="E9" t="s">
-        <v>2122</v>
+        <v>2269</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -8333,10 +8408,10 @@
         <v>1216</v>
       </c>
       <c r="U9" t="s">
+        <v>2120</v>
+      </c>
+      <c r="V9" t="s">
         <v>2048</v>
-      </c>
-      <c r="V9" t="s">
-        <v>687</v>
       </c>
       <c r="W9" t="s">
         <v>2049</v>
@@ -8345,28 +8420,28 @@
         <v>2028</v>
       </c>
       <c r="Y9" t="s">
+        <v>2114</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>1860</v>
+      </c>
+      <c r="AB9" t="s">
         <v>2061</v>
       </c>
-      <c r="Z9" t="s">
-        <v>2114</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>425</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>1860</v>
-      </c>
       <c r="AC9" t="s">
+        <v>900</v>
+      </c>
+      <c r="AD9" t="s">
         <v>1417</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>900</v>
       </c>
       <c r="AE9" t="s">
         <v>2031</v>
       </c>
       <c r="AF9" t="s">
-        <v>2120</v>
+        <v>687</v>
       </c>
       <c r="AG9" t="s">
         <v>1253</v>
@@ -8375,7 +8450,7 @@
         <v>2121</v>
       </c>
       <c r="AI9" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -8386,13 +8461,13 @@
         <v>5142355</v>
       </c>
       <c r="C10" t="s">
-        <v>844</v>
+        <v>268</v>
       </c>
       <c r="D10" t="s">
-        <v>2128</v>
+        <v>2272</v>
       </c>
       <c r="E10" t="s">
-        <v>2127</v>
+        <v>2271</v>
       </c>
       <c r="G10" t="s">
         <v>653</v>
@@ -8407,49 +8482,49 @@
         <v>2072</v>
       </c>
       <c r="U10" t="s">
+        <v>2126</v>
+      </c>
+      <c r="V10" t="s">
+        <v>2216</v>
+      </c>
+      <c r="W10" t="s">
         <v>2038</v>
       </c>
-      <c r="V10" t="s">
-        <v>2110</v>
-      </c>
-      <c r="W10" t="s">
-        <v>687</v>
-      </c>
       <c r="X10" t="s">
+        <v>1956</v>
+      </c>
+      <c r="Y10" t="s">
         <v>805</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>2061</v>
       </c>
       <c r="Z10" t="s">
         <v>413</v>
       </c>
       <c r="AA10" t="s">
-        <v>2124</v>
+        <v>2270</v>
       </c>
       <c r="AB10" t="s">
+        <v>2030</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>2125</v>
+      </c>
+      <c r="AD10" t="s">
         <v>1419</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>2030</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>2125</v>
       </c>
       <c r="AE10" t="s">
         <v>570</v>
       </c>
       <c r="AF10" t="s">
-        <v>2126</v>
+        <v>687</v>
       </c>
       <c r="AG10" t="s">
         <v>1224</v>
       </c>
       <c r="AH10" t="s">
-        <v>1956</v>
+        <v>2124</v>
       </c>
       <c r="AI10" t="s">
-        <v>844</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -8460,13 +8535,13 @@
         <v>1628438</v>
       </c>
       <c r="C11" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="D11" t="s">
-        <v>2130</v>
+        <v>1451</v>
       </c>
       <c r="E11" t="s">
-        <v>2129</v>
+        <v>2273</v>
       </c>
       <c r="G11" t="s">
         <v>452</v>
@@ -8481,7 +8556,7 @@
         <v>2040</v>
       </c>
       <c r="U11" t="s">
-        <v>687</v>
+        <v>2065</v>
       </c>
       <c r="V11" t="s">
         <v>1859</v>
@@ -8490,40 +8565,40 @@
         <v>2049</v>
       </c>
       <c r="X11" t="s">
-        <v>2065</v>
+        <v>1932</v>
       </c>
       <c r="Y11" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>738</v>
+      </c>
+      <c r="AA11" t="s">
         <v>2061</v>
       </c>
-      <c r="Z11" t="s">
-        <v>953</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>738</v>
-      </c>
       <c r="AB11" t="s">
-        <v>383</v>
+        <v>2067</v>
       </c>
       <c r="AC11" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AD11" t="s">
         <v>2033</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>1417</v>
       </c>
       <c r="AE11" t="s">
         <v>1930</v>
       </c>
       <c r="AF11" t="s">
-        <v>2067</v>
+        <v>687</v>
       </c>
       <c r="AG11" t="s">
-        <v>1932</v>
+        <v>953</v>
       </c>
       <c r="AH11" t="s">
         <v>2114</v>
       </c>
       <c r="AI11" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -8534,13 +8609,13 @@
         <v>1427447</v>
       </c>
       <c r="C12" t="s">
-        <v>703</v>
+        <v>1558</v>
       </c>
       <c r="D12" t="s">
-        <v>2133</v>
+        <v>2276</v>
       </c>
       <c r="E12" t="s">
-        <v>2132</v>
+        <v>2275</v>
       </c>
       <c r="G12" t="s">
         <v>653</v>
@@ -8561,22 +8636,22 @@
         <v>538</v>
       </c>
       <c r="W12" t="s">
-        <v>687</v>
+        <v>2214</v>
       </c>
       <c r="X12" t="s">
-        <v>2105</v>
+        <v>1253</v>
       </c>
       <c r="Y12" t="s">
+        <v>2274</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>977</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>738</v>
+      </c>
+      <c r="AB12" t="s">
         <v>2050</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>953</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>977</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>738</v>
       </c>
       <c r="AC12" t="s">
         <v>2030</v>
@@ -8588,16 +8663,16 @@
         <v>2031</v>
       </c>
       <c r="AF12" t="s">
-        <v>2131</v>
+        <v>687</v>
       </c>
       <c r="AG12" t="s">
-        <v>1253</v>
+        <v>953</v>
       </c>
       <c r="AH12" t="s">
         <v>2067</v>
       </c>
       <c r="AI12" t="s">
-        <v>703</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -8614,7 +8689,7 @@
         <v>2136</v>
       </c>
       <c r="E13" t="s">
-        <v>2135</v>
+        <v>2277</v>
       </c>
       <c r="G13" t="s">
         <v>706</v>
@@ -8682,13 +8757,13 @@
         <v>3452385</v>
       </c>
       <c r="C14" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
       <c r="D14" t="s">
-        <v>2141</v>
+        <v>1376</v>
       </c>
       <c r="E14" t="s">
-        <v>2140</v>
+        <v>2278</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -8706,7 +8781,7 @@
         <v>2049</v>
       </c>
       <c r="V14" t="s">
-        <v>2102</v>
+        <v>2220</v>
       </c>
       <c r="W14" t="s">
         <v>2043</v>
@@ -8736,7 +8811,7 @@
         <v>923</v>
       </c>
       <c r="AF14" t="s">
-        <v>2138</v>
+        <v>2226</v>
       </c>
       <c r="AG14" t="s">
         <v>685</v>
@@ -8745,7 +8820,7 @@
         <v>2139</v>
       </c>
       <c r="AI14" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -8756,13 +8831,13 @@
         <v>2297330</v>
       </c>
       <c r="C15" t="s">
-        <v>778</v>
+        <v>288</v>
       </c>
       <c r="D15" t="s">
-        <v>936</v>
+        <v>2280</v>
       </c>
       <c r="E15" t="s">
-        <v>2147</v>
+        <v>2279</v>
       </c>
       <c r="G15" t="s">
         <v>452</v>
@@ -8777,49 +8852,49 @@
         <v>581</v>
       </c>
       <c r="U15" t="s">
+        <v>2220</v>
+      </c>
+      <c r="V15" t="s">
+        <v>2146</v>
+      </c>
+      <c r="W15" t="s">
         <v>2142</v>
       </c>
-      <c r="V15" t="s">
-        <v>1430</v>
-      </c>
-      <c r="W15" t="s">
-        <v>2102</v>
-      </c>
       <c r="X15" t="s">
+        <v>805</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>2143</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA15" t="s">
         <v>383</v>
       </c>
-      <c r="Y15" t="s">
-        <v>969</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>2143</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>425</v>
-      </c>
       <c r="AB15" t="s">
+        <v>2144</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>2033</v>
+      </c>
+      <c r="AD15" t="s">
         <v>1268</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>2144</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>2033</v>
       </c>
       <c r="AE15" t="s">
         <v>2145</v>
       </c>
       <c r="AF15" t="s">
-        <v>805</v>
+        <v>969</v>
       </c>
       <c r="AG15" t="s">
-        <v>2146</v>
+        <v>1430</v>
       </c>
       <c r="AH15" t="s">
         <v>2036</v>
       </c>
       <c r="AI15" t="s">
-        <v>778</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -8836,7 +8911,7 @@
         <v>2153</v>
       </c>
       <c r="E16" t="s">
-        <v>2152</v>
+        <v>2281</v>
       </c>
       <c r="G16" t="s">
         <v>653</v>
@@ -8904,13 +8979,13 @@
         <v>5344757</v>
       </c>
       <c r="C17" t="s">
-        <v>268</v>
+        <v>301</v>
       </c>
       <c r="D17" t="s">
-        <v>2158</v>
+        <v>2284</v>
       </c>
       <c r="E17" t="s">
-        <v>2157</v>
+        <v>2283</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
@@ -8934,40 +9009,40 @@
         <v>1911</v>
       </c>
       <c r="X17" t="s">
+        <v>2155</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>2156</v>
+      </c>
+      <c r="Z17" t="s">
         <v>1505</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AA17" t="s">
         <v>1984</v>
       </c>
-      <c r="Z17" t="s">
-        <v>969</v>
-      </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>2028</v>
       </c>
-      <c r="AB17" t="s">
-        <v>1200</v>
-      </c>
       <c r="AC17" t="s">
-        <v>2030</v>
+        <v>2282</v>
       </c>
       <c r="AD17" t="s">
-        <v>1354</v>
+        <v>2067</v>
       </c>
       <c r="AE17" t="s">
         <v>2031</v>
       </c>
       <c r="AF17" t="s">
-        <v>2155</v>
+        <v>969</v>
       </c>
       <c r="AG17" t="s">
-        <v>2156</v>
+        <v>1200</v>
       </c>
       <c r="AH17" t="s">
-        <v>2067</v>
+        <v>1354</v>
       </c>
       <c r="AI17" t="s">
-        <v>268</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
punkte prev nachste button addition
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12344" uniqueCount="2457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14437" uniqueCount="2544">
   <si>
     <t>Places</t>
   </si>
@@ -7405,6 +7405,267 @@
   </si>
   <si>
     <t>841</t>
+  </si>
+  <si>
+    <t>Elyounoussi 0</t>
+  </si>
+  <si>
+    <t>963</t>
+  </si>
+  <si>
+    <t>A.Armstrong 2</t>
+  </si>
+  <si>
+    <t>973</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>951</t>
+  </si>
+  <si>
+    <t>Broja 2</t>
+  </si>
+  <si>
+    <t>387</t>
+  </si>
+  <si>
+    <t>928</t>
+  </si>
+  <si>
+    <t>Sá 10</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>936</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>937</t>
+  </si>
+  <si>
+    <t>Lamptey 8</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>938</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>923</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>355</t>
+  </si>
+  <si>
+    <t>929</t>
+  </si>
+  <si>
+    <t>374</t>
+  </si>
+  <si>
+    <t>601</t>
+  </si>
+  <si>
+    <t>924</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>931</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>Trossard 3</t>
+  </si>
+  <si>
+    <t>1,493</t>
+  </si>
+  <si>
+    <t>914</t>
+  </si>
+  <si>
+    <t>2,094</t>
+  </si>
+  <si>
+    <t>910</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1,976</t>
+  </si>
+  <si>
+    <t>998</t>
+  </si>
+  <si>
+    <t>918</t>
+  </si>
+  <si>
+    <t>478</t>
+  </si>
+  <si>
+    <t>926</t>
+  </si>
+  <si>
+    <t>1,349</t>
+  </si>
+  <si>
+    <t>915</t>
+  </si>
+  <si>
+    <t>487</t>
+  </si>
+  <si>
+    <t>1,962</t>
+  </si>
+  <si>
+    <t>1,149</t>
+  </si>
+  <si>
+    <t>917</t>
+  </si>
+  <si>
+    <t>2,849</t>
+  </si>
+  <si>
+    <t>906</t>
+  </si>
+  <si>
+    <t>899</t>
+  </si>
+  <si>
+    <t>2,640</t>
+  </si>
+  <si>
+    <t>907</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>927</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>930</t>
+  </si>
+  <si>
+    <t>5,744</t>
+  </si>
+  <si>
+    <t>896</t>
+  </si>
+  <si>
+    <t>1,551</t>
+  </si>
+  <si>
+    <t>913</t>
+  </si>
+  <si>
+    <t>966</t>
+  </si>
+  <si>
+    <t>919</t>
+  </si>
+  <si>
+    <t>720</t>
+  </si>
+  <si>
+    <t>367</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>753</t>
+  </si>
+  <si>
+    <t>921</t>
+  </si>
+  <si>
+    <t>Saïss 6</t>
+  </si>
+  <si>
+    <t>356,740</t>
+  </si>
+  <si>
+    <t>Semedo 5</t>
+  </si>
+  <si>
+    <t>Trincão 3</t>
+  </si>
+  <si>
+    <t>844,168</t>
+  </si>
+  <si>
+    <t>Wilson 2</t>
+  </si>
+  <si>
+    <t>1,282,848</t>
+  </si>
+  <si>
+    <t>1,622,046</t>
+  </si>
+  <si>
+    <t>Cash 1</t>
+  </si>
+  <si>
+    <t>2,744,060</t>
+  </si>
+  <si>
+    <t>673</t>
+  </si>
+  <si>
+    <t>El Ghazi 4</t>
+  </si>
+  <si>
+    <t>Hoever 1</t>
+  </si>
+  <si>
+    <t>2,357,088</t>
+  </si>
+  <si>
+    <t>688</t>
+  </si>
+  <si>
+    <t>Dunk 6</t>
+  </si>
+  <si>
+    <t>2,487,603</t>
+  </si>
+  <si>
+    <t>4,299,273</t>
+  </si>
+  <si>
+    <t>611</t>
   </si>
 </sst>
 </file>
@@ -10494,10 +10755,10 @@
     <col min="20" max="20" bestFit="true" customWidth="true" width="19.1796875" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="21.71875" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="18.8046875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="21.2578125" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="15.64453125" collapsed="true"/>
@@ -25131,19 +25392,19 @@
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.69921875" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="19.1796875" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="16.71875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.55078125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="17.828125" collapsed="true"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.91015625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="21.09375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="15.64453125" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="16.65234375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="18.70703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="17.515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.60546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="16.71875" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -25268,13 +25529,13 @@
         <v>1694</v>
       </c>
       <c r="C2" t="s">
-        <v>706</v>
+        <v>2246</v>
       </c>
       <c r="D2" t="s">
-        <v>2140</v>
+        <v>2487</v>
       </c>
       <c r="E2" t="s">
-        <v>2139</v>
+        <v>2486</v>
       </c>
       <c r="G2" t="s">
         <v>452</v>
@@ -25286,7 +25547,7 @@
         <v>1693</v>
       </c>
       <c r="T2" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U2" t="s">
         <v>2248</v>
@@ -25295,22 +25556,22 @@
         <v>2249</v>
       </c>
       <c r="W2" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X2" t="s">
         <v>2280</v>
       </c>
       <c r="Y2" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z2" t="s">
         <v>2309</v>
       </c>
       <c r="AA2" t="s">
-        <v>2352</v>
+        <v>2485</v>
       </c>
       <c r="AB2" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AC2" t="s">
         <v>2300</v>
@@ -25322,16 +25583,16 @@
         <v>2271</v>
       </c>
       <c r="AF2" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AG2" t="s">
         <v>2332</v>
       </c>
       <c r="AH2" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI2" t="s">
-        <v>706</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -25342,13 +25603,13 @@
         <v>2123</v>
       </c>
       <c r="C3" t="s">
-        <v>653</v>
+        <v>2418</v>
       </c>
       <c r="D3" t="s">
-        <v>1473</v>
+        <v>1580</v>
       </c>
       <c r="E3" t="s">
-        <v>2142</v>
+        <v>2526</v>
       </c>
       <c r="G3" t="s">
         <v>706</v>
@@ -25372,16 +25633,16 @@
         <v>565</v>
       </c>
       <c r="X3" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Y3" t="s">
         <v>2298</v>
       </c>
       <c r="Z3" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA3" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AB3" t="s">
         <v>2254</v>
@@ -25390,22 +25651,22 @@
         <v>2294</v>
       </c>
       <c r="AD3" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE3" t="s">
         <v>2303</v>
       </c>
       <c r="AF3" t="s">
-        <v>2360</v>
+        <v>2525</v>
       </c>
       <c r="AG3" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH3" t="s">
-        <v>2272</v>
+        <v>2397</v>
       </c>
       <c r="AI3" t="s">
-        <v>653</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -25416,13 +25677,13 @@
         <v>2125</v>
       </c>
       <c r="C4" t="s">
-        <v>706</v>
+        <v>2384</v>
       </c>
       <c r="D4" t="s">
-        <v>2145</v>
+        <v>1855</v>
       </c>
       <c r="E4" t="s">
-        <v>2144</v>
+        <v>2529</v>
       </c>
       <c r="G4" t="s">
         <v>653</v>
@@ -25434,7 +25695,7 @@
         <v>2124</v>
       </c>
       <c r="T4" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="U4" t="s">
         <v>2283</v>
@@ -25443,7 +25704,7 @@
         <v>2291</v>
       </c>
       <c r="W4" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="X4" t="s">
         <v>565</v>
@@ -25452,10 +25713,10 @@
         <v>2276</v>
       </c>
       <c r="Z4" t="s">
-        <v>2316</v>
+        <v>2421</v>
       </c>
       <c r="AA4" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB4" t="s">
         <v>2318</v>
@@ -25464,22 +25725,22 @@
         <v>2294</v>
       </c>
       <c r="AD4" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AE4" t="s">
         <v>2361</v>
       </c>
       <c r="AF4" t="s">
-        <v>2362</v>
+        <v>2527</v>
       </c>
       <c r="AG4" t="s">
         <v>2256</v>
       </c>
       <c r="AH4" t="s">
-        <v>2363</v>
+        <v>2528</v>
       </c>
       <c r="AI4" t="s">
-        <v>706</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -25490,13 +25751,13 @@
         <v>2127</v>
       </c>
       <c r="C5" t="s">
-        <v>672</v>
+        <v>821</v>
       </c>
       <c r="D5" t="s">
-        <v>1856</v>
+        <v>1466</v>
       </c>
       <c r="E5" t="s">
-        <v>2147</v>
+        <v>2531</v>
       </c>
       <c r="G5" t="s">
         <v>653</v>
@@ -25508,25 +25769,25 @@
         <v>2126</v>
       </c>
       <c r="T5" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="U5" t="s">
-        <v>2342</v>
+        <v>1221</v>
       </c>
       <c r="V5" t="s">
         <v>2291</v>
       </c>
       <c r="W5" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="X5" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Y5" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Z5" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AA5" t="s">
         <v>2276</v>
@@ -25535,7 +25796,7 @@
         <v>2300</v>
       </c>
       <c r="AC5" t="s">
-        <v>1818</v>
+        <v>2530</v>
       </c>
       <c r="AD5" t="s">
         <v>2263</v>
@@ -25550,10 +25811,10 @@
         <v>2281</v>
       </c>
       <c r="AH5" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI5" t="s">
-        <v>672</v>
+        <v>821</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -25564,13 +25825,13 @@
         <v>2129</v>
       </c>
       <c r="C6" t="s">
-        <v>672</v>
+        <v>2428</v>
       </c>
       <c r="D6" t="s">
-        <v>1886</v>
+        <v>2410</v>
       </c>
       <c r="E6" t="s">
-        <v>2149</v>
+        <v>2532</v>
       </c>
       <c r="G6" t="s">
         <v>706</v>
@@ -25585,7 +25846,7 @@
         <v>2267</v>
       </c>
       <c r="U6" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="V6" t="s">
         <v>2248</v>
@@ -25594,10 +25855,10 @@
         <v>2249</v>
       </c>
       <c r="X6" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="Y6" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z6" t="s">
         <v>2293</v>
@@ -25606,13 +25867,13 @@
         <v>2276</v>
       </c>
       <c r="AB6" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AC6" t="s">
         <v>2321</v>
       </c>
       <c r="AD6" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AE6" t="s">
         <v>2364</v>
@@ -25624,10 +25885,10 @@
         <v>2264</v>
       </c>
       <c r="AH6" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI6" t="s">
-        <v>672</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -25638,13 +25899,13 @@
         <v>2131</v>
       </c>
       <c r="C7" t="s">
-        <v>861</v>
+        <v>2381</v>
       </c>
       <c r="D7" t="s">
-        <v>2154</v>
+        <v>2535</v>
       </c>
       <c r="E7" t="s">
-        <v>2153</v>
+        <v>2534</v>
       </c>
       <c r="G7" t="s">
         <v>653</v>
@@ -25656,19 +25917,19 @@
         <v>2130</v>
       </c>
       <c r="T7" t="s">
-        <v>2322</v>
+        <v>804</v>
       </c>
       <c r="U7" t="s">
         <v>2274</v>
       </c>
       <c r="V7" t="s">
-        <v>2365</v>
+        <v>2533</v>
       </c>
       <c r="W7" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="X7" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Y7" t="s">
         <v>721</v>
@@ -25683,13 +25944,13 @@
         <v>2254</v>
       </c>
       <c r="AC7" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD7" t="s">
         <v>2300</v>
       </c>
       <c r="AE7" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF7" t="s">
         <v>2366</v>
@@ -25701,7 +25962,7 @@
         <v>2367</v>
       </c>
       <c r="AI7" t="s">
-        <v>861</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -25712,13 +25973,13 @@
         <v>2133</v>
       </c>
       <c r="C8" t="s">
-        <v>653</v>
+        <v>712</v>
       </c>
       <c r="D8" t="s">
-        <v>2160</v>
+        <v>2539</v>
       </c>
       <c r="E8" t="s">
-        <v>2159</v>
+        <v>2538</v>
       </c>
       <c r="G8" t="s">
         <v>653</v>
@@ -25730,7 +25991,7 @@
         <v>2132</v>
       </c>
       <c r="T8" t="s">
-        <v>2259</v>
+        <v>2393</v>
       </c>
       <c r="U8" t="s">
         <v>2297</v>
@@ -25739,22 +26000,22 @@
         <v>2368</v>
       </c>
       <c r="W8" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X8" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Y8" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z8" t="s">
         <v>2369</v>
       </c>
       <c r="AA8" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AB8" t="s">
-        <v>2325</v>
+        <v>1414</v>
       </c>
       <c r="AC8" t="s">
         <v>2294</v>
@@ -25763,19 +26024,19 @@
         <v>2311</v>
       </c>
       <c r="AE8" t="s">
-        <v>2333</v>
+        <v>2242</v>
       </c>
       <c r="AF8" t="s">
-        <v>2370</v>
+        <v>2536</v>
       </c>
       <c r="AG8" t="s">
-        <v>2371</v>
+        <v>2537</v>
       </c>
       <c r="AH8" t="s">
         <v>2274</v>
       </c>
       <c r="AI8" t="s">
-        <v>653</v>
+        <v>712</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -25786,13 +26047,13 @@
         <v>2135</v>
       </c>
       <c r="C9" t="s">
-        <v>2376</v>
+        <v>841</v>
       </c>
       <c r="D9" t="s">
-        <v>2163</v>
+        <v>1393</v>
       </c>
       <c r="E9" t="s">
-        <v>2162</v>
+        <v>2541</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -25804,7 +26065,7 @@
         <v>2134</v>
       </c>
       <c r="T9" t="s">
-        <v>686</v>
+        <v>1498</v>
       </c>
       <c r="U9" t="s">
         <v>2372</v>
@@ -25816,16 +26077,16 @@
         <v>2374</v>
       </c>
       <c r="X9" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y9" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Z9" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA9" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB9" t="s">
         <v>721</v>
@@ -25840,16 +26101,16 @@
         <v>2299</v>
       </c>
       <c r="AF9" t="s">
-        <v>2375</v>
+        <v>2540</v>
       </c>
       <c r="AG9" t="s">
-        <v>2257</v>
+        <v>2390</v>
       </c>
       <c r="AH9" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI9" t="s">
-        <v>2376</v>
+        <v>841</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -25860,13 +26121,13 @@
         <v>2137</v>
       </c>
       <c r="C10" t="s">
-        <v>2379</v>
+        <v>712</v>
       </c>
       <c r="D10" t="s">
-        <v>2166</v>
+        <v>2543</v>
       </c>
       <c r="E10" t="s">
-        <v>2165</v>
+        <v>2542</v>
       </c>
       <c r="G10" t="s">
         <v>653</v>
@@ -25878,16 +26139,16 @@
         <v>2136</v>
       </c>
       <c r="T10" t="s">
-        <v>2333</v>
+        <v>2242</v>
       </c>
       <c r="U10" t="s">
         <v>2297</v>
       </c>
       <c r="V10" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W10" t="s">
-        <v>2375</v>
+        <v>2540</v>
       </c>
       <c r="X10" t="s">
         <v>2256</v>
@@ -25896,13 +26157,13 @@
         <v>2377</v>
       </c>
       <c r="Z10" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA10" t="s">
         <v>2250</v>
       </c>
       <c r="AB10" t="s">
-        <v>2340</v>
+        <v>2441</v>
       </c>
       <c r="AC10" t="s">
         <v>2254</v>
@@ -25911,7 +26172,7 @@
         <v>2311</v>
       </c>
       <c r="AE10" t="s">
-        <v>2259</v>
+        <v>2393</v>
       </c>
       <c r="AF10" t="s">
         <v>2293</v>
@@ -25923,7 +26184,7 @@
         <v>2304</v>
       </c>
       <c r="AI10" t="s">
-        <v>2379</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -26319,21 +26580,21 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="10.13671875" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.3671875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="15.08203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.32421875" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="24.359375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="18.73828125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="21.09375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="15.39453125" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="15.08203125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="18.70703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="18.70703125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="21.7734375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.859375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="16.859375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="17.515625" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -26458,13 +26719,13 @@
         <v>1601</v>
       </c>
       <c r="C2" t="s">
-        <v>861</v>
+        <v>829</v>
       </c>
       <c r="D2" t="s">
-        <v>2168</v>
+        <v>2458</v>
       </c>
       <c r="E2" t="s">
-        <v>2167</v>
+        <v>1863</v>
       </c>
       <c r="G2" t="s">
         <v>706</v>
@@ -26476,28 +26737,28 @@
         <v>1600</v>
       </c>
       <c r="T2" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U2" t="s">
         <v>2249</v>
       </c>
       <c r="V2" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W2" t="s">
         <v>2248</v>
       </c>
       <c r="X2" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="Y2" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Z2" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA2" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AB2" t="s">
         <v>2307</v>
@@ -26506,22 +26767,22 @@
         <v>2294</v>
       </c>
       <c r="AD2" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE2" t="s">
         <v>2271</v>
       </c>
       <c r="AF2" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AG2" t="s">
-        <v>2346</v>
+        <v>2457</v>
       </c>
       <c r="AH2" t="s">
-        <v>481</v>
+        <v>692</v>
       </c>
       <c r="AI2" t="s">
-        <v>861</v>
+        <v>829</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -26532,13 +26793,13 @@
         <v>1625</v>
       </c>
       <c r="C3" t="s">
-        <v>653</v>
+        <v>278</v>
       </c>
       <c r="D3" t="s">
-        <v>2170</v>
+        <v>2460</v>
       </c>
       <c r="E3" t="s">
-        <v>2169</v>
+        <v>861</v>
       </c>
       <c r="G3" t="s">
         <v>706</v>
@@ -26550,13 +26811,13 @@
         <v>1624</v>
       </c>
       <c r="T3" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U3" t="s">
         <v>2248</v>
       </c>
       <c r="V3" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W3" t="s">
         <v>2249</v>
@@ -26565,16 +26826,16 @@
         <v>2280</v>
       </c>
       <c r="Y3" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z3" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA3" t="s">
-        <v>2315</v>
+        <v>2377</v>
       </c>
       <c r="AB3" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AC3" t="s">
         <v>2311</v>
@@ -26589,13 +26850,13 @@
         <v>2293</v>
       </c>
       <c r="AG3" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH3" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI3" t="s">
-        <v>653</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -26606,13 +26867,13 @@
         <v>1655</v>
       </c>
       <c r="C4" t="s">
-        <v>706</v>
+        <v>1949</v>
       </c>
       <c r="D4" t="s">
-        <v>2171</v>
+        <v>2462</v>
       </c>
       <c r="E4" t="s">
-        <v>785</v>
+        <v>2461</v>
       </c>
       <c r="G4" t="s">
         <v>706</v>
@@ -26624,10 +26885,10 @@
         <v>1654</v>
       </c>
       <c r="T4" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U4" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V4" t="s">
         <v>2280</v>
@@ -26636,19 +26897,19 @@
         <v>2249</v>
       </c>
       <c r="X4" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Y4" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z4" t="s">
         <v>2309</v>
       </c>
       <c r="AA4" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AB4" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AC4" t="s">
         <v>2311</v>
@@ -26660,16 +26921,16 @@
         <v>2271</v>
       </c>
       <c r="AF4" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG4" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH4" t="s">
         <v>2293</v>
       </c>
       <c r="AI4" t="s">
-        <v>706</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -26680,13 +26941,13 @@
         <v>1688</v>
       </c>
       <c r="C5" t="s">
-        <v>706</v>
+        <v>821</v>
       </c>
       <c r="D5" t="s">
-        <v>2174</v>
+        <v>2465</v>
       </c>
       <c r="E5" t="s">
-        <v>2173</v>
+        <v>2464</v>
       </c>
       <c r="G5" t="s">
         <v>706</v>
@@ -26698,31 +26959,31 @@
         <v>1687</v>
       </c>
       <c r="T5" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U5" t="s">
         <v>2280</v>
       </c>
       <c r="V5" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W5" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="X5" t="s">
         <v>2249</v>
       </c>
       <c r="Y5" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Z5" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA5" t="s">
         <v>2309</v>
       </c>
       <c r="AB5" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AC5" t="s">
         <v>2276</v>
@@ -26734,16 +26995,16 @@
         <v>2271</v>
       </c>
       <c r="AF5" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AG5" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH5" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AI5" t="s">
-        <v>706</v>
+        <v>821</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -26754,13 +27015,13 @@
         <v>2088</v>
       </c>
       <c r="C6" t="s">
-        <v>706</v>
+        <v>829</v>
       </c>
       <c r="D6" t="s">
-        <v>2174</v>
+        <v>2468</v>
       </c>
       <c r="E6" t="s">
-        <v>2176</v>
+        <v>2467</v>
       </c>
       <c r="G6" t="s">
         <v>706</v>
@@ -26772,13 +27033,13 @@
         <v>2087</v>
       </c>
       <c r="T6" t="s">
-        <v>2349</v>
+        <v>2466</v>
       </c>
       <c r="U6" t="s">
         <v>2248</v>
       </c>
       <c r="V6" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W6" t="s">
         <v>2249</v>
@@ -26787,37 +27048,37 @@
         <v>2291</v>
       </c>
       <c r="Y6" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Z6" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA6" t="s">
         <v>2298</v>
       </c>
       <c r="AB6" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AC6" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AD6" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE6" t="s">
-        <v>2336</v>
+        <v>399</v>
       </c>
       <c r="AF6" t="s">
         <v>2311</v>
       </c>
       <c r="AG6" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AH6" t="s">
         <v>2294</v>
       </c>
       <c r="AI6" t="s">
-        <v>706</v>
+        <v>829</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -26828,13 +27089,13 @@
         <v>1730</v>
       </c>
       <c r="C7" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
       <c r="D7" t="s">
-        <v>2179</v>
+        <v>2470</v>
       </c>
       <c r="E7" t="s">
-        <v>2178</v>
+        <v>2469</v>
       </c>
       <c r="G7" t="s">
         <v>672</v>
@@ -26846,10 +27107,10 @@
         <v>1729</v>
       </c>
       <c r="T7" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U7" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V7" t="s">
         <v>2249</v>
@@ -26858,7 +27119,7 @@
         <v>2248</v>
       </c>
       <c r="X7" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Y7" t="s">
         <v>2309</v>
@@ -26867,7 +27128,7 @@
         <v>2276</v>
       </c>
       <c r="AA7" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB7" t="s">
         <v>2350</v>
@@ -26876,13 +27137,13 @@
         <v>2311</v>
       </c>
       <c r="AD7" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE7" t="s">
         <v>2271</v>
       </c>
       <c r="AF7" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AG7" t="s">
         <v>2306</v>
@@ -26891,7 +27152,7 @@
         <v>2332</v>
       </c>
       <c r="AI7" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -26902,13 +27163,13 @@
         <v>1690</v>
       </c>
       <c r="C8" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
       <c r="D8" t="s">
-        <v>2182</v>
+        <v>2473</v>
       </c>
       <c r="E8" t="s">
-        <v>2181</v>
+        <v>2472</v>
       </c>
       <c r="G8" t="s">
         <v>672</v>
@@ -26920,25 +27181,25 @@
         <v>1689</v>
       </c>
       <c r="T8" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U8" t="s">
         <v>2249</v>
       </c>
       <c r="V8" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W8" t="s">
         <v>2248</v>
       </c>
       <c r="X8" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Y8" t="s">
         <v>2283</v>
       </c>
       <c r="Z8" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA8" t="s">
         <v>2309</v>
@@ -26947,7 +27208,7 @@
         <v>2293</v>
       </c>
       <c r="AC8" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AD8" t="s">
         <v>2270</v>
@@ -26959,13 +27220,13 @@
         <v>2294</v>
       </c>
       <c r="AG8" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AH8" t="s">
         <v>2332</v>
       </c>
       <c r="AI8" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -26976,13 +27237,13 @@
         <v>2090</v>
       </c>
       <c r="C9" t="s">
-        <v>706</v>
+        <v>1499</v>
       </c>
       <c r="D9" t="s">
-        <v>2182</v>
+        <v>2468</v>
       </c>
       <c r="E9" t="s">
-        <v>2185</v>
+        <v>2474</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -26994,13 +27255,13 @@
         <v>2089</v>
       </c>
       <c r="T9" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U9" t="s">
         <v>2248</v>
       </c>
       <c r="V9" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W9" t="s">
         <v>2249</v>
@@ -27009,22 +27270,22 @@
         <v>2309</v>
       </c>
       <c r="Y9" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Z9" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA9" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB9" t="s">
-        <v>2269</v>
+        <v>700</v>
       </c>
       <c r="AC9" t="s">
         <v>2270</v>
       </c>
       <c r="AD9" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE9" t="s">
         <v>2271</v>
@@ -27033,13 +27294,13 @@
         <v>2283</v>
       </c>
       <c r="AG9" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AH9" t="s">
         <v>2332</v>
       </c>
       <c r="AI9" t="s">
-        <v>706</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -27050,13 +27311,13 @@
         <v>1716</v>
       </c>
       <c r="C10" t="s">
-        <v>706</v>
+        <v>912</v>
       </c>
       <c r="D10" t="s">
-        <v>2182</v>
+        <v>2475</v>
       </c>
       <c r="E10" t="s">
-        <v>2186</v>
+        <v>1366</v>
       </c>
       <c r="G10" t="s">
         <v>706</v>
@@ -27068,13 +27329,13 @@
         <v>1715</v>
       </c>
       <c r="T10" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U10" t="s">
         <v>2248</v>
       </c>
       <c r="V10" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W10" t="s">
         <v>2291</v>
@@ -27083,22 +27344,22 @@
         <v>2249</v>
       </c>
       <c r="Y10" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z10" t="s">
         <v>2309</v>
       </c>
       <c r="AA10" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AB10" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AC10" t="s">
         <v>2276</v>
       </c>
       <c r="AD10" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AE10" t="s">
         <v>2271</v>
@@ -27107,13 +27368,13 @@
         <v>2294</v>
       </c>
       <c r="AG10" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH10" t="s">
-        <v>2345</v>
+        <v>532</v>
       </c>
       <c r="AI10" t="s">
-        <v>706</v>
+        <v>912</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -27124,13 +27385,13 @@
         <v>1698</v>
       </c>
       <c r="C11" t="s">
-        <v>706</v>
+        <v>268</v>
       </c>
       <c r="D11" t="s">
-        <v>2182</v>
+        <v>1896</v>
       </c>
       <c r="E11" t="s">
-        <v>1406</v>
+        <v>2476</v>
       </c>
       <c r="G11" t="s">
         <v>706</v>
@@ -27142,7 +27403,7 @@
         <v>1697</v>
       </c>
       <c r="T11" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U11" t="s">
         <v>2248</v>
@@ -27151,25 +27412,25 @@
         <v>2249</v>
       </c>
       <c r="W11" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X11" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Y11" t="s">
         <v>2293</v>
       </c>
       <c r="Z11" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA11" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB11" t="s">
         <v>2276</v>
       </c>
       <c r="AC11" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AD11" t="s">
         <v>2311</v>
@@ -27178,16 +27439,16 @@
         <v>2271</v>
       </c>
       <c r="AF11" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG11" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH11" t="s">
-        <v>2345</v>
+        <v>532</v>
       </c>
       <c r="AI11" t="s">
-        <v>706</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -27198,13 +27459,13 @@
         <v>1706</v>
       </c>
       <c r="C12" t="s">
-        <v>672</v>
+        <v>829</v>
       </c>
       <c r="D12" t="s">
-        <v>2189</v>
+        <v>2465</v>
       </c>
       <c r="E12" t="s">
-        <v>2188</v>
+        <v>2201</v>
       </c>
       <c r="G12" t="s">
         <v>706</v>
@@ -27216,28 +27477,28 @@
         <v>1705</v>
       </c>
       <c r="T12" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U12" t="s">
         <v>2248</v>
       </c>
       <c r="V12" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="W12" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X12" t="s">
         <v>2249</v>
       </c>
       <c r="Y12" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Z12" t="s">
-        <v>2316</v>
+        <v>2421</v>
       </c>
       <c r="AA12" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB12" t="s">
         <v>2318</v>
@@ -27246,7 +27507,7 @@
         <v>2294</v>
       </c>
       <c r="AD12" t="s">
-        <v>2302</v>
+        <v>2411</v>
       </c>
       <c r="AE12" t="s">
         <v>2271</v>
@@ -27255,13 +27516,13 @@
         <v>2293</v>
       </c>
       <c r="AG12" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH12" t="s">
         <v>2332</v>
       </c>
       <c r="AI12" t="s">
-        <v>672</v>
+        <v>829</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -27272,13 +27533,13 @@
         <v>1700</v>
       </c>
       <c r="C13" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
       <c r="D13" t="s">
-        <v>2191</v>
+        <v>2478</v>
       </c>
       <c r="E13" t="s">
-        <v>2190</v>
+        <v>2477</v>
       </c>
       <c r="G13" t="s">
         <v>706</v>
@@ -27290,7 +27551,7 @@
         <v>1699</v>
       </c>
       <c r="T13" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U13" t="s">
         <v>2248</v>
@@ -27299,22 +27560,22 @@
         <v>2249</v>
       </c>
       <c r="W13" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X13" t="s">
         <v>2293</v>
       </c>
       <c r="Y13" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z13" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA13" t="s">
         <v>2309</v>
       </c>
       <c r="AB13" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AC13" t="s">
         <v>2254</v>
@@ -27326,16 +27587,16 @@
         <v>2271</v>
       </c>
       <c r="AF13" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG13" t="s">
         <v>2332</v>
       </c>
       <c r="AH13" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI13" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -27346,13 +27607,13 @@
         <v>1708</v>
       </c>
       <c r="C14" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
       <c r="D14" t="s">
-        <v>2191</v>
+        <v>2478</v>
       </c>
       <c r="E14" t="s">
-        <v>2192</v>
+        <v>2479</v>
       </c>
       <c r="G14" t="s">
         <v>672</v>
@@ -27364,7 +27625,7 @@
         <v>1707</v>
       </c>
       <c r="T14" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U14" t="s">
         <v>2249</v>
@@ -27373,25 +27634,25 @@
         <v>2248</v>
       </c>
       <c r="W14" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X14" t="s">
         <v>2280</v>
       </c>
       <c r="Y14" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="Z14" t="s">
         <v>2293</v>
       </c>
       <c r="AA14" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB14" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC14" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AD14" t="s">
         <v>2270</v>
@@ -27403,13 +27664,13 @@
         <v>2294</v>
       </c>
       <c r="AG14" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AH14" t="s">
         <v>2332</v>
       </c>
       <c r="AI14" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -27420,13 +27681,13 @@
         <v>1696</v>
       </c>
       <c r="C15" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="D15" t="s">
-        <v>2191</v>
+        <v>2481</v>
       </c>
       <c r="E15" t="s">
-        <v>2192</v>
+        <v>2480</v>
       </c>
       <c r="G15" t="s">
         <v>706</v>
@@ -27438,7 +27699,7 @@
         <v>1695</v>
       </c>
       <c r="T15" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U15" t="s">
         <v>2249</v>
@@ -27447,16 +27708,16 @@
         <v>2248</v>
       </c>
       <c r="W15" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X15" t="s">
         <v>2280</v>
       </c>
       <c r="Y15" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Z15" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA15" t="s">
         <v>2309</v>
@@ -27465,7 +27726,7 @@
         <v>2293</v>
       </c>
       <c r="AC15" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AD15" t="s">
         <v>2270</v>
@@ -27474,7 +27735,7 @@
         <v>2271</v>
       </c>
       <c r="AF15" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AG15" t="s">
         <v>2294</v>
@@ -27483,7 +27744,7 @@
         <v>2332</v>
       </c>
       <c r="AI15" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -27494,13 +27755,13 @@
         <v>1692</v>
       </c>
       <c r="C16" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
       <c r="D16" t="s">
-        <v>2191</v>
+        <v>2483</v>
       </c>
       <c r="E16" t="s">
-        <v>2193</v>
+        <v>2482</v>
       </c>
       <c r="G16" t="s">
         <v>452</v>
@@ -27512,10 +27773,10 @@
         <v>1691</v>
       </c>
       <c r="T16" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U16" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V16" t="s">
         <v>2248</v>
@@ -27527,16 +27788,16 @@
         <v>2283</v>
       </c>
       <c r="Y16" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Z16" t="s">
         <v>2309</v>
       </c>
       <c r="AA16" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB16" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC16" t="s">
         <v>2293</v>
@@ -27554,10 +27815,10 @@
         <v>2332</v>
       </c>
       <c r="AH16" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AI16" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -27568,13 +27829,13 @@
         <v>1722</v>
       </c>
       <c r="C17" t="s">
-        <v>672</v>
+        <v>730</v>
       </c>
       <c r="D17" t="s">
-        <v>2140</v>
+        <v>1896</v>
       </c>
       <c r="E17" t="s">
-        <v>2194</v>
+        <v>2484</v>
       </c>
       <c r="G17" t="s">
         <v>706</v>
@@ -27586,10 +27847,10 @@
         <v>1721</v>
       </c>
       <c r="T17" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U17" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V17" t="s">
         <v>2248</v>
@@ -27598,19 +27859,19 @@
         <v>2249</v>
       </c>
       <c r="X17" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Y17" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z17" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AA17" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB17" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AC17" t="s">
         <v>2270</v>
@@ -27622,16 +27883,16 @@
         <v>2271</v>
       </c>
       <c r="AF17" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG17" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH17" t="s">
         <v>2332</v>
       </c>
       <c r="AI17" t="s">
-        <v>672</v>
+        <v>730</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -27642,13 +27903,13 @@
         <v>1694</v>
       </c>
       <c r="C18" t="s">
-        <v>706</v>
+        <v>2246</v>
       </c>
       <c r="D18" t="s">
-        <v>2140</v>
+        <v>2487</v>
       </c>
       <c r="E18" t="s">
-        <v>2139</v>
+        <v>2486</v>
       </c>
       <c r="G18" t="s">
         <v>452</v>
@@ -27660,7 +27921,7 @@
         <v>1693</v>
       </c>
       <c r="T18" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U18" t="s">
         <v>2248</v>
@@ -27669,22 +27930,22 @@
         <v>2249</v>
       </c>
       <c r="W18" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X18" t="s">
         <v>2280</v>
       </c>
       <c r="Y18" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z18" t="s">
         <v>2309</v>
       </c>
       <c r="AA18" t="s">
-        <v>2352</v>
+        <v>2485</v>
       </c>
       <c r="AB18" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AC18" t="s">
         <v>2300</v>
@@ -27696,16 +27957,16 @@
         <v>2271</v>
       </c>
       <c r="AF18" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AG18" t="s">
         <v>2332</v>
       </c>
       <c r="AH18" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI18" t="s">
-        <v>706</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -27716,13 +27977,13 @@
         <v>2092</v>
       </c>
       <c r="C19" t="s">
-        <v>653</v>
+        <v>2408</v>
       </c>
       <c r="D19" t="s">
-        <v>2140</v>
+        <v>2489</v>
       </c>
       <c r="E19" t="s">
-        <v>2196</v>
+        <v>2488</v>
       </c>
       <c r="G19" t="s">
         <v>706</v>
@@ -27734,7 +27995,7 @@
         <v>2091</v>
       </c>
       <c r="T19" t="s">
-        <v>2322</v>
+        <v>804</v>
       </c>
       <c r="U19" t="s">
         <v>2248</v>
@@ -27743,19 +28004,19 @@
         <v>2249</v>
       </c>
       <c r="W19" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X19" t="s">
         <v>2283</v>
       </c>
       <c r="Y19" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Z19" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AA19" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB19" t="s">
         <v>2294</v>
@@ -27767,19 +28028,19 @@
         <v>2311</v>
       </c>
       <c r="AE19" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF19" t="s">
         <v>2262</v>
       </c>
       <c r="AG19" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH19" t="s">
         <v>2353</v>
       </c>
       <c r="AI19" t="s">
-        <v>653</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
@@ -27790,13 +28051,13 @@
         <v>1742</v>
       </c>
       <c r="C20" t="s">
-        <v>672</v>
+        <v>1499</v>
       </c>
       <c r="D20" t="s">
-        <v>2198</v>
+        <v>2483</v>
       </c>
       <c r="E20" t="s">
-        <v>2197</v>
+        <v>2482</v>
       </c>
       <c r="G20" t="s">
         <v>672</v>
@@ -27808,10 +28069,10 @@
         <v>1741</v>
       </c>
       <c r="T20" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U20" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V20" t="s">
         <v>2248</v>
@@ -27823,19 +28084,19 @@
         <v>2283</v>
       </c>
       <c r="Y20" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Z20" t="s">
         <v>2276</v>
       </c>
       <c r="AA20" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AB20" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AC20" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AD20" t="s">
         <v>2311</v>
@@ -27847,13 +28108,13 @@
         <v>2294</v>
       </c>
       <c r="AG20" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH20" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI20" t="s">
-        <v>672</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -27864,13 +28125,13 @@
         <v>2094</v>
       </c>
       <c r="C21" t="s">
-        <v>861</v>
+        <v>286</v>
       </c>
       <c r="D21" t="s">
-        <v>2198</v>
+        <v>1896</v>
       </c>
       <c r="E21" t="s">
-        <v>2200</v>
+        <v>2490</v>
       </c>
       <c r="G21" t="s">
         <v>452</v>
@@ -27882,13 +28143,13 @@
         <v>2093</v>
       </c>
       <c r="T21" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U21" t="s">
         <v>2249</v>
       </c>
       <c r="V21" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W21" t="s">
         <v>2283</v>
@@ -27897,28 +28158,28 @@
         <v>2248</v>
       </c>
       <c r="Y21" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="Z21" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA21" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB21" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AC21" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AD21" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE21" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF21" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AG21" t="s">
         <v>2254</v>
@@ -27927,7 +28188,7 @@
         <v>2311</v>
       </c>
       <c r="AI21" t="s">
-        <v>861</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -27938,13 +28199,13 @@
         <v>1710</v>
       </c>
       <c r="C22" t="s">
-        <v>706</v>
+        <v>2491</v>
       </c>
       <c r="D22" t="s">
-        <v>2202</v>
+        <v>2489</v>
       </c>
       <c r="E22" t="s">
-        <v>2201</v>
+        <v>2492</v>
       </c>
       <c r="G22" t="s">
         <v>672</v>
@@ -27956,10 +28217,10 @@
         <v>1709</v>
       </c>
       <c r="T22" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U22" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V22" t="s">
         <v>2249</v>
@@ -27968,7 +28229,7 @@
         <v>2248</v>
       </c>
       <c r="X22" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="Y22" t="s">
         <v>2280</v>
@@ -27977,7 +28238,7 @@
         <v>2293</v>
       </c>
       <c r="AA22" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB22" t="s">
         <v>2298</v>
@@ -27998,10 +28259,10 @@
         <v>2332</v>
       </c>
       <c r="AH22" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AI22" t="s">
-        <v>706</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -28012,13 +28273,13 @@
         <v>1724</v>
       </c>
       <c r="C23" t="s">
-        <v>672</v>
+        <v>844</v>
       </c>
       <c r="D23" t="s">
-        <v>2202</v>
+        <v>2494</v>
       </c>
       <c r="E23" t="s">
-        <v>2203</v>
+        <v>2493</v>
       </c>
       <c r="G23" t="s">
         <v>653</v>
@@ -28030,10 +28291,10 @@
         <v>1723</v>
       </c>
       <c r="T23" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U23" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V23" t="s">
         <v>2248</v>
@@ -28042,16 +28303,16 @@
         <v>2249</v>
       </c>
       <c r="X23" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y23" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Z23" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA23" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB23" t="s">
         <v>2309</v>
@@ -28066,16 +28327,16 @@
         <v>2271</v>
       </c>
       <c r="AF23" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="AG23" t="s">
         <v>2294</v>
       </c>
       <c r="AH23" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI23" t="s">
-        <v>672</v>
+        <v>844</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -28086,13 +28347,13 @@
         <v>2096</v>
       </c>
       <c r="C24" t="s">
-        <v>653</v>
+        <v>1949</v>
       </c>
       <c r="D24" t="s">
-        <v>2202</v>
+        <v>2478</v>
       </c>
       <c r="E24" t="s">
-        <v>2203</v>
+        <v>2477</v>
       </c>
       <c r="G24" t="s">
         <v>706</v>
@@ -28104,10 +28365,10 @@
         <v>2095</v>
       </c>
       <c r="T24" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="U24" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V24" t="s">
         <v>2249</v>
@@ -28116,19 +28377,19 @@
         <v>2248</v>
       </c>
       <c r="X24" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Y24" t="s">
         <v>2309</v>
       </c>
       <c r="Z24" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA24" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB24" t="s">
-        <v>2302</v>
+        <v>2411</v>
       </c>
       <c r="AC24" t="s">
         <v>2311</v>
@@ -28143,13 +28404,13 @@
         <v>2293</v>
       </c>
       <c r="AG24" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH24" t="s">
         <v>1427</v>
       </c>
       <c r="AI24" t="s">
-        <v>653</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -28160,13 +28421,13 @@
         <v>2098</v>
       </c>
       <c r="C25" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
       <c r="D25" t="s">
-        <v>2202</v>
+        <v>2496</v>
       </c>
       <c r="E25" t="s">
-        <v>2203</v>
+        <v>2495</v>
       </c>
       <c r="G25" t="s">
         <v>672</v>
@@ -28178,10 +28439,10 @@
         <v>2097</v>
       </c>
       <c r="T25" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U25" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V25" t="s">
         <v>2248</v>
@@ -28193,19 +28454,19 @@
         <v>2280</v>
       </c>
       <c r="Y25" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z25" t="s">
         <v>2293</v>
       </c>
       <c r="AA25" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB25" t="s">
         <v>2309</v>
       </c>
       <c r="AC25" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD25" t="s">
         <v>2270</v>
@@ -28217,13 +28478,13 @@
         <v>2350</v>
       </c>
       <c r="AG25" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH25" t="s">
         <v>2332</v>
       </c>
       <c r="AI25" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -28234,13 +28495,13 @@
         <v>1734</v>
       </c>
       <c r="C26" t="s">
-        <v>706</v>
+        <v>821</v>
       </c>
       <c r="D26" t="s">
-        <v>2202</v>
+        <v>2498</v>
       </c>
       <c r="E26" t="s">
-        <v>1352</v>
+        <v>2497</v>
       </c>
       <c r="G26" t="s">
         <v>706</v>
@@ -28252,25 +28513,25 @@
         <v>1733</v>
       </c>
       <c r="T26" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U26" t="s">
         <v>2249</v>
       </c>
       <c r="V26" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W26" t="s">
         <v>2248</v>
       </c>
       <c r="X26" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Y26" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Z26" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA26" t="s">
         <v>2309</v>
@@ -28288,16 +28549,16 @@
         <v>2271</v>
       </c>
       <c r="AF26" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG26" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH26" t="s">
         <v>2332</v>
       </c>
       <c r="AI26" t="s">
-        <v>706</v>
+        <v>821</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -28308,13 +28569,13 @@
         <v>2100</v>
       </c>
       <c r="C27" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
       <c r="D27" t="s">
-        <v>2202</v>
+        <v>2496</v>
       </c>
       <c r="E27" t="s">
-        <v>2208</v>
+        <v>2499</v>
       </c>
       <c r="G27" t="s">
         <v>706</v>
@@ -28326,10 +28587,10 @@
         <v>2099</v>
       </c>
       <c r="T27" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U27" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V27" t="s">
         <v>2248</v>
@@ -28341,16 +28602,16 @@
         <v>2249</v>
       </c>
       <c r="Y27" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z27" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA27" t="s">
         <v>2309</v>
       </c>
       <c r="AB27" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AC27" t="s">
         <v>2311</v>
@@ -28362,16 +28623,16 @@
         <v>2271</v>
       </c>
       <c r="AF27" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AG27" t="s">
         <v>2293</v>
       </c>
       <c r="AH27" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AI27" t="s">
-        <v>706</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -28382,13 +28643,13 @@
         <v>1760</v>
       </c>
       <c r="C28" t="s">
-        <v>706</v>
+        <v>2461</v>
       </c>
       <c r="D28" t="s">
-        <v>2210</v>
+        <v>2489</v>
       </c>
       <c r="E28" t="s">
-        <v>2209</v>
+        <v>2500</v>
       </c>
       <c r="G28" t="s">
         <v>706</v>
@@ -28400,28 +28661,28 @@
         <v>1759</v>
       </c>
       <c r="T28" t="s">
-        <v>2259</v>
+        <v>2393</v>
       </c>
       <c r="U28" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V28" t="s">
         <v>2248</v>
       </c>
       <c r="W28" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="X28" t="s">
-        <v>2342</v>
+        <v>1221</v>
       </c>
       <c r="Y28" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z28" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AA28" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AB28" t="s">
         <v>2354</v>
@@ -28430,22 +28691,22 @@
         <v>2311</v>
       </c>
       <c r="AD28" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE28" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF28" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AG28" t="s">
         <v>2309</v>
       </c>
       <c r="AH28" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="AI28" t="s">
-        <v>706</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -28456,13 +28717,13 @@
         <v>2102</v>
       </c>
       <c r="C29" t="s">
-        <v>653</v>
+        <v>844</v>
       </c>
       <c r="D29" t="s">
-        <v>2210</v>
+        <v>2502</v>
       </c>
       <c r="E29" t="s">
-        <v>1392</v>
+        <v>2501</v>
       </c>
       <c r="G29" t="s">
         <v>706</v>
@@ -28474,7 +28735,7 @@
         <v>2101</v>
       </c>
       <c r="T29" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="U29" t="s">
         <v>2248</v>
@@ -28483,22 +28744,22 @@
         <v>2249</v>
       </c>
       <c r="W29" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X29" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y29" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="Z29" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA29" t="s">
         <v>2309</v>
       </c>
       <c r="AB29" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AC29" t="s">
         <v>2270</v>
@@ -28510,16 +28771,16 @@
         <v>2271</v>
       </c>
       <c r="AF29" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG29" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH29" t="s">
         <v>2332</v>
       </c>
       <c r="AI29" t="s">
-        <v>653</v>
+        <v>844</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -28530,13 +28791,13 @@
         <v>1776</v>
       </c>
       <c r="C30" t="s">
-        <v>706</v>
+        <v>1949</v>
       </c>
       <c r="D30" t="s">
-        <v>2210</v>
+        <v>2465</v>
       </c>
       <c r="E30" t="s">
-        <v>2212</v>
+        <v>745</v>
       </c>
       <c r="G30" t="s">
         <v>706</v>
@@ -28548,13 +28809,13 @@
         <v>1775</v>
       </c>
       <c r="T30" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U30" t="s">
         <v>2248</v>
       </c>
       <c r="V30" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W30" t="s">
         <v>2249</v>
@@ -28563,16 +28824,16 @@
         <v>2283</v>
       </c>
       <c r="Y30" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z30" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA30" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AB30" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AC30" t="s">
         <v>2294</v>
@@ -28587,13 +28848,13 @@
         <v>2309</v>
       </c>
       <c r="AG30" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH30" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI30" t="s">
-        <v>706</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -28604,13 +28865,13 @@
         <v>2104</v>
       </c>
       <c r="C31" t="s">
-        <v>706</v>
+        <v>778</v>
       </c>
       <c r="D31" t="s">
-        <v>2215</v>
+        <v>2168</v>
       </c>
       <c r="E31" t="s">
-        <v>2214</v>
+        <v>1297</v>
       </c>
       <c r="G31" t="s">
         <v>706</v>
@@ -28622,13 +28883,13 @@
         <v>2103</v>
       </c>
       <c r="T31" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U31" t="s">
         <v>2249</v>
       </c>
       <c r="V31" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W31" t="s">
         <v>2291</v>
@@ -28640,10 +28901,10 @@
         <v>2280</v>
       </c>
       <c r="Z31" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA31" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB31" t="s">
         <v>2293</v>
@@ -28658,16 +28919,16 @@
         <v>2271</v>
       </c>
       <c r="AF31" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AG31" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH31" t="s">
         <v>2332</v>
       </c>
       <c r="AI31" t="s">
-        <v>706</v>
+        <v>778</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -28678,13 +28939,13 @@
         <v>2106</v>
       </c>
       <c r="C32" t="s">
-        <v>653</v>
+        <v>2408</v>
       </c>
       <c r="D32" t="s">
-        <v>2215</v>
+        <v>2504</v>
       </c>
       <c r="E32" t="s">
-        <v>2218</v>
+        <v>2503</v>
       </c>
       <c r="G32" t="s">
         <v>672</v>
@@ -28696,7 +28957,7 @@
         <v>2105</v>
       </c>
       <c r="T32" t="s">
-        <v>2259</v>
+        <v>2393</v>
       </c>
       <c r="U32" t="s">
         <v>2248</v>
@@ -28705,13 +28966,13 @@
         <v>2249</v>
       </c>
       <c r="W32" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X32" t="s">
         <v>2280</v>
       </c>
       <c r="Y32" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z32" t="s">
         <v>2309</v>
@@ -28720,10 +28981,10 @@
         <v>2355</v>
       </c>
       <c r="AB32" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AC32" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD32" t="s">
         <v>2311</v>
@@ -28735,13 +28996,13 @@
         <v>2294</v>
       </c>
       <c r="AG32" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH32" t="s">
         <v>2356</v>
       </c>
       <c r="AI32" t="s">
-        <v>653</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -28752,13 +29013,13 @@
         <v>2108</v>
       </c>
       <c r="C33" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
       <c r="D33" t="s">
-        <v>2221</v>
+        <v>2170</v>
       </c>
       <c r="E33" t="s">
-        <v>2220</v>
+        <v>2505</v>
       </c>
       <c r="G33" t="s">
         <v>578</v>
@@ -28770,7 +29031,7 @@
         <v>2107</v>
       </c>
       <c r="T33" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U33" t="s">
         <v>2248</v>
@@ -28779,22 +29040,22 @@
         <v>2249</v>
       </c>
       <c r="W33" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X33" t="s">
         <v>2280</v>
       </c>
       <c r="Y33" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z33" t="s">
         <v>2309</v>
       </c>
       <c r="AA33" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB33" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AC33" t="s">
         <v>2270</v>
@@ -28809,13 +29070,13 @@
         <v>2293</v>
       </c>
       <c r="AG33" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH33" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AI33" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
@@ -28826,13 +29087,13 @@
         <v>1704</v>
       </c>
       <c r="C34" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
       <c r="D34" t="s">
-        <v>2223</v>
+        <v>2465</v>
       </c>
       <c r="E34" t="s">
-        <v>2222</v>
+        <v>2203</v>
       </c>
       <c r="G34" t="s">
         <v>672</v>
@@ -28844,7 +29105,7 @@
         <v>1703</v>
       </c>
       <c r="T34" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U34" t="s">
         <v>2283</v>
@@ -28856,19 +29117,19 @@
         <v>2248</v>
       </c>
       <c r="X34" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="Y34" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Z34" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA34" t="s">
         <v>2309</v>
       </c>
       <c r="AB34" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC34" t="s">
         <v>2293</v>
@@ -28883,13 +29144,13 @@
         <v>2294</v>
       </c>
       <c r="AG34" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AH34" t="s">
         <v>2332</v>
       </c>
       <c r="AI34" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -28900,13 +29161,13 @@
         <v>1768</v>
       </c>
       <c r="C35" t="s">
-        <v>653</v>
+        <v>2461</v>
       </c>
       <c r="D35" t="s">
-        <v>2223</v>
+        <v>2507</v>
       </c>
       <c r="E35" t="s">
-        <v>2222</v>
+        <v>2506</v>
       </c>
       <c r="G35" t="s">
         <v>706</v>
@@ -28918,13 +29179,13 @@
         <v>1767</v>
       </c>
       <c r="T35" t="s">
-        <v>2259</v>
+        <v>2393</v>
       </c>
       <c r="U35" t="s">
         <v>2249</v>
       </c>
       <c r="V35" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W35" t="s">
         <v>2280</v>
@@ -28933,13 +29194,13 @@
         <v>2264</v>
       </c>
       <c r="Y35" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Z35" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA35" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB35" t="s">
         <v>2270</v>
@@ -28948,22 +29209,22 @@
         <v>2294</v>
       </c>
       <c r="AD35" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE35" t="s">
-        <v>2322</v>
+        <v>804</v>
       </c>
       <c r="AF35" t="s">
         <v>2357</v>
       </c>
       <c r="AG35" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH35" t="s">
         <v>2332</v>
       </c>
       <c r="AI35" t="s">
-        <v>653</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -28974,13 +29235,13 @@
         <v>1770</v>
       </c>
       <c r="C36" t="s">
-        <v>706</v>
+        <v>270</v>
       </c>
       <c r="D36" t="s">
-        <v>2225</v>
+        <v>2478</v>
       </c>
       <c r="E36" t="s">
-        <v>1297</v>
+        <v>2477</v>
       </c>
       <c r="G36" t="s">
         <v>672</v>
@@ -28992,7 +29253,7 @@
         <v>1769</v>
       </c>
       <c r="T36" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U36" t="s">
         <v>2249</v>
@@ -29001,22 +29262,22 @@
         <v>2248</v>
       </c>
       <c r="W36" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X36" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Y36" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="Z36" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA36" t="s">
         <v>2309</v>
       </c>
       <c r="AB36" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AC36" t="s">
         <v>2311</v>
@@ -29028,16 +29289,16 @@
         <v>2271</v>
       </c>
       <c r="AF36" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AG36" t="s">
         <v>2332</v>
       </c>
       <c r="AH36" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI36" t="s">
-        <v>706</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
@@ -29048,13 +29309,13 @@
         <v>1712</v>
       </c>
       <c r="C37" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
       <c r="D37" t="s">
-        <v>2225</v>
+        <v>2509</v>
       </c>
       <c r="E37" t="s">
-        <v>1856</v>
+        <v>2508</v>
       </c>
       <c r="G37" t="s">
         <v>672</v>
@@ -29066,10 +29327,10 @@
         <v>1711</v>
       </c>
       <c r="T37" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U37" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V37" t="s">
         <v>2248</v>
@@ -29081,7 +29342,7 @@
         <v>2280</v>
       </c>
       <c r="Y37" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Z37" t="s">
         <v>2293</v>
@@ -29090,10 +29351,10 @@
         <v>2309</v>
       </c>
       <c r="AB37" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AC37" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AD37" t="s">
         <v>2254</v>
@@ -29105,13 +29366,13 @@
         <v>2294</v>
       </c>
       <c r="AG37" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AH37" t="s">
         <v>2332</v>
       </c>
       <c r="AI37" t="s">
-        <v>706</v>
+        <v>730</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
@@ -29122,13 +29383,13 @@
         <v>2110</v>
       </c>
       <c r="C38" t="s">
-        <v>706</v>
+        <v>278</v>
       </c>
       <c r="D38" t="s">
-        <v>2225</v>
+        <v>2511</v>
       </c>
       <c r="E38" t="s">
-        <v>1856</v>
+        <v>2510</v>
       </c>
       <c r="G38" t="s">
         <v>706</v>
@@ -29140,10 +29401,10 @@
         <v>2109</v>
       </c>
       <c r="T38" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U38" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V38" t="s">
         <v>2248</v>
@@ -29155,19 +29416,19 @@
         <v>2280</v>
       </c>
       <c r="Y38" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="Z38" t="s">
         <v>2293</v>
       </c>
       <c r="AA38" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB38" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AC38" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AD38" t="s">
         <v>2270</v>
@@ -29179,13 +29440,13 @@
         <v>2294</v>
       </c>
       <c r="AG38" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH38" t="s">
         <v>2332</v>
       </c>
       <c r="AI38" t="s">
-        <v>706</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
@@ -29196,13 +29457,13 @@
         <v>1746</v>
       </c>
       <c r="C39" t="s">
-        <v>672</v>
+        <v>907</v>
       </c>
       <c r="D39" t="s">
-        <v>2225</v>
+        <v>2513</v>
       </c>
       <c r="E39" t="s">
-        <v>1856</v>
+        <v>2512</v>
       </c>
       <c r="G39" t="s">
         <v>2359</v>
@@ -29214,10 +29475,10 @@
         <v>1745</v>
       </c>
       <c r="T39" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U39" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V39" t="s">
         <v>2249</v>
@@ -29229,13 +29490,13 @@
         <v>2280</v>
       </c>
       <c r="Y39" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z39" t="s">
         <v>2309</v>
       </c>
       <c r="AA39" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB39" t="s">
         <v>2276</v>
@@ -29250,16 +29511,16 @@
         <v>2271</v>
       </c>
       <c r="AF39" t="s">
-        <v>2287</v>
+        <v>1533</v>
       </c>
       <c r="AG39" t="s">
         <v>2294</v>
       </c>
       <c r="AH39" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI39" t="s">
-        <v>672</v>
+        <v>907</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
@@ -29270,13 +29531,13 @@
         <v>2111</v>
       </c>
       <c r="C40" t="s">
-        <v>672</v>
+        <v>844</v>
       </c>
       <c r="D40" t="s">
-        <v>2225</v>
+        <v>2515</v>
       </c>
       <c r="E40" t="s">
-        <v>1856</v>
+        <v>2514</v>
       </c>
       <c r="G40" t="s">
         <v>706</v>
@@ -29288,10 +29549,10 @@
         <v>1610</v>
       </c>
       <c r="T40" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U40" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V40" t="s">
         <v>2249</v>
@@ -29306,34 +29567,34 @@
         <v>2293</v>
       </c>
       <c r="Z40" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="AA40" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB40" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AC40" t="s">
         <v>2254</v>
       </c>
       <c r="AD40" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AE40" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF40" t="s">
-        <v>2344</v>
+        <v>1919</v>
       </c>
       <c r="AG40" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH40" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI40" t="s">
-        <v>672</v>
+        <v>844</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
@@ -29344,13 +29605,13 @@
         <v>1718</v>
       </c>
       <c r="C41" t="s">
-        <v>706</v>
+        <v>778</v>
       </c>
       <c r="D41" t="s">
-        <v>2225</v>
+        <v>2517</v>
       </c>
       <c r="E41" t="s">
-        <v>1458</v>
+        <v>2516</v>
       </c>
       <c r="G41" t="s">
         <v>672</v>
@@ -29362,13 +29623,13 @@
         <v>1717</v>
       </c>
       <c r="T41" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U41" t="s">
         <v>2249</v>
       </c>
       <c r="V41" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W41" t="s">
         <v>2248</v>
@@ -29383,10 +29644,10 @@
         <v>2309</v>
       </c>
       <c r="AA41" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB41" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC41" t="s">
         <v>2294</v>
@@ -29401,13 +29662,13 @@
         <v>1427</v>
       </c>
       <c r="AG41" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AH41" t="s">
         <v>2332</v>
       </c>
       <c r="AI41" t="s">
-        <v>706</v>
+        <v>778</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
@@ -29418,13 +29679,13 @@
         <v>1702</v>
       </c>
       <c r="C42" t="s">
-        <v>706</v>
+        <v>272</v>
       </c>
       <c r="D42" t="s">
-        <v>2225</v>
+        <v>2168</v>
       </c>
       <c r="E42" t="s">
-        <v>1458</v>
+        <v>2518</v>
       </c>
       <c r="G42" t="s">
         <v>672</v>
@@ -29436,7 +29697,7 @@
         <v>1701</v>
       </c>
       <c r="T42" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U42" t="s">
         <v>2248</v>
@@ -29445,22 +29706,22 @@
         <v>2249</v>
       </c>
       <c r="W42" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X42" t="s">
         <v>2280</v>
       </c>
       <c r="Y42" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Z42" t="s">
         <v>2293</v>
       </c>
       <c r="AA42" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB42" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC42" t="s">
         <v>2270</v>
@@ -29472,16 +29733,16 @@
         <v>2271</v>
       </c>
       <c r="AF42" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AG42" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH42" t="s">
         <v>2332</v>
       </c>
       <c r="AI42" t="s">
-        <v>706</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
@@ -29492,13 +29753,13 @@
         <v>2113</v>
       </c>
       <c r="C43" t="s">
-        <v>672</v>
+        <v>270</v>
       </c>
       <c r="D43" t="s">
-        <v>2225</v>
+        <v>2478</v>
       </c>
       <c r="E43" t="s">
-        <v>1458</v>
+        <v>2519</v>
       </c>
       <c r="G43" t="s">
         <v>706</v>
@@ -29510,10 +29771,10 @@
         <v>2112</v>
       </c>
       <c r="T43" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U43" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V43" t="s">
         <v>2249</v>
@@ -29522,22 +29783,22 @@
         <v>2248</v>
       </c>
       <c r="X43" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y43" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z43" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA43" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB43" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC43" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD43" t="s">
         <v>2270</v>
@@ -29549,13 +29810,13 @@
         <v>2294</v>
       </c>
       <c r="AG43" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH43" t="s">
-        <v>2265</v>
+        <v>710</v>
       </c>
       <c r="AI43" t="s">
-        <v>672</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -29566,13 +29827,13 @@
         <v>1748</v>
       </c>
       <c r="C44" t="s">
-        <v>672</v>
+        <v>730</v>
       </c>
       <c r="D44" t="s">
-        <v>2225</v>
+        <v>2509</v>
       </c>
       <c r="E44" t="s">
-        <v>1972</v>
+        <v>808</v>
       </c>
       <c r="G44" t="s">
         <v>706</v>
@@ -29584,34 +29845,34 @@
         <v>1747</v>
       </c>
       <c r="T44" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U44" t="s">
         <v>2249</v>
       </c>
       <c r="V44" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W44" t="s">
         <v>2248</v>
       </c>
       <c r="X44" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y44" t="s">
         <v>2309</v>
       </c>
       <c r="Z44" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AA44" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB44" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC44" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD44" t="s">
         <v>2254</v>
@@ -29620,16 +29881,16 @@
         <v>2271</v>
       </c>
       <c r="AF44" t="s">
-        <v>939</v>
+        <v>2380</v>
       </c>
       <c r="AG44" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH44" t="s">
-        <v>2348</v>
+        <v>2463</v>
       </c>
       <c r="AI44" t="s">
-        <v>672</v>
+        <v>730</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
@@ -29640,13 +29901,13 @@
         <v>2115</v>
       </c>
       <c r="C45" t="s">
-        <v>672</v>
+        <v>1949</v>
       </c>
       <c r="D45" t="s">
-        <v>2225</v>
+        <v>2170</v>
       </c>
       <c r="E45" t="s">
-        <v>1972</v>
+        <v>2202</v>
       </c>
       <c r="G45" t="s">
         <v>452</v>
@@ -29658,13 +29919,13 @@
         <v>2114</v>
       </c>
       <c r="T45" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U45" t="s">
         <v>2248</v>
       </c>
       <c r="V45" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="W45" t="s">
         <v>2249</v>
@@ -29673,16 +29934,16 @@
         <v>2280</v>
       </c>
       <c r="Y45" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z45" t="s">
-        <v>2261</v>
+        <v>691</v>
       </c>
       <c r="AA45" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB45" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC45" t="s">
         <v>2311</v>
@@ -29697,13 +29958,13 @@
         <v>2294</v>
       </c>
       <c r="AG45" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH45" t="s">
-        <v>2344</v>
+        <v>1919</v>
       </c>
       <c r="AI45" t="s">
-        <v>672</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
@@ -29714,13 +29975,13 @@
         <v>2117</v>
       </c>
       <c r="C46" t="s">
-        <v>672</v>
+        <v>1949</v>
       </c>
       <c r="D46" t="s">
-        <v>2225</v>
+        <v>2170</v>
       </c>
       <c r="E46" t="s">
-        <v>1473</v>
+        <v>2174</v>
       </c>
       <c r="G46" t="s">
         <v>452</v>
@@ -29732,7 +29993,7 @@
         <v>2116</v>
       </c>
       <c r="T46" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U46" t="s">
         <v>2248</v>
@@ -29741,25 +30002,25 @@
         <v>2249</v>
       </c>
       <c r="W46" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="X46" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="Y46" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z46" t="s">
         <v>2309</v>
       </c>
       <c r="AA46" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AB46" t="s">
         <v>2254</v>
       </c>
       <c r="AC46" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD46" t="s">
         <v>2311</v>
@@ -29768,7 +30029,7 @@
         <v>2271</v>
       </c>
       <c r="AF46" t="s">
-        <v>2351</v>
+        <v>2471</v>
       </c>
       <c r="AG46" t="s">
         <v>2332</v>
@@ -29777,7 +30038,7 @@
         <v>2306</v>
       </c>
       <c r="AI46" t="s">
-        <v>672</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
@@ -29788,13 +30049,13 @@
         <v>1750</v>
       </c>
       <c r="C47" t="s">
-        <v>672</v>
+        <v>1564</v>
       </c>
       <c r="D47" t="s">
-        <v>2235</v>
+        <v>2521</v>
       </c>
       <c r="E47" t="s">
-        <v>2234</v>
+        <v>2520</v>
       </c>
       <c r="G47" t="s">
         <v>672</v>
@@ -29806,10 +30067,10 @@
         <v>1749</v>
       </c>
       <c r="T47" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U47" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V47" t="s">
         <v>2248</v>
@@ -29818,22 +30079,22 @@
         <v>2249</v>
       </c>
       <c r="X47" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y47" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z47" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA47" t="s">
-        <v>2315</v>
+        <v>2377</v>
       </c>
       <c r="AB47" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AC47" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD47" t="s">
         <v>2254</v>
@@ -29845,13 +30106,13 @@
         <v>2332</v>
       </c>
       <c r="AG47" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH47" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AI47" t="s">
-        <v>672</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
@@ -29862,13 +30123,13 @@
         <v>1752</v>
       </c>
       <c r="C48" t="s">
-        <v>672</v>
+        <v>1564</v>
       </c>
       <c r="D48" t="s">
-        <v>2235</v>
+        <v>2521</v>
       </c>
       <c r="E48" t="s">
-        <v>2234</v>
+        <v>2520</v>
       </c>
       <c r="G48" t="s">
         <v>672</v>
@@ -29880,10 +30141,10 @@
         <v>1751</v>
       </c>
       <c r="T48" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U48" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V48" t="s">
         <v>2248</v>
@@ -29892,22 +30153,22 @@
         <v>2249</v>
       </c>
       <c r="X48" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y48" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z48" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA48" t="s">
-        <v>2315</v>
+        <v>2377</v>
       </c>
       <c r="AB48" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AC48" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD48" t="s">
         <v>2254</v>
@@ -29916,16 +30177,16 @@
         <v>2271</v>
       </c>
       <c r="AF48" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG48" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH48" t="s">
         <v>2332</v>
       </c>
       <c r="AI48" t="s">
-        <v>672</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.25">
@@ -29936,13 +30197,13 @@
         <v>1756</v>
       </c>
       <c r="C49" t="s">
-        <v>653</v>
+        <v>286</v>
       </c>
       <c r="D49" t="s">
-        <v>2235</v>
+        <v>2483</v>
       </c>
       <c r="E49" t="s">
-        <v>1570</v>
+        <v>2522</v>
       </c>
       <c r="G49" t="s">
         <v>706</v>
@@ -29954,10 +30215,10 @@
         <v>1755</v>
       </c>
       <c r="T49" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U49" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V49" t="s">
         <v>2248</v>
@@ -29966,22 +30227,22 @@
         <v>2249</v>
       </c>
       <c r="X49" t="s">
-        <v>2278</v>
+        <v>680</v>
       </c>
       <c r="Y49" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z49" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA49" t="s">
-        <v>2315</v>
+        <v>2377</v>
       </c>
       <c r="AB49" t="s">
         <v>2311</v>
       </c>
       <c r="AC49" t="s">
-        <v>2317</v>
+        <v>1428</v>
       </c>
       <c r="AD49" t="s">
         <v>2254</v>
@@ -29990,16 +30251,16 @@
         <v>2271</v>
       </c>
       <c r="AF49" t="s">
-        <v>2260</v>
+        <v>1235</v>
       </c>
       <c r="AG49" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AH49" t="s">
         <v>2332</v>
       </c>
       <c r="AI49" t="s">
-        <v>653</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.25">
@@ -30010,13 +30271,13 @@
         <v>2119</v>
       </c>
       <c r="C50" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
       <c r="D50" t="s">
-        <v>2235</v>
+        <v>2524</v>
       </c>
       <c r="E50" t="s">
-        <v>1524</v>
+        <v>2523</v>
       </c>
       <c r="G50" t="s">
         <v>706</v>
@@ -30028,10 +30289,10 @@
         <v>2118</v>
       </c>
       <c r="T50" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U50" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V50" t="s">
         <v>2248</v>
@@ -30046,16 +30307,16 @@
         <v>2309</v>
       </c>
       <c r="Z50" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AA50" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="AB50" t="s">
         <v>2293</v>
       </c>
       <c r="AC50" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AD50" t="s">
         <v>2311</v>
@@ -30067,13 +30328,13 @@
         <v>2294</v>
       </c>
       <c r="AG50" t="s">
-        <v>2347</v>
+        <v>2459</v>
       </c>
       <c r="AH50" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI50" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.25">
@@ -30084,13 +30345,13 @@
         <v>2121</v>
       </c>
       <c r="C51" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
       <c r="D51" t="s">
-        <v>2235</v>
+        <v>2524</v>
       </c>
       <c r="E51" t="s">
-        <v>1524</v>
+        <v>1546</v>
       </c>
       <c r="G51" t="s">
         <v>672</v>
@@ -30102,10 +30363,10 @@
         <v>2120</v>
       </c>
       <c r="T51" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U51" t="s">
-        <v>2247</v>
+        <v>2387</v>
       </c>
       <c r="V51" t="s">
         <v>2280</v>
@@ -30117,16 +30378,16 @@
         <v>2248</v>
       </c>
       <c r="Y51" t="s">
-        <v>2252</v>
+        <v>2388</v>
       </c>
       <c r="Z51" t="s">
         <v>2276</v>
       </c>
       <c r="AA51" t="s">
-        <v>2251</v>
+        <v>721</v>
       </c>
       <c r="AB51" t="s">
-        <v>2268</v>
+        <v>2396</v>
       </c>
       <c r="AC51" t="s">
         <v>2309</v>
@@ -30135,19 +30396,19 @@
         <v>2311</v>
       </c>
       <c r="AE51" t="s">
-        <v>2255</v>
+        <v>2389</v>
       </c>
       <c r="AF51" t="s">
-        <v>2279</v>
+        <v>1416</v>
       </c>
       <c r="AG51" t="s">
         <v>2294</v>
       </c>
       <c r="AH51" t="s">
-        <v>2258</v>
+        <v>2391</v>
       </c>
       <c r="AI51" t="s">
-        <v>672</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
am commit check gw13
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14437" uniqueCount="2544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15541" uniqueCount="2615">
   <si>
     <t>Places</t>
   </si>
@@ -7666,6 +7666,219 @@
   </si>
   <si>
     <t>611</t>
+  </si>
+  <si>
+    <t>Reguilón -</t>
+  </si>
+  <si>
+    <t>Thiago Silva MUN (H)</t>
+  </si>
+  <si>
+    <t>Rashica 3</t>
+  </si>
+  <si>
+    <t>Benrahma 1</t>
+  </si>
+  <si>
+    <t>Son -</t>
+  </si>
+  <si>
+    <t>Vardy 9</t>
+  </si>
+  <si>
+    <t>1,427,331</t>
+  </si>
+  <si>
+    <t>727</t>
+  </si>
+  <si>
+    <t>Kane -</t>
+  </si>
+  <si>
+    <t>Foster 0</t>
+  </si>
+  <si>
+    <t>Brownhill -</t>
+  </si>
+  <si>
+    <t>102,907</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>Dier -</t>
+  </si>
+  <si>
+    <t>Jesus 1</t>
+  </si>
+  <si>
+    <t>121,672</t>
+  </si>
+  <si>
+    <t>835</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold 18$ captain</t>
+  </si>
+  <si>
+    <t>Dennis 4</t>
+  </si>
+  <si>
+    <t>Gray 0</t>
+  </si>
+  <si>
+    <t>Jansson 6</t>
+  </si>
+  <si>
+    <t>617,204</t>
+  </si>
+  <si>
+    <t>van Dijk 15</t>
+  </si>
+  <si>
+    <t>1,014,596</t>
+  </si>
+  <si>
+    <t>Townsend 1</t>
+  </si>
+  <si>
+    <t>2,138,584</t>
+  </si>
+  <si>
+    <t>697</t>
+  </si>
+  <si>
+    <t>1,944,315</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>Skipp -</t>
+  </si>
+  <si>
+    <t>Jesus 2$ captain</t>
+  </si>
+  <si>
+    <t>Wan-Bissaka CHE (A)</t>
+  </si>
+  <si>
+    <t>5,191,746</t>
+  </si>
+  <si>
+    <t>573</t>
+  </si>
+  <si>
+    <t>Vardy 10</t>
+  </si>
+  <si>
+    <t>Dennis 9</t>
+  </si>
+  <si>
+    <t>412,695</t>
+  </si>
+  <si>
+    <t>Keane 2</t>
+  </si>
+  <si>
+    <t>Dallas 3</t>
+  </si>
+  <si>
+    <t>2,257,692</t>
+  </si>
+  <si>
+    <t>Pinnock 6</t>
+  </si>
+  <si>
+    <t>3,382,519</t>
+  </si>
+  <si>
+    <t>648</t>
+  </si>
+  <si>
+    <t>Watkins 2</t>
+  </si>
+  <si>
+    <t>Højbjerg -</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>1,915,378</t>
+  </si>
+  <si>
+    <t>Kane -$ captain</t>
+  </si>
+  <si>
+    <t>Aarons 6</t>
+  </si>
+  <si>
+    <t>5,471,016</t>
+  </si>
+  <si>
+    <t>561</t>
+  </si>
+  <si>
+    <t>Willock 2</t>
+  </si>
+  <si>
+    <t>5,585,339</t>
+  </si>
+  <si>
+    <t>556</t>
+  </si>
+  <si>
+    <t>Mings 2</t>
+  </si>
+  <si>
+    <t>Mount MUN (H)</t>
+  </si>
+  <si>
+    <t>Lukaku MUN (H)$ captain</t>
+  </si>
+  <si>
+    <t>Bednarek -1</t>
+  </si>
+  <si>
+    <t>7,731,166</t>
+  </si>
+  <si>
+    <t>Cancelo 5</t>
+  </si>
+  <si>
+    <t>Cornet -</t>
+  </si>
+  <si>
+    <t>Walker 6</t>
+  </si>
+  <si>
+    <t>Bergwijn -</t>
+  </si>
+  <si>
+    <t>Mbeumo 3</t>
+  </si>
+  <si>
+    <t>Scarlett -</t>
+  </si>
+  <si>
+    <t>Bernardo 3</t>
+  </si>
+  <si>
+    <t>Lloris -</t>
+  </si>
+  <si>
+    <t>Richardson -</t>
+  </si>
+  <si>
+    <t>Castagne 1</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Emerson Royal -</t>
   </si>
 </sst>
 </file>
@@ -8499,26 +8712,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="21" max="22" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="27" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="15.734375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.64453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="15.64453125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="19.62890625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="17.14453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -8642,13 +8859,13 @@
         <v>5695560</v>
       </c>
       <c r="C2" t="s">
-        <v>288</v>
+        <v>2491</v>
       </c>
       <c r="D2" t="s">
-        <v>1933</v>
+        <v>2551</v>
       </c>
       <c r="E2" t="s">
-        <v>2062</v>
+        <v>2550</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -8660,52 +8877,52 @@
         <v>882</v>
       </c>
       <c r="T2" t="s">
-        <v>1974</v>
+        <v>1294</v>
       </c>
       <c r="U2" t="s">
-        <v>2022</v>
+        <v>2544</v>
       </c>
       <c r="V2" t="s">
-        <v>1854</v>
+        <v>2545</v>
       </c>
       <c r="W2" t="s">
-        <v>1847</v>
+        <v>968</v>
       </c>
       <c r="X2" t="s">
-        <v>1975</v>
+        <v>2388</v>
       </c>
       <c r="Y2" t="s">
-        <v>738</v>
+        <v>2546</v>
       </c>
       <c r="Z2" t="s">
-        <v>383</v>
+        <v>2547</v>
       </c>
       <c r="AA2" t="s">
-        <v>1923</v>
+        <v>2548</v>
       </c>
       <c r="AB2" t="s">
-        <v>894</v>
+        <v>2549</v>
       </c>
       <c r="AC2" t="s">
-        <v>682</v>
+        <v>1414</v>
       </c>
       <c r="AD2" t="s">
-        <v>1492</v>
+        <v>956</v>
       </c>
       <c r="AE2" t="s">
         <v>880</v>
       </c>
       <c r="AF2" t="s">
-        <v>687</v>
+        <v>750</v>
       </c>
       <c r="AG2" t="s">
-        <v>1929</v>
+        <v>2397</v>
       </c>
       <c r="AH2" t="s">
         <v>881</v>
       </c>
       <c r="AI2" t="s">
-        <v>288</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -8716,16 +8933,16 @@
         <v>1153704</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>2246</v>
       </c>
       <c r="D3" t="s">
-        <v>1892</v>
+        <v>2556</v>
       </c>
       <c r="E3" t="s">
-        <v>2063</v>
+        <v>2555</v>
       </c>
       <c r="G3" t="s">
-        <v>672</v>
+        <v>452</v>
       </c>
       <c r="R3" t="s">
         <v>885</v>
@@ -8734,52 +8951,52 @@
         <v>884</v>
       </c>
       <c r="T3" t="s">
-        <v>1912</v>
+        <v>1498</v>
       </c>
       <c r="U3" t="s">
-        <v>2016</v>
+        <v>1233</v>
       </c>
       <c r="V3" t="s">
-        <v>1921</v>
+        <v>2387</v>
       </c>
       <c r="W3" t="s">
-        <v>1852</v>
+        <v>2248</v>
       </c>
       <c r="X3" t="s">
-        <v>425</v>
+        <v>968</v>
       </c>
       <c r="Y3" t="s">
-        <v>817</v>
+        <v>2280</v>
       </c>
       <c r="Z3" t="s">
-        <v>1425</v>
+        <v>1250</v>
       </c>
       <c r="AA3" t="s">
-        <v>1923</v>
+        <v>438</v>
       </c>
       <c r="AB3" t="s">
-        <v>1976</v>
+        <v>2388</v>
       </c>
       <c r="AC3" t="s">
-        <v>682</v>
+        <v>721</v>
       </c>
       <c r="AD3" t="s">
-        <v>1268</v>
+        <v>2552</v>
       </c>
       <c r="AE3" t="s">
-        <v>1905</v>
+        <v>2553</v>
       </c>
       <c r="AF3" t="s">
-        <v>687</v>
+        <v>956</v>
       </c>
       <c r="AG3" t="s">
-        <v>1214</v>
+        <v>2554</v>
       </c>
       <c r="AH3" t="s">
         <v>532</v>
       </c>
       <c r="AI3" t="s">
-        <v>280</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -8790,16 +9007,16 @@
         <v>440807</v>
       </c>
       <c r="C4" t="s">
-        <v>1564</v>
+        <v>778</v>
       </c>
       <c r="D4" t="s">
-        <v>1459</v>
+        <v>2049</v>
       </c>
       <c r="E4" t="s">
-        <v>2032</v>
+        <v>2416</v>
       </c>
       <c r="G4" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R4" t="s">
         <v>418</v>
@@ -8808,52 +9025,52 @@
         <v>289</v>
       </c>
       <c r="T4" t="s">
-        <v>1977</v>
+        <v>1498</v>
       </c>
       <c r="U4" t="s">
-        <v>1938</v>
+        <v>968</v>
       </c>
       <c r="V4" t="s">
-        <v>2018</v>
+        <v>2291</v>
       </c>
       <c r="W4" t="s">
-        <v>1850</v>
+        <v>2380</v>
       </c>
       <c r="X4" t="s">
-        <v>1909</v>
+        <v>2557</v>
       </c>
       <c r="Y4" t="s">
-        <v>425</v>
+        <v>2307</v>
       </c>
       <c r="Z4" t="s">
-        <v>1902</v>
+        <v>2388</v>
       </c>
       <c r="AA4" t="s">
-        <v>1220</v>
+        <v>691</v>
       </c>
       <c r="AB4" t="s">
-        <v>1923</v>
+        <v>721</v>
       </c>
       <c r="AC4" t="s">
-        <v>682</v>
+        <v>2549</v>
       </c>
       <c r="AD4" t="s">
         <v>1416</v>
       </c>
       <c r="AE4" t="s">
-        <v>1912</v>
+        <v>777</v>
       </c>
       <c r="AF4" t="s">
-        <v>687</v>
+        <v>438</v>
       </c>
       <c r="AG4" t="s">
-        <v>1976</v>
+        <v>956</v>
       </c>
       <c r="AH4" t="s">
-        <v>1492</v>
+        <v>2391</v>
       </c>
       <c r="AI4" t="s">
-        <v>1564</v>
+        <v>778</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -8864,16 +9081,16 @@
         <v>4642646</v>
       </c>
       <c r="C5" t="s">
-        <v>1264</v>
+        <v>282</v>
       </c>
       <c r="D5" t="s">
-        <v>2065</v>
+        <v>2560</v>
       </c>
       <c r="E5" t="s">
-        <v>2064</v>
+        <v>2559</v>
       </c>
       <c r="G5" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R5" t="s">
         <v>887</v>
@@ -8882,52 +9099,52 @@
         <v>886</v>
       </c>
       <c r="T5" t="s">
-        <v>1905</v>
+        <v>2389</v>
       </c>
       <c r="U5" t="s">
-        <v>1921</v>
+        <v>2248</v>
       </c>
       <c r="V5" t="s">
-        <v>1922</v>
+        <v>1233</v>
       </c>
       <c r="W5" t="s">
-        <v>1850</v>
+        <v>2387</v>
       </c>
       <c r="X5" t="s">
-        <v>2016</v>
+        <v>2388</v>
       </c>
       <c r="Y5" t="s">
-        <v>1909</v>
+        <v>2548</v>
       </c>
       <c r="Z5" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
       <c r="AA5" t="s">
-        <v>1923</v>
+        <v>691</v>
       </c>
       <c r="AB5" t="s">
-        <v>425</v>
+        <v>2558</v>
       </c>
       <c r="AC5" t="s">
-        <v>1948</v>
+        <v>1428</v>
       </c>
       <c r="AD5" t="s">
         <v>1910</v>
       </c>
       <c r="AE5" t="s">
-        <v>1857</v>
+        <v>2553</v>
       </c>
       <c r="AF5" t="s">
-        <v>953</v>
+        <v>2380</v>
       </c>
       <c r="AG5" t="s">
-        <v>1408</v>
+        <v>680</v>
       </c>
       <c r="AH5" t="s">
-        <v>1978</v>
+        <v>2391</v>
       </c>
       <c r="AI5" t="s">
-        <v>1264</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -8938,16 +9155,16 @@
         <v>1364835</v>
       </c>
       <c r="C6" t="s">
-        <v>1264</v>
+        <v>778</v>
       </c>
       <c r="D6" t="s">
-        <v>2067</v>
+        <v>1521</v>
       </c>
       <c r="E6" t="s">
-        <v>2066</v>
+        <v>2565</v>
       </c>
       <c r="G6" t="s">
-        <v>706</v>
+        <v>452</v>
       </c>
       <c r="R6" t="s">
         <v>889</v>
@@ -8956,52 +9173,52 @@
         <v>888</v>
       </c>
       <c r="T6" t="s">
-        <v>1216</v>
+        <v>2289</v>
       </c>
       <c r="U6" t="s">
-        <v>1852</v>
+        <v>2248</v>
       </c>
       <c r="V6" t="s">
-        <v>1921</v>
+        <v>2561</v>
       </c>
       <c r="W6" t="s">
-        <v>2016</v>
+        <v>1233</v>
       </c>
       <c r="X6" t="s">
-        <v>1858</v>
+        <v>1235</v>
       </c>
       <c r="Y6" t="s">
-        <v>1253</v>
+        <v>2548</v>
       </c>
       <c r="Z6" t="s">
-        <v>383</v>
+        <v>2421</v>
       </c>
       <c r="AA6" t="s">
-        <v>1923</v>
+        <v>691</v>
       </c>
       <c r="AB6" t="s">
-        <v>1902</v>
+        <v>2562</v>
       </c>
       <c r="AC6" t="s">
-        <v>1492</v>
+        <v>2549</v>
       </c>
       <c r="AD6" t="s">
-        <v>1924</v>
+        <v>692</v>
       </c>
       <c r="AE6" t="s">
-        <v>1410</v>
+        <v>2553</v>
       </c>
       <c r="AF6" t="s">
         <v>805</v>
       </c>
       <c r="AG6" t="s">
-        <v>1979</v>
+        <v>2563</v>
       </c>
       <c r="AH6" t="s">
-        <v>1940</v>
+        <v>2564</v>
       </c>
       <c r="AI6" t="s">
-        <v>1264</v>
+        <v>778</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -9012,16 +9229,16 @@
         <v>5306515</v>
       </c>
       <c r="C7" t="s">
-        <v>1260</v>
+        <v>785</v>
       </c>
       <c r="D7" t="s">
-        <v>2069</v>
+        <v>1453</v>
       </c>
       <c r="E7" t="s">
-        <v>2068</v>
+        <v>2567</v>
       </c>
       <c r="G7" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R7" t="s">
         <v>897</v>
@@ -9030,52 +9247,52 @@
         <v>896</v>
       </c>
       <c r="T7" t="s">
-        <v>1915</v>
+        <v>2242</v>
       </c>
       <c r="U7" t="s">
-        <v>1850</v>
+        <v>2566</v>
       </c>
       <c r="V7" t="s">
-        <v>1922</v>
+        <v>968</v>
       </c>
       <c r="W7" t="s">
-        <v>950</v>
+        <v>2248</v>
       </c>
       <c r="X7" t="s">
-        <v>1911</v>
+        <v>2391</v>
       </c>
       <c r="Y7" t="s">
-        <v>1980</v>
+        <v>2547</v>
       </c>
       <c r="Z7" t="s">
-        <v>738</v>
+        <v>2388</v>
       </c>
       <c r="AA7" t="s">
-        <v>1902</v>
+        <v>680</v>
       </c>
       <c r="AB7" t="s">
-        <v>817</v>
+        <v>691</v>
       </c>
       <c r="AC7" t="s">
-        <v>1924</v>
+        <v>956</v>
       </c>
       <c r="AD7" t="s">
-        <v>682</v>
+        <v>2558</v>
       </c>
       <c r="AE7" t="s">
         <v>1974</v>
       </c>
       <c r="AF7" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
       <c r="AG7" t="s">
-        <v>953</v>
+        <v>2420</v>
       </c>
       <c r="AH7" t="s">
-        <v>1978</v>
+        <v>2554</v>
       </c>
       <c r="AI7" t="s">
-        <v>1260</v>
+        <v>785</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -9086,16 +9303,16 @@
         <v>2249991</v>
       </c>
       <c r="C8" t="s">
-        <v>703</v>
+        <v>829</v>
       </c>
       <c r="D8" t="s">
-        <v>1379</v>
+        <v>2570</v>
       </c>
       <c r="E8" t="s">
-        <v>2070</v>
+        <v>2569</v>
       </c>
       <c r="G8" t="s">
-        <v>672</v>
+        <v>706</v>
       </c>
       <c r="R8" t="s">
         <v>899</v>
@@ -9104,52 +9321,52 @@
         <v>898</v>
       </c>
       <c r="T8" t="s">
+        <v>2389</v>
+      </c>
+      <c r="U8" t="s">
+        <v>2557</v>
+      </c>
+      <c r="V8" t="s">
+        <v>2248</v>
+      </c>
+      <c r="W8" t="s">
+        <v>968</v>
+      </c>
+      <c r="X8" t="s">
+        <v>691</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>2568</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>2388</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>956</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>2263</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AE8" t="s">
         <v>1974</v>
       </c>
-      <c r="U8" t="s">
-        <v>1858</v>
-      </c>
-      <c r="V8" t="s">
-        <v>1852</v>
-      </c>
-      <c r="W8" t="s">
-        <v>1850</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="AF8" t="s">
         <v>805</v>
       </c>
-      <c r="Y8" t="s">
-        <v>1851</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>977</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>1923</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>1904</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>682</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>1924</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>1857</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>687</v>
-      </c>
       <c r="AG8" t="s">
-        <v>2018</v>
+        <v>1235</v>
       </c>
       <c r="AH8" t="s">
-        <v>1902</v>
+        <v>2391</v>
       </c>
       <c r="AI8" t="s">
-        <v>703</v>
+        <v>829</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -9160,13 +9377,13 @@
         <v>2056865</v>
       </c>
       <c r="C9" t="s">
-        <v>319</v>
+        <v>268</v>
       </c>
       <c r="D9" t="s">
-        <v>1366</v>
+        <v>2572</v>
       </c>
       <c r="E9" t="s">
-        <v>2071</v>
+        <v>2571</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -9178,52 +9395,52 @@
         <v>901</v>
       </c>
       <c r="T9" t="s">
-        <v>1216</v>
+        <v>2289</v>
       </c>
       <c r="U9" t="s">
-        <v>1981</v>
+        <v>2387</v>
       </c>
       <c r="V9" t="s">
-        <v>1921</v>
+        <v>968</v>
       </c>
       <c r="W9" t="s">
-        <v>1922</v>
+        <v>2248</v>
       </c>
       <c r="X9" t="s">
-        <v>1902</v>
+        <v>691</v>
       </c>
       <c r="Y9" t="s">
-        <v>1979</v>
+        <v>2388</v>
       </c>
       <c r="Z9" t="s">
-        <v>425</v>
+        <v>737</v>
       </c>
       <c r="AA9" t="s">
-        <v>1851</v>
+        <v>721</v>
       </c>
       <c r="AB9" t="s">
-        <v>1934</v>
+        <v>2396</v>
       </c>
       <c r="AC9" t="s">
-        <v>900</v>
+        <v>1416</v>
       </c>
       <c r="AD9" t="s">
-        <v>1416</v>
+        <v>2552</v>
       </c>
       <c r="AE9" t="s">
-        <v>1905</v>
+        <v>2553</v>
       </c>
       <c r="AF9" t="s">
-        <v>687</v>
+        <v>2533</v>
       </c>
       <c r="AG9" t="s">
-        <v>1253</v>
+        <v>2564</v>
       </c>
       <c r="AH9" t="s">
         <v>1982</v>
       </c>
       <c r="AI9" t="s">
-        <v>319</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -9234,13 +9451,13 @@
         <v>5142355</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>2461</v>
       </c>
       <c r="D10" t="s">
-        <v>2074</v>
+        <v>2577</v>
       </c>
       <c r="E10" t="s">
-        <v>2073</v>
+        <v>2576</v>
       </c>
       <c r="G10" t="s">
         <v>653</v>
@@ -9252,52 +9469,52 @@
         <v>913</v>
       </c>
       <c r="T10" t="s">
-        <v>1945</v>
+        <v>2417</v>
       </c>
       <c r="U10" t="s">
-        <v>1985</v>
+        <v>2420</v>
       </c>
       <c r="V10" t="s">
-        <v>2018</v>
+        <v>2557</v>
       </c>
       <c r="W10" t="s">
-        <v>1911</v>
+        <v>968</v>
       </c>
       <c r="X10" t="s">
-        <v>1859</v>
+        <v>805</v>
       </c>
       <c r="Y10" t="s">
-        <v>805</v>
+        <v>2421</v>
       </c>
       <c r="Z10" t="s">
         <v>413</v>
       </c>
       <c r="AA10" t="s">
-        <v>2072</v>
+        <v>2573</v>
       </c>
       <c r="AB10" t="s">
-        <v>1904</v>
+        <v>2463</v>
       </c>
       <c r="AC10" t="s">
-        <v>1984</v>
+        <v>2263</v>
       </c>
       <c r="AD10" t="s">
-        <v>1418</v>
+        <v>2574</v>
       </c>
       <c r="AE10" t="s">
-        <v>570</v>
+        <v>2393</v>
       </c>
       <c r="AF10" t="s">
-        <v>687</v>
+        <v>2575</v>
       </c>
       <c r="AG10" t="s">
-        <v>1224</v>
+        <v>959</v>
       </c>
       <c r="AH10" t="s">
-        <v>1983</v>
+        <v>2425</v>
       </c>
       <c r="AI10" t="s">
-        <v>268</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -9308,16 +9525,16 @@
         <v>1628438</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="D11" t="s">
-        <v>1447</v>
+        <v>1548</v>
       </c>
       <c r="E11" t="s">
-        <v>2075</v>
+        <v>2580</v>
       </c>
       <c r="G11" t="s">
-        <v>452</v>
+        <v>653</v>
       </c>
       <c r="R11" t="s">
         <v>916</v>
@@ -9326,52 +9543,52 @@
         <v>915</v>
       </c>
       <c r="T11" t="s">
-        <v>1913</v>
+        <v>1498</v>
       </c>
       <c r="U11" t="s">
-        <v>1938</v>
+        <v>2387</v>
       </c>
       <c r="V11" t="s">
-        <v>1850</v>
+        <v>2544</v>
       </c>
       <c r="W11" t="s">
-        <v>1922</v>
+        <v>1233</v>
       </c>
       <c r="X11" t="s">
-        <v>1858</v>
+        <v>2248</v>
       </c>
       <c r="Y11" t="s">
-        <v>383</v>
+        <v>2388</v>
       </c>
       <c r="Z11" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
       <c r="AA11" t="s">
-        <v>1934</v>
+        <v>2548</v>
       </c>
       <c r="AB11" t="s">
-        <v>1940</v>
+        <v>2396</v>
       </c>
       <c r="AC11" t="s">
-        <v>1416</v>
+        <v>2578</v>
       </c>
       <c r="AD11" t="s">
-        <v>1906</v>
+        <v>2579</v>
       </c>
       <c r="AE11" t="s">
-        <v>1857</v>
+        <v>804</v>
       </c>
       <c r="AF11" t="s">
-        <v>687</v>
+        <v>1235</v>
       </c>
       <c r="AG11" t="s">
-        <v>953</v>
+        <v>2412</v>
       </c>
       <c r="AH11" t="s">
-        <v>1979</v>
+        <v>532</v>
       </c>
       <c r="AI11" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -9382,13 +9599,13 @@
         <v>1427447</v>
       </c>
       <c r="C12" t="s">
-        <v>1551</v>
+        <v>2246</v>
       </c>
       <c r="D12" t="s">
-        <v>2078</v>
+        <v>1297</v>
       </c>
       <c r="E12" t="s">
-        <v>2077</v>
+        <v>2583</v>
       </c>
       <c r="G12" t="s">
         <v>653</v>
@@ -9400,52 +9617,52 @@
         <v>918</v>
       </c>
       <c r="T12" t="s">
-        <v>1915</v>
+        <v>2242</v>
       </c>
       <c r="U12" t="s">
-        <v>1921</v>
+        <v>2387</v>
       </c>
       <c r="V12" t="s">
-        <v>538</v>
+        <v>2581</v>
       </c>
       <c r="W12" t="s">
-        <v>2016</v>
+        <v>968</v>
       </c>
       <c r="X12" t="s">
-        <v>1253</v>
+        <v>1233</v>
       </c>
       <c r="Y12" t="s">
-        <v>2076</v>
+        <v>2388</v>
       </c>
       <c r="Z12" t="s">
-        <v>977</v>
+        <v>680</v>
       </c>
       <c r="AA12" t="s">
-        <v>738</v>
+        <v>2568</v>
       </c>
       <c r="AB12" t="s">
-        <v>1923</v>
+        <v>2547</v>
       </c>
       <c r="AC12" t="s">
-        <v>1904</v>
+        <v>2263</v>
       </c>
       <c r="AD12" t="s">
         <v>1416</v>
       </c>
       <c r="AE12" t="s">
-        <v>1905</v>
+        <v>2553</v>
       </c>
       <c r="AF12" t="s">
-        <v>687</v>
+        <v>2582</v>
       </c>
       <c r="AG12" t="s">
-        <v>953</v>
+        <v>2564</v>
       </c>
       <c r="AH12" t="s">
-        <v>1940</v>
+        <v>2579</v>
       </c>
       <c r="AI12" t="s">
-        <v>1551</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -9456,16 +9673,16 @@
         <v>5648774</v>
       </c>
       <c r="C13" t="s">
-        <v>771</v>
+        <v>272</v>
       </c>
       <c r="D13" t="s">
-        <v>1988</v>
+        <v>2586</v>
       </c>
       <c r="E13" t="s">
-        <v>2079</v>
+        <v>2585</v>
       </c>
       <c r="G13" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R13" t="s">
         <v>922</v>
@@ -9474,52 +9691,52 @@
         <v>921</v>
       </c>
       <c r="T13" t="s">
-        <v>1860</v>
+        <v>411</v>
       </c>
       <c r="U13" t="s">
-        <v>1858</v>
+        <v>1235</v>
       </c>
       <c r="V13" t="s">
-        <v>1850</v>
+        <v>2391</v>
       </c>
       <c r="W13" t="s">
-        <v>1249</v>
+        <v>2584</v>
       </c>
       <c r="X13" t="s">
-        <v>1916</v>
+        <v>395</v>
       </c>
       <c r="Y13" t="s">
-        <v>1923</v>
+        <v>2388</v>
       </c>
       <c r="Z13" t="s">
-        <v>1851</v>
+        <v>2396</v>
       </c>
       <c r="AA13" t="s">
-        <v>738</v>
+        <v>2547</v>
       </c>
       <c r="AB13" t="s">
         <v>1861</v>
       </c>
       <c r="AC13" t="s">
-        <v>1904</v>
+        <v>2263</v>
       </c>
       <c r="AD13" t="s">
-        <v>1492</v>
+        <v>2578</v>
       </c>
       <c r="AE13" t="s">
         <v>399</v>
       </c>
       <c r="AF13" t="s">
-        <v>1859</v>
+        <v>2425</v>
       </c>
       <c r="AG13" t="s">
-        <v>1987</v>
+        <v>1196</v>
       </c>
       <c r="AH13" t="s">
         <v>920</v>
       </c>
       <c r="AI13" t="s">
-        <v>771</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -9530,16 +9747,16 @@
         <v>3452385</v>
       </c>
       <c r="C14" t="s">
-        <v>297</v>
+        <v>2589</v>
       </c>
       <c r="D14" t="s">
-        <v>1376</v>
+        <v>1593</v>
       </c>
       <c r="E14" t="s">
-        <v>2080</v>
+        <v>2590</v>
       </c>
       <c r="G14" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R14" t="s">
         <v>925</v>
@@ -9551,40 +9768,40 @@
         <v>717</v>
       </c>
       <c r="U14" t="s">
-        <v>1922</v>
+        <v>2248</v>
       </c>
       <c r="V14" t="s">
-        <v>2022</v>
+        <v>2544</v>
       </c>
       <c r="W14" t="s">
-        <v>1916</v>
+        <v>395</v>
       </c>
       <c r="X14" t="s">
-        <v>738</v>
+        <v>2547</v>
       </c>
       <c r="Y14" t="s">
-        <v>1934</v>
+        <v>2388</v>
       </c>
       <c r="Z14" t="s">
-        <v>1918</v>
+        <v>2568</v>
       </c>
       <c r="AA14" t="s">
-        <v>1220</v>
+        <v>737</v>
       </c>
       <c r="AB14" t="s">
-        <v>682</v>
+        <v>956</v>
       </c>
       <c r="AC14" t="s">
-        <v>1906</v>
+        <v>2263</v>
       </c>
       <c r="AD14" t="s">
-        <v>1989</v>
+        <v>2587</v>
       </c>
       <c r="AE14" t="s">
         <v>923</v>
       </c>
       <c r="AF14" t="s">
-        <v>2028</v>
+        <v>2588</v>
       </c>
       <c r="AG14" t="s">
         <v>685</v>
@@ -9593,7 +9810,7 @@
         <v>1990</v>
       </c>
       <c r="AI14" t="s">
-        <v>297</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -9604,16 +9821,16 @@
         <v>2297330</v>
       </c>
       <c r="C15" t="s">
-        <v>288</v>
+        <v>2381</v>
       </c>
       <c r="D15" t="s">
-        <v>2082</v>
+        <v>2594</v>
       </c>
       <c r="E15" t="s">
-        <v>2081</v>
+        <v>2593</v>
       </c>
       <c r="G15" t="s">
-        <v>452</v>
+        <v>706</v>
       </c>
       <c r="R15" t="s">
         <v>927</v>
@@ -9622,52 +9839,52 @@
         <v>926</v>
       </c>
       <c r="T15" t="s">
-        <v>581</v>
+        <v>2275</v>
       </c>
       <c r="U15" t="s">
-        <v>2022</v>
+        <v>1996</v>
       </c>
       <c r="V15" t="s">
-        <v>1996</v>
+        <v>2380</v>
       </c>
       <c r="W15" t="s">
-        <v>1992</v>
+        <v>2544</v>
       </c>
       <c r="X15" t="s">
-        <v>805</v>
+        <v>2548</v>
       </c>
       <c r="Y15" t="s">
+        <v>969</v>
+      </c>
+      <c r="Z15" t="s">
         <v>1993</v>
       </c>
-      <c r="Z15" t="s">
-        <v>425</v>
-      </c>
       <c r="AA15" t="s">
-        <v>383</v>
+        <v>721</v>
       </c>
       <c r="AB15" t="s">
-        <v>1994</v>
+        <v>2591</v>
       </c>
       <c r="AC15" t="s">
-        <v>1906</v>
+        <v>956</v>
       </c>
       <c r="AD15" t="s">
-        <v>1268</v>
+        <v>2263</v>
       </c>
       <c r="AE15" t="s">
         <v>1995</v>
       </c>
       <c r="AF15" t="s">
-        <v>969</v>
+        <v>805</v>
       </c>
       <c r="AG15" t="s">
+        <v>2592</v>
+      </c>
+      <c r="AH15" t="s">
         <v>1427</v>
       </c>
-      <c r="AH15" t="s">
-        <v>1909</v>
-      </c>
       <c r="AI15" t="s">
-        <v>288</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -9678,16 +9895,16 @@
         <v>5361878</v>
       </c>
       <c r="C16" t="s">
-        <v>1949</v>
+        <v>2491</v>
       </c>
       <c r="D16" t="s">
-        <v>2001</v>
+        <v>2597</v>
       </c>
       <c r="E16" t="s">
-        <v>2083</v>
+        <v>2596</v>
       </c>
       <c r="G16" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R16" t="s">
         <v>930</v>
@@ -9696,52 +9913,52 @@
         <v>929</v>
       </c>
       <c r="T16" t="s">
-        <v>1945</v>
+        <v>2417</v>
       </c>
       <c r="U16" t="s">
-        <v>1421</v>
+        <v>1233</v>
       </c>
       <c r="V16" t="s">
-        <v>1997</v>
+        <v>2248</v>
       </c>
       <c r="W16" t="s">
-        <v>1922</v>
+        <v>2280</v>
       </c>
       <c r="X16" t="s">
-        <v>1923</v>
+        <v>2388</v>
       </c>
       <c r="Y16" t="s">
-        <v>1976</v>
+        <v>2595</v>
       </c>
       <c r="Z16" t="s">
-        <v>969</v>
+        <v>2307</v>
       </c>
       <c r="AA16" t="s">
-        <v>1220</v>
+        <v>438</v>
       </c>
       <c r="AB16" t="s">
-        <v>1948</v>
+        <v>1428</v>
       </c>
       <c r="AC16" t="s">
-        <v>1998</v>
+        <v>2441</v>
       </c>
       <c r="AD16" t="s">
-        <v>1418</v>
+        <v>2463</v>
       </c>
       <c r="AE16" t="s">
         <v>717</v>
       </c>
       <c r="AF16" t="s">
+        <v>2281</v>
+      </c>
+      <c r="AG16" t="s">
         <v>1999</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>707</v>
       </c>
       <c r="AH16" t="s">
         <v>2000</v>
       </c>
       <c r="AI16" t="s">
-        <v>1949</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -9752,13 +9969,13 @@
         <v>5344757</v>
       </c>
       <c r="C17" t="s">
-        <v>301</v>
+        <v>2379</v>
       </c>
       <c r="D17" t="s">
-        <v>2086</v>
+        <v>847</v>
       </c>
       <c r="E17" t="s">
-        <v>2085</v>
+        <v>2602</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
@@ -9770,52 +9987,52 @@
         <v>931</v>
       </c>
       <c r="T17" t="s">
-        <v>581</v>
+        <v>2275</v>
       </c>
       <c r="U17" t="s">
-        <v>2002</v>
+        <v>2598</v>
       </c>
       <c r="V17" t="s">
-        <v>1981</v>
+        <v>2533</v>
       </c>
       <c r="W17" t="s">
-        <v>1854</v>
+        <v>2545</v>
       </c>
       <c r="X17" t="s">
-        <v>2003</v>
+        <v>739</v>
       </c>
       <c r="Y17" t="s">
-        <v>2004</v>
+        <v>2599</v>
       </c>
       <c r="Z17" t="s">
-        <v>1500</v>
+        <v>969</v>
       </c>
       <c r="AA17" t="s">
-        <v>1862</v>
+        <v>691</v>
       </c>
       <c r="AB17" t="s">
-        <v>1902</v>
+        <v>2341</v>
       </c>
       <c r="AC17" t="s">
-        <v>2084</v>
+        <v>2263</v>
       </c>
       <c r="AD17" t="s">
-        <v>1940</v>
+        <v>2600</v>
       </c>
       <c r="AE17" t="s">
-        <v>1905</v>
+        <v>2553</v>
       </c>
       <c r="AF17" t="s">
-        <v>969</v>
+        <v>2601</v>
       </c>
       <c r="AG17" t="s">
-        <v>1200</v>
+        <v>2424</v>
       </c>
       <c r="AH17" t="s">
-        <v>1354</v>
+        <v>2579</v>
       </c>
       <c r="AI17" t="s">
-        <v>301</v>
+        <v>2379</v>
       </c>
     </row>
   </sheetData>
@@ -10752,21 +10969,21 @@
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="19.1796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="21.71875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="15.734375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="18.8046875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="21.2578125" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="15.64453125" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="18.27734375" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.82421875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="16.46484375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="16.859375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="16.46484375" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -10891,7 +11108,7 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>712</v>
+        <v>286</v>
       </c>
       <c r="D2" t="s">
         <v>1842</v>
@@ -10918,13 +11135,13 @@
         <v>2248</v>
       </c>
       <c r="W2" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X2" t="s">
         <v>2380</v>
       </c>
       <c r="Y2" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="Z2" t="s">
         <v>721</v>
@@ -10936,7 +11153,7 @@
         <v>2253</v>
       </c>
       <c r="AC2" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD2" t="s">
         <v>692</v>
@@ -10945,7 +11162,7 @@
         <v>2389</v>
       </c>
       <c r="AF2" t="s">
-        <v>2256</v>
+        <v>2568</v>
       </c>
       <c r="AG2" t="s">
         <v>2390</v>
@@ -10954,7 +11171,7 @@
         <v>2391</v>
       </c>
       <c r="AI2" t="s">
-        <v>712</v>
+        <v>286</v>
       </c>
       <c r="AJ2" t="s">
         <v>1840</v>
@@ -10971,7 +11188,7 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>2394</v>
+        <v>778</v>
       </c>
       <c r="D3" t="s">
         <v>1991</v>
@@ -10995,7 +11212,7 @@
         <v>2391</v>
       </c>
       <c r="V3" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W3" t="s">
         <v>2387</v>
@@ -11013,19 +11230,19 @@
         <v>691</v>
       </c>
       <c r="AB3" t="s">
-        <v>2262</v>
+        <v>2604</v>
       </c>
       <c r="AC3" t="s">
         <v>2263</v>
       </c>
       <c r="AD3" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE3" t="s">
         <v>2389</v>
       </c>
       <c r="AF3" t="s">
-        <v>2264</v>
+        <v>1979</v>
       </c>
       <c r="AG3" t="s">
         <v>710</v>
@@ -11034,7 +11251,7 @@
         <v>946</v>
       </c>
       <c r="AI3" t="s">
-        <v>2394</v>
+        <v>778</v>
       </c>
       <c r="AJ3" t="s">
         <v>1927</v>
@@ -11051,7 +11268,7 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>1499</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
         <v>1561</v>
@@ -11069,7 +11286,7 @@
         <v>722</v>
       </c>
       <c r="T4" t="s">
-        <v>2267</v>
+        <v>947</v>
       </c>
       <c r="U4" t="s">
         <v>2248</v>
@@ -11096,25 +11313,25 @@
         <v>700</v>
       </c>
       <c r="AC4" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AD4" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE4" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF4" t="s">
         <v>2397</v>
       </c>
       <c r="AG4" t="s">
-        <v>2273</v>
+        <v>2557</v>
       </c>
       <c r="AH4" t="s">
-        <v>2274</v>
+        <v>685</v>
       </c>
       <c r="AI4" t="s">
-        <v>1499</v>
+        <v>294</v>
       </c>
       <c r="AJ4" t="s">
         <v>1931</v>
@@ -11131,7 +11348,7 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>2399</v>
+        <v>2418</v>
       </c>
       <c r="D5" t="s">
         <v>2401</v>
@@ -11155,16 +11372,16 @@
         <v>1235</v>
       </c>
       <c r="V5" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W5" t="s">
         <v>2380</v>
       </c>
       <c r="X5" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="Y5" t="s">
-        <v>2277</v>
+        <v>2588</v>
       </c>
       <c r="Z5" t="s">
         <v>2388</v>
@@ -11179,10 +11396,10 @@
         <v>1416</v>
       </c>
       <c r="AD5" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AE5" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF5" t="s">
         <v>2280</v>
@@ -11194,7 +11411,7 @@
         <v>2281</v>
       </c>
       <c r="AI5" t="s">
-        <v>2399</v>
+        <v>2418</v>
       </c>
       <c r="AJ5" t="s">
         <v>1933</v>
@@ -11211,7 +11428,7 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>841</v>
+        <v>280</v>
       </c>
       <c r="D6" t="s">
         <v>1471</v>
@@ -11235,13 +11452,13 @@
         <v>2402</v>
       </c>
       <c r="V6" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W6" t="s">
-        <v>2283</v>
+        <v>2544</v>
       </c>
       <c r="X6" t="s">
-        <v>2284</v>
+        <v>2605</v>
       </c>
       <c r="Y6" t="s">
         <v>2387</v>
@@ -11250,13 +11467,13 @@
         <v>721</v>
       </c>
       <c r="AA6" t="s">
-        <v>2285</v>
+        <v>2606</v>
       </c>
       <c r="AB6" t="s">
         <v>2388</v>
       </c>
       <c r="AC6" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD6" t="s">
         <v>2263</v>
@@ -11265,7 +11482,7 @@
         <v>411</v>
       </c>
       <c r="AF6" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="AG6" t="s">
         <v>1533</v>
@@ -11274,7 +11491,7 @@
         <v>742</v>
       </c>
       <c r="AI6" t="s">
-        <v>841</v>
+        <v>280</v>
       </c>
       <c r="AJ6" t="s">
         <v>1507</v>
@@ -11291,7 +11508,7 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>2384</v>
+        <v>912</v>
       </c>
       <c r="D7" t="s">
         <v>1404</v>
@@ -11315,7 +11532,7 @@
         <v>1235</v>
       </c>
       <c r="V7" t="s">
-        <v>2284</v>
+        <v>2605</v>
       </c>
       <c r="W7" t="s">
         <v>750</v>
@@ -11336,7 +11553,7 @@
         <v>1416</v>
       </c>
       <c r="AC7" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD7" t="s">
         <v>2263</v>
@@ -11345,7 +11562,7 @@
         <v>2393</v>
       </c>
       <c r="AF7" t="s">
-        <v>2256</v>
+        <v>2568</v>
       </c>
       <c r="AG7" t="s">
         <v>2391</v>
@@ -11354,7 +11571,7 @@
         <v>2397</v>
       </c>
       <c r="AI7" t="s">
-        <v>2384</v>
+        <v>912</v>
       </c>
       <c r="AJ7" t="s">
         <v>1509</v>
@@ -11371,7 +11588,7 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>1949</v>
+        <v>703</v>
       </c>
       <c r="D8" t="s">
         <v>2407</v>
@@ -11395,7 +11612,7 @@
         <v>2291</v>
       </c>
       <c r="V8" t="s">
-        <v>2292</v>
+        <v>2584</v>
       </c>
       <c r="W8" t="s">
         <v>2387</v>
@@ -11404,7 +11621,7 @@
         <v>691</v>
       </c>
       <c r="Y8" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="Z8" t="s">
         <v>680</v>
@@ -11416,7 +11633,7 @@
         <v>2388</v>
       </c>
       <c r="AC8" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AD8" t="s">
         <v>2263</v>
@@ -11431,10 +11648,10 @@
         <v>2405</v>
       </c>
       <c r="AH8" t="s">
-        <v>2296</v>
+        <v>2608</v>
       </c>
       <c r="AI8" t="s">
-        <v>1949</v>
+        <v>703</v>
       </c>
       <c r="AJ8" t="s">
         <v>1591</v>
@@ -11451,7 +11668,7 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>2408</v>
+        <v>912</v>
       </c>
       <c r="D9" t="s">
         <v>2410</v>
@@ -11475,7 +11692,7 @@
         <v>2387</v>
       </c>
       <c r="V9" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="W9" t="s">
         <v>2248</v>
@@ -11484,13 +11701,13 @@
         <v>750</v>
       </c>
       <c r="Y9" t="s">
-        <v>2298</v>
+        <v>2609</v>
       </c>
       <c r="Z9" t="s">
         <v>2388</v>
       </c>
       <c r="AA9" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AB9" t="s">
         <v>739</v>
@@ -11502,19 +11719,19 @@
         <v>2263</v>
       </c>
       <c r="AE9" t="s">
-        <v>2299</v>
+        <v>1410</v>
       </c>
       <c r="AF9" t="s">
-        <v>2277</v>
+        <v>2588</v>
       </c>
       <c r="AG9" t="s">
-        <v>2300</v>
+        <v>2579</v>
       </c>
       <c r="AH9" t="s">
         <v>1427</v>
       </c>
       <c r="AI9" t="s">
-        <v>2408</v>
+        <v>912</v>
       </c>
       <c r="AJ9" t="s">
         <v>1508</v>
@@ -11531,7 +11748,7 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>2399</v>
+        <v>2461</v>
       </c>
       <c r="D10" t="s">
         <v>2414</v>
@@ -11549,7 +11766,7 @@
         <v>285</v>
       </c>
       <c r="T10" t="s">
-        <v>2301</v>
+        <v>2610</v>
       </c>
       <c r="U10" t="s">
         <v>2387</v>
@@ -11567,10 +11784,10 @@
         <v>691</v>
       </c>
       <c r="Z10" t="s">
-        <v>2264</v>
+        <v>1979</v>
       </c>
       <c r="AA10" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="AB10" t="s">
         <v>2411</v>
@@ -11579,13 +11796,13 @@
         <v>2263</v>
       </c>
       <c r="AD10" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE10" t="s">
-        <v>2303</v>
+        <v>766</v>
       </c>
       <c r="AF10" t="s">
-        <v>2304</v>
+        <v>782</v>
       </c>
       <c r="AG10" t="s">
         <v>2412</v>
@@ -11594,7 +11811,7 @@
         <v>2306</v>
       </c>
       <c r="AI10" t="s">
-        <v>2399</v>
+        <v>2461</v>
       </c>
       <c r="AJ10" t="s">
         <v>1856</v>
@@ -11611,7 +11828,7 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>912</v>
+        <v>316</v>
       </c>
       <c r="D11" t="s">
         <v>2060</v>
@@ -11635,13 +11852,13 @@
         <v>2387</v>
       </c>
       <c r="V11" t="s">
-        <v>2283</v>
+        <v>2544</v>
       </c>
       <c r="W11" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X11" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="Y11" t="s">
         <v>721</v>
@@ -11653,28 +11870,28 @@
         <v>2388</v>
       </c>
       <c r="AB11" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="AC11" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AD11" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE11" t="s">
-        <v>2299</v>
+        <v>1410</v>
       </c>
       <c r="AF11" t="s">
-        <v>2300</v>
+        <v>2579</v>
       </c>
       <c r="AG11" t="s">
-        <v>2292</v>
+        <v>2584</v>
       </c>
       <c r="AH11" t="s">
-        <v>2264</v>
+        <v>1979</v>
       </c>
       <c r="AI11" t="s">
-        <v>912</v>
+        <v>316</v>
       </c>
       <c r="AJ11" t="s">
         <v>1886</v>
@@ -11691,7 +11908,7 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>874</v>
+        <v>1499</v>
       </c>
       <c r="D12" t="s">
         <v>2049</v>
@@ -11712,7 +11929,7 @@
         <v>1498</v>
       </c>
       <c r="U12" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="V12" t="s">
         <v>2291</v>
@@ -11721,7 +11938,7 @@
         <v>2380</v>
       </c>
       <c r="X12" t="s">
-        <v>2273</v>
+        <v>2557</v>
       </c>
       <c r="Y12" t="s">
         <v>2307</v>
@@ -11736,25 +11953,25 @@
         <v>721</v>
       </c>
       <c r="AC12" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD12" t="s">
         <v>1416</v>
       </c>
       <c r="AE12" t="s">
-        <v>2308</v>
+        <v>1977</v>
       </c>
       <c r="AF12" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="AG12" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AH12" t="s">
         <v>2391</v>
       </c>
       <c r="AI12" t="s">
-        <v>874</v>
+        <v>1499</v>
       </c>
       <c r="AJ12" t="s">
         <v>1842</v>
@@ -11771,7 +11988,7 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>2418</v>
+        <v>1504</v>
       </c>
       <c r="D13" t="s">
         <v>1458</v>
@@ -11801,40 +12018,40 @@
         <v>1235</v>
       </c>
       <c r="X13" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="Y13" t="s">
         <v>691</v>
       </c>
       <c r="Z13" t="s">
-        <v>2264</v>
+        <v>1979</v>
       </c>
       <c r="AA13" t="s">
         <v>2388</v>
       </c>
       <c r="AB13" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AC13" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AD13" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE13" t="s">
         <v>1498</v>
       </c>
       <c r="AF13" t="s">
-        <v>2304</v>
+        <v>782</v>
       </c>
       <c r="AG13" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="AH13" t="s">
         <v>2397</v>
       </c>
       <c r="AI13" t="s">
-        <v>2418</v>
+        <v>1504</v>
       </c>
       <c r="AJ13" t="s">
         <v>1947</v>
@@ -11851,7 +12068,7 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>2408</v>
+        <v>2461</v>
       </c>
       <c r="D14" t="s">
         <v>1393</v>
@@ -11869,7 +12086,7 @@
         <v>796</v>
       </c>
       <c r="T14" t="s">
-        <v>2301</v>
+        <v>2610</v>
       </c>
       <c r="U14" t="s">
         <v>565</v>
@@ -11878,16 +12095,16 @@
         <v>2420</v>
       </c>
       <c r="W14" t="s">
-        <v>2313</v>
+        <v>792</v>
       </c>
       <c r="X14" t="s">
-        <v>2314</v>
+        <v>789</v>
       </c>
       <c r="Y14" t="s">
         <v>2377</v>
       </c>
       <c r="Z14" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AA14" t="s">
         <v>2421</v>
@@ -11899,10 +12116,10 @@
         <v>692</v>
       </c>
       <c r="AD14" t="s">
-        <v>2318</v>
+        <v>2591</v>
       </c>
       <c r="AE14" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF14" t="s">
         <v>2248</v>
@@ -11914,7 +12131,7 @@
         <v>2412</v>
       </c>
       <c r="AI14" t="s">
-        <v>2408</v>
+        <v>2461</v>
       </c>
       <c r="AJ14" t="s">
         <v>1387</v>
@@ -11931,7 +12148,7 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>821</v>
+        <v>730</v>
       </c>
       <c r="D15" t="s">
         <v>2049</v>
@@ -11958,7 +12175,7 @@
         <v>2387</v>
       </c>
       <c r="W15" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X15" t="s">
         <v>1235</v>
@@ -11970,19 +12187,19 @@
         <v>691</v>
       </c>
       <c r="AA15" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AB15" t="s">
         <v>721</v>
       </c>
       <c r="AC15" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AD15" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE15" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF15" t="s">
         <v>2391</v>
@@ -11994,7 +12211,7 @@
         <v>1416</v>
       </c>
       <c r="AI15" t="s">
-        <v>821</v>
+        <v>730</v>
       </c>
       <c r="AJ15" t="s">
         <v>1458</v>
@@ -12011,7 +12228,7 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D16" t="s">
         <v>2427</v>
@@ -12035,7 +12252,7 @@
         <v>2387</v>
       </c>
       <c r="V16" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="W16" t="s">
         <v>2424</v>
@@ -12050,7 +12267,7 @@
         <v>2388</v>
       </c>
       <c r="AA16" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AB16" t="s">
         <v>2321</v>
@@ -12059,7 +12276,7 @@
         <v>1428</v>
       </c>
       <c r="AD16" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE16" t="s">
         <v>804</v>
@@ -12068,13 +12285,13 @@
         <v>2425</v>
       </c>
       <c r="AG16" t="s">
-        <v>2324</v>
+        <v>805</v>
       </c>
       <c r="AH16" t="s">
-        <v>2274</v>
+        <v>685</v>
       </c>
       <c r="AI16" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="AJ16" t="s">
         <v>1953</v>
@@ -12091,7 +12308,7 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>2428</v>
+        <v>829</v>
       </c>
       <c r="D17" t="s">
         <v>2430</v>
@@ -12115,7 +12332,7 @@
         <v>2391</v>
       </c>
       <c r="V17" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W17" t="s">
         <v>2306</v>
@@ -12130,31 +12347,31 @@
         <v>2388</v>
       </c>
       <c r="AA17" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="AB17" t="s">
         <v>1414</v>
       </c>
       <c r="AC17" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD17" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE17" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF17" t="s">
         <v>1914</v>
       </c>
       <c r="AG17" t="s">
-        <v>2324</v>
+        <v>805</v>
       </c>
       <c r="AH17" t="s">
         <v>400</v>
       </c>
       <c r="AI17" t="s">
-        <v>2428</v>
+        <v>829</v>
       </c>
       <c r="AJ17" t="s">
         <v>1955</v>
@@ -12171,7 +12388,7 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>907</v>
+        <v>1499</v>
       </c>
       <c r="D18" t="s">
         <v>2012</v>
@@ -12189,7 +12406,7 @@
         <v>813</v>
       </c>
       <c r="T18" t="s">
-        <v>2267</v>
+        <v>947</v>
       </c>
       <c r="U18" t="s">
         <v>1235</v>
@@ -12198,7 +12415,7 @@
         <v>2387</v>
       </c>
       <c r="W18" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X18" t="s">
         <v>2380</v>
@@ -12216,25 +12433,25 @@
         <v>2421</v>
       </c>
       <c r="AC18" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD18" t="s">
         <v>2328</v>
       </c>
       <c r="AE18" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF18" t="s">
-        <v>2292</v>
+        <v>2584</v>
       </c>
       <c r="AG18" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="AH18" t="s">
         <v>812</v>
       </c>
       <c r="AI18" t="s">
-        <v>907</v>
+        <v>1499</v>
       </c>
       <c r="AJ18" t="s">
         <v>1947</v>
@@ -12251,7 +12468,7 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>671</v>
+        <v>297</v>
       </c>
       <c r="D19" t="s">
         <v>2433</v>
@@ -12278,7 +12495,7 @@
         <v>2248</v>
       </c>
       <c r="W19" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X19" t="s">
         <v>2388</v>
@@ -12293,28 +12510,28 @@
         <v>2396</v>
       </c>
       <c r="AB19" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AC19" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AD19" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE19" t="s">
-        <v>2299</v>
+        <v>1410</v>
       </c>
       <c r="AF19" t="s">
-        <v>2331</v>
+        <v>2009</v>
       </c>
       <c r="AG19" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AH19" t="s">
         <v>2391</v>
       </c>
       <c r="AI19" t="s">
-        <v>671</v>
+        <v>297</v>
       </c>
       <c r="AJ19" t="s">
         <v>1466</v>
@@ -12331,7 +12548,7 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>2418</v>
+        <v>829</v>
       </c>
       <c r="D20" t="s">
         <v>2435</v>
@@ -12361,13 +12578,13 @@
         <v>2387</v>
       </c>
       <c r="X20" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="Y20" t="s">
         <v>680</v>
       </c>
       <c r="Z20" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AA20" t="s">
         <v>2388</v>
@@ -12376,7 +12593,7 @@
         <v>1416</v>
       </c>
       <c r="AC20" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD20" t="s">
         <v>700</v>
@@ -12394,7 +12611,7 @@
         <v>2397</v>
       </c>
       <c r="AI20" t="s">
-        <v>2418</v>
+        <v>829</v>
       </c>
       <c r="AJ20" t="s">
         <v>1917</v>
@@ -12411,7 +12628,7 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>821</v>
+        <v>268</v>
       </c>
       <c r="D21" t="s">
         <v>1880</v>
@@ -12438,13 +12655,13 @@
         <v>2387</v>
       </c>
       <c r="W21" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X21" t="s">
         <v>2388</v>
       </c>
       <c r="Y21" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="Z21" t="s">
         <v>691</v>
@@ -12453,28 +12670,28 @@
         <v>680</v>
       </c>
       <c r="AB21" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AC21" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AD21" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE21" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF21" t="s">
         <v>1235</v>
       </c>
       <c r="AG21" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AH21" t="s">
         <v>2391</v>
       </c>
       <c r="AI21" t="s">
-        <v>821</v>
+        <v>268</v>
       </c>
       <c r="AJ21" t="s">
         <v>1535</v>
@@ -12491,7 +12708,7 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>771</v>
+        <v>1949</v>
       </c>
       <c r="D22" t="s">
         <v>2438</v>
@@ -12509,13 +12726,13 @@
         <v>830</v>
       </c>
       <c r="T22" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="U22" t="s">
         <v>2387</v>
       </c>
       <c r="V22" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W22" t="s">
         <v>2248</v>
@@ -12524,7 +12741,7 @@
         <v>2280</v>
       </c>
       <c r="Y22" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="Z22" t="s">
         <v>2396</v>
@@ -12539,22 +12756,22 @@
         <v>2411</v>
       </c>
       <c r="AD22" t="s">
-        <v>2334</v>
+        <v>1413</v>
       </c>
       <c r="AE22" t="s">
         <v>2389</v>
       </c>
       <c r="AF22" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="AG22" t="s">
         <v>1235</v>
       </c>
       <c r="AH22" t="s">
-        <v>2335</v>
+        <v>2611</v>
       </c>
       <c r="AI22" t="s">
-        <v>771</v>
+        <v>1949</v>
       </c>
       <c r="AJ22" t="s">
         <v>1855</v>
@@ -12571,7 +12788,7 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>821</v>
+        <v>1564</v>
       </c>
       <c r="D23" t="s">
         <v>1842</v>
@@ -12601,13 +12818,13 @@
         <v>2387</v>
       </c>
       <c r="X23" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="Y23" t="s">
         <v>2388</v>
       </c>
       <c r="Z23" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AA23" t="s">
         <v>691</v>
@@ -12616,16 +12833,16 @@
         <v>721</v>
       </c>
       <c r="AC23" t="s">
-        <v>2300</v>
+        <v>2579</v>
       </c>
       <c r="AD23" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AE23" t="s">
         <v>399</v>
       </c>
       <c r="AF23" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AG23" t="s">
         <v>2391</v>
@@ -12634,7 +12851,7 @@
         <v>1914</v>
       </c>
       <c r="AI23" t="s">
-        <v>821</v>
+        <v>1564</v>
       </c>
       <c r="AJ23" t="s">
         <v>1947</v>
@@ -12651,7 +12868,7 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>2399</v>
+        <v>2246</v>
       </c>
       <c r="D24" t="s">
         <v>1558</v>
@@ -12672,13 +12889,13 @@
         <v>2440</v>
       </c>
       <c r="U24" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="V24" t="s">
         <v>2248</v>
       </c>
       <c r="W24" t="s">
-        <v>2339</v>
+        <v>2612</v>
       </c>
       <c r="X24" t="s">
         <v>721</v>
@@ -12687,13 +12904,13 @@
         <v>691</v>
       </c>
       <c r="Z24" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AA24" t="s">
         <v>2388</v>
       </c>
       <c r="AB24" t="s">
-        <v>2298</v>
+        <v>2609</v>
       </c>
       <c r="AC24" t="s">
         <v>2441</v>
@@ -12702,7 +12919,7 @@
         <v>2263</v>
       </c>
       <c r="AE24" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF24" t="s">
         <v>710</v>
@@ -12711,10 +12928,10 @@
         <v>2391</v>
       </c>
       <c r="AH24" t="s">
-        <v>2296</v>
+        <v>2608</v>
       </c>
       <c r="AI24" t="s">
-        <v>2399</v>
+        <v>2246</v>
       </c>
       <c r="AJ24" t="s">
         <v>1855</v>
@@ -12731,7 +12948,7 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>2167</v>
+        <v>2613</v>
       </c>
       <c r="D25" t="s">
         <v>2444</v>
@@ -12758,31 +12975,31 @@
         <v>2280</v>
       </c>
       <c r="W25" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="X25" t="s">
-        <v>2250</v>
+        <v>2547</v>
       </c>
       <c r="Y25" t="s">
         <v>2341</v>
       </c>
       <c r="Z25" t="s">
-        <v>2256</v>
+        <v>2568</v>
       </c>
       <c r="AA25" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AB25" t="s">
         <v>1428</v>
       </c>
       <c r="AC25" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AD25" t="s">
         <v>2328</v>
       </c>
       <c r="AE25" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF25" t="s">
         <v>2281</v>
@@ -12794,7 +13011,7 @@
         <v>2397</v>
       </c>
       <c r="AI25" t="s">
-        <v>2167</v>
+        <v>2613</v>
       </c>
       <c r="AJ25" t="s">
         <v>1964</v>
@@ -12811,7 +13028,7 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>874</v>
+        <v>841</v>
       </c>
       <c r="D26" t="s">
         <v>1445</v>
@@ -12838,7 +13055,7 @@
         <v>2248</v>
       </c>
       <c r="W26" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X26" t="s">
         <v>2380</v>
@@ -12847,7 +13064,7 @@
         <v>2388</v>
       </c>
       <c r="Z26" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="AA26" t="s">
         <v>691</v>
@@ -12856,25 +13073,25 @@
         <v>1416</v>
       </c>
       <c r="AC26" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AD26" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AE26" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF26" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="AG26" t="s">
         <v>2391</v>
       </c>
       <c r="AH26" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AI26" t="s">
-        <v>874</v>
+        <v>841</v>
       </c>
       <c r="AJ26" t="s">
         <v>1920</v>
@@ -12891,7 +13108,7 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>829</v>
+        <v>270</v>
       </c>
       <c r="D27" t="s">
         <v>2447</v>
@@ -12915,7 +13132,7 @@
         <v>2387</v>
       </c>
       <c r="V27" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W27" t="s">
         <v>2248</v>
@@ -12936,16 +13153,16 @@
         <v>1428</v>
       </c>
       <c r="AC27" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AD27" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AE27" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF27" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="AG27" t="s">
         <v>1412</v>
@@ -12954,7 +13171,7 @@
         <v>2391</v>
       </c>
       <c r="AI27" t="s">
-        <v>829</v>
+        <v>270</v>
       </c>
       <c r="AJ27" t="s">
         <v>1563</v>
@@ -12971,7 +13188,7 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>841</v>
+        <v>297</v>
       </c>
       <c r="D28" t="s">
         <v>2449</v>
@@ -12992,7 +13209,7 @@
         <v>2389</v>
       </c>
       <c r="U28" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="V28" t="s">
         <v>2387</v>
@@ -13004,25 +13221,25 @@
         <v>2388</v>
       </c>
       <c r="Y28" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="Z28" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="AA28" t="s">
         <v>2396</v>
       </c>
       <c r="AB28" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AC28" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AD28" t="s">
-        <v>2300</v>
+        <v>2579</v>
       </c>
       <c r="AE28" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF28" t="s">
         <v>2412</v>
@@ -13034,7 +13251,7 @@
         <v>1221</v>
       </c>
       <c r="AI28" t="s">
-        <v>841</v>
+        <v>297</v>
       </c>
       <c r="AJ28" t="s">
         <v>1458</v>
@@ -13051,7 +13268,7 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>771</v>
+        <v>272</v>
       </c>
       <c r="D29" t="s">
         <v>2451</v>
@@ -13072,10 +13289,10 @@
         <v>2393</v>
       </c>
       <c r="U29" t="s">
-        <v>2343</v>
+        <v>2614</v>
       </c>
       <c r="V29" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="W29" t="s">
         <v>2248</v>
@@ -13084,7 +13301,7 @@
         <v>2387</v>
       </c>
       <c r="Y29" t="s">
-        <v>2276</v>
+        <v>2548</v>
       </c>
       <c r="Z29" t="s">
         <v>691</v>
@@ -13096,13 +13313,13 @@
         <v>2396</v>
       </c>
       <c r="AC29" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AD29" t="s">
         <v>1416</v>
       </c>
       <c r="AE29" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF29" t="s">
         <v>1919</v>
@@ -13114,7 +13331,7 @@
         <v>532</v>
       </c>
       <c r="AI29" t="s">
-        <v>771</v>
+        <v>272</v>
       </c>
       <c r="AJ29" t="s">
         <v>1846</v>
@@ -13131,7 +13348,7 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D30" t="s">
         <v>1876</v>
@@ -13152,7 +13369,7 @@
         <v>1498</v>
       </c>
       <c r="U30" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="V30" t="s">
         <v>2387</v>
@@ -13161,7 +13378,7 @@
         <v>2248</v>
       </c>
       <c r="X30" t="s">
-        <v>2309</v>
+        <v>438</v>
       </c>
       <c r="Y30" t="s">
         <v>2388</v>
@@ -13173,28 +13390,28 @@
         <v>691</v>
       </c>
       <c r="AB30" t="s">
-        <v>2300</v>
+        <v>2579</v>
       </c>
       <c r="AC30" t="s">
-        <v>2311</v>
+        <v>1910</v>
       </c>
       <c r="AD30" t="s">
         <v>2263</v>
       </c>
       <c r="AE30" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF30" t="s">
         <v>2425</v>
       </c>
       <c r="AG30" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AH30" t="s">
         <v>2391</v>
       </c>
       <c r="AI30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AJ30" t="s">
         <v>1846</v>
@@ -13211,7 +13428,7 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>1949</v>
+        <v>286</v>
       </c>
       <c r="D31" t="s">
         <v>2065</v>
@@ -13232,7 +13449,7 @@
         <v>1498</v>
       </c>
       <c r="U31" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="V31" t="s">
         <v>2248</v>
@@ -13241,7 +13458,7 @@
         <v>2387</v>
       </c>
       <c r="X31" t="s">
-        <v>2273</v>
+        <v>2557</v>
       </c>
       <c r="Y31" t="s">
         <v>680</v>
@@ -13253,28 +13470,28 @@
         <v>2388</v>
       </c>
       <c r="AB31" t="s">
-        <v>2293</v>
+        <v>2607</v>
       </c>
       <c r="AC31" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AD31" t="s">
         <v>1416</v>
       </c>
       <c r="AE31" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF31" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AG31" t="s">
         <v>2391</v>
       </c>
       <c r="AH31" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AI31" t="s">
-        <v>1949</v>
+        <v>286</v>
       </c>
       <c r="AJ31" t="s">
         <v>1920</v>
@@ -13291,7 +13508,7 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>912</v>
+        <v>316</v>
       </c>
       <c r="D32" t="s">
         <v>1528</v>
@@ -13318,10 +13535,10 @@
         <v>2248</v>
       </c>
       <c r="W32" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="X32" t="s">
-        <v>2297</v>
+        <v>424</v>
       </c>
       <c r="Y32" t="s">
         <v>721</v>
@@ -13333,28 +13550,28 @@
         <v>691</v>
       </c>
       <c r="AB32" t="s">
-        <v>2298</v>
+        <v>2609</v>
       </c>
       <c r="AC32" t="s">
-        <v>2254</v>
+        <v>2578</v>
       </c>
       <c r="AD32" t="s">
         <v>1428</v>
       </c>
       <c r="AE32" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF32" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AG32" t="s">
         <v>1427</v>
       </c>
       <c r="AH32" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AI32" t="s">
-        <v>912</v>
+        <v>316</v>
       </c>
       <c r="AJ32" t="s">
         <v>1972</v>
@@ -13371,7 +13588,7 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="D33" t="s">
         <v>2456</v>
@@ -13392,7 +13609,7 @@
         <v>1498</v>
       </c>
       <c r="U33" t="s">
-        <v>2249</v>
+        <v>2603</v>
       </c>
       <c r="V33" t="s">
         <v>2248</v>
@@ -13404,7 +13621,7 @@
         <v>691</v>
       </c>
       <c r="Y33" t="s">
-        <v>2293</v>
+        <v>1425</v>
       </c>
       <c r="Z33" t="s">
         <v>2388</v>
@@ -13413,28 +13630,28 @@
         <v>2396</v>
       </c>
       <c r="AB33" t="s">
-        <v>2270</v>
+        <v>2552</v>
       </c>
       <c r="AC33" t="s">
         <v>1416</v>
       </c>
       <c r="AD33" t="s">
-        <v>2294</v>
+        <v>682</v>
       </c>
       <c r="AE33" t="s">
-        <v>2271</v>
+        <v>2553</v>
       </c>
       <c r="AF33" t="s">
         <v>2380</v>
       </c>
       <c r="AG33" t="s">
-        <v>2332</v>
+        <v>2554</v>
       </c>
       <c r="AH33" t="s">
         <v>2391</v>
       </c>
       <c r="AI33" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="AJ33" t="s">
         <v>1517</v>

</xml_diff>

<commit_message>
gw 13 final done
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9021" uniqueCount="2313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10221" uniqueCount="2382">
   <si>
     <t>Places</t>
   </si>
@@ -6973,6 +6973,213 @@
   </si>
   <si>
     <t>4,655</t>
+  </si>
+  <si>
+    <t>1,395,041</t>
+  </si>
+  <si>
+    <t>746</t>
+  </si>
+  <si>
+    <t>2,658,952</t>
+  </si>
+  <si>
+    <t>694</t>
+  </si>
+  <si>
+    <t>530,105</t>
+  </si>
+  <si>
+    <t>797</t>
+  </si>
+  <si>
+    <t>1,053,473</t>
+  </si>
+  <si>
+    <t>1,475,879</t>
+  </si>
+  <si>
+    <t>2,268,836</t>
+  </si>
+  <si>
+    <t>939,955</t>
+  </si>
+  <si>
+    <t>1,656,869</t>
+  </si>
+  <si>
+    <t>1,497,991</t>
+  </si>
+  <si>
+    <t>552,799</t>
+  </si>
+  <si>
+    <t>579,404</t>
+  </si>
+  <si>
+    <t>1,127,371</t>
+  </si>
+  <si>
+    <t>Digne 3</t>
+  </si>
+  <si>
+    <t>Jiménez 4</t>
+  </si>
+  <si>
+    <t>607,253</t>
+  </si>
+  <si>
+    <t>855,791</t>
+  </si>
+  <si>
+    <t>1,870,706</t>
+  </si>
+  <si>
+    <t>1,045,769</t>
+  </si>
+  <si>
+    <t>311,176</t>
+  </si>
+  <si>
+    <t>964,330</t>
+  </si>
+  <si>
+    <t>147,997</t>
+  </si>
+  <si>
+    <t>844</t>
+  </si>
+  <si>
+    <t>274,696</t>
+  </si>
+  <si>
+    <t>1,230,812</t>
+  </si>
+  <si>
+    <t>445,818</t>
+  </si>
+  <si>
+    <t>4,954,130</t>
+  </si>
+  <si>
+    <t>603</t>
+  </si>
+  <si>
+    <t>451,474</t>
+  </si>
+  <si>
+    <t>44,076</t>
+  </si>
+  <si>
+    <t>874</t>
+  </si>
+  <si>
+    <t>467,282</t>
+  </si>
+  <si>
+    <t>214,897</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>118,969</t>
+  </si>
+  <si>
+    <t>302,935</t>
+  </si>
+  <si>
+    <t>109,358</t>
+  </si>
+  <si>
+    <t>853</t>
+  </si>
+  <si>
+    <t>Pickford 3</t>
+  </si>
+  <si>
+    <t>Thiago Silva 8</t>
+  </si>
+  <si>
+    <t>1,156,947</t>
+  </si>
+  <si>
+    <t>757</t>
+  </si>
+  <si>
+    <t>123,253</t>
+  </si>
+  <si>
+    <t>106,113</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>465,067</t>
+  </si>
+  <si>
+    <t>1,179,905</t>
+  </si>
+  <si>
+    <t>756</t>
+  </si>
+  <si>
+    <t>2,427,231</t>
+  </si>
+  <si>
+    <t>703</t>
+  </si>
+  <si>
+    <t>Cucho 2</t>
+  </si>
+  <si>
+    <t>2,224,335</t>
+  </si>
+  <si>
+    <t>711</t>
+  </si>
+  <si>
+    <t>Jesus 4$ captain</t>
+  </si>
+  <si>
+    <t>5,372,697</t>
+  </si>
+  <si>
+    <t>320,857</t>
+  </si>
+  <si>
+    <t>2,524,720</t>
+  </si>
+  <si>
+    <t>699</t>
+  </si>
+  <si>
+    <t>Rice 2</t>
+  </si>
+  <si>
+    <t>3,071,000</t>
+  </si>
+  <si>
+    <t>2,118,969</t>
+  </si>
+  <si>
+    <t>715</t>
+  </si>
+  <si>
+    <t>5,628,365</t>
+  </si>
+  <si>
+    <t>574</t>
+  </si>
+  <si>
+    <t>5,933,260</t>
+  </si>
+  <si>
+    <t>Lukaku 2$ captain</t>
+  </si>
+  <si>
+    <t>7,716,777</t>
   </si>
 </sst>
 </file>
@@ -7806,25 +8013,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="24" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="19.99609375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.8046875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.9453125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.48828125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -7948,13 +8162,13 @@
         <v>5695560</v>
       </c>
       <c r="C2" t="s">
-        <v>2123</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>2183</v>
+        <v>2356</v>
       </c>
       <c r="E2" t="s">
-        <v>2182</v>
+        <v>2355</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -7966,37 +8180,37 @@
         <v>882</v>
       </c>
       <c r="T2" t="s">
-        <v>1255</v>
+        <v>2353</v>
       </c>
       <c r="U2" t="s">
         <v>2176</v>
       </c>
       <c r="V2" t="s">
-        <v>2177</v>
+        <v>2354</v>
       </c>
       <c r="W2" t="s">
-        <v>949</v>
+        <v>1200</v>
       </c>
       <c r="X2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>2179</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="AA2" t="s">
         <v>2051</v>
       </c>
-      <c r="Y2" t="s">
-        <v>2178</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>2179</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>2180</v>
-      </c>
       <c r="AB2" t="s">
-        <v>2181</v>
+        <v>1374</v>
       </c>
       <c r="AC2" t="s">
-        <v>1374</v>
+        <v>682</v>
       </c>
       <c r="AD2" t="s">
-        <v>946</v>
+        <v>2262</v>
       </c>
       <c r="AE2" t="s">
         <v>880</v>
@@ -8005,13 +8219,19 @@
         <v>750</v>
       </c>
       <c r="AG2" t="s">
-        <v>2057</v>
+        <v>2180</v>
       </c>
       <c r="AH2" t="s">
         <v>881</v>
       </c>
       <c r="AI2" t="s">
         <v>2123</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>2356</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>2355</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -8022,13 +8242,13 @@
         <v>1153704</v>
       </c>
       <c r="C3" t="s">
-        <v>1988</v>
+        <v>829</v>
       </c>
       <c r="D3" t="s">
-        <v>2188</v>
+        <v>1473</v>
       </c>
       <c r="E3" t="s">
-        <v>2187</v>
+        <v>2357</v>
       </c>
       <c r="G3" t="s">
         <v>452</v>
@@ -8046,28 +8266,28 @@
         <v>1195</v>
       </c>
       <c r="V3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="W3" t="s">
         <v>2050</v>
       </c>
-      <c r="W3" t="s">
-        <v>1989</v>
-      </c>
       <c r="X3" t="s">
-        <v>949</v>
+        <v>2261</v>
       </c>
       <c r="Y3" t="s">
-        <v>2003</v>
+        <v>2269</v>
       </c>
       <c r="Z3" t="s">
-        <v>1211</v>
+        <v>1385</v>
       </c>
       <c r="AA3" t="s">
-        <v>438</v>
+        <v>2051</v>
       </c>
       <c r="AB3" t="s">
-        <v>2051</v>
+        <v>721</v>
       </c>
       <c r="AC3" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="AD3" t="s">
         <v>2184</v>
@@ -8076,7 +8296,7 @@
         <v>2185</v>
       </c>
       <c r="AF3" t="s">
-        <v>946</v>
+        <v>438</v>
       </c>
       <c r="AG3" t="s">
         <v>2186</v>
@@ -8086,6 +8306,12 @@
       </c>
       <c r="AI3" t="s">
         <v>1988</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>2357</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -8096,13 +8322,13 @@
         <v>440807</v>
       </c>
       <c r="C4" t="s">
-        <v>778</v>
+        <v>730</v>
       </c>
       <c r="D4" t="s">
-        <v>1902</v>
+        <v>1514</v>
       </c>
       <c r="E4" t="s">
-        <v>2064</v>
+        <v>2326</v>
       </c>
       <c r="G4" t="s">
         <v>653</v>
@@ -8117,49 +8343,55 @@
         <v>1458</v>
       </c>
       <c r="U4" t="s">
-        <v>949</v>
+        <v>688</v>
       </c>
       <c r="V4" t="s">
-        <v>2007</v>
+        <v>2047</v>
       </c>
       <c r="W4" t="s">
-        <v>2047</v>
+        <v>1200</v>
       </c>
       <c r="X4" t="s">
-        <v>2189</v>
+        <v>2054</v>
       </c>
       <c r="Y4" t="s">
-        <v>2017</v>
+        <v>721</v>
       </c>
       <c r="Z4" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA4" t="s">
         <v>2051</v>
       </c>
-      <c r="AA4" t="s">
-        <v>691</v>
-      </c>
       <c r="AB4" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="AC4" t="s">
-        <v>2181</v>
+        <v>2262</v>
       </c>
       <c r="AD4" t="s">
         <v>1376</v>
       </c>
       <c r="AE4" t="s">
-        <v>777</v>
+        <v>2244</v>
       </c>
       <c r="AF4" t="s">
         <v>438</v>
       </c>
       <c r="AG4" t="s">
-        <v>946</v>
+        <v>2189</v>
       </c>
       <c r="AH4" t="s">
-        <v>2054</v>
+        <v>2279</v>
       </c>
       <c r="AI4" t="s">
         <v>778</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>1514</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>2326</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -8170,13 +8402,13 @@
         <v>4642646</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
-        <v>2192</v>
+        <v>2359</v>
       </c>
       <c r="E5" t="s">
-        <v>2191</v>
+        <v>2358</v>
       </c>
       <c r="G5" t="s">
         <v>672</v>
@@ -8191,40 +8423,40 @@
         <v>2052</v>
       </c>
       <c r="U5" t="s">
-        <v>1989</v>
+        <v>2050</v>
       </c>
       <c r="V5" t="s">
+        <v>2261</v>
+      </c>
+      <c r="W5" t="s">
         <v>1195</v>
       </c>
-      <c r="W5" t="s">
-        <v>2050</v>
-      </c>
       <c r="X5" t="s">
+        <v>2047</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>721</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA5" t="s">
         <v>2051</v>
       </c>
-      <c r="Y5" t="s">
-        <v>2180</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>721</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>691</v>
-      </c>
       <c r="AB5" t="s">
-        <v>2190</v>
+        <v>1373</v>
       </c>
       <c r="AC5" t="s">
         <v>1388</v>
       </c>
       <c r="AD5" t="s">
-        <v>1848</v>
+        <v>2281</v>
       </c>
       <c r="AE5" t="s">
         <v>2185</v>
       </c>
       <c r="AF5" t="s">
-        <v>2047</v>
+        <v>2180</v>
       </c>
       <c r="AG5" t="s">
         <v>680</v>
@@ -8234,6 +8466,12 @@
       </c>
       <c r="AI5" t="s">
         <v>282</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>2359</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>2358</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -8244,13 +8482,13 @@
         <v>1364835</v>
       </c>
       <c r="C6" t="s">
-        <v>778</v>
+        <v>1522</v>
       </c>
       <c r="D6" t="s">
-        <v>1479</v>
+        <v>1488</v>
       </c>
       <c r="E6" t="s">
-        <v>2197</v>
+        <v>2360</v>
       </c>
       <c r="G6" t="s">
         <v>452</v>
@@ -8262,52 +8500,58 @@
         <v>888</v>
       </c>
       <c r="T6" t="s">
-        <v>2006</v>
+        <v>726</v>
       </c>
       <c r="U6" t="s">
-        <v>1989</v>
+        <v>2193</v>
       </c>
       <c r="V6" t="s">
-        <v>2193</v>
+        <v>1195</v>
       </c>
       <c r="W6" t="s">
-        <v>1195</v>
+        <v>2261</v>
       </c>
       <c r="X6" t="s">
-        <v>1197</v>
+        <v>805</v>
       </c>
       <c r="Y6" t="s">
-        <v>2180</v>
+        <v>2068</v>
       </c>
       <c r="Z6" t="s">
-        <v>2068</v>
+        <v>691</v>
       </c>
       <c r="AA6" t="s">
-        <v>691</v>
+        <v>1893</v>
       </c>
       <c r="AB6" t="s">
-        <v>2194</v>
+        <v>2262</v>
       </c>
       <c r="AC6" t="s">
-        <v>2181</v>
+        <v>692</v>
       </c>
       <c r="AD6" t="s">
-        <v>692</v>
+        <v>2275</v>
       </c>
       <c r="AE6" t="s">
         <v>2185</v>
       </c>
       <c r="AF6" t="s">
-        <v>805</v>
+        <v>1197</v>
       </c>
       <c r="AG6" t="s">
-        <v>2195</v>
+        <v>2180</v>
       </c>
       <c r="AH6" t="s">
-        <v>2196</v>
+        <v>782</v>
       </c>
       <c r="AI6" t="s">
         <v>778</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>2360</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -8318,13 +8562,13 @@
         <v>5306515</v>
       </c>
       <c r="C7" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="D7" t="s">
-        <v>1413</v>
+        <v>2362</v>
       </c>
       <c r="E7" t="s">
-        <v>2199</v>
+        <v>2361</v>
       </c>
       <c r="G7" t="s">
         <v>653</v>
@@ -8342,10 +8586,10 @@
         <v>2198</v>
       </c>
       <c r="V7" t="s">
-        <v>949</v>
+        <v>1200</v>
       </c>
       <c r="W7" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="X7" t="s">
         <v>2054</v>
@@ -8363,13 +8607,13 @@
         <v>691</v>
       </c>
       <c r="AC7" t="s">
-        <v>946</v>
+        <v>682</v>
       </c>
       <c r="AD7" t="s">
-        <v>2190</v>
+        <v>1373</v>
       </c>
       <c r="AE7" t="s">
-        <v>1892</v>
+        <v>2353</v>
       </c>
       <c r="AF7" t="s">
         <v>692</v>
@@ -8382,6 +8626,12 @@
       </c>
       <c r="AI7" t="s">
         <v>785</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>2362</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>2361</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -8392,13 +8642,13 @@
         <v>2249991</v>
       </c>
       <c r="C8" t="s">
-        <v>829</v>
+        <v>282</v>
       </c>
       <c r="D8" t="s">
-        <v>2202</v>
+        <v>2364</v>
       </c>
       <c r="E8" t="s">
-        <v>2201</v>
+        <v>2363</v>
       </c>
       <c r="G8" t="s">
         <v>706</v>
@@ -8413,37 +8663,37 @@
         <v>2052</v>
       </c>
       <c r="U8" t="s">
-        <v>2189</v>
+        <v>1200</v>
       </c>
       <c r="V8" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="W8" t="s">
-        <v>949</v>
+        <v>2054</v>
       </c>
       <c r="X8" t="s">
-        <v>691</v>
+        <v>2056</v>
       </c>
       <c r="Y8" t="s">
         <v>2200</v>
       </c>
       <c r="Z8" t="s">
-        <v>2056</v>
+        <v>691</v>
       </c>
       <c r="AA8" t="s">
         <v>2051</v>
       </c>
       <c r="AB8" t="s">
-        <v>946</v>
+        <v>2265</v>
       </c>
       <c r="AC8" t="s">
-        <v>1995</v>
+        <v>682</v>
       </c>
       <c r="AD8" t="s">
         <v>692</v>
       </c>
       <c r="AE8" t="s">
-        <v>1892</v>
+        <v>2353</v>
       </c>
       <c r="AF8" t="s">
         <v>805</v>
@@ -8452,10 +8702,16 @@
         <v>1197</v>
       </c>
       <c r="AH8" t="s">
-        <v>2054</v>
+        <v>2189</v>
       </c>
       <c r="AI8" t="s">
         <v>829</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>2364</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>2363</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -8466,13 +8722,13 @@
         <v>2056865</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s">
-        <v>2204</v>
+        <v>2367</v>
       </c>
       <c r="E9" t="s">
-        <v>2203</v>
+        <v>2366</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -8484,22 +8740,22 @@
         <v>901</v>
       </c>
       <c r="T9" t="s">
-        <v>2006</v>
+        <v>726</v>
       </c>
       <c r="U9" t="s">
+        <v>1200</v>
+      </c>
+      <c r="V9" t="s">
         <v>2050</v>
       </c>
-      <c r="V9" t="s">
-        <v>949</v>
-      </c>
       <c r="W9" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="X9" t="s">
+        <v>2165</v>
+      </c>
+      <c r="Y9" t="s">
         <v>691</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>2051</v>
       </c>
       <c r="Z9" t="s">
         <v>737</v>
@@ -8511,25 +8767,31 @@
         <v>2056</v>
       </c>
       <c r="AC9" t="s">
+        <v>2051</v>
+      </c>
+      <c r="AD9" t="s">
         <v>1376</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>2184</v>
       </c>
       <c r="AE9" t="s">
         <v>2185</v>
       </c>
       <c r="AF9" t="s">
-        <v>2165</v>
+        <v>2184</v>
       </c>
       <c r="AG9" t="s">
-        <v>2196</v>
+        <v>782</v>
       </c>
       <c r="AH9" t="s">
-        <v>1894</v>
+        <v>2365</v>
       </c>
       <c r="AI9" t="s">
         <v>268</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>2367</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>2366</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -8540,13 +8802,13 @@
         <v>5142355</v>
       </c>
       <c r="C10" t="s">
-        <v>2093</v>
+        <v>844</v>
       </c>
       <c r="D10" t="s">
-        <v>2209</v>
+        <v>1234</v>
       </c>
       <c r="E10" t="s">
-        <v>2208</v>
+        <v>2369</v>
       </c>
       <c r="G10" t="s">
         <v>653</v>
@@ -8561,49 +8823,55 @@
         <v>2065</v>
       </c>
       <c r="U10" t="s">
+        <v>1200</v>
+      </c>
+      <c r="V10" t="s">
+        <v>873</v>
+      </c>
+      <c r="W10" t="s">
         <v>2067</v>
-      </c>
-      <c r="V10" t="s">
-        <v>2189</v>
-      </c>
-      <c r="W10" t="s">
-        <v>949</v>
       </c>
       <c r="X10" t="s">
         <v>805</v>
       </c>
       <c r="Y10" t="s">
+        <v>413</v>
+      </c>
+      <c r="Z10" t="s">
         <v>2068</v>
       </c>
-      <c r="Z10" t="s">
-        <v>413</v>
-      </c>
       <c r="AA10" t="s">
-        <v>2205</v>
+        <v>947</v>
       </c>
       <c r="AB10" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>2368</v>
+      </c>
+      <c r="AD10" t="s">
         <v>2095</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>1995</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>2206</v>
       </c>
       <c r="AE10" t="s">
         <v>2055</v>
       </c>
       <c r="AF10" t="s">
-        <v>2207</v>
+        <v>2189</v>
       </c>
       <c r="AG10" t="s">
-        <v>947</v>
+        <v>2205</v>
       </c>
       <c r="AH10" t="s">
         <v>2072</v>
       </c>
       <c r="AI10" t="s">
         <v>2093</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>1234</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>2369</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -8614,13 +8882,13 @@
         <v>1628438</v>
       </c>
       <c r="C11" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>1506</v>
+        <v>1746</v>
       </c>
       <c r="E11" t="s">
-        <v>2212</v>
+        <v>2370</v>
       </c>
       <c r="G11" t="s">
         <v>653</v>
@@ -8635,34 +8903,34 @@
         <v>1458</v>
       </c>
       <c r="U11" t="s">
+        <v>1195</v>
+      </c>
+      <c r="V11" t="s">
         <v>2050</v>
       </c>
-      <c r="V11" t="s">
-        <v>2176</v>
-      </c>
       <c r="W11" t="s">
-        <v>1195</v>
+        <v>2261</v>
       </c>
       <c r="X11" t="s">
-        <v>1989</v>
+        <v>2063</v>
       </c>
       <c r="Y11" t="s">
+        <v>721</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>2180</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>2056</v>
+      </c>
+      <c r="AB11" t="s">
         <v>2051</v>
       </c>
-      <c r="Z11" t="s">
-        <v>721</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>2180</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>2056</v>
-      </c>
       <c r="AC11" t="s">
-        <v>2210</v>
+        <v>2275</v>
       </c>
       <c r="AD11" t="s">
-        <v>2211</v>
+        <v>2262</v>
       </c>
       <c r="AE11" t="s">
         <v>804</v>
@@ -8671,13 +8939,19 @@
         <v>1197</v>
       </c>
       <c r="AG11" t="s">
-        <v>2063</v>
+        <v>2176</v>
       </c>
       <c r="AH11" t="s">
         <v>532</v>
       </c>
       <c r="AI11" t="s">
         <v>301</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>1746</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>2370</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -8688,13 +8962,13 @@
         <v>1427447</v>
       </c>
       <c r="C12" t="s">
-        <v>1988</v>
+        <v>912</v>
       </c>
       <c r="D12" t="s">
-        <v>1258</v>
+        <v>2372</v>
       </c>
       <c r="E12" t="s">
-        <v>2215</v>
+        <v>2371</v>
       </c>
       <c r="G12" t="s">
         <v>653</v>
@@ -8715,7 +8989,7 @@
         <v>2213</v>
       </c>
       <c r="W12" t="s">
-        <v>949</v>
+        <v>1200</v>
       </c>
       <c r="X12" t="s">
         <v>1195</v>
@@ -8733,7 +9007,7 @@
         <v>2179</v>
       </c>
       <c r="AC12" t="s">
-        <v>1995</v>
+        <v>2265</v>
       </c>
       <c r="AD12" t="s">
         <v>1376</v>
@@ -8745,13 +9019,19 @@
         <v>2214</v>
       </c>
       <c r="AG12" t="s">
-        <v>2196</v>
+        <v>782</v>
       </c>
       <c r="AH12" t="s">
-        <v>2211</v>
+        <v>2275</v>
       </c>
       <c r="AI12" t="s">
         <v>1988</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>2372</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>2371</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -8762,13 +9042,13 @@
         <v>5648774</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="D13" t="s">
-        <v>2218</v>
+        <v>1344</v>
       </c>
       <c r="E13" t="s">
-        <v>2217</v>
+        <v>2374</v>
       </c>
       <c r="G13" t="s">
         <v>653</v>
@@ -8783,7 +9063,7 @@
         <v>411</v>
       </c>
       <c r="U13" t="s">
-        <v>1197</v>
+        <v>2072</v>
       </c>
       <c r="V13" t="s">
         <v>2054</v>
@@ -8792,7 +9072,7 @@
         <v>2216</v>
       </c>
       <c r="X13" t="s">
-        <v>395</v>
+        <v>2298</v>
       </c>
       <c r="Y13" t="s">
         <v>2051</v>
@@ -8804,19 +9084,19 @@
         <v>2179</v>
       </c>
       <c r="AB13" t="s">
-        <v>1808</v>
+        <v>2373</v>
       </c>
       <c r="AC13" t="s">
-        <v>1995</v>
+        <v>2265</v>
       </c>
       <c r="AD13" t="s">
-        <v>2210</v>
+        <v>2262</v>
       </c>
       <c r="AE13" t="s">
         <v>399</v>
       </c>
       <c r="AF13" t="s">
-        <v>2072</v>
+        <v>1197</v>
       </c>
       <c r="AG13" t="s">
         <v>1168</v>
@@ -8826,6 +9106,12 @@
       </c>
       <c r="AI13" t="s">
         <v>272</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>2374</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -8836,13 +9122,13 @@
         <v>3452385</v>
       </c>
       <c r="C14" t="s">
-        <v>2221</v>
+        <v>2060</v>
       </c>
       <c r="D14" t="s">
-        <v>1551</v>
+        <v>2376</v>
       </c>
       <c r="E14" t="s">
-        <v>2222</v>
+        <v>2375</v>
       </c>
       <c r="G14" t="s">
         <v>672</v>
@@ -8854,16 +9140,16 @@
         <v>924</v>
       </c>
       <c r="T14" t="s">
-        <v>717</v>
+        <v>942</v>
       </c>
       <c r="U14" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="V14" t="s">
         <v>2176</v>
       </c>
       <c r="W14" t="s">
-        <v>395</v>
+        <v>2298</v>
       </c>
       <c r="X14" t="s">
         <v>2179</v>
@@ -8878,10 +9164,10 @@
         <v>737</v>
       </c>
       <c r="AB14" t="s">
-        <v>946</v>
+        <v>682</v>
       </c>
       <c r="AC14" t="s">
-        <v>1995</v>
+        <v>2265</v>
       </c>
       <c r="AD14" t="s">
         <v>2219</v>
@@ -8900,6 +9186,12 @@
       </c>
       <c r="AI14" t="s">
         <v>2221</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>2376</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>2375</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -8910,13 +9202,13 @@
         <v>2297330</v>
       </c>
       <c r="C15" t="s">
-        <v>2048</v>
+        <v>2066</v>
       </c>
       <c r="D15" t="s">
-        <v>2226</v>
+        <v>2378</v>
       </c>
       <c r="E15" t="s">
-        <v>2225</v>
+        <v>2377</v>
       </c>
       <c r="G15" t="s">
         <v>706</v>
@@ -8928,52 +9220,58 @@
         <v>926</v>
       </c>
       <c r="T15" t="s">
-        <v>2001</v>
+        <v>2268</v>
       </c>
       <c r="U15" t="s">
-        <v>1898</v>
+        <v>2224</v>
       </c>
       <c r="V15" t="s">
         <v>2047</v>
       </c>
       <c r="W15" t="s">
-        <v>2176</v>
+        <v>1898</v>
       </c>
       <c r="X15" t="s">
+        <v>805</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1896</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA15" t="s">
         <v>2180</v>
       </c>
-      <c r="Y15" t="s">
-        <v>950</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>1896</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>721</v>
-      </c>
       <c r="AB15" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AD15" t="s">
         <v>2223</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>946</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>1995</v>
       </c>
       <c r="AE15" t="s">
         <v>1897</v>
       </c>
       <c r="AF15" t="s">
-        <v>805</v>
+        <v>950</v>
       </c>
       <c r="AG15" t="s">
-        <v>2224</v>
+        <v>2176</v>
       </c>
       <c r="AH15" t="s">
         <v>1387</v>
       </c>
       <c r="AI15" t="s">
         <v>2048</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>2378</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>2377</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -8984,13 +9282,13 @@
         <v>5361878</v>
       </c>
       <c r="C16" t="s">
-        <v>2123</v>
+        <v>907</v>
       </c>
       <c r="D16" t="s">
-        <v>2229</v>
+        <v>1190</v>
       </c>
       <c r="E16" t="s">
-        <v>2228</v>
+        <v>2379</v>
       </c>
       <c r="G16" t="s">
         <v>672</v>
@@ -9008,10 +9306,10 @@
         <v>1195</v>
       </c>
       <c r="V16" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="W16" t="s">
-        <v>2003</v>
+        <v>2269</v>
       </c>
       <c r="X16" t="s">
         <v>2051</v>
@@ -9020,7 +9318,7 @@
         <v>2227</v>
       </c>
       <c r="Z16" t="s">
-        <v>2017</v>
+        <v>2279</v>
       </c>
       <c r="AA16" t="s">
         <v>438</v>
@@ -9035,10 +9333,10 @@
         <v>2095</v>
       </c>
       <c r="AE16" t="s">
-        <v>717</v>
+        <v>942</v>
       </c>
       <c r="AF16" t="s">
-        <v>2004</v>
+        <v>952</v>
       </c>
       <c r="AG16" t="s">
         <v>1899</v>
@@ -9048,6 +9346,12 @@
       </c>
       <c r="AI16" t="s">
         <v>2123</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>1190</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>2379</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -9058,13 +9362,13 @@
         <v>5344757</v>
       </c>
       <c r="C17" t="s">
-        <v>2046</v>
+        <v>2093</v>
       </c>
       <c r="D17" t="s">
-        <v>847</v>
+        <v>911</v>
       </c>
       <c r="E17" t="s">
-        <v>2234</v>
+        <v>2381</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
@@ -9076,7 +9380,7 @@
         <v>930</v>
       </c>
       <c r="T17" t="s">
-        <v>2001</v>
+        <v>2268</v>
       </c>
       <c r="U17" t="s">
         <v>2230</v>
@@ -9085,43 +9389,49 @@
         <v>2165</v>
       </c>
       <c r="W17" t="s">
-        <v>2177</v>
+        <v>2354</v>
       </c>
       <c r="X17" t="s">
+        <v>2233</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>2071</v>
+      </c>
+      <c r="Z17" t="s">
         <v>739</v>
       </c>
-      <c r="Y17" t="s">
-        <v>2231</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>950</v>
-      </c>
       <c r="AA17" t="s">
+        <v>1392</v>
+      </c>
+      <c r="AB17" t="s">
         <v>691</v>
       </c>
-      <c r="AB17" t="s">
-        <v>2026</v>
-      </c>
       <c r="AC17" t="s">
-        <v>1995</v>
+        <v>2265</v>
       </c>
       <c r="AD17" t="s">
-        <v>2232</v>
+        <v>2380</v>
       </c>
       <c r="AE17" t="s">
         <v>2185</v>
       </c>
       <c r="AF17" t="s">
-        <v>2233</v>
+        <v>950</v>
       </c>
       <c r="AG17" t="s">
-        <v>2071</v>
+        <v>1170</v>
       </c>
       <c r="AH17" t="s">
-        <v>2211</v>
+        <v>2275</v>
       </c>
       <c r="AI17" t="s">
         <v>2046</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>911</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>2381</v>
       </c>
     </row>
   </sheetData>
@@ -10048,27 +10358,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="21" max="24" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="26" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.34375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.484375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="14.859375" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10195,10 +10512,10 @@
         <v>290</v>
       </c>
       <c r="D2" t="s">
-        <v>2264</v>
+        <v>2314</v>
       </c>
       <c r="E2" t="s">
-        <v>2263</v>
+        <v>2313</v>
       </c>
       <c r="G2" t="s">
         <v>452</v>
@@ -10258,10 +10575,10 @@
         <v>290</v>
       </c>
       <c r="AJ2" t="s">
-        <v>1798</v>
+        <v>2314</v>
       </c>
       <c r="AK2" t="s">
-        <v>1853</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -10272,13 +10589,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>771</v>
+        <v>829</v>
       </c>
       <c r="D3" t="s">
-        <v>1365</v>
+        <v>2316</v>
       </c>
       <c r="E3" t="s">
-        <v>2266</v>
+        <v>2315</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
@@ -10293,40 +10610,40 @@
         <v>2055</v>
       </c>
       <c r="U3" t="s">
-        <v>2054</v>
+        <v>2050</v>
       </c>
       <c r="V3" t="s">
         <v>1195</v>
       </c>
       <c r="W3" t="s">
-        <v>2050</v>
+        <v>2054</v>
       </c>
       <c r="X3" t="s">
-        <v>1197</v>
+        <v>1893</v>
       </c>
       <c r="Y3" t="s">
-        <v>721</v>
+        <v>691</v>
       </c>
       <c r="Z3" t="s">
         <v>2051</v>
       </c>
       <c r="AA3" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="AB3" t="s">
         <v>2235</v>
       </c>
       <c r="AC3" t="s">
+        <v>2262</v>
+      </c>
+      <c r="AD3" t="s">
         <v>2265</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>2262</v>
       </c>
       <c r="AE3" t="s">
         <v>2052</v>
       </c>
       <c r="AF3" t="s">
-        <v>1893</v>
+        <v>1197</v>
       </c>
       <c r="AG3" t="s">
         <v>710</v>
@@ -10338,10 +10655,10 @@
         <v>771</v>
       </c>
       <c r="AJ3" t="s">
-        <v>1855</v>
+        <v>2316</v>
       </c>
       <c r="AK3" t="s">
-        <v>1854</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -10352,13 +10669,13 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D4" t="s">
-        <v>1514</v>
+        <v>2318</v>
       </c>
       <c r="E4" t="s">
-        <v>2267</v>
+        <v>2317</v>
       </c>
       <c r="G4" t="s">
         <v>706</v>
@@ -10382,31 +10699,31 @@
         <v>2050</v>
       </c>
       <c r="X4" t="s">
-        <v>691</v>
+        <v>2051</v>
       </c>
       <c r="Y4" t="s">
         <v>2056</v>
       </c>
       <c r="Z4" t="s">
-        <v>2051</v>
+        <v>691</v>
       </c>
       <c r="AA4" t="s">
         <v>721</v>
       </c>
       <c r="AB4" t="s">
+        <v>2057</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>2262</v>
+      </c>
+      <c r="AD4" t="s">
         <v>700</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>2184</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>2262</v>
       </c>
       <c r="AE4" t="s">
         <v>2185</v>
       </c>
       <c r="AF4" t="s">
-        <v>2057</v>
+        <v>2184</v>
       </c>
       <c r="AG4" t="s">
         <v>2189</v>
@@ -10418,10 +10735,10 @@
         <v>305</v>
       </c>
       <c r="AJ4" t="s">
-        <v>1857</v>
+        <v>2318</v>
       </c>
       <c r="AK4" t="s">
-        <v>1856</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -10432,13 +10749,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>2093</v>
+        <v>821</v>
       </c>
       <c r="D5" t="s">
-        <v>1524</v>
+        <v>2074</v>
       </c>
       <c r="E5" t="s">
-        <v>2270</v>
+        <v>2319</v>
       </c>
       <c r="G5" t="s">
         <v>706</v>
@@ -10453,43 +10770,43 @@
         <v>2268</v>
       </c>
       <c r="U5" t="s">
-        <v>1197</v>
+        <v>2047</v>
       </c>
       <c r="V5" t="s">
+        <v>2269</v>
+      </c>
+      <c r="W5" t="s">
         <v>1195</v>
       </c>
-      <c r="W5" t="s">
-        <v>2047</v>
-      </c>
       <c r="X5" t="s">
-        <v>2180</v>
+        <v>2051</v>
       </c>
       <c r="Y5" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA5" t="s">
         <v>2220</v>
       </c>
-      <c r="Z5" t="s">
-        <v>2051</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>680</v>
-      </c>
       <c r="AB5" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="AC5" t="s">
+        <v>2184</v>
+      </c>
+      <c r="AD5" t="s">
         <v>1376</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>2184</v>
       </c>
       <c r="AE5" t="s">
         <v>2185</v>
       </c>
       <c r="AF5" t="s">
-        <v>2269</v>
+        <v>1197</v>
       </c>
       <c r="AG5" t="s">
-        <v>700</v>
+        <v>2180</v>
       </c>
       <c r="AH5" t="s">
         <v>952</v>
@@ -10498,10 +10815,10 @@
         <v>2093</v>
       </c>
       <c r="AJ5" t="s">
-        <v>1859</v>
+        <v>2074</v>
       </c>
       <c r="AK5" t="s">
-        <v>1858</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -10512,13 +10829,13 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>703</v>
+        <v>297</v>
       </c>
       <c r="D6" t="s">
-        <v>2272</v>
+        <v>1901</v>
       </c>
       <c r="E6" t="s">
-        <v>2271</v>
+        <v>2320</v>
       </c>
       <c r="G6" t="s">
         <v>672</v>
@@ -10533,55 +10850,55 @@
         <v>1458</v>
       </c>
       <c r="U6" t="s">
+        <v>2242</v>
+      </c>
+      <c r="V6" t="s">
+        <v>2050</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1195</v>
+      </c>
+      <c r="X6" t="s">
         <v>2058</v>
       </c>
-      <c r="V6" t="s">
-        <v>1195</v>
-      </c>
-      <c r="W6" t="s">
-        <v>2176</v>
-      </c>
-      <c r="X6" t="s">
-        <v>2242</v>
-      </c>
       <c r="Y6" t="s">
-        <v>2050</v>
+        <v>2179</v>
       </c>
       <c r="Z6" t="s">
+        <v>742</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>2051</v>
+      </c>
+      <c r="AB6" t="s">
         <v>721</v>
       </c>
-      <c r="AA6" t="s">
-        <v>2236</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>2051</v>
-      </c>
       <c r="AC6" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AD6" t="s">
         <v>2262</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>2265</v>
       </c>
       <c r="AE6" t="s">
         <v>411</v>
       </c>
       <c r="AF6" t="s">
-        <v>2179</v>
+        <v>2176</v>
       </c>
       <c r="AG6" t="s">
         <v>1491</v>
       </c>
       <c r="AH6" t="s">
-        <v>742</v>
+        <v>2236</v>
       </c>
       <c r="AI6" t="s">
         <v>703</v>
       </c>
       <c r="AJ6" t="s">
-        <v>1465</v>
+        <v>1901</v>
       </c>
       <c r="AK6" t="s">
-        <v>1860</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -10592,13 +10909,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>844</v>
+        <v>673</v>
       </c>
       <c r="D7" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="E7" t="s">
-        <v>2273</v>
+        <v>2321</v>
       </c>
       <c r="G7" t="s">
         <v>653</v>
@@ -10613,16 +10930,16 @@
         <v>726</v>
       </c>
       <c r="U7" t="s">
-        <v>1197</v>
+        <v>2261</v>
       </c>
       <c r="V7" t="s">
         <v>2242</v>
       </c>
       <c r="W7" t="s">
-        <v>750</v>
+        <v>2054</v>
       </c>
       <c r="X7" t="s">
-        <v>2261</v>
+        <v>2200</v>
       </c>
       <c r="Y7" t="s">
         <v>680</v>
@@ -10634,22 +10951,22 @@
         <v>2051</v>
       </c>
       <c r="AB7" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AC7" t="s">
         <v>1376</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>2262</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>2265</v>
       </c>
       <c r="AE7" t="s">
         <v>2055</v>
       </c>
       <c r="AF7" t="s">
-        <v>2200</v>
+        <v>1197</v>
       </c>
       <c r="AG7" t="s">
-        <v>2054</v>
+        <v>750</v>
       </c>
       <c r="AH7" t="s">
         <v>2057</v>
@@ -10658,10 +10975,10 @@
         <v>844</v>
       </c>
       <c r="AJ7" t="s">
-        <v>1467</v>
+        <v>1549</v>
       </c>
       <c r="AK7" t="s">
-        <v>1861</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -10678,7 +10995,7 @@
         <v>1501</v>
       </c>
       <c r="E8" t="s">
-        <v>2274</v>
+        <v>2322</v>
       </c>
       <c r="G8" t="s">
         <v>706</v>
@@ -10738,10 +11055,10 @@
         <v>316</v>
       </c>
       <c r="AJ8" t="s">
-        <v>1549</v>
+        <v>1501</v>
       </c>
       <c r="AK8" t="s">
-        <v>1862</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -10752,13 +11069,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>907</v>
+        <v>829</v>
       </c>
       <c r="D9" t="s">
-        <v>2277</v>
+        <v>1426</v>
       </c>
       <c r="E9" t="s">
-        <v>2276</v>
+        <v>2323</v>
       </c>
       <c r="G9" t="s">
         <v>706</v>
@@ -10782,19 +11099,19 @@
         <v>2261</v>
       </c>
       <c r="X9" t="s">
-        <v>750</v>
+        <v>739</v>
       </c>
       <c r="Y9" t="s">
         <v>2243</v>
       </c>
       <c r="Z9" t="s">
+        <v>2180</v>
+      </c>
+      <c r="AA9" t="s">
         <v>2051</v>
       </c>
-      <c r="AA9" t="s">
-        <v>2180</v>
-      </c>
       <c r="AB9" t="s">
-        <v>739</v>
+        <v>2275</v>
       </c>
       <c r="AC9" t="s">
         <v>1376</v>
@@ -10809,7 +11126,7 @@
         <v>2220</v>
       </c>
       <c r="AG9" t="s">
-        <v>2275</v>
+        <v>750</v>
       </c>
       <c r="AH9" t="s">
         <v>1387</v>
@@ -10818,10 +11135,10 @@
         <v>907</v>
       </c>
       <c r="AJ9" t="s">
-        <v>1466</v>
+        <v>1426</v>
       </c>
       <c r="AK9" t="s">
-        <v>1863</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -10832,13 +11149,13 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>2066</v>
+        <v>912</v>
       </c>
       <c r="D10" t="s">
-        <v>2272</v>
+        <v>1852</v>
       </c>
       <c r="E10" t="s">
-        <v>2271</v>
+        <v>2324</v>
       </c>
       <c r="G10" t="s">
         <v>672</v>
@@ -10853,13 +11170,13 @@
         <v>2238</v>
       </c>
       <c r="U10" t="s">
+        <v>2261</v>
+      </c>
+      <c r="V10" t="s">
+        <v>782</v>
+      </c>
+      <c r="W10" t="s">
         <v>2050</v>
-      </c>
-      <c r="V10" t="s">
-        <v>1197</v>
-      </c>
-      <c r="W10" t="s">
-        <v>2261</v>
       </c>
       <c r="X10" t="s">
         <v>2051</v>
@@ -10868,25 +11185,25 @@
         <v>691</v>
       </c>
       <c r="Z10" t="s">
+        <v>2179</v>
+      </c>
+      <c r="AA10" t="s">
         <v>1893</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>2179</v>
       </c>
       <c r="AB10" t="s">
         <v>2062</v>
       </c>
       <c r="AC10" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD10" t="s">
         <v>2265</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>682</v>
       </c>
       <c r="AE10" t="s">
         <v>766</v>
       </c>
       <c r="AF10" t="s">
-        <v>782</v>
+        <v>1197</v>
       </c>
       <c r="AG10" t="s">
         <v>2063</v>
@@ -10898,10 +11215,10 @@
         <v>2066</v>
       </c>
       <c r="AJ10" t="s">
-        <v>1807</v>
+        <v>1852</v>
       </c>
       <c r="AK10" t="s">
-        <v>1864</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -10912,13 +11229,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D11" t="s">
-        <v>1903</v>
+        <v>1477</v>
       </c>
       <c r="E11" t="s">
-        <v>2278</v>
+        <v>2325</v>
       </c>
       <c r="G11" t="s">
         <v>653</v>
@@ -10933,28 +11250,28 @@
         <v>2052</v>
       </c>
       <c r="U11" t="s">
+        <v>1195</v>
+      </c>
+      <c r="V11" t="s">
         <v>2050</v>
       </c>
-      <c r="V11" t="s">
-        <v>2176</v>
-      </c>
       <c r="W11" t="s">
-        <v>1195</v>
+        <v>1200</v>
       </c>
       <c r="X11" t="s">
-        <v>1200</v>
+        <v>721</v>
       </c>
       <c r="Y11" t="s">
-        <v>721</v>
+        <v>2051</v>
       </c>
       <c r="Z11" t="s">
+        <v>2179</v>
+      </c>
+      <c r="AA11" t="s">
         <v>680</v>
       </c>
-      <c r="AA11" t="s">
-        <v>2051</v>
-      </c>
       <c r="AB11" t="s">
-        <v>2179</v>
+        <v>2275</v>
       </c>
       <c r="AC11" t="s">
         <v>682</v>
@@ -10966,7 +11283,7 @@
         <v>1370</v>
       </c>
       <c r="AF11" t="s">
-        <v>2275</v>
+        <v>2176</v>
       </c>
       <c r="AG11" t="s">
         <v>2216</v>
@@ -10978,10 +11295,10 @@
         <v>278</v>
       </c>
       <c r="AJ11" t="s">
-        <v>1832</v>
+        <v>1477</v>
       </c>
       <c r="AK11" t="s">
-        <v>1865</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -10992,13 +11309,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>1459</v>
+        <v>730</v>
       </c>
       <c r="D12" t="s">
-        <v>1526</v>
+        <v>1514</v>
       </c>
       <c r="E12" t="s">
-        <v>2280</v>
+        <v>2326</v>
       </c>
       <c r="G12" t="s">
         <v>653</v>
@@ -11013,28 +11330,28 @@
         <v>1458</v>
       </c>
       <c r="U12" t="s">
+        <v>688</v>
+      </c>
+      <c r="V12" t="s">
+        <v>2047</v>
+      </c>
+      <c r="W12" t="s">
         <v>1200</v>
       </c>
-      <c r="V12" t="s">
-        <v>688</v>
-      </c>
-      <c r="W12" t="s">
-        <v>2047</v>
-      </c>
       <c r="X12" t="s">
-        <v>2189</v>
+        <v>2054</v>
       </c>
       <c r="Y12" t="s">
-        <v>2279</v>
+        <v>721</v>
       </c>
       <c r="Z12" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA12" t="s">
         <v>2051</v>
       </c>
-      <c r="AA12" t="s">
-        <v>691</v>
-      </c>
       <c r="AB12" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="AC12" t="s">
         <v>2262</v>
@@ -11049,19 +11366,19 @@
         <v>438</v>
       </c>
       <c r="AG12" t="s">
-        <v>682</v>
+        <v>2189</v>
       </c>
       <c r="AH12" t="s">
-        <v>2054</v>
+        <v>2279</v>
       </c>
       <c r="AI12" t="s">
         <v>1459</v>
       </c>
       <c r="AJ12" t="s">
-        <v>1800</v>
+        <v>1514</v>
       </c>
       <c r="AK12" t="s">
-        <v>1866</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -11072,13 +11389,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D13" t="s">
-        <v>2283</v>
+        <v>1524</v>
       </c>
       <c r="E13" t="s">
-        <v>2282</v>
+        <v>2327</v>
       </c>
       <c r="G13" t="s">
         <v>706</v>
@@ -11093,25 +11410,25 @@
         <v>2065</v>
       </c>
       <c r="U13" t="s">
+        <v>2050</v>
+      </c>
+      <c r="V13" t="s">
         <v>2261</v>
       </c>
-      <c r="V13" t="s">
-        <v>2050</v>
-      </c>
       <c r="W13" t="s">
-        <v>1197</v>
+        <v>782</v>
       </c>
       <c r="X13" t="s">
         <v>1195</v>
       </c>
       <c r="Y13" t="s">
-        <v>691</v>
+        <v>2051</v>
       </c>
       <c r="Z13" t="s">
         <v>1893</v>
       </c>
       <c r="AA13" t="s">
-        <v>2051</v>
+        <v>691</v>
       </c>
       <c r="AB13" t="s">
         <v>2281</v>
@@ -11126,7 +11443,7 @@
         <v>1458</v>
       </c>
       <c r="AF13" t="s">
-        <v>782</v>
+        <v>1197</v>
       </c>
       <c r="AG13" t="s">
         <v>2179</v>
@@ -11138,10 +11455,10 @@
         <v>290</v>
       </c>
       <c r="AJ13" t="s">
-        <v>1868</v>
+        <v>1524</v>
       </c>
       <c r="AK13" t="s">
-        <v>1867</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -11152,13 +11469,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>2093</v>
+        <v>673</v>
       </c>
       <c r="D14" t="s">
-        <v>1354</v>
+        <v>2316</v>
       </c>
       <c r="E14" t="s">
-        <v>2069</v>
+        <v>2315</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -11173,55 +11490,55 @@
         <v>2238</v>
       </c>
       <c r="U14" t="s">
-        <v>565</v>
+        <v>789</v>
       </c>
       <c r="V14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="W14" t="s">
+        <v>2328</v>
+      </c>
+      <c r="X14" t="s">
         <v>2067</v>
-      </c>
-      <c r="W14" t="s">
-        <v>792</v>
-      </c>
-      <c r="X14" t="s">
-        <v>789</v>
       </c>
       <c r="Y14" t="s">
         <v>2044</v>
       </c>
       <c r="Z14" t="s">
-        <v>2180</v>
+        <v>2057</v>
       </c>
       <c r="AA14" t="s">
         <v>2068</v>
       </c>
       <c r="AB14" t="s">
-        <v>1388</v>
+        <v>2063</v>
       </c>
       <c r="AC14" t="s">
         <v>692</v>
       </c>
       <c r="AD14" t="s">
-        <v>2223</v>
+        <v>2329</v>
       </c>
       <c r="AE14" t="s">
         <v>2185</v>
       </c>
       <c r="AF14" t="s">
-        <v>1989</v>
+        <v>565</v>
       </c>
       <c r="AG14" t="s">
-        <v>2057</v>
+        <v>2180</v>
       </c>
       <c r="AH14" t="s">
-        <v>2063</v>
+        <v>2223</v>
       </c>
       <c r="AI14" t="s">
         <v>2093</v>
       </c>
       <c r="AJ14" t="s">
-        <v>1348</v>
+        <v>2316</v>
       </c>
       <c r="AK14" t="s">
-        <v>1870</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -11232,13 +11549,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>268</v>
+        <v>671</v>
       </c>
       <c r="D15" t="s">
-        <v>1902</v>
+        <v>1405</v>
       </c>
       <c r="E15" t="s">
-        <v>2070</v>
+        <v>2330</v>
       </c>
       <c r="G15" t="s">
         <v>672</v>
@@ -11253,16 +11570,16 @@
         <v>1458</v>
       </c>
       <c r="U15" t="s">
-        <v>1989</v>
+        <v>2050</v>
       </c>
       <c r="V15" t="s">
-        <v>2050</v>
+        <v>2054</v>
       </c>
       <c r="W15" t="s">
         <v>1195</v>
       </c>
       <c r="X15" t="s">
-        <v>1197</v>
+        <v>2261</v>
       </c>
       <c r="Y15" t="s">
         <v>2051</v>
@@ -11271,25 +11588,25 @@
         <v>691</v>
       </c>
       <c r="AA15" t="s">
-        <v>2180</v>
+        <v>721</v>
       </c>
       <c r="AB15" t="s">
-        <v>721</v>
+        <v>1372</v>
       </c>
       <c r="AC15" t="s">
         <v>682</v>
       </c>
       <c r="AD15" t="s">
-        <v>2210</v>
+        <v>2262</v>
       </c>
       <c r="AE15" t="s">
         <v>2185</v>
       </c>
       <c r="AF15" t="s">
-        <v>2054</v>
+        <v>1197</v>
       </c>
       <c r="AG15" t="s">
-        <v>1372</v>
+        <v>2180</v>
       </c>
       <c r="AH15" t="s">
         <v>1376</v>
@@ -11298,10 +11615,10 @@
         <v>268</v>
       </c>
       <c r="AJ15" t="s">
-        <v>1418</v>
+        <v>1405</v>
       </c>
       <c r="AK15" t="s">
-        <v>1871</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -11312,13 +11629,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>671</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>2074</v>
+        <v>1479</v>
       </c>
       <c r="E16" t="s">
-        <v>2073</v>
+        <v>2331</v>
       </c>
       <c r="G16" t="s">
         <v>706</v>
@@ -11333,31 +11650,31 @@
         <v>2052</v>
       </c>
       <c r="U16" t="s">
+        <v>2071</v>
+      </c>
+      <c r="V16" t="s">
         <v>2050</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>1200</v>
       </c>
-      <c r="W16" t="s">
-        <v>2071</v>
-      </c>
       <c r="X16" t="s">
+        <v>2072</v>
+      </c>
+      <c r="Y16" t="s">
         <v>721</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>691</v>
       </c>
       <c r="Z16" t="s">
         <v>2051</v>
       </c>
       <c r="AA16" t="s">
-        <v>2180</v>
+        <v>691</v>
       </c>
       <c r="AB16" t="s">
+        <v>1388</v>
+      </c>
+      <c r="AC16" t="s">
         <v>2021</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>1388</v>
       </c>
       <c r="AD16" t="s">
         <v>682</v>
@@ -11366,7 +11683,7 @@
         <v>804</v>
       </c>
       <c r="AF16" t="s">
-        <v>2072</v>
+        <v>2180</v>
       </c>
       <c r="AG16" t="s">
         <v>805</v>
@@ -11378,10 +11695,10 @@
         <v>671</v>
       </c>
       <c r="AJ16" t="s">
-        <v>1873</v>
+        <v>1479</v>
       </c>
       <c r="AK16" t="s">
-        <v>1872</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -11392,13 +11709,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>673</v>
+        <v>829</v>
       </c>
       <c r="D17" t="s">
-        <v>2077</v>
+        <v>1241</v>
       </c>
       <c r="E17" t="s">
-        <v>2076</v>
+        <v>2332</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
@@ -11419,10 +11736,10 @@
         <v>1195</v>
       </c>
       <c r="W17" t="s">
-        <v>2016</v>
+        <v>1197</v>
       </c>
       <c r="X17" t="s">
-        <v>1197</v>
+        <v>805</v>
       </c>
       <c r="Y17" t="s">
         <v>721</v>
@@ -11437,10 +11754,10 @@
         <v>1374</v>
       </c>
       <c r="AC17" t="s">
-        <v>2210</v>
+        <v>682</v>
       </c>
       <c r="AD17" t="s">
-        <v>682</v>
+        <v>2262</v>
       </c>
       <c r="AE17" t="s">
         <v>2185</v>
@@ -11449,7 +11766,7 @@
         <v>1849</v>
       </c>
       <c r="AG17" t="s">
-        <v>805</v>
+        <v>449</v>
       </c>
       <c r="AH17" t="s">
         <v>400</v>
@@ -11458,10 +11775,10 @@
         <v>673</v>
       </c>
       <c r="AJ17" t="s">
-        <v>1875</v>
+        <v>1241</v>
       </c>
       <c r="AK17" t="s">
-        <v>1874</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -11472,13 +11789,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="D18" t="s">
-        <v>1901</v>
+        <v>2074</v>
       </c>
       <c r="E18" t="s">
-        <v>2078</v>
+        <v>2333</v>
       </c>
       <c r="G18" t="s">
         <v>653</v>
@@ -11493,16 +11810,16 @@
         <v>942</v>
       </c>
       <c r="U18" t="s">
-        <v>1197</v>
+        <v>2050</v>
       </c>
       <c r="V18" t="s">
-        <v>2050</v>
+        <v>2216</v>
       </c>
       <c r="W18" t="s">
+        <v>2047</v>
+      </c>
+      <c r="X18" t="s">
         <v>1195</v>
-      </c>
-      <c r="X18" t="s">
-        <v>2047</v>
       </c>
       <c r="Y18" t="s">
         <v>680</v>
@@ -11517,7 +11834,7 @@
         <v>2068</v>
       </c>
       <c r="AC18" t="s">
-        <v>2210</v>
+        <v>2262</v>
       </c>
       <c r="AD18" t="s">
         <v>2022</v>
@@ -11526,7 +11843,7 @@
         <v>2185</v>
       </c>
       <c r="AF18" t="s">
-        <v>2216</v>
+        <v>1197</v>
       </c>
       <c r="AG18" t="s">
         <v>438</v>
@@ -11538,10 +11855,10 @@
         <v>282</v>
       </c>
       <c r="AJ18" t="s">
-        <v>1868</v>
+        <v>2074</v>
       </c>
       <c r="AK18" t="s">
-        <v>1876</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -11552,13 +11869,13 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>703</v>
+        <v>305</v>
       </c>
       <c r="D19" t="s">
-        <v>2080</v>
+        <v>1823</v>
       </c>
       <c r="E19" t="s">
-        <v>2079</v>
+        <v>2334</v>
       </c>
       <c r="G19" t="s">
         <v>706</v>
@@ -11576,13 +11893,13 @@
         <v>2058</v>
       </c>
       <c r="V19" t="s">
-        <v>1989</v>
+        <v>1195</v>
       </c>
       <c r="W19" t="s">
-        <v>1195</v>
+        <v>2261</v>
       </c>
       <c r="X19" t="s">
-        <v>2051</v>
+        <v>2245</v>
       </c>
       <c r="Y19" t="s">
         <v>680</v>
@@ -11594,19 +11911,19 @@
         <v>2056</v>
       </c>
       <c r="AB19" t="s">
-        <v>1848</v>
+        <v>2051</v>
       </c>
       <c r="AC19" t="s">
-        <v>2184</v>
+        <v>682</v>
       </c>
       <c r="AD19" t="s">
-        <v>682</v>
+        <v>2281</v>
       </c>
       <c r="AE19" t="s">
         <v>1370</v>
       </c>
       <c r="AF19" t="s">
-        <v>2245</v>
+        <v>2184</v>
       </c>
       <c r="AG19" t="s">
         <v>2186</v>
@@ -11618,10 +11935,10 @@
         <v>703</v>
       </c>
       <c r="AJ19" t="s">
-        <v>1426</v>
+        <v>1823</v>
       </c>
       <c r="AK19" t="s">
-        <v>1877</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -11632,13 +11949,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>829</v>
+        <v>268</v>
       </c>
       <c r="D20" t="s">
-        <v>2082</v>
+        <v>1433</v>
       </c>
       <c r="E20" t="s">
-        <v>2081</v>
+        <v>2335</v>
       </c>
       <c r="G20" t="s">
         <v>672</v>
@@ -11653,55 +11970,55 @@
         <v>1987</v>
       </c>
       <c r="U20" t="s">
-        <v>1989</v>
+        <v>2054</v>
       </c>
       <c r="V20" t="s">
-        <v>1387</v>
+        <v>2261</v>
       </c>
       <c r="W20" t="s">
         <v>2050</v>
       </c>
       <c r="X20" t="s">
+        <v>2057</v>
+      </c>
+      <c r="Y20" t="s">
         <v>2179</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>680</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>2180</v>
       </c>
       <c r="AA20" t="s">
         <v>2051</v>
       </c>
       <c r="AB20" t="s">
+        <v>2262</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>700</v>
+      </c>
+      <c r="AD20" t="s">
         <v>1376</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>2210</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>700</v>
       </c>
       <c r="AE20" t="s">
         <v>2052</v>
       </c>
       <c r="AF20" t="s">
-        <v>2016</v>
+        <v>449</v>
       </c>
       <c r="AG20" t="s">
-        <v>2054</v>
+        <v>1387</v>
       </c>
       <c r="AH20" t="s">
-        <v>2057</v>
+        <v>2180</v>
       </c>
       <c r="AI20" t="s">
         <v>829</v>
       </c>
       <c r="AJ20" t="s">
-        <v>1850</v>
+        <v>1433</v>
       </c>
       <c r="AK20" t="s">
-        <v>1878</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -11712,13 +12029,13 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>778</v>
+        <v>268</v>
       </c>
       <c r="D21" t="s">
-        <v>1826</v>
+        <v>2337</v>
       </c>
       <c r="E21" t="s">
-        <v>2083</v>
+        <v>2336</v>
       </c>
       <c r="G21" t="s">
         <v>706</v>
@@ -11733,19 +12050,19 @@
         <v>1458</v>
       </c>
       <c r="U21" t="s">
-        <v>1989</v>
+        <v>1195</v>
       </c>
       <c r="V21" t="s">
         <v>2050</v>
       </c>
       <c r="W21" t="s">
-        <v>1195</v>
+        <v>2261</v>
       </c>
       <c r="X21" t="s">
+        <v>2054</v>
+      </c>
+      <c r="Y21" t="s">
         <v>2051</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>438</v>
       </c>
       <c r="Z21" t="s">
         <v>691</v>
@@ -11757,7 +12074,7 @@
         <v>2184</v>
       </c>
       <c r="AC21" t="s">
-        <v>1848</v>
+        <v>2281</v>
       </c>
       <c r="AD21" t="s">
         <v>682</v>
@@ -11772,16 +12089,16 @@
         <v>2186</v>
       </c>
       <c r="AH21" t="s">
-        <v>2054</v>
+        <v>438</v>
       </c>
       <c r="AI21" t="s">
         <v>778</v>
       </c>
       <c r="AJ21" t="s">
-        <v>1493</v>
+        <v>2337</v>
       </c>
       <c r="AK21" t="s">
-        <v>1879</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -11792,13 +12109,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>841</v>
+        <v>290</v>
       </c>
       <c r="D22" t="s">
-        <v>2085</v>
+        <v>1817</v>
       </c>
       <c r="E22" t="s">
-        <v>2084</v>
+        <v>2338</v>
       </c>
       <c r="G22" t="s">
         <v>452</v>
@@ -11810,31 +12127,31 @@
         <v>830</v>
       </c>
       <c r="T22" t="s">
-        <v>2185</v>
+        <v>2052</v>
       </c>
       <c r="U22" t="s">
+        <v>2269</v>
+      </c>
+      <c r="V22" t="s">
         <v>2050</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
+        <v>2261</v>
+      </c>
+      <c r="X22" t="s">
         <v>1195</v>
       </c>
-      <c r="W22" t="s">
-        <v>1989</v>
-      </c>
-      <c r="X22" t="s">
-        <v>2003</v>
-      </c>
       <c r="Y22" t="s">
-        <v>438</v>
+        <v>680</v>
       </c>
       <c r="Z22" t="s">
+        <v>2051</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AB22" t="s">
         <v>2056</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>680</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>2051</v>
       </c>
       <c r="AC22" t="s">
         <v>2062</v>
@@ -11843,10 +12160,10 @@
         <v>1373</v>
       </c>
       <c r="AE22" t="s">
-        <v>2052</v>
+        <v>2185</v>
       </c>
       <c r="AF22" t="s">
-        <v>1385</v>
+        <v>438</v>
       </c>
       <c r="AG22" t="s">
         <v>1197</v>
@@ -11858,10 +12175,10 @@
         <v>841</v>
       </c>
       <c r="AJ22" t="s">
-        <v>1806</v>
+        <v>1817</v>
       </c>
       <c r="AK22" t="s">
-        <v>1880</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -11872,13 +12189,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>278</v>
+        <v>703</v>
       </c>
       <c r="D23" t="s">
-        <v>1800</v>
+        <v>1890</v>
       </c>
       <c r="E23" t="s">
-        <v>2086</v>
+        <v>2339</v>
       </c>
       <c r="G23" t="s">
         <v>2025</v>
@@ -11893,43 +12210,43 @@
         <v>2065</v>
       </c>
       <c r="U23" t="s">
-        <v>2016</v>
+        <v>1195</v>
       </c>
       <c r="V23" t="s">
-        <v>1197</v>
+        <v>2054</v>
       </c>
       <c r="W23" t="s">
         <v>2050</v>
       </c>
       <c r="X23" t="s">
-        <v>1195</v>
+        <v>2180</v>
       </c>
       <c r="Y23" t="s">
         <v>2051</v>
       </c>
       <c r="Z23" t="s">
-        <v>2180</v>
+        <v>721</v>
       </c>
       <c r="AA23" t="s">
         <v>691</v>
       </c>
       <c r="AB23" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="AC23" t="s">
-        <v>2211</v>
+        <v>2262</v>
       </c>
       <c r="AD23" t="s">
-        <v>2210</v>
+        <v>2275</v>
       </c>
       <c r="AE23" t="s">
         <v>399</v>
       </c>
       <c r="AF23" t="s">
-        <v>682</v>
+        <v>449</v>
       </c>
       <c r="AG23" t="s">
-        <v>2054</v>
+        <v>1197</v>
       </c>
       <c r="AH23" t="s">
         <v>1849</v>
@@ -11938,10 +12255,10 @@
         <v>278</v>
       </c>
       <c r="AJ23" t="s">
-        <v>1868</v>
+        <v>1890</v>
       </c>
       <c r="AK23" t="s">
-        <v>1867</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -11952,13 +12269,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>2093</v>
+        <v>2066</v>
       </c>
       <c r="D24" t="s">
-        <v>2247</v>
+        <v>2080</v>
       </c>
       <c r="E24" t="s">
-        <v>2246</v>
+        <v>2340</v>
       </c>
       <c r="G24" t="s">
         <v>672</v>
@@ -11976,31 +12293,31 @@
         <v>1195</v>
       </c>
       <c r="V24" t="s">
-        <v>1989</v>
+        <v>2240</v>
       </c>
       <c r="W24" t="s">
-        <v>2240</v>
+        <v>2261</v>
       </c>
       <c r="X24" t="s">
+        <v>2054</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>2051</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA24" t="s">
         <v>721</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>691</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>2180</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>2051</v>
       </c>
       <c r="AB24" t="s">
         <v>2243</v>
       </c>
       <c r="AC24" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AD24" t="s">
         <v>2088</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>1995</v>
       </c>
       <c r="AE24" t="s">
         <v>2185</v>
@@ -12009,7 +12326,7 @@
         <v>710</v>
       </c>
       <c r="AG24" t="s">
-        <v>2054</v>
+        <v>2180</v>
       </c>
       <c r="AH24" t="s">
         <v>2237</v>
@@ -12018,10 +12335,10 @@
         <v>2093</v>
       </c>
       <c r="AJ24" t="s">
-        <v>1806</v>
+        <v>2080</v>
       </c>
       <c r="AK24" t="s">
-        <v>1880</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -12032,13 +12349,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>1805</v>
+        <v>2048</v>
       </c>
       <c r="D25" t="s">
-        <v>2249</v>
+        <v>2342</v>
       </c>
       <c r="E25" t="s">
-        <v>2248</v>
+        <v>2341</v>
       </c>
       <c r="G25" t="s">
         <v>653</v>
@@ -12050,58 +12367,58 @@
         <v>487</v>
       </c>
       <c r="T25" t="s">
-        <v>2006</v>
+        <v>726</v>
       </c>
       <c r="U25" t="s">
-        <v>2007</v>
+        <v>1200</v>
       </c>
       <c r="V25" t="s">
-        <v>2003</v>
+        <v>2269</v>
       </c>
       <c r="W25" t="s">
-        <v>1200</v>
+        <v>688</v>
       </c>
       <c r="X25" t="s">
+        <v>2200</v>
+      </c>
+      <c r="Y25" t="s">
         <v>2179</v>
       </c>
-      <c r="Y25" t="s">
-        <v>2026</v>
-      </c>
       <c r="Z25" t="s">
-        <v>2200</v>
+        <v>2057</v>
       </c>
       <c r="AA25" t="s">
-        <v>2180</v>
+        <v>1170</v>
       </c>
       <c r="AB25" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>2022</v>
+      </c>
+      <c r="AD25" t="s">
         <v>1388</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>682</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>2022</v>
       </c>
       <c r="AE25" t="s">
         <v>2185</v>
       </c>
       <c r="AF25" t="s">
-        <v>2004</v>
+        <v>952</v>
       </c>
       <c r="AG25" t="s">
         <v>750</v>
       </c>
       <c r="AH25" t="s">
-        <v>2057</v>
+        <v>2180</v>
       </c>
       <c r="AI25" t="s">
         <v>1805</v>
       </c>
       <c r="AJ25" t="s">
-        <v>1882</v>
+        <v>2342</v>
       </c>
       <c r="AK25" t="s">
-        <v>1881</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -12112,13 +12429,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>712</v>
+        <v>272</v>
       </c>
       <c r="D26" t="s">
-        <v>1538</v>
+        <v>2247</v>
       </c>
       <c r="E26" t="s">
-        <v>2250</v>
+        <v>2343</v>
       </c>
       <c r="G26" t="s">
         <v>706</v>
@@ -12133,43 +12450,43 @@
         <v>2055</v>
       </c>
       <c r="U26" t="s">
+        <v>1195</v>
+      </c>
+      <c r="V26" t="s">
+        <v>2047</v>
+      </c>
+      <c r="W26" t="s">
+        <v>2261</v>
+      </c>
+      <c r="X26" t="s">
         <v>2050</v>
       </c>
-      <c r="V26" t="s">
-        <v>1989</v>
-      </c>
-      <c r="W26" t="s">
-        <v>1195</v>
-      </c>
-      <c r="X26" t="s">
-        <v>2047</v>
-      </c>
       <c r="Y26" t="s">
+        <v>2054</v>
+      </c>
+      <c r="Z26" t="s">
         <v>2051</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>2180</v>
       </c>
       <c r="AA26" t="s">
         <v>691</v>
       </c>
       <c r="AB26" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AC26" t="s">
         <v>1376</v>
       </c>
-      <c r="AC26" t="s">
-        <v>1848</v>
-      </c>
       <c r="AD26" t="s">
-        <v>2184</v>
+        <v>2281</v>
       </c>
       <c r="AE26" t="s">
         <v>2185</v>
       </c>
       <c r="AF26" t="s">
-        <v>1385</v>
+        <v>2180</v>
       </c>
       <c r="AG26" t="s">
-        <v>2054</v>
+        <v>2184</v>
       </c>
       <c r="AH26" t="s">
         <v>2186</v>
@@ -12178,10 +12495,10 @@
         <v>712</v>
       </c>
       <c r="AJ26" t="s">
-        <v>1852</v>
+        <v>2247</v>
       </c>
       <c r="AK26" t="s">
-        <v>1883</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -12192,13 +12509,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>1459</v>
+        <v>290</v>
       </c>
       <c r="D27" t="s">
-        <v>2252</v>
+        <v>2345</v>
       </c>
       <c r="E27" t="s">
-        <v>2251</v>
+        <v>2344</v>
       </c>
       <c r="G27" t="s">
         <v>653</v>
@@ -12216,37 +12533,37 @@
         <v>2050</v>
       </c>
       <c r="V27" t="s">
+        <v>688</v>
+      </c>
+      <c r="W27" t="s">
         <v>1195</v>
       </c>
-      <c r="W27" t="s">
-        <v>1989</v>
-      </c>
       <c r="X27" t="s">
-        <v>2007</v>
+        <v>2261</v>
       </c>
       <c r="Y27" t="s">
+        <v>2051</v>
+      </c>
+      <c r="Z27" t="s">
         <v>680</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AA27" t="s">
         <v>2044</v>
       </c>
-      <c r="AA27" t="s">
-        <v>2051</v>
-      </c>
       <c r="AB27" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AC27" t="s">
         <v>1388</v>
       </c>
-      <c r="AC27" t="s">
-        <v>1848</v>
-      </c>
       <c r="AD27" t="s">
-        <v>2184</v>
+        <v>2281</v>
       </c>
       <c r="AE27" t="s">
         <v>2185</v>
       </c>
       <c r="AF27" t="s">
-        <v>1385</v>
+        <v>2184</v>
       </c>
       <c r="AG27" t="s">
         <v>1372</v>
@@ -12258,10 +12575,10 @@
         <v>1459</v>
       </c>
       <c r="AJ27" t="s">
-        <v>1521</v>
+        <v>2345</v>
       </c>
       <c r="AK27" t="s">
-        <v>1884</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -12272,13 +12589,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>1522</v>
+        <v>297</v>
       </c>
       <c r="D28" t="s">
-        <v>1538</v>
+        <v>1488</v>
       </c>
       <c r="E28" t="s">
-        <v>2253</v>
+        <v>2346</v>
       </c>
       <c r="G28" t="s">
         <v>452</v>
@@ -12293,43 +12610,43 @@
         <v>2052</v>
       </c>
       <c r="U28" t="s">
+        <v>2050</v>
+      </c>
+      <c r="V28" t="s">
+        <v>688</v>
+      </c>
+      <c r="W28" t="s">
         <v>1195</v>
       </c>
-      <c r="V28" t="s">
-        <v>2050</v>
-      </c>
-      <c r="W28" t="s">
-        <v>2007</v>
-      </c>
       <c r="X28" t="s">
+        <v>2054</v>
+      </c>
+      <c r="Y28" t="s">
         <v>2051</v>
       </c>
-      <c r="Y28" t="s">
-        <v>438</v>
-      </c>
       <c r="Z28" t="s">
+        <v>2063</v>
+      </c>
+      <c r="AA28" t="s">
         <v>1385</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>2056</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AC28" t="s">
+        <v>2275</v>
+      </c>
+      <c r="AD28" t="s">
         <v>682</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>2184</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>2211</v>
       </c>
       <c r="AE28" t="s">
         <v>2185</v>
       </c>
       <c r="AF28" t="s">
-        <v>2063</v>
+        <v>438</v>
       </c>
       <c r="AG28" t="s">
-        <v>2054</v>
+        <v>2184</v>
       </c>
       <c r="AH28" t="s">
         <v>1183</v>
@@ -12338,10 +12655,10 @@
         <v>1522</v>
       </c>
       <c r="AJ28" t="s">
-        <v>1418</v>
+        <v>1488</v>
       </c>
       <c r="AK28" t="s">
-        <v>1885</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -12352,13 +12669,13 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>829</v>
+        <v>841</v>
       </c>
       <c r="D29" t="s">
-        <v>1815</v>
+        <v>1471</v>
       </c>
       <c r="E29" t="s">
-        <v>2254</v>
+        <v>2347</v>
       </c>
       <c r="G29" t="s">
         <v>653</v>
@@ -12373,40 +12690,40 @@
         <v>2055</v>
       </c>
       <c r="U29" t="s">
-        <v>2241</v>
+        <v>1195</v>
       </c>
       <c r="V29" t="s">
-        <v>1195</v>
+        <v>2050</v>
       </c>
       <c r="W29" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="X29" t="s">
-        <v>2050</v>
+        <v>1851</v>
       </c>
       <c r="Y29" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>2056</v>
+      </c>
+      <c r="AA29" t="s">
         <v>2180</v>
       </c>
-      <c r="Z29" t="s">
-        <v>691</v>
-      </c>
-      <c r="AA29" t="s">
+      <c r="AB29" t="s">
         <v>2051</v>
       </c>
-      <c r="AB29" t="s">
-        <v>2056</v>
-      </c>
       <c r="AC29" t="s">
+        <v>1376</v>
+      </c>
+      <c r="AD29" t="s">
         <v>2184</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>1376</v>
       </c>
       <c r="AE29" t="s">
         <v>2185</v>
       </c>
       <c r="AF29" t="s">
-        <v>1851</v>
+        <v>2241</v>
       </c>
       <c r="AG29" t="s">
         <v>710</v>
@@ -12418,10 +12735,10 @@
         <v>829</v>
       </c>
       <c r="AJ29" t="s">
-        <v>1804</v>
+        <v>1471</v>
       </c>
       <c r="AK29" t="s">
-        <v>1886</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -12432,13 +12749,13 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>294</v>
+        <v>2348</v>
       </c>
       <c r="D30" t="s">
-        <v>2256</v>
+        <v>1810</v>
       </c>
       <c r="E30" t="s">
-        <v>2255</v>
+        <v>2349</v>
       </c>
       <c r="G30" t="s">
         <v>578</v>
@@ -12459,34 +12776,34 @@
         <v>2050</v>
       </c>
       <c r="W30" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="X30" t="s">
-        <v>438</v>
+        <v>2072</v>
       </c>
       <c r="Y30" t="s">
         <v>2051</v>
       </c>
       <c r="Z30" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA30" t="s">
         <v>2056</v>
       </c>
-      <c r="AA30" t="s">
-        <v>691</v>
-      </c>
       <c r="AB30" t="s">
-        <v>2211</v>
+        <v>2275</v>
       </c>
       <c r="AC30" t="s">
-        <v>1848</v>
+        <v>2265</v>
       </c>
       <c r="AD30" t="s">
-        <v>1995</v>
+        <v>2281</v>
       </c>
       <c r="AE30" t="s">
         <v>2185</v>
       </c>
       <c r="AF30" t="s">
-        <v>2072</v>
+        <v>438</v>
       </c>
       <c r="AG30" t="s">
         <v>2186</v>
@@ -12498,10 +12815,10 @@
         <v>294</v>
       </c>
       <c r="AJ30" t="s">
-        <v>1804</v>
+        <v>1810</v>
       </c>
       <c r="AK30" t="s">
-        <v>1887</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -12512,13 +12829,13 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>730</v>
+        <v>278</v>
       </c>
       <c r="D31" t="s">
-        <v>1486</v>
+        <v>2080</v>
       </c>
       <c r="E31" t="s">
-        <v>2257</v>
+        <v>2340</v>
       </c>
       <c r="G31" t="s">
         <v>452</v>
@@ -12533,31 +12850,31 @@
         <v>1458</v>
       </c>
       <c r="U31" t="s">
+        <v>2050</v>
+      </c>
+      <c r="V31" t="s">
         <v>1195</v>
       </c>
-      <c r="V31" t="s">
-        <v>1989</v>
-      </c>
       <c r="W31" t="s">
-        <v>2050</v>
+        <v>2261</v>
       </c>
       <c r="X31" t="s">
-        <v>2189</v>
+        <v>2054</v>
       </c>
       <c r="Y31" t="s">
+        <v>2051</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AA31" t="s">
         <v>680</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AB31" t="s">
         <v>2056</v>
       </c>
-      <c r="AA31" t="s">
-        <v>2051</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>1385</v>
-      </c>
       <c r="AC31" t="s">
-        <v>2184</v>
+        <v>682</v>
       </c>
       <c r="AD31" t="s">
         <v>1376</v>
@@ -12566,10 +12883,10 @@
         <v>2185</v>
       </c>
       <c r="AF31" t="s">
-        <v>682</v>
+        <v>2189</v>
       </c>
       <c r="AG31" t="s">
-        <v>2054</v>
+        <v>2184</v>
       </c>
       <c r="AH31" t="s">
         <v>2186</v>
@@ -12578,10 +12895,10 @@
         <v>730</v>
       </c>
       <c r="AJ31" t="s">
-        <v>1852</v>
+        <v>2080</v>
       </c>
       <c r="AK31" t="s">
-        <v>1888</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -12592,13 +12909,13 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>730</v>
+        <v>278</v>
       </c>
       <c r="D32" t="s">
-        <v>1540</v>
+        <v>1517</v>
       </c>
       <c r="E32" t="s">
-        <v>2258</v>
+        <v>2350</v>
       </c>
       <c r="G32" t="s">
         <v>672</v>
@@ -12616,7 +12933,7 @@
         <v>2050</v>
       </c>
       <c r="V32" t="s">
-        <v>1989</v>
+        <v>2261</v>
       </c>
       <c r="W32" t="s">
         <v>1195</v>
@@ -12637,7 +12954,7 @@
         <v>2243</v>
       </c>
       <c r="AC32" t="s">
-        <v>2210</v>
+        <v>2262</v>
       </c>
       <c r="AD32" t="s">
         <v>1388</v>
@@ -12658,10 +12975,10 @@
         <v>730</v>
       </c>
       <c r="AJ32" t="s">
-        <v>1890</v>
+        <v>1517</v>
       </c>
       <c r="AK32" t="s">
-        <v>1889</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -12672,13 +12989,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
+        <v>703</v>
       </c>
       <c r="D33" t="s">
-        <v>2260</v>
+        <v>2352</v>
       </c>
       <c r="E33" t="s">
-        <v>2259</v>
+        <v>2351</v>
       </c>
       <c r="G33" t="s">
         <v>672</v>
@@ -12693,28 +13010,28 @@
         <v>1458</v>
       </c>
       <c r="U33" t="s">
+        <v>2261</v>
+      </c>
+      <c r="V33" t="s">
         <v>1195</v>
-      </c>
-      <c r="V33" t="s">
-        <v>1989</v>
       </c>
       <c r="W33" t="s">
         <v>2050</v>
       </c>
       <c r="X33" t="s">
+        <v>2047</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>2051</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>2056</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="AB33" t="s">
         <v>691</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>1385</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>2051</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>2056</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>2184</v>
       </c>
       <c r="AC33" t="s">
         <v>1376</v>
@@ -12726,7 +13043,7 @@
         <v>2185</v>
       </c>
       <c r="AF33" t="s">
-        <v>2047</v>
+        <v>2184</v>
       </c>
       <c r="AG33" t="s">
         <v>2186</v>
@@ -12738,10 +13055,10 @@
         <v>288</v>
       </c>
       <c r="AJ33" t="s">
-        <v>1475</v>
+        <v>2352</v>
       </c>
       <c r="AK33" t="s">
-        <v>1891</v>
+        <v>2351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested ticket10 with comics grp
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24138" uniqueCount="3369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24163" uniqueCount="3372">
   <si>
     <t>Places</t>
   </si>
@@ -10141,6 +10141,15 @@
   </si>
   <si>
     <t>1090</t>
+  </si>
+  <si>
+    <t>Foden NEW (A)$ captain</t>
+  </si>
+  <si>
+    <t>Goode -</t>
+  </si>
+  <si>
+    <t>3,323</t>
   </si>
 </sst>
 </file>
@@ -27572,18 +27581,18 @@
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.69921875" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="12.34765625" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="24.9296875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="22.171875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="17.3515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.66796875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="11.20703125" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="14.859375" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="14.5078125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.66796875" collapsed="true"/>
     <col min="32" max="32" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="14.953125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.9921875" collapsed="true"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="11.55859375" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
@@ -27711,16 +27720,16 @@
         <v>1646</v>
       </c>
       <c r="C2" t="s">
-        <v>299</v>
+        <v>672</v>
       </c>
       <c r="D2" t="s">
-        <v>3163</v>
+        <v>3172</v>
       </c>
       <c r="E2" t="s">
-        <v>3177</v>
+        <v>3371</v>
       </c>
       <c r="G2" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R2" t="s">
         <v>1742</v>
@@ -27729,34 +27738,34 @@
         <v>1645</v>
       </c>
       <c r="T2" t="s">
-        <v>2924</v>
+        <v>2402</v>
       </c>
       <c r="U2" t="s">
-        <v>587</v>
+        <v>3242</v>
       </c>
       <c r="V2" t="s">
-        <v>1988</v>
+        <v>3241</v>
       </c>
       <c r="W2" t="s">
-        <v>3024</v>
+        <v>3250</v>
       </c>
       <c r="X2" t="s">
-        <v>3015</v>
+        <v>3249</v>
       </c>
       <c r="Y2" t="s">
-        <v>2537</v>
+        <v>3274</v>
       </c>
       <c r="Z2" t="s">
-        <v>2904</v>
+        <v>3369</v>
       </c>
       <c r="AA2" t="s">
-        <v>3021</v>
+        <v>3282</v>
       </c>
       <c r="AB2" t="s">
-        <v>2933</v>
+        <v>2089</v>
       </c>
       <c r="AC2" t="s">
-        <v>2771</v>
+        <v>3260</v>
       </c>
       <c r="AD2" t="s">
         <v>2925</v>
@@ -27765,22 +27774,22 @@
         <v>2931</v>
       </c>
       <c r="AF2" t="s">
-        <v>2089</v>
+        <v>2771</v>
       </c>
       <c r="AG2" t="s">
-        <v>3176</v>
+        <v>3266</v>
       </c>
       <c r="AH2" t="s">
-        <v>689</v>
+        <v>3370</v>
       </c>
       <c r="AI2" t="s">
-        <v>299</v>
+        <v>672</v>
       </c>
       <c r="AJ2" t="s">
-        <v>3163</v>
+        <v>3172</v>
       </c>
       <c r="AK2" t="s">
-        <v>3177</v>
+        <v>3371</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ticket 11 fixed log improvement
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15189" uniqueCount="2843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15593" uniqueCount="2886">
   <si>
     <t>Places</t>
   </si>
@@ -8563,6 +8563,135 @@
   </si>
   <si>
     <t>Dalot 1</t>
+  </si>
+  <si>
+    <t>1,442,096</t>
+  </si>
+  <si>
+    <t>1086</t>
+  </si>
+  <si>
+    <t>Thiago Silva 0</t>
+  </si>
+  <si>
+    <t>34,117</t>
+  </si>
+  <si>
+    <t>497,565</t>
+  </si>
+  <si>
+    <t>Mitchell 8</t>
+  </si>
+  <si>
+    <t>27,084</t>
+  </si>
+  <si>
+    <t>1281</t>
+  </si>
+  <si>
+    <t>Guéhi 6</t>
+  </si>
+  <si>
+    <t>466,025</t>
+  </si>
+  <si>
+    <t>1170</t>
+  </si>
+  <si>
+    <t>van Dijk 2</t>
+  </si>
+  <si>
+    <t>Hayden -</t>
+  </si>
+  <si>
+    <t>1,291,695</t>
+  </si>
+  <si>
+    <t>1096</t>
+  </si>
+  <si>
+    <t>2,263,359</t>
+  </si>
+  <si>
+    <t>Cucho 1</t>
+  </si>
+  <si>
+    <t>Wood 2</t>
+  </si>
+  <si>
+    <t>1,493,943</t>
+  </si>
+  <si>
+    <t>Zaha 0</t>
+  </si>
+  <si>
+    <t>Skipp 0</t>
+  </si>
+  <si>
+    <t>Jesus 4$ captain</t>
+  </si>
+  <si>
+    <t>5,502,915</t>
+  </si>
+  <si>
+    <t>863</t>
+  </si>
+  <si>
+    <t>400,267</t>
+  </si>
+  <si>
+    <t>Sancho 5</t>
+  </si>
+  <si>
+    <t>2,038,567</t>
+  </si>
+  <si>
+    <t>1051</t>
+  </si>
+  <si>
+    <t>Rice 0</t>
+  </si>
+  <si>
+    <t>S.Longstaff -</t>
+  </si>
+  <si>
+    <t>3,455,306</t>
+  </si>
+  <si>
+    <t>Gunn 2</t>
+  </si>
+  <si>
+    <t>2,210,709</t>
+  </si>
+  <si>
+    <t>Ward-Prowse 9</t>
+  </si>
+  <si>
+    <t>3,958,983</t>
+  </si>
+  <si>
+    <t>951</t>
+  </si>
+  <si>
+    <t>Digne -</t>
+  </si>
+  <si>
+    <t>Schmeichel 15</t>
+  </si>
+  <si>
+    <t>Holding -</t>
+  </si>
+  <si>
+    <t>Xhaka -</t>
+  </si>
+  <si>
+    <t>5,525,886</t>
+  </si>
+  <si>
+    <t>862</t>
+  </si>
+  <si>
+    <t>6,944,746</t>
   </si>
 </sst>
 </file>
@@ -9405,21 +9534,21 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="18.58984375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.46484375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.45703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="15.19140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.296875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="15.96484375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="15.296875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="19.203125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="13.36328125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.8828125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.41796875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.19140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.89453125" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
@@ -9546,13 +9675,13 @@
         <v>5695560</v>
       </c>
       <c r="C2" t="s">
-        <v>1452</v>
+        <v>829</v>
       </c>
       <c r="D2" t="s">
-        <v>2357</v>
+        <v>2844</v>
       </c>
       <c r="E2" t="s">
-        <v>2423</v>
+        <v>2843</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -9567,31 +9696,31 @@
         <v>2104</v>
       </c>
       <c r="U2" t="s">
-        <v>2265</v>
+        <v>554</v>
       </c>
       <c r="V2" t="s">
-        <v>734</v>
+        <v>2845</v>
       </c>
       <c r="W2" t="s">
-        <v>2270</v>
+        <v>424</v>
       </c>
       <c r="X2" t="s">
-        <v>2247</v>
+        <v>2671</v>
       </c>
       <c r="Y2" t="s">
-        <v>1947</v>
+        <v>2725</v>
       </c>
       <c r="Z2" t="s">
-        <v>2246</v>
+        <v>2707</v>
       </c>
       <c r="AA2" t="s">
-        <v>1951</v>
+        <v>2672</v>
       </c>
       <c r="AB2" t="s">
         <v>2115</v>
       </c>
       <c r="AC2" t="s">
-        <v>2011</v>
+        <v>2674</v>
       </c>
       <c r="AD2" t="s">
         <v>1958</v>
@@ -9600,22 +9729,22 @@
         <v>2080</v>
       </c>
       <c r="AF2" t="s">
-        <v>2272</v>
+        <v>2688</v>
       </c>
       <c r="AG2" t="s">
-        <v>751</v>
+        <v>1363</v>
       </c>
       <c r="AH2" t="s">
         <v>881</v>
       </c>
       <c r="AI2" t="s">
-        <v>1452</v>
+        <v>829</v>
       </c>
       <c r="AJ2" t="s">
-        <v>2357</v>
+        <v>2844</v>
       </c>
       <c r="AK2" t="s">
-        <v>2423</v>
+        <v>2843</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -9626,16 +9755,16 @@
         <v>1153704</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>1921</v>
       </c>
       <c r="D3" t="s">
-        <v>2426</v>
+        <v>2503</v>
       </c>
       <c r="E3" t="s">
-        <v>2425</v>
+        <v>2846</v>
       </c>
       <c r="G3" t="s">
-        <v>653</v>
+        <v>452</v>
       </c>
       <c r="R3" t="s">
         <v>885</v>
@@ -9644,58 +9773,58 @@
         <v>884</v>
       </c>
       <c r="T3" t="s">
-        <v>686</v>
+        <v>2559</v>
       </c>
       <c r="U3" t="s">
-        <v>1940</v>
+        <v>476</v>
       </c>
       <c r="V3" t="s">
-        <v>2251</v>
+        <v>2767</v>
       </c>
       <c r="W3" t="s">
-        <v>2258</v>
+        <v>360</v>
       </c>
       <c r="X3" t="s">
-        <v>2265</v>
+        <v>554</v>
       </c>
       <c r="Y3" t="s">
-        <v>2259</v>
+        <v>2058</v>
       </c>
       <c r="Z3" t="s">
-        <v>2280</v>
+        <v>2776</v>
       </c>
       <c r="AA3" t="s">
-        <v>2303</v>
+        <v>2768</v>
       </c>
       <c r="AB3" t="s">
-        <v>2306</v>
+        <v>756</v>
       </c>
       <c r="AC3" t="s">
-        <v>2287</v>
+        <v>2671</v>
       </c>
       <c r="AD3" t="s">
-        <v>683</v>
+        <v>1958</v>
       </c>
       <c r="AE3" t="s">
-        <v>1411</v>
+        <v>1929</v>
       </c>
       <c r="AF3" t="s">
-        <v>2298</v>
+        <v>2059</v>
       </c>
       <c r="AG3" t="s">
-        <v>2260</v>
+        <v>1932</v>
       </c>
       <c r="AH3" t="s">
-        <v>2424</v>
+        <v>2077</v>
       </c>
       <c r="AI3" t="s">
-        <v>284</v>
+        <v>1921</v>
       </c>
       <c r="AJ3" t="s">
-        <v>2426</v>
+        <v>2503</v>
       </c>
       <c r="AK3" t="s">
-        <v>2425</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -9706,16 +9835,16 @@
         <v>440807</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>2355</v>
+        <v>2051</v>
       </c>
       <c r="E4" t="s">
-        <v>2354</v>
+        <v>2847</v>
       </c>
       <c r="G4" t="s">
-        <v>452</v>
+        <v>706</v>
       </c>
       <c r="R4" t="s">
         <v>418</v>
@@ -9724,58 +9853,58 @@
         <v>289</v>
       </c>
       <c r="T4" t="s">
-        <v>686</v>
+        <v>2799</v>
       </c>
       <c r="U4" t="s">
-        <v>2270</v>
+        <v>424</v>
       </c>
       <c r="V4" t="s">
-        <v>688</v>
+        <v>2789</v>
       </c>
       <c r="W4" t="s">
-        <v>1913</v>
+        <v>2767</v>
       </c>
       <c r="X4" t="s">
-        <v>1940</v>
+        <v>554</v>
       </c>
       <c r="Y4" t="s">
-        <v>1949</v>
+        <v>2575</v>
       </c>
       <c r="Z4" t="s">
-        <v>2013</v>
+        <v>2672</v>
       </c>
       <c r="AA4" t="s">
-        <v>2287</v>
+        <v>2768</v>
       </c>
       <c r="AB4" t="s">
-        <v>2092</v>
+        <v>2775</v>
       </c>
       <c r="AC4" t="s">
-        <v>2255</v>
+        <v>2674</v>
       </c>
       <c r="AD4" t="s">
-        <v>683</v>
+        <v>2839</v>
       </c>
       <c r="AE4" t="s">
-        <v>1931</v>
+        <v>2559</v>
       </c>
       <c r="AF4" t="s">
-        <v>691</v>
+        <v>509</v>
       </c>
       <c r="AG4" t="s">
-        <v>2011</v>
+        <v>2573</v>
       </c>
       <c r="AH4" t="s">
         <v>2288</v>
       </c>
       <c r="AI4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2355</v>
+        <v>2051</v>
       </c>
       <c r="AK4" t="s">
-        <v>2354</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -9786,16 +9915,16 @@
         <v>4642646</v>
       </c>
       <c r="C5" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D5" t="s">
-        <v>2429</v>
+        <v>2850</v>
       </c>
       <c r="E5" t="s">
-        <v>2428</v>
+        <v>2849</v>
       </c>
       <c r="G5" t="s">
-        <v>906</v>
+        <v>706</v>
       </c>
       <c r="R5" t="s">
         <v>887</v>
@@ -9804,58 +9933,58 @@
         <v>886</v>
       </c>
       <c r="T5" t="s">
-        <v>2339</v>
+        <v>2841</v>
       </c>
       <c r="U5" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="V5" t="s">
-        <v>1913</v>
+        <v>360</v>
       </c>
       <c r="W5" t="s">
-        <v>2251</v>
+        <v>476</v>
       </c>
       <c r="X5" t="s">
-        <v>2258</v>
+        <v>2848</v>
       </c>
       <c r="Y5" t="s">
-        <v>2287</v>
+        <v>2672</v>
       </c>
       <c r="Z5" t="s">
-        <v>2255</v>
+        <v>2775</v>
       </c>
       <c r="AA5" t="s">
-        <v>2013</v>
+        <v>756</v>
       </c>
       <c r="AB5" t="s">
-        <v>1961</v>
+        <v>1367</v>
       </c>
       <c r="AC5" t="s">
-        <v>2427</v>
+        <v>2839</v>
       </c>
       <c r="AD5" t="s">
-        <v>683</v>
+        <v>2627</v>
       </c>
       <c r="AE5" t="s">
-        <v>2026</v>
+        <v>1154</v>
       </c>
       <c r="AF5" t="s">
-        <v>2271</v>
+        <v>2573</v>
       </c>
       <c r="AG5" t="s">
-        <v>2245</v>
+        <v>2590</v>
       </c>
       <c r="AH5" t="s">
-        <v>2023</v>
+        <v>2066</v>
       </c>
       <c r="AI5" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="AJ5" t="s">
-        <v>2429</v>
+        <v>2850</v>
       </c>
       <c r="AK5" t="s">
-        <v>2428</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -9866,16 +9995,16 @@
         <v>1364835</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="D6" t="s">
-        <v>1991</v>
+        <v>2853</v>
       </c>
       <c r="E6" t="s">
-        <v>2431</v>
+        <v>2852</v>
       </c>
       <c r="G6" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R6" t="s">
         <v>889</v>
@@ -9884,58 +10013,58 @@
         <v>888</v>
       </c>
       <c r="T6" t="s">
-        <v>726</v>
+        <v>2785</v>
       </c>
       <c r="U6" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="V6" t="s">
-        <v>2251</v>
+        <v>360</v>
       </c>
       <c r="W6" t="s">
-        <v>1208</v>
+        <v>2795</v>
       </c>
       <c r="X6" t="s">
-        <v>2280</v>
+        <v>476</v>
       </c>
       <c r="Y6" t="s">
-        <v>691</v>
+        <v>2851</v>
       </c>
       <c r="Z6" t="s">
-        <v>2259</v>
+        <v>2575</v>
       </c>
       <c r="AA6" t="s">
-        <v>2013</v>
+        <v>2673</v>
       </c>
       <c r="AB6" t="s">
-        <v>2287</v>
+        <v>2742</v>
       </c>
       <c r="AC6" t="s">
-        <v>1964</v>
+        <v>2674</v>
       </c>
       <c r="AD6" t="s">
-        <v>2250</v>
+        <v>2769</v>
       </c>
       <c r="AE6" t="s">
-        <v>2014</v>
+        <v>1929</v>
       </c>
       <c r="AF6" t="s">
-        <v>2430</v>
+        <v>2059</v>
       </c>
       <c r="AG6" t="s">
-        <v>2245</v>
+        <v>2611</v>
       </c>
       <c r="AH6" t="s">
-        <v>2011</v>
+        <v>2573</v>
       </c>
       <c r="AI6" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="AJ6" t="s">
-        <v>1991</v>
+        <v>2853</v>
       </c>
       <c r="AK6" t="s">
-        <v>2431</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -9946,16 +10075,16 @@
         <v>5306515</v>
       </c>
       <c r="C7" t="s">
-        <v>1512</v>
+        <v>2636</v>
       </c>
       <c r="D7" t="s">
-        <v>2434</v>
+        <v>2857</v>
       </c>
       <c r="E7" t="s">
-        <v>2433</v>
+        <v>2856</v>
       </c>
       <c r="G7" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R7" t="s">
         <v>897</v>
@@ -9964,58 +10093,58 @@
         <v>896</v>
       </c>
       <c r="T7" t="s">
-        <v>2410</v>
+        <v>2104</v>
       </c>
       <c r="U7" t="s">
-        <v>2270</v>
+        <v>2854</v>
       </c>
       <c r="V7" t="s">
-        <v>1940</v>
+        <v>424</v>
       </c>
       <c r="W7" t="s">
-        <v>2265</v>
+        <v>2767</v>
       </c>
       <c r="X7" t="s">
-        <v>1951</v>
+        <v>1916</v>
       </c>
       <c r="Y7" t="s">
-        <v>2246</v>
+        <v>2671</v>
       </c>
       <c r="Z7" t="s">
-        <v>2013</v>
+        <v>2707</v>
       </c>
       <c r="AA7" t="s">
-        <v>691</v>
+        <v>2855</v>
       </c>
       <c r="AB7" t="s">
-        <v>2314</v>
+        <v>2575</v>
       </c>
       <c r="AC7" t="s">
-        <v>892</v>
+        <v>1445</v>
       </c>
       <c r="AD7" t="s">
-        <v>1958</v>
+        <v>2701</v>
       </c>
       <c r="AE7" t="s">
-        <v>2432</v>
+        <v>2131</v>
       </c>
       <c r="AF7" t="s">
-        <v>2427</v>
+        <v>2445</v>
       </c>
       <c r="AG7" t="s">
-        <v>1941</v>
+        <v>2573</v>
       </c>
       <c r="AH7" t="s">
-        <v>1191</v>
+        <v>2059</v>
       </c>
       <c r="AI7" t="s">
-        <v>1512</v>
+        <v>2636</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2434</v>
+        <v>2857</v>
       </c>
       <c r="AK7" t="s">
-        <v>2433</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -10026,13 +10155,13 @@
         <v>2249991</v>
       </c>
       <c r="C8" t="s">
-        <v>1921</v>
+        <v>912</v>
       </c>
       <c r="D8" t="s">
-        <v>2436</v>
+        <v>2283</v>
       </c>
       <c r="E8" t="s">
-        <v>2435</v>
+        <v>2858</v>
       </c>
       <c r="G8" t="s">
         <v>653</v>
@@ -10044,58 +10173,58 @@
         <v>898</v>
       </c>
       <c r="T8" t="s">
-        <v>686</v>
+        <v>2770</v>
       </c>
       <c r="U8" t="s">
-        <v>2270</v>
+        <v>509</v>
       </c>
       <c r="V8" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="W8" t="s">
-        <v>1941</v>
+        <v>424</v>
       </c>
       <c r="X8" t="s">
-        <v>1949</v>
+        <v>476</v>
       </c>
       <c r="Y8" t="s">
-        <v>2271</v>
+        <v>756</v>
       </c>
       <c r="Z8" t="s">
-        <v>1947</v>
+        <v>2671</v>
       </c>
       <c r="AA8" t="s">
-        <v>2247</v>
+        <v>2725</v>
       </c>
       <c r="AB8" t="s">
-        <v>700</v>
+        <v>2589</v>
       </c>
       <c r="AC8" t="s">
-        <v>683</v>
+        <v>2674</v>
       </c>
       <c r="AD8" t="s">
-        <v>2011</v>
+        <v>2840</v>
       </c>
       <c r="AE8" t="s">
-        <v>2249</v>
+        <v>2559</v>
       </c>
       <c r="AF8" t="s">
-        <v>2245</v>
+        <v>2071</v>
       </c>
       <c r="AG8" t="s">
-        <v>2040</v>
+        <v>1233</v>
       </c>
       <c r="AH8" t="s">
-        <v>2071</v>
+        <v>1916</v>
       </c>
       <c r="AI8" t="s">
-        <v>1921</v>
+        <v>912</v>
       </c>
       <c r="AJ8" t="s">
-        <v>2436</v>
+        <v>2283</v>
       </c>
       <c r="AK8" t="s">
-        <v>2435</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -10106,13 +10235,13 @@
         <v>2056865</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>1919</v>
       </c>
       <c r="D9" t="s">
-        <v>2440</v>
+        <v>2772</v>
       </c>
       <c r="E9" t="s">
-        <v>2439</v>
+        <v>2861</v>
       </c>
       <c r="G9" t="s">
         <v>653</v>
@@ -10124,58 +10253,58 @@
         <v>901</v>
       </c>
       <c r="T9" t="s">
-        <v>2339</v>
+        <v>2785</v>
       </c>
       <c r="U9" t="s">
-        <v>2251</v>
+        <v>476</v>
       </c>
       <c r="V9" t="s">
-        <v>1208</v>
+        <v>424</v>
       </c>
       <c r="W9" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="X9" t="s">
-        <v>2303</v>
+        <v>2768</v>
       </c>
       <c r="Y9" t="s">
-        <v>2280</v>
+        <v>2671</v>
       </c>
       <c r="Z9" t="s">
-        <v>2259</v>
+        <v>2775</v>
       </c>
       <c r="AA9" t="s">
-        <v>2287</v>
+        <v>756</v>
       </c>
       <c r="AB9" t="s">
-        <v>683</v>
+        <v>2859</v>
       </c>
       <c r="AC9" t="s">
-        <v>2115</v>
+        <v>2860</v>
       </c>
       <c r="AD9" t="s">
-        <v>2250</v>
+        <v>1367</v>
       </c>
       <c r="AE9" t="s">
-        <v>2014</v>
+        <v>1929</v>
       </c>
       <c r="AF9" t="s">
-        <v>2437</v>
+        <v>2795</v>
       </c>
       <c r="AG9" t="s">
-        <v>2197</v>
+        <v>2079</v>
       </c>
       <c r="AH9" t="s">
-        <v>2438</v>
+        <v>2611</v>
       </c>
       <c r="AI9" t="s">
-        <v>290</v>
+        <v>1919</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2440</v>
+        <v>2772</v>
       </c>
       <c r="AK9" t="s">
-        <v>2439</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -10186,13 +10315,13 @@
         <v>5142355</v>
       </c>
       <c r="C10" t="s">
-        <v>1402</v>
+        <v>1324</v>
       </c>
       <c r="D10" t="s">
-        <v>2447</v>
+        <v>2866</v>
       </c>
       <c r="E10" t="s">
-        <v>2446</v>
+        <v>2865</v>
       </c>
       <c r="G10" t="s">
         <v>653</v>
@@ -10204,58 +10333,58 @@
         <v>913</v>
       </c>
       <c r="T10" t="s">
-        <v>2291</v>
+        <v>1943</v>
       </c>
       <c r="U10" t="s">
-        <v>2270</v>
+        <v>2445</v>
       </c>
       <c r="V10" t="s">
-        <v>1949</v>
+        <v>509</v>
       </c>
       <c r="W10" t="s">
-        <v>806</v>
+        <v>424</v>
       </c>
       <c r="X10" t="s">
         <v>2071</v>
       </c>
       <c r="Y10" t="s">
-        <v>2441</v>
+        <v>2678</v>
       </c>
       <c r="Z10" t="s">
-        <v>2253</v>
+        <v>2862</v>
       </c>
       <c r="AA10" t="s">
-        <v>2442</v>
+        <v>2863</v>
       </c>
       <c r="AB10" t="s">
-        <v>683</v>
+        <v>1372</v>
       </c>
       <c r="AC10" t="s">
-        <v>2443</v>
+        <v>2840</v>
       </c>
       <c r="AD10" t="s">
-        <v>2260</v>
+        <v>2864</v>
       </c>
       <c r="AE10" t="s">
-        <v>2012</v>
+        <v>1384</v>
       </c>
       <c r="AF10" t="s">
-        <v>2444</v>
+        <v>873</v>
       </c>
       <c r="AG10" t="s">
         <v>2150</v>
       </c>
       <c r="AH10" t="s">
-        <v>2445</v>
+        <v>2646</v>
       </c>
       <c r="AI10" t="s">
-        <v>1402</v>
+        <v>1324</v>
       </c>
       <c r="AJ10" t="s">
-        <v>2447</v>
+        <v>2866</v>
       </c>
       <c r="AK10" t="s">
-        <v>2446</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -10266,16 +10395,16 @@
         <v>1628438</v>
       </c>
       <c r="C11" t="s">
-        <v>821</v>
+        <v>272</v>
       </c>
       <c r="D11" t="s">
-        <v>2449</v>
+        <v>2680</v>
       </c>
       <c r="E11" t="s">
-        <v>2448</v>
+        <v>2867</v>
       </c>
       <c r="G11" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R11" t="s">
         <v>916</v>
@@ -10284,58 +10413,58 @@
         <v>915</v>
       </c>
       <c r="T11" t="s">
-        <v>2249</v>
+        <v>2770</v>
       </c>
       <c r="U11" t="s">
-        <v>2270</v>
+        <v>424</v>
       </c>
       <c r="V11" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="W11" t="s">
-        <v>688</v>
+        <v>2789</v>
       </c>
       <c r="X11" t="s">
-        <v>1941</v>
+        <v>2707</v>
       </c>
       <c r="Y11" t="s">
-        <v>1191</v>
+        <v>2768</v>
       </c>
       <c r="Z11" t="s">
-        <v>2246</v>
+        <v>2671</v>
       </c>
       <c r="AA11" t="s">
-        <v>2092</v>
+        <v>756</v>
       </c>
       <c r="AB11" t="s">
-        <v>2013</v>
+        <v>2840</v>
       </c>
       <c r="AC11" t="s">
-        <v>892</v>
+        <v>2674</v>
       </c>
       <c r="AD11" t="s">
-        <v>2011</v>
+        <v>1958</v>
       </c>
       <c r="AE11" t="s">
         <v>804</v>
       </c>
       <c r="AF11" t="s">
-        <v>2253</v>
+        <v>1206</v>
       </c>
       <c r="AG11" t="s">
-        <v>2271</v>
+        <v>1916</v>
       </c>
       <c r="AH11" t="s">
-        <v>2288</v>
+        <v>1191</v>
       </c>
       <c r="AI11" t="s">
-        <v>821</v>
+        <v>272</v>
       </c>
       <c r="AJ11" t="s">
-        <v>2449</v>
+        <v>2680</v>
       </c>
       <c r="AK11" t="s">
-        <v>2448</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -10349,13 +10478,13 @@
         <v>282</v>
       </c>
       <c r="D12" t="s">
-        <v>2453</v>
+        <v>2870</v>
       </c>
       <c r="E12" t="s">
-        <v>2452</v>
+        <v>2869</v>
       </c>
       <c r="G12" t="s">
-        <v>653</v>
+        <v>906</v>
       </c>
       <c r="R12" t="s">
         <v>919</v>
@@ -10364,58 +10493,58 @@
         <v>918</v>
       </c>
       <c r="T12" t="s">
-        <v>2410</v>
+        <v>436</v>
       </c>
       <c r="U12" t="s">
-        <v>1940</v>
+        <v>476</v>
       </c>
       <c r="V12" t="s">
-        <v>1913</v>
+        <v>2134</v>
       </c>
       <c r="W12" t="s">
-        <v>2270</v>
+        <v>424</v>
       </c>
       <c r="X12" t="s">
-        <v>2251</v>
+        <v>360</v>
       </c>
       <c r="Y12" t="s">
-        <v>1951</v>
+        <v>2671</v>
       </c>
       <c r="Z12" t="s">
-        <v>1947</v>
+        <v>2725</v>
       </c>
       <c r="AA12" t="s">
-        <v>2450</v>
+        <v>2868</v>
       </c>
       <c r="AB12" t="s">
-        <v>2246</v>
+        <v>2707</v>
       </c>
       <c r="AC12" t="s">
-        <v>700</v>
+        <v>1958</v>
       </c>
       <c r="AD12" t="s">
-        <v>892</v>
+        <v>2674</v>
       </c>
       <c r="AE12" t="s">
-        <v>2014</v>
+        <v>1929</v>
       </c>
       <c r="AF12" t="s">
-        <v>2013</v>
+        <v>2461</v>
       </c>
       <c r="AG12" t="s">
-        <v>2451</v>
+        <v>2288</v>
       </c>
       <c r="AH12" t="s">
-        <v>1208</v>
+        <v>2795</v>
       </c>
       <c r="AI12" t="s">
         <v>282</v>
       </c>
       <c r="AJ12" t="s">
-        <v>2453</v>
+        <v>2870</v>
       </c>
       <c r="AK12" t="s">
-        <v>2452</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -10426,13 +10555,13 @@
         <v>5648774</v>
       </c>
       <c r="C13" t="s">
-        <v>2458</v>
+        <v>821</v>
       </c>
       <c r="D13" t="s">
-        <v>2460</v>
+        <v>1827</v>
       </c>
       <c r="E13" t="s">
-        <v>2459</v>
+        <v>2873</v>
       </c>
       <c r="G13" t="s">
         <v>653</v>
@@ -10444,58 +10573,58 @@
         <v>920</v>
       </c>
       <c r="T13" t="s">
-        <v>2410</v>
+        <v>2131</v>
       </c>
       <c r="U13" t="s">
-        <v>2251</v>
+        <v>2646</v>
       </c>
       <c r="V13" t="s">
-        <v>1913</v>
+        <v>360</v>
       </c>
       <c r="W13" t="s">
-        <v>806</v>
+        <v>2571</v>
       </c>
       <c r="X13" t="s">
-        <v>2454</v>
+        <v>2456</v>
       </c>
       <c r="Y13" t="s">
-        <v>2247</v>
+        <v>2671</v>
       </c>
       <c r="Z13" t="s">
-        <v>2271</v>
+        <v>756</v>
       </c>
       <c r="AA13" t="s">
-        <v>2246</v>
+        <v>2707</v>
       </c>
       <c r="AB13" t="s">
-        <v>2455</v>
+        <v>2871</v>
       </c>
       <c r="AC13" t="s">
-        <v>939</v>
+        <v>2840</v>
       </c>
       <c r="AD13" t="s">
-        <v>2011</v>
+        <v>2674</v>
       </c>
       <c r="AE13" t="s">
-        <v>399</v>
+        <v>2074</v>
       </c>
       <c r="AF13" t="s">
-        <v>2245</v>
+        <v>476</v>
       </c>
       <c r="AG13" t="s">
-        <v>2456</v>
+        <v>2872</v>
       </c>
       <c r="AH13" t="s">
         <v>2457</v>
       </c>
       <c r="AI13" t="s">
-        <v>2458</v>
+        <v>821</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2460</v>
+        <v>1827</v>
       </c>
       <c r="AK13" t="s">
-        <v>2459</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -10506,13 +10635,13 @@
         <v>3452385</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="D14" t="s">
-        <v>2463</v>
+        <v>2293</v>
       </c>
       <c r="E14" t="s">
-        <v>2462</v>
+        <v>2875</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -10524,43 +10653,43 @@
         <v>923</v>
       </c>
       <c r="T14" t="s">
-        <v>1931</v>
+        <v>2799</v>
       </c>
       <c r="U14" t="s">
-        <v>2251</v>
+        <v>2767</v>
       </c>
       <c r="V14" t="s">
-        <v>1940</v>
+        <v>476</v>
       </c>
       <c r="W14" t="s">
-        <v>2265</v>
+        <v>360</v>
       </c>
       <c r="X14" t="s">
-        <v>691</v>
+        <v>554</v>
       </c>
       <c r="Y14" t="s">
-        <v>1952</v>
+        <v>2742</v>
       </c>
       <c r="Z14" t="s">
-        <v>2253</v>
+        <v>2678</v>
       </c>
       <c r="AA14" t="s">
-        <v>2287</v>
+        <v>2575</v>
       </c>
       <c r="AB14" t="s">
-        <v>2250</v>
+        <v>1206</v>
       </c>
       <c r="AC14" t="s">
         <v>1958</v>
       </c>
       <c r="AD14" t="s">
-        <v>2011</v>
+        <v>2674</v>
       </c>
       <c r="AE14" t="s">
-        <v>922</v>
+        <v>2874</v>
       </c>
       <c r="AF14" t="s">
-        <v>2245</v>
+        <v>2769</v>
       </c>
       <c r="AG14" t="s">
         <v>2445</v>
@@ -10569,13 +10698,13 @@
         <v>2461</v>
       </c>
       <c r="AI14" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2463</v>
+        <v>2293</v>
       </c>
       <c r="AK14" t="s">
-        <v>2462</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -10586,16 +10715,16 @@
         <v>2297330</v>
       </c>
       <c r="C15" t="s">
-        <v>1229</v>
+        <v>1452</v>
       </c>
       <c r="D15" t="s">
-        <v>2467</v>
+        <v>2878</v>
       </c>
       <c r="E15" t="s">
-        <v>2466</v>
+        <v>2877</v>
       </c>
       <c r="G15" t="s">
-        <v>672</v>
+        <v>706</v>
       </c>
       <c r="R15" t="s">
         <v>926</v>
@@ -10604,58 +10733,58 @@
         <v>925</v>
       </c>
       <c r="T15" t="s">
-        <v>2339</v>
+        <v>2841</v>
       </c>
       <c r="U15" t="s">
-        <v>2298</v>
+        <v>2805</v>
       </c>
       <c r="V15" t="s">
-        <v>1913</v>
+        <v>2465</v>
       </c>
       <c r="W15" t="s">
-        <v>2265</v>
+        <v>554</v>
       </c>
       <c r="X15" t="s">
-        <v>1951</v>
+        <v>2672</v>
       </c>
       <c r="Y15" t="s">
-        <v>2255</v>
+        <v>2775</v>
       </c>
       <c r="Z15" t="s">
-        <v>2464</v>
+        <v>2876</v>
       </c>
       <c r="AA15" t="s">
-        <v>2013</v>
+        <v>2725</v>
       </c>
       <c r="AB15" t="s">
         <v>2123</v>
       </c>
       <c r="AC15" t="s">
-        <v>2260</v>
+        <v>1372</v>
       </c>
       <c r="AD15" t="s">
-        <v>2277</v>
+        <v>2840</v>
       </c>
       <c r="AE15" t="s">
         <v>1834</v>
       </c>
       <c r="AF15" t="s">
-        <v>1947</v>
+        <v>2573</v>
       </c>
       <c r="AG15" t="s">
-        <v>2465</v>
+        <v>2571</v>
       </c>
       <c r="AH15" t="s">
-        <v>2347</v>
+        <v>2726</v>
       </c>
       <c r="AI15" t="s">
-        <v>1229</v>
+        <v>1452</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2467</v>
+        <v>2878</v>
       </c>
       <c r="AK15" t="s">
-        <v>2466</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -10666,13 +10795,13 @@
         <v>5361878</v>
       </c>
       <c r="C16" t="s">
-        <v>771</v>
+        <v>1402</v>
       </c>
       <c r="D16" t="s">
-        <v>1463</v>
+        <v>2884</v>
       </c>
       <c r="E16" t="s">
-        <v>2470</v>
+        <v>2883</v>
       </c>
       <c r="G16" t="s">
         <v>452</v>
@@ -10684,58 +10813,58 @@
         <v>927</v>
       </c>
       <c r="T16" t="s">
-        <v>2402</v>
+        <v>1943</v>
       </c>
       <c r="U16" t="s">
-        <v>1942</v>
+        <v>1932</v>
       </c>
       <c r="V16" t="s">
-        <v>1940</v>
+        <v>2767</v>
       </c>
       <c r="W16" t="s">
-        <v>2468</v>
+        <v>2879</v>
       </c>
       <c r="X16" t="s">
-        <v>2251</v>
+        <v>360</v>
       </c>
       <c r="Y16" t="s">
-        <v>2469</v>
+        <v>1944</v>
       </c>
       <c r="Z16" t="s">
-        <v>2007</v>
+        <v>2671</v>
       </c>
       <c r="AA16" t="s">
-        <v>691</v>
+        <v>2768</v>
       </c>
       <c r="AB16" t="s">
-        <v>2284</v>
+        <v>2575</v>
       </c>
       <c r="AC16" t="s">
-        <v>2277</v>
+        <v>2638</v>
       </c>
       <c r="AD16" t="s">
-        <v>2260</v>
+        <v>1372</v>
       </c>
       <c r="AE16" t="s">
-        <v>2291</v>
+        <v>2880</v>
       </c>
       <c r="AF16" t="s">
-        <v>1953</v>
+        <v>2881</v>
       </c>
       <c r="AG16" t="s">
-        <v>2316</v>
+        <v>2635</v>
       </c>
       <c r="AH16" t="s">
-        <v>2253</v>
+        <v>2882</v>
       </c>
       <c r="AI16" t="s">
-        <v>771</v>
+        <v>1402</v>
       </c>
       <c r="AJ16" t="s">
-        <v>1463</v>
+        <v>2884</v>
       </c>
       <c r="AK16" t="s">
-        <v>2470</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -10746,13 +10875,13 @@
         <v>5344757</v>
       </c>
       <c r="C17" t="s">
-        <v>1832</v>
+        <v>1978</v>
       </c>
       <c r="D17" t="s">
-        <v>2472</v>
+        <v>1514</v>
       </c>
       <c r="E17" t="s">
-        <v>2471</v>
+        <v>2885</v>
       </c>
       <c r="G17" t="s">
         <v>653</v>
@@ -10764,58 +10893,58 @@
         <v>929</v>
       </c>
       <c r="T17" t="s">
-        <v>2339</v>
+        <v>2841</v>
       </c>
       <c r="U17" t="s">
-        <v>2261</v>
+        <v>2060</v>
       </c>
       <c r="V17" t="s">
-        <v>1949</v>
+        <v>509</v>
       </c>
       <c r="W17" t="s">
-        <v>2265</v>
+        <v>554</v>
       </c>
       <c r="X17" t="s">
-        <v>2021</v>
+        <v>2603</v>
       </c>
       <c r="Y17" t="s">
-        <v>2276</v>
+        <v>2775</v>
       </c>
       <c r="Z17" t="s">
-        <v>2255</v>
+        <v>2768</v>
       </c>
       <c r="AA17" t="s">
-        <v>2092</v>
+        <v>2575</v>
       </c>
       <c r="AB17" t="s">
-        <v>691</v>
+        <v>2671</v>
       </c>
       <c r="AC17" t="s">
-        <v>939</v>
+        <v>2840</v>
       </c>
       <c r="AD17" t="s">
-        <v>2250</v>
+        <v>2674</v>
       </c>
       <c r="AE17" t="s">
-        <v>2014</v>
+        <v>1929</v>
       </c>
       <c r="AF17" t="s">
         <v>2445</v>
       </c>
       <c r="AG17" t="s">
-        <v>2247</v>
+        <v>2612</v>
       </c>
       <c r="AH17" t="s">
-        <v>2011</v>
+        <v>2769</v>
       </c>
       <c r="AI17" t="s">
-        <v>1832</v>
+        <v>1978</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2472</v>
+        <v>1514</v>
       </c>
       <c r="AK17" t="s">
-        <v>2471</v>
+        <v>2885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PoI FPL webScrapping Mavenised
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9089" uniqueCount="2271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9289" uniqueCount="2284">
   <si>
     <t>Places</t>
   </si>
@@ -6847,12 +6847,52 @@
   </si>
   <si>
     <t>118,870</t>
+  </si>
+  <si>
+    <t>Bowen 42$ captain</t>
+  </si>
+  <si>
+    <t>Calvert-Lewin 0</t>
+  </si>
+  <si>
+    <t>Antonio 9</t>
+  </si>
+  <si>
+    <t>1463</t>
+  </si>
+  <si>
+    <t>Coufal 12</t>
+  </si>
+  <si>
+    <t>Livramento 0</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>1515</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>9,831</t>
+  </si>
+  <si>
+    <t>1375</t>
+  </si>
+  <si>
+    <t>1,595</t>
+  </si>
+  <si>
+    <t>1409</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7333,19 +7373,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="3.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="21" width="4.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="5.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="7" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
+    <col min="4" max="7" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="8" max="12" bestFit="true" customWidth="true" style="3" width="3.28515625" collapsed="true"/>
+    <col min="13" max="21" bestFit="true" customWidth="true" style="3" width="4.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="5.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" style="3" width="7.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="6.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -7680,28 +7720,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="24" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="34" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="21" max="24" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="33" max="34" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -9114,28 +9154,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="25" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="23" max="25" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -9415,18 +9455,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="30" max="34" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="20" max="28" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="30" max="34" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10024,28 +10064,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="27" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="30" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="22" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="27" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="28" max="30" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -12737,27 +12777,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="28" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="22" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="26" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -16589,32 +16629,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -16906,26 +16946,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="24" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="21" max="24" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -19277,27 +19317,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="34" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="21" max="22" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="33" max="34" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -20423,23 +20463,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="24" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="28" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="34" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="21" max="24" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="25" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="33" max="34" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -24271,29 +24311,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="21" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -25145,9 +25185,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25515,27 +25555,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="30" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="21" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="26" max="27" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="28" max="30" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -29667,26 +29707,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="28" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.25390625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.45703125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="9.91796875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.32421875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="9.9140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="7.4140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -29810,13 +29855,13 @@
         <v>1049</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>1219</v>
       </c>
       <c r="D2" t="s">
-        <v>2130</v>
+        <v>2274</v>
       </c>
       <c r="E2" t="s">
-        <v>1934</v>
+        <v>912</v>
       </c>
       <c r="G2" t="s">
         <v>452</v>
@@ -29840,25 +29885,25 @@
         <v>1964</v>
       </c>
       <c r="X2" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Y2" t="s">
         <v>1936</v>
       </c>
       <c r="Z2" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="AA2" t="s">
         <v>438</v>
       </c>
       <c r="AB2" t="s">
-        <v>2052</v>
+        <v>2272</v>
       </c>
       <c r="AC2" t="s">
         <v>2076</v>
       </c>
       <c r="AD2" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AE2" t="s">
         <v>1963</v>
@@ -29873,13 +29918,13 @@
         <v>2037</v>
       </c>
       <c r="AI2" t="s">
-        <v>272</v>
+        <v>1219</v>
       </c>
       <c r="AJ2" t="s">
-        <v>2130</v>
+        <v>2274</v>
       </c>
       <c r="AK2" t="s">
-        <v>1934</v>
+        <v>912</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -29890,10 +29935,10 @@
         <v>1051</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>2277</v>
       </c>
       <c r="D3" t="s">
-        <v>2131</v>
+        <v>2278</v>
       </c>
       <c r="E3" t="s">
         <v>706</v>
@@ -29914,7 +29959,7 @@
         <v>1997</v>
       </c>
       <c r="V3" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="W3" t="s">
         <v>1964</v>
@@ -29923,7 +29968,7 @@
         <v>2062</v>
       </c>
       <c r="Y3" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z3" t="s">
         <v>438</v>
@@ -29938,7 +29983,7 @@
         <v>1223</v>
       </c>
       <c r="AD3" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AE3" t="s">
         <v>1963</v>
@@ -29947,16 +29992,16 @@
         <v>2000</v>
       </c>
       <c r="AG3" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AH3" t="s">
         <v>1988</v>
       </c>
       <c r="AI3" t="s">
-        <v>272</v>
+        <v>2277</v>
       </c>
       <c r="AJ3" t="s">
-        <v>2131</v>
+        <v>2278</v>
       </c>
       <c r="AK3" t="s">
         <v>706</v>
@@ -29970,13 +30015,13 @@
         <v>949</v>
       </c>
       <c r="C4" t="s">
-        <v>1832</v>
+        <v>2279</v>
       </c>
       <c r="D4" t="s">
-        <v>2200</v>
+        <v>2281</v>
       </c>
       <c r="E4" t="s">
-        <v>2199</v>
+        <v>2280</v>
       </c>
       <c r="G4" t="s">
         <v>906</v>
@@ -30000,7 +30045,7 @@
         <v>1997</v>
       </c>
       <c r="X4" t="s">
-        <v>2049</v>
+        <v>538</v>
       </c>
       <c r="Y4" t="s">
         <v>2069</v>
@@ -30009,16 +30054,16 @@
         <v>2066</v>
       </c>
       <c r="AA4" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="AB4" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="AC4" t="s">
         <v>2076</v>
       </c>
       <c r="AD4" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AE4" t="s">
         <v>1963</v>
@@ -30033,13 +30078,13 @@
         <v>1943</v>
       </c>
       <c r="AI4" t="s">
-        <v>1832</v>
+        <v>2279</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2200</v>
+        <v>2281</v>
       </c>
       <c r="AK4" t="s">
-        <v>2199</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -30050,13 +30095,13 @@
         <v>1053</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>2277</v>
       </c>
       <c r="D5" t="s">
-        <v>1962</v>
+        <v>2283</v>
       </c>
       <c r="E5" t="s">
-        <v>2201</v>
+        <v>2282</v>
       </c>
       <c r="G5" t="s">
         <v>452</v>
@@ -30080,7 +30125,7 @@
         <v>1964</v>
       </c>
       <c r="X5" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="Y5" t="s">
         <v>2066</v>
@@ -30092,13 +30137,13 @@
         <v>438</v>
       </c>
       <c r="AB5" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="AC5" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AD5" t="s">
-        <v>2057</v>
+        <v>799</v>
       </c>
       <c r="AE5" t="s">
         <v>1963</v>
@@ -30113,13 +30158,13 @@
         <v>1917</v>
       </c>
       <c r="AI5" t="s">
-        <v>282</v>
+        <v>2277</v>
       </c>
       <c r="AJ5" t="s">
-        <v>1962</v>
+        <v>2283</v>
       </c>
       <c r="AK5" t="s">
-        <v>2201</v>
+        <v>2282</v>
       </c>
     </row>
   </sheetData>
@@ -30162,10 +30207,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -30551,10 +30596,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -31910,10 +31955,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -32182,16 +32227,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -34968,27 +35013,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="34" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="32" max="34" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -37488,10 +37533,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="13" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="13" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FPL GW 21 after WHU
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9289" uniqueCount="2284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10089" uniqueCount="2363">
   <si>
     <t>Places</t>
   </si>
@@ -6886,6 +6886,243 @@
   </si>
   <si>
     <t>1409</t>
+  </si>
+  <si>
+    <t>Benrahma 6</t>
+  </si>
+  <si>
+    <t>1,573,543</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>3,039,014</t>
+  </si>
+  <si>
+    <t>Antonio 18$ captain</t>
+  </si>
+  <si>
+    <t>558,762</t>
+  </si>
+  <si>
+    <t>1218</t>
+  </si>
+  <si>
+    <t>Maddison -</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>454,458</t>
+  </si>
+  <si>
+    <t>1232</t>
+  </si>
+  <si>
+    <t>Jansson 2</t>
+  </si>
+  <si>
+    <t>Canós 3</t>
+  </si>
+  <si>
+    <t>Gray 4$ captain</t>
+  </si>
+  <si>
+    <t>Bowen 21</t>
+  </si>
+  <si>
+    <t>1,313,715</t>
+  </si>
+  <si>
+    <t>1149</t>
+  </si>
+  <si>
+    <t>Allan 5</t>
+  </si>
+  <si>
+    <t>2,781,970</t>
+  </si>
+  <si>
+    <t>1061</t>
+  </si>
+  <si>
+    <t>Pinnock 3</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>585,641</t>
+  </si>
+  <si>
+    <t>1215</t>
+  </si>
+  <si>
+    <t>667,533</t>
+  </si>
+  <si>
+    <t>Ward -</t>
+  </si>
+  <si>
+    <t>1,112,759</t>
+  </si>
+  <si>
+    <t>1164</t>
+  </si>
+  <si>
+    <t>418,670</t>
+  </si>
+  <si>
+    <t>1237</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>340,124</t>
+  </si>
+  <si>
+    <t>1250</t>
+  </si>
+  <si>
+    <t>1,487,273</t>
+  </si>
+  <si>
+    <t>1137</t>
+  </si>
+  <si>
+    <t>2,291,166</t>
+  </si>
+  <si>
+    <t>590,391</t>
+  </si>
+  <si>
+    <t>1214</t>
+  </si>
+  <si>
+    <t>826,864</t>
+  </si>
+  <si>
+    <t>1189</t>
+  </si>
+  <si>
+    <t>1,206,683</t>
+  </si>
+  <si>
+    <t>1157</t>
+  </si>
+  <si>
+    <t>Fabianski 9</t>
+  </si>
+  <si>
+    <t>Ward-Prowse 7</t>
+  </si>
+  <si>
+    <t>Doucouré 2</t>
+  </si>
+  <si>
+    <t>1,111,959</t>
+  </si>
+  <si>
+    <t>297,656</t>
+  </si>
+  <si>
+    <t>1258</t>
+  </si>
+  <si>
+    <t>Amartey -</t>
+  </si>
+  <si>
+    <t>499,643</t>
+  </si>
+  <si>
+    <t>1226</t>
+  </si>
+  <si>
+    <t>111,655</t>
+  </si>
+  <si>
+    <t>1305</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>139,862</t>
+  </si>
+  <si>
+    <t>1296</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>766,074</t>
+  </si>
+  <si>
+    <t>1195</t>
+  </si>
+  <si>
+    <t>Williams 1</t>
+  </si>
+  <si>
+    <t>430,103</t>
+  </si>
+  <si>
+    <t>1236</t>
+  </si>
+  <si>
+    <t>5,543,055</t>
+  </si>
+  <si>
+    <t>902</t>
+  </si>
+  <si>
+    <t>395,551</t>
+  </si>
+  <si>
+    <t>1241</t>
+  </si>
+  <si>
+    <t>22,884</t>
+  </si>
+  <si>
+    <t>Dawson 7</t>
+  </si>
+  <si>
+    <t>472,094</t>
+  </si>
+  <si>
+    <t>1230</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>139,569</t>
+  </si>
+  <si>
+    <t>94,489</t>
+  </si>
+  <si>
+    <t>269,047</t>
+  </si>
+  <si>
+    <t>1264</t>
+  </si>
+  <si>
+    <t>98,422</t>
+  </si>
+  <si>
+    <t>1310</t>
+  </si>
+  <si>
+    <t>107,162</t>
+  </si>
+  <si>
+    <t>1307</t>
   </si>
 </sst>
 </file>
@@ -10064,28 +10301,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="22" max="23" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="24" max="27" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="28" max="30" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0078125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="26.59765625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="26.46875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="19.1171875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="19.1171875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.1171875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -10209,13 +10452,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
         <v>2065</v>
       </c>
       <c r="E2" t="s">
-        <v>2229</v>
+        <v>2285</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -10230,55 +10473,55 @@
         <v>1963</v>
       </c>
       <c r="U2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="W2" t="s">
         <v>2062</v>
       </c>
-      <c r="V2" t="s">
-        <v>2037</v>
-      </c>
-      <c r="W2" t="s">
-        <v>1964</v>
-      </c>
       <c r="X2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>2284</v>
+      </c>
+      <c r="AA2" t="s">
         <v>1936</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1992</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>2038</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>2063</v>
       </c>
       <c r="AB2" t="s">
         <v>2064</v>
       </c>
       <c r="AC2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="AD2" t="s">
         <v>749</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>2039</v>
       </c>
       <c r="AE2" t="s">
         <v>2040</v>
       </c>
       <c r="AF2" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AG2" t="s">
         <v>940</v>
       </c>
       <c r="AH2" t="s">
-        <v>1966</v>
+        <v>2037</v>
       </c>
       <c r="AI2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AJ2" t="s">
         <v>2065</v>
       </c>
       <c r="AK2" t="s">
-        <v>2229</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -10289,13 +10532,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>1913</v>
+        <v>2286</v>
       </c>
       <c r="D3" t="s">
         <v>2231</v>
       </c>
       <c r="E3" t="s">
-        <v>2230</v>
+        <v>2287</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
@@ -10310,55 +10553,55 @@
         <v>2040</v>
       </c>
       <c r="U3" t="s">
-        <v>1965</v>
+        <v>2062</v>
       </c>
       <c r="V3" t="s">
         <v>1964</v>
       </c>
       <c r="W3" t="s">
-        <v>2062</v>
+        <v>2276</v>
       </c>
       <c r="X3" t="s">
-        <v>2037</v>
+        <v>679</v>
       </c>
       <c r="Y3" t="s">
-        <v>1967</v>
+        <v>1932</v>
       </c>
       <c r="Z3" t="s">
         <v>2066</v>
       </c>
       <c r="AA3" t="s">
-        <v>1932</v>
+        <v>1967</v>
       </c>
       <c r="AB3" t="s">
         <v>2038</v>
       </c>
       <c r="AC3" t="s">
+        <v>2211</v>
+      </c>
+      <c r="AD3" t="s">
         <v>749</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>2211</v>
       </c>
       <c r="AE3" t="s">
         <v>1912</v>
       </c>
       <c r="AF3" t="s">
-        <v>2041</v>
+        <v>2037</v>
       </c>
       <c r="AG3" t="s">
-        <v>1969</v>
+        <v>710</v>
       </c>
       <c r="AH3" t="s">
         <v>940</v>
       </c>
       <c r="AI3" t="s">
-        <v>1913</v>
+        <v>2286</v>
       </c>
       <c r="AJ3" t="s">
         <v>2231</v>
       </c>
       <c r="AK3" t="s">
-        <v>2230</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -10369,13 +10612,13 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>771</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>2003</v>
+        <v>2290</v>
       </c>
       <c r="E4" t="s">
-        <v>2232</v>
+        <v>2289</v>
       </c>
       <c r="G4" t="s">
         <v>672</v>
@@ -10390,7 +10633,7 @@
         <v>2040</v>
       </c>
       <c r="U4" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="V4" t="s">
         <v>2042</v>
@@ -10411,7 +10654,7 @@
         <v>438</v>
       </c>
       <c r="AB4" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AC4" t="s">
         <v>749</v>
@@ -10432,13 +10675,13 @@
         <v>1967</v>
       </c>
       <c r="AI4" t="s">
-        <v>771</v>
+        <v>286</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2003</v>
+        <v>2290</v>
       </c>
       <c r="AK4" t="s">
-        <v>2232</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -10449,13 +10692,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>2292</v>
       </c>
       <c r="D5" t="s">
-        <v>2070</v>
+        <v>2294</v>
       </c>
       <c r="E5" t="s">
-        <v>2234</v>
+        <v>2293</v>
       </c>
       <c r="G5" t="s">
         <v>653</v>
@@ -10470,55 +10713,55 @@
         <v>2044</v>
       </c>
       <c r="U5" t="s">
+        <v>1974</v>
+      </c>
+      <c r="V5" t="s">
         <v>1964</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>2062</v>
-      </c>
-      <c r="W5" t="s">
-        <v>2233</v>
       </c>
       <c r="X5" t="s">
         <v>1936</v>
       </c>
       <c r="Y5" t="s">
-        <v>1994</v>
+        <v>2045</v>
       </c>
       <c r="Z5" t="s">
+        <v>2271</v>
+      </c>
+      <c r="AA5" t="s">
         <v>2069</v>
       </c>
-      <c r="AA5" t="s">
-        <v>2045</v>
-      </c>
       <c r="AB5" t="s">
-        <v>1972</v>
+        <v>1995</v>
       </c>
       <c r="AC5" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AD5" t="s">
-        <v>1973</v>
+        <v>1265</v>
       </c>
       <c r="AE5" t="s">
         <v>1915</v>
       </c>
       <c r="AF5" t="s">
-        <v>1995</v>
+        <v>2291</v>
       </c>
       <c r="AG5" t="s">
-        <v>1974</v>
+        <v>2233</v>
       </c>
       <c r="AH5" t="s">
         <v>1966</v>
       </c>
       <c r="AI5" t="s">
-        <v>282</v>
+        <v>2292</v>
       </c>
       <c r="AJ5" t="s">
-        <v>2070</v>
+        <v>2294</v>
       </c>
       <c r="AK5" t="s">
-        <v>2234</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -10529,13 +10772,13 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>874</v>
+        <v>297</v>
       </c>
       <c r="D6" t="s">
-        <v>2053</v>
+        <v>2300</v>
       </c>
       <c r="E6" t="s">
-        <v>2235</v>
+        <v>2299</v>
       </c>
       <c r="G6" t="s">
         <v>653</v>
@@ -10547,37 +10790,37 @@
         <v>1942</v>
       </c>
       <c r="T6" t="s">
-        <v>2047</v>
+        <v>1411</v>
       </c>
       <c r="U6" t="s">
-        <v>2048</v>
+        <v>2295</v>
       </c>
       <c r="V6" t="s">
-        <v>2049</v>
+        <v>538</v>
       </c>
       <c r="W6" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="X6" t="s">
-        <v>2050</v>
+        <v>2296</v>
       </c>
       <c r="Y6" t="s">
         <v>1936</v>
       </c>
       <c r="Z6" t="s">
-        <v>2051</v>
+        <v>2297</v>
       </c>
       <c r="AA6" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AB6" t="s">
         <v>1223</v>
       </c>
       <c r="AC6" t="s">
-        <v>2052</v>
+        <v>2272</v>
       </c>
       <c r="AD6" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AE6" t="s">
         <v>1963</v>
@@ -10592,13 +10835,13 @@
         <v>2042</v>
       </c>
       <c r="AI6" t="s">
-        <v>874</v>
+        <v>297</v>
       </c>
       <c r="AJ6" t="s">
-        <v>2053</v>
+        <v>2300</v>
       </c>
       <c r="AK6" t="s">
-        <v>2235</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -10609,13 +10852,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>673</v>
+        <v>1512</v>
       </c>
       <c r="D7" t="s">
-        <v>2237</v>
+        <v>2303</v>
       </c>
       <c r="E7" t="s">
-        <v>2236</v>
+        <v>2302</v>
       </c>
       <c r="G7" t="s">
         <v>672</v>
@@ -10630,55 +10873,55 @@
         <v>726</v>
       </c>
       <c r="U7" t="s">
-        <v>1965</v>
+        <v>1997</v>
       </c>
       <c r="V7" t="s">
         <v>1194</v>
       </c>
       <c r="W7" t="s">
-        <v>1997</v>
+        <v>2054</v>
       </c>
       <c r="X7" t="s">
-        <v>2054</v>
+        <v>2042</v>
       </c>
       <c r="Y7" t="s">
         <v>2069</v>
       </c>
       <c r="Z7" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AA7" t="s">
-        <v>1932</v>
+        <v>2301</v>
       </c>
       <c r="AB7" t="s">
-        <v>2055</v>
+        <v>749</v>
       </c>
       <c r="AC7" t="s">
-        <v>2046</v>
+        <v>2211</v>
       </c>
       <c r="AD7" t="s">
-        <v>2211</v>
+        <v>2273</v>
       </c>
       <c r="AE7" t="s">
         <v>804</v>
       </c>
       <c r="AF7" t="s">
-        <v>749</v>
+        <v>2276</v>
       </c>
       <c r="AG7" t="s">
-        <v>2042</v>
+        <v>1932</v>
       </c>
       <c r="AH7" t="s">
         <v>2066</v>
       </c>
       <c r="AI7" t="s">
-        <v>673</v>
+        <v>1512</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2237</v>
+        <v>2303</v>
       </c>
       <c r="AK7" t="s">
-        <v>2236</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -10689,13 +10932,13 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>2305</v>
       </c>
       <c r="D8" t="s">
-        <v>2239</v>
+        <v>2307</v>
       </c>
       <c r="E8" t="s">
-        <v>2238</v>
+        <v>2306</v>
       </c>
       <c r="G8" t="s">
         <v>906</v>
@@ -10710,7 +10953,7 @@
         <v>2040</v>
       </c>
       <c r="U8" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="V8" t="s">
         <v>2062</v>
@@ -10719,7 +10962,7 @@
         <v>1974</v>
       </c>
       <c r="X8" t="s">
-        <v>2056</v>
+        <v>2304</v>
       </c>
       <c r="Y8" t="s">
         <v>2069</v>
@@ -10731,10 +10974,10 @@
         <v>2066</v>
       </c>
       <c r="AB8" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AC8" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AD8" t="s">
         <v>939</v>
@@ -10752,13 +10995,13 @@
         <v>757</v>
       </c>
       <c r="AI8" t="s">
-        <v>288</v>
+        <v>2305</v>
       </c>
       <c r="AJ8" t="s">
-        <v>2239</v>
+        <v>2307</v>
       </c>
       <c r="AK8" t="s">
-        <v>2238</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -10769,13 +11012,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>673</v>
+        <v>778</v>
       </c>
       <c r="D9" t="s">
-        <v>2068</v>
+        <v>2003</v>
       </c>
       <c r="E9" t="s">
-        <v>2240</v>
+        <v>2308</v>
       </c>
       <c r="G9" t="s">
         <v>653</v>
@@ -10796,49 +11039,49 @@
         <v>1194</v>
       </c>
       <c r="W9" t="s">
-        <v>2037</v>
+        <v>2042</v>
       </c>
       <c r="X9" t="s">
         <v>2038</v>
       </c>
       <c r="Y9" t="s">
+        <v>1975</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>1998</v>
+      </c>
+      <c r="AA9" t="s">
         <v>2066</v>
       </c>
-      <c r="Z9" t="s">
-        <v>1972</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>1998</v>
-      </c>
       <c r="AB9" t="s">
+        <v>2273</v>
+      </c>
+      <c r="AC9" t="s">
         <v>749</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>939</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>2046</v>
       </c>
       <c r="AE9" t="s">
         <v>2044</v>
       </c>
       <c r="AF9" t="s">
-        <v>1975</v>
+        <v>2291</v>
       </c>
       <c r="AG9" t="s">
-        <v>2042</v>
+        <v>2037</v>
       </c>
       <c r="AH9" t="s">
         <v>1939</v>
       </c>
       <c r="AI9" t="s">
-        <v>673</v>
+        <v>778</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2068</v>
+        <v>2003</v>
       </c>
       <c r="AK9" t="s">
-        <v>2240</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -10849,13 +11092,13 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>730</v>
+        <v>308</v>
       </c>
       <c r="D10" t="s">
-        <v>2242</v>
+        <v>2311</v>
       </c>
       <c r="E10" t="s">
-        <v>2241</v>
+        <v>2310</v>
       </c>
       <c r="G10" t="s">
         <v>672</v>
@@ -10870,7 +11113,7 @@
         <v>2044</v>
       </c>
       <c r="U10" t="s">
-        <v>2048</v>
+        <v>2295</v>
       </c>
       <c r="V10" t="s">
         <v>1964</v>
@@ -10882,16 +11125,16 @@
         <v>2062</v>
       </c>
       <c r="Y10" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z10" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="AA10" t="s">
         <v>1936</v>
       </c>
       <c r="AB10" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AC10" t="s">
         <v>939</v>
@@ -10900,7 +11143,7 @@
         <v>749</v>
       </c>
       <c r="AE10" t="s">
-        <v>1976</v>
+        <v>2309</v>
       </c>
       <c r="AF10" t="s">
         <v>1977</v>
@@ -10912,13 +11155,13 @@
         <v>1932</v>
       </c>
       <c r="AI10" t="s">
-        <v>730</v>
+        <v>308</v>
       </c>
       <c r="AJ10" t="s">
-        <v>2242</v>
+        <v>2311</v>
       </c>
       <c r="AK10" t="s">
-        <v>2241</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -10929,13 +11172,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>671</v>
+        <v>270</v>
       </c>
       <c r="D11" t="s">
-        <v>1921</v>
+        <v>2313</v>
       </c>
       <c r="E11" t="s">
-        <v>2243</v>
+        <v>2312</v>
       </c>
       <c r="G11" t="s">
         <v>653</v>
@@ -10971,16 +11214,16 @@
         <v>2063</v>
       </c>
       <c r="AB11" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AC11" t="s">
-        <v>2057</v>
+        <v>799</v>
       </c>
       <c r="AD11" t="s">
         <v>749</v>
       </c>
       <c r="AE11" t="s">
-        <v>2058</v>
+        <v>1364</v>
       </c>
       <c r="AF11" t="s">
         <v>1967</v>
@@ -10989,16 +11232,16 @@
         <v>2045</v>
       </c>
       <c r="AH11" t="s">
-        <v>2056</v>
+        <v>2304</v>
       </c>
       <c r="AI11" t="s">
-        <v>671</v>
+        <v>270</v>
       </c>
       <c r="AJ11" t="s">
-        <v>1921</v>
+        <v>2313</v>
       </c>
       <c r="AK11" t="s">
-        <v>2243</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -11009,13 +11252,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>1832</v>
+        <v>2314</v>
       </c>
       <c r="D12" t="s">
-        <v>2073</v>
+        <v>2316</v>
       </c>
       <c r="E12" t="s">
-        <v>2205</v>
+        <v>2315</v>
       </c>
       <c r="G12" t="s">
         <v>653</v>
@@ -11027,22 +11270,22 @@
         <v>289</v>
       </c>
       <c r="T12" t="s">
-        <v>2060</v>
+        <v>1249</v>
       </c>
       <c r="U12" t="s">
         <v>2062</v>
       </c>
       <c r="V12" t="s">
-        <v>2048</v>
+        <v>2295</v>
       </c>
       <c r="W12" t="s">
-        <v>2049</v>
+        <v>538</v>
       </c>
       <c r="X12" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Y12" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z12" t="s">
         <v>1936</v>
@@ -11051,13 +11294,13 @@
         <v>2066</v>
       </c>
       <c r="AB12" t="s">
-        <v>1992</v>
+        <v>2284</v>
       </c>
       <c r="AC12" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AD12" t="s">
-        <v>2057</v>
+        <v>799</v>
       </c>
       <c r="AE12" t="s">
         <v>1963</v>
@@ -11069,16 +11312,16 @@
         <v>2204</v>
       </c>
       <c r="AH12" t="s">
-        <v>1973</v>
+        <v>1265</v>
       </c>
       <c r="AI12" t="s">
-        <v>1832</v>
+        <v>2314</v>
       </c>
       <c r="AJ12" t="s">
-        <v>2073</v>
+        <v>2316</v>
       </c>
       <c r="AK12" t="s">
-        <v>2205</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -11089,13 +11332,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>912</v>
+        <v>1277</v>
       </c>
       <c r="D13" t="s">
-        <v>2245</v>
+        <v>2318</v>
       </c>
       <c r="E13" t="s">
-        <v>2244</v>
+        <v>2317</v>
       </c>
       <c r="G13" t="s">
         <v>578</v>
@@ -11107,31 +11350,31 @@
         <v>291</v>
       </c>
       <c r="T13" t="s">
-        <v>475</v>
+        <v>1963</v>
       </c>
       <c r="U13" t="s">
-        <v>2048</v>
+        <v>2062</v>
       </c>
       <c r="V13" t="s">
-        <v>2062</v>
+        <v>1964</v>
       </c>
       <c r="W13" t="s">
-        <v>1964</v>
+        <v>2295</v>
       </c>
       <c r="X13" t="s">
-        <v>1992</v>
+        <v>1943</v>
       </c>
       <c r="Y13" t="s">
-        <v>2209</v>
+        <v>2066</v>
       </c>
       <c r="Z13" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="AA13" t="s">
-        <v>2066</v>
+        <v>2284</v>
       </c>
       <c r="AB13" t="s">
-        <v>2057</v>
+        <v>799</v>
       </c>
       <c r="AC13" t="s">
         <v>749</v>
@@ -11140,10 +11383,10 @@
         <v>939</v>
       </c>
       <c r="AE13" t="s">
-        <v>1963</v>
+        <v>475</v>
       </c>
       <c r="AF13" t="s">
-        <v>1943</v>
+        <v>2209</v>
       </c>
       <c r="AG13" t="s">
         <v>1998</v>
@@ -11152,13 +11395,13 @@
         <v>1974</v>
       </c>
       <c r="AI13" t="s">
-        <v>912</v>
+        <v>1277</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2245</v>
+        <v>2318</v>
       </c>
       <c r="AK13" t="s">
-        <v>2244</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -11169,13 +11412,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>730</v>
+        <v>278</v>
       </c>
       <c r="D14" t="s">
         <v>1952</v>
       </c>
       <c r="E14" t="s">
-        <v>2246</v>
+        <v>2319</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -11196,10 +11439,10 @@
         <v>1945</v>
       </c>
       <c r="W14" t="s">
-        <v>1222</v>
+        <v>1966</v>
       </c>
       <c r="X14" t="s">
-        <v>2037</v>
+        <v>2074</v>
       </c>
       <c r="Y14" t="s">
         <v>2038</v>
@@ -11211,34 +11454,34 @@
         <v>2063</v>
       </c>
       <c r="AB14" t="s">
+        <v>1223</v>
+      </c>
+      <c r="AC14" t="s">
         <v>1938</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>2039</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>1223</v>
       </c>
       <c r="AE14" t="s">
         <v>1915</v>
       </c>
       <c r="AF14" t="s">
-        <v>1966</v>
+        <v>1222</v>
       </c>
       <c r="AG14" t="s">
-        <v>2074</v>
+        <v>2037</v>
       </c>
       <c r="AH14" t="s">
-        <v>1981</v>
+        <v>767</v>
       </c>
       <c r="AI14" t="s">
-        <v>730</v>
+        <v>278</v>
       </c>
       <c r="AJ14" t="s">
         <v>1952</v>
       </c>
       <c r="AK14" t="s">
-        <v>2246</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -11249,13 +11492,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>912</v>
+        <v>673</v>
       </c>
       <c r="D15" t="s">
-        <v>2008</v>
+        <v>2321</v>
       </c>
       <c r="E15" t="s">
-        <v>2247</v>
+        <v>2320</v>
       </c>
       <c r="G15" t="s">
         <v>653</v>
@@ -11291,7 +11534,7 @@
         <v>2069</v>
       </c>
       <c r="AB15" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AC15" t="s">
         <v>749</v>
@@ -11306,19 +11549,19 @@
         <v>1967</v>
       </c>
       <c r="AG15" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AH15" t="s">
         <v>2037</v>
       </c>
       <c r="AI15" t="s">
-        <v>912</v>
+        <v>673</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2008</v>
+        <v>2321</v>
       </c>
       <c r="AK15" t="s">
-        <v>2247</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -11329,13 +11572,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>829</v>
+        <v>268</v>
       </c>
       <c r="D16" t="s">
-        <v>1919</v>
+        <v>2323</v>
       </c>
       <c r="E16" t="s">
-        <v>2249</v>
+        <v>2322</v>
       </c>
       <c r="G16" t="s">
         <v>706</v>
@@ -11353,52 +11596,52 @@
         <v>1978</v>
       </c>
       <c r="V16" t="s">
+        <v>2062</v>
+      </c>
+      <c r="W16" t="s">
         <v>1194</v>
       </c>
-      <c r="W16" t="s">
-        <v>2062</v>
-      </c>
       <c r="X16" t="s">
-        <v>1992</v>
+        <v>1983</v>
       </c>
       <c r="Y16" t="s">
+        <v>1308</v>
+      </c>
+      <c r="Z16" t="s">
         <v>1936</v>
       </c>
-      <c r="Z16" t="s">
-        <v>1999</v>
-      </c>
       <c r="AA16" t="s">
+        <v>2284</v>
+      </c>
+      <c r="AB16" t="s">
         <v>2066</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>749</v>
       </c>
-      <c r="AC16" t="s">
-        <v>2043</v>
-      </c>
       <c r="AD16" t="s">
-        <v>2076</v>
+        <v>2288</v>
       </c>
       <c r="AE16" t="s">
         <v>2248</v>
       </c>
       <c r="AF16" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AG16" t="s">
         <v>1932</v>
       </c>
       <c r="AH16" t="s">
-        <v>1983</v>
+        <v>2076</v>
       </c>
       <c r="AI16" t="s">
-        <v>829</v>
+        <v>268</v>
       </c>
       <c r="AJ16" t="s">
-        <v>1919</v>
+        <v>2323</v>
       </c>
       <c r="AK16" t="s">
-        <v>2249</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -11409,13 +11652,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>1452</v>
+        <v>274</v>
       </c>
       <c r="D17" t="s">
-        <v>2077</v>
+        <v>2325</v>
       </c>
       <c r="E17" t="s">
-        <v>2250</v>
+        <v>2324</v>
       </c>
       <c r="G17" t="s">
         <v>906</v>
@@ -11433,52 +11676,52 @@
         <v>1997</v>
       </c>
       <c r="V17" t="s">
+        <v>2062</v>
+      </c>
+      <c r="W17" t="s">
         <v>1964</v>
       </c>
-      <c r="W17" t="s">
-        <v>2062</v>
-      </c>
       <c r="X17" t="s">
-        <v>1996</v>
+        <v>2066</v>
       </c>
       <c r="Y17" t="s">
-        <v>2066</v>
+        <v>1967</v>
       </c>
       <c r="Z17" t="s">
         <v>2069</v>
       </c>
       <c r="AA17" t="s">
-        <v>438</v>
+        <v>2298</v>
       </c>
       <c r="AB17" t="s">
+        <v>749</v>
+      </c>
+      <c r="AC17" t="s">
         <v>2000</v>
       </c>
-      <c r="AC17" t="s">
-        <v>2043</v>
-      </c>
       <c r="AD17" t="s">
-        <v>749</v>
+        <v>2288</v>
       </c>
       <c r="AE17" t="s">
         <v>1963</v>
       </c>
       <c r="AF17" t="s">
-        <v>1967</v>
+        <v>438</v>
       </c>
       <c r="AG17" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AH17" t="s">
         <v>1983</v>
       </c>
       <c r="AI17" t="s">
-        <v>1452</v>
+        <v>274</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2077</v>
+        <v>2325</v>
       </c>
       <c r="AK17" t="s">
-        <v>2250</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -11489,13 +11732,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>829</v>
+        <v>1210</v>
       </c>
       <c r="D18" t="s">
-        <v>1922</v>
+        <v>2311</v>
       </c>
       <c r="E18" t="s">
-        <v>2251</v>
+        <v>2329</v>
       </c>
       <c r="G18" t="s">
         <v>653</v>
@@ -11507,37 +11750,37 @@
         <v>813</v>
       </c>
       <c r="T18" t="s">
-        <v>2001</v>
+        <v>2326</v>
       </c>
       <c r="U18" t="s">
         <v>2062</v>
       </c>
       <c r="V18" t="s">
-        <v>2048</v>
+        <v>2295</v>
       </c>
       <c r="W18" t="s">
         <v>1964</v>
       </c>
       <c r="X18" t="s">
-        <v>1984</v>
+        <v>2327</v>
       </c>
       <c r="Y18" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Z18" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AA18" t="s">
         <v>1936</v>
       </c>
       <c r="AB18" t="s">
-        <v>2078</v>
+        <v>2328</v>
       </c>
       <c r="AC18" t="s">
         <v>939</v>
       </c>
       <c r="AD18" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AE18" t="s">
         <v>1833</v>
@@ -11549,16 +11792,16 @@
         <v>1974</v>
       </c>
       <c r="AH18" t="s">
-        <v>1973</v>
+        <v>1265</v>
       </c>
       <c r="AI18" t="s">
-        <v>829</v>
+        <v>1210</v>
       </c>
       <c r="AJ18" t="s">
-        <v>1922</v>
+        <v>2311</v>
       </c>
       <c r="AK18" t="s">
-        <v>2251</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -11569,13 +11812,13 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>778</v>
+        <v>1219</v>
       </c>
       <c r="D19" t="s">
-        <v>2253</v>
+        <v>2331</v>
       </c>
       <c r="E19" t="s">
-        <v>2252</v>
+        <v>2330</v>
       </c>
       <c r="G19" t="s">
         <v>452</v>
@@ -11590,55 +11833,55 @@
         <v>2198</v>
       </c>
       <c r="U19" t="s">
-        <v>2002</v>
+        <v>1964</v>
       </c>
       <c r="V19" t="s">
-        <v>1964</v>
+        <v>2275</v>
       </c>
       <c r="W19" t="s">
         <v>1997</v>
       </c>
       <c r="X19" t="s">
+        <v>2045</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>2298</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>1986</v>
+      </c>
+      <c r="AA19" t="s">
         <v>1936</v>
       </c>
-      <c r="Y19" t="s">
-        <v>1986</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>1996</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>2045</v>
-      </c>
       <c r="AB19" t="s">
-        <v>2057</v>
+        <v>2069</v>
       </c>
       <c r="AC19" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AD19" t="s">
-        <v>2076</v>
+        <v>799</v>
       </c>
       <c r="AE19" t="s">
         <v>1963</v>
       </c>
       <c r="AF19" t="s">
-        <v>2069</v>
+        <v>2076</v>
       </c>
       <c r="AG19" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AH19" t="s">
         <v>1983</v>
       </c>
       <c r="AI19" t="s">
-        <v>778</v>
+        <v>1219</v>
       </c>
       <c r="AJ19" t="s">
-        <v>2253</v>
+        <v>2331</v>
       </c>
       <c r="AK19" t="s">
-        <v>2252</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -11649,13 +11892,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D20" t="s">
-        <v>2255</v>
+        <v>2334</v>
       </c>
       <c r="E20" t="s">
-        <v>2254</v>
+        <v>2333</v>
       </c>
       <c r="G20" t="s">
         <v>452</v>
@@ -11679,7 +11922,7 @@
         <v>2004</v>
       </c>
       <c r="X20" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="Y20" t="s">
         <v>2005</v>
@@ -11691,7 +11934,7 @@
         <v>1936</v>
       </c>
       <c r="AB20" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AC20" t="s">
         <v>749</v>
@@ -11709,16 +11952,16 @@
         <v>2037</v>
       </c>
       <c r="AH20" t="s">
-        <v>1987</v>
+        <v>2332</v>
       </c>
       <c r="AI20" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="AJ20" t="s">
-        <v>2255</v>
+        <v>2334</v>
       </c>
       <c r="AK20" t="s">
-        <v>2254</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -11729,13 +11972,13 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>785</v>
+        <v>1459</v>
       </c>
       <c r="D21" t="s">
-        <v>2024</v>
+        <v>2336</v>
       </c>
       <c r="E21" t="s">
-        <v>2256</v>
+        <v>2335</v>
       </c>
       <c r="G21" t="s">
         <v>706</v>
@@ -11750,55 +11993,55 @@
         <v>2198</v>
       </c>
       <c r="U21" t="s">
+        <v>1964</v>
+      </c>
+      <c r="V21" t="s">
         <v>2062</v>
       </c>
-      <c r="V21" t="s">
-        <v>2002</v>
-      </c>
       <c r="W21" t="s">
-        <v>1964</v>
+        <v>2275</v>
       </c>
       <c r="X21" t="s">
-        <v>1996</v>
+        <v>1974</v>
       </c>
       <c r="Y21" t="s">
+        <v>2298</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>2069</v>
+      </c>
+      <c r="AA21" t="s">
         <v>2045</v>
       </c>
-      <c r="Z21" t="s">
-        <v>438</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>2069</v>
-      </c>
       <c r="AB21" t="s">
-        <v>2043</v>
+        <v>2076</v>
       </c>
       <c r="AC21" t="s">
         <v>939</v>
       </c>
       <c r="AD21" t="s">
-        <v>2076</v>
+        <v>2288</v>
       </c>
       <c r="AE21" t="s">
         <v>1915</v>
       </c>
       <c r="AF21" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AG21" t="s">
-        <v>1974</v>
+        <v>438</v>
       </c>
       <c r="AH21" t="s">
         <v>1932</v>
       </c>
       <c r="AI21" t="s">
-        <v>785</v>
+        <v>1459</v>
       </c>
       <c r="AJ21" t="s">
-        <v>2024</v>
+        <v>2336</v>
       </c>
       <c r="AK21" t="s">
-        <v>2256</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -11809,13 +12052,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>829</v>
+        <v>2337</v>
       </c>
       <c r="D22" t="s">
-        <v>2258</v>
+        <v>2339</v>
       </c>
       <c r="E22" t="s">
-        <v>2257</v>
+        <v>2338</v>
       </c>
       <c r="G22" t="s">
         <v>578</v>
@@ -11833,37 +12076,37 @@
         <v>2062</v>
       </c>
       <c r="V22" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="W22" t="s">
         <v>1964</v>
       </c>
       <c r="X22" t="s">
-        <v>438</v>
+        <v>1943</v>
       </c>
       <c r="Y22" t="s">
+        <v>2271</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>1936</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB22" t="s">
         <v>2069</v>
       </c>
-      <c r="Z22" t="s">
-        <v>1994</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>1936</v>
-      </c>
       <c r="AC22" t="s">
+        <v>2273</v>
+      </c>
+      <c r="AD22" t="s">
         <v>749</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>2046</v>
       </c>
       <c r="AE22" t="s">
         <v>1963</v>
       </c>
       <c r="AF22" t="s">
-        <v>1943</v>
+        <v>438</v>
       </c>
       <c r="AG22" t="s">
         <v>1917</v>
@@ -11872,13 +12115,13 @@
         <v>828</v>
       </c>
       <c r="AI22" t="s">
-        <v>829</v>
+        <v>2337</v>
       </c>
       <c r="AJ22" t="s">
-        <v>2258</v>
+        <v>2339</v>
       </c>
       <c r="AK22" t="s">
-        <v>2257</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -11889,13 +12132,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>2340</v>
       </c>
       <c r="D23" t="s">
-        <v>1947</v>
+        <v>2342</v>
       </c>
       <c r="E23" t="s">
-        <v>2259</v>
+        <v>2341</v>
       </c>
       <c r="G23" t="s">
         <v>653</v>
@@ -11910,31 +12153,31 @@
         <v>475</v>
       </c>
       <c r="U23" t="s">
+        <v>1997</v>
+      </c>
+      <c r="V23" t="s">
+        <v>1964</v>
+      </c>
+      <c r="W23" t="s">
+        <v>1945</v>
+      </c>
+      <c r="X23" t="s">
         <v>2062</v>
       </c>
-      <c r="V23" t="s">
-        <v>1945</v>
-      </c>
-      <c r="W23" t="s">
-        <v>1964</v>
-      </c>
-      <c r="X23" t="s">
-        <v>1997</v>
-      </c>
       <c r="Y23" t="s">
-        <v>1932</v>
+        <v>1940</v>
       </c>
       <c r="Z23" t="s">
         <v>2066</v>
       </c>
       <c r="AA23" t="s">
-        <v>1940</v>
+        <v>1988</v>
       </c>
       <c r="AB23" t="s">
-        <v>2076</v>
+        <v>1967</v>
       </c>
       <c r="AC23" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AD23" t="s">
         <v>749</v>
@@ -11943,22 +12186,22 @@
         <v>399</v>
       </c>
       <c r="AF23" t="s">
-        <v>1988</v>
+        <v>1932</v>
       </c>
       <c r="AG23" t="s">
-        <v>1967</v>
+        <v>2076</v>
       </c>
       <c r="AH23" t="s">
         <v>1966</v>
       </c>
       <c r="AI23" t="s">
-        <v>272</v>
+        <v>2340</v>
       </c>
       <c r="AJ23" t="s">
-        <v>1947</v>
+        <v>2342</v>
       </c>
       <c r="AK23" t="s">
-        <v>2259</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -11969,13 +12212,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>841</v>
+        <v>1750</v>
       </c>
       <c r="D24" t="s">
-        <v>2061</v>
+        <v>2345</v>
       </c>
       <c r="E24" t="s">
-        <v>2260</v>
+        <v>2344</v>
       </c>
       <c r="G24" t="s">
         <v>452</v>
@@ -11993,13 +12236,13 @@
         <v>1964</v>
       </c>
       <c r="V24" t="s">
-        <v>2002</v>
+        <v>2275</v>
       </c>
       <c r="W24" t="s">
         <v>2062</v>
       </c>
       <c r="X24" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="Y24" t="s">
         <v>2067</v>
@@ -12017,7 +12260,7 @@
         <v>1223</v>
       </c>
       <c r="AD24" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AE24" t="s">
         <v>1915</v>
@@ -12026,19 +12269,19 @@
         <v>1967</v>
       </c>
       <c r="AG24" t="s">
-        <v>1989</v>
+        <v>2343</v>
       </c>
       <c r="AH24" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AI24" t="s">
-        <v>841</v>
+        <v>1750</v>
       </c>
       <c r="AJ24" t="s">
-        <v>2061</v>
+        <v>2345</v>
       </c>
       <c r="AK24" t="s">
-        <v>2260</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -12049,13 +12292,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>268</v>
+        <v>1750</v>
       </c>
       <c r="D25" t="s">
-        <v>2079</v>
+        <v>2347</v>
       </c>
       <c r="E25" t="s">
-        <v>2261</v>
+        <v>2346</v>
       </c>
       <c r="G25" t="s">
         <v>653</v>
@@ -12067,7 +12310,7 @@
         <v>487</v>
       </c>
       <c r="T25" t="s">
-        <v>2001</v>
+        <v>2326</v>
       </c>
       <c r="U25" t="s">
         <v>1997</v>
@@ -12082,10 +12325,10 @@
         <v>2045</v>
       </c>
       <c r="Y25" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Z25" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AA25" t="s">
         <v>1936</v>
@@ -12094,10 +12337,10 @@
         <v>1986</v>
       </c>
       <c r="AC25" t="s">
-        <v>2057</v>
+        <v>799</v>
       </c>
       <c r="AD25" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AE25" t="s">
         <v>1915</v>
@@ -12112,13 +12355,13 @@
         <v>2042</v>
       </c>
       <c r="AI25" t="s">
-        <v>268</v>
+        <v>1750</v>
       </c>
       <c r="AJ25" t="s">
-        <v>2079</v>
+        <v>2347</v>
       </c>
       <c r="AK25" t="s">
-        <v>2261</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -12129,13 +12372,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>673</v>
+        <v>284</v>
       </c>
       <c r="D26" t="s">
-        <v>2263</v>
+        <v>2349</v>
       </c>
       <c r="E26" t="s">
-        <v>2262</v>
+        <v>2348</v>
       </c>
       <c r="G26" t="s">
         <v>578</v>
@@ -12162,16 +12405,16 @@
         <v>2069</v>
       </c>
       <c r="Y26" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z26" t="s">
         <v>1990</v>
       </c>
       <c r="AA26" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="AB26" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AC26" t="s">
         <v>2000</v>
@@ -12186,19 +12429,19 @@
         <v>1932</v>
       </c>
       <c r="AG26" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AH26" t="s">
         <v>1966</v>
       </c>
       <c r="AI26" t="s">
-        <v>673</v>
+        <v>284</v>
       </c>
       <c r="AJ26" t="s">
-        <v>2263</v>
+        <v>2349</v>
       </c>
       <c r="AK26" t="s">
-        <v>2262</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -12209,13 +12452,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>671</v>
+        <v>2305</v>
       </c>
       <c r="D27" t="s">
-        <v>1957</v>
+        <v>2140</v>
       </c>
       <c r="E27" t="s">
-        <v>2264</v>
+        <v>2350</v>
       </c>
       <c r="G27" t="s">
         <v>452</v>
@@ -12239,7 +12482,7 @@
         <v>2062</v>
       </c>
       <c r="X27" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Y27" t="s">
         <v>2069</v>
@@ -12248,7 +12491,7 @@
         <v>1936</v>
       </c>
       <c r="AA27" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="AB27" t="s">
         <v>1991</v>
@@ -12257,7 +12500,7 @@
         <v>2000</v>
       </c>
       <c r="AD27" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AE27" t="s">
         <v>1915</v>
@@ -12272,13 +12515,13 @@
         <v>1945</v>
       </c>
       <c r="AI27" t="s">
-        <v>671</v>
+        <v>2305</v>
       </c>
       <c r="AJ27" t="s">
-        <v>1957</v>
+        <v>2140</v>
       </c>
       <c r="AK27" t="s">
-        <v>2264</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -12289,13 +12532,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>841</v>
+        <v>274</v>
       </c>
       <c r="D28" t="s">
-        <v>1941</v>
+        <v>2353</v>
       </c>
       <c r="E28" t="s">
-        <v>2265</v>
+        <v>2352</v>
       </c>
       <c r="G28" t="s">
         <v>906</v>
@@ -12313,7 +12556,7 @@
         <v>1964</v>
       </c>
       <c r="V28" t="s">
-        <v>2006</v>
+        <v>2351</v>
       </c>
       <c r="W28" t="s">
         <v>2062</v>
@@ -12322,7 +12565,7 @@
         <v>1990</v>
       </c>
       <c r="Y28" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Z28" t="s">
         <v>1936</v>
@@ -12331,10 +12574,10 @@
         <v>2069</v>
       </c>
       <c r="AB28" t="s">
-        <v>1996</v>
+        <v>2298</v>
       </c>
       <c r="AC28" t="s">
-        <v>2043</v>
+        <v>2288</v>
       </c>
       <c r="AD28" t="s">
         <v>939</v>
@@ -12346,19 +12589,19 @@
         <v>1997</v>
       </c>
       <c r="AG28" t="s">
-        <v>1973</v>
+        <v>1265</v>
       </c>
       <c r="AH28" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="AI28" t="s">
-        <v>841</v>
+        <v>274</v>
       </c>
       <c r="AJ28" t="s">
-        <v>1941</v>
+        <v>2353</v>
       </c>
       <c r="AK28" t="s">
-        <v>2265</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -12369,13 +12612,13 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>771</v>
+        <v>2354</v>
       </c>
       <c r="D29" t="s">
-        <v>1958</v>
+        <v>2339</v>
       </c>
       <c r="E29" t="s">
-        <v>2266</v>
+        <v>2355</v>
       </c>
       <c r="G29" t="s">
         <v>906</v>
@@ -12390,7 +12633,7 @@
         <v>2198</v>
       </c>
       <c r="U29" t="s">
-        <v>2049</v>
+        <v>538</v>
       </c>
       <c r="V29" t="s">
         <v>1964</v>
@@ -12399,10 +12642,10 @@
         <v>2062</v>
       </c>
       <c r="X29" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Y29" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z29" t="s">
         <v>2132</v>
@@ -12411,7 +12654,7 @@
         <v>2069</v>
       </c>
       <c r="AB29" t="s">
-        <v>2052</v>
+        <v>2272</v>
       </c>
       <c r="AC29" t="s">
         <v>1223</v>
@@ -12432,13 +12675,13 @@
         <v>2081</v>
       </c>
       <c r="AI29" t="s">
-        <v>771</v>
+        <v>2354</v>
       </c>
       <c r="AJ29" t="s">
-        <v>1958</v>
+        <v>2339</v>
       </c>
       <c r="AK29" t="s">
-        <v>2266</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -12449,13 +12692,13 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>841</v>
+        <v>1219</v>
       </c>
       <c r="D30" t="s">
-        <v>1918</v>
+        <v>2084</v>
       </c>
       <c r="E30" t="s">
-        <v>2267</v>
+        <v>2356</v>
       </c>
       <c r="G30" t="s">
         <v>452</v>
@@ -12470,40 +12713,40 @@
         <v>2198</v>
       </c>
       <c r="U30" t="s">
-        <v>2062</v>
+        <v>1964</v>
       </c>
       <c r="V30" t="s">
         <v>2004</v>
       </c>
       <c r="W30" t="s">
-        <v>1964</v>
+        <v>2062</v>
       </c>
       <c r="X30" t="s">
-        <v>1932</v>
+        <v>679</v>
       </c>
       <c r="Y30" t="s">
+        <v>2271</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>1977</v>
+      </c>
+      <c r="AA30" t="s">
         <v>2069</v>
       </c>
-      <c r="Z30" t="s">
-        <v>1994</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>2041</v>
-      </c>
       <c r="AB30" t="s">
-        <v>2046</v>
+        <v>1223</v>
       </c>
       <c r="AC30" t="s">
-        <v>1223</v>
+        <v>939</v>
       </c>
       <c r="AD30" t="s">
-        <v>939</v>
+        <v>2273</v>
       </c>
       <c r="AE30" t="s">
         <v>1915</v>
       </c>
       <c r="AF30" t="s">
-        <v>1977</v>
+        <v>1932</v>
       </c>
       <c r="AG30" t="s">
         <v>2233</v>
@@ -12512,13 +12755,13 @@
         <v>2037</v>
       </c>
       <c r="AI30" t="s">
-        <v>841</v>
+        <v>1219</v>
       </c>
       <c r="AJ30" t="s">
-        <v>1918</v>
+        <v>2084</v>
       </c>
       <c r="AK30" t="s">
-        <v>2267</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -12529,13 +12772,13 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>912</v>
+        <v>1750</v>
       </c>
       <c r="D31" t="s">
-        <v>1953</v>
+        <v>2358</v>
       </c>
       <c r="E31" t="s">
-        <v>2268</v>
+        <v>2357</v>
       </c>
       <c r="G31" t="s">
         <v>452</v>
@@ -12550,55 +12793,55 @@
         <v>2198</v>
       </c>
       <c r="U31" t="s">
-        <v>1965</v>
+        <v>1993</v>
       </c>
       <c r="V31" t="s">
+        <v>2062</v>
+      </c>
+      <c r="W31" t="s">
         <v>1964</v>
       </c>
-      <c r="W31" t="s">
-        <v>2062</v>
-      </c>
       <c r="X31" t="s">
+        <v>2271</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>2069</v>
+      </c>
+      <c r="AA31" t="s">
         <v>1936</v>
       </c>
-      <c r="Y31" t="s">
-        <v>2069</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>1994</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>2041</v>
-      </c>
       <c r="AB31" t="s">
-        <v>2076</v>
+        <v>1967</v>
       </c>
       <c r="AC31" t="s">
+        <v>939</v>
+      </c>
+      <c r="AD31" t="s">
         <v>749</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>939</v>
       </c>
       <c r="AE31" t="s">
         <v>1915</v>
       </c>
       <c r="AF31" t="s">
-        <v>1993</v>
+        <v>2276</v>
       </c>
       <c r="AG31" t="s">
-        <v>1967</v>
+        <v>2076</v>
       </c>
       <c r="AH31" t="s">
         <v>2037</v>
       </c>
       <c r="AI31" t="s">
-        <v>912</v>
+        <v>1750</v>
       </c>
       <c r="AJ31" t="s">
-        <v>1953</v>
+        <v>2358</v>
       </c>
       <c r="AK31" t="s">
-        <v>2268</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -12609,13 +12852,13 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>671</v>
+        <v>2305</v>
       </c>
       <c r="D32" t="s">
-        <v>1927</v>
+        <v>2360</v>
       </c>
       <c r="E32" t="s">
-        <v>2269</v>
+        <v>2359</v>
       </c>
       <c r="G32" t="s">
         <v>452</v>
@@ -12642,7 +12885,7 @@
         <v>1936</v>
       </c>
       <c r="Y32" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="Z32" t="s">
         <v>2038</v>
@@ -12654,7 +12897,7 @@
         <v>1991</v>
       </c>
       <c r="AC32" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AD32" t="s">
         <v>749</v>
@@ -12672,13 +12915,13 @@
         <v>1939</v>
       </c>
       <c r="AI32" t="s">
-        <v>671</v>
+        <v>2305</v>
       </c>
       <c r="AJ32" t="s">
-        <v>1927</v>
+        <v>2360</v>
       </c>
       <c r="AK32" t="s">
-        <v>2269</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -12689,13 +12932,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>829</v>
+        <v>1210</v>
       </c>
       <c r="D33" t="s">
-        <v>2024</v>
+        <v>2362</v>
       </c>
       <c r="E33" t="s">
-        <v>2270</v>
+        <v>2361</v>
       </c>
       <c r="G33" t="s">
         <v>578</v>
@@ -12710,7 +12953,7 @@
         <v>1963</v>
       </c>
       <c r="U33" t="s">
-        <v>1965</v>
+        <v>2276</v>
       </c>
       <c r="V33" t="s">
         <v>1964</v>
@@ -12722,16 +12965,16 @@
         <v>2069</v>
       </c>
       <c r="Y33" t="s">
-        <v>2041</v>
+        <v>679</v>
       </c>
       <c r="Z33" t="s">
         <v>1936</v>
       </c>
       <c r="AA33" t="s">
-        <v>1994</v>
+        <v>2271</v>
       </c>
       <c r="AB33" t="s">
-        <v>2046</v>
+        <v>2273</v>
       </c>
       <c r="AC33" t="s">
         <v>939</v>
@@ -12752,13 +12995,13 @@
         <v>2037</v>
       </c>
       <c r="AI33" t="s">
-        <v>829</v>
+        <v>1210</v>
       </c>
       <c r="AJ33" t="s">
-        <v>2024</v>
+        <v>2362</v>
       </c>
       <c r="AK33" t="s">
-        <v>2270</v>
+        <v>2361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GW23 and FPL homebutton
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12487" uniqueCount="2656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14887" uniqueCount="2833">
   <si>
     <t>Places</t>
   </si>
@@ -8002,6 +8002,537 @@
   </si>
   <si>
     <t>993</t>
+  </si>
+  <si>
+    <t>Ramsdale BUR (H)</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold CRY (A)</t>
+  </si>
+  <si>
+    <t>James TOT (H)</t>
+  </si>
+  <si>
+    <t>Cancelo SOU (A)</t>
+  </si>
+  <si>
+    <t>Son CHE (A)</t>
+  </si>
+  <si>
+    <t>Bernardo SOU (A)</t>
+  </si>
+  <si>
+    <t>Salah CRY (A)$ captain</t>
+  </si>
+  <si>
+    <t>Hudson-Odoi TOT (H)</t>
+  </si>
+  <si>
+    <t>Dennis -1, BUR (A)</t>
+  </si>
+  <si>
+    <t>Maupay LEI (A)</t>
+  </si>
+  <si>
+    <t>Livramento MCI (H)</t>
+  </si>
+  <si>
+    <t>White BUR (H)</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>1,846,615</t>
+  </si>
+  <si>
+    <t>1172</t>
+  </si>
+  <si>
+    <t>Coady 1</t>
+  </si>
+  <si>
+    <t>Smith Rowe BUR (H)</t>
+  </si>
+  <si>
+    <t>Bowen 1</t>
+  </si>
+  <si>
+    <t>Gallagher LIV (H)</t>
+  </si>
+  <si>
+    <t>Guaita LIV (H)</t>
+  </si>
+  <si>
+    <t>2,886,574</t>
+  </si>
+  <si>
+    <t>Foster 0, BUR (A)</t>
+  </si>
+  <si>
+    <t>Mount TOT (H)</t>
+  </si>
+  <si>
+    <t>De Bruyne SOU (A)</t>
+  </si>
+  <si>
+    <t>Foden SOU (A)</t>
+  </si>
+  <si>
+    <t>Tsimikas CRY (A)</t>
+  </si>
+  <si>
+    <t>Dier CHE (A)</t>
+  </si>
+  <si>
+    <t>721,339</t>
+  </si>
+  <si>
+    <t>1262</t>
+  </si>
+  <si>
+    <t>Tierney BUR (H)</t>
+  </si>
+  <si>
+    <t>Jota CRY (A)</t>
+  </si>
+  <si>
+    <t>Maddison BHA (H)</t>
+  </si>
+  <si>
+    <t>Dennis -2, BUR (A)$ captain</t>
+  </si>
+  <si>
+    <t>Lloris CHE (A)</t>
+  </si>
+  <si>
+    <t>Edouard LIV (H)</t>
+  </si>
+  <si>
+    <t>Broja MCI (H)</t>
+  </si>
+  <si>
+    <t>Dalot 1</t>
+  </si>
+  <si>
+    <t>399,924</t>
+  </si>
+  <si>
+    <t>1305</t>
+  </si>
+  <si>
+    <t>Bachmann 1, BUR (A)</t>
+  </si>
+  <si>
+    <t>Mings 5</t>
+  </si>
+  <si>
+    <t>Varane 1</t>
+  </si>
+  <si>
+    <t>Sissoko 2, BUR (A)</t>
+  </si>
+  <si>
+    <t>Mac Allister LEI (A)</t>
+  </si>
+  <si>
+    <t>Kane CHE (A)</t>
+  </si>
+  <si>
+    <t>Arrizabalaga TOT (H)</t>
+  </si>
+  <si>
+    <t>Davies CHE (A)</t>
+  </si>
+  <si>
+    <t>Winks CHE (A)</t>
+  </si>
+  <si>
+    <t>1,016,459</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>Dias SOU (A)</t>
+  </si>
+  <si>
+    <t>Reguilón CHE (A)</t>
+  </si>
+  <si>
+    <t>Duffy LEI (A)</t>
+  </si>
+  <si>
+    <t>Salah CRY (A)</t>
+  </si>
+  <si>
+    <t>Antonio 1</t>
+  </si>
+  <si>
+    <t>Steele LEI (A)</t>
+  </si>
+  <si>
+    <t>3,175,193</t>
+  </si>
+  <si>
+    <t>1095</t>
+  </si>
+  <si>
+    <t>Veltman LEI (A)</t>
+  </si>
+  <si>
+    <t>Carson SOU (A)</t>
+  </si>
+  <si>
+    <t>Pinnock 1</t>
+  </si>
+  <si>
+    <t>Ødegaard BUR (H)</t>
+  </si>
+  <si>
+    <t>620,701</t>
+  </si>
+  <si>
+    <t>1274</t>
+  </si>
+  <si>
+    <t>Højbjerg CHE (A)</t>
+  </si>
+  <si>
+    <t>947,342</t>
+  </si>
+  <si>
+    <t>1239</t>
+  </si>
+  <si>
+    <t>Gabriel BUR (H)</t>
+  </si>
+  <si>
+    <t>Coutinho 3</t>
+  </si>
+  <si>
+    <t>Martinelli BUR (H)</t>
+  </si>
+  <si>
+    <t>Ward BHA (H)</t>
+  </si>
+  <si>
+    <t>747,302</t>
+  </si>
+  <si>
+    <t>1259</t>
+  </si>
+  <si>
+    <t>Jota CRY (A)$ captain</t>
+  </si>
+  <si>
+    <t>416,379</t>
+  </si>
+  <si>
+    <t>1302</t>
+  </si>
+  <si>
+    <t>Rüdiger TOT (H)</t>
+  </si>
+  <si>
+    <t>Robertson CRY (A)</t>
+  </si>
+  <si>
+    <t>Ederson SOU (A)</t>
+  </si>
+  <si>
+    <t>Alonso TOT (H)</t>
+  </si>
+  <si>
+    <t>Lucas Moura CHE (A)</t>
+  </si>
+  <si>
+    <t>548,141</t>
+  </si>
+  <si>
+    <t>Alisson CRY (A)</t>
+  </si>
+  <si>
+    <t>Fred 1</t>
+  </si>
+  <si>
+    <t>1,261,174</t>
+  </si>
+  <si>
+    <t>Laporte SOU (A)</t>
+  </si>
+  <si>
+    <t>van Dijk CRY (A)</t>
+  </si>
+  <si>
+    <t>Sterling SOU (A)</t>
+  </si>
+  <si>
+    <t>Matip CRY (A)</t>
+  </si>
+  <si>
+    <t>2,039,848</t>
+  </si>
+  <si>
+    <t>1160</t>
+  </si>
+  <si>
+    <t>de Gea 1</t>
+  </si>
+  <si>
+    <t>Lamptey LEI (A)</t>
+  </si>
+  <si>
+    <t>728,349</t>
+  </si>
+  <si>
+    <t>Sá 1</t>
+  </si>
+  <si>
+    <t>Tomiyasu BUR (H)</t>
+  </si>
+  <si>
+    <t>Soucek 1</t>
+  </si>
+  <si>
+    <t>1,159,663</t>
+  </si>
+  <si>
+    <t>Fernandes 2$ captain</t>
+  </si>
+  <si>
+    <t>1,235,967</t>
+  </si>
+  <si>
+    <t>1215</t>
+  </si>
+  <si>
+    <t>Lowton ARS (A), WAT (H)</t>
+  </si>
+  <si>
+    <t>Obafemi MCI (H)</t>
+  </si>
+  <si>
+    <t>658,720</t>
+  </si>
+  <si>
+    <t>1269</t>
+  </si>
+  <si>
+    <t>136,263</t>
+  </si>
+  <si>
+    <t>Amartey BHA (H)</t>
+  </si>
+  <si>
+    <t>Bissouma LEI (A)</t>
+  </si>
+  <si>
+    <t>458,971</t>
+  </si>
+  <si>
+    <t>1296</t>
+  </si>
+  <si>
+    <t>Foden SOU (A)$ captain</t>
+  </si>
+  <si>
+    <t>Digne 9</t>
+  </si>
+  <si>
+    <t>110,783</t>
+  </si>
+  <si>
+    <t>Trossard LEI (A)</t>
+  </si>
+  <si>
+    <t>145,619</t>
+  </si>
+  <si>
+    <t>Saka BUR (H)</t>
+  </si>
+  <si>
+    <t>604,536</t>
+  </si>
+  <si>
+    <t>Jiménez 0</t>
+  </si>
+  <si>
+    <t>João Pedro 4, BUR (A)$ captain</t>
+  </si>
+  <si>
+    <t>Williams 7</t>
+  </si>
+  <si>
+    <t>334,863</t>
+  </si>
+  <si>
+    <t>1317</t>
+  </si>
+  <si>
+    <t>Mendy TOT (H)</t>
+  </si>
+  <si>
+    <t>Townsend 1</t>
+  </si>
+  <si>
+    <t>Aubameyang BUR (H)$ captain</t>
+  </si>
+  <si>
+    <t>5,681,113</t>
+  </si>
+  <si>
+    <t>948</t>
+  </si>
+  <si>
+    <t>Cash 5</t>
+  </si>
+  <si>
+    <t>268,838</t>
+  </si>
+  <si>
+    <t>1330</t>
+  </si>
+  <si>
+    <t>Douglas Luiz 3</t>
+  </si>
+  <si>
+    <t>30,932</t>
+  </si>
+  <si>
+    <t>Gündogan SOU (A)</t>
+  </si>
+  <si>
+    <t>639,001</t>
+  </si>
+  <si>
+    <t>Calvert-Lewin 1</t>
+  </si>
+  <si>
+    <t>Keane 0</t>
+  </si>
+  <si>
+    <t>Ramsey 3</t>
+  </si>
+  <si>
+    <t>87,389</t>
+  </si>
+  <si>
+    <t>1385</t>
+  </si>
+  <si>
+    <t>83,965</t>
+  </si>
+  <si>
+    <t>Burn LEI (A)</t>
+  </si>
+  <si>
+    <t>189,181</t>
+  </si>
+  <si>
+    <t>De Bruyne SOU (A)$ captain</t>
+  </si>
+  <si>
+    <t>Lacazette BUR (H)</t>
+  </si>
+  <si>
+    <t>74,868</t>
+  </si>
+  <si>
+    <t>1391</t>
+  </si>
+  <si>
+    <t>99,311</t>
+  </si>
+  <si>
+    <t>1380</t>
+  </si>
+  <si>
+    <t>Bernardo 1</t>
+  </si>
+  <si>
+    <t>Bowen 2</t>
+  </si>
+  <si>
+    <t>Coufal 6</t>
+  </si>
+  <si>
+    <t>Raphinha 2</t>
+  </si>
+  <si>
+    <t>Foden 1</t>
+  </si>
+  <si>
+    <t>Dalot 6</t>
+  </si>
+  <si>
+    <t>Varane 6</t>
+  </si>
+  <si>
+    <t>Fernandes 3</t>
+  </si>
+  <si>
+    <t>Mbeumo 5</t>
+  </si>
+  <si>
+    <t>Dias 1</t>
+  </si>
+  <si>
+    <t>Manquillo 4</t>
+  </si>
+  <si>
+    <t>Jansson 0</t>
+  </si>
+  <si>
+    <t>Toney 6</t>
+  </si>
+  <si>
+    <t>Fred 3</t>
+  </si>
+  <si>
+    <t>Laporte 1</t>
+  </si>
+  <si>
+    <t>Sterling 1</t>
+  </si>
+  <si>
+    <t>Fernandes 6$ captain</t>
+  </si>
+  <si>
+    <t>Foden 2$ captain</t>
+  </si>
+  <si>
+    <t>Greenwood 3</t>
+  </si>
+  <si>
+    <t>Gündogan 0</t>
+  </si>
+  <si>
+    <t>Dawson 2</t>
+  </si>
+  <si>
+    <t>Harrison 2</t>
+  </si>
+  <si>
+    <t>Bernardo 2</t>
+  </si>
+  <si>
+    <t>De Bruyne 5</t>
+  </si>
+  <si>
+    <t>Foden 2</t>
+  </si>
+  <si>
+    <t>Ederson 2</t>
+  </si>
+  <si>
+    <t>Laporte 8</t>
+  </si>
+  <si>
+    <t>Foden 4$ captain</t>
+  </si>
+  <si>
+    <t>De Bruyne 10$ captain</t>
   </si>
 </sst>
 </file>
@@ -11192,22 +11723,22 @@
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="16.234375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.11328125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="18.55078125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="14.05859375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.89453125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.3828125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.8203125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="23.8203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.8203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="21.28125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.69921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="21.0625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="25.60546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="25.60546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="28.6953125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="19.2265625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="19.69921875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="17.31640625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
@@ -11333,13 +11864,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>829</v>
+        <v>861</v>
       </c>
       <c r="D2" t="s">
-        <v>2561</v>
+        <v>2670</v>
       </c>
       <c r="E2" t="s">
-        <v>2560</v>
+        <v>2669</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -11351,40 +11882,40 @@
         <v>269</v>
       </c>
       <c r="T2" t="s">
-        <v>1184</v>
+        <v>2656</v>
       </c>
       <c r="U2" t="s">
-        <v>2078</v>
+        <v>2657</v>
       </c>
       <c r="V2" t="s">
-        <v>1945</v>
+        <v>2658</v>
       </c>
       <c r="W2" t="s">
-        <v>1212</v>
+        <v>1929</v>
       </c>
       <c r="X2" t="s">
-        <v>2037</v>
+        <v>2660</v>
       </c>
       <c r="Y2" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="Z2" t="s">
-        <v>2337</v>
+        <v>2826</v>
       </c>
       <c r="AA2" t="s">
-        <v>2444</v>
+        <v>2662</v>
       </c>
       <c r="AB2" t="s">
-        <v>2558</v>
+        <v>2663</v>
       </c>
       <c r="AC2" t="s">
-        <v>2496</v>
+        <v>2664</v>
       </c>
       <c r="AD2" t="s">
-        <v>2559</v>
+        <v>2665</v>
       </c>
       <c r="AE2" t="s">
-        <v>2035</v>
+        <v>2076</v>
       </c>
       <c r="AF2" t="s">
         <v>1974</v>
@@ -11393,16 +11924,16 @@
         <v>940</v>
       </c>
       <c r="AH2" t="s">
-        <v>2039</v>
+        <v>2667</v>
       </c>
       <c r="AI2" t="s">
-        <v>829</v>
+        <v>861</v>
       </c>
       <c r="AJ2" t="s">
-        <v>2561</v>
+        <v>2670</v>
       </c>
       <c r="AK2" t="s">
-        <v>2560</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -11413,16 +11944,16 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>276</v>
+        <v>2075</v>
       </c>
       <c r="D3" t="s">
-        <v>2563</v>
+        <v>2117</v>
       </c>
       <c r="E3" t="s">
-        <v>2562</v>
+        <v>2676</v>
       </c>
       <c r="G3" t="s">
-        <v>672</v>
+        <v>653</v>
       </c>
       <c r="R3" t="s">
         <v>714</v>
@@ -11431,40 +11962,40 @@
         <v>713</v>
       </c>
       <c r="T3" t="s">
-        <v>1184</v>
+        <v>2076</v>
       </c>
       <c r="U3" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="V3" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="W3" t="s">
-        <v>2082</v>
+        <v>791</v>
       </c>
       <c r="X3" t="s">
         <v>679</v>
       </c>
       <c r="Y3" t="s">
-        <v>2041</v>
+        <v>2672</v>
       </c>
       <c r="Z3" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="AA3" t="s">
-        <v>1988</v>
+        <v>2674</v>
       </c>
       <c r="AB3" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="AC3" t="s">
-        <v>2438</v>
+        <v>2664</v>
       </c>
       <c r="AD3" t="s">
         <v>2445</v>
       </c>
       <c r="AE3" t="s">
-        <v>1989</v>
+        <v>2675</v>
       </c>
       <c r="AF3" t="s">
         <v>1974</v>
@@ -11476,13 +12007,13 @@
         <v>940</v>
       </c>
       <c r="AI3" t="s">
-        <v>276</v>
+        <v>2075</v>
       </c>
       <c r="AJ3" t="s">
-        <v>2563</v>
+        <v>2117</v>
       </c>
       <c r="AK3" t="s">
-        <v>2562</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -11493,16 +12024,16 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>778</v>
+        <v>653</v>
       </c>
       <c r="D4" t="s">
-        <v>2566</v>
+        <v>2684</v>
       </c>
       <c r="E4" t="s">
-        <v>2565</v>
+        <v>2683</v>
       </c>
       <c r="G4" t="s">
-        <v>653</v>
+        <v>578</v>
       </c>
       <c r="R4" t="s">
         <v>723</v>
@@ -11511,58 +12042,58 @@
         <v>722</v>
       </c>
       <c r="T4" t="s">
-        <v>1184</v>
+        <v>2677</v>
       </c>
       <c r="U4" t="s">
-        <v>825</v>
+        <v>2806</v>
       </c>
       <c r="V4" t="s">
-        <v>2564</v>
+        <v>2667</v>
       </c>
       <c r="W4" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X4" t="s">
-        <v>1988</v>
+        <v>2807</v>
       </c>
       <c r="Y4" t="s">
-        <v>2344</v>
+        <v>2678</v>
       </c>
       <c r="Z4" t="s">
-        <v>2455</v>
+        <v>2827</v>
       </c>
       <c r="AA4" t="s">
-        <v>1372</v>
+        <v>2828</v>
       </c>
       <c r="AB4" t="s">
+        <v>2323</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>2664</v>
+      </c>
+      <c r="AD4" t="s">
         <v>939</v>
       </c>
-      <c r="AC4" t="s">
-        <v>2438</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>2345</v>
-      </c>
       <c r="AE4" t="s">
-        <v>693</v>
+        <v>2076</v>
       </c>
       <c r="AF4" t="s">
-        <v>750</v>
+        <v>2674</v>
       </c>
       <c r="AG4" t="s">
-        <v>2039</v>
+        <v>2681</v>
       </c>
       <c r="AH4" t="s">
-        <v>2041</v>
+        <v>2682</v>
       </c>
       <c r="AI4" t="s">
-        <v>778</v>
+        <v>653</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2566</v>
+        <v>2684</v>
       </c>
       <c r="AK4" t="s">
-        <v>2565</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -11573,16 +12104,16 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>305</v>
+        <v>2002</v>
       </c>
       <c r="D5" t="s">
-        <v>2568</v>
+        <v>2694</v>
       </c>
       <c r="E5" t="s">
-        <v>2567</v>
+        <v>2693</v>
       </c>
       <c r="G5" t="s">
-        <v>653</v>
+        <v>452</v>
       </c>
       <c r="R5" t="s">
         <v>583</v>
@@ -11591,58 +12122,58 @@
         <v>731</v>
       </c>
       <c r="T5" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U5" t="s">
-        <v>2434</v>
+        <v>1929</v>
       </c>
       <c r="V5" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="W5" t="s">
-        <v>2435</v>
+        <v>2685</v>
       </c>
       <c r="X5" t="s">
-        <v>2455</v>
+        <v>2667</v>
       </c>
       <c r="Y5" t="s">
-        <v>2341</v>
+        <v>2827</v>
       </c>
       <c r="Z5" t="s">
-        <v>2348</v>
+        <v>2805</v>
       </c>
       <c r="AA5" t="s">
-        <v>2436</v>
+        <v>2686</v>
       </c>
       <c r="AB5" t="s">
-        <v>2439</v>
+        <v>2807</v>
       </c>
       <c r="AC5" t="s">
-        <v>939</v>
+        <v>2687</v>
       </c>
       <c r="AD5" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AE5" t="s">
-        <v>2091</v>
+        <v>2689</v>
       </c>
       <c r="AF5" t="s">
-        <v>2092</v>
+        <v>2690</v>
       </c>
       <c r="AG5" t="s">
-        <v>750</v>
+        <v>2178</v>
       </c>
       <c r="AH5" t="s">
-        <v>685</v>
+        <v>2809</v>
       </c>
       <c r="AI5" t="s">
-        <v>305</v>
+        <v>2002</v>
       </c>
       <c r="AJ5" t="s">
-        <v>2568</v>
+        <v>2694</v>
       </c>
       <c r="AK5" t="s">
-        <v>2567</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -11653,16 +12184,16 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>299</v>
+        <v>2167</v>
       </c>
       <c r="D6" t="s">
-        <v>1954</v>
+        <v>2705</v>
       </c>
       <c r="E6" t="s">
-        <v>2573</v>
+        <v>2704</v>
       </c>
       <c r="G6" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R6" t="s">
         <v>495</v>
@@ -11671,58 +12202,58 @@
         <v>1925</v>
       </c>
       <c r="T6" t="s">
-        <v>2569</v>
+        <v>2695</v>
       </c>
       <c r="U6" t="s">
-        <v>2485</v>
+        <v>2657</v>
       </c>
       <c r="V6" t="s">
-        <v>2443</v>
+        <v>2696</v>
       </c>
       <c r="W6" t="s">
-        <v>2570</v>
+        <v>2810</v>
       </c>
       <c r="X6" t="s">
-        <v>2571</v>
+        <v>1929</v>
       </c>
       <c r="Y6" t="s">
-        <v>1461</v>
+        <v>2698</v>
       </c>
       <c r="Z6" t="s">
-        <v>2462</v>
+        <v>2811</v>
       </c>
       <c r="AA6" t="s">
-        <v>2572</v>
+        <v>2699</v>
       </c>
       <c r="AB6" t="s">
-        <v>1938</v>
+        <v>2323</v>
       </c>
       <c r="AC6" t="s">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="AD6" t="s">
         <v>939</v>
       </c>
       <c r="AE6" t="s">
-        <v>1154</v>
+        <v>2701</v>
       </c>
       <c r="AF6" t="s">
-        <v>2528</v>
+        <v>2812</v>
       </c>
       <c r="AG6" t="s">
-        <v>1212</v>
+        <v>2702</v>
       </c>
       <c r="AH6" t="s">
-        <v>2078</v>
+        <v>2703</v>
       </c>
       <c r="AI6" t="s">
-        <v>299</v>
+        <v>2167</v>
       </c>
       <c r="AJ6" t="s">
-        <v>1954</v>
+        <v>2705</v>
       </c>
       <c r="AK6" t="s">
-        <v>2573</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -11733,16 +12264,16 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>1912</v>
+        <v>2002</v>
       </c>
       <c r="D7" t="s">
-        <v>2575</v>
+        <v>2713</v>
       </c>
       <c r="E7" t="s">
-        <v>2574</v>
+        <v>2712</v>
       </c>
       <c r="G7" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R7" t="s">
         <v>432</v>
@@ -11751,58 +12282,58 @@
         <v>435</v>
       </c>
       <c r="T7" t="s">
-        <v>2035</v>
+        <v>2656</v>
       </c>
       <c r="U7" t="s">
-        <v>687</v>
+        <v>1193</v>
       </c>
       <c r="V7" t="s">
-        <v>2452</v>
+        <v>2707</v>
       </c>
       <c r="W7" t="s">
-        <v>1190</v>
+        <v>2708</v>
       </c>
       <c r="X7" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Y7" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Z7" t="s">
-        <v>1988</v>
+        <v>2674</v>
       </c>
       <c r="AA7" t="s">
-        <v>2344</v>
+        <v>2709</v>
       </c>
       <c r="AB7" t="s">
-        <v>2438</v>
+        <v>2664</v>
       </c>
       <c r="AC7" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AD7" t="s">
         <v>2445</v>
       </c>
       <c r="AE7" t="s">
-        <v>804</v>
+        <v>2711</v>
       </c>
       <c r="AF7" t="s">
         <v>2101</v>
       </c>
       <c r="AG7" t="s">
-        <v>750</v>
+        <v>2681</v>
       </c>
       <c r="AH7" t="s">
         <v>1974</v>
       </c>
       <c r="AI7" t="s">
-        <v>1912</v>
+        <v>2002</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2575</v>
+        <v>2713</v>
       </c>
       <c r="AK7" t="s">
-        <v>2574</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -11813,16 +12344,16 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>703</v>
+        <v>1791</v>
       </c>
       <c r="D8" t="s">
-        <v>2578</v>
+        <v>2719</v>
       </c>
       <c r="E8" t="s">
-        <v>2577</v>
+        <v>2718</v>
       </c>
       <c r="G8" t="s">
-        <v>906</v>
+        <v>653</v>
       </c>
       <c r="R8" t="s">
         <v>573</v>
@@ -11831,58 +12362,58 @@
         <v>758</v>
       </c>
       <c r="T8" t="s">
-        <v>1184</v>
+        <v>2076</v>
       </c>
       <c r="U8" t="s">
-        <v>2576</v>
+        <v>2714</v>
       </c>
       <c r="V8" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="W8" t="s">
-        <v>755</v>
+        <v>2685</v>
       </c>
       <c r="X8" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Y8" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="Z8" t="s">
-        <v>2437</v>
+        <v>2687</v>
       </c>
       <c r="AA8" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="AB8" t="s">
-        <v>1938</v>
+        <v>2323</v>
       </c>
       <c r="AC8" t="s">
-        <v>2445</v>
+        <v>939</v>
       </c>
       <c r="AD8" t="s">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="AE8" t="s">
         <v>1832</v>
       </c>
       <c r="AF8" t="s">
-        <v>825</v>
+        <v>2806</v>
       </c>
       <c r="AG8" t="s">
-        <v>2054</v>
+        <v>2716</v>
       </c>
       <c r="AH8" t="s">
-        <v>2055</v>
+        <v>2717</v>
       </c>
       <c r="AI8" t="s">
-        <v>703</v>
+        <v>1791</v>
       </c>
       <c r="AJ8" t="s">
-        <v>2578</v>
+        <v>2719</v>
       </c>
       <c r="AK8" t="s">
-        <v>2577</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -11893,16 +12424,16 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>874</v>
+        <v>2002</v>
       </c>
       <c r="D9" t="s">
-        <v>2580</v>
+        <v>2722</v>
       </c>
       <c r="E9" t="s">
-        <v>2579</v>
+        <v>2721</v>
       </c>
       <c r="G9" t="s">
-        <v>672</v>
+        <v>653</v>
       </c>
       <c r="R9" t="s">
         <v>566</v>
@@ -11911,58 +12442,58 @@
         <v>763</v>
       </c>
       <c r="T9" t="s">
-        <v>1184</v>
+        <v>2076</v>
       </c>
       <c r="U9" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="V9" t="s">
-        <v>687</v>
+        <v>1193</v>
       </c>
       <c r="W9" t="s">
-        <v>750</v>
+        <v>2681</v>
       </c>
       <c r="X9" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="Y9" t="s">
-        <v>2055</v>
+        <v>2717</v>
       </c>
       <c r="Z9" t="s">
-        <v>2455</v>
+        <v>2678</v>
       </c>
       <c r="AA9" t="s">
-        <v>1205</v>
+        <v>2720</v>
       </c>
       <c r="AB9" t="s">
-        <v>2438</v>
+        <v>2664</v>
       </c>
       <c r="AC9" t="s">
         <v>2445</v>
       </c>
       <c r="AD9" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AE9" t="s">
-        <v>2461</v>
+        <v>2689</v>
       </c>
       <c r="AF9" t="s">
-        <v>2344</v>
+        <v>2709</v>
       </c>
       <c r="AG9" t="s">
         <v>478</v>
       </c>
       <c r="AH9" t="s">
-        <v>1380</v>
+        <v>2814</v>
       </c>
       <c r="AI9" t="s">
-        <v>874</v>
+        <v>2002</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2580</v>
+        <v>2722</v>
       </c>
       <c r="AK9" t="s">
-        <v>2579</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -11973,16 +12504,16 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>1224</v>
+        <v>2002</v>
       </c>
       <c r="D10" t="s">
-        <v>1978</v>
+        <v>2728</v>
       </c>
       <c r="E10" t="s">
-        <v>2583</v>
+        <v>2727</v>
       </c>
       <c r="G10" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R10" t="s">
         <v>768</v>
@@ -11991,58 +12522,58 @@
         <v>285</v>
       </c>
       <c r="T10" t="s">
-        <v>2433</v>
+        <v>2689</v>
       </c>
       <c r="U10" t="s">
-        <v>2452</v>
+        <v>2723</v>
       </c>
       <c r="V10" t="s">
-        <v>2443</v>
+        <v>1929</v>
       </c>
       <c r="W10" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X10" t="s">
-        <v>2454</v>
+        <v>2805</v>
       </c>
       <c r="Y10" t="s">
-        <v>2341</v>
+        <v>2724</v>
       </c>
       <c r="Z10" t="s">
-        <v>2489</v>
+        <v>2725</v>
       </c>
       <c r="AA10" t="s">
-        <v>2581</v>
+        <v>2674</v>
       </c>
       <c r="AB10" t="s">
-        <v>2455</v>
+        <v>682</v>
       </c>
       <c r="AC10" t="s">
         <v>939</v>
       </c>
       <c r="AD10" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AE10" t="s">
-        <v>1184</v>
+        <v>2726</v>
       </c>
       <c r="AF10" t="s">
-        <v>2352</v>
+        <v>679</v>
       </c>
       <c r="AG10" t="s">
-        <v>2582</v>
+        <v>2815</v>
       </c>
       <c r="AH10" t="s">
-        <v>2359</v>
+        <v>2707</v>
       </c>
       <c r="AI10" t="s">
-        <v>1224</v>
+        <v>2002</v>
       </c>
       <c r="AJ10" t="s">
-        <v>1978</v>
+        <v>2728</v>
       </c>
       <c r="AK10" t="s">
-        <v>2583</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -12053,16 +12584,16 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>297</v>
+        <v>2075</v>
       </c>
       <c r="D11" t="s">
-        <v>2586</v>
+        <v>2731</v>
       </c>
       <c r="E11" t="s">
-        <v>2585</v>
+        <v>2730</v>
       </c>
       <c r="G11" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R11" t="s">
         <v>773</v>
@@ -12071,58 +12602,58 @@
         <v>772</v>
       </c>
       <c r="T11" t="s">
-        <v>1184</v>
+        <v>2076</v>
       </c>
       <c r="U11" t="s">
-        <v>2078</v>
+        <v>2657</v>
       </c>
       <c r="V11" t="s">
-        <v>1212</v>
+        <v>1929</v>
       </c>
       <c r="W11" t="s">
-        <v>2452</v>
+        <v>2707</v>
       </c>
       <c r="X11" t="s">
-        <v>755</v>
+        <v>2672</v>
       </c>
       <c r="Y11" t="s">
-        <v>2037</v>
+        <v>2729</v>
       </c>
       <c r="Z11" t="s">
-        <v>2348</v>
+        <v>2698</v>
       </c>
       <c r="AA11" t="s">
-        <v>2584</v>
+        <v>2807</v>
       </c>
       <c r="AB11" t="s">
-        <v>2438</v>
+        <v>2098</v>
       </c>
       <c r="AC11" t="s">
-        <v>2352</v>
+        <v>2816</v>
       </c>
       <c r="AD11" t="s">
-        <v>2547</v>
+        <v>2664</v>
       </c>
       <c r="AE11" t="s">
         <v>1363</v>
       </c>
       <c r="AF11" t="s">
-        <v>2041</v>
+        <v>1193</v>
       </c>
       <c r="AG11" t="s">
-        <v>2344</v>
+        <v>2709</v>
       </c>
       <c r="AH11" t="s">
-        <v>687</v>
+        <v>2716</v>
       </c>
       <c r="AI11" t="s">
-        <v>297</v>
+        <v>2075</v>
       </c>
       <c r="AJ11" t="s">
-        <v>2586</v>
+        <v>2731</v>
       </c>
       <c r="AK11" t="s">
-        <v>2585</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -12133,13 +12664,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>912</v>
+        <v>2034</v>
       </c>
       <c r="D12" t="s">
-        <v>2588</v>
+        <v>2142</v>
       </c>
       <c r="E12" t="s">
-        <v>2587</v>
+        <v>2737</v>
       </c>
       <c r="G12" t="s">
         <v>452</v>
@@ -12151,58 +12682,58 @@
         <v>289</v>
       </c>
       <c r="T12" t="s">
-        <v>2060</v>
+        <v>2656</v>
       </c>
       <c r="U12" t="s">
-        <v>2435</v>
+        <v>1193</v>
       </c>
       <c r="V12" t="s">
-        <v>2443</v>
+        <v>2732</v>
       </c>
       <c r="W12" t="s">
-        <v>2452</v>
+        <v>2733</v>
       </c>
       <c r="X12" t="s">
-        <v>687</v>
+        <v>2707</v>
       </c>
       <c r="Y12" t="s">
-        <v>1988</v>
+        <v>2672</v>
       </c>
       <c r="Z12" t="s">
-        <v>2455</v>
+        <v>2826</v>
       </c>
       <c r="AA12" t="s">
-        <v>2037</v>
+        <v>2678</v>
       </c>
       <c r="AB12" t="s">
-        <v>2436</v>
+        <v>2098</v>
       </c>
       <c r="AC12" t="s">
-        <v>2456</v>
+        <v>2688</v>
       </c>
       <c r="AD12" t="s">
         <v>939</v>
       </c>
       <c r="AE12" t="s">
-        <v>2035</v>
+        <v>2829</v>
       </c>
       <c r="AF12" t="s">
-        <v>2564</v>
+        <v>2735</v>
       </c>
       <c r="AG12" t="s">
-        <v>2041</v>
+        <v>2736</v>
       </c>
       <c r="AH12" t="s">
-        <v>1971</v>
+        <v>2674</v>
       </c>
       <c r="AI12" t="s">
-        <v>912</v>
+        <v>2034</v>
       </c>
       <c r="AJ12" t="s">
-        <v>2588</v>
+        <v>2142</v>
       </c>
       <c r="AK12" t="s">
-        <v>2587</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -12213,16 +12744,16 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>299</v>
+        <v>2075</v>
       </c>
       <c r="D13" t="s">
-        <v>2591</v>
+        <v>1973</v>
       </c>
       <c r="E13" t="s">
-        <v>2590</v>
+        <v>2740</v>
       </c>
       <c r="G13" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R13" t="s">
         <v>512</v>
@@ -12231,58 +12762,58 @@
         <v>291</v>
       </c>
       <c r="T13" t="s">
-        <v>2367</v>
+        <v>2738</v>
       </c>
       <c r="U13" t="s">
-        <v>1212</v>
+        <v>2732</v>
       </c>
       <c r="V13" t="s">
-        <v>2078</v>
+        <v>2657</v>
       </c>
       <c r="W13" t="s">
-        <v>2435</v>
+        <v>1929</v>
       </c>
       <c r="X13" t="s">
-        <v>2589</v>
+        <v>2685</v>
       </c>
       <c r="Y13" t="s">
-        <v>2341</v>
+        <v>2724</v>
       </c>
       <c r="Z13" t="s">
-        <v>2495</v>
+        <v>2817</v>
       </c>
       <c r="AA13" t="s">
-        <v>1205</v>
+        <v>2805</v>
       </c>
       <c r="AB13" t="s">
-        <v>2547</v>
+        <v>2811</v>
       </c>
       <c r="AC13" t="s">
-        <v>2456</v>
+        <v>2688</v>
       </c>
       <c r="AD13" t="s">
         <v>939</v>
       </c>
       <c r="AE13" t="s">
-        <v>2035</v>
+        <v>2656</v>
       </c>
       <c r="AF13" t="s">
-        <v>2054</v>
+        <v>2816</v>
       </c>
       <c r="AG13" t="s">
-        <v>2344</v>
+        <v>2720</v>
       </c>
       <c r="AH13" t="s">
-        <v>2337</v>
+        <v>2815</v>
       </c>
       <c r="AI13" t="s">
-        <v>299</v>
+        <v>2075</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2591</v>
+        <v>1973</v>
       </c>
       <c r="AK13" t="s">
-        <v>2590</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -12293,13 +12824,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>301</v>
+        <v>1923</v>
       </c>
       <c r="D14" t="s">
-        <v>2593</v>
+        <v>2746</v>
       </c>
       <c r="E14" t="s">
-        <v>2592</v>
+        <v>2745</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -12311,58 +12842,58 @@
         <v>796</v>
       </c>
       <c r="T14" t="s">
-        <v>2461</v>
+        <v>2677</v>
       </c>
       <c r="U14" t="s">
-        <v>2115</v>
+        <v>2685</v>
       </c>
       <c r="V14" t="s">
-        <v>2371</v>
+        <v>2830</v>
       </c>
       <c r="W14" t="s">
-        <v>942</v>
+        <v>2742</v>
       </c>
       <c r="X14" t="s">
-        <v>2426</v>
+        <v>2667</v>
       </c>
       <c r="Y14" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="Z14" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AA14" t="s">
-        <v>2061</v>
+        <v>2819</v>
       </c>
       <c r="AB14" t="s">
-        <v>2439</v>
+        <v>2807</v>
       </c>
       <c r="AC14" t="s">
-        <v>1938</v>
+        <v>2700</v>
       </c>
       <c r="AD14" t="s">
-        <v>2496</v>
+        <v>2323</v>
       </c>
       <c r="AE14" t="s">
-        <v>693</v>
+        <v>2689</v>
       </c>
       <c r="AF14" t="s">
-        <v>2039</v>
+        <v>2744</v>
       </c>
       <c r="AG14" t="s">
-        <v>2054</v>
+        <v>2665</v>
       </c>
       <c r="AH14" t="s">
         <v>767</v>
       </c>
       <c r="AI14" t="s">
-        <v>301</v>
+        <v>1923</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2593</v>
+        <v>2746</v>
       </c>
       <c r="AK14" t="s">
-        <v>2592</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -12373,16 +12904,16 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>1831</v>
+        <v>2088</v>
       </c>
       <c r="D15" t="s">
         <v>2595</v>
       </c>
       <c r="E15" t="s">
-        <v>2594</v>
+        <v>2749</v>
       </c>
       <c r="G15" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R15" t="s">
         <v>801</v>
@@ -12391,58 +12922,58 @@
         <v>800</v>
       </c>
       <c r="T15" t="s">
-        <v>2433</v>
+        <v>2656</v>
       </c>
       <c r="U15" t="s">
-        <v>2479</v>
+        <v>2735</v>
       </c>
       <c r="V15" t="s">
-        <v>2443</v>
+        <v>2657</v>
       </c>
       <c r="W15" t="s">
-        <v>1212</v>
+        <v>1929</v>
       </c>
       <c r="X15" t="s">
-        <v>2426</v>
+        <v>2805</v>
       </c>
       <c r="Y15" t="s">
-        <v>2436</v>
+        <v>2807</v>
       </c>
       <c r="Z15" t="s">
-        <v>2455</v>
+        <v>2736</v>
       </c>
       <c r="AA15" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AB15" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AC15" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AD15" t="s">
-        <v>2445</v>
+        <v>2098</v>
       </c>
       <c r="AE15" t="s">
-        <v>2035</v>
+        <v>581</v>
       </c>
       <c r="AF15" t="s">
-        <v>2341</v>
+        <v>2748</v>
       </c>
       <c r="AG15" t="s">
         <v>1176</v>
       </c>
       <c r="AH15" t="s">
-        <v>2078</v>
+        <v>2678</v>
       </c>
       <c r="AI15" t="s">
-        <v>1831</v>
+        <v>2088</v>
       </c>
       <c r="AJ15" t="s">
         <v>2595</v>
       </c>
       <c r="AK15" t="s">
-        <v>2594</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -12453,16 +12984,16 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>912</v>
+        <v>1791</v>
       </c>
       <c r="D16" t="s">
-        <v>2361</v>
+        <v>1954</v>
       </c>
       <c r="E16" t="s">
-        <v>2596</v>
+        <v>2753</v>
       </c>
       <c r="G16" t="s">
-        <v>653</v>
+        <v>578</v>
       </c>
       <c r="R16" t="s">
         <v>406</v>
@@ -12471,58 +13002,58 @@
         <v>296</v>
       </c>
       <c r="T16" t="s">
-        <v>1184</v>
+        <v>2750</v>
       </c>
       <c r="U16" t="s">
-        <v>2062</v>
+        <v>2723</v>
       </c>
       <c r="V16" t="s">
-        <v>1212</v>
+        <v>1193</v>
       </c>
       <c r="W16" t="s">
-        <v>687</v>
+        <v>2657</v>
       </c>
       <c r="X16" t="s">
-        <v>1988</v>
+        <v>2751</v>
       </c>
       <c r="Y16" t="s">
-        <v>2444</v>
+        <v>2826</v>
       </c>
       <c r="Z16" t="s">
-        <v>2337</v>
+        <v>2686</v>
       </c>
       <c r="AA16" t="s">
-        <v>2344</v>
+        <v>2811</v>
       </c>
       <c r="AB16" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AC16" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD16" t="s">
         <v>2119</v>
       </c>
-      <c r="AD16" t="s">
-        <v>2345</v>
-      </c>
       <c r="AE16" t="s">
-        <v>2120</v>
+        <v>2076</v>
       </c>
       <c r="AF16" t="s">
         <v>1974</v>
       </c>
       <c r="AG16" t="s">
-        <v>2377</v>
+        <v>2674</v>
       </c>
       <c r="AH16" t="s">
-        <v>2063</v>
+        <v>1307</v>
       </c>
       <c r="AI16" t="s">
-        <v>912</v>
+        <v>1791</v>
       </c>
       <c r="AJ16" t="s">
-        <v>2361</v>
+        <v>1954</v>
       </c>
       <c r="AK16" t="s">
-        <v>2596</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -12533,16 +13064,16 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>278</v>
+        <v>2067</v>
       </c>
       <c r="D17" t="s">
-        <v>2598</v>
+        <v>2756</v>
       </c>
       <c r="E17" t="s">
-        <v>2597</v>
+        <v>2755</v>
       </c>
       <c r="G17" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R17" t="s">
         <v>348</v>
@@ -12551,58 +13082,58 @@
         <v>298</v>
       </c>
       <c r="T17" t="s">
-        <v>2433</v>
+        <v>2656</v>
       </c>
       <c r="U17" t="s">
-        <v>2452</v>
+        <v>2707</v>
       </c>
       <c r="V17" t="s">
-        <v>2454</v>
+        <v>1929</v>
       </c>
       <c r="W17" t="s">
-        <v>2435</v>
+        <v>2657</v>
       </c>
       <c r="X17" t="s">
-        <v>2443</v>
+        <v>2805</v>
       </c>
       <c r="Y17" t="s">
-        <v>2455</v>
+        <v>2820</v>
       </c>
       <c r="Z17" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AA17" t="s">
-        <v>2436</v>
+        <v>2828</v>
       </c>
       <c r="AB17" t="s">
-        <v>1938</v>
+        <v>2098</v>
       </c>
       <c r="AC17" t="s">
-        <v>2439</v>
+        <v>682</v>
       </c>
       <c r="AD17" t="s">
-        <v>939</v>
+        <v>2664</v>
       </c>
       <c r="AE17" t="s">
-        <v>2035</v>
+        <v>2076</v>
       </c>
       <c r="AF17" t="s">
-        <v>2341</v>
+        <v>2672</v>
       </c>
       <c r="AG17" t="s">
-        <v>2021</v>
+        <v>1974</v>
       </c>
       <c r="AH17" t="s">
-        <v>750</v>
+        <v>2751</v>
       </c>
       <c r="AI17" t="s">
-        <v>278</v>
+        <v>2067</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2598</v>
+        <v>2756</v>
       </c>
       <c r="AK17" t="s">
-        <v>2597</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -12613,13 +13144,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>1312</v>
+        <v>2002</v>
       </c>
       <c r="D18" t="s">
-        <v>2392</v>
+        <v>2760</v>
       </c>
       <c r="E18" t="s">
-        <v>2599</v>
+        <v>2759</v>
       </c>
       <c r="G18" t="s">
         <v>706</v>
@@ -12631,58 +13162,58 @@
         <v>813</v>
       </c>
       <c r="T18" t="s">
-        <v>693</v>
+        <v>2677</v>
       </c>
       <c r="U18" t="s">
-        <v>1212</v>
+        <v>2757</v>
       </c>
       <c r="V18" t="s">
-        <v>2435</v>
+        <v>1929</v>
       </c>
       <c r="W18" t="s">
-        <v>2078</v>
+        <v>2657</v>
       </c>
       <c r="X18" t="s">
-        <v>2426</v>
+        <v>2674</v>
       </c>
       <c r="Y18" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="Z18" t="s">
-        <v>2489</v>
+        <v>2811</v>
       </c>
       <c r="AA18" t="s">
-        <v>1988</v>
+        <v>2807</v>
       </c>
       <c r="AB18" t="s">
-        <v>2437</v>
+        <v>2687</v>
       </c>
       <c r="AC18" t="s">
-        <v>2352</v>
+        <v>2688</v>
       </c>
       <c r="AD18" t="s">
-        <v>2438</v>
+        <v>682</v>
       </c>
       <c r="AE18" t="s">
-        <v>2035</v>
+        <v>2656</v>
       </c>
       <c r="AF18" t="s">
-        <v>1190</v>
+        <v>2732</v>
       </c>
       <c r="AG18" t="s">
-        <v>2039</v>
+        <v>2667</v>
       </c>
       <c r="AH18" t="s">
         <v>812</v>
       </c>
       <c r="AI18" t="s">
-        <v>1312</v>
+        <v>2002</v>
       </c>
       <c r="AJ18" t="s">
-        <v>2392</v>
+        <v>2760</v>
       </c>
       <c r="AK18" t="s">
-        <v>2599</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -12693,16 +13224,16 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>1312</v>
+        <v>2077</v>
       </c>
       <c r="D19" t="s">
-        <v>2601</v>
+        <v>2261</v>
       </c>
       <c r="E19" t="s">
-        <v>2600</v>
+        <v>2761</v>
       </c>
       <c r="G19" t="s">
-        <v>452</v>
+        <v>706</v>
       </c>
       <c r="R19" t="s">
         <v>373</v>
@@ -12711,58 +13242,58 @@
         <v>818</v>
       </c>
       <c r="T19" t="s">
-        <v>2433</v>
+        <v>2656</v>
       </c>
       <c r="U19" t="s">
-        <v>825</v>
+        <v>2751</v>
       </c>
       <c r="V19" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="W19" t="s">
-        <v>2452</v>
+        <v>2830</v>
       </c>
       <c r="X19" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Y19" t="s">
-        <v>2125</v>
+        <v>2827</v>
       </c>
       <c r="Z19" t="s">
-        <v>2341</v>
+        <v>2807</v>
       </c>
       <c r="AA19" t="s">
-        <v>2489</v>
+        <v>2811</v>
       </c>
       <c r="AB19" t="s">
-        <v>2547</v>
+        <v>2805</v>
       </c>
       <c r="AC19" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AD19" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AE19" t="s">
-        <v>2035</v>
+        <v>581</v>
       </c>
       <c r="AF19" t="s">
-        <v>2426</v>
+        <v>2816</v>
       </c>
       <c r="AG19" t="s">
-        <v>2063</v>
+        <v>2806</v>
       </c>
       <c r="AH19" t="s">
         <v>1974</v>
       </c>
       <c r="AI19" t="s">
-        <v>1312</v>
+        <v>2077</v>
       </c>
       <c r="AJ19" t="s">
-        <v>2601</v>
+        <v>2261</v>
       </c>
       <c r="AK19" t="s">
-        <v>2600</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -12773,13 +13304,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>1209</v>
+        <v>2074</v>
       </c>
       <c r="D20" t="s">
-        <v>2603</v>
+        <v>2765</v>
       </c>
       <c r="E20" t="s">
-        <v>2602</v>
+        <v>2764</v>
       </c>
       <c r="G20" t="s">
         <v>452</v>
@@ -12791,58 +13322,58 @@
         <v>822</v>
       </c>
       <c r="T20" t="s">
-        <v>2433</v>
+        <v>581</v>
       </c>
       <c r="U20" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="V20" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="W20" t="s">
-        <v>2485</v>
+        <v>2685</v>
       </c>
       <c r="X20" t="s">
-        <v>2462</v>
+        <v>2827</v>
       </c>
       <c r="Y20" t="s">
-        <v>2341</v>
+        <v>2811</v>
       </c>
       <c r="Z20" t="s">
-        <v>2436</v>
+        <v>2805</v>
       </c>
       <c r="AA20" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AB20" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AC20" t="s">
-        <v>2456</v>
+        <v>2688</v>
       </c>
       <c r="AD20" t="s">
-        <v>939</v>
+        <v>2098</v>
       </c>
       <c r="AE20" t="s">
         <v>1832</v>
       </c>
       <c r="AF20" t="s">
-        <v>2054</v>
+        <v>2762</v>
       </c>
       <c r="AG20" t="s">
-        <v>751</v>
+        <v>2702</v>
       </c>
       <c r="AH20" t="s">
-        <v>685</v>
+        <v>2763</v>
       </c>
       <c r="AI20" t="s">
-        <v>1209</v>
+        <v>2074</v>
       </c>
       <c r="AJ20" t="s">
-        <v>2603</v>
+        <v>2765</v>
       </c>
       <c r="AK20" t="s">
-        <v>2602</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -12853,16 +13384,16 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>316</v>
+        <v>1401</v>
       </c>
       <c r="D21" t="s">
-        <v>2605</v>
+        <v>2630</v>
       </c>
       <c r="E21" t="s">
-        <v>2604</v>
+        <v>2768</v>
       </c>
       <c r="G21" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R21" t="s">
         <v>401</v>
@@ -12871,58 +13402,58 @@
         <v>304</v>
       </c>
       <c r="T21" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U21" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="V21" t="s">
-        <v>825</v>
+        <v>1929</v>
       </c>
       <c r="W21" t="s">
-        <v>2078</v>
+        <v>2685</v>
       </c>
       <c r="X21" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Y21" t="s">
-        <v>2426</v>
+        <v>2807</v>
       </c>
       <c r="Z21" t="s">
-        <v>1372</v>
+        <v>2831</v>
       </c>
       <c r="AA21" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AB21" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AC21" t="s">
-        <v>2445</v>
+        <v>939</v>
       </c>
       <c r="AD21" t="s">
         <v>2119</v>
       </c>
       <c r="AE21" t="s">
-        <v>693</v>
+        <v>581</v>
       </c>
       <c r="AF21" t="s">
-        <v>1988</v>
+        <v>2767</v>
       </c>
       <c r="AG21" t="s">
-        <v>2054</v>
+        <v>2674</v>
       </c>
       <c r="AH21" t="s">
         <v>1974</v>
       </c>
       <c r="AI21" t="s">
-        <v>316</v>
+        <v>1401</v>
       </c>
       <c r="AJ21" t="s">
-        <v>2605</v>
+        <v>2630</v>
       </c>
       <c r="AK21" t="s">
-        <v>2604</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -12933,13 +13464,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>703</v>
+        <v>2088</v>
       </c>
       <c r="D22" t="s">
         <v>2388</v>
       </c>
       <c r="E22" t="s">
-        <v>2608</v>
+        <v>2770</v>
       </c>
       <c r="G22" t="s">
         <v>706</v>
@@ -12951,58 +13482,58 @@
         <v>830</v>
       </c>
       <c r="T22" t="s">
-        <v>2433</v>
+        <v>2656</v>
       </c>
       <c r="U22" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="V22" t="s">
-        <v>2435</v>
+        <v>2735</v>
       </c>
       <c r="W22" t="s">
-        <v>2443</v>
+        <v>1929</v>
       </c>
       <c r="X22" t="s">
-        <v>2078</v>
+        <v>2828</v>
       </c>
       <c r="Y22" t="s">
-        <v>2606</v>
+        <v>2769</v>
       </c>
       <c r="Z22" t="s">
+        <v>2686</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>2805</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>2098</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>682</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>2688</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>581</v>
+      </c>
+      <c r="AF22" t="s">
         <v>679</v>
       </c>
-      <c r="AA22" t="s">
-        <v>2348</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>2341</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>2352</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>2438</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>2035</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>1372</v>
-      </c>
       <c r="AG22" t="s">
-        <v>825</v>
+        <v>2732</v>
       </c>
       <c r="AH22" t="s">
-        <v>2607</v>
+        <v>2806</v>
       </c>
       <c r="AI22" t="s">
-        <v>703</v>
+        <v>2088</v>
       </c>
       <c r="AJ22" t="s">
         <v>2388</v>
       </c>
       <c r="AK22" t="s">
-        <v>2608</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -13013,16 +13544,16 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>308</v>
+        <v>2074</v>
       </c>
       <c r="D23" t="s">
-        <v>2610</v>
+        <v>1969</v>
       </c>
       <c r="E23" t="s">
-        <v>2609</v>
+        <v>2772</v>
       </c>
       <c r="G23" t="s">
-        <v>578</v>
+        <v>452</v>
       </c>
       <c r="R23" t="s">
         <v>835</v>
@@ -13031,58 +13562,58 @@
         <v>307</v>
       </c>
       <c r="T23" t="s">
-        <v>2367</v>
+        <v>2738</v>
       </c>
       <c r="U23" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="V23" t="s">
-        <v>2115</v>
+        <v>2830</v>
       </c>
       <c r="W23" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="X23" t="s">
-        <v>2452</v>
+        <v>2667</v>
       </c>
       <c r="Y23" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Z23" t="s">
-        <v>2462</v>
+        <v>2811</v>
       </c>
       <c r="AA23" t="s">
-        <v>1988</v>
+        <v>2771</v>
       </c>
       <c r="AB23" t="s">
-        <v>2119</v>
+        <v>2827</v>
       </c>
       <c r="AC23" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AD23" t="s">
-        <v>2456</v>
+        <v>2688</v>
       </c>
       <c r="AE23" t="s">
         <v>399</v>
       </c>
       <c r="AF23" t="s">
-        <v>2065</v>
+        <v>2707</v>
       </c>
       <c r="AG23" t="s">
-        <v>2039</v>
+        <v>2674</v>
       </c>
       <c r="AH23" t="s">
-        <v>2444</v>
+        <v>2178</v>
       </c>
       <c r="AI23" t="s">
-        <v>308</v>
+        <v>2074</v>
       </c>
       <c r="AJ23" t="s">
-        <v>2610</v>
+        <v>1969</v>
       </c>
       <c r="AK23" t="s">
-        <v>2609</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -13093,16 +13624,16 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>305</v>
+        <v>1922</v>
       </c>
       <c r="D24" t="s">
-        <v>2612</v>
+        <v>2777</v>
       </c>
       <c r="E24" t="s">
-        <v>2611</v>
+        <v>2776</v>
       </c>
       <c r="G24" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R24" t="s">
         <v>588</v>
@@ -13111,58 +13642,58 @@
         <v>309</v>
       </c>
       <c r="T24" t="s">
-        <v>693</v>
+        <v>2677</v>
       </c>
       <c r="U24" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="V24" t="s">
-        <v>825</v>
+        <v>2767</v>
       </c>
       <c r="W24" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X24" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Y24" t="s">
-        <v>2504</v>
+        <v>2678</v>
       </c>
       <c r="Z24" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AA24" t="s">
-        <v>2037</v>
+        <v>2826</v>
       </c>
       <c r="AB24" t="s">
-        <v>1195</v>
+        <v>2773</v>
       </c>
       <c r="AC24" t="s">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="AD24" t="s">
-        <v>2352</v>
+        <v>2774</v>
       </c>
       <c r="AE24" t="s">
-        <v>2035</v>
+        <v>2656</v>
       </c>
       <c r="AF24" t="s">
-        <v>2135</v>
+        <v>2775</v>
       </c>
       <c r="AG24" t="s">
-        <v>2041</v>
+        <v>2672</v>
       </c>
       <c r="AH24" t="s">
         <v>1974</v>
       </c>
       <c r="AI24" t="s">
-        <v>305</v>
+        <v>1922</v>
       </c>
       <c r="AJ24" t="s">
-        <v>2612</v>
+        <v>2777</v>
       </c>
       <c r="AK24" t="s">
-        <v>2611</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -13173,13 +13704,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>778</v>
+        <v>2088</v>
       </c>
       <c r="D25" t="s">
-        <v>2616</v>
+        <v>2782</v>
       </c>
       <c r="E25" t="s">
-        <v>2615</v>
+        <v>2781</v>
       </c>
       <c r="G25" t="s">
         <v>653</v>
@@ -13191,58 +13722,58 @@
         <v>487</v>
       </c>
       <c r="T25" t="s">
-        <v>693</v>
+        <v>2778</v>
       </c>
       <c r="U25" t="s">
-        <v>687</v>
+        <v>2732</v>
       </c>
       <c r="V25" t="s">
-        <v>2443</v>
+        <v>2735</v>
       </c>
       <c r="W25" t="s">
-        <v>2435</v>
+        <v>1193</v>
       </c>
       <c r="X25" t="s">
-        <v>2070</v>
+        <v>2337</v>
       </c>
       <c r="Y25" t="s">
-        <v>2337</v>
+        <v>2822</v>
       </c>
       <c r="Z25" t="s">
-        <v>2444</v>
+        <v>2779</v>
       </c>
       <c r="AA25" t="s">
-        <v>2613</v>
+        <v>2660</v>
       </c>
       <c r="AB25" t="s">
-        <v>2352</v>
+        <v>2773</v>
       </c>
       <c r="AC25" t="s">
-        <v>2071</v>
+        <v>682</v>
       </c>
       <c r="AD25" t="s">
-        <v>1195</v>
+        <v>2780</v>
       </c>
       <c r="AE25" t="s">
-        <v>1272</v>
+        <v>2677</v>
       </c>
       <c r="AF25" t="s">
         <v>2614</v>
       </c>
       <c r="AG25" t="s">
-        <v>750</v>
+        <v>2681</v>
       </c>
       <c r="AH25" t="s">
-        <v>751</v>
+        <v>2763</v>
       </c>
       <c r="AI25" t="s">
-        <v>778</v>
+        <v>2088</v>
       </c>
       <c r="AJ25" t="s">
-        <v>2616</v>
+        <v>2782</v>
       </c>
       <c r="AK25" t="s">
-        <v>2615</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -13253,16 +13784,16 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>1749</v>
+        <v>2074</v>
       </c>
       <c r="D26" t="s">
-        <v>1941</v>
+        <v>2785</v>
       </c>
       <c r="E26" t="s">
-        <v>2617</v>
+        <v>2784</v>
       </c>
       <c r="G26" t="s">
-        <v>706</v>
+        <v>653</v>
       </c>
       <c r="R26" t="s">
         <v>595</v>
@@ -13271,58 +13802,58 @@
         <v>849</v>
       </c>
       <c r="T26" t="s">
-        <v>1989</v>
+        <v>2656</v>
       </c>
       <c r="U26" t="s">
-        <v>1955</v>
+        <v>1929</v>
       </c>
       <c r="V26" t="s">
-        <v>2078</v>
+        <v>2667</v>
       </c>
       <c r="W26" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X26" t="s">
-        <v>2341</v>
+        <v>2783</v>
       </c>
       <c r="Y26" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Z26" t="s">
-        <v>1988</v>
+        <v>2805</v>
       </c>
       <c r="AA26" t="s">
-        <v>2462</v>
+        <v>2811</v>
       </c>
       <c r="AB26" t="s">
-        <v>2445</v>
+        <v>682</v>
       </c>
       <c r="AC26" t="s">
-        <v>1938</v>
+        <v>2323</v>
       </c>
       <c r="AD26" t="s">
-        <v>2352</v>
+        <v>939</v>
       </c>
       <c r="AE26" t="s">
-        <v>2035</v>
+        <v>2675</v>
       </c>
       <c r="AF26" t="s">
         <v>679</v>
       </c>
       <c r="AG26" t="s">
-        <v>2039</v>
+        <v>2674</v>
       </c>
       <c r="AH26" t="s">
         <v>1974</v>
       </c>
       <c r="AI26" t="s">
-        <v>1749</v>
+        <v>2074</v>
       </c>
       <c r="AJ26" t="s">
-        <v>1941</v>
+        <v>2785</v>
       </c>
       <c r="AK26" t="s">
-        <v>2617</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -13333,16 +13864,16 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>1498</v>
+        <v>1922</v>
       </c>
       <c r="D27" t="s">
-        <v>2269</v>
+        <v>2279</v>
       </c>
       <c r="E27" t="s">
-        <v>2618</v>
+        <v>2787</v>
       </c>
       <c r="G27" t="s">
-        <v>906</v>
+        <v>706</v>
       </c>
       <c r="R27" t="s">
         <v>854</v>
@@ -13351,58 +13882,58 @@
         <v>853</v>
       </c>
       <c r="T27" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U27" t="s">
-        <v>2452</v>
+        <v>1929</v>
       </c>
       <c r="V27" t="s">
-        <v>2443</v>
+        <v>2657</v>
       </c>
       <c r="W27" t="s">
-        <v>1212</v>
+        <v>2830</v>
       </c>
       <c r="X27" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Y27" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Z27" t="s">
-        <v>2462</v>
+        <v>2811</v>
       </c>
       <c r="AA27" t="s">
         <v>679</v>
       </c>
       <c r="AB27" t="s">
-        <v>2445</v>
+        <v>2688</v>
       </c>
       <c r="AC27" t="s">
-        <v>1938</v>
+        <v>2098</v>
       </c>
       <c r="AD27" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AE27" t="s">
-        <v>693</v>
+        <v>581</v>
       </c>
       <c r="AF27" t="s">
-        <v>2078</v>
+        <v>2735</v>
       </c>
       <c r="AG27" t="s">
-        <v>695</v>
+        <v>2786</v>
       </c>
       <c r="AH27" t="s">
-        <v>2115</v>
+        <v>2707</v>
       </c>
       <c r="AI27" t="s">
-        <v>1498</v>
+        <v>1922</v>
       </c>
       <c r="AJ27" t="s">
-        <v>2269</v>
+        <v>2279</v>
       </c>
       <c r="AK27" t="s">
-        <v>2618</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -13413,13 +13944,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>1831</v>
+        <v>2088</v>
       </c>
       <c r="D28" t="s">
-        <v>1969</v>
+        <v>2111</v>
       </c>
       <c r="E28" t="s">
-        <v>2619</v>
+        <v>2789</v>
       </c>
       <c r="G28" t="s">
         <v>452</v>
@@ -13431,58 +13962,58 @@
         <v>857</v>
       </c>
       <c r="T28" t="s">
-        <v>1154</v>
+        <v>2656</v>
       </c>
       <c r="U28" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="V28" t="s">
-        <v>2452</v>
+        <v>2707</v>
       </c>
       <c r="W28" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X28" t="s">
-        <v>679</v>
+        <v>2828</v>
       </c>
       <c r="Y28" t="s">
-        <v>2455</v>
+        <v>2678</v>
       </c>
       <c r="Z28" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AA28" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="AB28" t="s">
-        <v>2352</v>
+        <v>682</v>
       </c>
       <c r="AC28" t="s">
-        <v>2445</v>
+        <v>2688</v>
       </c>
       <c r="AD28" t="s">
-        <v>1938</v>
+        <v>2098</v>
       </c>
       <c r="AE28" t="s">
-        <v>2035</v>
+        <v>2695</v>
       </c>
       <c r="AF28" t="s">
-        <v>2401</v>
+        <v>2823</v>
       </c>
       <c r="AG28" t="s">
-        <v>1933</v>
+        <v>2824</v>
       </c>
       <c r="AH28" t="s">
         <v>1974</v>
       </c>
       <c r="AI28" t="s">
-        <v>1831</v>
+        <v>2088</v>
       </c>
       <c r="AJ28" t="s">
-        <v>1969</v>
+        <v>2111</v>
       </c>
       <c r="AK28" t="s">
-        <v>2619</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -13493,16 +14024,16 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>1214</v>
+        <v>2067</v>
       </c>
       <c r="D29" t="s">
-        <v>2283</v>
+        <v>2794</v>
       </c>
       <c r="E29" t="s">
-        <v>2621</v>
+        <v>2793</v>
       </c>
       <c r="G29" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="R29" t="s">
         <v>863</v>
@@ -13511,58 +14042,58 @@
         <v>862</v>
       </c>
       <c r="T29" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U29" t="s">
-        <v>2145</v>
+        <v>1193</v>
       </c>
       <c r="V29" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="W29" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X29" t="s">
+        <v>2685</v>
+      </c>
+      <c r="Y29" t="s">
         <v>679</v>
       </c>
-      <c r="Y29" t="s">
-        <v>2341</v>
-      </c>
       <c r="Z29" t="s">
-        <v>2620</v>
+        <v>2825</v>
       </c>
       <c r="AA29" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AB29" t="s">
-        <v>2146</v>
+        <v>2790</v>
       </c>
       <c r="AC29" t="s">
-        <v>2500</v>
+        <v>2323</v>
       </c>
       <c r="AD29" t="s">
-        <v>2445</v>
+        <v>939</v>
       </c>
       <c r="AE29" t="s">
-        <v>693</v>
+        <v>581</v>
       </c>
       <c r="AF29" t="s">
-        <v>687</v>
+        <v>2805</v>
       </c>
       <c r="AG29" t="s">
-        <v>2054</v>
+        <v>2791</v>
       </c>
       <c r="AH29" t="s">
-        <v>2147</v>
+        <v>2792</v>
       </c>
       <c r="AI29" t="s">
-        <v>1214</v>
+        <v>2067</v>
       </c>
       <c r="AJ29" t="s">
-        <v>2283</v>
+        <v>2794</v>
       </c>
       <c r="AK29" t="s">
-        <v>2621</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -13573,16 +14104,16 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>319</v>
+        <v>2040</v>
       </c>
       <c r="D30" t="s">
-        <v>2623</v>
+        <v>1943</v>
       </c>
       <c r="E30" t="s">
-        <v>2622</v>
+        <v>2795</v>
       </c>
       <c r="G30" t="s">
-        <v>706</v>
+        <v>452</v>
       </c>
       <c r="R30" t="s">
         <v>866</v>
@@ -13591,58 +14122,58 @@
         <v>315</v>
       </c>
       <c r="T30" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U30" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="V30" t="s">
-        <v>2485</v>
+        <v>2809</v>
       </c>
       <c r="W30" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="X30" t="s">
-        <v>1988</v>
+        <v>2725</v>
       </c>
       <c r="Y30" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Z30" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="AA30" t="s">
-        <v>679</v>
+        <v>2827</v>
       </c>
       <c r="AB30" t="s">
-        <v>2438</v>
+        <v>2664</v>
       </c>
       <c r="AC30" t="s">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="AD30" t="s">
-        <v>2445</v>
+        <v>2323</v>
       </c>
       <c r="AE30" t="s">
-        <v>693</v>
+        <v>581</v>
       </c>
       <c r="AF30" t="s">
-        <v>2073</v>
+        <v>2674</v>
       </c>
       <c r="AG30" t="s">
-        <v>2515</v>
+        <v>2702</v>
       </c>
       <c r="AH30" t="s">
-        <v>1945</v>
+        <v>2658</v>
       </c>
       <c r="AI30" t="s">
-        <v>319</v>
+        <v>2040</v>
       </c>
       <c r="AJ30" t="s">
-        <v>2623</v>
+        <v>1943</v>
       </c>
       <c r="AK30" t="s">
-        <v>2622</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -13653,16 +14184,16 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>1209</v>
+        <v>1922</v>
       </c>
       <c r="D31" t="s">
-        <v>2152</v>
+        <v>2514</v>
       </c>
       <c r="E31" t="s">
-        <v>2625</v>
+        <v>2797</v>
       </c>
       <c r="G31" t="s">
-        <v>452</v>
+        <v>706</v>
       </c>
       <c r="R31" t="s">
         <v>870</v>
@@ -13671,25 +14202,25 @@
         <v>869</v>
       </c>
       <c r="T31" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U31" t="s">
-        <v>2624</v>
+        <v>2830</v>
       </c>
       <c r="V31" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="W31" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X31" t="s">
-        <v>2462</v>
+        <v>2811</v>
       </c>
       <c r="Y31" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Z31" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="AA31" t="s">
         <v>679</v>
@@ -13698,31 +14229,31 @@
         <v>2119</v>
       </c>
       <c r="AC31" t="s">
-        <v>2438</v>
+        <v>2688</v>
       </c>
       <c r="AD31" t="s">
-        <v>2445</v>
+        <v>939</v>
       </c>
       <c r="AE31" t="s">
-        <v>693</v>
+        <v>581</v>
       </c>
       <c r="AF31" t="s">
-        <v>2041</v>
+        <v>2672</v>
       </c>
       <c r="AG31" t="s">
-        <v>2564</v>
+        <v>2796</v>
       </c>
       <c r="AH31" t="s">
         <v>1974</v>
       </c>
       <c r="AI31" t="s">
-        <v>1209</v>
+        <v>1922</v>
       </c>
       <c r="AJ31" t="s">
-        <v>2152</v>
+        <v>2514</v>
       </c>
       <c r="AK31" t="s">
-        <v>2625</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -13733,16 +14264,16 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>1228</v>
+        <v>1922</v>
       </c>
       <c r="D32" t="s">
-        <v>2628</v>
+        <v>2801</v>
       </c>
       <c r="E32" t="s">
-        <v>2627</v>
+        <v>2800</v>
       </c>
       <c r="G32" t="s">
-        <v>653</v>
+        <v>452</v>
       </c>
       <c r="R32" t="s">
         <v>520</v>
@@ -13751,58 +14282,58 @@
         <v>875</v>
       </c>
       <c r="T32" t="s">
-        <v>2433</v>
+        <v>2677</v>
       </c>
       <c r="U32" t="s">
-        <v>2435</v>
+        <v>1193</v>
       </c>
       <c r="V32" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="W32" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X32" t="s">
-        <v>2348</v>
+        <v>2832</v>
       </c>
       <c r="Y32" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="Z32" t="s">
-        <v>2455</v>
+        <v>2686</v>
       </c>
       <c r="AA32" t="s">
-        <v>2462</v>
+        <v>2807</v>
       </c>
       <c r="AB32" t="s">
-        <v>2445</v>
+        <v>2799</v>
       </c>
       <c r="AC32" t="s">
-        <v>2496</v>
+        <v>682</v>
       </c>
       <c r="AD32" t="s">
-        <v>2438</v>
+        <v>2664</v>
       </c>
       <c r="AE32" t="s">
-        <v>693</v>
+        <v>2689</v>
       </c>
       <c r="AF32" t="s">
-        <v>2624</v>
+        <v>2672</v>
       </c>
       <c r="AG32" t="s">
-        <v>2626</v>
+        <v>2814</v>
       </c>
       <c r="AH32" t="s">
-        <v>2474</v>
+        <v>2658</v>
       </c>
       <c r="AI32" t="s">
-        <v>1228</v>
+        <v>1922</v>
       </c>
       <c r="AJ32" t="s">
-        <v>2628</v>
+        <v>2801</v>
       </c>
       <c r="AK32" t="s">
-        <v>2627</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -13813,16 +14344,16 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>290</v>
+        <v>1401</v>
       </c>
       <c r="D33" t="s">
-        <v>2630</v>
+        <v>2803</v>
       </c>
       <c r="E33" t="s">
-        <v>2629</v>
+        <v>2802</v>
       </c>
       <c r="G33" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="R33" t="s">
         <v>444</v>
@@ -13831,58 +14362,58 @@
         <v>267</v>
       </c>
       <c r="T33" t="s">
-        <v>693</v>
+        <v>2677</v>
       </c>
       <c r="U33" t="s">
-        <v>2443</v>
+        <v>2735</v>
       </c>
       <c r="V33" t="s">
-        <v>2078</v>
+        <v>1929</v>
       </c>
       <c r="W33" t="s">
-        <v>1212</v>
+        <v>2657</v>
       </c>
       <c r="X33" t="s">
-        <v>2348</v>
+        <v>2686</v>
       </c>
       <c r="Y33" t="s">
         <v>679</v>
       </c>
       <c r="Z33" t="s">
-        <v>1988</v>
+        <v>2827</v>
       </c>
       <c r="AA33" t="s">
-        <v>2341</v>
+        <v>2805</v>
       </c>
       <c r="AB33" t="s">
-        <v>2352</v>
+        <v>2664</v>
       </c>
       <c r="AC33" t="s">
-        <v>2445</v>
+        <v>939</v>
       </c>
       <c r="AD33" t="s">
-        <v>1938</v>
+        <v>2323</v>
       </c>
       <c r="AE33" t="s">
-        <v>2035</v>
+        <v>2656</v>
       </c>
       <c r="AF33" t="s">
-        <v>2444</v>
+        <v>2674</v>
       </c>
       <c r="AG33" t="s">
         <v>1974</v>
       </c>
       <c r="AH33" t="s">
-        <v>1945</v>
+        <v>2658</v>
       </c>
       <c r="AI33" t="s">
-        <v>290</v>
+        <v>1401</v>
       </c>
       <c r="AJ33" t="s">
-        <v>2630</v>
+        <v>2803</v>
       </c>
       <c r="AK33" t="s">
-        <v>2629</v>
+        <v>2802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gw 23 md3 after bonus
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16487" uniqueCount="2967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17287" uniqueCount="3015">
   <si>
     <t>Places</t>
   </si>
@@ -8935,6 +8935,150 @@
   </si>
   <si>
     <t>1401</t>
+  </si>
+  <si>
+    <t>Ramsdale 8</t>
+  </si>
+  <si>
+    <t>Hudson-Odoi 6</t>
+  </si>
+  <si>
+    <t>1,956,118</t>
+  </si>
+  <si>
+    <t>1195</t>
+  </si>
+  <si>
+    <t>3,022,767</t>
+  </si>
+  <si>
+    <t>682,515</t>
+  </si>
+  <si>
+    <t>1297</t>
+  </si>
+  <si>
+    <t>Tierney 8</t>
+  </si>
+  <si>
+    <t>Edouard 8</t>
+  </si>
+  <si>
+    <t>371,561</t>
+  </si>
+  <si>
+    <t>Arrizabalaga 8</t>
+  </si>
+  <si>
+    <t>1,116,056</t>
+  </si>
+  <si>
+    <t>3,288,472</t>
+  </si>
+  <si>
+    <t>641,919</t>
+  </si>
+  <si>
+    <t>997,263</t>
+  </si>
+  <si>
+    <t>1265</t>
+  </si>
+  <si>
+    <t>829,886</t>
+  </si>
+  <si>
+    <t>424,302</t>
+  </si>
+  <si>
+    <t>Rüdiger 7</t>
+  </si>
+  <si>
+    <t>Robertson 11</t>
+  </si>
+  <si>
+    <t>Alonso 1</t>
+  </si>
+  <si>
+    <t>514,983</t>
+  </si>
+  <si>
+    <t>1318</t>
+  </si>
+  <si>
+    <t>1,280,139</t>
+  </si>
+  <si>
+    <t>1,845,350</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>799,959</t>
+  </si>
+  <si>
+    <t>1284</t>
+  </si>
+  <si>
+    <t>1,254,578</t>
+  </si>
+  <si>
+    <t>1,280,668</t>
+  </si>
+  <si>
+    <t>790,808</t>
+  </si>
+  <si>
+    <t>105,469</t>
+  </si>
+  <si>
+    <t>422,015</t>
+  </si>
+  <si>
+    <t>115,238</t>
+  </si>
+  <si>
+    <t>161,614</t>
+  </si>
+  <si>
+    <t>523,924</t>
+  </si>
+  <si>
+    <t>368,494</t>
+  </si>
+  <si>
+    <t>5,848,888</t>
+  </si>
+  <si>
+    <t>962</t>
+  </si>
+  <si>
+    <t>267,775</t>
+  </si>
+  <si>
+    <t>32,659</t>
+  </si>
+  <si>
+    <t>669,300</t>
+  </si>
+  <si>
+    <t>105,229</t>
+  </si>
+  <si>
+    <t>74,363</t>
+  </si>
+  <si>
+    <t>1420</t>
+  </si>
+  <si>
+    <t>201,968</t>
+  </si>
+  <si>
+    <t>62,172</t>
+  </si>
+  <si>
+    <t>116,267</t>
   </si>
 </sst>
 </file>
@@ -12128,7 +12272,7 @@
     <col min="20" max="20" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.8203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="21.28125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="20.203125" collapsed="true"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="17.16015625" collapsed="true"/>
@@ -12137,9 +12281,9 @@
     <col min="29" max="29" bestFit="true" customWidth="true" width="25.60546875" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="28.6953125" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="16.0234375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="13.3359375" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.8046875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
@@ -12266,13 +12410,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>2074</v>
+        <v>1323</v>
       </c>
       <c r="D2" t="s">
-        <v>2897</v>
+        <v>2970</v>
       </c>
       <c r="E2" t="s">
-        <v>2896</v>
+        <v>2969</v>
       </c>
       <c r="G2" t="s">
         <v>653</v>
@@ -12284,7 +12428,7 @@
         <v>269</v>
       </c>
       <c r="T2" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U2" t="s">
         <v>476</v>
@@ -12308,7 +12452,7 @@
         <v>2338</v>
       </c>
       <c r="AB2" t="s">
-        <v>2892</v>
+        <v>2968</v>
       </c>
       <c r="AC2" t="s">
         <v>2664</v>
@@ -12317,7 +12461,7 @@
         <v>2893</v>
       </c>
       <c r="AE2" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="AF2" t="s">
         <v>1974</v>
@@ -12326,16 +12470,16 @@
         <v>940</v>
       </c>
       <c r="AH2" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="AI2" t="s">
-        <v>2074</v>
+        <v>1323</v>
       </c>
       <c r="AJ2" t="s">
-        <v>2897</v>
+        <v>2970</v>
       </c>
       <c r="AK2" t="s">
-        <v>2896</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -12346,13 +12490,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>2077</v>
+        <v>2031</v>
       </c>
       <c r="D3" t="s">
         <v>2900</v>
       </c>
       <c r="E3" t="s">
-        <v>2899</v>
+        <v>2971</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
@@ -12364,7 +12508,7 @@
         <v>713</v>
       </c>
       <c r="T3" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="U3" t="s">
         <v>1929</v>
@@ -12409,13 +12553,13 @@
         <v>940</v>
       </c>
       <c r="AI3" t="s">
-        <v>2077</v>
+        <v>2031</v>
       </c>
       <c r="AJ3" t="s">
         <v>2900</v>
       </c>
       <c r="AK3" t="s">
-        <v>2899</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -12426,13 +12570,13 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="D4" t="s">
-        <v>2904</v>
+        <v>2973</v>
       </c>
       <c r="E4" t="s">
-        <v>2903</v>
+        <v>2972</v>
       </c>
       <c r="G4" t="s">
         <v>578</v>
@@ -12450,7 +12594,7 @@
         <v>2837</v>
       </c>
       <c r="V4" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="W4" t="s">
         <v>476</v>
@@ -12477,7 +12621,7 @@
         <v>939</v>
       </c>
       <c r="AE4" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="AF4" t="s">
         <v>2898</v>
@@ -12489,13 +12633,13 @@
         <v>2902</v>
       </c>
       <c r="AI4" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2904</v>
+        <v>2973</v>
       </c>
       <c r="AK4" t="s">
-        <v>2903</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -12506,13 +12650,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>821</v>
+        <v>673</v>
       </c>
       <c r="D5" t="s">
         <v>2908</v>
       </c>
       <c r="E5" t="s">
-        <v>2907</v>
+        <v>2976</v>
       </c>
       <c r="G5" t="s">
         <v>452</v>
@@ -12533,10 +12677,10 @@
         <v>476</v>
       </c>
       <c r="W5" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="X5" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="Y5" t="s">
         <v>2838</v>
@@ -12557,10 +12701,10 @@
         <v>2688</v>
       </c>
       <c r="AE5" t="s">
-        <v>2461</v>
+        <v>436</v>
       </c>
       <c r="AF5" t="s">
-        <v>2906</v>
+        <v>2975</v>
       </c>
       <c r="AG5" t="s">
         <v>2178</v>
@@ -12569,13 +12713,13 @@
         <v>2840</v>
       </c>
       <c r="AI5" t="s">
-        <v>821</v>
+        <v>673</v>
       </c>
       <c r="AJ5" t="s">
         <v>2908</v>
       </c>
       <c r="AK5" t="s">
-        <v>2907</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -12589,10 +12733,10 @@
         <v>1910</v>
       </c>
       <c r="D6" t="s">
-        <v>2913</v>
+        <v>2068</v>
       </c>
       <c r="E6" t="s">
-        <v>2912</v>
+        <v>2978</v>
       </c>
       <c r="G6" t="s">
         <v>706</v>
@@ -12637,7 +12781,7 @@
         <v>939</v>
       </c>
       <c r="AE6" t="s">
-        <v>2910</v>
+        <v>2977</v>
       </c>
       <c r="AF6" t="s">
         <v>2812</v>
@@ -12652,10 +12796,10 @@
         <v>1910</v>
       </c>
       <c r="AJ6" t="s">
-        <v>2913</v>
+        <v>2068</v>
       </c>
       <c r="AK6" t="s">
-        <v>2912</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -12666,13 +12810,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>2255</v>
+        <v>2031</v>
       </c>
       <c r="D7" t="s">
         <v>2915</v>
       </c>
       <c r="E7" t="s">
-        <v>2914</v>
+        <v>2979</v>
       </c>
       <c r="G7" t="s">
         <v>653</v>
@@ -12684,7 +12828,7 @@
         <v>435</v>
       </c>
       <c r="T7" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U7" t="s">
         <v>1193</v>
@@ -12729,13 +12873,13 @@
         <v>1974</v>
       </c>
       <c r="AI7" t="s">
-        <v>2255</v>
+        <v>2031</v>
       </c>
       <c r="AJ7" t="s">
         <v>2915</v>
       </c>
       <c r="AK7" t="s">
-        <v>2914</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -12746,13 +12890,13 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>874</v>
+        <v>912</v>
       </c>
       <c r="D8" t="s">
-        <v>2603</v>
+        <v>2731</v>
       </c>
       <c r="E8" t="s">
-        <v>2917</v>
+        <v>2980</v>
       </c>
       <c r="G8" t="s">
         <v>653</v>
@@ -12764,7 +12908,7 @@
         <v>758</v>
       </c>
       <c r="T8" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="U8" t="s">
         <v>2916</v>
@@ -12773,7 +12917,7 @@
         <v>476</v>
       </c>
       <c r="W8" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="X8" t="s">
         <v>1952</v>
@@ -12809,13 +12953,13 @@
         <v>739</v>
       </c>
       <c r="AI8" t="s">
-        <v>874</v>
+        <v>912</v>
       </c>
       <c r="AJ8" t="s">
-        <v>2603</v>
+        <v>2731</v>
       </c>
       <c r="AK8" t="s">
-        <v>2917</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -12826,13 +12970,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>2167</v>
+        <v>1911</v>
       </c>
       <c r="D9" t="s">
-        <v>2094</v>
+        <v>2982</v>
       </c>
       <c r="E9" t="s">
-        <v>2918</v>
+        <v>2981</v>
       </c>
       <c r="G9" t="s">
         <v>653</v>
@@ -12844,7 +12988,7 @@
         <v>763</v>
       </c>
       <c r="T9" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="U9" t="s">
         <v>476</v>
@@ -12877,7 +13021,7 @@
         <v>682</v>
       </c>
       <c r="AE9" t="s">
-        <v>2461</v>
+        <v>436</v>
       </c>
       <c r="AF9" t="s">
         <v>2344</v>
@@ -12889,13 +13033,13 @@
         <v>2814</v>
       </c>
       <c r="AI9" t="s">
-        <v>2167</v>
+        <v>1911</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2094</v>
+        <v>2982</v>
       </c>
       <c r="AK9" t="s">
-        <v>2918</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -12906,13 +13050,13 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>2077</v>
+        <v>2031</v>
       </c>
       <c r="D10" t="s">
-        <v>1942</v>
+        <v>2386</v>
       </c>
       <c r="E10" t="s">
-        <v>2921</v>
+        <v>2983</v>
       </c>
       <c r="G10" t="s">
         <v>706</v>
@@ -12924,7 +13068,7 @@
         <v>285</v>
       </c>
       <c r="T10" t="s">
-        <v>2461</v>
+        <v>436</v>
       </c>
       <c r="U10" t="s">
         <v>2919</v>
@@ -12969,13 +13113,13 @@
         <v>554</v>
       </c>
       <c r="AI10" t="s">
-        <v>2077</v>
+        <v>2031</v>
       </c>
       <c r="AJ10" t="s">
-        <v>1942</v>
+        <v>2386</v>
       </c>
       <c r="AK10" t="s">
-        <v>2921</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -12986,13 +13130,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>874</v>
+        <v>821</v>
       </c>
       <c r="D11" t="s">
         <v>2132</v>
       </c>
       <c r="E11" t="s">
-        <v>2923</v>
+        <v>2984</v>
       </c>
       <c r="G11" t="s">
         <v>672</v>
@@ -13004,7 +13148,7 @@
         <v>772</v>
       </c>
       <c r="T11" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="U11" t="s">
         <v>476</v>
@@ -13049,13 +13193,13 @@
         <v>2716</v>
       </c>
       <c r="AI11" t="s">
-        <v>874</v>
+        <v>821</v>
       </c>
       <c r="AJ11" t="s">
         <v>2132</v>
       </c>
       <c r="AK11" t="s">
-        <v>2923</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -13066,13 +13210,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>912</v>
+        <v>829</v>
       </c>
       <c r="D12" t="s">
-        <v>2398</v>
+        <v>2989</v>
       </c>
       <c r="E12" t="s">
-        <v>2927</v>
+        <v>2988</v>
       </c>
       <c r="G12" t="s">
         <v>452</v>
@@ -13084,16 +13228,16 @@
         <v>289</v>
       </c>
       <c r="T12" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U12" t="s">
         <v>1193</v>
       </c>
       <c r="V12" t="s">
-        <v>2924</v>
+        <v>2985</v>
       </c>
       <c r="W12" t="s">
-        <v>2925</v>
+        <v>2986</v>
       </c>
       <c r="X12" t="s">
         <v>554</v>
@@ -13120,7 +13264,7 @@
         <v>2829</v>
       </c>
       <c r="AF12" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="AG12" t="s">
         <v>2926</v>
@@ -13129,13 +13273,13 @@
         <v>2898</v>
       </c>
       <c r="AI12" t="s">
-        <v>912</v>
+        <v>829</v>
       </c>
       <c r="AJ12" t="s">
-        <v>2398</v>
+        <v>2989</v>
       </c>
       <c r="AK12" t="s">
-        <v>2927</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -13146,13 +13290,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>1912</v>
+        <v>821</v>
       </c>
       <c r="D13" t="s">
-        <v>2930</v>
+        <v>2940</v>
       </c>
       <c r="E13" t="s">
-        <v>2929</v>
+        <v>2990</v>
       </c>
       <c r="G13" t="s">
         <v>672</v>
@@ -13167,7 +13311,7 @@
         <v>2928</v>
       </c>
       <c r="U13" t="s">
-        <v>2924</v>
+        <v>2985</v>
       </c>
       <c r="V13" t="s">
         <v>476</v>
@@ -13176,7 +13320,7 @@
         <v>1929</v>
       </c>
       <c r="X13" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="Y13" t="s">
         <v>2724</v>
@@ -13197,7 +13341,7 @@
         <v>939</v>
       </c>
       <c r="AE13" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="AF13" t="s">
         <v>2853</v>
@@ -13209,13 +13353,13 @@
         <v>2815</v>
       </c>
       <c r="AI13" t="s">
-        <v>1912</v>
+        <v>821</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2930</v>
+        <v>2940</v>
       </c>
       <c r="AK13" t="s">
-        <v>2929</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -13226,13 +13370,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>268</v>
+        <v>730</v>
       </c>
       <c r="D14" t="s">
-        <v>2934</v>
+        <v>2992</v>
       </c>
       <c r="E14" t="s">
-        <v>2933</v>
+        <v>2991</v>
       </c>
       <c r="G14" t="s">
         <v>653</v>
@@ -13247,7 +13391,7 @@
         <v>2677</v>
       </c>
       <c r="U14" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="V14" t="s">
         <v>2859</v>
@@ -13256,7 +13400,7 @@
         <v>2931</v>
       </c>
       <c r="X14" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="Y14" t="s">
         <v>2826</v>
@@ -13289,13 +13433,13 @@
         <v>767</v>
       </c>
       <c r="AI14" t="s">
-        <v>268</v>
+        <v>730</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2934</v>
+        <v>2992</v>
       </c>
       <c r="AK14" t="s">
-        <v>2933</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -13306,13 +13450,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>2077</v>
+        <v>2167</v>
       </c>
       <c r="D15" t="s">
-        <v>2610</v>
+        <v>2994</v>
       </c>
       <c r="E15" t="s">
-        <v>2936</v>
+        <v>2993</v>
       </c>
       <c r="G15" t="s">
         <v>706</v>
@@ -13324,10 +13468,10 @@
         <v>800</v>
       </c>
       <c r="T15" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U15" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="V15" t="s">
         <v>476</v>
@@ -13369,13 +13513,13 @@
         <v>2901</v>
       </c>
       <c r="AI15" t="s">
-        <v>2077</v>
+        <v>2167</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2610</v>
+        <v>2994</v>
       </c>
       <c r="AK15" t="s">
-        <v>2936</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -13392,7 +13536,7 @@
         <v>2376</v>
       </c>
       <c r="E16" t="s">
-        <v>2938</v>
+        <v>2995</v>
       </c>
       <c r="G16" t="s">
         <v>578</v>
@@ -13437,7 +13581,7 @@
         <v>2119</v>
       </c>
       <c r="AE16" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="AF16" t="s">
         <v>1974</v>
@@ -13455,7 +13599,7 @@
         <v>2376</v>
       </c>
       <c r="AK16" t="s">
-        <v>2938</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -13466,13 +13610,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>1975</v>
+        <v>1912</v>
       </c>
       <c r="D17" t="s">
         <v>2940</v>
       </c>
       <c r="E17" t="s">
-        <v>2939</v>
+        <v>2996</v>
       </c>
       <c r="G17" t="s">
         <v>706</v>
@@ -13484,7 +13628,7 @@
         <v>298</v>
       </c>
       <c r="T17" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U17" t="s">
         <v>554</v>
@@ -13517,7 +13661,7 @@
         <v>2664</v>
       </c>
       <c r="AE17" t="s">
-        <v>2894</v>
+        <v>1184</v>
       </c>
       <c r="AF17" t="s">
         <v>721</v>
@@ -13529,13 +13673,13 @@
         <v>2937</v>
       </c>
       <c r="AI17" t="s">
-        <v>1975</v>
+        <v>1912</v>
       </c>
       <c r="AJ17" t="s">
         <v>2940</v>
       </c>
       <c r="AK17" t="s">
-        <v>2939</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -13552,7 +13696,7 @@
         <v>2943</v>
       </c>
       <c r="E18" t="s">
-        <v>2942</v>
+        <v>2997</v>
       </c>
       <c r="G18" t="s">
         <v>706</v>
@@ -13597,13 +13741,13 @@
         <v>682</v>
       </c>
       <c r="AE18" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="AF18" t="s">
-        <v>2924</v>
+        <v>2985</v>
       </c>
       <c r="AG18" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="AH18" t="s">
         <v>812</v>
@@ -13615,7 +13759,7 @@
         <v>2943</v>
       </c>
       <c r="AK18" t="s">
-        <v>2942</v>
+        <v>2997</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -13626,13 +13770,13 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="D19" t="s">
         <v>1964</v>
       </c>
       <c r="E19" t="s">
-        <v>2944</v>
+        <v>2998</v>
       </c>
       <c r="G19" t="s">
         <v>706</v>
@@ -13644,7 +13788,7 @@
         <v>818</v>
       </c>
       <c r="T19" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U19" t="s">
         <v>2937</v>
@@ -13689,13 +13833,13 @@
         <v>1974</v>
       </c>
       <c r="AI19" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="AJ19" t="s">
         <v>1964</v>
       </c>
       <c r="AK19" t="s">
-        <v>2944</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -13706,13 +13850,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>844</v>
+        <v>785</v>
       </c>
       <c r="D20" t="s">
         <v>2216</v>
       </c>
       <c r="E20" t="s">
-        <v>2945</v>
+        <v>2999</v>
       </c>
       <c r="G20" t="s">
         <v>452</v>
@@ -13733,7 +13877,7 @@
         <v>476</v>
       </c>
       <c r="W20" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="X20" t="s">
         <v>2838</v>
@@ -13769,13 +13913,13 @@
         <v>751</v>
       </c>
       <c r="AI20" t="s">
-        <v>844</v>
+        <v>785</v>
       </c>
       <c r="AJ20" t="s">
         <v>2216</v>
       </c>
       <c r="AK20" t="s">
-        <v>2945</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -13786,13 +13930,13 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>2190</v>
+        <v>907</v>
       </c>
       <c r="D21" t="s">
         <v>2329</v>
       </c>
       <c r="E21" t="s">
-        <v>2946</v>
+        <v>3000</v>
       </c>
       <c r="G21" t="s">
         <v>706</v>
@@ -13813,7 +13957,7 @@
         <v>1929</v>
       </c>
       <c r="W21" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="X21" t="s">
         <v>2805</v>
@@ -13849,13 +13993,13 @@
         <v>1974</v>
       </c>
       <c r="AI21" t="s">
-        <v>2190</v>
+        <v>907</v>
       </c>
       <c r="AJ21" t="s">
         <v>2329</v>
       </c>
       <c r="AK21" t="s">
-        <v>2946</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -13866,13 +14010,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>2031</v>
+        <v>1911</v>
       </c>
       <c r="D22" t="s">
-        <v>1963</v>
+        <v>1943</v>
       </c>
       <c r="E22" t="s">
-        <v>2948</v>
+        <v>3001</v>
       </c>
       <c r="G22" t="s">
         <v>706</v>
@@ -13884,13 +14028,13 @@
         <v>830</v>
       </c>
       <c r="T22" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U22" t="s">
         <v>476</v>
       </c>
       <c r="V22" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="W22" t="s">
         <v>1929</v>
@@ -13923,19 +14067,19 @@
         <v>679</v>
       </c>
       <c r="AG22" t="s">
-        <v>2924</v>
+        <v>2985</v>
       </c>
       <c r="AH22" t="s">
         <v>2837</v>
       </c>
       <c r="AI22" t="s">
-        <v>2031</v>
+        <v>1911</v>
       </c>
       <c r="AJ22" t="s">
-        <v>1963</v>
+        <v>1943</v>
       </c>
       <c r="AK22" t="s">
-        <v>2948</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -13946,13 +14090,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>712</v>
+        <v>829</v>
       </c>
       <c r="D23" t="s">
         <v>2777</v>
       </c>
       <c r="E23" t="s">
-        <v>2949</v>
+        <v>3002</v>
       </c>
       <c r="G23" t="s">
         <v>452</v>
@@ -13976,7 +14120,7 @@
         <v>1929</v>
       </c>
       <c r="X23" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="Y23" t="s">
         <v>2805</v>
@@ -14009,13 +14153,13 @@
         <v>2178</v>
       </c>
       <c r="AI23" t="s">
-        <v>712</v>
+        <v>829</v>
       </c>
       <c r="AJ23" t="s">
         <v>2777</v>
       </c>
       <c r="AK23" t="s">
-        <v>2949</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -14029,10 +14173,10 @@
         <v>673</v>
       </c>
       <c r="D24" t="s">
-        <v>2951</v>
+        <v>2881</v>
       </c>
       <c r="E24" t="s">
-        <v>2950</v>
+        <v>3003</v>
       </c>
       <c r="G24" t="s">
         <v>672</v>
@@ -14077,7 +14221,7 @@
         <v>2774</v>
       </c>
       <c r="AE24" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="AF24" t="s">
         <v>2775</v>
@@ -14092,10 +14236,10 @@
         <v>673</v>
       </c>
       <c r="AJ24" t="s">
-        <v>2951</v>
+        <v>2881</v>
       </c>
       <c r="AK24" t="s">
-        <v>2950</v>
+        <v>3003</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -14106,13 +14250,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>2059</v>
+        <v>1401</v>
       </c>
       <c r="D25" t="s">
-        <v>2879</v>
+        <v>3005</v>
       </c>
       <c r="E25" t="s">
-        <v>2953</v>
+        <v>3004</v>
       </c>
       <c r="G25" t="s">
         <v>653</v>
@@ -14127,10 +14271,10 @@
         <v>1272</v>
       </c>
       <c r="U25" t="s">
-        <v>2924</v>
+        <v>2985</v>
       </c>
       <c r="V25" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="W25" t="s">
         <v>1193</v>
@@ -14169,13 +14313,13 @@
         <v>751</v>
       </c>
       <c r="AI25" t="s">
-        <v>2059</v>
+        <v>1401</v>
       </c>
       <c r="AJ25" t="s">
-        <v>2879</v>
+        <v>3005</v>
       </c>
       <c r="AK25" t="s">
-        <v>2953</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -14186,13 +14330,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>712</v>
+        <v>841</v>
       </c>
       <c r="D26" t="s">
         <v>2955</v>
       </c>
       <c r="E26" t="s">
-        <v>2954</v>
+        <v>3006</v>
       </c>
       <c r="G26" t="s">
         <v>653</v>
@@ -14204,13 +14348,13 @@
         <v>849</v>
       </c>
       <c r="T26" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U26" t="s">
         <v>1929</v>
       </c>
       <c r="V26" t="s">
-        <v>2895</v>
+        <v>1445</v>
       </c>
       <c r="W26" t="s">
         <v>476</v>
@@ -14249,13 +14393,13 @@
         <v>1974</v>
       </c>
       <c r="AI26" t="s">
-        <v>712</v>
+        <v>841</v>
       </c>
       <c r="AJ26" t="s">
         <v>2955</v>
       </c>
       <c r="AK26" t="s">
-        <v>2954</v>
+        <v>3006</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -14272,7 +14416,7 @@
         <v>2294</v>
       </c>
       <c r="E27" t="s">
-        <v>2956</v>
+        <v>3007</v>
       </c>
       <c r="G27" t="s">
         <v>706</v>
@@ -14320,7 +14464,7 @@
         <v>581</v>
       </c>
       <c r="AF27" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="AG27" t="s">
         <v>2786</v>
@@ -14335,7 +14479,7 @@
         <v>2294</v>
       </c>
       <c r="AK27" t="s">
-        <v>2956</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -14346,13 +14490,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>2155</v>
+        <v>2190</v>
       </c>
       <c r="D28" t="s">
-        <v>2958</v>
+        <v>2586</v>
       </c>
       <c r="E28" t="s">
-        <v>2957</v>
+        <v>3008</v>
       </c>
       <c r="G28" t="s">
         <v>452</v>
@@ -14364,7 +14508,7 @@
         <v>857</v>
       </c>
       <c r="T28" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="U28" t="s">
         <v>1929</v>
@@ -14409,13 +14553,13 @@
         <v>1974</v>
       </c>
       <c r="AI28" t="s">
-        <v>2155</v>
+        <v>2190</v>
       </c>
       <c r="AJ28" t="s">
-        <v>2958</v>
+        <v>2586</v>
       </c>
       <c r="AK28" t="s">
-        <v>2957</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -14426,13 +14570,13 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>1975</v>
+        <v>1912</v>
       </c>
       <c r="D29" t="s">
         <v>1964</v>
       </c>
       <c r="E29" t="s">
-        <v>2959</v>
+        <v>3009</v>
       </c>
       <c r="G29" t="s">
         <v>706</v>
@@ -14456,7 +14600,7 @@
         <v>476</v>
       </c>
       <c r="X29" t="s">
-        <v>790</v>
+        <v>2974</v>
       </c>
       <c r="Y29" t="s">
         <v>679</v>
@@ -14489,13 +14633,13 @@
         <v>2792</v>
       </c>
       <c r="AI29" t="s">
-        <v>1975</v>
+        <v>1912</v>
       </c>
       <c r="AJ29" t="s">
         <v>1964</v>
       </c>
       <c r="AK29" t="s">
-        <v>2959</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -14509,10 +14653,10 @@
         <v>844</v>
       </c>
       <c r="D30" t="s">
-        <v>2519</v>
+        <v>3011</v>
       </c>
       <c r="E30" t="s">
-        <v>2960</v>
+        <v>3010</v>
       </c>
       <c r="G30" t="s">
         <v>452</v>
@@ -14572,10 +14716,10 @@
         <v>844</v>
       </c>
       <c r="AJ30" t="s">
-        <v>2519</v>
+        <v>3011</v>
       </c>
       <c r="AK30" t="s">
-        <v>2960</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -14592,7 +14736,7 @@
         <v>1927</v>
       </c>
       <c r="E31" t="s">
-        <v>2962</v>
+        <v>3012</v>
       </c>
       <c r="G31" t="s">
         <v>706</v>
@@ -14655,7 +14799,7 @@
         <v>1927</v>
       </c>
       <c r="AK31" t="s">
-        <v>2962</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -14672,7 +14816,7 @@
         <v>2277</v>
       </c>
       <c r="E32" t="s">
-        <v>2964</v>
+        <v>3013</v>
       </c>
       <c r="G32" t="s">
         <v>452</v>
@@ -14735,7 +14879,7 @@
         <v>2277</v>
       </c>
       <c r="AK32" t="s">
-        <v>2964</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -14746,13 +14890,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>1911</v>
+        <v>2155</v>
       </c>
       <c r="D33" t="s">
-        <v>2966</v>
+        <v>2329</v>
       </c>
       <c r="E33" t="s">
-        <v>2965</v>
+        <v>3014</v>
       </c>
       <c r="G33" t="s">
         <v>672</v>
@@ -14767,7 +14911,7 @@
         <v>2677</v>
       </c>
       <c r="U33" t="s">
-        <v>707</v>
+        <v>2987</v>
       </c>
       <c r="V33" t="s">
         <v>1929</v>
@@ -14797,7 +14941,7 @@
         <v>2323</v>
       </c>
       <c r="AE33" t="s">
-        <v>686</v>
+        <v>2967</v>
       </c>
       <c r="AF33" t="s">
         <v>2898</v>
@@ -14809,13 +14953,13 @@
         <v>1945</v>
       </c>
       <c r="AI33" t="s">
-        <v>1911</v>
+        <v>2155</v>
       </c>
       <c r="AJ33" t="s">
-        <v>2966</v>
+        <v>2329</v>
       </c>
       <c r="AK33" t="s">
-        <v>2965</v>
+        <v>3014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unix date to localTime
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9060" uniqueCount="2352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9066" uniqueCount="2354">
   <si>
     <t>Places</t>
   </si>
@@ -7090,6 +7090,12 @@
   </si>
   <si>
     <t>1.13</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>2.92</t>
   </si>
 </sst>
 </file>
@@ -25387,7 +25393,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -25647,6 +25653,28 @@
         <v>2351</v>
       </c>
       <c r="E22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>2350</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2352</v>
+      </c>
+      <c r="E23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>2350</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2353</v>
+      </c>
+      <c r="E24" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
date is also dataTzpe
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9066" uniqueCount="2354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9071" uniqueCount="2358">
   <si>
     <t>Places</t>
   </si>
@@ -7096,6 +7096,18 @@
   </si>
   <si>
     <t>2.92</t>
+  </si>
+  <si>
+    <t>Marčana</t>
+  </si>
+  <si>
+    <t>-2.34</t>
+  </si>
+  <si>
+    <t>Lat : 45long : 14</t>
+  </si>
+  <si>
+    <t>2022-15-02 12:15:08</t>
   </si>
 </sst>
 </file>
@@ -25393,7 +25405,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -25402,8 +25414,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.89453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.96484375" collapsed="true" bestFit="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.8984375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
   </cols>
@@ -25676,6 +25688,23 @@
       </c>
       <c r="E24" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2356</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2357</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2355</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GW 25 first scrapped to xl
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13339" uniqueCount="3154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14139" uniqueCount="3281">
   <si>
     <t>Places</t>
   </si>
@@ -9496,6 +9496,387 @@
   </si>
   <si>
     <t>93,631</t>
+  </si>
+  <si>
+    <t>Salah 6$ captain</t>
+  </si>
+  <si>
+    <t>Maupay 6, MUN (A)</t>
+  </si>
+  <si>
+    <t>Sánchez 6, MUN (A)</t>
+  </si>
+  <si>
+    <t>Livramento 1</t>
+  </si>
+  <si>
+    <t>2,149,463</t>
+  </si>
+  <si>
+    <t>1272</t>
+  </si>
+  <si>
+    <t>Coady 6</t>
+  </si>
+  <si>
+    <t>Gray 0</t>
+  </si>
+  <si>
+    <t>Bowen 1</t>
+  </si>
+  <si>
+    <t>Gallagher 3</t>
+  </si>
+  <si>
+    <t>Ronaldo 4, BHA (H)$ captain</t>
+  </si>
+  <si>
+    <t>3,294,217</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>Romero 1</t>
+  </si>
+  <si>
+    <t>Dalot 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>Salah 3</t>
+  </si>
+  <si>
+    <t>Ramsey 1</t>
+  </si>
+  <si>
+    <t>Fernandes 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>808,419</t>
+  </si>
+  <si>
+    <t>1380</t>
+  </si>
+  <si>
+    <t>Jota 1</t>
+  </si>
+  <si>
+    <t>314,551</t>
+  </si>
+  <si>
+    <t>Mings 2</t>
+  </si>
+  <si>
+    <t>Varane 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>Mac Allister 1, MUN (A)</t>
+  </si>
+  <si>
+    <t>Fernandes 4, BHA (H)$ captain</t>
+  </si>
+  <si>
+    <t>Ronaldo 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>Mbeumo 3</t>
+  </si>
+  <si>
+    <t>1,500,196</t>
+  </si>
+  <si>
+    <t>Dias 10</t>
+  </si>
+  <si>
+    <t>Duffy 1, MUN (A)</t>
+  </si>
+  <si>
+    <t>Antonio 1</t>
+  </si>
+  <si>
+    <t>Steele 0, MUN (A)</t>
+  </si>
+  <si>
+    <t>3,408,829</t>
+  </si>
+  <si>
+    <t>1193</t>
+  </si>
+  <si>
+    <t>Sánchez View player information</t>
+  </si>
+  <si>
+    <t>Veltman View player information</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold View player information</t>
+  </si>
+  <si>
+    <t>Shaw 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>Pogba 1, BHA (H)</t>
+  </si>
+  <si>
+    <t>Bowen 6</t>
+  </si>
+  <si>
+    <t>Pinnock 7</t>
+  </si>
+  <si>
+    <t>Ødegaard -</t>
+  </si>
+  <si>
+    <t>688,759</t>
+  </si>
+  <si>
+    <t>1394</t>
+  </si>
+  <si>
+    <t>Højbjerg 0</t>
+  </si>
+  <si>
+    <t>Saïss 6</t>
+  </si>
+  <si>
+    <t>1,307,519</t>
+  </si>
+  <si>
+    <t>1333</t>
+  </si>
+  <si>
+    <t>Jansson 7</t>
+  </si>
+  <si>
+    <t>Coutinho 2</t>
+  </si>
+  <si>
+    <t>Gabriel -</t>
+  </si>
+  <si>
+    <t>771,235</t>
+  </si>
+  <si>
+    <t>Raya 10</t>
+  </si>
+  <si>
+    <t>387,462</t>
+  </si>
+  <si>
+    <t>1437</t>
+  </si>
+  <si>
+    <t>Ederson 7</t>
+  </si>
+  <si>
+    <t>541,970</t>
+  </si>
+  <si>
+    <t>1413</t>
+  </si>
+  <si>
+    <t>De Bruyne 0$ captain</t>
+  </si>
+  <si>
+    <t>1,336,759</t>
+  </si>
+  <si>
+    <t>de Gea 3, BHA (H)</t>
+  </si>
+  <si>
+    <t>Matip 6</t>
+  </si>
+  <si>
+    <t>Sancho 9, BHA (H)</t>
+  </si>
+  <si>
+    <t>Sterling 18</t>
+  </si>
+  <si>
+    <t>Maupay 12, MUN (A)$ captain</t>
+  </si>
+  <si>
+    <t>Gilmour 2</t>
+  </si>
+  <si>
+    <t>1,166,228</t>
+  </si>
+  <si>
+    <t>1345</t>
+  </si>
+  <si>
+    <t>Lamptey 11, MUN (A)</t>
+  </si>
+  <si>
+    <t>779,674</t>
+  </si>
+  <si>
+    <t>1383</t>
+  </si>
+  <si>
+    <t>Sá 8</t>
+  </si>
+  <si>
+    <t>Dennis 2$ captain</t>
+  </si>
+  <si>
+    <t>Soucek 1</t>
+  </si>
+  <si>
+    <t>1,262,883</t>
+  </si>
+  <si>
+    <t>Foden 8</t>
+  </si>
+  <si>
+    <t>1,194,016</t>
+  </si>
+  <si>
+    <t>1343</t>
+  </si>
+  <si>
+    <t>Maguire 2, BHA (H)</t>
+  </si>
+  <si>
+    <t>1,034,564</t>
+  </si>
+  <si>
+    <t>1357</t>
+  </si>
+  <si>
+    <t>100,366</t>
+  </si>
+  <si>
+    <t>1511</t>
+  </si>
+  <si>
+    <t>De Bruyne 0</t>
+  </si>
+  <si>
+    <t>396,562</t>
+  </si>
+  <si>
+    <t>111,887</t>
+  </si>
+  <si>
+    <t>Bowen 12$ captain</t>
+  </si>
+  <si>
+    <t>Trossard 0, MUN (A)</t>
+  </si>
+  <si>
+    <t>178,362</t>
+  </si>
+  <si>
+    <t>Alisson 7</t>
+  </si>
+  <si>
+    <t>Pogba 2, BHA (H)$ captain</t>
+  </si>
+  <si>
+    <t>Daka 1</t>
+  </si>
+  <si>
+    <t>624,952</t>
+  </si>
+  <si>
+    <t>Mitchell 6</t>
+  </si>
+  <si>
+    <t>Podence 3</t>
+  </si>
+  <si>
+    <t>Zaha 3</t>
+  </si>
+  <si>
+    <t>James 1</t>
+  </si>
+  <si>
+    <t>Weghorst 2</t>
+  </si>
+  <si>
+    <t>265,327</t>
+  </si>
+  <si>
+    <t>1462</t>
+  </si>
+  <si>
+    <t>Greenwood 0, BHA (H)</t>
+  </si>
+  <si>
+    <t>Jiménez 6</t>
+  </si>
+  <si>
+    <t>Aubameyang -$ captain</t>
+  </si>
+  <si>
+    <t>Bissouma 1, MUN (A)</t>
+  </si>
+  <si>
+    <t>6,064,362</t>
+  </si>
+  <si>
+    <t>1018</t>
+  </si>
+  <si>
+    <t>Cash 2</t>
+  </si>
+  <si>
+    <t>233,971</t>
+  </si>
+  <si>
+    <t>37,834</t>
+  </si>
+  <si>
+    <t>1547</t>
+  </si>
+  <si>
+    <t>Ait Nouri 5</t>
+  </si>
+  <si>
+    <t>618,344</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>Keane 13</t>
+  </si>
+  <si>
+    <t>Idah 0</t>
+  </si>
+  <si>
+    <t>102,689</t>
+  </si>
+  <si>
+    <t>1510</t>
+  </si>
+  <si>
+    <t>98,580</t>
+  </si>
+  <si>
+    <t>1512</t>
+  </si>
+  <si>
+    <t>Burn 5</t>
+  </si>
+  <si>
+    <t>215,442</t>
+  </si>
+  <si>
+    <t>1474</t>
+  </si>
+  <si>
+    <t>Lacazette -</t>
+  </si>
+  <si>
+    <t>56,842</t>
+  </si>
+  <si>
+    <t>1533</t>
+  </si>
+  <si>
+    <t>102,895</t>
   </si>
 </sst>
 </file>
@@ -12686,25 +13067,25 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.2265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.13671875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="31.82421875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="30.703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="38.89453125" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="21.28125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="21.28125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.1484375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="21.28125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="14.8984375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="20.34765625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="28.12890625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="26.328125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="18.78515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.53125" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="15.34765625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
@@ -12831,13 +13212,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>1297</v>
       </c>
       <c r="D2" t="s">
-        <v>3106</v>
+        <v>3159</v>
       </c>
       <c r="E2" t="s">
-        <v>3105</v>
+        <v>3158</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -12849,58 +13230,58 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>3014</v>
+        <v>1927</v>
       </c>
       <c r="U2" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="V2" t="s">
-        <v>651</v>
+        <v>2837</v>
       </c>
       <c r="W2" t="s">
-        <v>3015</v>
+        <v>663</v>
       </c>
       <c r="X2" t="s">
+        <v>357</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="Z2" t="s">
         <v>1929</v>
       </c>
-      <c r="Y2" t="s">
-        <v>3018</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>2840</v>
-      </c>
       <c r="AA2" t="s">
-        <v>3017</v>
+        <v>3154</v>
       </c>
       <c r="AB2" t="s">
         <v>2843</v>
       </c>
       <c r="AC2" t="s">
-        <v>2844</v>
+        <v>723</v>
       </c>
       <c r="AD2" t="s">
-        <v>2020</v>
+        <v>3155</v>
       </c>
       <c r="AE2" t="s">
-        <v>2845</v>
+        <v>3156</v>
       </c>
       <c r="AF2" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AG2" t="s">
         <v>914</v>
       </c>
       <c r="AH2" t="s">
-        <v>2837</v>
+        <v>1930</v>
       </c>
       <c r="AI2" t="s">
-        <v>256</v>
+        <v>1297</v>
       </c>
       <c r="AJ2" t="s">
-        <v>3106</v>
+        <v>3159</v>
       </c>
       <c r="AK2" t="s">
-        <v>3105</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -12911,13 +13292,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>759</v>
+        <v>1886</v>
       </c>
       <c r="D3" t="s">
-        <v>3108</v>
+        <v>3166</v>
       </c>
       <c r="E3" t="s">
-        <v>3107</v>
+        <v>3165</v>
       </c>
       <c r="G3" t="s">
         <v>627</v>
@@ -12929,43 +13310,43 @@
         <v>687</v>
       </c>
       <c r="T3" t="s">
-        <v>683</v>
+        <v>3156</v>
       </c>
       <c r="U3" t="s">
+        <v>663</v>
+      </c>
+      <c r="V3" t="s">
         <v>3015</v>
       </c>
-      <c r="V3" t="s">
-        <v>765</v>
-      </c>
       <c r="W3" t="s">
-        <v>3016</v>
+        <v>3160</v>
       </c>
       <c r="X3" t="s">
-        <v>2214</v>
+        <v>3161</v>
       </c>
       <c r="Y3" t="s">
-        <v>2854</v>
+        <v>1932</v>
       </c>
       <c r="Z3" t="s">
-        <v>3021</v>
+        <v>3162</v>
       </c>
       <c r="AA3" t="s">
+        <v>3163</v>
+      </c>
+      <c r="AB3" t="s">
         <v>1929</v>
       </c>
-      <c r="AB3" t="s">
-        <v>2852</v>
-      </c>
       <c r="AC3" t="s">
-        <v>866</v>
+        <v>723</v>
       </c>
       <c r="AD3" t="s">
-        <v>2020</v>
+        <v>3164</v>
       </c>
       <c r="AE3" t="s">
-        <v>2845</v>
+        <v>1357</v>
       </c>
       <c r="AF3" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AG3" t="s">
         <v>684</v>
@@ -12974,13 +13355,13 @@
         <v>914</v>
       </c>
       <c r="AI3" t="s">
-        <v>759</v>
+        <v>1886</v>
       </c>
       <c r="AJ3" t="s">
-        <v>3108</v>
+        <v>3166</v>
       </c>
       <c r="AK3" t="s">
-        <v>3107</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -12991,16 +13372,16 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>1969</v>
       </c>
       <c r="D4" t="s">
-        <v>2968</v>
+        <v>3173</v>
       </c>
       <c r="E4" t="s">
-        <v>3109</v>
+        <v>3172</v>
       </c>
       <c r="G4" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R4" t="s">
         <v>697</v>
@@ -13009,58 +13390,58 @@
         <v>696</v>
       </c>
       <c r="T4" t="s">
-        <v>667</v>
+        <v>3156</v>
       </c>
       <c r="U4" t="s">
-        <v>2860</v>
+        <v>3167</v>
       </c>
       <c r="V4" t="s">
-        <v>651</v>
+        <v>3168</v>
       </c>
       <c r="W4" t="s">
         <v>3015</v>
       </c>
       <c r="X4" t="s">
-        <v>2186</v>
+        <v>1151</v>
       </c>
       <c r="Y4" t="s">
-        <v>2214</v>
+        <v>3169</v>
       </c>
       <c r="Z4" t="s">
-        <v>1956</v>
+        <v>3170</v>
       </c>
       <c r="AA4" t="s">
-        <v>3024</v>
+        <v>3171</v>
       </c>
       <c r="AB4" t="s">
-        <v>3025</v>
+        <v>1967</v>
       </c>
       <c r="AC4" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AD4" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AE4" t="s">
-        <v>2845</v>
+        <v>667</v>
       </c>
       <c r="AF4" t="s">
-        <v>2137</v>
+        <v>3160</v>
       </c>
       <c r="AG4" t="s">
-        <v>724</v>
+        <v>1930</v>
       </c>
       <c r="AH4" t="s">
-        <v>2867</v>
+        <v>1937</v>
       </c>
       <c r="AI4" t="s">
-        <v>256</v>
+        <v>1969</v>
       </c>
       <c r="AJ4" t="s">
-        <v>2968</v>
+        <v>3173</v>
       </c>
       <c r="AK4" t="s">
-        <v>3109</v>
+        <v>3172</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -13071,13 +13452,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>266</v>
+        <v>1885</v>
       </c>
       <c r="D5" t="s">
-        <v>3111</v>
+        <v>1981</v>
       </c>
       <c r="E5" t="s">
-        <v>3110</v>
+        <v>3175</v>
       </c>
       <c r="G5" t="s">
         <v>680</v>
@@ -13089,58 +13470,58 @@
         <v>705</v>
       </c>
       <c r="T5" t="s">
-        <v>1180</v>
+        <v>410</v>
       </c>
       <c r="U5" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="V5" t="s">
         <v>3015</v>
       </c>
       <c r="W5" t="s">
-        <v>764</v>
+        <v>3168</v>
       </c>
       <c r="X5" t="s">
-        <v>2872</v>
+        <v>3154</v>
       </c>
       <c r="Y5" t="s">
-        <v>3027</v>
+        <v>3162</v>
       </c>
       <c r="Z5" t="s">
-        <v>2854</v>
+        <v>3174</v>
       </c>
       <c r="AA5" t="s">
-        <v>3028</v>
+        <v>3163</v>
       </c>
       <c r="AB5" t="s">
-        <v>2214</v>
+        <v>767</v>
       </c>
       <c r="AC5" t="s">
-        <v>2217</v>
+        <v>1967</v>
       </c>
       <c r="AD5" t="s">
-        <v>3025</v>
+        <v>1386</v>
       </c>
       <c r="AE5" t="s">
         <v>667</v>
       </c>
       <c r="AF5" t="s">
-        <v>651</v>
+        <v>723</v>
       </c>
       <c r="AG5" t="s">
-        <v>3029</v>
+        <v>1933</v>
       </c>
       <c r="AH5" t="s">
-        <v>2020</v>
+        <v>1930</v>
       </c>
       <c r="AI5" t="s">
-        <v>266</v>
+        <v>1885</v>
       </c>
       <c r="AJ5" t="s">
-        <v>3111</v>
+        <v>1981</v>
       </c>
       <c r="AK5" t="s">
-        <v>3110</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -13151,16 +13532,16 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>1886</v>
+        <v>1910</v>
       </c>
       <c r="D6" t="s">
-        <v>3032</v>
+        <v>2245</v>
       </c>
       <c r="E6" t="s">
-        <v>3112</v>
+        <v>3182</v>
       </c>
       <c r="G6" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R6" t="s">
         <v>469</v>
@@ -13169,58 +13550,58 @@
         <v>1894</v>
       </c>
       <c r="T6" t="s">
-        <v>683</v>
+        <v>1357</v>
       </c>
       <c r="U6" t="s">
         <v>3015</v>
       </c>
       <c r="V6" t="s">
-        <v>386</v>
+        <v>3176</v>
       </c>
       <c r="W6" t="s">
-        <v>757</v>
+        <v>3177</v>
       </c>
       <c r="X6" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="Y6" t="s">
         <v>2064</v>
       </c>
       <c r="Z6" t="s">
-        <v>2219</v>
+        <v>3178</v>
       </c>
       <c r="AA6" t="s">
-        <v>2883</v>
+        <v>3179</v>
       </c>
       <c r="AB6" t="s">
         <v>1899</v>
       </c>
       <c r="AC6" t="s">
-        <v>874</v>
+        <v>1196</v>
       </c>
       <c r="AD6" t="s">
-        <v>657</v>
+        <v>3180</v>
       </c>
       <c r="AE6" t="s">
         <v>1128</v>
       </c>
       <c r="AF6" t="s">
-        <v>1178</v>
+        <v>3181</v>
       </c>
       <c r="AG6" t="s">
         <v>1206</v>
       </c>
       <c r="AH6" t="s">
-        <v>2886</v>
+        <v>2219</v>
       </c>
       <c r="AI6" t="s">
-        <v>1886</v>
+        <v>1910</v>
       </c>
       <c r="AJ6" t="s">
-        <v>3032</v>
+        <v>2245</v>
       </c>
       <c r="AK6" t="s">
-        <v>3112</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -13231,13 +13612,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>1964</v>
       </c>
       <c r="D7" t="s">
-        <v>3114</v>
+        <v>3188</v>
       </c>
       <c r="E7" t="s">
-        <v>3113</v>
+        <v>3187</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -13249,58 +13630,58 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>3014</v>
+        <v>3089</v>
       </c>
       <c r="U7" t="s">
-        <v>398</v>
+        <v>3183</v>
       </c>
       <c r="V7" t="s">
-        <v>2031</v>
+        <v>528</v>
       </c>
       <c r="W7" t="s">
-        <v>2891</v>
+        <v>3184</v>
       </c>
       <c r="X7" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="Y7" t="s">
-        <v>2854</v>
+        <v>3162</v>
       </c>
       <c r="Z7" t="s">
-        <v>2214</v>
+        <v>3163</v>
       </c>
       <c r="AA7" t="s">
-        <v>3033</v>
+        <v>3169</v>
       </c>
       <c r="AB7" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AC7" t="s">
-        <v>656</v>
+        <v>3185</v>
       </c>
       <c r="AD7" t="s">
-        <v>866</v>
+        <v>3164</v>
       </c>
       <c r="AE7" t="s">
-        <v>2893</v>
+        <v>3186</v>
       </c>
       <c r="AF7" t="s">
-        <v>1154</v>
+        <v>1427</v>
       </c>
       <c r="AG7" t="s">
         <v>724</v>
       </c>
       <c r="AH7" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AI7" t="s">
-        <v>262</v>
+        <v>1964</v>
       </c>
       <c r="AJ7" t="s">
-        <v>3114</v>
+        <v>3188</v>
       </c>
       <c r="AK7" t="s">
-        <v>3113</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -13311,16 +13692,16 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>627</v>
       </c>
       <c r="D8" t="s">
-        <v>3116</v>
+        <v>3198</v>
       </c>
       <c r="E8" t="s">
-        <v>3115</v>
+        <v>3197</v>
       </c>
       <c r="G8" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R8" t="s">
         <v>547</v>
@@ -13329,34 +13710,34 @@
         <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>2845</v>
+        <v>3189</v>
       </c>
       <c r="U8" t="s">
-        <v>764</v>
+        <v>3190</v>
       </c>
       <c r="V8" t="s">
-        <v>2860</v>
+        <v>3191</v>
       </c>
       <c r="W8" t="s">
-        <v>3015</v>
+        <v>3192</v>
       </c>
       <c r="X8" t="s">
-        <v>2854</v>
+        <v>3174</v>
       </c>
       <c r="Y8" t="s">
-        <v>3028</v>
+        <v>3193</v>
       </c>
       <c r="Z8" t="s">
-        <v>1929</v>
+        <v>767</v>
       </c>
       <c r="AA8" t="s">
-        <v>2217</v>
+        <v>3194</v>
       </c>
       <c r="AB8" t="s">
-        <v>2896</v>
+        <v>1899</v>
       </c>
       <c r="AC8" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AD8" t="s">
         <v>1196</v>
@@ -13365,22 +13746,22 @@
         <v>1806</v>
       </c>
       <c r="AF8" t="s">
-        <v>2895</v>
+        <v>799</v>
       </c>
       <c r="AG8" t="s">
-        <v>2173</v>
+        <v>3195</v>
       </c>
       <c r="AH8" t="s">
-        <v>713</v>
+        <v>3196</v>
       </c>
       <c r="AI8" t="s">
-        <v>264</v>
+        <v>627</v>
       </c>
       <c r="AJ8" t="s">
-        <v>3116</v>
+        <v>3198</v>
       </c>
       <c r="AK8" t="s">
-        <v>3115</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -13391,13 +13772,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>795</v>
+        <v>881</v>
       </c>
       <c r="D9" t="s">
-        <v>3118</v>
+        <v>3202</v>
       </c>
       <c r="E9" t="s">
-        <v>3117</v>
+        <v>3201</v>
       </c>
       <c r="G9" t="s">
         <v>627</v>
@@ -13409,58 +13790,58 @@
         <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>1180</v>
+        <v>3189</v>
       </c>
       <c r="U9" t="s">
         <v>3015</v>
       </c>
       <c r="V9" t="s">
-        <v>1266</v>
+        <v>3183</v>
       </c>
       <c r="W9" t="s">
-        <v>398</v>
+        <v>724</v>
       </c>
       <c r="X9" t="s">
-        <v>713</v>
+        <v>1929</v>
       </c>
       <c r="Y9" t="s">
-        <v>1929</v>
+        <v>3196</v>
       </c>
       <c r="Z9" t="s">
-        <v>3033</v>
+        <v>2867</v>
       </c>
       <c r="AA9" t="s">
-        <v>3037</v>
+        <v>3199</v>
       </c>
       <c r="AB9" t="s">
-        <v>656</v>
+        <v>723</v>
       </c>
       <c r="AC9" t="s">
-        <v>2020</v>
+        <v>3164</v>
       </c>
       <c r="AD9" t="s">
-        <v>866</v>
+        <v>3185</v>
       </c>
       <c r="AE9" t="s">
-        <v>2845</v>
+        <v>410</v>
       </c>
       <c r="AF9" t="s">
-        <v>2867</v>
+        <v>3169</v>
       </c>
       <c r="AG9" t="s">
-        <v>724</v>
+        <v>3200</v>
       </c>
       <c r="AH9" t="s">
         <v>2905</v>
       </c>
       <c r="AI9" t="s">
-        <v>795</v>
+        <v>881</v>
       </c>
       <c r="AJ9" t="s">
-        <v>3118</v>
+        <v>3202</v>
       </c>
       <c r="AK9" t="s">
-        <v>3117</v>
+        <v>3201</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -13471,16 +13852,16 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>1432</v>
+        <v>818</v>
       </c>
       <c r="D10" t="s">
-        <v>3120</v>
+        <v>2052</v>
       </c>
       <c r="E10" t="s">
-        <v>3119</v>
+        <v>3206</v>
       </c>
       <c r="G10" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R10" t="s">
         <v>742</v>
@@ -13489,58 +13870,58 @@
         <v>259</v>
       </c>
       <c r="T10" t="s">
-        <v>1180</v>
+        <v>410</v>
       </c>
       <c r="U10" t="s">
-        <v>3039</v>
+        <v>3203</v>
       </c>
       <c r="V10" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W10" t="s">
         <v>3015</v>
       </c>
       <c r="X10" t="s">
-        <v>2031</v>
+        <v>3194</v>
       </c>
       <c r="Y10" t="s">
-        <v>2910</v>
+        <v>3204</v>
       </c>
       <c r="Z10" t="s">
-        <v>3040</v>
+        <v>3163</v>
       </c>
       <c r="AA10" t="s">
-        <v>3041</v>
+        <v>3169</v>
       </c>
       <c r="AB10" t="s">
-        <v>2214</v>
+        <v>1967</v>
       </c>
       <c r="AC10" t="s">
-        <v>656</v>
+        <v>3164</v>
       </c>
       <c r="AD10" t="s">
-        <v>657</v>
+        <v>723</v>
       </c>
       <c r="AE10" t="s">
         <v>740</v>
       </c>
       <c r="AF10" t="s">
-        <v>2020</v>
+        <v>528</v>
       </c>
       <c r="AG10" t="s">
-        <v>2852</v>
+        <v>1941</v>
       </c>
       <c r="AH10" t="s">
-        <v>1181</v>
+        <v>3205</v>
       </c>
       <c r="AI10" t="s">
-        <v>1432</v>
+        <v>818</v>
       </c>
       <c r="AJ10" t="s">
-        <v>3120</v>
+        <v>2052</v>
       </c>
       <c r="AK10" t="s">
-        <v>3119</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -13551,13 +13932,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>290</v>
+        <v>745</v>
       </c>
       <c r="D11" t="s">
-        <v>2090</v>
+        <v>3209</v>
       </c>
       <c r="E11" t="s">
-        <v>3121</v>
+        <v>3208</v>
       </c>
       <c r="G11" t="s">
         <v>680</v>
@@ -13569,58 +13950,58 @@
         <v>746</v>
       </c>
       <c r="T11" t="s">
-        <v>918</v>
+        <v>3156</v>
       </c>
       <c r="U11" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="V11" t="s">
-        <v>3015</v>
+        <v>663</v>
       </c>
       <c r="W11" t="s">
-        <v>2031</v>
+        <v>528</v>
       </c>
       <c r="X11" t="s">
-        <v>398</v>
+        <v>3183</v>
       </c>
       <c r="Y11" t="s">
-        <v>3021</v>
+        <v>3195</v>
       </c>
       <c r="Z11" t="s">
+        <v>3169</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>3174</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>3179</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>1899</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>723</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>3207</v>
+      </c>
+      <c r="AF11" t="s">
         <v>1206</v>
       </c>
-      <c r="AA11" t="s">
-        <v>3028</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>3043</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>1899</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>2845</v>
-      </c>
-      <c r="AF11" t="s">
+      <c r="AG11" t="s">
+        <v>1932</v>
+      </c>
+      <c r="AH11" t="s">
         <v>3044</v>
       </c>
-      <c r="AG11" t="s">
-        <v>3033</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>2173</v>
-      </c>
       <c r="AI11" t="s">
-        <v>290</v>
+        <v>745</v>
       </c>
       <c r="AJ11" t="s">
-        <v>2090</v>
+        <v>3209</v>
       </c>
       <c r="AK11" t="s">
-        <v>3121</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -13631,16 +14012,16 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>645</v>
+        <v>1425</v>
       </c>
       <c r="D12" t="s">
-        <v>3123</v>
+        <v>3212</v>
       </c>
       <c r="E12" t="s">
-        <v>3122</v>
+        <v>3211</v>
       </c>
       <c r="G12" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R12" t="s">
         <v>392</v>
@@ -13649,58 +14030,58 @@
         <v>263</v>
       </c>
       <c r="T12" t="s">
-        <v>3014</v>
+        <v>3210</v>
       </c>
       <c r="U12" t="s">
-        <v>398</v>
+        <v>3183</v>
       </c>
       <c r="V12" t="s">
         <v>3046</v>
       </c>
       <c r="W12" t="s">
-        <v>2031</v>
+        <v>528</v>
       </c>
       <c r="X12" t="s">
-        <v>2854</v>
+        <v>3177</v>
       </c>
       <c r="Y12" t="s">
-        <v>3021</v>
+        <v>3194</v>
       </c>
       <c r="Z12" t="s">
-        <v>3047</v>
+        <v>1929</v>
       </c>
       <c r="AA12" t="s">
-        <v>3048</v>
+        <v>2224</v>
       </c>
       <c r="AB12" t="s">
-        <v>2214</v>
+        <v>3163</v>
       </c>
       <c r="AC12" t="s">
-        <v>1899</v>
+        <v>3155</v>
       </c>
       <c r="AD12" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AE12" t="s">
-        <v>3049</v>
+        <v>1927</v>
       </c>
       <c r="AF12" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AG12" t="s">
-        <v>2927</v>
+        <v>1932</v>
       </c>
       <c r="AH12" t="s">
         <v>2928</v>
       </c>
       <c r="AI12" t="s">
-        <v>645</v>
+        <v>1425</v>
       </c>
       <c r="AJ12" t="s">
-        <v>3123</v>
+        <v>3212</v>
       </c>
       <c r="AK12" t="s">
-        <v>3122</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -13711,16 +14092,16 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>3054</v>
+        <v>1964</v>
       </c>
       <c r="D13" t="s">
-        <v>2869</v>
+        <v>2978</v>
       </c>
       <c r="E13" t="s">
-        <v>3124</v>
+        <v>3214</v>
       </c>
       <c r="G13" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R13" t="s">
         <v>486</v>
@@ -13729,58 +14110,58 @@
         <v>265</v>
       </c>
       <c r="T13" t="s">
-        <v>3049</v>
+        <v>667</v>
       </c>
       <c r="U13" t="s">
-        <v>3053</v>
+        <v>1349</v>
       </c>
       <c r="V13" t="s">
         <v>3046</v>
       </c>
       <c r="W13" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="X13" t="s">
-        <v>2860</v>
+        <v>799</v>
       </c>
       <c r="Y13" t="s">
-        <v>3017</v>
+        <v>3213</v>
       </c>
       <c r="Z13" t="s">
-        <v>3040</v>
+        <v>3204</v>
       </c>
       <c r="AA13" t="s">
-        <v>2214</v>
+        <v>3163</v>
       </c>
       <c r="AB13" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AC13" t="s">
-        <v>3018</v>
+        <v>3169</v>
       </c>
       <c r="AD13" t="s">
-        <v>2932</v>
+        <v>666</v>
       </c>
       <c r="AE13" t="s">
-        <v>3014</v>
+        <v>1927</v>
       </c>
       <c r="AF13" t="s">
-        <v>764</v>
+        <v>723</v>
       </c>
       <c r="AG13" t="s">
-        <v>2020</v>
+        <v>1967</v>
       </c>
       <c r="AH13" t="s">
-        <v>3029</v>
+        <v>1933</v>
       </c>
       <c r="AI13" t="s">
-        <v>3054</v>
+        <v>1964</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2869</v>
+        <v>2978</v>
       </c>
       <c r="AK13" t="s">
-        <v>3124</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -13791,13 +14172,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D14" t="s">
-        <v>2232</v>
+        <v>3222</v>
       </c>
       <c r="E14" t="s">
-        <v>3125</v>
+        <v>3221</v>
       </c>
       <c r="G14" t="s">
         <v>680</v>
@@ -13809,34 +14190,34 @@
         <v>770</v>
       </c>
       <c r="T14" t="s">
-        <v>1180</v>
+        <v>3215</v>
       </c>
       <c r="U14" t="s">
-        <v>764</v>
+        <v>1349</v>
       </c>
       <c r="V14" t="s">
-        <v>3053</v>
+        <v>916</v>
       </c>
       <c r="W14" t="s">
-        <v>3056</v>
+        <v>3216</v>
       </c>
       <c r="X14" t="s">
-        <v>3057</v>
+        <v>1151</v>
       </c>
       <c r="Y14" t="s">
-        <v>2186</v>
+        <v>3217</v>
       </c>
       <c r="Z14" t="s">
-        <v>2938</v>
+        <v>3174</v>
       </c>
       <c r="AA14" t="s">
-        <v>3028</v>
+        <v>3218</v>
       </c>
       <c r="AB14" t="s">
-        <v>3058</v>
+        <v>1196</v>
       </c>
       <c r="AC14" t="s">
-        <v>874</v>
+        <v>3219</v>
       </c>
       <c r="AD14" t="s">
         <v>1899</v>
@@ -13845,22 +14226,22 @@
         <v>667</v>
       </c>
       <c r="AF14" t="s">
-        <v>651</v>
+        <v>1930</v>
       </c>
       <c r="AG14" t="s">
-        <v>2844</v>
+        <v>1933</v>
       </c>
       <c r="AH14" t="s">
-        <v>3059</v>
+        <v>3220</v>
       </c>
       <c r="AI14" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2232</v>
+        <v>3222</v>
       </c>
       <c r="AK14" t="s">
-        <v>3125</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -13871,13 +14252,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>745</v>
       </c>
       <c r="D15" t="s">
-        <v>2093</v>
+        <v>3225</v>
       </c>
       <c r="E15" t="s">
-        <v>3126</v>
+        <v>3224</v>
       </c>
       <c r="G15" t="s">
         <v>680</v>
@@ -13889,7 +14270,7 @@
         <v>774</v>
       </c>
       <c r="T15" t="s">
-        <v>2943</v>
+        <v>3215</v>
       </c>
       <c r="U15" t="s">
         <v>3046</v>
@@ -13898,49 +14279,49 @@
         <v>3015</v>
       </c>
       <c r="W15" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="X15" t="s">
-        <v>2854</v>
+        <v>3223</v>
       </c>
       <c r="Y15" t="s">
-        <v>2186</v>
+        <v>3194</v>
       </c>
       <c r="Z15" t="s">
-        <v>3048</v>
+        <v>1151</v>
       </c>
       <c r="AA15" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="AB15" t="s">
-        <v>656</v>
+        <v>3179</v>
       </c>
       <c r="AC15" t="s">
-        <v>2020</v>
+        <v>3185</v>
       </c>
       <c r="AD15" t="s">
+        <v>723</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>1927</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>2224</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="AH15" t="s">
         <v>1899</v>
       </c>
-      <c r="AE15" t="s">
-        <v>3014</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>2944</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>3062</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>2867</v>
-      </c>
       <c r="AI15" t="s">
-        <v>279</v>
+        <v>745</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2093</v>
+        <v>3225</v>
       </c>
       <c r="AK15" t="s">
-        <v>3126</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -13951,13 +14332,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>677</v>
+        <v>886</v>
       </c>
       <c r="D16" t="s">
-        <v>3118</v>
+        <v>2930</v>
       </c>
       <c r="E16" t="s">
-        <v>3127</v>
+        <v>3229</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -13969,58 +14350,58 @@
         <v>270</v>
       </c>
       <c r="T16" t="s">
-        <v>807</v>
+        <v>3226</v>
       </c>
       <c r="U16" t="s">
-        <v>3039</v>
+        <v>3205</v>
       </c>
       <c r="V16" t="s">
+        <v>3183</v>
+      </c>
+      <c r="W16" t="s">
         <v>3015</v>
       </c>
-      <c r="W16" t="s">
-        <v>398</v>
-      </c>
       <c r="X16" t="s">
-        <v>2214</v>
+        <v>1936</v>
       </c>
       <c r="Y16" t="s">
-        <v>3028</v>
+        <v>1929</v>
       </c>
       <c r="Z16" t="s">
-        <v>1929</v>
+        <v>3174</v>
       </c>
       <c r="AA16" t="s">
-        <v>2883</v>
+        <v>3171</v>
       </c>
       <c r="AB16" t="s">
-        <v>2035</v>
+        <v>3227</v>
       </c>
       <c r="AC16" t="s">
+        <v>3185</v>
+      </c>
+      <c r="AD16" t="s">
         <v>1954</v>
       </c>
-      <c r="AD16" t="s">
-        <v>656</v>
-      </c>
       <c r="AE16" t="s">
-        <v>2845</v>
+        <v>3156</v>
       </c>
       <c r="AF16" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AG16" t="s">
-        <v>2229</v>
+        <v>3163</v>
       </c>
       <c r="AH16" t="s">
-        <v>2950</v>
+        <v>3228</v>
       </c>
       <c r="AI16" t="s">
-        <v>677</v>
+        <v>886</v>
       </c>
       <c r="AJ16" t="s">
-        <v>3118</v>
+        <v>2930</v>
       </c>
       <c r="AK16" t="s">
-        <v>3127</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -14031,13 +14412,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>271</v>
+        <v>752</v>
       </c>
       <c r="D17" t="s">
-        <v>2572</v>
+        <v>3232</v>
       </c>
       <c r="E17" t="s">
-        <v>3128</v>
+        <v>3231</v>
       </c>
       <c r="G17" t="s">
         <v>680</v>
@@ -14049,58 +14430,58 @@
         <v>272</v>
       </c>
       <c r="T17" t="s">
-        <v>3014</v>
+        <v>3156</v>
       </c>
       <c r="U17" t="s">
-        <v>2031</v>
+        <v>663</v>
       </c>
       <c r="V17" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="W17" t="s">
-        <v>3015</v>
+        <v>766</v>
       </c>
       <c r="X17" t="s">
-        <v>3067</v>
+        <v>3194</v>
       </c>
       <c r="Y17" t="s">
-        <v>2854</v>
+        <v>3179</v>
       </c>
       <c r="Z17" t="s">
-        <v>2955</v>
+        <v>3174</v>
       </c>
       <c r="AA17" t="s">
-        <v>3028</v>
+        <v>3230</v>
       </c>
       <c r="AB17" t="s">
-        <v>1346</v>
+        <v>1899</v>
       </c>
       <c r="AC17" t="s">
-        <v>1899</v>
+        <v>3155</v>
       </c>
       <c r="AD17" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AE17" t="s">
-        <v>2845</v>
+        <v>1927</v>
       </c>
       <c r="AF17" t="s">
-        <v>3021</v>
+        <v>1932</v>
       </c>
       <c r="AG17" t="s">
-        <v>656</v>
+        <v>528</v>
       </c>
       <c r="AH17" t="s">
-        <v>2229</v>
+        <v>1936</v>
       </c>
       <c r="AI17" t="s">
-        <v>271</v>
+        <v>752</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2572</v>
+        <v>3232</v>
       </c>
       <c r="AK17" t="s">
-        <v>3128</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -14111,13 +14492,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>686</v>
+        <v>1942</v>
       </c>
       <c r="D18" t="s">
-        <v>2930</v>
+        <v>3235</v>
       </c>
       <c r="E18" t="s">
-        <v>3129</v>
+        <v>3234</v>
       </c>
       <c r="G18" t="s">
         <v>680</v>
@@ -14129,40 +14510,40 @@
         <v>787</v>
       </c>
       <c r="T18" t="s">
-        <v>3014</v>
+        <v>667</v>
       </c>
       <c r="U18" t="s">
-        <v>2156</v>
+        <v>3233</v>
       </c>
       <c r="V18" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W18" t="s">
         <v>3015</v>
       </c>
       <c r="X18" t="s">
-        <v>2214</v>
+        <v>3163</v>
       </c>
       <c r="Y18" t="s">
-        <v>1929</v>
+        <v>3174</v>
       </c>
       <c r="Z18" t="s">
-        <v>2883</v>
+        <v>3179</v>
       </c>
       <c r="AA18" t="s">
-        <v>2186</v>
+        <v>1151</v>
       </c>
       <c r="AB18" t="s">
-        <v>2217</v>
+        <v>767</v>
       </c>
       <c r="AC18" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AD18" t="s">
-        <v>867</v>
+        <v>3185</v>
       </c>
       <c r="AE18" t="s">
-        <v>667</v>
+        <v>1927</v>
       </c>
       <c r="AF18" t="s">
         <v>2595</v>
@@ -14174,13 +14555,13 @@
         <v>786</v>
       </c>
       <c r="AI18" t="s">
-        <v>686</v>
+        <v>1942</v>
       </c>
       <c r="AJ18" t="s">
-        <v>2930</v>
+        <v>3235</v>
       </c>
       <c r="AK18" t="s">
-        <v>3129</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -14191,16 +14572,16 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>266</v>
+        <v>1885</v>
       </c>
       <c r="D19" t="s">
-        <v>3131</v>
+        <v>3237</v>
       </c>
       <c r="E19" t="s">
-        <v>3130</v>
+        <v>3236</v>
       </c>
       <c r="G19" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R19" t="s">
         <v>347</v>
@@ -14209,58 +14590,58 @@
         <v>792</v>
       </c>
       <c r="T19" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U19" t="s">
-        <v>2860</v>
+        <v>799</v>
       </c>
       <c r="V19" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W19" t="s">
-        <v>3053</v>
+        <v>1349</v>
       </c>
       <c r="X19" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="Y19" t="s">
-        <v>3027</v>
+        <v>3169</v>
       </c>
       <c r="Z19" t="s">
-        <v>2186</v>
+        <v>1151</v>
       </c>
       <c r="AA19" t="s">
-        <v>2883</v>
+        <v>3179</v>
       </c>
       <c r="AB19" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AC19" t="s">
-        <v>656</v>
+        <v>3155</v>
       </c>
       <c r="AD19" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AE19" t="s">
-        <v>3014</v>
+        <v>1927</v>
       </c>
       <c r="AF19" t="s">
         <v>3044</v>
       </c>
       <c r="AG19" t="s">
-        <v>2229</v>
+        <v>3157</v>
       </c>
       <c r="AH19" t="s">
-        <v>1909</v>
+        <v>1936</v>
       </c>
       <c r="AI19" t="s">
-        <v>266</v>
+        <v>1885</v>
       </c>
       <c r="AJ19" t="s">
-        <v>3131</v>
+        <v>3237</v>
       </c>
       <c r="AK19" t="s">
-        <v>3130</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -14271,16 +14652,16 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>266</v>
+        <v>1886</v>
       </c>
       <c r="D20" t="s">
-        <v>3133</v>
+        <v>2030</v>
       </c>
       <c r="E20" t="s">
-        <v>3132</v>
+        <v>3239</v>
       </c>
       <c r="G20" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R20" t="s">
         <v>516</v>
@@ -14289,58 +14670,58 @@
         <v>796</v>
       </c>
       <c r="T20" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U20" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="V20" t="s">
         <v>3015</v>
       </c>
       <c r="W20" t="s">
-        <v>764</v>
+        <v>2064</v>
       </c>
       <c r="X20" t="s">
-        <v>2064</v>
+        <v>3238</v>
       </c>
       <c r="Y20" t="s">
-        <v>3027</v>
+        <v>3179</v>
       </c>
       <c r="Z20" t="s">
-        <v>2883</v>
+        <v>3194</v>
       </c>
       <c r="AA20" t="s">
-        <v>2854</v>
+        <v>3174</v>
       </c>
       <c r="AB20" t="s">
-        <v>3028</v>
+        <v>3204</v>
       </c>
       <c r="AC20" t="s">
-        <v>656</v>
+        <v>3155</v>
       </c>
       <c r="AD20" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AE20" t="s">
         <v>1806</v>
       </c>
       <c r="AF20" t="s">
+        <v>1899</v>
+      </c>
+      <c r="AG20" t="s">
         <v>915</v>
       </c>
-      <c r="AG20" t="s">
-        <v>1899</v>
-      </c>
       <c r="AH20" t="s">
-        <v>2966</v>
+        <v>1933</v>
       </c>
       <c r="AI20" t="s">
-        <v>266</v>
+        <v>1886</v>
       </c>
       <c r="AJ20" t="s">
-        <v>3133</v>
+        <v>2030</v>
       </c>
       <c r="AK20" t="s">
-        <v>3132</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -14351,16 +14732,16 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>3054</v>
+        <v>1886</v>
       </c>
       <c r="D21" t="s">
-        <v>2055</v>
+        <v>2118</v>
       </c>
       <c r="E21" t="s">
-        <v>3134</v>
+        <v>3240</v>
       </c>
       <c r="G21" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R21" t="s">
         <v>375</v>
@@ -14369,58 +14750,58 @@
         <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U21" t="s">
         <v>3015</v>
       </c>
       <c r="V21" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W21" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="X21" t="s">
-        <v>3067</v>
+        <v>3194</v>
       </c>
       <c r="Y21" t="s">
-        <v>2854</v>
+        <v>3163</v>
       </c>
       <c r="Z21" t="s">
-        <v>2214</v>
+        <v>3179</v>
       </c>
       <c r="AA21" t="s">
-        <v>1346</v>
+        <v>3174</v>
       </c>
       <c r="AB21" t="s">
-        <v>3075</v>
+        <v>1151</v>
       </c>
       <c r="AC21" t="s">
-        <v>2186</v>
+        <v>3180</v>
       </c>
       <c r="AD21" t="s">
-        <v>657</v>
+        <v>1954</v>
       </c>
       <c r="AE21" t="s">
         <v>667</v>
       </c>
       <c r="AF21" t="s">
-        <v>1954</v>
+        <v>1967</v>
       </c>
       <c r="AG21" t="s">
-        <v>656</v>
+        <v>3157</v>
       </c>
       <c r="AH21" t="s">
-        <v>1909</v>
+        <v>1933</v>
       </c>
       <c r="AI21" t="s">
-        <v>3054</v>
+        <v>1886</v>
       </c>
       <c r="AJ21" t="s">
-        <v>2055</v>
+        <v>2118</v>
       </c>
       <c r="AK21" t="s">
-        <v>3134</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -14431,13 +14812,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>1183</v>
+        <v>795</v>
       </c>
       <c r="D22" t="s">
-        <v>3136</v>
+        <v>2096</v>
       </c>
       <c r="E22" t="s">
-        <v>3135</v>
+        <v>3243</v>
       </c>
       <c r="G22" t="s">
         <v>627</v>
@@ -14449,43 +14830,43 @@
         <v>804</v>
       </c>
       <c r="T22" t="s">
-        <v>3014</v>
+        <v>3215</v>
       </c>
       <c r="U22" t="s">
         <v>3015</v>
       </c>
       <c r="V22" t="s">
-        <v>2860</v>
+        <v>799</v>
       </c>
       <c r="W22" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="X22" t="s">
-        <v>1346</v>
+        <v>3230</v>
       </c>
       <c r="Y22" t="s">
-        <v>2852</v>
+        <v>3161</v>
       </c>
       <c r="Z22" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="AA22" t="s">
-        <v>2910</v>
+        <v>3241</v>
       </c>
       <c r="AB22" t="s">
+        <v>3242</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>3185</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>723</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>1927</v>
+      </c>
+      <c r="AF22" t="s">
         <v>1899</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>656</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>2963</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>2972</v>
       </c>
       <c r="AG22" t="s">
         <v>2928</v>
@@ -14494,13 +14875,13 @@
         <v>2927</v>
       </c>
       <c r="AI22" t="s">
-        <v>1183</v>
+        <v>795</v>
       </c>
       <c r="AJ22" t="s">
-        <v>3136</v>
+        <v>2096</v>
       </c>
       <c r="AK22" t="s">
-        <v>3135</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -14511,16 +14892,16 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>273</v>
+        <v>1963</v>
       </c>
       <c r="D23" t="s">
-        <v>3081</v>
+        <v>1994</v>
       </c>
       <c r="E23" t="s">
-        <v>3137</v>
+        <v>3247</v>
       </c>
       <c r="G23" t="s">
-        <v>627</v>
+        <v>552</v>
       </c>
       <c r="R23" t="s">
         <v>809</v>
@@ -14529,58 +14910,58 @@
         <v>281</v>
       </c>
       <c r="T23" t="s">
-        <v>3079</v>
+        <v>3244</v>
       </c>
       <c r="U23" t="s">
         <v>3015</v>
       </c>
       <c r="V23" t="s">
-        <v>3053</v>
+        <v>1349</v>
       </c>
       <c r="W23" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="X23" t="s">
-        <v>2031</v>
+        <v>3192</v>
       </c>
       <c r="Y23" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="Z23" t="s">
-        <v>2883</v>
+        <v>3171</v>
       </c>
       <c r="AA23" t="s">
-        <v>664</v>
+        <v>3238</v>
       </c>
       <c r="AB23" t="s">
-        <v>3027</v>
+        <v>3245</v>
       </c>
       <c r="AC23" t="s">
-        <v>2214</v>
+        <v>723</v>
       </c>
       <c r="AD23" t="s">
-        <v>656</v>
+        <v>3246</v>
       </c>
       <c r="AE23" t="s">
         <v>373</v>
       </c>
       <c r="AF23" t="s">
-        <v>651</v>
+        <v>1930</v>
       </c>
       <c r="AG23" t="s">
-        <v>2020</v>
+        <v>1937</v>
       </c>
       <c r="AH23" t="s">
-        <v>3029</v>
+        <v>1967</v>
       </c>
       <c r="AI23" t="s">
-        <v>273</v>
+        <v>1963</v>
       </c>
       <c r="AJ23" t="s">
-        <v>3081</v>
+        <v>1994</v>
       </c>
       <c r="AK23" t="s">
-        <v>3137</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -14591,16 +14972,16 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>1472</v>
+        <v>759</v>
       </c>
       <c r="D24" t="s">
-        <v>2260</v>
+        <v>3254</v>
       </c>
       <c r="E24" t="s">
-        <v>3138</v>
+        <v>3253</v>
       </c>
       <c r="G24" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R24" t="s">
         <v>562</v>
@@ -14609,58 +14990,58 @@
         <v>283</v>
       </c>
       <c r="T24" t="s">
-        <v>3014</v>
+        <v>667</v>
       </c>
       <c r="U24" t="s">
-        <v>3016</v>
+        <v>2016</v>
       </c>
       <c r="V24" t="s">
-        <v>3067</v>
+        <v>3248</v>
       </c>
       <c r="W24" t="s">
         <v>3015</v>
       </c>
       <c r="X24" t="s">
-        <v>2854</v>
+        <v>3249</v>
       </c>
       <c r="Y24" t="s">
-        <v>3082</v>
+        <v>3250</v>
       </c>
       <c r="Z24" t="s">
-        <v>3028</v>
+        <v>3251</v>
       </c>
       <c r="AA24" t="s">
-        <v>1929</v>
+        <v>3169</v>
       </c>
       <c r="AB24" t="s">
-        <v>1355</v>
+        <v>3230</v>
       </c>
       <c r="AC24" t="s">
-        <v>874</v>
+        <v>3164</v>
       </c>
       <c r="AD24" t="s">
-        <v>2981</v>
+        <v>723</v>
       </c>
       <c r="AE24" t="s">
-        <v>667</v>
+        <v>1927</v>
       </c>
       <c r="AF24" t="s">
-        <v>3021</v>
+        <v>3200</v>
       </c>
       <c r="AG24" t="s">
-        <v>3083</v>
+        <v>3252</v>
       </c>
       <c r="AH24" t="s">
-        <v>1909</v>
+        <v>1933</v>
       </c>
       <c r="AI24" t="s">
-        <v>1472</v>
+        <v>759</v>
       </c>
       <c r="AJ24" t="s">
-        <v>2260</v>
+        <v>3254</v>
       </c>
       <c r="AK24" t="s">
-        <v>3138</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -14671,13 +15052,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>1910</v>
+        <v>2957</v>
       </c>
       <c r="D25" t="s">
-        <v>3140</v>
+        <v>3260</v>
       </c>
       <c r="E25" t="s">
-        <v>3139</v>
+        <v>3259</v>
       </c>
       <c r="G25" t="s">
         <v>627</v>
@@ -14689,58 +15070,58 @@
         <v>461</v>
       </c>
       <c r="T25" t="s">
+        <v>2986</v>
+      </c>
+      <c r="U25" t="s">
+        <v>2928</v>
+      </c>
+      <c r="V25" t="s">
+        <v>2927</v>
+      </c>
+      <c r="W25" t="s">
+        <v>3183</v>
+      </c>
+      <c r="X25" t="s">
+        <v>2001</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>3255</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1940</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>3256</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>3185</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>3257</v>
+      </c>
+      <c r="AE25" t="s">
         <v>667</v>
       </c>
-      <c r="U25" t="s">
-        <v>398</v>
-      </c>
-      <c r="V25" t="s">
-        <v>2988</v>
-      </c>
-      <c r="W25" t="s">
-        <v>2928</v>
-      </c>
-      <c r="X25" t="s">
-        <v>921</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>2840</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>3017</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>1138</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>656</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>2234</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>1355</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>2986</v>
-      </c>
       <c r="AF25" t="s">
-        <v>2927</v>
+        <v>3192</v>
       </c>
       <c r="AG25" t="s">
         <v>724</v>
       </c>
       <c r="AH25" t="s">
-        <v>2966</v>
+        <v>3258</v>
       </c>
       <c r="AI25" t="s">
-        <v>1910</v>
+        <v>2957</v>
       </c>
       <c r="AJ25" t="s">
-        <v>3140</v>
+        <v>3260</v>
       </c>
       <c r="AK25" t="s">
-        <v>3139</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -14751,13 +15132,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>1188</v>
+        <v>795</v>
       </c>
       <c r="D26" t="s">
-        <v>3142</v>
+        <v>2252</v>
       </c>
       <c r="E26" t="s">
-        <v>3141</v>
+        <v>3262</v>
       </c>
       <c r="G26" t="s">
         <v>680</v>
@@ -14769,58 +15150,58 @@
         <v>572</v>
       </c>
       <c r="T26" t="s">
-        <v>3014</v>
+        <v>1357</v>
       </c>
       <c r="U26" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="V26" t="s">
         <v>3015</v>
       </c>
       <c r="W26" t="s">
-        <v>3090</v>
+        <v>3261</v>
       </c>
       <c r="X26" t="s">
-        <v>651</v>
+        <v>3163</v>
       </c>
       <c r="Y26" t="s">
-        <v>2214</v>
+        <v>3174</v>
       </c>
       <c r="Z26" t="s">
-        <v>3028</v>
+        <v>3194</v>
       </c>
       <c r="AA26" t="s">
-        <v>2910</v>
+        <v>3171</v>
       </c>
       <c r="AB26" t="s">
-        <v>2883</v>
+        <v>3170</v>
       </c>
       <c r="AC26" t="s">
-        <v>656</v>
+        <v>1967</v>
       </c>
       <c r="AD26" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AE26" t="s">
-        <v>683</v>
+        <v>1927</v>
       </c>
       <c r="AF26" t="s">
+        <v>1930</v>
+      </c>
+      <c r="AG26" t="s">
         <v>1899</v>
       </c>
-      <c r="AG26" t="s">
-        <v>3091</v>
-      </c>
       <c r="AH26" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AI26" t="s">
-        <v>1188</v>
+        <v>795</v>
       </c>
       <c r="AJ26" t="s">
-        <v>3142</v>
+        <v>2252</v>
       </c>
       <c r="AK26" t="s">
-        <v>3141</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -14831,16 +15212,16 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>1432</v>
+        <v>1885</v>
       </c>
       <c r="D27" t="s">
-        <v>3144</v>
+        <v>3264</v>
       </c>
       <c r="E27" t="s">
-        <v>3143</v>
+        <v>3263</v>
       </c>
       <c r="G27" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R27" t="s">
         <v>828</v>
@@ -14849,58 +15230,58 @@
         <v>827</v>
       </c>
       <c r="T27" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U27" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="V27" t="s">
         <v>3015</v>
       </c>
       <c r="W27" t="s">
-        <v>3053</v>
+        <v>1349</v>
       </c>
       <c r="X27" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="Y27" t="s">
-        <v>3075</v>
+        <v>3174</v>
       </c>
       <c r="Z27" t="s">
-        <v>2883</v>
+        <v>3179</v>
       </c>
       <c r="AA27" t="s">
-        <v>2852</v>
+        <v>1151</v>
       </c>
       <c r="AB27" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AC27" t="s">
         <v>1899</v>
       </c>
       <c r="AD27" t="s">
-        <v>656</v>
+        <v>3180</v>
       </c>
       <c r="AE27" t="s">
         <v>667</v>
       </c>
       <c r="AF27" t="s">
-        <v>2031</v>
+        <v>528</v>
       </c>
       <c r="AG27" t="s">
-        <v>669</v>
+        <v>1140</v>
       </c>
       <c r="AH27" t="s">
         <v>2927</v>
       </c>
       <c r="AI27" t="s">
-        <v>1432</v>
+        <v>1885</v>
       </c>
       <c r="AJ27" t="s">
-        <v>3144</v>
+        <v>3264</v>
       </c>
       <c r="AK27" t="s">
-        <v>3143</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -14911,16 +15292,16 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>273</v>
+        <v>759</v>
       </c>
       <c r="D28" t="s">
-        <v>3146</v>
+        <v>3267</v>
       </c>
       <c r="E28" t="s">
-        <v>3145</v>
+        <v>3266</v>
       </c>
       <c r="G28" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R28" t="s">
         <v>832</v>
@@ -14929,10 +15310,10 @@
         <v>831</v>
       </c>
       <c r="T28" t="s">
-        <v>3014</v>
+        <v>3156</v>
       </c>
       <c r="U28" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="V28" t="s">
         <v>3046</v>
@@ -14941,46 +15322,46 @@
         <v>3015</v>
       </c>
       <c r="X28" t="s">
-        <v>3067</v>
+        <v>766</v>
       </c>
       <c r="Y28" t="s">
-        <v>3027</v>
+        <v>3169</v>
       </c>
       <c r="Z28" t="s">
-        <v>2883</v>
+        <v>3179</v>
       </c>
       <c r="AA28" t="s">
-        <v>3041</v>
+        <v>3170</v>
       </c>
       <c r="AB28" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AC28" t="s">
-        <v>3025</v>
+        <v>1967</v>
       </c>
       <c r="AD28" t="s">
         <v>1954</v>
       </c>
       <c r="AE28" t="s">
-        <v>2845</v>
+        <v>1927</v>
       </c>
       <c r="AF28" t="s">
-        <v>3029</v>
+        <v>1386</v>
       </c>
       <c r="AG28" t="s">
-        <v>3095</v>
+        <v>3265</v>
       </c>
       <c r="AH28" t="s">
-        <v>3091</v>
+        <v>1941</v>
       </c>
       <c r="AI28" t="s">
-        <v>273</v>
+        <v>759</v>
       </c>
       <c r="AJ28" t="s">
-        <v>3146</v>
+        <v>3267</v>
       </c>
       <c r="AK28" t="s">
-        <v>3145</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -14991,16 +15372,16 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>271</v>
+        <v>759</v>
       </c>
       <c r="D29" t="s">
-        <v>3148</v>
+        <v>3271</v>
       </c>
       <c r="E29" t="s">
-        <v>3147</v>
+        <v>3270</v>
       </c>
       <c r="G29" t="s">
-        <v>680</v>
+        <v>646</v>
       </c>
       <c r="R29" t="s">
         <v>837</v>
@@ -15009,58 +15390,58 @@
         <v>836</v>
       </c>
       <c r="T29" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U29" t="s">
-        <v>398</v>
+        <v>3183</v>
       </c>
       <c r="V29" t="s">
-        <v>764</v>
+        <v>663</v>
       </c>
       <c r="W29" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="X29" t="s">
-        <v>3015</v>
+        <v>3169</v>
       </c>
       <c r="Y29" t="s">
-        <v>2852</v>
+        <v>3170</v>
       </c>
       <c r="Z29" t="s">
-        <v>3028</v>
+        <v>3194</v>
       </c>
       <c r="AA29" t="s">
-        <v>2854</v>
+        <v>3174</v>
       </c>
       <c r="AB29" t="s">
         <v>2197</v>
       </c>
       <c r="AC29" t="s">
-        <v>3098</v>
+        <v>1954</v>
       </c>
       <c r="AD29" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AE29" t="s">
         <v>667</v>
       </c>
       <c r="AF29" t="s">
-        <v>3001</v>
+        <v>3268</v>
       </c>
       <c r="AG29" t="s">
-        <v>512</v>
+        <v>3269</v>
       </c>
       <c r="AH29" t="s">
-        <v>3091</v>
+        <v>1933</v>
       </c>
       <c r="AI29" t="s">
-        <v>271</v>
+        <v>759</v>
       </c>
       <c r="AJ29" t="s">
-        <v>3148</v>
+        <v>3271</v>
       </c>
       <c r="AK29" t="s">
-        <v>3147</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -15071,16 +15452,16 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>250</v>
+        <v>1969</v>
       </c>
       <c r="D30" t="s">
-        <v>3072</v>
+        <v>3273</v>
       </c>
       <c r="E30" t="s">
-        <v>3149</v>
+        <v>3272</v>
       </c>
       <c r="G30" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R30" t="s">
         <v>840</v>
@@ -15089,58 +15470,58 @@
         <v>289</v>
       </c>
       <c r="T30" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U30" t="s">
         <v>3015</v>
       </c>
       <c r="V30" t="s">
-        <v>2872</v>
+        <v>3168</v>
       </c>
       <c r="W30" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="X30" t="s">
         <v>2064</v>
       </c>
       <c r="Y30" t="s">
-        <v>2214</v>
+        <v>3163</v>
       </c>
       <c r="Z30" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AA30" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="AB30" t="s">
-        <v>1956</v>
+        <v>3179</v>
       </c>
       <c r="AC30" t="s">
-        <v>3041</v>
+        <v>723</v>
       </c>
       <c r="AD30" t="s">
-        <v>874</v>
+        <v>1196</v>
       </c>
       <c r="AE30" t="s">
         <v>667</v>
       </c>
       <c r="AF30" t="s">
+        <v>1941</v>
+      </c>
+      <c r="AG30" t="s">
         <v>1899</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>2020</v>
       </c>
       <c r="AH30" t="s">
         <v>2837</v>
       </c>
       <c r="AI30" t="s">
-        <v>250</v>
+        <v>1969</v>
       </c>
       <c r="AJ30" t="s">
-        <v>3072</v>
+        <v>3273</v>
       </c>
       <c r="AK30" t="s">
-        <v>3149</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -15151,16 +15532,16 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>3054</v>
+        <v>1885</v>
       </c>
       <c r="D31" t="s">
-        <v>2616</v>
+        <v>3276</v>
       </c>
       <c r="E31" t="s">
-        <v>3150</v>
+        <v>3275</v>
       </c>
       <c r="G31" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R31" t="s">
         <v>844</v>
@@ -15169,58 +15550,58 @@
         <v>843</v>
       </c>
       <c r="T31" t="s">
-        <v>2963</v>
+        <v>3215</v>
       </c>
       <c r="U31" t="s">
-        <v>3053</v>
+        <v>1349</v>
       </c>
       <c r="V31" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W31" t="s">
         <v>3015</v>
       </c>
       <c r="X31" t="s">
-        <v>2883</v>
+        <v>3171</v>
       </c>
       <c r="Y31" t="s">
-        <v>3075</v>
+        <v>3174</v>
       </c>
       <c r="Z31" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AA31" t="s">
-        <v>2852</v>
+        <v>3170</v>
       </c>
       <c r="AB31" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AC31" t="s">
         <v>1954</v>
       </c>
       <c r="AD31" t="s">
-        <v>657</v>
+        <v>3164</v>
       </c>
       <c r="AE31" t="s">
         <v>667</v>
       </c>
       <c r="AF31" t="s">
-        <v>3021</v>
+        <v>1932</v>
       </c>
       <c r="AG31" t="s">
-        <v>3006</v>
+        <v>3274</v>
       </c>
       <c r="AH31" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AI31" t="s">
-        <v>3054</v>
+        <v>1885</v>
       </c>
       <c r="AJ31" t="s">
-        <v>2616</v>
+        <v>3276</v>
       </c>
       <c r="AK31" t="s">
-        <v>3150</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -15231,16 +15612,16 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>1188</v>
+        <v>818</v>
       </c>
       <c r="D32" t="s">
-        <v>3152</v>
+        <v>3279</v>
       </c>
       <c r="E32" t="s">
-        <v>3151</v>
+        <v>3278</v>
       </c>
       <c r="G32" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R32" t="s">
         <v>494</v>
@@ -15249,58 +15630,58 @@
         <v>849</v>
       </c>
       <c r="T32" t="s">
-        <v>1180</v>
+        <v>410</v>
       </c>
       <c r="U32" t="s">
-        <v>398</v>
+        <v>3183</v>
       </c>
       <c r="V32" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W32" t="s">
         <v>3015</v>
       </c>
       <c r="X32" t="s">
-        <v>1956</v>
+        <v>3163</v>
       </c>
       <c r="Y32" t="s">
-        <v>2854</v>
+        <v>3179</v>
       </c>
       <c r="Z32" t="s">
-        <v>3028</v>
+        <v>3194</v>
       </c>
       <c r="AA32" t="s">
-        <v>2186</v>
+        <v>3174</v>
       </c>
       <c r="AB32" t="s">
-        <v>3102</v>
+        <v>3204</v>
       </c>
       <c r="AC32" t="s">
-        <v>656</v>
+        <v>3185</v>
       </c>
       <c r="AD32" t="s">
-        <v>2020</v>
+        <v>723</v>
       </c>
       <c r="AE32" t="s">
         <v>667</v>
       </c>
       <c r="AF32" t="s">
-        <v>2214</v>
+        <v>2905</v>
       </c>
       <c r="AG32" t="s">
-        <v>2905</v>
+        <v>3277</v>
       </c>
       <c r="AH32" t="s">
         <v>2837</v>
       </c>
       <c r="AI32" t="s">
-        <v>1188</v>
+        <v>818</v>
       </c>
       <c r="AJ32" t="s">
-        <v>3152</v>
+        <v>3279</v>
       </c>
       <c r="AK32" t="s">
-        <v>3151</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -15311,13 +15692,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>266</v>
+        <v>1969</v>
       </c>
       <c r="D33" t="s">
-        <v>1975</v>
+        <v>3271</v>
       </c>
       <c r="E33" t="s">
-        <v>3153</v>
+        <v>3280</v>
       </c>
       <c r="G33" t="s">
         <v>680</v>
@@ -15329,58 +15710,58 @@
         <v>241</v>
       </c>
       <c r="T33" t="s">
-        <v>3014</v>
+        <v>667</v>
       </c>
       <c r="U33" t="s">
-        <v>3067</v>
+        <v>766</v>
       </c>
       <c r="V33" t="s">
-        <v>3016</v>
+        <v>663</v>
       </c>
       <c r="W33" t="s">
         <v>3015</v>
       </c>
       <c r="X33" t="s">
-        <v>3028</v>
+        <v>3174</v>
       </c>
       <c r="Y33" t="s">
-        <v>2852</v>
+        <v>3163</v>
       </c>
       <c r="Z33" t="s">
-        <v>3027</v>
+        <v>3179</v>
       </c>
       <c r="AA33" t="s">
-        <v>2854</v>
+        <v>3194</v>
       </c>
       <c r="AB33" t="s">
-        <v>2214</v>
+        <v>723</v>
       </c>
       <c r="AC33" t="s">
-        <v>657</v>
+        <v>3180</v>
       </c>
       <c r="AD33" t="s">
         <v>1899</v>
       </c>
       <c r="AE33" t="s">
-        <v>667</v>
+        <v>1927</v>
       </c>
       <c r="AF33" t="s">
-        <v>2020</v>
+        <v>3161</v>
       </c>
       <c r="AG33" t="s">
         <v>2927</v>
       </c>
       <c r="AH33" t="s">
-        <v>1909</v>
+        <v>3157</v>
       </c>
       <c r="AI33" t="s">
-        <v>266</v>
+        <v>1969</v>
       </c>
       <c r="AJ33" t="s">
-        <v>1975</v>
+        <v>3271</v>
       </c>
       <c r="AK33" t="s">
-        <v>3153</v>
+        <v>3280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GW 25 after LEIWHU
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14139" uniqueCount="3281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14939" uniqueCount="3299">
   <si>
     <t>Places</t>
   </si>
@@ -9877,6 +9877,60 @@
   </si>
   <si>
     <t>102,895</t>
+  </si>
+  <si>
+    <t>2,149,465</t>
+  </si>
+  <si>
+    <t>Bowen 10</t>
+  </si>
+  <si>
+    <t>3,294,219</t>
+  </si>
+  <si>
+    <t>Maddison 5</t>
+  </si>
+  <si>
+    <t>1,500,198</t>
+  </si>
+  <si>
+    <t>3,408,831</t>
+  </si>
+  <si>
+    <t>Veltman 7, MUN (A)</t>
+  </si>
+  <si>
+    <t>1,307,520</t>
+  </si>
+  <si>
+    <t>541,971</t>
+  </si>
+  <si>
+    <t>1,336,760</t>
+  </si>
+  <si>
+    <t>1,166,229</t>
+  </si>
+  <si>
+    <t>1,262,884</t>
+  </si>
+  <si>
+    <t>1,034,565</t>
+  </si>
+  <si>
+    <t>Bowen 20$ captain</t>
+  </si>
+  <si>
+    <t>Daka 2</t>
+  </si>
+  <si>
+    <t>624,953</t>
+  </si>
+  <si>
+    <t>37,835</t>
+  </si>
+  <si>
+    <t>610,921</t>
   </si>
 </sst>
 </file>
@@ -13072,8 +13126,8 @@
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="31.82421875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="30.703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="38.89453125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="19.06640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="20.34765625" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
@@ -13212,13 +13266,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>1297</v>
+        <v>627</v>
       </c>
       <c r="D2" t="s">
         <v>3159</v>
       </c>
       <c r="E2" t="s">
-        <v>3158</v>
+        <v>3281</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -13230,7 +13284,7 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>1927</v>
+        <v>3089</v>
       </c>
       <c r="U2" t="s">
         <v>3015</v>
@@ -13245,7 +13299,7 @@
         <v>357</v>
       </c>
       <c r="Y2" t="s">
-        <v>2001</v>
+        <v>2840</v>
       </c>
       <c r="Z2" t="s">
         <v>1929</v>
@@ -13275,13 +13329,13 @@
         <v>1930</v>
       </c>
       <c r="AI2" t="s">
-        <v>1297</v>
+        <v>627</v>
       </c>
       <c r="AJ2" t="s">
         <v>3159</v>
       </c>
       <c r="AK2" t="s">
-        <v>3158</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -13292,13 +13346,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>1886</v>
+        <v>686</v>
       </c>
       <c r="D3" t="s">
         <v>3166</v>
       </c>
       <c r="E3" t="s">
-        <v>3165</v>
+        <v>3283</v>
       </c>
       <c r="G3" t="s">
         <v>627</v>
@@ -13328,7 +13382,7 @@
         <v>1932</v>
       </c>
       <c r="Z3" t="s">
-        <v>3162</v>
+        <v>3282</v>
       </c>
       <c r="AA3" t="s">
         <v>3163</v>
@@ -13355,13 +13409,13 @@
         <v>914</v>
       </c>
       <c r="AI3" t="s">
-        <v>1886</v>
+        <v>686</v>
       </c>
       <c r="AJ3" t="s">
         <v>3166</v>
       </c>
       <c r="AK3" t="s">
-        <v>3165</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -13452,7 +13506,7 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>1885</v>
+        <v>686</v>
       </c>
       <c r="D5" t="s">
         <v>1981</v>
@@ -13485,7 +13539,7 @@
         <v>3154</v>
       </c>
       <c r="Y5" t="s">
-        <v>3162</v>
+        <v>3282</v>
       </c>
       <c r="Z5" t="s">
         <v>3174</v>
@@ -13494,7 +13548,7 @@
         <v>3163</v>
       </c>
       <c r="AB5" t="s">
-        <v>767</v>
+        <v>3284</v>
       </c>
       <c r="AC5" t="s">
         <v>1967</v>
@@ -13515,7 +13569,7 @@
         <v>1930</v>
       </c>
       <c r="AI5" t="s">
-        <v>1885</v>
+        <v>686</v>
       </c>
       <c r="AJ5" t="s">
         <v>1981</v>
@@ -13538,7 +13592,7 @@
         <v>2245</v>
       </c>
       <c r="E6" t="s">
-        <v>3182</v>
+        <v>3285</v>
       </c>
       <c r="G6" t="s">
         <v>627</v>
@@ -13601,7 +13655,7 @@
         <v>2245</v>
       </c>
       <c r="AK6" t="s">
-        <v>3182</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -13612,13 +13666,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>1964</v>
+        <v>627</v>
       </c>
       <c r="D7" t="s">
         <v>3188</v>
       </c>
       <c r="E7" t="s">
-        <v>3187</v>
+        <v>3286</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -13630,7 +13684,7 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>3089</v>
+        <v>1927</v>
       </c>
       <c r="U7" t="s">
         <v>3183</v>
@@ -13645,7 +13699,7 @@
         <v>3174</v>
       </c>
       <c r="Y7" t="s">
-        <v>3162</v>
+        <v>3282</v>
       </c>
       <c r="Z7" t="s">
         <v>3163</v>
@@ -13657,7 +13711,7 @@
         <v>723</v>
       </c>
       <c r="AC7" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD7" t="s">
         <v>3164</v>
@@ -13675,13 +13729,13 @@
         <v>3157</v>
       </c>
       <c r="AI7" t="s">
-        <v>1964</v>
+        <v>627</v>
       </c>
       <c r="AJ7" t="s">
         <v>3188</v>
       </c>
       <c r="AK7" t="s">
-        <v>3187</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -13692,7 +13746,7 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>627</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
         <v>3198</v>
@@ -13710,13 +13764,13 @@
         <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>3189</v>
+        <v>3156</v>
       </c>
       <c r="U8" t="s">
-        <v>3190</v>
+        <v>3287</v>
       </c>
       <c r="V8" t="s">
-        <v>3191</v>
+        <v>3015</v>
       </c>
       <c r="W8" t="s">
         <v>3192</v>
@@ -13728,10 +13782,10 @@
         <v>3193</v>
       </c>
       <c r="Z8" t="s">
-        <v>767</v>
+        <v>3284</v>
       </c>
       <c r="AA8" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AB8" t="s">
         <v>1899</v>
@@ -13755,7 +13809,7 @@
         <v>3196</v>
       </c>
       <c r="AI8" t="s">
-        <v>627</v>
+        <v>242</v>
       </c>
       <c r="AJ8" t="s">
         <v>3198</v>
@@ -13772,13 +13826,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>881</v>
+        <v>848</v>
       </c>
       <c r="D9" t="s">
         <v>3202</v>
       </c>
       <c r="E9" t="s">
-        <v>3201</v>
+        <v>3288</v>
       </c>
       <c r="G9" t="s">
         <v>627</v>
@@ -13790,7 +13844,7 @@
         <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>3189</v>
+        <v>3156</v>
       </c>
       <c r="U9" t="s">
         <v>3015</v>
@@ -13820,7 +13874,7 @@
         <v>3164</v>
       </c>
       <c r="AD9" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AE9" t="s">
         <v>410</v>
@@ -13835,13 +13889,13 @@
         <v>2905</v>
       </c>
       <c r="AI9" t="s">
-        <v>881</v>
+        <v>848</v>
       </c>
       <c r="AJ9" t="s">
         <v>3202</v>
       </c>
       <c r="AK9" t="s">
-        <v>3201</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -13852,7 +13906,7 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>818</v>
+        <v>745</v>
       </c>
       <c r="D10" t="s">
         <v>2052</v>
@@ -13882,7 +13936,7 @@
         <v>3015</v>
       </c>
       <c r="X10" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Y10" t="s">
         <v>3204</v>
@@ -13915,7 +13969,7 @@
         <v>3205</v>
       </c>
       <c r="AI10" t="s">
-        <v>818</v>
+        <v>745</v>
       </c>
       <c r="AJ10" t="s">
         <v>2052</v>
@@ -14012,13 +14066,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>1425</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
         <v>3212</v>
       </c>
       <c r="E12" t="s">
-        <v>3211</v>
+        <v>3289</v>
       </c>
       <c r="G12" t="s">
         <v>426</v>
@@ -14045,7 +14099,7 @@
         <v>3177</v>
       </c>
       <c r="Y12" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Z12" t="s">
         <v>1929</v>
@@ -14075,13 +14129,13 @@
         <v>2928</v>
       </c>
       <c r="AI12" t="s">
-        <v>1425</v>
+        <v>244</v>
       </c>
       <c r="AJ12" t="s">
         <v>3212</v>
       </c>
       <c r="AK12" t="s">
-        <v>3211</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -14092,13 +14146,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>1964</v>
+        <v>1969</v>
       </c>
       <c r="D13" t="s">
         <v>2978</v>
       </c>
       <c r="E13" t="s">
-        <v>3214</v>
+        <v>3290</v>
       </c>
       <c r="G13" t="s">
         <v>426</v>
@@ -14134,7 +14188,7 @@
         <v>3163</v>
       </c>
       <c r="AB13" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AC13" t="s">
         <v>3169</v>
@@ -14155,13 +14209,13 @@
         <v>1933</v>
       </c>
       <c r="AI13" t="s">
-        <v>1964</v>
+        <v>1969</v>
       </c>
       <c r="AJ13" t="s">
         <v>2978</v>
       </c>
       <c r="AK13" t="s">
-        <v>3214</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -14178,7 +14232,7 @@
         <v>3222</v>
       </c>
       <c r="E14" t="s">
-        <v>3221</v>
+        <v>3291</v>
       </c>
       <c r="G14" t="s">
         <v>680</v>
@@ -14241,7 +14295,7 @@
         <v>3222</v>
       </c>
       <c r="AK14" t="s">
-        <v>3221</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -14252,7 +14306,7 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>745</v>
+        <v>246</v>
       </c>
       <c r="D15" t="s">
         <v>3225</v>
@@ -14285,7 +14339,7 @@
         <v>3223</v>
       </c>
       <c r="Y15" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Z15" t="s">
         <v>1151</v>
@@ -14297,7 +14351,7 @@
         <v>3179</v>
       </c>
       <c r="AC15" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD15" t="s">
         <v>723</v>
@@ -14315,7 +14369,7 @@
         <v>1899</v>
       </c>
       <c r="AI15" t="s">
-        <v>745</v>
+        <v>246</v>
       </c>
       <c r="AJ15" t="s">
         <v>3225</v>
@@ -14332,13 +14386,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>886</v>
+        <v>818</v>
       </c>
       <c r="D16" t="s">
         <v>2930</v>
       </c>
       <c r="E16" t="s">
-        <v>3229</v>
+        <v>3292</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -14377,7 +14431,7 @@
         <v>3227</v>
       </c>
       <c r="AC16" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD16" t="s">
         <v>1954</v>
@@ -14392,16 +14446,16 @@
         <v>3163</v>
       </c>
       <c r="AH16" t="s">
-        <v>3228</v>
+        <v>1281</v>
       </c>
       <c r="AI16" t="s">
-        <v>886</v>
+        <v>818</v>
       </c>
       <c r="AJ16" t="s">
         <v>2930</v>
       </c>
       <c r="AK16" t="s">
-        <v>3229</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -14412,7 +14466,7 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>752</v>
+        <v>242</v>
       </c>
       <c r="D17" t="s">
         <v>3232</v>
@@ -14442,7 +14496,7 @@
         <v>766</v>
       </c>
       <c r="X17" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Y17" t="s">
         <v>3179</v>
@@ -14475,7 +14529,7 @@
         <v>1936</v>
       </c>
       <c r="AI17" t="s">
-        <v>752</v>
+        <v>242</v>
       </c>
       <c r="AJ17" t="s">
         <v>3232</v>
@@ -14492,13 +14546,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>1942</v>
+        <v>1963</v>
       </c>
       <c r="D18" t="s">
         <v>3235</v>
       </c>
       <c r="E18" t="s">
-        <v>3234</v>
+        <v>3293</v>
       </c>
       <c r="G18" t="s">
         <v>680</v>
@@ -14534,13 +14588,13 @@
         <v>1151</v>
       </c>
       <c r="AB18" t="s">
-        <v>767</v>
+        <v>3284</v>
       </c>
       <c r="AC18" t="s">
         <v>723</v>
       </c>
       <c r="AD18" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AE18" t="s">
         <v>1927</v>
@@ -14555,13 +14609,13 @@
         <v>786</v>
       </c>
       <c r="AI18" t="s">
-        <v>1942</v>
+        <v>1963</v>
       </c>
       <c r="AJ18" t="s">
         <v>3235</v>
       </c>
       <c r="AK18" t="s">
-        <v>3234</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -14572,7 +14626,7 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>1885</v>
+        <v>627</v>
       </c>
       <c r="D19" t="s">
         <v>3237</v>
@@ -14614,7 +14668,7 @@
         <v>3179</v>
       </c>
       <c r="AB19" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AC19" t="s">
         <v>3155</v>
@@ -14635,7 +14689,7 @@
         <v>1936</v>
       </c>
       <c r="AI19" t="s">
-        <v>1885</v>
+        <v>627</v>
       </c>
       <c r="AJ19" t="s">
         <v>3237</v>
@@ -14652,7 +14706,7 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="D20" t="s">
         <v>2030</v>
@@ -14688,7 +14742,7 @@
         <v>3179</v>
       </c>
       <c r="Z20" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA20" t="s">
         <v>3174</v>
@@ -14715,7 +14769,7 @@
         <v>1933</v>
       </c>
       <c r="AI20" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="AJ20" t="s">
         <v>2030</v>
@@ -14732,7 +14786,7 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="D21" t="s">
         <v>2118</v>
@@ -14762,7 +14816,7 @@
         <v>766</v>
       </c>
       <c r="X21" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Y21" t="s">
         <v>3163</v>
@@ -14795,7 +14849,7 @@
         <v>1933</v>
       </c>
       <c r="AI21" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="AJ21" t="s">
         <v>2118</v>
@@ -14812,7 +14866,7 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>795</v>
+        <v>752</v>
       </c>
       <c r="D22" t="s">
         <v>2096</v>
@@ -14851,13 +14905,13 @@
         <v>3174</v>
       </c>
       <c r="AA22" t="s">
-        <v>3241</v>
+        <v>3294</v>
       </c>
       <c r="AB22" t="s">
         <v>3242</v>
       </c>
       <c r="AC22" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD22" t="s">
         <v>723</v>
@@ -14875,7 +14929,7 @@
         <v>2927</v>
       </c>
       <c r="AI22" t="s">
-        <v>795</v>
+        <v>752</v>
       </c>
       <c r="AJ22" t="s">
         <v>2096</v>
@@ -14892,13 +14946,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>1963</v>
+        <v>627</v>
       </c>
       <c r="D23" t="s">
         <v>1994</v>
       </c>
       <c r="E23" t="s">
-        <v>3247</v>
+        <v>3296</v>
       </c>
       <c r="G23" t="s">
         <v>552</v>
@@ -14925,7 +14979,7 @@
         <v>3192</v>
       </c>
       <c r="Y23" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Z23" t="s">
         <v>3171</v>
@@ -14940,7 +14994,7 @@
         <v>723</v>
       </c>
       <c r="AD23" t="s">
-        <v>3246</v>
+        <v>3295</v>
       </c>
       <c r="AE23" t="s">
         <v>373</v>
@@ -14955,13 +15009,13 @@
         <v>1967</v>
       </c>
       <c r="AI23" t="s">
-        <v>1963</v>
+        <v>627</v>
       </c>
       <c r="AJ23" t="s">
         <v>1994</v>
       </c>
       <c r="AK23" t="s">
-        <v>3247</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -15052,7 +15106,7 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>2957</v>
+        <v>2933</v>
       </c>
       <c r="D25" t="s">
         <v>3260</v>
@@ -15082,7 +15136,7 @@
         <v>3183</v>
       </c>
       <c r="X25" t="s">
-        <v>2001</v>
+        <v>2840</v>
       </c>
       <c r="Y25" t="s">
         <v>3255</v>
@@ -15097,7 +15151,7 @@
         <v>3256</v>
       </c>
       <c r="AC25" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD25" t="s">
         <v>3257</v>
@@ -15115,7 +15169,7 @@
         <v>3258</v>
       </c>
       <c r="AI25" t="s">
-        <v>2957</v>
+        <v>2933</v>
       </c>
       <c r="AJ25" t="s">
         <v>3260</v>
@@ -15132,7 +15186,7 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>795</v>
+        <v>647</v>
       </c>
       <c r="D26" t="s">
         <v>2252</v>
@@ -15168,7 +15222,7 @@
         <v>3174</v>
       </c>
       <c r="Z26" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA26" t="s">
         <v>3171</v>
@@ -15195,7 +15249,7 @@
         <v>3157</v>
       </c>
       <c r="AI26" t="s">
-        <v>795</v>
+        <v>647</v>
       </c>
       <c r="AJ26" t="s">
         <v>2252</v>
@@ -15212,13 +15266,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="D27" t="s">
         <v>3264</v>
       </c>
       <c r="E27" t="s">
-        <v>3263</v>
+        <v>3297</v>
       </c>
       <c r="G27" t="s">
         <v>646</v>
@@ -15242,7 +15296,7 @@
         <v>1349</v>
       </c>
       <c r="X27" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="Y27" t="s">
         <v>3174</v>
@@ -15275,13 +15329,13 @@
         <v>2927</v>
       </c>
       <c r="AI27" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="AJ27" t="s">
         <v>3264</v>
       </c>
       <c r="AK27" t="s">
-        <v>3263</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -15292,13 +15346,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="D28" t="s">
-        <v>3267</v>
+        <v>3212</v>
       </c>
       <c r="E28" t="s">
-        <v>3266</v>
+        <v>3298</v>
       </c>
       <c r="G28" t="s">
         <v>680</v>
@@ -15334,7 +15388,7 @@
         <v>3170</v>
       </c>
       <c r="AB28" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AC28" t="s">
         <v>1967</v>
@@ -15355,13 +15409,13 @@
         <v>1941</v>
       </c>
       <c r="AI28" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="AJ28" t="s">
-        <v>3267</v>
+        <v>3212</v>
       </c>
       <c r="AK28" t="s">
-        <v>3266</v>
+        <v>3298</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -15372,7 +15426,7 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="D29" t="s">
         <v>3271</v>
@@ -15408,7 +15462,7 @@
         <v>3170</v>
       </c>
       <c r="Z29" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA29" t="s">
         <v>3174</v>
@@ -15435,7 +15489,7 @@
         <v>1933</v>
       </c>
       <c r="AI29" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="AJ29" t="s">
         <v>3271</v>
@@ -15452,7 +15506,7 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>1969</v>
+        <v>795</v>
       </c>
       <c r="D30" t="s">
         <v>3273</v>
@@ -15488,7 +15542,7 @@
         <v>3163</v>
       </c>
       <c r="Z30" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA30" t="s">
         <v>3174</v>
@@ -15515,7 +15569,7 @@
         <v>2837</v>
       </c>
       <c r="AI30" t="s">
-        <v>1969</v>
+        <v>795</v>
       </c>
       <c r="AJ30" t="s">
         <v>3273</v>
@@ -15532,7 +15586,7 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="D31" t="s">
         <v>3276</v>
@@ -15568,7 +15622,7 @@
         <v>3174</v>
       </c>
       <c r="Z31" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA31" t="s">
         <v>3170</v>
@@ -15595,7 +15649,7 @@
         <v>3157</v>
       </c>
       <c r="AI31" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="AJ31" t="s">
         <v>3276</v>
@@ -15612,7 +15666,7 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>818</v>
+        <v>803</v>
       </c>
       <c r="D32" t="s">
         <v>3279</v>
@@ -15648,7 +15702,7 @@
         <v>3179</v>
       </c>
       <c r="Z32" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AA32" t="s">
         <v>3174</v>
@@ -15657,7 +15711,7 @@
         <v>3204</v>
       </c>
       <c r="AC32" t="s">
-        <v>3185</v>
+        <v>656</v>
       </c>
       <c r="AD32" t="s">
         <v>723</v>
@@ -15675,7 +15729,7 @@
         <v>2837</v>
       </c>
       <c r="AI32" t="s">
-        <v>818</v>
+        <v>803</v>
       </c>
       <c r="AJ32" t="s">
         <v>3279</v>
@@ -15692,7 +15746,7 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>1969</v>
+        <v>795</v>
       </c>
       <c r="D33" t="s">
         <v>3271</v>
@@ -15731,7 +15785,7 @@
         <v>3179</v>
       </c>
       <c r="AA33" t="s">
-        <v>3194</v>
+        <v>3282</v>
       </c>
       <c r="AB33" t="s">
         <v>723</v>
@@ -15755,7 +15809,7 @@
         <v>3157</v>
       </c>
       <c r="AI33" t="s">
-        <v>1969</v>
+        <v>795</v>
       </c>
       <c r="AJ33" t="s">
         <v>3271</v>

</xml_diff>

<commit_message>
GW 26 2nd last matchday
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15739" uniqueCount="3375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16539" uniqueCount="3532">
   <si>
     <t>Places</t>
   </si>
@@ -10159,6 +10159,477 @@
   </si>
   <si>
     <t>1552</t>
+  </si>
+  <si>
+    <t>Ramsdale 2, WOL (H)</t>
+  </si>
+  <si>
+    <t>Son 12</t>
+  </si>
+  <si>
+    <t>Bernardo 5</t>
+  </si>
+  <si>
+    <t>Salah 52$ captain</t>
+  </si>
+  <si>
+    <t>Hudson-Odoi 0</t>
+  </si>
+  <si>
+    <t>Dennis 11</t>
+  </si>
+  <si>
+    <t>Maupay 2</t>
+  </si>
+  <si>
+    <t>Livramento 12</t>
+  </si>
+  <si>
+    <t>White 2, WOL (H)</t>
+  </si>
+  <si>
+    <t>2,221,947</t>
+  </si>
+  <si>
+    <t>Guaita 1</t>
+  </si>
+  <si>
+    <t>Coady 2, ARS (A)</t>
+  </si>
+  <si>
+    <t>Smith Rowe 11, WOL (H)</t>
+  </si>
+  <si>
+    <t>Gallagher 10</t>
+  </si>
+  <si>
+    <t>Mané 13</t>
+  </si>
+  <si>
+    <t>Adams 5</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>2,967,807</t>
+  </si>
+  <si>
+    <t>Dalot 0</t>
+  </si>
+  <si>
+    <t>Raphinha 7</t>
+  </si>
+  <si>
+    <t>Saka 10, WOL (H)</t>
+  </si>
+  <si>
+    <t>Ramsey 2</t>
+  </si>
+  <si>
+    <t>Foster 7</t>
+  </si>
+  <si>
+    <t>Robertson 9</t>
+  </si>
+  <si>
+    <t>Lacazette 5, WOL (H)</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>634,598</t>
+  </si>
+  <si>
+    <t>1480</t>
+  </si>
+  <si>
+    <t>Tierney 2, WOL (H)</t>
+  </si>
+  <si>
+    <t>Salah 78$ captain</t>
+  </si>
+  <si>
+    <t>Edouard 0</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>362,618</t>
+  </si>
+  <si>
+    <t>Ait Nouri 1, ARS (A)</t>
+  </si>
+  <si>
+    <t>Davies 3</t>
+  </si>
+  <si>
+    <t>Kane 15</t>
+  </si>
+  <si>
+    <t>Rodriguez 6</t>
+  </si>
+  <si>
+    <t>Winks 1</t>
+  </si>
+  <si>
+    <t>Sissoko 10</t>
+  </si>
+  <si>
+    <t>1,246,255</t>
+  </si>
+  <si>
+    <t>4 (-8 pts)</t>
+  </si>
+  <si>
+    <t>Dias 1</t>
+  </si>
+  <si>
+    <t>Jota 0</t>
+  </si>
+  <si>
+    <t>Tsimikas 5</t>
+  </si>
+  <si>
+    <t>3,336,872</t>
+  </si>
+  <si>
+    <t>Veltman 1</t>
+  </si>
+  <si>
+    <t>Zaha 4</t>
+  </si>
+  <si>
+    <t>Sarr 9</t>
+  </si>
+  <si>
+    <t>Semedo 2, ARS (A)</t>
+  </si>
+  <si>
+    <t>Ødegaard 2, WOL (H)</t>
+  </si>
+  <si>
+    <t>673,126</t>
+  </si>
+  <si>
+    <t>7 (-24 pts)</t>
+  </si>
+  <si>
+    <t>Saïss 2, ARS (A)</t>
+  </si>
+  <si>
+    <t>Højbjerg 3</t>
+  </si>
+  <si>
+    <t>1,274,904</t>
+  </si>
+  <si>
+    <t>Gabriel 1, WOL (H)</t>
+  </si>
+  <si>
+    <t>Firmino 0</t>
+  </si>
+  <si>
+    <t>Jiménez 5, ARS (A)</t>
+  </si>
+  <si>
+    <t>Mee 18</t>
+  </si>
+  <si>
+    <t>683,156</t>
+  </si>
+  <si>
+    <t>Kilman 2, ARS (A)</t>
+  </si>
+  <si>
+    <t>395,935</t>
+  </si>
+  <si>
+    <t>1519</t>
+  </si>
+  <si>
+    <t>Rüdiger 6</t>
+  </si>
+  <si>
+    <t>Varane 1</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>463,436</t>
+  </si>
+  <si>
+    <t>Coufal 0</t>
+  </si>
+  <si>
+    <t>Laporte 1</t>
+  </si>
+  <si>
+    <t>Saint-Maximin 0</t>
+  </si>
+  <si>
+    <t>1,247,218</t>
+  </si>
+  <si>
+    <t>Matip 14</t>
+  </si>
+  <si>
+    <t>Kane 45$ captain</t>
+  </si>
+  <si>
+    <t>Sterling 2</t>
+  </si>
+  <si>
+    <t>1,035,406</t>
+  </si>
+  <si>
+    <t>Arrizabalaga 0</t>
+  </si>
+  <si>
+    <t>Sargent 5</t>
+  </si>
+  <si>
+    <t>Brownhill 15</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>668,126</t>
+  </si>
+  <si>
+    <t>Sá 4, ARS (A)</t>
+  </si>
+  <si>
+    <t>Tomiyasu 0, WOL (H)</t>
+  </si>
+  <si>
+    <t>Jota 0$ captain</t>
+  </si>
+  <si>
+    <t>Watkins 1</t>
+  </si>
+  <si>
+    <t>1,485,364</t>
+  </si>
+  <si>
+    <t>Tarkowski 6</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>1,019,963</t>
+  </si>
+  <si>
+    <t>1434</t>
+  </si>
+  <si>
+    <t>Maguire 7</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>879,344</t>
+  </si>
+  <si>
+    <t>1449</t>
+  </si>
+  <si>
+    <t>Zaha 14</t>
+  </si>
+  <si>
+    <t>Matthews 0</t>
+  </si>
+  <si>
+    <t>Kelly 0</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>63,635</t>
+  </si>
+  <si>
+    <t>1624</t>
+  </si>
+  <si>
+    <t>309,669</t>
+  </si>
+  <si>
+    <t>1538</t>
+  </si>
+  <si>
+    <t>Weghorst 14</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>68,266</t>
+  </si>
+  <si>
+    <t>1621</t>
+  </si>
+  <si>
+    <t>181,058</t>
+  </si>
+  <si>
+    <t>1573</t>
+  </si>
+  <si>
+    <t>Alisson 11</t>
+  </si>
+  <si>
+    <t>Mitchell 7</t>
+  </si>
+  <si>
+    <t>436,053</t>
+  </si>
+  <si>
+    <t>Emerson Royal 8</t>
+  </si>
+  <si>
+    <t>Podence 8, ARS (A)</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>193,993</t>
+  </si>
+  <si>
+    <t>Alonso 4</t>
+  </si>
+  <si>
+    <t>Aubameyang 0, WOL (H)$ captain</t>
+  </si>
+  <si>
+    <t>Shaw 3</t>
+  </si>
+  <si>
+    <t>Bissouma 2</t>
+  </si>
+  <si>
+    <t>6,158,263</t>
+  </si>
+  <si>
+    <t>1070</t>
+  </si>
+  <si>
+    <t>196,471</t>
+  </si>
+  <si>
+    <t>1568</t>
+  </si>
+  <si>
+    <t>Cornet 1</t>
+  </si>
+  <si>
+    <t>41,234</t>
+  </si>
+  <si>
+    <t>1641</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>531,289</t>
+  </si>
+  <si>
+    <t>1496</t>
+  </si>
+  <si>
+    <t>Harrison 3</t>
+  </si>
+  <si>
+    <t>Mané 18</t>
+  </si>
+  <si>
+    <t>86,622</t>
+  </si>
+  <si>
+    <t>1611</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>65,582</t>
+  </si>
+  <si>
+    <t>1623</t>
+  </si>
+  <si>
+    <t>White View player information</t>
+  </si>
+  <si>
+    <t>van Dijk View player information</t>
+  </si>
+  <si>
+    <t>Saïss View player information</t>
+  </si>
+  <si>
+    <t>Salah View player information$ captain</t>
+  </si>
+  <si>
+    <t>Son View player information</t>
+  </si>
+  <si>
+    <t>Coutinho View player information</t>
+  </si>
+  <si>
+    <t>Raphinha View player information</t>
+  </si>
+  <si>
+    <t>Lacazette View player information</t>
+  </si>
+  <si>
+    <t>Jiménez View player information</t>
+  </si>
+  <si>
+    <t>Foster View player information</t>
+  </si>
+  <si>
+    <t>Digne View player information</t>
+  </si>
+  <si>
+    <t>Broja View player information</t>
+  </si>
+  <si>
+    <t>Ramsey View player information</t>
+  </si>
+  <si>
+    <t>157,574</t>
+  </si>
+  <si>
+    <t>1581</t>
+  </si>
+  <si>
+    <t>Olise 3</t>
+  </si>
+  <si>
+    <t>Forster 6</t>
+  </si>
+  <si>
+    <t>69,961</t>
+  </si>
+  <si>
+    <t>1620</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>74,084</t>
+  </si>
+  <si>
+    <t>1618</t>
   </si>
 </sst>
 </file>
@@ -13349,26 +13820,26 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.13671875" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.8828125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="22.14453125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.89453125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.80078125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="31.82421875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="28.6015625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="30.234375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="38.89453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="36.1328125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="26.4765625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="31.3515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="31.58203125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="31.64453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="31.171875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="28.78125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="28.29296875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="30.10546875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.3828125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
@@ -13494,13 +13965,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>818</v>
+        <v>1212</v>
       </c>
       <c r="D2" t="s">
-        <v>3302</v>
+        <v>2601</v>
       </c>
       <c r="E2" t="s">
-        <v>3301</v>
+        <v>3384</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -13512,58 +13983,58 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>3299</v>
+        <v>3375</v>
       </c>
       <c r="U2" t="s">
-        <v>3157</v>
+        <v>3015</v>
       </c>
       <c r="V2" t="s">
-        <v>2837</v>
+        <v>1900</v>
       </c>
       <c r="W2" t="s">
-        <v>3015</v>
+        <v>1162</v>
       </c>
       <c r="X2" t="s">
-        <v>1929</v>
+        <v>3376</v>
       </c>
       <c r="Y2" t="s">
-        <v>3154</v>
+        <v>712</v>
       </c>
       <c r="Z2" t="s">
-        <v>2840</v>
+        <v>3377</v>
       </c>
       <c r="AA2" t="s">
-        <v>357</v>
+        <v>3378</v>
       </c>
       <c r="AB2" t="s">
-        <v>2843</v>
+        <v>3379</v>
       </c>
       <c r="AC2" t="s">
-        <v>3300</v>
+        <v>3380</v>
       </c>
       <c r="AD2" t="s">
-        <v>723</v>
+        <v>3381</v>
       </c>
       <c r="AE2" t="s">
-        <v>1927</v>
+        <v>2266</v>
       </c>
       <c r="AF2" t="s">
-        <v>663</v>
+        <v>3382</v>
       </c>
       <c r="AG2" t="s">
         <v>914</v>
       </c>
       <c r="AH2" t="s">
-        <v>1930</v>
+        <v>3383</v>
       </c>
       <c r="AI2" t="s">
-        <v>818</v>
+        <v>1212</v>
       </c>
       <c r="AJ2" t="s">
-        <v>3302</v>
+        <v>2601</v>
       </c>
       <c r="AK2" t="s">
-        <v>3301</v>
+        <v>3384</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -13574,16 +14045,16 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>3391</v>
       </c>
       <c r="D3" t="s">
-        <v>3306</v>
+        <v>2232</v>
       </c>
       <c r="E3" t="s">
-        <v>3305</v>
+        <v>3392</v>
       </c>
       <c r="G3" t="s">
-        <v>627</v>
+        <v>552</v>
       </c>
       <c r="R3" t="s">
         <v>688</v>
@@ -13592,43 +14063,43 @@
         <v>687</v>
       </c>
       <c r="T3" t="s">
-        <v>3299</v>
+        <v>3385</v>
       </c>
       <c r="U3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="V3" t="s">
         <v>3015</v>
       </c>
-      <c r="V3" t="s">
-        <v>3160</v>
-      </c>
       <c r="W3" t="s">
-        <v>3157</v>
+        <v>3386</v>
       </c>
       <c r="X3" t="s">
-        <v>3163</v>
+        <v>3378</v>
       </c>
       <c r="Y3" t="s">
-        <v>3303</v>
+        <v>3387</v>
       </c>
       <c r="Z3" t="s">
-        <v>1932</v>
+        <v>3162</v>
       </c>
       <c r="AA3" t="s">
-        <v>1929</v>
+        <v>3388</v>
       </c>
       <c r="AB3" t="s">
-        <v>3161</v>
+        <v>3389</v>
       </c>
       <c r="AC3" t="s">
-        <v>3304</v>
+        <v>3380</v>
       </c>
       <c r="AD3" t="s">
-        <v>723</v>
+        <v>3390</v>
       </c>
       <c r="AE3" t="s">
-        <v>1357</v>
+        <v>2266</v>
       </c>
       <c r="AF3" t="s">
-        <v>663</v>
+        <v>3382</v>
       </c>
       <c r="AG3" t="s">
         <v>684</v>
@@ -13637,13 +14108,13 @@
         <v>914</v>
       </c>
       <c r="AI3" t="s">
-        <v>250</v>
+        <v>3391</v>
       </c>
       <c r="AJ3" t="s">
-        <v>3306</v>
+        <v>2232</v>
       </c>
       <c r="AK3" t="s">
-        <v>3305</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -13654,16 +14125,16 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>3400</v>
       </c>
       <c r="D4" t="s">
-        <v>3310</v>
+        <v>3402</v>
       </c>
       <c r="E4" t="s">
-        <v>3309</v>
+        <v>3401</v>
       </c>
       <c r="G4" t="s">
-        <v>627</v>
+        <v>880</v>
       </c>
       <c r="R4" t="s">
         <v>697</v>
@@ -13672,58 +14143,58 @@
         <v>696</v>
       </c>
       <c r="T4" t="s">
-        <v>3299</v>
+        <v>2266</v>
       </c>
       <c r="U4" t="s">
-        <v>3167</v>
+        <v>3386</v>
       </c>
       <c r="V4" t="s">
-        <v>3307</v>
+        <v>3383</v>
       </c>
       <c r="W4" t="s">
+        <v>3393</v>
+      </c>
+      <c r="X4" t="s">
+        <v>3394</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>3378</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>3395</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>3376</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>3396</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>1967</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>3380</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>3397</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>3398</v>
+      </c>
+      <c r="AG4" t="s">
         <v>3015</v>
       </c>
-      <c r="X4" t="s">
-        <v>1151</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>3169</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>3170</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>3308</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>1967</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>723</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>3304</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>667</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>3160</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>1930</v>
-      </c>
       <c r="AH4" t="s">
-        <v>1937</v>
+        <v>3399</v>
       </c>
       <c r="AI4" t="s">
-        <v>279</v>
+        <v>3400</v>
       </c>
       <c r="AJ4" t="s">
-        <v>3310</v>
+        <v>3402</v>
       </c>
       <c r="AK4" t="s">
-        <v>3309</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -13734,16 +14205,16 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>1425</v>
+        <v>3406</v>
       </c>
       <c r="D5" t="s">
-        <v>2023</v>
+        <v>3370</v>
       </c>
       <c r="E5" t="s">
-        <v>3311</v>
+        <v>3407</v>
       </c>
       <c r="G5" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R5" t="s">
         <v>557</v>
@@ -13752,58 +14223,58 @@
         <v>705</v>
       </c>
       <c r="T5" t="s">
-        <v>410</v>
+        <v>1180</v>
       </c>
       <c r="U5" t="s">
-        <v>663</v>
+        <v>3403</v>
       </c>
       <c r="V5" t="s">
         <v>3015</v>
       </c>
       <c r="W5" t="s">
-        <v>3307</v>
+        <v>3383</v>
       </c>
       <c r="X5" t="s">
-        <v>3154</v>
+        <v>3398</v>
       </c>
       <c r="Y5" t="s">
-        <v>3303</v>
+        <v>1162</v>
       </c>
       <c r="Z5" t="s">
-        <v>3174</v>
+        <v>3404</v>
       </c>
       <c r="AA5" t="s">
-        <v>3163</v>
+        <v>3162</v>
       </c>
       <c r="AB5" t="s">
-        <v>3284</v>
+        <v>3395</v>
       </c>
       <c r="AC5" t="s">
+        <v>3380</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>3405</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>3397</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>3388</v>
+      </c>
+      <c r="AG5" t="s">
         <v>1967</v>
       </c>
-      <c r="AD5" t="s">
-        <v>1386</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>667</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>723</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>1933</v>
-      </c>
       <c r="AH5" t="s">
-        <v>1930</v>
+        <v>767</v>
       </c>
       <c r="AI5" t="s">
-        <v>1425</v>
+        <v>3406</v>
       </c>
       <c r="AJ5" t="s">
-        <v>2023</v>
+        <v>3370</v>
       </c>
       <c r="AK5" t="s">
-        <v>3311</v>
+        <v>3407</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -13814,16 +14285,16 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>3406</v>
       </c>
       <c r="D6" t="s">
-        <v>2093</v>
+        <v>3133</v>
       </c>
       <c r="E6" t="s">
-        <v>3314</v>
+        <v>3414</v>
       </c>
       <c r="G6" t="s">
-        <v>627</v>
+        <v>3415</v>
       </c>
       <c r="R6" t="s">
         <v>469</v>
@@ -13832,58 +14303,58 @@
         <v>717</v>
       </c>
       <c r="T6" t="s">
-        <v>1357</v>
+        <v>3385</v>
       </c>
       <c r="U6" t="s">
         <v>3015</v>
       </c>
       <c r="V6" t="s">
-        <v>757</v>
+        <v>3408</v>
       </c>
       <c r="W6" t="s">
-        <v>3176</v>
+        <v>1162</v>
       </c>
       <c r="X6" t="s">
-        <v>2064</v>
+        <v>3409</v>
       </c>
       <c r="Y6" t="s">
-        <v>3181</v>
+        <v>3395</v>
       </c>
       <c r="Z6" t="s">
-        <v>3312</v>
+        <v>3378</v>
       </c>
       <c r="AA6" t="s">
-        <v>2218</v>
+        <v>3308</v>
       </c>
       <c r="AB6" t="s">
-        <v>3313</v>
+        <v>2584</v>
       </c>
       <c r="AC6" t="s">
-        <v>1899</v>
+        <v>3410</v>
       </c>
       <c r="AD6" t="s">
-        <v>1196</v>
+        <v>3411</v>
       </c>
       <c r="AE6" t="s">
         <v>1128</v>
       </c>
       <c r="AF6" t="s">
-        <v>663</v>
+        <v>3412</v>
       </c>
       <c r="AG6" t="s">
-        <v>1206</v>
+        <v>3413</v>
       </c>
       <c r="AH6" t="s">
-        <v>2219</v>
+        <v>3176</v>
       </c>
       <c r="AI6" t="s">
-        <v>268</v>
+        <v>3406</v>
       </c>
       <c r="AJ6" t="s">
-        <v>2093</v>
+        <v>3133</v>
       </c>
       <c r="AK6" t="s">
-        <v>3314</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -13894,13 +14365,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>260</v>
+        <v>1202</v>
       </c>
       <c r="D7" t="s">
-        <v>3317</v>
+        <v>2959</v>
       </c>
       <c r="E7" t="s">
-        <v>3316</v>
+        <v>3419</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -13912,58 +14383,58 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>1927</v>
+        <v>3375</v>
       </c>
       <c r="U7" t="s">
-        <v>3157</v>
+        <v>3416</v>
       </c>
       <c r="V7" t="s">
-        <v>3183</v>
+        <v>528</v>
       </c>
       <c r="W7" t="s">
-        <v>3315</v>
+        <v>1164</v>
       </c>
       <c r="X7" t="s">
-        <v>3174</v>
+        <v>3417</v>
       </c>
       <c r="Y7" t="s">
-        <v>3303</v>
+        <v>3162</v>
       </c>
       <c r="Z7" t="s">
-        <v>3163</v>
+        <v>3388</v>
       </c>
       <c r="AA7" t="s">
-        <v>3169</v>
+        <v>3378</v>
       </c>
       <c r="AB7" t="s">
-        <v>3304</v>
+        <v>3380</v>
       </c>
       <c r="AC7" t="s">
-        <v>723</v>
+        <v>656</v>
       </c>
       <c r="AD7" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="AE7" t="s">
         <v>778</v>
       </c>
       <c r="AF7" t="s">
-        <v>1427</v>
+        <v>3418</v>
       </c>
       <c r="AG7" t="s">
-        <v>724</v>
+        <v>1952</v>
       </c>
       <c r="AH7" t="s">
-        <v>528</v>
+        <v>3382</v>
       </c>
       <c r="AI7" t="s">
-        <v>260</v>
+        <v>1202</v>
       </c>
       <c r="AJ7" t="s">
-        <v>3317</v>
+        <v>2959</v>
       </c>
       <c r="AK7" t="s">
-        <v>3316</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -13974,16 +14445,16 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>1243</v>
       </c>
       <c r="D8" t="s">
-        <v>1987</v>
+        <v>2023</v>
       </c>
       <c r="E8" t="s">
-        <v>3320</v>
+        <v>3425</v>
       </c>
       <c r="G8" t="s">
-        <v>646</v>
+        <v>3426</v>
       </c>
       <c r="R8" t="s">
         <v>547</v>
@@ -13992,58 +14463,58 @@
         <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>3299</v>
+        <v>3397</v>
       </c>
       <c r="U8" t="s">
-        <v>3318</v>
+        <v>3420</v>
       </c>
       <c r="V8" t="s">
         <v>3015</v>
       </c>
       <c r="W8" t="s">
-        <v>354</v>
+        <v>3403</v>
       </c>
       <c r="X8" t="s">
-        <v>3174</v>
+        <v>3421</v>
       </c>
       <c r="Y8" t="s">
-        <v>3319</v>
+        <v>3422</v>
       </c>
       <c r="Z8" t="s">
-        <v>3284</v>
+        <v>3378</v>
       </c>
       <c r="AA8" t="s">
-        <v>3303</v>
+        <v>3162</v>
       </c>
       <c r="AB8" t="s">
-        <v>1899</v>
+        <v>2584</v>
       </c>
       <c r="AC8" t="s">
-        <v>3304</v>
+        <v>3399</v>
       </c>
       <c r="AD8" t="s">
-        <v>1196</v>
+        <v>3410</v>
       </c>
       <c r="AE8" t="s">
         <v>1806</v>
       </c>
       <c r="AF8" t="s">
-        <v>799</v>
+        <v>3423</v>
       </c>
       <c r="AG8" t="s">
-        <v>3195</v>
+        <v>2173</v>
       </c>
       <c r="AH8" t="s">
-        <v>3196</v>
+        <v>3424</v>
       </c>
       <c r="AI8" t="s">
-        <v>266</v>
+        <v>1243</v>
       </c>
       <c r="AJ8" t="s">
-        <v>1987</v>
+        <v>2023</v>
       </c>
       <c r="AK8" t="s">
-        <v>3320</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -14054,16 +14525,16 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>2069</v>
       </c>
       <c r="D9" t="s">
-        <v>3116</v>
+        <v>3074</v>
       </c>
       <c r="E9" t="s">
-        <v>3321</v>
+        <v>3429</v>
       </c>
       <c r="G9" t="s">
-        <v>627</v>
+        <v>646</v>
       </c>
       <c r="R9" t="s">
         <v>540</v>
@@ -14072,58 +14543,58 @@
         <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>3299</v>
+        <v>1180</v>
       </c>
       <c r="U9" t="s">
         <v>3015</v>
       </c>
       <c r="V9" t="s">
-        <v>3200</v>
+        <v>3418</v>
       </c>
       <c r="W9" t="s">
-        <v>3183</v>
+        <v>3427</v>
       </c>
       <c r="X9" t="s">
-        <v>2905</v>
+        <v>3378</v>
       </c>
       <c r="Y9" t="s">
-        <v>3169</v>
+        <v>3424</v>
       </c>
       <c r="Z9" t="s">
-        <v>1929</v>
+        <v>3162</v>
       </c>
       <c r="AA9" t="s">
-        <v>3199</v>
+        <v>3428</v>
       </c>
       <c r="AB9" t="s">
-        <v>656</v>
+        <v>3380</v>
       </c>
       <c r="AC9" t="s">
-        <v>723</v>
+        <v>657</v>
       </c>
       <c r="AD9" t="s">
-        <v>3304</v>
+        <v>3390</v>
       </c>
       <c r="AE9" t="s">
-        <v>410</v>
+        <v>2266</v>
       </c>
       <c r="AF9" t="s">
-        <v>3196</v>
+        <v>3416</v>
       </c>
       <c r="AG9" t="s">
-        <v>724</v>
+        <v>3377</v>
       </c>
       <c r="AH9" t="s">
-        <v>2867</v>
+        <v>1354</v>
       </c>
       <c r="AI9" t="s">
-        <v>268</v>
+        <v>2069</v>
       </c>
       <c r="AJ9" t="s">
-        <v>3116</v>
+        <v>3074</v>
       </c>
       <c r="AK9" t="s">
-        <v>3321</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -14134,16 +14605,16 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>290</v>
+        <v>1702</v>
       </c>
       <c r="D10" t="s">
-        <v>3212</v>
+        <v>2997</v>
       </c>
       <c r="E10" t="s">
-        <v>3322</v>
+        <v>3434</v>
       </c>
       <c r="G10" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="R10" t="s">
         <v>742</v>
@@ -14152,58 +14623,58 @@
         <v>259</v>
       </c>
       <c r="T10" t="s">
-        <v>410</v>
+        <v>3375</v>
       </c>
       <c r="U10" t="s">
-        <v>3203</v>
+        <v>3430</v>
       </c>
       <c r="V10" t="s">
-        <v>663</v>
+        <v>3386</v>
       </c>
       <c r="W10" t="s">
         <v>3015</v>
       </c>
       <c r="X10" t="s">
-        <v>3303</v>
+        <v>2266</v>
       </c>
       <c r="Y10" t="s">
-        <v>3204</v>
+        <v>3395</v>
       </c>
       <c r="Z10" t="s">
-        <v>3163</v>
+        <v>3376</v>
       </c>
       <c r="AA10" t="s">
-        <v>3169</v>
+        <v>3378</v>
       </c>
       <c r="AB10" t="s">
-        <v>1967</v>
+        <v>3431</v>
       </c>
       <c r="AC10" t="s">
-        <v>3304</v>
+        <v>3380</v>
       </c>
       <c r="AD10" t="s">
-        <v>723</v>
+        <v>3432</v>
       </c>
       <c r="AE10" t="s">
         <v>740</v>
       </c>
       <c r="AF10" t="s">
-        <v>528</v>
+        <v>1370</v>
       </c>
       <c r="AG10" t="s">
-        <v>1941</v>
+        <v>3433</v>
       </c>
       <c r="AH10" t="s">
-        <v>3205</v>
+        <v>3162</v>
       </c>
       <c r="AI10" t="s">
-        <v>290</v>
+        <v>1702</v>
       </c>
       <c r="AJ10" t="s">
-        <v>3212</v>
+        <v>2997</v>
       </c>
       <c r="AK10" t="s">
-        <v>3322</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -14214,16 +14685,16 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>1285</v>
       </c>
       <c r="D11" t="s">
-        <v>3324</v>
+        <v>3437</v>
       </c>
       <c r="E11" t="s">
-        <v>3323</v>
+        <v>3436</v>
       </c>
       <c r="G11" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R11" t="s">
         <v>747</v>
@@ -14232,58 +14703,58 @@
         <v>746</v>
       </c>
       <c r="T11" t="s">
-        <v>3299</v>
+        <v>3397</v>
       </c>
       <c r="U11" t="s">
         <v>3015</v>
       </c>
       <c r="V11" t="s">
-        <v>528</v>
+        <v>3430</v>
       </c>
       <c r="W11" t="s">
-        <v>3195</v>
+        <v>3403</v>
       </c>
       <c r="X11" t="s">
-        <v>3183</v>
+        <v>3435</v>
       </c>
       <c r="Y11" t="s">
-        <v>1206</v>
+        <v>3396</v>
       </c>
       <c r="Z11" t="s">
-        <v>3169</v>
+        <v>3395</v>
       </c>
       <c r="AA11" t="s">
-        <v>3174</v>
+        <v>3378</v>
       </c>
       <c r="AB11" t="s">
-        <v>3312</v>
+        <v>3376</v>
       </c>
       <c r="AC11" t="s">
-        <v>723</v>
+        <v>3405</v>
       </c>
       <c r="AD11" t="s">
-        <v>1899</v>
+        <v>3432</v>
       </c>
       <c r="AE11" t="s">
-        <v>3207</v>
+        <v>2266</v>
       </c>
       <c r="AF11" t="s">
-        <v>663</v>
+        <v>1162</v>
       </c>
       <c r="AG11" t="s">
-        <v>1932</v>
+        <v>3162</v>
       </c>
       <c r="AH11" t="s">
-        <v>3044</v>
+        <v>1967</v>
       </c>
       <c r="AI11" t="s">
-        <v>254</v>
+        <v>1285</v>
       </c>
       <c r="AJ11" t="s">
-        <v>3324</v>
+        <v>3437</v>
       </c>
       <c r="AK11" t="s">
-        <v>3323</v>
+        <v>3436</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -14294,16 +14765,16 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>1183</v>
+        <v>3440</v>
       </c>
       <c r="D12" t="s">
-        <v>3327</v>
+        <v>2116</v>
       </c>
       <c r="E12" t="s">
-        <v>3326</v>
+        <v>3441</v>
       </c>
       <c r="G12" t="s">
-        <v>426</v>
+        <v>880</v>
       </c>
       <c r="R12" t="s">
         <v>392</v>
@@ -14312,58 +14783,58 @@
         <v>263</v>
       </c>
       <c r="T12" t="s">
-        <v>3210</v>
+        <v>3375</v>
       </c>
       <c r="U12" t="s">
-        <v>3325</v>
+        <v>3416</v>
       </c>
       <c r="V12" t="s">
-        <v>757</v>
+        <v>3398</v>
       </c>
       <c r="W12" t="s">
-        <v>3183</v>
+        <v>2226</v>
       </c>
       <c r="X12" t="s">
-        <v>3163</v>
+        <v>3438</v>
       </c>
       <c r="Y12" t="s">
-        <v>3303</v>
+        <v>3404</v>
       </c>
       <c r="Z12" t="s">
-        <v>1929</v>
+        <v>3377</v>
       </c>
       <c r="AA12" t="s">
-        <v>2224</v>
+        <v>2018</v>
       </c>
       <c r="AB12" t="s">
-        <v>723</v>
+        <v>3387</v>
       </c>
       <c r="AC12" t="s">
-        <v>3304</v>
+        <v>3381</v>
       </c>
       <c r="AD12" t="s">
-        <v>3300</v>
+        <v>3380</v>
       </c>
       <c r="AE12" t="s">
-        <v>1927</v>
+        <v>751</v>
       </c>
       <c r="AF12" t="s">
-        <v>528</v>
+        <v>3162</v>
       </c>
       <c r="AG12" t="s">
-        <v>1932</v>
+        <v>3439</v>
       </c>
       <c r="AH12" t="s">
-        <v>2928</v>
+        <v>802</v>
       </c>
       <c r="AI12" t="s">
-        <v>1183</v>
+        <v>3440</v>
       </c>
       <c r="AJ12" t="s">
-        <v>3327</v>
+        <v>2116</v>
       </c>
       <c r="AK12" t="s">
-        <v>3326</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -14374,16 +14845,16 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>686</v>
+        <v>3440</v>
       </c>
       <c r="D13" t="s">
-        <v>3330</v>
+        <v>3133</v>
       </c>
       <c r="E13" t="s">
-        <v>3329</v>
+        <v>3445</v>
       </c>
       <c r="G13" t="s">
-        <v>426</v>
+        <v>880</v>
       </c>
       <c r="R13" t="s">
         <v>486</v>
@@ -14392,58 +14863,58 @@
         <v>265</v>
       </c>
       <c r="T13" t="s">
-        <v>667</v>
+        <v>3375</v>
       </c>
       <c r="U13" t="s">
-        <v>3325</v>
+        <v>3398</v>
       </c>
       <c r="V13" t="s">
-        <v>1349</v>
+        <v>2226</v>
       </c>
       <c r="W13" t="s">
-        <v>799</v>
+        <v>3442</v>
       </c>
       <c r="X13" t="s">
-        <v>3328</v>
+        <v>3403</v>
       </c>
       <c r="Y13" t="s">
-        <v>3303</v>
+        <v>3395</v>
       </c>
       <c r="Z13" t="s">
-        <v>3163</v>
+        <v>3376</v>
       </c>
       <c r="AA13" t="s">
         <v>3204</v>
       </c>
       <c r="AB13" t="s">
-        <v>723</v>
+        <v>3162</v>
       </c>
       <c r="AC13" t="s">
+        <v>3404</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>3380</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>3397</v>
+      </c>
+      <c r="AF13" t="s">
         <v>1967</v>
       </c>
-      <c r="AD13" t="s">
-        <v>666</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>663</v>
-      </c>
       <c r="AG13" t="s">
-        <v>3213</v>
+        <v>3443</v>
       </c>
       <c r="AH13" t="s">
-        <v>1933</v>
+        <v>3444</v>
       </c>
       <c r="AI13" t="s">
-        <v>686</v>
+        <v>3440</v>
       </c>
       <c r="AJ13" t="s">
-        <v>3330</v>
+        <v>3133</v>
       </c>
       <c r="AK13" t="s">
-        <v>3329</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -14454,16 +14925,16 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>1723</v>
+        <v>2135</v>
       </c>
       <c r="D14" t="s">
-        <v>3335</v>
+        <v>2626</v>
       </c>
       <c r="E14" t="s">
-        <v>3334</v>
+        <v>3449</v>
       </c>
       <c r="G14" t="s">
-        <v>680</v>
+        <v>646</v>
       </c>
       <c r="R14" t="s">
         <v>433</v>
@@ -14472,58 +14943,58 @@
         <v>770</v>
       </c>
       <c r="T14" t="s">
-        <v>3331</v>
+        <v>3397</v>
       </c>
       <c r="U14" t="s">
-        <v>1349</v>
+        <v>3383</v>
       </c>
       <c r="V14" t="s">
-        <v>916</v>
+        <v>2226</v>
       </c>
       <c r="W14" t="s">
-        <v>3216</v>
+        <v>3446</v>
       </c>
       <c r="X14" t="s">
-        <v>1151</v>
+        <v>3403</v>
       </c>
       <c r="Y14" t="s">
-        <v>3332</v>
+        <v>3394</v>
       </c>
       <c r="Z14" t="s">
-        <v>3174</v>
+        <v>722</v>
       </c>
       <c r="AA14" t="s">
-        <v>3218</v>
+        <v>3389</v>
       </c>
       <c r="AB14" t="s">
-        <v>1196</v>
+        <v>3447</v>
       </c>
       <c r="AC14" t="s">
-        <v>3333</v>
+        <v>3381</v>
       </c>
       <c r="AD14" t="s">
-        <v>1899</v>
+        <v>2584</v>
       </c>
       <c r="AE14" t="s">
-        <v>667</v>
+        <v>2963</v>
       </c>
       <c r="AF14" t="s">
-        <v>1930</v>
+        <v>3448</v>
       </c>
       <c r="AG14" t="s">
-        <v>1933</v>
+        <v>3443</v>
       </c>
       <c r="AH14" t="s">
         <v>3220</v>
       </c>
       <c r="AI14" t="s">
-        <v>1723</v>
+        <v>2135</v>
       </c>
       <c r="AJ14" t="s">
-        <v>3335</v>
+        <v>2626</v>
       </c>
       <c r="AK14" t="s">
-        <v>3334</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -14534,16 +15005,16 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>1233</v>
+        <v>3453</v>
       </c>
       <c r="D15" t="s">
-        <v>2622</v>
+        <v>2023</v>
       </c>
       <c r="E15" t="s">
-        <v>3337</v>
+        <v>3454</v>
       </c>
       <c r="G15" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R15" t="s">
         <v>775</v>
@@ -14552,58 +15023,58 @@
         <v>774</v>
       </c>
       <c r="T15" t="s">
-        <v>3331</v>
+        <v>3375</v>
       </c>
       <c r="U15" t="s">
+        <v>3398</v>
+      </c>
+      <c r="V15" t="s">
         <v>3015</v>
       </c>
-      <c r="V15" t="s">
-        <v>3336</v>
-      </c>
       <c r="W15" t="s">
-        <v>3325</v>
+        <v>3403</v>
       </c>
       <c r="X15" t="s">
-        <v>2224</v>
+        <v>3408</v>
       </c>
       <c r="Y15" t="s">
-        <v>3312</v>
+        <v>1162</v>
       </c>
       <c r="Z15" t="s">
-        <v>3303</v>
+        <v>3376</v>
       </c>
       <c r="AA15" t="s">
-        <v>1151</v>
+        <v>3394</v>
       </c>
       <c r="AB15" t="s">
-        <v>3174</v>
+        <v>3378</v>
       </c>
       <c r="AC15" t="s">
-        <v>656</v>
+        <v>3162</v>
       </c>
       <c r="AD15" t="s">
-        <v>723</v>
+        <v>3399</v>
       </c>
       <c r="AE15" t="s">
-        <v>1927</v>
+        <v>3450</v>
       </c>
       <c r="AF15" t="s">
-        <v>663</v>
+        <v>3451</v>
       </c>
       <c r="AG15" t="s">
-        <v>1150</v>
+        <v>3452</v>
       </c>
       <c r="AH15" t="s">
-        <v>1899</v>
+        <v>3411</v>
       </c>
       <c r="AI15" t="s">
-        <v>1233</v>
+        <v>3453</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2622</v>
+        <v>2023</v>
       </c>
       <c r="AK15" t="s">
-        <v>3337</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -14614,13 +15085,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
-        <v>1904</v>
+        <v>3343</v>
       </c>
       <c r="E16" t="s">
-        <v>3339</v>
+        <v>3459</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -14632,58 +15103,58 @@
         <v>270</v>
       </c>
       <c r="T16" t="s">
-        <v>3338</v>
+        <v>3455</v>
       </c>
       <c r="U16" t="s">
-        <v>3157</v>
+        <v>3430</v>
       </c>
       <c r="V16" t="s">
         <v>3015</v>
       </c>
       <c r="W16" t="s">
-        <v>3183</v>
+        <v>3456</v>
       </c>
       <c r="X16" t="s">
-        <v>3163</v>
+        <v>3377</v>
       </c>
       <c r="Y16" t="s">
-        <v>3174</v>
+        <v>3457</v>
       </c>
       <c r="Z16" t="s">
-        <v>1929</v>
+        <v>3308</v>
       </c>
       <c r="AA16" t="s">
-        <v>3308</v>
+        <v>1281</v>
       </c>
       <c r="AB16" t="s">
-        <v>3227</v>
+        <v>3380</v>
       </c>
       <c r="AC16" t="s">
-        <v>1954</v>
+        <v>656</v>
       </c>
       <c r="AD16" t="s">
-        <v>656</v>
+        <v>3458</v>
       </c>
       <c r="AE16" t="s">
-        <v>3299</v>
+        <v>2266</v>
       </c>
       <c r="AF16" t="s">
-        <v>1936</v>
+        <v>3382</v>
       </c>
       <c r="AG16" t="s">
-        <v>3205</v>
+        <v>3388</v>
       </c>
       <c r="AH16" t="s">
-        <v>1281</v>
+        <v>3416</v>
       </c>
       <c r="AI16" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="AJ16" t="s">
-        <v>1904</v>
+        <v>3343</v>
       </c>
       <c r="AK16" t="s">
-        <v>3339</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -14694,16 +15165,16 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>1432</v>
+        <v>3461</v>
       </c>
       <c r="D17" t="s">
-        <v>3173</v>
+        <v>3463</v>
       </c>
       <c r="E17" t="s">
-        <v>3340</v>
+        <v>3462</v>
       </c>
       <c r="G17" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R17" t="s">
         <v>322</v>
@@ -14712,58 +15183,58 @@
         <v>272</v>
       </c>
       <c r="T17" t="s">
-        <v>3299</v>
+        <v>3375</v>
       </c>
       <c r="U17" t="s">
-        <v>663</v>
+        <v>3460</v>
       </c>
       <c r="V17" t="s">
         <v>3015</v>
       </c>
       <c r="W17" t="s">
+        <v>528</v>
+      </c>
+      <c r="X17" t="s">
         <v>766</v>
       </c>
-      <c r="X17" t="s">
-        <v>3303</v>
-      </c>
       <c r="Y17" t="s">
-        <v>3312</v>
+        <v>1162</v>
       </c>
       <c r="Z17" t="s">
-        <v>3174</v>
+        <v>3162</v>
       </c>
       <c r="AA17" t="s">
-        <v>3230</v>
+        <v>3404</v>
       </c>
       <c r="AB17" t="s">
-        <v>1899</v>
+        <v>3387</v>
       </c>
       <c r="AC17" t="s">
-        <v>3300</v>
+        <v>2584</v>
       </c>
       <c r="AD17" t="s">
-        <v>723</v>
+        <v>3380</v>
       </c>
       <c r="AE17" t="s">
-        <v>1927</v>
+        <v>2266</v>
       </c>
       <c r="AF17" t="s">
-        <v>1932</v>
+        <v>3381</v>
       </c>
       <c r="AG17" t="s">
-        <v>528</v>
+        <v>2199</v>
       </c>
       <c r="AH17" t="s">
-        <v>1936</v>
+        <v>3417</v>
       </c>
       <c r="AI17" t="s">
-        <v>1432</v>
+        <v>3461</v>
       </c>
       <c r="AJ17" t="s">
-        <v>3173</v>
+        <v>3463</v>
       </c>
       <c r="AK17" t="s">
-        <v>3340</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -14774,16 +15245,16 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>2004</v>
+        <v>3465</v>
       </c>
       <c r="D18" t="s">
-        <v>3343</v>
+        <v>3467</v>
       </c>
       <c r="E18" t="s">
-        <v>3342</v>
+        <v>3466</v>
       </c>
       <c r="G18" t="s">
-        <v>680</v>
+        <v>880</v>
       </c>
       <c r="R18" t="s">
         <v>501</v>
@@ -14792,58 +15263,58 @@
         <v>787</v>
       </c>
       <c r="T18" t="s">
-        <v>667</v>
+        <v>3375</v>
       </c>
       <c r="U18" t="s">
-        <v>3341</v>
+        <v>3383</v>
       </c>
       <c r="V18" t="s">
-        <v>663</v>
+        <v>1162</v>
       </c>
       <c r="W18" t="s">
         <v>3015</v>
       </c>
       <c r="X18" t="s">
-        <v>3163</v>
+        <v>3403</v>
       </c>
       <c r="Y18" t="s">
-        <v>3174</v>
+        <v>3404</v>
       </c>
       <c r="Z18" t="s">
-        <v>3312</v>
+        <v>3308</v>
       </c>
       <c r="AA18" t="s">
-        <v>1151</v>
+        <v>3394</v>
       </c>
       <c r="AB18" t="s">
-        <v>3284</v>
+        <v>767</v>
       </c>
       <c r="AC18" t="s">
-        <v>723</v>
+        <v>3380</v>
       </c>
       <c r="AD18" t="s">
         <v>656</v>
       </c>
       <c r="AE18" t="s">
-        <v>1927</v>
+        <v>2569</v>
       </c>
       <c r="AF18" t="s">
-        <v>2595</v>
+        <v>3388</v>
       </c>
       <c r="AG18" t="s">
-        <v>2928</v>
+        <v>3464</v>
       </c>
       <c r="AH18" t="s">
         <v>786</v>
       </c>
       <c r="AI18" t="s">
-        <v>2004</v>
+        <v>3465</v>
       </c>
       <c r="AJ18" t="s">
-        <v>3343</v>
+        <v>3467</v>
       </c>
       <c r="AK18" t="s">
-        <v>3342</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -14854,16 +15325,16 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>279</v>
+        <v>3471</v>
       </c>
       <c r="D19" t="s">
-        <v>3345</v>
+        <v>3473</v>
       </c>
       <c r="E19" t="s">
-        <v>3344</v>
+        <v>3472</v>
       </c>
       <c r="G19" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="R19" t="s">
         <v>347</v>
@@ -14872,58 +15343,58 @@
         <v>792</v>
       </c>
       <c r="T19" t="s">
-        <v>3331</v>
+        <v>3375</v>
       </c>
       <c r="U19" t="s">
-        <v>3157</v>
+        <v>3427</v>
       </c>
       <c r="V19" t="s">
-        <v>799</v>
+        <v>3015</v>
       </c>
       <c r="W19" t="s">
-        <v>1349</v>
+        <v>3403</v>
       </c>
       <c r="X19" t="s">
-        <v>1151</v>
+        <v>3378</v>
       </c>
       <c r="Y19" t="s">
-        <v>3303</v>
+        <v>3389</v>
       </c>
       <c r="Z19" t="s">
-        <v>3169</v>
+        <v>3376</v>
       </c>
       <c r="AA19" t="s">
-        <v>3174</v>
+        <v>3395</v>
       </c>
       <c r="AB19" t="s">
-        <v>3312</v>
+        <v>3468</v>
       </c>
       <c r="AC19" t="s">
-        <v>3300</v>
+        <v>3432</v>
       </c>
       <c r="AD19" t="s">
-        <v>723</v>
+        <v>3380</v>
       </c>
       <c r="AE19" t="s">
-        <v>1927</v>
+        <v>3469</v>
       </c>
       <c r="AF19" t="s">
-        <v>3044</v>
+        <v>3470</v>
       </c>
       <c r="AG19" t="s">
-        <v>663</v>
+        <v>802</v>
       </c>
       <c r="AH19" t="s">
-        <v>1936</v>
+        <v>915</v>
       </c>
       <c r="AI19" t="s">
-        <v>279</v>
+        <v>3471</v>
       </c>
       <c r="AJ19" t="s">
-        <v>3345</v>
+        <v>3473</v>
       </c>
       <c r="AK19" t="s">
-        <v>3344</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -14934,16 +15405,16 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>248</v>
+        <v>1286</v>
       </c>
       <c r="D20" t="s">
-        <v>3347</v>
+        <v>3475</v>
       </c>
       <c r="E20" t="s">
-        <v>3346</v>
+        <v>3474</v>
       </c>
       <c r="G20" t="s">
-        <v>646</v>
+        <v>426</v>
       </c>
       <c r="R20" t="s">
         <v>516</v>
@@ -14952,58 +15423,58 @@
         <v>796</v>
       </c>
       <c r="T20" t="s">
-        <v>3331</v>
+        <v>2963</v>
       </c>
       <c r="U20" t="s">
-        <v>2064</v>
+        <v>3403</v>
       </c>
       <c r="V20" t="s">
-        <v>915</v>
+        <v>3015</v>
       </c>
       <c r="W20" t="s">
-        <v>3015</v>
+        <v>3409</v>
       </c>
       <c r="X20" t="s">
-        <v>3174</v>
+        <v>3378</v>
       </c>
       <c r="Y20" t="s">
-        <v>3303</v>
+        <v>3308</v>
       </c>
       <c r="Z20" t="s">
-        <v>3312</v>
+        <v>3162</v>
       </c>
       <c r="AA20" t="s">
         <v>3204</v>
       </c>
       <c r="AB20" t="s">
-        <v>1899</v>
+        <v>3395</v>
       </c>
       <c r="AC20" t="s">
-        <v>723</v>
+        <v>2584</v>
       </c>
       <c r="AD20" t="s">
-        <v>3300</v>
+        <v>3380</v>
       </c>
       <c r="AE20" t="s">
         <v>1806</v>
       </c>
       <c r="AF20" t="s">
-        <v>3238</v>
+        <v>3381</v>
       </c>
       <c r="AG20" t="s">
-        <v>663</v>
+        <v>1162</v>
       </c>
       <c r="AH20" t="s">
-        <v>1933</v>
+        <v>915</v>
       </c>
       <c r="AI20" t="s">
-        <v>248</v>
+        <v>1286</v>
       </c>
       <c r="AJ20" t="s">
-        <v>3347</v>
+        <v>3475</v>
       </c>
       <c r="AK20" t="s">
-        <v>3346</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -15014,16 +15485,16 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>1432</v>
+        <v>3477</v>
       </c>
       <c r="D21" t="s">
-        <v>3345</v>
+        <v>3479</v>
       </c>
       <c r="E21" t="s">
-        <v>3348</v>
+        <v>3478</v>
       </c>
       <c r="G21" t="s">
-        <v>646</v>
+        <v>880</v>
       </c>
       <c r="R21" t="s">
         <v>375</v>
@@ -15032,58 +15503,58 @@
         <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>3331</v>
+        <v>2569</v>
       </c>
       <c r="U21" t="s">
-        <v>3157</v>
+        <v>3015</v>
       </c>
       <c r="V21" t="s">
-        <v>3015</v>
+        <v>1162</v>
       </c>
       <c r="W21" t="s">
-        <v>766</v>
+        <v>3403</v>
       </c>
       <c r="X21" t="s">
-        <v>3303</v>
+        <v>3162</v>
       </c>
       <c r="Y21" t="s">
-        <v>3174</v>
+        <v>3388</v>
       </c>
       <c r="Z21" t="s">
-        <v>3163</v>
+        <v>3308</v>
       </c>
       <c r="AA21" t="s">
-        <v>3312</v>
+        <v>3404</v>
       </c>
       <c r="AB21" t="s">
-        <v>1151</v>
+        <v>3394</v>
       </c>
       <c r="AC21" t="s">
-        <v>1954</v>
+        <v>3399</v>
       </c>
       <c r="AD21" t="s">
-        <v>3313</v>
+        <v>3476</v>
       </c>
       <c r="AE21" t="s">
-        <v>667</v>
+        <v>2963</v>
       </c>
       <c r="AF21" t="s">
         <v>1967</v>
       </c>
       <c r="AG21" t="s">
-        <v>663</v>
+        <v>766</v>
       </c>
       <c r="AH21" t="s">
-        <v>1933</v>
+        <v>3382</v>
       </c>
       <c r="AI21" t="s">
-        <v>1432</v>
+        <v>3477</v>
       </c>
       <c r="AJ21" t="s">
-        <v>3345</v>
+        <v>3479</v>
       </c>
       <c r="AK21" t="s">
-        <v>3348</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -15094,16 +15565,16 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>677</v>
+        <v>3465</v>
       </c>
       <c r="D22" t="s">
-        <v>3352</v>
+        <v>3481</v>
       </c>
       <c r="E22" t="s">
-        <v>3351</v>
+        <v>3480</v>
       </c>
       <c r="G22" t="s">
-        <v>627</v>
+        <v>3415</v>
       </c>
       <c r="R22" t="s">
         <v>573</v>
@@ -15112,58 +15583,58 @@
         <v>804</v>
       </c>
       <c r="T22" t="s">
-        <v>3331</v>
+        <v>3375</v>
       </c>
       <c r="U22" t="s">
         <v>3015</v>
       </c>
       <c r="V22" t="s">
-        <v>799</v>
+        <v>3430</v>
       </c>
       <c r="W22" t="s">
-        <v>663</v>
+        <v>1162</v>
       </c>
       <c r="X22" t="s">
-        <v>3349</v>
+        <v>3398</v>
       </c>
       <c r="Y22" t="s">
-        <v>3350</v>
+        <v>2199</v>
       </c>
       <c r="Z22" t="s">
-        <v>3230</v>
+        <v>3404</v>
       </c>
       <c r="AA22" t="s">
-        <v>3174</v>
+        <v>3162</v>
       </c>
       <c r="AB22" t="s">
-        <v>1899</v>
+        <v>3395</v>
       </c>
       <c r="AC22" t="s">
+        <v>2584</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>3380</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>2963</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>3442</v>
+      </c>
+      <c r="AG22" t="s">
         <v>656</v>
       </c>
-      <c r="AD22" t="s">
-        <v>723</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF22" t="s">
+      <c r="AH22" t="s">
         <v>3161</v>
       </c>
-      <c r="AG22" t="s">
-        <v>2928</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>2927</v>
-      </c>
       <c r="AI22" t="s">
-        <v>677</v>
+        <v>3465</v>
       </c>
       <c r="AJ22" t="s">
-        <v>3352</v>
+        <v>3481</v>
       </c>
       <c r="AK22" t="s">
-        <v>3351</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -15174,16 +15645,16 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>279</v>
+        <v>3406</v>
       </c>
       <c r="D23" t="s">
-        <v>3356</v>
+        <v>3273</v>
       </c>
       <c r="E23" t="s">
-        <v>3355</v>
+        <v>3484</v>
       </c>
       <c r="G23" t="s">
-        <v>552</v>
+        <v>627</v>
       </c>
       <c r="R23" t="s">
         <v>809</v>
@@ -15192,58 +15663,58 @@
         <v>281</v>
       </c>
       <c r="T23" t="s">
-        <v>3353</v>
+        <v>3482</v>
       </c>
       <c r="U23" t="s">
-        <v>354</v>
+        <v>3015</v>
       </c>
       <c r="V23" t="s">
-        <v>1349</v>
+        <v>3383</v>
       </c>
       <c r="W23" t="s">
-        <v>3015</v>
+        <v>3403</v>
       </c>
       <c r="X23" t="s">
-        <v>3238</v>
+        <v>3483</v>
       </c>
       <c r="Y23" t="s">
-        <v>3308</v>
+        <v>3395</v>
       </c>
       <c r="Z23" t="s">
-        <v>3303</v>
+        <v>3422</v>
       </c>
       <c r="AA23" t="s">
-        <v>3354</v>
+        <v>3378</v>
       </c>
       <c r="AB23" t="s">
-        <v>1967</v>
+        <v>3376</v>
       </c>
       <c r="AC23" t="s">
-        <v>3295</v>
+        <v>3380</v>
       </c>
       <c r="AD23" t="s">
-        <v>723</v>
+        <v>3025</v>
       </c>
       <c r="AE23" t="s">
         <v>373</v>
       </c>
       <c r="AF23" t="s">
-        <v>1930</v>
+        <v>3162</v>
       </c>
       <c r="AG23" t="s">
-        <v>1937</v>
+        <v>3443</v>
       </c>
       <c r="AH23" t="s">
-        <v>663</v>
+        <v>1967</v>
       </c>
       <c r="AI23" t="s">
-        <v>279</v>
+        <v>3406</v>
       </c>
       <c r="AJ23" t="s">
-        <v>3356</v>
+        <v>3273</v>
       </c>
       <c r="AK23" t="s">
-        <v>3355</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -15254,16 +15725,16 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>2004</v>
+        <v>3487</v>
       </c>
       <c r="D24" t="s">
-        <v>3148</v>
+        <v>3372</v>
       </c>
       <c r="E24" t="s">
-        <v>3357</v>
+        <v>3488</v>
       </c>
       <c r="G24" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R24" t="s">
         <v>562</v>
@@ -15272,58 +15743,58 @@
         <v>283</v>
       </c>
       <c r="T24" t="s">
-        <v>667</v>
+        <v>2569</v>
       </c>
       <c r="U24" t="s">
-        <v>2016</v>
+        <v>3485</v>
       </c>
       <c r="V24" t="s">
-        <v>3248</v>
+        <v>3483</v>
       </c>
       <c r="W24" t="s">
         <v>3015</v>
       </c>
       <c r="X24" t="s">
-        <v>3249</v>
+        <v>3486</v>
       </c>
       <c r="Y24" t="s">
-        <v>3250</v>
+        <v>3468</v>
       </c>
       <c r="Z24" t="s">
-        <v>3251</v>
+        <v>1370</v>
       </c>
       <c r="AA24" t="s">
-        <v>3169</v>
+        <v>3378</v>
       </c>
       <c r="AB24" t="s">
-        <v>3230</v>
+        <v>3395</v>
       </c>
       <c r="AC24" t="s">
-        <v>3304</v>
+        <v>3410</v>
       </c>
       <c r="AD24" t="s">
-        <v>723</v>
+        <v>3380</v>
       </c>
       <c r="AE24" t="s">
-        <v>1927</v>
+        <v>3375</v>
       </c>
       <c r="AF24" t="s">
-        <v>3200</v>
+        <v>3427</v>
       </c>
       <c r="AG24" t="s">
-        <v>3252</v>
+        <v>3476</v>
       </c>
       <c r="AH24" t="s">
-        <v>1933</v>
+        <v>3403</v>
       </c>
       <c r="AI24" t="s">
-        <v>2004</v>
+        <v>3487</v>
       </c>
       <c r="AJ24" t="s">
-        <v>3148</v>
+        <v>3372</v>
       </c>
       <c r="AK24" t="s">
-        <v>3357</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -15334,13 +15805,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>795</v>
+        <v>686</v>
       </c>
       <c r="D25" t="s">
-        <v>3360</v>
+        <v>3494</v>
       </c>
       <c r="E25" t="s">
-        <v>3359</v>
+        <v>3493</v>
       </c>
       <c r="G25" t="s">
         <v>627</v>
@@ -15352,58 +15823,58 @@
         <v>461</v>
       </c>
       <c r="T25" t="s">
-        <v>667</v>
+        <v>1145</v>
       </c>
       <c r="U25" t="s">
-        <v>3183</v>
+        <v>3438</v>
       </c>
       <c r="V25" t="s">
-        <v>354</v>
+        <v>3489</v>
       </c>
       <c r="W25" t="s">
-        <v>2928</v>
+        <v>3416</v>
       </c>
       <c r="X25" t="s">
-        <v>3358</v>
+        <v>712</v>
       </c>
       <c r="Y25" t="s">
-        <v>2840</v>
+        <v>1138</v>
       </c>
       <c r="Z25" t="s">
-        <v>357</v>
+        <v>2179</v>
       </c>
       <c r="AA25" t="s">
-        <v>1138</v>
+        <v>3376</v>
       </c>
       <c r="AB25" t="s">
+        <v>3432</v>
+      </c>
+      <c r="AC25" t="s">
         <v>656</v>
       </c>
-      <c r="AC25" t="s">
-        <v>3257</v>
-      </c>
       <c r="AD25" t="s">
-        <v>3256</v>
+        <v>3490</v>
       </c>
       <c r="AE25" t="s">
-        <v>2986</v>
+        <v>2569</v>
       </c>
       <c r="AF25" t="s">
-        <v>2927</v>
+        <v>3491</v>
       </c>
       <c r="AG25" t="s">
-        <v>724</v>
+        <v>3418</v>
       </c>
       <c r="AH25" t="s">
-        <v>1940</v>
+        <v>3492</v>
       </c>
       <c r="AI25" t="s">
-        <v>795</v>
+        <v>686</v>
       </c>
       <c r="AJ25" t="s">
-        <v>3360</v>
+        <v>3494</v>
       </c>
       <c r="AK25" t="s">
-        <v>3359</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -15414,16 +15885,16 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>1502</v>
       </c>
       <c r="D26" t="s">
-        <v>2057</v>
+        <v>3496</v>
       </c>
       <c r="E26" t="s">
-        <v>3361</v>
+        <v>3495</v>
       </c>
       <c r="G26" t="s">
-        <v>680</v>
+        <v>3415</v>
       </c>
       <c r="R26" t="s">
         <v>569</v>
@@ -15432,58 +15903,58 @@
         <v>572</v>
       </c>
       <c r="T26" t="s">
-        <v>1357</v>
+        <v>3375</v>
       </c>
       <c r="U26" t="s">
-        <v>3157</v>
+        <v>3015</v>
       </c>
       <c r="V26" t="s">
-        <v>3261</v>
+        <v>2226</v>
       </c>
       <c r="W26" t="s">
-        <v>3015</v>
+        <v>3383</v>
       </c>
       <c r="X26" t="s">
-        <v>3303</v>
+        <v>1162</v>
       </c>
       <c r="Y26" t="s">
-        <v>3174</v>
+        <v>3378</v>
       </c>
       <c r="Z26" t="s">
-        <v>3163</v>
+        <v>3308</v>
       </c>
       <c r="AA26" t="s">
-        <v>3308</v>
+        <v>3162</v>
       </c>
       <c r="AB26" t="s">
-        <v>3170</v>
+        <v>3395</v>
       </c>
       <c r="AC26" t="s">
-        <v>3304</v>
+        <v>3432</v>
       </c>
       <c r="AD26" t="s">
+        <v>2584</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>3385</v>
+      </c>
+      <c r="AF26" t="s">
         <v>1967</v>
       </c>
-      <c r="AE26" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>1930</v>
-      </c>
       <c r="AG26" t="s">
-        <v>1899</v>
+        <v>3396</v>
       </c>
       <c r="AH26" t="s">
-        <v>663</v>
+        <v>2180</v>
       </c>
       <c r="AI26" t="s">
-        <v>273</v>
+        <v>1502</v>
       </c>
       <c r="AJ26" t="s">
-        <v>2057</v>
+        <v>3496</v>
       </c>
       <c r="AK26" t="s">
-        <v>3361</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -15494,16 +15965,16 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>293</v>
+        <v>1223</v>
       </c>
       <c r="D27" t="s">
-        <v>3363</v>
+        <v>3499</v>
       </c>
       <c r="E27" t="s">
-        <v>3362</v>
+        <v>3498</v>
       </c>
       <c r="G27" t="s">
-        <v>646</v>
+        <v>1252</v>
       </c>
       <c r="R27" t="s">
         <v>828</v>
@@ -15512,58 +15983,58 @@
         <v>827</v>
       </c>
       <c r="T27" t="s">
-        <v>3331</v>
+        <v>2569</v>
       </c>
       <c r="U27" t="s">
-        <v>663</v>
+        <v>3015</v>
       </c>
       <c r="V27" t="s">
-        <v>3015</v>
+        <v>528</v>
       </c>
       <c r="W27" t="s">
-        <v>1349</v>
+        <v>3430</v>
       </c>
       <c r="X27" t="s">
-        <v>3303</v>
+        <v>3162</v>
       </c>
       <c r="Y27" t="s">
-        <v>3174</v>
+        <v>3497</v>
       </c>
       <c r="Z27" t="s">
-        <v>3312</v>
+        <v>3378</v>
       </c>
       <c r="AA27" t="s">
-        <v>1151</v>
+        <v>3394</v>
       </c>
       <c r="AB27" t="s">
-        <v>723</v>
+        <v>3380</v>
       </c>
       <c r="AC27" t="s">
-        <v>1899</v>
+        <v>2584</v>
       </c>
       <c r="AD27" t="s">
-        <v>3313</v>
+        <v>3410</v>
       </c>
       <c r="AE27" t="s">
-        <v>667</v>
+        <v>2963</v>
       </c>
       <c r="AF27" t="s">
-        <v>528</v>
+        <v>1162</v>
       </c>
       <c r="AG27" t="s">
+        <v>3443</v>
+      </c>
+      <c r="AH27" t="s">
         <v>1140</v>
       </c>
-      <c r="AH27" t="s">
-        <v>2927</v>
-      </c>
       <c r="AI27" t="s">
-        <v>293</v>
+        <v>1223</v>
       </c>
       <c r="AJ27" t="s">
-        <v>3363</v>
+        <v>3499</v>
       </c>
       <c r="AK27" t="s">
-        <v>3362</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -15574,16 +16045,16 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>1250</v>
+        <v>3500</v>
       </c>
       <c r="D28" t="s">
-        <v>2124</v>
+        <v>3502</v>
       </c>
       <c r="E28" t="s">
-        <v>3364</v>
+        <v>3501</v>
       </c>
       <c r="G28" t="s">
-        <v>680</v>
+        <v>1252</v>
       </c>
       <c r="R28" t="s">
         <v>832</v>
@@ -15592,58 +16063,58 @@
         <v>831</v>
       </c>
       <c r="T28" t="s">
-        <v>3299</v>
+        <v>3375</v>
       </c>
       <c r="U28" t="s">
+        <v>1162</v>
+      </c>
+      <c r="V28" t="s">
+        <v>3398</v>
+      </c>
+      <c r="W28" t="s">
         <v>3015</v>
       </c>
-      <c r="V28" t="s">
-        <v>3325</v>
-      </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
+        <v>3408</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>3404</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>3376</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>3394</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>3162</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>3432</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>3476</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>2266</v>
+      </c>
+      <c r="AF28" t="s">
         <v>766</v>
       </c>
-      <c r="X28" t="s">
-        <v>3303</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>3169</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>3312</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>3170</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>1386</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>1954</v>
-      </c>
-      <c r="AD28" t="s">
+      <c r="AG28" t="s">
         <v>1967</v>
       </c>
-      <c r="AE28" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>663</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>3265</v>
-      </c>
       <c r="AH28" t="s">
-        <v>1941</v>
+        <v>3396</v>
       </c>
       <c r="AI28" t="s">
-        <v>1250</v>
+        <v>3500</v>
       </c>
       <c r="AJ28" t="s">
-        <v>2124</v>
+        <v>3502</v>
       </c>
       <c r="AK28" t="s">
-        <v>3364</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -15654,16 +16125,16 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>2147</v>
+        <v>3406</v>
       </c>
       <c r="D29" t="s">
-        <v>3366</v>
+        <v>3506</v>
       </c>
       <c r="E29" t="s">
-        <v>3365</v>
+        <v>3505</v>
       </c>
       <c r="G29" t="s">
-        <v>646</v>
+        <v>426</v>
       </c>
       <c r="R29" t="s">
         <v>837</v>
@@ -15672,58 +16143,58 @@
         <v>836</v>
       </c>
       <c r="T29" t="s">
-        <v>3331</v>
+        <v>2569</v>
       </c>
       <c r="U29" t="s">
-        <v>3183</v>
+        <v>3403</v>
       </c>
       <c r="V29" t="s">
-        <v>3268</v>
+        <v>1162</v>
       </c>
       <c r="W29" t="s">
         <v>3015</v>
       </c>
       <c r="X29" t="s">
-        <v>3170</v>
+        <v>3404</v>
       </c>
       <c r="Y29" t="s">
-        <v>3169</v>
+        <v>3162</v>
       </c>
       <c r="Z29" t="s">
-        <v>3174</v>
+        <v>3503</v>
       </c>
       <c r="AA29" t="s">
-        <v>2197</v>
+        <v>3396</v>
       </c>
       <c r="AB29" t="s">
-        <v>3303</v>
+        <v>3504</v>
       </c>
       <c r="AC29" t="s">
-        <v>1954</v>
+        <v>3458</v>
       </c>
       <c r="AD29" t="s">
-        <v>3304</v>
+        <v>3432</v>
       </c>
       <c r="AE29" t="s">
-        <v>667</v>
+        <v>2963</v>
       </c>
       <c r="AF29" t="s">
-        <v>663</v>
+        <v>3416</v>
       </c>
       <c r="AG29" t="s">
+        <v>512</v>
+      </c>
+      <c r="AH29" t="s">
         <v>3269</v>
       </c>
-      <c r="AH29" t="s">
-        <v>1933</v>
-      </c>
       <c r="AI29" t="s">
-        <v>2147</v>
+        <v>3406</v>
       </c>
       <c r="AJ29" t="s">
-        <v>3366</v>
+        <v>3506</v>
       </c>
       <c r="AK29" t="s">
-        <v>3365</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -15734,16 +16205,16 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>258</v>
+        <v>3507</v>
       </c>
       <c r="D30" t="s">
-        <v>3368</v>
+        <v>3509</v>
       </c>
       <c r="E30" t="s">
-        <v>3367</v>
+        <v>3508</v>
       </c>
       <c r="G30" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R30" t="s">
         <v>840</v>
@@ -15752,58 +16223,58 @@
         <v>289</v>
       </c>
       <c r="T30" t="s">
-        <v>3331</v>
+        <v>3375</v>
       </c>
       <c r="U30" t="s">
-        <v>2064</v>
+        <v>3015</v>
       </c>
       <c r="V30" t="s">
-        <v>3307</v>
+        <v>2226</v>
       </c>
       <c r="W30" t="s">
-        <v>3015</v>
+        <v>3403</v>
       </c>
       <c r="X30" t="s">
-        <v>3312</v>
+        <v>3204</v>
       </c>
       <c r="Y30" t="s">
-        <v>3303</v>
+        <v>3396</v>
       </c>
       <c r="Z30" t="s">
-        <v>3163</v>
+        <v>3395</v>
       </c>
       <c r="AA30" t="s">
-        <v>3174</v>
+        <v>3394</v>
       </c>
       <c r="AB30" t="s">
-        <v>1899</v>
+        <v>3378</v>
       </c>
       <c r="AC30" t="s">
-        <v>1196</v>
+        <v>3432</v>
       </c>
       <c r="AD30" t="s">
-        <v>723</v>
+        <v>3410</v>
       </c>
       <c r="AE30" t="s">
-        <v>667</v>
+        <v>2569</v>
       </c>
       <c r="AF30" t="s">
-        <v>1941</v>
+        <v>3435</v>
       </c>
       <c r="AG30" t="s">
-        <v>663</v>
+        <v>3386</v>
       </c>
       <c r="AH30" t="s">
-        <v>2837</v>
+        <v>1967</v>
       </c>
       <c r="AI30" t="s">
-        <v>258</v>
+        <v>3507</v>
       </c>
       <c r="AJ30" t="s">
-        <v>3368</v>
+        <v>3509</v>
       </c>
       <c r="AK30" t="s">
-        <v>3367</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -15814,16 +16285,16 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>3054</v>
+        <v>627</v>
       </c>
       <c r="D31" t="s">
-        <v>3370</v>
+        <v>3524</v>
       </c>
       <c r="E31" t="s">
-        <v>3369</v>
+        <v>3523</v>
       </c>
       <c r="G31" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R31" t="s">
         <v>844</v>
@@ -15832,58 +16303,58 @@
         <v>843</v>
       </c>
       <c r="T31" t="s">
-        <v>3331</v>
+        <v>3089</v>
       </c>
       <c r="U31" t="s">
-        <v>3274</v>
+        <v>3510</v>
       </c>
       <c r="V31" t="s">
-        <v>3015</v>
+        <v>3511</v>
       </c>
       <c r="W31" t="s">
-        <v>3157</v>
+        <v>3191</v>
       </c>
       <c r="X31" t="s">
-        <v>3303</v>
+        <v>3512</v>
       </c>
       <c r="Y31" t="s">
-        <v>3170</v>
+        <v>3513</v>
       </c>
       <c r="Z31" t="s">
-        <v>3174</v>
+        <v>3514</v>
       </c>
       <c r="AA31" t="s">
-        <v>3308</v>
+        <v>3515</v>
       </c>
       <c r="AB31" t="s">
-        <v>3304</v>
+        <v>3516</v>
       </c>
       <c r="AC31" t="s">
-        <v>1954</v>
+        <v>3517</v>
       </c>
       <c r="AD31" t="s">
-        <v>723</v>
+        <v>3518</v>
       </c>
       <c r="AE31" t="s">
-        <v>667</v>
+        <v>3519</v>
       </c>
       <c r="AF31" t="s">
-        <v>1932</v>
+        <v>3520</v>
       </c>
       <c r="AG31" t="s">
-        <v>1349</v>
+        <v>3521</v>
       </c>
       <c r="AH31" t="s">
-        <v>663</v>
+        <v>3522</v>
       </c>
       <c r="AI31" t="s">
-        <v>3054</v>
+        <v>627</v>
       </c>
       <c r="AJ31" t="s">
-        <v>3370</v>
+        <v>3524</v>
       </c>
       <c r="AK31" t="s">
-        <v>3369</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -15894,16 +16365,16 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>275</v>
+        <v>1243</v>
       </c>
       <c r="D32" t="s">
-        <v>3372</v>
+        <v>3528</v>
       </c>
       <c r="E32" t="s">
-        <v>3371</v>
+        <v>3527</v>
       </c>
       <c r="G32" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R32" t="s">
         <v>494</v>
@@ -15912,58 +16383,58 @@
         <v>849</v>
       </c>
       <c r="T32" t="s">
-        <v>410</v>
+        <v>3375</v>
       </c>
       <c r="U32" t="s">
-        <v>3183</v>
+        <v>3403</v>
       </c>
       <c r="V32" t="s">
+        <v>3446</v>
+      </c>
+      <c r="W32" t="s">
         <v>3015</v>
       </c>
-      <c r="W32" t="s">
-        <v>2905</v>
-      </c>
       <c r="X32" t="s">
-        <v>3303</v>
+        <v>3423</v>
       </c>
       <c r="Y32" t="s">
-        <v>3312</v>
+        <v>3378</v>
       </c>
       <c r="Z32" t="s">
-        <v>3163</v>
+        <v>3525</v>
       </c>
       <c r="AA32" t="s">
-        <v>3174</v>
+        <v>3376</v>
       </c>
       <c r="AB32" t="s">
         <v>3204</v>
       </c>
       <c r="AC32" t="s">
-        <v>723</v>
+        <v>3399</v>
       </c>
       <c r="AD32" t="s">
-        <v>656</v>
+        <v>3432</v>
       </c>
       <c r="AE32" t="s">
-        <v>667</v>
+        <v>3526</v>
       </c>
       <c r="AF32" t="s">
-        <v>663</v>
+        <v>3162</v>
       </c>
       <c r="AG32" t="s">
-        <v>3277</v>
+        <v>3390</v>
       </c>
       <c r="AH32" t="s">
-        <v>2837</v>
+        <v>3420</v>
       </c>
       <c r="AI32" t="s">
-        <v>275</v>
+        <v>1243</v>
       </c>
       <c r="AJ32" t="s">
-        <v>3372</v>
+        <v>3528</v>
       </c>
       <c r="AK32" t="s">
-        <v>3371</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -15974,16 +16445,16 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>275</v>
+        <v>3529</v>
       </c>
       <c r="D33" t="s">
-        <v>3374</v>
+        <v>3531</v>
       </c>
       <c r="E33" t="s">
-        <v>3373</v>
+        <v>3530</v>
       </c>
       <c r="G33" t="s">
-        <v>680</v>
+        <v>880</v>
       </c>
       <c r="R33" t="s">
         <v>418</v>
@@ -15992,58 +16463,58 @@
         <v>241</v>
       </c>
       <c r="T33" t="s">
-        <v>667</v>
+        <v>3375</v>
       </c>
       <c r="U33" t="s">
         <v>766</v>
       </c>
       <c r="V33" t="s">
-        <v>3157</v>
+        <v>1162</v>
       </c>
       <c r="W33" t="s">
         <v>3015</v>
       </c>
       <c r="X33" t="s">
-        <v>3303</v>
+        <v>3395</v>
       </c>
       <c r="Y33" t="s">
-        <v>3174</v>
+        <v>3404</v>
       </c>
       <c r="Z33" t="s">
-        <v>3163</v>
+        <v>3308</v>
       </c>
       <c r="AA33" t="s">
-        <v>3312</v>
+        <v>3162</v>
       </c>
       <c r="AB33" t="s">
-        <v>1899</v>
+        <v>3380</v>
       </c>
       <c r="AC33" t="s">
-        <v>3313</v>
+        <v>3432</v>
       </c>
       <c r="AD33" t="s">
-        <v>723</v>
+        <v>2584</v>
       </c>
       <c r="AE33" t="s">
-        <v>1927</v>
+        <v>2569</v>
       </c>
       <c r="AF33" t="s">
-        <v>3161</v>
+        <v>3489</v>
       </c>
       <c r="AG33" t="s">
-        <v>2927</v>
+        <v>3388</v>
       </c>
       <c r="AH33" t="s">
-        <v>663</v>
+        <v>3382</v>
       </c>
       <c r="AI33" t="s">
-        <v>275</v>
+        <v>3529</v>
       </c>
       <c r="AJ33" t="s">
-        <v>3374</v>
+        <v>3531</v>
       </c>
       <c r="AK33" t="s">
-        <v>3373</v>
+        <v>3530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GW 27 2nd last MD
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17339" uniqueCount="3628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20314" uniqueCount="3986">
   <si>
     <t>Places</t>
   </si>
@@ -10918,6 +10918,1080 @@
   </si>
   <si>
     <t>1685</t>
+  </si>
+  <si>
+    <t>Alexander-Arnold -</t>
+  </si>
+  <si>
+    <t>Cancelo EVE (A)</t>
+  </si>
+  <si>
+    <t>Son LEE (A)</t>
+  </si>
+  <si>
+    <t>Benrahma WOL (H)</t>
+  </si>
+  <si>
+    <t>Bernardo EVE (A)</t>
+  </si>
+  <si>
+    <t>Salah -$ captain</t>
+  </si>
+  <si>
+    <t>Dennis MUN (A)</t>
+  </si>
+  <si>
+    <t>Maupay AVL (H)</t>
+  </si>
+  <si>
+    <t>Sánchez AVL (H)</t>
+  </si>
+  <si>
+    <t>Livramento 8</t>
+  </si>
+  <si>
+    <t>Archer BHA (A)</t>
+  </si>
+  <si>
+    <t>2,056,925</t>
+  </si>
+  <si>
+    <t>Guaita BUR (H)</t>
+  </si>
+  <si>
+    <t>Coady WHU (A)</t>
+  </si>
+  <si>
+    <t>Bowen WOL (H)</t>
+  </si>
+  <si>
+    <t>Gallagher BUR (H)</t>
+  </si>
+  <si>
+    <t>Mané -</t>
+  </si>
+  <si>
+    <t>Adams 6</t>
+  </si>
+  <si>
+    <t>2,478,922</t>
+  </si>
+  <si>
+    <t>Pope CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>Walker-Peters 9</t>
+  </si>
+  <si>
+    <t>Roberts CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>Sterling EVE (A)</t>
+  </si>
+  <si>
+    <t>Mahrez EVE (A)</t>
+  </si>
+  <si>
+    <t>Sancho WAT (H)</t>
+  </si>
+  <si>
+    <t>Weghorst CRY (A), LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>Kane LEE (A)</t>
+  </si>
+  <si>
+    <t>Matthews BUR (H)</t>
+  </si>
+  <si>
+    <t>Amartey BUR (A)</t>
+  </si>
+  <si>
+    <t>Dewsbury-Hall BUR (A)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>535,398</t>
+  </si>
+  <si>
+    <t>1561</t>
+  </si>
+  <si>
+    <t>Lloris LEE (A)</t>
+  </si>
+  <si>
+    <t>Maddison BUR (A)</t>
+  </si>
+  <si>
+    <t>Gallagher BUR (H)$ captain</t>
+  </si>
+  <si>
+    <t>Saint-Maximin BRE (A)</t>
+  </si>
+  <si>
+    <t>Foster MUN (A)</t>
+  </si>
+  <si>
+    <t>Robertson -</t>
+  </si>
+  <si>
+    <t>Salah -</t>
+  </si>
+  <si>
+    <t>285,332</t>
+  </si>
+  <si>
+    <t>1614</t>
+  </si>
+  <si>
+    <t>Ait Nouri WHU (A)</t>
+  </si>
+  <si>
+    <t>Davies LEE (A)</t>
+  </si>
+  <si>
+    <t>Mings BHA (A)</t>
+  </si>
+  <si>
+    <t>Sissoko MUN (A)</t>
+  </si>
+  <si>
+    <t>Winks LEE (A)</t>
+  </si>
+  <si>
+    <t>Fernandes WAT (H)$ captain</t>
+  </si>
+  <si>
+    <t>Hwang WHU (A)</t>
+  </si>
+  <si>
+    <t>Rodriguez CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>Bachmann MUN (A)</t>
+  </si>
+  <si>
+    <t>1,220,778</t>
+  </si>
+  <si>
+    <t>Dias EVE (A)</t>
+  </si>
+  <si>
+    <t>Reguilón LEE (A)</t>
+  </si>
+  <si>
+    <t>Duffy AVL (H)</t>
+  </si>
+  <si>
+    <t>Jota -</t>
+  </si>
+  <si>
+    <t>Antonio WOL (H)</t>
+  </si>
+  <si>
+    <t>Ronaldo WAT (H)</t>
+  </si>
+  <si>
+    <t>Steele AVL (H)</t>
+  </si>
+  <si>
+    <t>Tsimikas -</t>
+  </si>
+  <si>
+    <t>Allan MCI (H)</t>
+  </si>
+  <si>
+    <t>3,164,026</t>
+  </si>
+  <si>
+    <t>Veltman AVL (H)</t>
+  </si>
+  <si>
+    <t>Pinnock NEW (H)</t>
+  </si>
+  <si>
+    <t>Semedo WHU (A)</t>
+  </si>
+  <si>
+    <t>Zaha BUR (H)</t>
+  </si>
+  <si>
+    <t>Sarr MUN (A)</t>
+  </si>
+  <si>
+    <t>De Bruyne EVE (A)</t>
+  </si>
+  <si>
+    <t>Carson EVE (A)</t>
+  </si>
+  <si>
+    <t>682,708</t>
+  </si>
+  <si>
+    <t>Saïss WHU (A)</t>
+  </si>
+  <si>
+    <t>Højbjerg LEE (A)</t>
+  </si>
+  <si>
+    <t>Manquillo BRE (A)</t>
+  </si>
+  <si>
+    <t>1,275,887</t>
+  </si>
+  <si>
+    <t>1467</t>
+  </si>
+  <si>
+    <t>Jansson NEW (H)</t>
+  </si>
+  <si>
+    <t>Coutinho BHA (A)</t>
+  </si>
+  <si>
+    <t>Ward BUR (A)</t>
+  </si>
+  <si>
+    <t>727,226</t>
+  </si>
+  <si>
+    <t>1531</t>
+  </si>
+  <si>
+    <t>Mee CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>McNeil CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>Weghorst CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>King MUN (A)</t>
+  </si>
+  <si>
+    <t>Raya NEW (H)</t>
+  </si>
+  <si>
+    <t>522,857</t>
+  </si>
+  <si>
+    <t>1563</t>
+  </si>
+  <si>
+    <t>Ederson EVE (A)</t>
+  </si>
+  <si>
+    <t>van Dijk -</t>
+  </si>
+  <si>
+    <t>Tarkowski CRY (A), LEI (H)</t>
+  </si>
+  <si>
+    <t>Varane WAT (H)</t>
+  </si>
+  <si>
+    <t>Lucas Moura LEE (A)</t>
+  </si>
+  <si>
+    <t>Bowen WOL (H)$ captain</t>
+  </si>
+  <si>
+    <t>400,827</t>
+  </si>
+  <si>
+    <t>1587</t>
+  </si>
+  <si>
+    <t>Laporte EVE (A)</t>
+  </si>
+  <si>
+    <t>Son LEE (A)$ captain</t>
+  </si>
+  <si>
+    <t>872,858</t>
+  </si>
+  <si>
+    <t>de Gea WAT (H)</t>
+  </si>
+  <si>
+    <t>Mee CRY (A), LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>Kilman WHU (A)</t>
+  </si>
+  <si>
+    <t>Raphinha TOT (H)</t>
+  </si>
+  <si>
+    <t>Ward-Prowse 3</t>
+  </si>
+  <si>
+    <t>Matip -</t>
+  </si>
+  <si>
+    <t>1,103,373</t>
+  </si>
+  <si>
+    <t>Marçal WHU (A)</t>
+  </si>
+  <si>
+    <t>Lamptey AVL (H)</t>
+  </si>
+  <si>
+    <t>618,966</t>
+  </si>
+  <si>
+    <t>Sá WHU (A)</t>
+  </si>
+  <si>
+    <t>Jota -$ captain</t>
+  </si>
+  <si>
+    <t>Fernandes WAT (H)</t>
+  </si>
+  <si>
+    <t>Soucek WOL (H)</t>
+  </si>
+  <si>
+    <t>Watkins BHA (A)</t>
+  </si>
+  <si>
+    <t>1,600,294</t>
+  </si>
+  <si>
+    <t>Digne BHA (A)</t>
+  </si>
+  <si>
+    <t>Foden EVE (A)</t>
+  </si>
+  <si>
+    <t>Dennis MUN (A)$ captain</t>
+  </si>
+  <si>
+    <t>946,876</t>
+  </si>
+  <si>
+    <t>Bednarek 6</t>
+  </si>
+  <si>
+    <t>Maguire WAT (H)</t>
+  </si>
+  <si>
+    <t>771,318</t>
+  </si>
+  <si>
+    <t>1525</t>
+  </si>
+  <si>
+    <t>Coufal WOL (H)</t>
+  </si>
+  <si>
+    <t>43,471</t>
+  </si>
+  <si>
+    <t>1715</t>
+  </si>
+  <si>
+    <t>415,723</t>
+  </si>
+  <si>
+    <t>1584</t>
+  </si>
+  <si>
+    <t>44,392</t>
+  </si>
+  <si>
+    <t>1714</t>
+  </si>
+  <si>
+    <t>Dawson WOL (H)</t>
+  </si>
+  <si>
+    <t>Chambers BHA (A)</t>
+  </si>
+  <si>
+    <t>Ramsey BHA (A)</t>
+  </si>
+  <si>
+    <t>130,525</t>
+  </si>
+  <si>
+    <t>1665</t>
+  </si>
+  <si>
+    <t>Alisson -</t>
+  </si>
+  <si>
+    <t>Shaw WAT (H)</t>
+  </si>
+  <si>
+    <t>Pogba WAT (H)$ captain</t>
+  </si>
+  <si>
+    <t>Daka BUR (A)</t>
+  </si>
+  <si>
+    <t>439,756</t>
+  </si>
+  <si>
+    <t>Emerson Royal LEE (A)</t>
+  </si>
+  <si>
+    <t>Mitchell BUR (H)</t>
+  </si>
+  <si>
+    <t>Podence WHU (A)</t>
+  </si>
+  <si>
+    <t>James TOT (H)</t>
+  </si>
+  <si>
+    <t>164,032</t>
+  </si>
+  <si>
+    <t>1652</t>
+  </si>
+  <si>
+    <t>Greenwood WAT (H)</t>
+  </si>
+  <si>
+    <t>Townsend MCI (H)</t>
+  </si>
+  <si>
+    <t>Jiménez WHU (A)</t>
+  </si>
+  <si>
+    <t>Bissouma AVL (H)</t>
+  </si>
+  <si>
+    <t>6,393,963</t>
+  </si>
+  <si>
+    <t>Johnson WOL (H)</t>
+  </si>
+  <si>
+    <t>Sterling EVE (A)$ captain</t>
+  </si>
+  <si>
+    <t>Okonkwo -</t>
+  </si>
+  <si>
+    <t>Gordon MCI (H)</t>
+  </si>
+  <si>
+    <t>225,298</t>
+  </si>
+  <si>
+    <t>1631</t>
+  </si>
+  <si>
+    <t>Gunn 3</t>
+  </si>
+  <si>
+    <t>McArthur BUR (H)</t>
+  </si>
+  <si>
+    <t>62,257</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
+    <t>431,172</t>
+  </si>
+  <si>
+    <t>Telles WAT (H)</t>
+  </si>
+  <si>
+    <t>Kane LEE (A)$ captain</t>
+  </si>
+  <si>
+    <t>Elanga WAT (H)</t>
+  </si>
+  <si>
+    <t>Kulusevski LEE (A)</t>
+  </si>
+  <si>
+    <t>56,171</t>
+  </si>
+  <si>
+    <t>1705</t>
+  </si>
+  <si>
+    <t>Cresswell WOL (H)</t>
+  </si>
+  <si>
+    <t>81,212</t>
+  </si>
+  <si>
+    <t>1689</t>
+  </si>
+  <si>
+    <t>147,792</t>
+  </si>
+  <si>
+    <t>1658</t>
+  </si>
+  <si>
+    <t>Olise BUR (H)</t>
+  </si>
+  <si>
+    <t>57,446</t>
+  </si>
+  <si>
+    <t>81,574</t>
+  </si>
+  <si>
+    <t>Son 8</t>
+  </si>
+  <si>
+    <t>2,032,293</t>
+  </si>
+  <si>
+    <t>1407</t>
+  </si>
+  <si>
+    <t>2,555,972</t>
+  </si>
+  <si>
+    <t>Pope 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>Roberts 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>Weghorst 2, LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>Kane 9</t>
+  </si>
+  <si>
+    <t>488,964</t>
+  </si>
+  <si>
+    <t>1578</t>
+  </si>
+  <si>
+    <t>Lloris 6</t>
+  </si>
+  <si>
+    <t>Gallagher 2$ captain</t>
+  </si>
+  <si>
+    <t>299,937</t>
+  </si>
+  <si>
+    <t>Davies 5</t>
+  </si>
+  <si>
+    <t>Winks 3</t>
+  </si>
+  <si>
+    <t>Fernandes 2$ captain</t>
+  </si>
+  <si>
+    <t>Rodriguez 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>1,124,696</t>
+  </si>
+  <si>
+    <t>1490</t>
+  </si>
+  <si>
+    <t>3,239,009</t>
+  </si>
+  <si>
+    <t>Pinnock 0</t>
+  </si>
+  <si>
+    <t>676,310</t>
+  </si>
+  <si>
+    <t>Højbjerg 6</t>
+  </si>
+  <si>
+    <t>1,225,063</t>
+  </si>
+  <si>
+    <t>Coutinho 1</t>
+  </si>
+  <si>
+    <t>740,000</t>
+  </si>
+  <si>
+    <t>Mee 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>McNeil 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>Weghorst 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>King 1</t>
+  </si>
+  <si>
+    <t>571,487</t>
+  </si>
+  <si>
+    <t>Tarkowski 1, LEI (H)</t>
+  </si>
+  <si>
+    <t>Lucas Moura 0</t>
+  </si>
+  <si>
+    <t>444,266</t>
+  </si>
+  <si>
+    <t>Son 16$ captain</t>
+  </si>
+  <si>
+    <t>807,779</t>
+  </si>
+  <si>
+    <t>1528</t>
+  </si>
+  <si>
+    <t>de Gea 1</t>
+  </si>
+  <si>
+    <t>Mee 2, LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>1,067,683</t>
+  </si>
+  <si>
+    <t>658,420</t>
+  </si>
+  <si>
+    <t>1549</t>
+  </si>
+  <si>
+    <t>1,673,486</t>
+  </si>
+  <si>
+    <t>1,009,085</t>
+  </si>
+  <si>
+    <t>Maguire 0</t>
+  </si>
+  <si>
+    <t>813,524</t>
+  </si>
+  <si>
+    <t>57,307</t>
+  </si>
+  <si>
+    <t>1717</t>
+  </si>
+  <si>
+    <t>362,085</t>
+  </si>
+  <si>
+    <t>1605</t>
+  </si>
+  <si>
+    <t>47,989</t>
+  </si>
+  <si>
+    <t>1724</t>
+  </si>
+  <si>
+    <t>Chambers 0</t>
+  </si>
+  <si>
+    <t>118,719</t>
+  </si>
+  <si>
+    <t>1682</t>
+  </si>
+  <si>
+    <t>Pogba 2$ captain</t>
+  </si>
+  <si>
+    <t>485,211</t>
+  </si>
+  <si>
+    <t>James 2</t>
+  </si>
+  <si>
+    <t>166,755</t>
+  </si>
+  <si>
+    <t>1662</t>
+  </si>
+  <si>
+    <t>Pope 3, LEI (H)</t>
+  </si>
+  <si>
+    <t>Roberts 2, LEI (H)</t>
+  </si>
+  <si>
+    <t>Sancho 1</t>
+  </si>
+  <si>
+    <t>Weghorst 4, LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>Gallagher 4$ captain</t>
+  </si>
+  <si>
+    <t>Mings 8</t>
+  </si>
+  <si>
+    <t>Sissoko 3</t>
+  </si>
+  <si>
+    <t>Rodriguez 2, LEI (H)</t>
+  </si>
+  <si>
+    <t>Veltman 0</t>
+  </si>
+  <si>
+    <t>Zaha 2</t>
+  </si>
+  <si>
+    <t>Sarr 3</t>
+  </si>
+  <si>
+    <t>Mee 2, LEI (H)</t>
+  </si>
+  <si>
+    <t>McNeil 2, LEI (H)</t>
+  </si>
+  <si>
+    <t>Weghorst 2, LEI (H)</t>
+  </si>
+  <si>
+    <t>Raya 4</t>
+  </si>
+  <si>
+    <t>Varane 6</t>
+  </si>
+  <si>
+    <t>Mee 4, LEI (H)$ captain</t>
+  </si>
+  <si>
+    <t>Watkins 5</t>
+  </si>
+  <si>
+    <t>Digne 6</t>
+  </si>
+  <si>
+    <t>Pogba 6$ captain</t>
+  </si>
+  <si>
+    <t>Mitchell 2</t>
+  </si>
+  <si>
+    <t>6,353,885</t>
+  </si>
+  <si>
+    <t>1089</t>
+  </si>
+  <si>
+    <t>205,326</t>
+  </si>
+  <si>
+    <t>1648</t>
+  </si>
+  <si>
+    <t>McArthur 2</t>
+  </si>
+  <si>
+    <t>56,202</t>
+  </si>
+  <si>
+    <t>1718</t>
+  </si>
+  <si>
+    <t>426,198</t>
+  </si>
+  <si>
+    <t>Kane 18$ captain</t>
+  </si>
+  <si>
+    <t>Elanga 3</t>
+  </si>
+  <si>
+    <t>Kulusevski 8</t>
+  </si>
+  <si>
+    <t>40,147</t>
+  </si>
+  <si>
+    <t>1731</t>
+  </si>
+  <si>
+    <t>61,644</t>
+  </si>
+  <si>
+    <t>134,346</t>
+  </si>
+  <si>
+    <t>1675</t>
+  </si>
+  <si>
+    <t>Olise 5</t>
+  </si>
+  <si>
+    <t>64,240</t>
+  </si>
+  <si>
+    <t>1712</t>
+  </si>
+  <si>
+    <t>89,429</t>
+  </si>
+  <si>
+    <t>1697</t>
+  </si>
+  <si>
+    <t>Cancelo 9</t>
+  </si>
+  <si>
+    <t>Son 9</t>
+  </si>
+  <si>
+    <t>2,169,173</t>
+  </si>
+  <si>
+    <t>Bowen 3</t>
+  </si>
+  <si>
+    <t>2,675,136</t>
+  </si>
+  <si>
+    <t>1385</t>
+  </si>
+  <si>
+    <t>Mahrez 1</t>
+  </si>
+  <si>
+    <t>517,838</t>
+  </si>
+  <si>
+    <t>1604</t>
+  </si>
+  <si>
+    <t>Foster 10</t>
+  </si>
+  <si>
+    <t>362,154</t>
+  </si>
+  <si>
+    <t>1636</t>
+  </si>
+  <si>
+    <t>Ait Nouri 0</t>
+  </si>
+  <si>
+    <t>Mings 11</t>
+  </si>
+  <si>
+    <t>1,082,347</t>
+  </si>
+  <si>
+    <t>Dias 7</t>
+  </si>
+  <si>
+    <t>3,315,221</t>
+  </si>
+  <si>
+    <t>Semedo 0</t>
+  </si>
+  <si>
+    <t>De Bruyne 3</t>
+  </si>
+  <si>
+    <t>696,993</t>
+  </si>
+  <si>
+    <t>1575</t>
+  </si>
+  <si>
+    <t>Saïss 2</t>
+  </si>
+  <si>
+    <t>1,434,372</t>
+  </si>
+  <si>
+    <t>775,675</t>
+  </si>
+  <si>
+    <t>538,872</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>Bowen 6$ captain</t>
+  </si>
+  <si>
+    <t>441,246</t>
+  </si>
+  <si>
+    <t>1619</t>
+  </si>
+  <si>
+    <t>Son 18$ captain</t>
+  </si>
+  <si>
+    <t>836,749</t>
+  </si>
+  <si>
+    <t>Kilman 2</t>
+  </si>
+  <si>
+    <t>1,088,827</t>
+  </si>
+  <si>
+    <t>1524</t>
+  </si>
+  <si>
+    <t>646,757</t>
+  </si>
+  <si>
+    <t>1582</t>
+  </si>
+  <si>
+    <t>Soucek 11</t>
+  </si>
+  <si>
+    <t>1,651,510</t>
+  </si>
+  <si>
+    <t>1468</t>
+  </si>
+  <si>
+    <t>Foden 7</t>
+  </si>
+  <si>
+    <t>890,742</t>
+  </si>
+  <si>
+    <t>1548</t>
+  </si>
+  <si>
+    <t>805,498</t>
+  </si>
+  <si>
+    <t>46,886</t>
+  </si>
+  <si>
+    <t>1756</t>
+  </si>
+  <si>
+    <t>359,182</t>
+  </si>
+  <si>
+    <t>1637</t>
+  </si>
+  <si>
+    <t>44,385</t>
+  </si>
+  <si>
+    <t>1758</t>
+  </si>
+  <si>
+    <t>Dawson 6</t>
+  </si>
+  <si>
+    <t>132,382</t>
+  </si>
+  <si>
+    <t>1707</t>
+  </si>
+  <si>
+    <t>471,350</t>
+  </si>
+  <si>
+    <t>1613</t>
+  </si>
+  <si>
+    <t>Podence 1</t>
+  </si>
+  <si>
+    <t>167,752</t>
+  </si>
+  <si>
+    <t>Jiménez 1</t>
+  </si>
+  <si>
+    <t>6,444,213</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>Johnson 6</t>
+  </si>
+  <si>
+    <t>Sterling 6$ captain</t>
+  </si>
+  <si>
+    <t>Gordon 3</t>
+  </si>
+  <si>
+    <t>194,526</t>
+  </si>
+  <si>
+    <t>1683</t>
+  </si>
+  <si>
+    <t>McArthur 3</t>
+  </si>
+  <si>
+    <t>63,189</t>
+  </si>
+  <si>
+    <t>1744</t>
+  </si>
+  <si>
+    <t>442,594</t>
+  </si>
+  <si>
+    <t>Telles 9</t>
+  </si>
+  <si>
+    <t>34,819</t>
+  </si>
+  <si>
+    <t>1767</t>
+  </si>
+  <si>
+    <t>Cresswell 7</t>
+  </si>
+  <si>
+    <t>60,084</t>
+  </si>
+  <si>
+    <t>1746</t>
+  </si>
+  <si>
+    <t>130,211</t>
+  </si>
+  <si>
+    <t>1708</t>
+  </si>
+  <si>
+    <t>Olise 8</t>
+  </si>
+  <si>
+    <t>78,346</t>
+  </si>
+  <si>
+    <t>1734</t>
+  </si>
+  <si>
+    <t>72,343</t>
+  </si>
+  <si>
+    <t>1738</t>
   </si>
 </sst>
 </file>
@@ -14108,26 +15182,26 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.671875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.13671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0234375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="19.9140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.74609375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="17.45703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="12.53125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="13.7421875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.9140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.3828125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="19.41015625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="20.203125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="21.50390625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
@@ -14253,13 +15327,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>3535</v>
+        <v>1964</v>
       </c>
       <c r="D2" t="s">
-        <v>3537</v>
+        <v>2260</v>
       </c>
       <c r="E2" t="s">
-        <v>3536</v>
+        <v>3907</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -14271,58 +15345,58 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>3532</v>
+        <v>1927</v>
       </c>
       <c r="U2" t="s">
-        <v>1162</v>
+        <v>3628</v>
       </c>
       <c r="V2" t="s">
-        <v>3382</v>
+        <v>2837</v>
       </c>
       <c r="W2" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="X2" t="s">
-        <v>3533</v>
+        <v>3906</v>
       </c>
       <c r="Y2" t="s">
-        <v>3377</v>
+        <v>2001</v>
       </c>
       <c r="Z2" t="s">
-        <v>3534</v>
+        <v>1929</v>
       </c>
       <c r="AA2" t="s">
-        <v>712</v>
+        <v>3633</v>
       </c>
       <c r="AB2" t="s">
-        <v>3376</v>
+        <v>2843</v>
       </c>
       <c r="AC2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="AD2" t="s">
         <v>3381</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>3380</v>
       </c>
       <c r="AE2" t="s">
         <v>2266</v>
       </c>
       <c r="AF2" t="s">
-        <v>1900</v>
+        <v>3637</v>
       </c>
       <c r="AG2" t="s">
         <v>914</v>
       </c>
       <c r="AH2" t="s">
-        <v>3379</v>
+        <v>1930</v>
       </c>
       <c r="AI2" t="s">
-        <v>3535</v>
+        <v>1964</v>
       </c>
       <c r="AJ2" t="s">
-        <v>3537</v>
+        <v>2260</v>
       </c>
       <c r="AK2" t="s">
-        <v>3536</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -14333,16 +15407,16 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>3542</v>
+        <v>1297</v>
       </c>
       <c r="D3" t="s">
-        <v>2144</v>
+        <v>3910</v>
       </c>
       <c r="E3" t="s">
-        <v>3543</v>
+        <v>3909</v>
       </c>
       <c r="G3" t="s">
-        <v>552</v>
+        <v>627</v>
       </c>
       <c r="R3" t="s">
         <v>688</v>
@@ -14351,43 +15425,43 @@
         <v>687</v>
       </c>
       <c r="T3" t="s">
-        <v>3385</v>
+        <v>1917</v>
       </c>
       <c r="U3" t="s">
-        <v>1162</v>
+        <v>3905</v>
       </c>
       <c r="V3" t="s">
-        <v>3015</v>
+        <v>3628</v>
       </c>
       <c r="W3" t="s">
-        <v>3538</v>
+        <v>765</v>
       </c>
       <c r="X3" t="s">
-        <v>3534</v>
+        <v>3633</v>
       </c>
       <c r="Y3" t="s">
-        <v>3539</v>
+        <v>1932</v>
       </c>
       <c r="Z3" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="AA3" t="s">
-        <v>3540</v>
+        <v>665</v>
       </c>
       <c r="AB3" t="s">
-        <v>3541</v>
+        <v>3644</v>
       </c>
       <c r="AC3" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AD3" t="s">
-        <v>3390</v>
+        <v>3645</v>
       </c>
       <c r="AE3" t="s">
         <v>2266</v>
       </c>
       <c r="AF3" t="s">
-        <v>3382</v>
+        <v>3637</v>
       </c>
       <c r="AG3" t="s">
         <v>684</v>
@@ -14396,13 +15470,13 @@
         <v>914</v>
       </c>
       <c r="AI3" t="s">
-        <v>3542</v>
+        <v>1297</v>
       </c>
       <c r="AJ3" t="s">
-        <v>2144</v>
+        <v>3910</v>
       </c>
       <c r="AK3" t="s">
-        <v>3543</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -14413,16 +15487,16 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>3547</v>
+        <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>3549</v>
+        <v>3913</v>
       </c>
       <c r="E4" t="s">
-        <v>3548</v>
+        <v>3912</v>
       </c>
       <c r="G4" t="s">
-        <v>880</v>
+        <v>627</v>
       </c>
       <c r="R4" t="s">
         <v>697</v>
@@ -14431,58 +15505,58 @@
         <v>696</v>
       </c>
       <c r="T4" t="s">
-        <v>2266</v>
+        <v>3863</v>
       </c>
       <c r="U4" t="s">
-        <v>3538</v>
+        <v>3648</v>
       </c>
       <c r="V4" t="s">
-        <v>3533</v>
+        <v>3905</v>
       </c>
       <c r="W4" t="s">
-        <v>3544</v>
+        <v>3864</v>
       </c>
       <c r="X4" t="s">
-        <v>3545</v>
+        <v>1935</v>
       </c>
       <c r="Y4" t="s">
-        <v>3376</v>
+        <v>3911</v>
       </c>
       <c r="Z4" t="s">
-        <v>3534</v>
+        <v>3906</v>
       </c>
       <c r="AA4" t="s">
-        <v>3394</v>
+        <v>3865</v>
       </c>
       <c r="AB4" t="s">
-        <v>3396</v>
+        <v>3866</v>
       </c>
       <c r="AC4" t="s">
-        <v>3380</v>
+        <v>1967</v>
       </c>
       <c r="AD4" t="s">
-        <v>1967</v>
+        <v>2079</v>
       </c>
       <c r="AE4" t="s">
-        <v>2569</v>
+        <v>3469</v>
       </c>
       <c r="AF4" t="s">
-        <v>3393</v>
+        <v>3656</v>
       </c>
       <c r="AG4" t="s">
-        <v>3015</v>
+        <v>780</v>
       </c>
       <c r="AH4" t="s">
-        <v>3546</v>
+        <v>3657</v>
       </c>
       <c r="AI4" t="s">
-        <v>3547</v>
+        <v>2004</v>
       </c>
       <c r="AJ4" t="s">
-        <v>3549</v>
+        <v>3913</v>
       </c>
       <c r="AK4" t="s">
-        <v>3548</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -14493,13 +15567,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>3552</v>
+        <v>1886</v>
       </c>
       <c r="D5" t="s">
-        <v>3554</v>
+        <v>3916</v>
       </c>
       <c r="E5" t="s">
-        <v>3553</v>
+        <v>3915</v>
       </c>
       <c r="G5" t="s">
         <v>426</v>
@@ -14511,58 +15585,58 @@
         <v>705</v>
       </c>
       <c r="T5" t="s">
-        <v>1180</v>
+        <v>3813</v>
       </c>
       <c r="U5" t="s">
-        <v>3550</v>
+        <v>1933</v>
       </c>
       <c r="V5" t="s">
-        <v>3015</v>
+        <v>3628</v>
       </c>
       <c r="W5" t="s">
-        <v>3533</v>
+        <v>1930</v>
       </c>
       <c r="X5" t="s">
-        <v>3544</v>
+        <v>3905</v>
       </c>
       <c r="Y5" t="s">
-        <v>1162</v>
+        <v>3662</v>
       </c>
       <c r="Z5" t="s">
-        <v>3551</v>
+        <v>3908</v>
       </c>
       <c r="AA5" t="s">
-        <v>3162</v>
+        <v>3867</v>
       </c>
       <c r="AB5" t="s">
-        <v>3545</v>
+        <v>1967</v>
       </c>
       <c r="AC5" t="s">
-        <v>3380</v>
+        <v>3645</v>
       </c>
       <c r="AD5" t="s">
-        <v>3025</v>
+        <v>3444</v>
       </c>
       <c r="AE5" t="s">
-        <v>2569</v>
+        <v>3914</v>
       </c>
       <c r="AF5" t="s">
-        <v>3540</v>
+        <v>1937</v>
       </c>
       <c r="AG5" t="s">
-        <v>1967</v>
+        <v>3666</v>
       </c>
       <c r="AH5" t="s">
-        <v>767</v>
+        <v>3667</v>
       </c>
       <c r="AI5" t="s">
-        <v>3552</v>
+        <v>1886</v>
       </c>
       <c r="AJ5" t="s">
-        <v>3554</v>
+        <v>3916</v>
       </c>
       <c r="AK5" t="s">
-        <v>3553</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -14573,16 +15647,16 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>3471</v>
+        <v>677</v>
       </c>
       <c r="D6" t="s">
-        <v>3557</v>
+        <v>3749</v>
       </c>
       <c r="E6" t="s">
-        <v>3556</v>
+        <v>3919</v>
       </c>
       <c r="G6" t="s">
-        <v>3415</v>
+        <v>426</v>
       </c>
       <c r="R6" t="s">
         <v>469</v>
@@ -14591,58 +15665,58 @@
         <v>717</v>
       </c>
       <c r="T6" t="s">
-        <v>3385</v>
+        <v>3526</v>
       </c>
       <c r="U6" t="s">
-        <v>3015</v>
+        <v>3917</v>
       </c>
       <c r="V6" t="s">
-        <v>3555</v>
+        <v>3905</v>
       </c>
       <c r="W6" t="s">
-        <v>1162</v>
+        <v>3816</v>
       </c>
       <c r="X6" t="s">
-        <v>3409</v>
+        <v>3918</v>
       </c>
       <c r="Y6" t="s">
-        <v>3545</v>
+        <v>3869</v>
       </c>
       <c r="Z6" t="s">
-        <v>3534</v>
+        <v>3817</v>
       </c>
       <c r="AA6" t="s">
-        <v>3308</v>
+        <v>2193</v>
       </c>
       <c r="AB6" t="s">
-        <v>2584</v>
+        <v>1343</v>
       </c>
       <c r="AC6" t="s">
-        <v>3410</v>
+        <v>2079</v>
       </c>
       <c r="AD6" t="s">
-        <v>3411</v>
+        <v>3870</v>
       </c>
       <c r="AE6" t="s">
         <v>1128</v>
       </c>
       <c r="AF6" t="s">
-        <v>3412</v>
+        <v>1937</v>
       </c>
       <c r="AG6" t="s">
-        <v>3413</v>
+        <v>3628</v>
       </c>
       <c r="AH6" t="s">
-        <v>3176</v>
+        <v>3667</v>
       </c>
       <c r="AI6" t="s">
-        <v>3471</v>
+        <v>677</v>
       </c>
       <c r="AJ6" t="s">
-        <v>3557</v>
+        <v>3749</v>
       </c>
       <c r="AK6" t="s">
-        <v>3556</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -14653,13 +15727,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>1212</v>
+        <v>3086</v>
       </c>
       <c r="D7" t="s">
-        <v>2245</v>
+        <v>2586</v>
       </c>
       <c r="E7" t="s">
-        <v>3558</v>
+        <v>3921</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -14671,58 +15745,58 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>3532</v>
+        <v>1927</v>
       </c>
       <c r="U7" t="s">
-        <v>3418</v>
+        <v>3920</v>
       </c>
       <c r="V7" t="s">
-        <v>3416</v>
+        <v>528</v>
       </c>
       <c r="W7" t="s">
         <v>1164</v>
       </c>
       <c r="X7" t="s">
-        <v>1952</v>
+        <v>3683</v>
       </c>
       <c r="Y7" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="Z7" t="s">
-        <v>3540</v>
+        <v>665</v>
       </c>
       <c r="AA7" t="s">
-        <v>3534</v>
+        <v>3633</v>
       </c>
       <c r="AB7" t="s">
-        <v>657</v>
+        <v>2020</v>
       </c>
       <c r="AC7" t="s">
-        <v>3380</v>
+        <v>2007</v>
       </c>
       <c r="AD7" t="s">
-        <v>656</v>
+        <v>913</v>
       </c>
       <c r="AE7" t="s">
         <v>778</v>
       </c>
       <c r="AF7" t="s">
-        <v>528</v>
+        <v>3687</v>
       </c>
       <c r="AG7" t="s">
-        <v>3417</v>
+        <v>1154</v>
       </c>
       <c r="AH7" t="s">
-        <v>3382</v>
+        <v>3637</v>
       </c>
       <c r="AI7" t="s">
-        <v>1212</v>
+        <v>3086</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2245</v>
+        <v>2586</v>
       </c>
       <c r="AK7" t="s">
-        <v>3558</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -14733,16 +15807,16 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>3400</v>
+        <v>686</v>
       </c>
       <c r="D8" t="s">
-        <v>3563</v>
+        <v>3925</v>
       </c>
       <c r="E8" t="s">
-        <v>3562</v>
+        <v>3924</v>
       </c>
       <c r="G8" t="s">
-        <v>3426</v>
+        <v>880</v>
       </c>
       <c r="R8" t="s">
         <v>547</v>
@@ -14751,58 +15825,58 @@
         <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>2569</v>
+        <v>3914</v>
       </c>
       <c r="U8" t="s">
-        <v>3420</v>
+        <v>3871</v>
       </c>
       <c r="V8" t="s">
-        <v>3015</v>
+        <v>2173</v>
       </c>
       <c r="W8" t="s">
-        <v>3550</v>
+        <v>3922</v>
       </c>
       <c r="X8" t="s">
-        <v>3559</v>
+        <v>3872</v>
       </c>
       <c r="Y8" t="s">
-        <v>3422</v>
+        <v>3873</v>
       </c>
       <c r="Z8" t="s">
-        <v>3534</v>
+        <v>3923</v>
       </c>
       <c r="AA8" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="AB8" t="s">
-        <v>2584</v>
+        <v>3866</v>
       </c>
       <c r="AC8" t="s">
-        <v>3546</v>
+        <v>1967</v>
       </c>
       <c r="AD8" t="s">
-        <v>3410</v>
+        <v>2079</v>
       </c>
       <c r="AE8" t="s">
         <v>1806</v>
       </c>
       <c r="AF8" t="s">
-        <v>3560</v>
+        <v>1933</v>
       </c>
       <c r="AG8" t="s">
-        <v>2173</v>
+        <v>3628</v>
       </c>
       <c r="AH8" t="s">
-        <v>3561</v>
+        <v>3196</v>
       </c>
       <c r="AI8" t="s">
-        <v>3400</v>
+        <v>686</v>
       </c>
       <c r="AJ8" t="s">
-        <v>3563</v>
+        <v>3925</v>
       </c>
       <c r="AK8" t="s">
-        <v>3562</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -14813,16 +15887,16 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>3453</v>
+        <v>1963</v>
       </c>
       <c r="D9" t="s">
-        <v>3324</v>
+        <v>2049</v>
       </c>
       <c r="E9" t="s">
-        <v>3565</v>
+        <v>3927</v>
       </c>
       <c r="G9" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="R9" t="s">
         <v>540</v>
@@ -14831,58 +15905,58 @@
         <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>1180</v>
+        <v>3813</v>
       </c>
       <c r="U9" t="s">
-        <v>3015</v>
+        <v>3628</v>
       </c>
       <c r="V9" t="s">
-        <v>3418</v>
+        <v>3687</v>
       </c>
       <c r="W9" t="s">
-        <v>3564</v>
+        <v>3926</v>
       </c>
       <c r="X9" t="s">
-        <v>3534</v>
+        <v>3633</v>
       </c>
       <c r="Y9" t="s">
-        <v>3561</v>
+        <v>3196</v>
       </c>
       <c r="Z9" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="AA9" t="s">
-        <v>3428</v>
+        <v>3825</v>
       </c>
       <c r="AB9" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AC9" t="s">
-        <v>657</v>
+        <v>913</v>
       </c>
       <c r="AD9" t="s">
-        <v>3390</v>
+        <v>3645</v>
       </c>
       <c r="AE9" t="s">
         <v>2266</v>
       </c>
       <c r="AF9" t="s">
-        <v>3416</v>
+        <v>3920</v>
       </c>
       <c r="AG9" t="s">
-        <v>3377</v>
+        <v>1929</v>
       </c>
       <c r="AH9" t="s">
         <v>1354</v>
       </c>
       <c r="AI9" t="s">
-        <v>3453</v>
+        <v>1963</v>
       </c>
       <c r="AJ9" t="s">
-        <v>3324</v>
+        <v>2049</v>
       </c>
       <c r="AK9" t="s">
-        <v>3565</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -14893,16 +15967,16 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>3568</v>
+        <v>1884</v>
       </c>
       <c r="D10" t="s">
-        <v>3279</v>
+        <v>3714</v>
       </c>
       <c r="E10" t="s">
-        <v>3569</v>
+        <v>3928</v>
       </c>
       <c r="G10" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R10" t="s">
         <v>742</v>
@@ -14911,58 +15985,58 @@
         <v>259</v>
       </c>
       <c r="T10" t="s">
-        <v>3532</v>
+        <v>3813</v>
       </c>
       <c r="U10" t="s">
-        <v>3538</v>
+        <v>1181</v>
       </c>
       <c r="V10" t="s">
-        <v>3566</v>
+        <v>3905</v>
       </c>
       <c r="W10" t="s">
-        <v>3015</v>
+        <v>3864</v>
       </c>
       <c r="X10" t="s">
-        <v>2266</v>
+        <v>3908</v>
       </c>
       <c r="Y10" t="s">
-        <v>3376</v>
+        <v>2174</v>
       </c>
       <c r="Z10" t="s">
-        <v>3545</v>
+        <v>665</v>
       </c>
       <c r="AA10" t="s">
-        <v>3534</v>
+        <v>3667</v>
       </c>
       <c r="AB10" t="s">
-        <v>1370</v>
+        <v>1967</v>
       </c>
       <c r="AC10" t="s">
-        <v>3380</v>
+        <v>3866</v>
       </c>
       <c r="AD10" t="s">
-        <v>3256</v>
+        <v>2020</v>
       </c>
       <c r="AE10" t="s">
-        <v>740</v>
+        <v>3705</v>
       </c>
       <c r="AF10" t="s">
-        <v>3431</v>
+        <v>3628</v>
       </c>
       <c r="AG10" t="s">
-        <v>3567</v>
+        <v>1941</v>
       </c>
       <c r="AH10" t="s">
-        <v>3162</v>
+        <v>3205</v>
       </c>
       <c r="AI10" t="s">
-        <v>3568</v>
+        <v>1884</v>
       </c>
       <c r="AJ10" t="s">
-        <v>3279</v>
+        <v>3714</v>
       </c>
       <c r="AK10" t="s">
-        <v>3569</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -14973,16 +16047,16 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>3571</v>
+        <v>647</v>
       </c>
       <c r="D11" t="s">
-        <v>3573</v>
+        <v>3930</v>
       </c>
       <c r="E11" t="s">
-        <v>3572</v>
+        <v>3929</v>
       </c>
       <c r="G11" t="s">
-        <v>627</v>
+        <v>880</v>
       </c>
       <c r="R11" t="s">
         <v>747</v>
@@ -14991,58 +16065,58 @@
         <v>746</v>
       </c>
       <c r="T11" t="s">
-        <v>2569</v>
+        <v>2266</v>
       </c>
       <c r="U11" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="V11" t="s">
-        <v>3566</v>
+        <v>3874</v>
       </c>
       <c r="W11" t="s">
-        <v>3550</v>
+        <v>3920</v>
       </c>
       <c r="X11" t="s">
-        <v>3570</v>
+        <v>2173</v>
       </c>
       <c r="Y11" t="s">
-        <v>3396</v>
+        <v>3875</v>
       </c>
       <c r="Z11" t="s">
-        <v>3545</v>
+        <v>3869</v>
       </c>
       <c r="AA11" t="s">
-        <v>3534</v>
+        <v>2193</v>
       </c>
       <c r="AB11" t="s">
-        <v>3376</v>
+        <v>3876</v>
       </c>
       <c r="AC11" t="s">
-        <v>3025</v>
+        <v>1899</v>
       </c>
       <c r="AD11" t="s">
-        <v>3256</v>
+        <v>2020</v>
       </c>
       <c r="AE11" t="s">
-        <v>2266</v>
+        <v>3877</v>
       </c>
       <c r="AF11" t="s">
-        <v>1162</v>
+        <v>3667</v>
       </c>
       <c r="AG11" t="s">
-        <v>3162</v>
+        <v>1932</v>
       </c>
       <c r="AH11" t="s">
-        <v>1967</v>
+        <v>3628</v>
       </c>
       <c r="AI11" t="s">
-        <v>3571</v>
+        <v>647</v>
       </c>
       <c r="AJ11" t="s">
-        <v>3573</v>
+        <v>3930</v>
       </c>
       <c r="AK11" t="s">
-        <v>3572</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -15053,16 +16127,16 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>3575</v>
+        <v>848</v>
       </c>
       <c r="D12" t="s">
-        <v>3577</v>
+        <v>3933</v>
       </c>
       <c r="E12" t="s">
-        <v>3576</v>
+        <v>3932</v>
       </c>
       <c r="G12" t="s">
-        <v>880</v>
+        <v>426</v>
       </c>
       <c r="R12" t="s">
         <v>392</v>
@@ -15071,58 +16145,58 @@
         <v>263</v>
       </c>
       <c r="T12" t="s">
-        <v>3532</v>
+        <v>397</v>
       </c>
       <c r="U12" t="s">
-        <v>3416</v>
+        <v>3920</v>
       </c>
       <c r="V12" t="s">
-        <v>3544</v>
+        <v>3666</v>
       </c>
       <c r="W12" t="s">
-        <v>3574</v>
+        <v>3716</v>
       </c>
       <c r="X12" t="s">
-        <v>3438</v>
+        <v>3834</v>
       </c>
       <c r="Y12" t="s">
-        <v>3551</v>
+        <v>3878</v>
       </c>
       <c r="Z12" t="s">
-        <v>3377</v>
+        <v>1929</v>
       </c>
       <c r="AA12" t="s">
-        <v>2018</v>
+        <v>3835</v>
       </c>
       <c r="AB12" t="s">
-        <v>3539</v>
+        <v>3931</v>
       </c>
       <c r="AC12" t="s">
         <v>3381</v>
       </c>
       <c r="AD12" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AE12" t="s">
-        <v>751</v>
+        <v>1927</v>
       </c>
       <c r="AF12" t="s">
-        <v>3162</v>
+        <v>1932</v>
       </c>
       <c r="AG12" t="s">
-        <v>3439</v>
+        <v>3667</v>
       </c>
       <c r="AH12" t="s">
-        <v>802</v>
+        <v>3876</v>
       </c>
       <c r="AI12" t="s">
-        <v>3575</v>
+        <v>848</v>
       </c>
       <c r="AJ12" t="s">
-        <v>3577</v>
+        <v>3933</v>
       </c>
       <c r="AK12" t="s">
-        <v>3576</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -15133,16 +16207,16 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>3578</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
-        <v>2071</v>
+        <v>3345</v>
       </c>
       <c r="E13" t="s">
-        <v>3579</v>
+        <v>3935</v>
       </c>
       <c r="G13" t="s">
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="R13" t="s">
         <v>486</v>
@@ -15151,58 +16225,58 @@
         <v>265</v>
       </c>
       <c r="T13" t="s">
-        <v>3532</v>
+        <v>3914</v>
       </c>
       <c r="U13" t="s">
-        <v>3544</v>
+        <v>3666</v>
       </c>
       <c r="V13" t="s">
-        <v>3574</v>
+        <v>1953</v>
       </c>
       <c r="W13" t="s">
-        <v>3550</v>
+        <v>3637</v>
       </c>
       <c r="X13" t="s">
-        <v>3551</v>
+        <v>1933</v>
       </c>
       <c r="Y13" t="s">
-        <v>3162</v>
+        <v>3934</v>
       </c>
       <c r="Z13" t="s">
-        <v>3545</v>
+        <v>2174</v>
       </c>
       <c r="AA13" t="s">
-        <v>3376</v>
+        <v>3908</v>
       </c>
       <c r="AB13" t="s">
-        <v>3204</v>
+        <v>3444</v>
       </c>
       <c r="AC13" t="s">
         <v>1967</v>
       </c>
       <c r="AD13" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AE13" t="s">
-        <v>2569</v>
+        <v>1927</v>
       </c>
       <c r="AF13" t="s">
-        <v>3442</v>
+        <v>1937</v>
       </c>
       <c r="AG13" t="s">
-        <v>3443</v>
+        <v>3716</v>
       </c>
       <c r="AH13" t="s">
-        <v>3444</v>
+        <v>3667</v>
       </c>
       <c r="AI13" t="s">
-        <v>3578</v>
+        <v>252</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2071</v>
+        <v>3345</v>
       </c>
       <c r="AK13" t="s">
-        <v>3579</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -15213,16 +16287,16 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>3471</v>
+        <v>256</v>
       </c>
       <c r="D14" t="s">
-        <v>2049</v>
+        <v>3938</v>
       </c>
       <c r="E14" t="s">
-        <v>3580</v>
+        <v>3937</v>
       </c>
       <c r="G14" t="s">
-        <v>646</v>
+        <v>880</v>
       </c>
       <c r="R14" t="s">
         <v>433</v>
@@ -15231,58 +16305,58 @@
         <v>770</v>
       </c>
       <c r="T14" t="s">
-        <v>2569</v>
+        <v>555</v>
       </c>
       <c r="U14" t="s">
-        <v>3533</v>
+        <v>1953</v>
       </c>
       <c r="V14" t="s">
-        <v>3574</v>
+        <v>3879</v>
       </c>
       <c r="W14" t="s">
-        <v>3446</v>
+        <v>3936</v>
       </c>
       <c r="X14" t="s">
-        <v>3550</v>
+        <v>3220</v>
       </c>
       <c r="Y14" t="s">
-        <v>3394</v>
+        <v>2186</v>
       </c>
       <c r="Z14" t="s">
-        <v>722</v>
+        <v>3730</v>
       </c>
       <c r="AA14" t="s">
-        <v>3541</v>
+        <v>1935</v>
       </c>
       <c r="AB14" t="s">
-        <v>3447</v>
+        <v>2079</v>
       </c>
       <c r="AC14" t="s">
         <v>3381</v>
       </c>
       <c r="AD14" t="s">
-        <v>2584</v>
+        <v>3876</v>
       </c>
       <c r="AE14" t="s">
-        <v>2963</v>
+        <v>3914</v>
       </c>
       <c r="AF14" t="s">
-        <v>3448</v>
+        <v>3644</v>
       </c>
       <c r="AG14" t="s">
-        <v>3443</v>
+        <v>3731</v>
       </c>
       <c r="AH14" t="s">
-        <v>3220</v>
+        <v>1933</v>
       </c>
       <c r="AI14" t="s">
-        <v>3471</v>
+        <v>256</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2049</v>
+        <v>3938</v>
       </c>
       <c r="AK14" t="s">
-        <v>3580</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -15293,16 +16367,16 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>3582</v>
+        <v>759</v>
       </c>
       <c r="D15" t="s">
-        <v>3563</v>
+        <v>3940</v>
       </c>
       <c r="E15" t="s">
-        <v>3583</v>
+        <v>3939</v>
       </c>
       <c r="G15" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R15" t="s">
         <v>775</v>
@@ -15311,58 +16385,58 @@
         <v>774</v>
       </c>
       <c r="T15" t="s">
-        <v>3532</v>
+        <v>555</v>
       </c>
       <c r="U15" t="s">
-        <v>3544</v>
+        <v>3062</v>
       </c>
       <c r="V15" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="W15" t="s">
-        <v>3550</v>
+        <v>2228</v>
       </c>
       <c r="X15" t="s">
-        <v>3555</v>
+        <v>3908</v>
       </c>
       <c r="Y15" t="s">
-        <v>1162</v>
+        <v>2186</v>
       </c>
       <c r="Z15" t="s">
-        <v>3376</v>
+        <v>3835</v>
       </c>
       <c r="AA15" t="s">
-        <v>3394</v>
+        <v>2193</v>
       </c>
       <c r="AB15" t="s">
-        <v>3534</v>
+        <v>3730</v>
       </c>
       <c r="AC15" t="s">
-        <v>3162</v>
+        <v>2007</v>
       </c>
       <c r="AD15" t="s">
-        <v>3546</v>
+        <v>2020</v>
       </c>
       <c r="AE15" t="s">
-        <v>3450</v>
+        <v>1927</v>
       </c>
       <c r="AF15" t="s">
-        <v>3451</v>
+        <v>1899</v>
       </c>
       <c r="AG15" t="s">
-        <v>3581</v>
+        <v>3628</v>
       </c>
       <c r="AH15" t="s">
-        <v>3411</v>
+        <v>3666</v>
       </c>
       <c r="AI15" t="s">
-        <v>3582</v>
+        <v>759</v>
       </c>
       <c r="AJ15" t="s">
-        <v>3563</v>
+        <v>3940</v>
       </c>
       <c r="AK15" t="s">
-        <v>3583</v>
+        <v>3939</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -15373,13 +16447,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>3586</v>
+        <v>881</v>
       </c>
       <c r="D16" t="s">
-        <v>3209</v>
+        <v>3943</v>
       </c>
       <c r="E16" t="s">
-        <v>3587</v>
+        <v>3942</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -15391,58 +16465,58 @@
         <v>270</v>
       </c>
       <c r="T16" t="s">
-        <v>3584</v>
+        <v>1173</v>
       </c>
       <c r="U16" t="s">
-        <v>3382</v>
+        <v>3205</v>
       </c>
       <c r="V16" t="s">
-        <v>3566</v>
+        <v>3628</v>
       </c>
       <c r="W16" t="s">
-        <v>3015</v>
+        <v>1936</v>
       </c>
       <c r="X16" t="s">
-        <v>1281</v>
+        <v>1929</v>
       </c>
       <c r="Y16" t="s">
-        <v>3540</v>
+        <v>3737</v>
       </c>
       <c r="Z16" t="s">
-        <v>3377</v>
+        <v>2187</v>
       </c>
       <c r="AA16" t="s">
-        <v>3585</v>
+        <v>3941</v>
       </c>
       <c r="AB16" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AC16" t="s">
-        <v>3458</v>
+        <v>2007</v>
       </c>
       <c r="AD16" t="s">
-        <v>656</v>
+        <v>3880</v>
       </c>
       <c r="AE16" t="s">
         <v>2266</v>
       </c>
       <c r="AF16" t="s">
-        <v>2229</v>
+        <v>3637</v>
       </c>
       <c r="AG16" t="s">
-        <v>3457</v>
+        <v>665</v>
       </c>
       <c r="AH16" t="s">
-        <v>3416</v>
+        <v>3920</v>
       </c>
       <c r="AI16" t="s">
-        <v>3586</v>
+        <v>881</v>
       </c>
       <c r="AJ16" t="s">
-        <v>3209</v>
+        <v>3943</v>
       </c>
       <c r="AK16" t="s">
-        <v>3587</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -15453,13 +16527,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>3529</v>
+        <v>246</v>
       </c>
       <c r="D17" t="s">
-        <v>2116</v>
+        <v>3946</v>
       </c>
       <c r="E17" t="s">
-        <v>3588</v>
+        <v>3945</v>
       </c>
       <c r="G17" t="s">
         <v>426</v>
@@ -15471,58 +16545,58 @@
         <v>272</v>
       </c>
       <c r="T17" t="s">
-        <v>3532</v>
+        <v>2266</v>
       </c>
       <c r="U17" t="s">
-        <v>766</v>
+        <v>3834</v>
       </c>
       <c r="V17" t="s">
-        <v>3015</v>
+        <v>3920</v>
       </c>
       <c r="W17" t="s">
-        <v>1162</v>
+        <v>3881</v>
       </c>
       <c r="X17" t="s">
-        <v>3460</v>
+        <v>3905</v>
       </c>
       <c r="Y17" t="s">
-        <v>3539</v>
+        <v>2174</v>
       </c>
       <c r="Z17" t="s">
-        <v>3551</v>
+        <v>3908</v>
       </c>
       <c r="AA17" t="s">
-        <v>3162</v>
+        <v>3944</v>
       </c>
       <c r="AB17" t="s">
         <v>3381</v>
       </c>
       <c r="AC17" t="s">
-        <v>3380</v>
+        <v>1899</v>
       </c>
       <c r="AD17" t="s">
-        <v>2584</v>
+        <v>2035</v>
       </c>
       <c r="AE17" t="s">
-        <v>2266</v>
+        <v>1927</v>
       </c>
       <c r="AF17" t="s">
-        <v>528</v>
+        <v>1932</v>
       </c>
       <c r="AG17" t="s">
-        <v>2199</v>
+        <v>3667</v>
       </c>
       <c r="AH17" t="s">
-        <v>3417</v>
+        <v>3628</v>
       </c>
       <c r="AI17" t="s">
-        <v>3529</v>
+        <v>246</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2116</v>
+        <v>3946</v>
       </c>
       <c r="AK17" t="s">
-        <v>3588</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -15533,16 +16607,16 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>3500</v>
+        <v>745</v>
       </c>
       <c r="D18" t="s">
-        <v>3437</v>
+        <v>3366</v>
       </c>
       <c r="E18" t="s">
-        <v>3589</v>
+        <v>3947</v>
       </c>
       <c r="G18" t="s">
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="R18" t="s">
         <v>501</v>
@@ -15551,58 +16625,58 @@
         <v>787</v>
       </c>
       <c r="T18" t="s">
-        <v>3532</v>
+        <v>3914</v>
       </c>
       <c r="U18" t="s">
-        <v>3533</v>
+        <v>3746</v>
       </c>
       <c r="V18" t="s">
-        <v>1162</v>
+        <v>3905</v>
       </c>
       <c r="W18" t="s">
-        <v>3015</v>
+        <v>3847</v>
       </c>
       <c r="X18" t="s">
-        <v>3550</v>
+        <v>1933</v>
       </c>
       <c r="Y18" t="s">
-        <v>3551</v>
+        <v>3867</v>
       </c>
       <c r="Z18" t="s">
-        <v>3308</v>
+        <v>2187</v>
       </c>
       <c r="AA18" t="s">
-        <v>3394</v>
+        <v>2186</v>
       </c>
       <c r="AB18" t="s">
-        <v>767</v>
+        <v>3662</v>
       </c>
       <c r="AC18" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AD18" t="s">
-        <v>656</v>
+        <v>2007</v>
       </c>
       <c r="AE18" t="s">
-        <v>2569</v>
+        <v>1927</v>
       </c>
       <c r="AF18" t="s">
-        <v>3540</v>
+        <v>3667</v>
       </c>
       <c r="AG18" t="s">
-        <v>3464</v>
+        <v>3628</v>
       </c>
       <c r="AH18" t="s">
         <v>786</v>
       </c>
       <c r="AI18" t="s">
-        <v>3500</v>
+        <v>745</v>
       </c>
       <c r="AJ18" t="s">
-        <v>3437</v>
+        <v>3366</v>
       </c>
       <c r="AK18" t="s">
-        <v>3589</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -15613,16 +16687,16 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>3590</v>
+        <v>645</v>
       </c>
       <c r="D19" t="s">
-        <v>3592</v>
+        <v>3949</v>
       </c>
       <c r="E19" t="s">
-        <v>3591</v>
+        <v>3948</v>
       </c>
       <c r="G19" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R19" t="s">
         <v>347</v>
@@ -15631,58 +16705,58 @@
         <v>792</v>
       </c>
       <c r="T19" t="s">
-        <v>3532</v>
+        <v>555</v>
       </c>
       <c r="U19" t="s">
-        <v>3564</v>
+        <v>3905</v>
       </c>
       <c r="V19" t="s">
-        <v>3015</v>
+        <v>1953</v>
       </c>
       <c r="W19" t="s">
-        <v>3550</v>
+        <v>3637</v>
       </c>
       <c r="X19" t="s">
-        <v>3534</v>
+        <v>2174</v>
       </c>
       <c r="Y19" t="s">
-        <v>3541</v>
+        <v>2186</v>
       </c>
       <c r="Z19" t="s">
-        <v>3376</v>
+        <v>2187</v>
       </c>
       <c r="AA19" t="s">
-        <v>3545</v>
+        <v>3908</v>
       </c>
       <c r="AB19" t="s">
-        <v>3559</v>
+        <v>3381</v>
       </c>
       <c r="AC19" t="s">
-        <v>3256</v>
+        <v>2020</v>
       </c>
       <c r="AD19" t="s">
-        <v>3380</v>
+        <v>3866</v>
       </c>
       <c r="AE19" t="s">
-        <v>3469</v>
+        <v>1927</v>
       </c>
       <c r="AF19" t="s">
-        <v>3470</v>
+        <v>3442</v>
       </c>
       <c r="AG19" t="s">
-        <v>802</v>
+        <v>3667</v>
       </c>
       <c r="AH19" t="s">
-        <v>915</v>
+        <v>1936</v>
       </c>
       <c r="AI19" t="s">
-        <v>3590</v>
+        <v>645</v>
       </c>
       <c r="AJ19" t="s">
-        <v>3592</v>
+        <v>3949</v>
       </c>
       <c r="AK19" t="s">
-        <v>3591</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -15693,13 +16767,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>3507</v>
+        <v>252</v>
       </c>
       <c r="D20" t="s">
-        <v>3594</v>
+        <v>3951</v>
       </c>
       <c r="E20" t="s">
-        <v>3593</v>
+        <v>3950</v>
       </c>
       <c r="G20" t="s">
         <v>426</v>
@@ -15711,58 +16785,58 @@
         <v>796</v>
       </c>
       <c r="T20" t="s">
-        <v>2963</v>
+        <v>555</v>
       </c>
       <c r="U20" t="s">
-        <v>3550</v>
+        <v>3656</v>
       </c>
       <c r="V20" t="s">
-        <v>3015</v>
+        <v>3816</v>
       </c>
       <c r="W20" t="s">
-        <v>3409</v>
+        <v>3905</v>
       </c>
       <c r="X20" t="s">
-        <v>3534</v>
+        <v>3934</v>
       </c>
       <c r="Y20" t="s">
-        <v>3308</v>
+        <v>2187</v>
       </c>
       <c r="Z20" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="AA20" t="s">
-        <v>3204</v>
+        <v>2174</v>
       </c>
       <c r="AB20" t="s">
-        <v>3545</v>
+        <v>3381</v>
       </c>
       <c r="AC20" t="s">
-        <v>2584</v>
+        <v>3876</v>
       </c>
       <c r="AD20" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AE20" t="s">
         <v>1806</v>
       </c>
       <c r="AF20" t="s">
-        <v>3381</v>
+        <v>1933</v>
       </c>
       <c r="AG20" t="s">
-        <v>1162</v>
+        <v>1937</v>
       </c>
       <c r="AH20" t="s">
-        <v>915</v>
+        <v>3628</v>
       </c>
       <c r="AI20" t="s">
-        <v>3507</v>
+        <v>252</v>
       </c>
       <c r="AJ20" t="s">
-        <v>3594</v>
+        <v>3951</v>
       </c>
       <c r="AK20" t="s">
-        <v>3593</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -15773,16 +16847,16 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>3595</v>
+        <v>2004</v>
       </c>
       <c r="D21" t="s">
-        <v>3597</v>
+        <v>3953</v>
       </c>
       <c r="E21" t="s">
-        <v>3596</v>
+        <v>3952</v>
       </c>
       <c r="G21" t="s">
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="R21" t="s">
         <v>375</v>
@@ -15791,58 +16865,58 @@
         <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>2569</v>
+        <v>555</v>
       </c>
       <c r="U21" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="V21" t="s">
-        <v>1162</v>
+        <v>3637</v>
       </c>
       <c r="W21" t="s">
-        <v>3550</v>
+        <v>3881</v>
       </c>
       <c r="X21" t="s">
-        <v>3162</v>
+        <v>2186</v>
       </c>
       <c r="Y21" t="s">
-        <v>3540</v>
+        <v>3908</v>
       </c>
       <c r="Z21" t="s">
-        <v>3308</v>
+        <v>3906</v>
       </c>
       <c r="AA21" t="s">
-        <v>3551</v>
+        <v>2187</v>
       </c>
       <c r="AB21" t="s">
-        <v>3394</v>
+        <v>665</v>
       </c>
       <c r="AC21" t="s">
-        <v>3546</v>
+        <v>1967</v>
       </c>
       <c r="AD21" t="s">
-        <v>3476</v>
+        <v>3866</v>
       </c>
       <c r="AE21" t="s">
-        <v>2963</v>
+        <v>3914</v>
       </c>
       <c r="AF21" t="s">
-        <v>1967</v>
+        <v>3628</v>
       </c>
       <c r="AG21" t="s">
-        <v>766</v>
+        <v>1933</v>
       </c>
       <c r="AH21" t="s">
-        <v>3382</v>
+        <v>3277</v>
       </c>
       <c r="AI21" t="s">
-        <v>3595</v>
+        <v>2004</v>
       </c>
       <c r="AJ21" t="s">
-        <v>3597</v>
+        <v>3953</v>
       </c>
       <c r="AK21" t="s">
-        <v>3596</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -15853,16 +16927,16 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>3552</v>
+        <v>252</v>
       </c>
       <c r="D22" t="s">
-        <v>3599</v>
+        <v>3956</v>
       </c>
       <c r="E22" t="s">
-        <v>3598</v>
+        <v>3955</v>
       </c>
       <c r="G22" t="s">
-        <v>3415</v>
+        <v>627</v>
       </c>
       <c r="R22" t="s">
         <v>573</v>
@@ -15871,58 +16945,58 @@
         <v>804</v>
       </c>
       <c r="T22" t="s">
-        <v>3532</v>
+        <v>3863</v>
       </c>
       <c r="U22" t="s">
-        <v>3015</v>
+        <v>3874</v>
       </c>
       <c r="V22" t="s">
-        <v>3566</v>
+        <v>3905</v>
       </c>
       <c r="W22" t="s">
-        <v>1162</v>
+        <v>3746</v>
       </c>
       <c r="X22" t="s">
-        <v>3544</v>
+        <v>3730</v>
       </c>
       <c r="Y22" t="s">
-        <v>2199</v>
+        <v>2187</v>
       </c>
       <c r="Z22" t="s">
-        <v>3551</v>
+        <v>3865</v>
       </c>
       <c r="AA22" t="s">
-        <v>3162</v>
+        <v>3906</v>
       </c>
       <c r="AB22" t="s">
-        <v>3545</v>
+        <v>2079</v>
       </c>
       <c r="AC22" t="s">
-        <v>2584</v>
+        <v>1967</v>
       </c>
       <c r="AD22" t="s">
-        <v>3380</v>
+        <v>3866</v>
       </c>
       <c r="AE22" t="s">
-        <v>2963</v>
+        <v>3914</v>
       </c>
       <c r="AF22" t="s">
-        <v>3442</v>
+        <v>3954</v>
       </c>
       <c r="AG22" t="s">
-        <v>656</v>
+        <v>3855</v>
       </c>
       <c r="AH22" t="s">
-        <v>3161</v>
+        <v>2184</v>
       </c>
       <c r="AI22" t="s">
-        <v>3552</v>
+        <v>252</v>
       </c>
       <c r="AJ22" t="s">
-        <v>3599</v>
+        <v>3956</v>
       </c>
       <c r="AK22" t="s">
-        <v>3598</v>
+        <v>3955</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -15933,16 +17007,16 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>3600</v>
+        <v>818</v>
       </c>
       <c r="D23" t="s">
-        <v>3602</v>
+        <v>3958</v>
       </c>
       <c r="E23" t="s">
-        <v>3601</v>
+        <v>3957</v>
       </c>
       <c r="G23" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R23" t="s">
         <v>809</v>
@@ -15951,58 +17025,58 @@
         <v>281</v>
       </c>
       <c r="T23" t="s">
-        <v>3482</v>
+        <v>3762</v>
       </c>
       <c r="U23" t="s">
-        <v>3015</v>
+        <v>1953</v>
       </c>
       <c r="V23" t="s">
-        <v>3533</v>
+        <v>3905</v>
       </c>
       <c r="W23" t="s">
-        <v>3550</v>
+        <v>1348</v>
       </c>
       <c r="X23" t="s">
-        <v>3483</v>
+        <v>3908</v>
       </c>
       <c r="Y23" t="s">
-        <v>3545</v>
+        <v>2187</v>
       </c>
       <c r="Z23" t="s">
-        <v>3422</v>
+        <v>3923</v>
       </c>
       <c r="AA23" t="s">
-        <v>3534</v>
+        <v>3882</v>
       </c>
       <c r="AB23" t="s">
-        <v>3376</v>
+        <v>1967</v>
       </c>
       <c r="AC23" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AD23" t="s">
-        <v>3025</v>
+        <v>3765</v>
       </c>
       <c r="AE23" t="s">
-        <v>373</v>
+        <v>3877</v>
       </c>
       <c r="AF23" t="s">
-        <v>3162</v>
+        <v>1930</v>
       </c>
       <c r="AG23" t="s">
-        <v>3443</v>
+        <v>1937</v>
       </c>
       <c r="AH23" t="s">
-        <v>1967</v>
+        <v>3628</v>
       </c>
       <c r="AI23" t="s">
-        <v>3600</v>
+        <v>818</v>
       </c>
       <c r="AJ23" t="s">
-        <v>3602</v>
+        <v>3958</v>
       </c>
       <c r="AK23" t="s">
-        <v>3601</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -16013,13 +17087,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>1290</v>
+        <v>256</v>
       </c>
       <c r="D24" t="s">
-        <v>3605</v>
+        <v>3611</v>
       </c>
       <c r="E24" t="s">
-        <v>3604</v>
+        <v>3960</v>
       </c>
       <c r="G24" t="s">
         <v>426</v>
@@ -16031,58 +17105,58 @@
         <v>283</v>
       </c>
       <c r="T24" t="s">
-        <v>2569</v>
+        <v>3914</v>
       </c>
       <c r="U24" t="s">
-        <v>3485</v>
+        <v>2016</v>
       </c>
       <c r="V24" t="s">
-        <v>3483</v>
+        <v>3883</v>
       </c>
       <c r="W24" t="s">
-        <v>3015</v>
+        <v>3881</v>
       </c>
       <c r="X24" t="s">
-        <v>3603</v>
+        <v>3926</v>
       </c>
       <c r="Y24" t="s">
-        <v>3559</v>
+        <v>3959</v>
       </c>
       <c r="Z24" t="s">
-        <v>1370</v>
+        <v>3872</v>
       </c>
       <c r="AA24" t="s">
-        <v>3534</v>
+        <v>3730</v>
       </c>
       <c r="AB24" t="s">
-        <v>3545</v>
+        <v>3866</v>
       </c>
       <c r="AC24" t="s">
-        <v>3410</v>
+        <v>2079</v>
       </c>
       <c r="AD24" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AE24" t="s">
-        <v>3532</v>
+        <v>1927</v>
       </c>
       <c r="AF24" t="s">
-        <v>3564</v>
+        <v>3860</v>
       </c>
       <c r="AG24" t="s">
-        <v>3476</v>
+        <v>3667</v>
       </c>
       <c r="AH24" t="s">
-        <v>3550</v>
+        <v>3628</v>
       </c>
       <c r="AI24" t="s">
-        <v>1290</v>
+        <v>256</v>
       </c>
       <c r="AJ24" t="s">
-        <v>3605</v>
+        <v>3611</v>
       </c>
       <c r="AK24" t="s">
-        <v>3604</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -16093,13 +17167,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>1425</v>
+        <v>2933</v>
       </c>
       <c r="D25" t="s">
-        <v>3607</v>
+        <v>3963</v>
       </c>
       <c r="E25" t="s">
-        <v>3606</v>
+        <v>3962</v>
       </c>
       <c r="G25" t="s">
         <v>627</v>
@@ -16111,58 +17185,58 @@
         <v>461</v>
       </c>
       <c r="T25" t="s">
-        <v>1145</v>
+        <v>2986</v>
       </c>
       <c r="U25" t="s">
-        <v>3416</v>
+        <v>2928</v>
       </c>
       <c r="V25" t="s">
-        <v>3489</v>
+        <v>2927</v>
       </c>
       <c r="W25" t="s">
-        <v>3438</v>
+        <v>3920</v>
       </c>
       <c r="X25" t="s">
-        <v>3491</v>
+        <v>2001</v>
       </c>
       <c r="Y25" t="s">
-        <v>3418</v>
+        <v>1138</v>
       </c>
       <c r="Z25" t="s">
-        <v>2179</v>
+        <v>1940</v>
       </c>
       <c r="AA25" t="s">
-        <v>712</v>
+        <v>3906</v>
       </c>
       <c r="AB25" t="s">
-        <v>3376</v>
+        <v>3961</v>
       </c>
       <c r="AC25" t="s">
-        <v>656</v>
+        <v>2007</v>
       </c>
       <c r="AD25" t="s">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="AE25" t="s">
-        <v>2569</v>
+        <v>3914</v>
       </c>
       <c r="AF25" t="s">
-        <v>1138</v>
+        <v>1348</v>
       </c>
       <c r="AG25" t="s">
-        <v>2234</v>
+        <v>3687</v>
       </c>
       <c r="AH25" t="s">
-        <v>3492</v>
+        <v>1336</v>
       </c>
       <c r="AI25" t="s">
-        <v>1425</v>
+        <v>2933</v>
       </c>
       <c r="AJ25" t="s">
-        <v>3607</v>
+        <v>3963</v>
       </c>
       <c r="AK25" t="s">
-        <v>3606</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -16173,16 +17247,16 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>3400</v>
+        <v>2004</v>
       </c>
       <c r="D26" t="s">
-        <v>3609</v>
+        <v>3968</v>
       </c>
       <c r="E26" t="s">
-        <v>3608</v>
+        <v>3967</v>
       </c>
       <c r="G26" t="s">
-        <v>3415</v>
+        <v>627</v>
       </c>
       <c r="R26" t="s">
         <v>569</v>
@@ -16191,58 +17265,58 @@
         <v>572</v>
       </c>
       <c r="T26" t="s">
-        <v>3532</v>
+        <v>3863</v>
       </c>
       <c r="U26" t="s">
-        <v>3015</v>
+        <v>3864</v>
       </c>
       <c r="V26" t="s">
-        <v>3574</v>
+        <v>3964</v>
       </c>
       <c r="W26" t="s">
-        <v>3533</v>
+        <v>3905</v>
       </c>
       <c r="X26" t="s">
-        <v>1162</v>
+        <v>3911</v>
       </c>
       <c r="Y26" t="s">
-        <v>3534</v>
+        <v>2187</v>
       </c>
       <c r="Z26" t="s">
-        <v>3308</v>
+        <v>3965</v>
       </c>
       <c r="AA26" t="s">
-        <v>3162</v>
+        <v>3906</v>
       </c>
       <c r="AB26" t="s">
-        <v>3545</v>
+        <v>1967</v>
       </c>
       <c r="AC26" t="s">
-        <v>3256</v>
+        <v>3876</v>
       </c>
       <c r="AD26" t="s">
-        <v>2584</v>
+        <v>2079</v>
       </c>
       <c r="AE26" t="s">
-        <v>3385</v>
+        <v>3780</v>
       </c>
       <c r="AF26" t="s">
-        <v>1967</v>
+        <v>3687</v>
       </c>
       <c r="AG26" t="s">
-        <v>3396</v>
+        <v>3656</v>
       </c>
       <c r="AH26" t="s">
-        <v>2180</v>
+        <v>3966</v>
       </c>
       <c r="AI26" t="s">
-        <v>3400</v>
+        <v>2004</v>
       </c>
       <c r="AJ26" t="s">
-        <v>3609</v>
+        <v>3968</v>
       </c>
       <c r="AK26" t="s">
-        <v>3608</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -16253,16 +17327,16 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>3571</v>
+        <v>262</v>
       </c>
       <c r="D27" t="s">
-        <v>3611</v>
+        <v>3971</v>
       </c>
       <c r="E27" t="s">
-        <v>3610</v>
+        <v>3970</v>
       </c>
       <c r="G27" t="s">
-        <v>1252</v>
+        <v>627</v>
       </c>
       <c r="R27" t="s">
         <v>828</v>
@@ -16271,58 +17345,58 @@
         <v>827</v>
       </c>
       <c r="T27" t="s">
-        <v>2569</v>
+        <v>3526</v>
       </c>
       <c r="U27" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="V27" t="s">
-        <v>1162</v>
+        <v>3874</v>
       </c>
       <c r="W27" t="s">
-        <v>3566</v>
+        <v>3834</v>
       </c>
       <c r="X27" t="s">
-        <v>3534</v>
+        <v>3911</v>
       </c>
       <c r="Y27" t="s">
-        <v>3162</v>
+        <v>1935</v>
       </c>
       <c r="Z27" t="s">
-        <v>3394</v>
+        <v>2187</v>
       </c>
       <c r="AA27" t="s">
-        <v>3497</v>
+        <v>3906</v>
       </c>
       <c r="AB27" t="s">
-        <v>2584</v>
+        <v>1967</v>
       </c>
       <c r="AC27" t="s">
-        <v>3380</v>
+        <v>3866</v>
       </c>
       <c r="AD27" t="s">
-        <v>3410</v>
+        <v>2079</v>
       </c>
       <c r="AE27" t="s">
-        <v>2963</v>
+        <v>3784</v>
       </c>
       <c r="AF27" t="s">
-        <v>528</v>
+        <v>3969</v>
       </c>
       <c r="AG27" t="s">
-        <v>3443</v>
+        <v>3637</v>
       </c>
       <c r="AH27" t="s">
-        <v>1140</v>
+        <v>3687</v>
       </c>
       <c r="AI27" t="s">
-        <v>3571</v>
+        <v>262</v>
       </c>
       <c r="AJ27" t="s">
-        <v>3611</v>
+        <v>3971</v>
       </c>
       <c r="AK27" t="s">
-        <v>3610</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -16333,16 +17407,16 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>3612</v>
+        <v>745</v>
       </c>
       <c r="D28" t="s">
-        <v>3614</v>
+        <v>3933</v>
       </c>
       <c r="E28" t="s">
-        <v>3613</v>
+        <v>3972</v>
       </c>
       <c r="G28" t="s">
-        <v>1252</v>
+        <v>627</v>
       </c>
       <c r="R28" t="s">
         <v>832</v>
@@ -16351,58 +17425,58 @@
         <v>831</v>
       </c>
       <c r="T28" t="s">
-        <v>3532</v>
+        <v>2266</v>
       </c>
       <c r="U28" t="s">
-        <v>1162</v>
+        <v>3905</v>
       </c>
       <c r="V28" t="s">
-        <v>3544</v>
+        <v>3881</v>
       </c>
       <c r="W28" t="s">
-        <v>3015</v>
+        <v>3917</v>
       </c>
       <c r="X28" t="s">
-        <v>3555</v>
+        <v>2184</v>
       </c>
       <c r="Y28" t="s">
-        <v>3551</v>
+        <v>3906</v>
       </c>
       <c r="Z28" t="s">
-        <v>3376</v>
+        <v>2186</v>
       </c>
       <c r="AA28" t="s">
-        <v>3394</v>
+        <v>3908</v>
       </c>
       <c r="AB28" t="s">
-        <v>3162</v>
+        <v>3961</v>
       </c>
       <c r="AC28" t="s">
-        <v>3256</v>
+        <v>3866</v>
       </c>
       <c r="AD28" t="s">
-        <v>3476</v>
+        <v>1967</v>
       </c>
       <c r="AE28" t="s">
-        <v>2266</v>
+        <v>1927</v>
       </c>
       <c r="AF28" t="s">
-        <v>766</v>
+        <v>3666</v>
       </c>
       <c r="AG28" t="s">
-        <v>1967</v>
+        <v>3628</v>
       </c>
       <c r="AH28" t="s">
-        <v>3396</v>
+        <v>3667</v>
       </c>
       <c r="AI28" t="s">
-        <v>3612</v>
+        <v>745</v>
       </c>
       <c r="AJ28" t="s">
-        <v>3614</v>
+        <v>3933</v>
       </c>
       <c r="AK28" t="s">
-        <v>3613</v>
+        <v>3972</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -16413,16 +17487,16 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>3615</v>
+        <v>3054</v>
       </c>
       <c r="D29" t="s">
-        <v>3617</v>
+        <v>3975</v>
       </c>
       <c r="E29" t="s">
-        <v>3616</v>
+        <v>3974</v>
       </c>
       <c r="G29" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R29" t="s">
         <v>837</v>
@@ -16431,58 +17505,58 @@
         <v>836</v>
       </c>
       <c r="T29" t="s">
-        <v>2569</v>
+        <v>3863</v>
       </c>
       <c r="U29" t="s">
-        <v>3550</v>
+        <v>3637</v>
       </c>
       <c r="V29" t="s">
-        <v>1162</v>
+        <v>3905</v>
       </c>
       <c r="W29" t="s">
-        <v>3015</v>
+        <v>3973</v>
       </c>
       <c r="X29" t="s">
-        <v>3551</v>
+        <v>3874</v>
       </c>
       <c r="Y29" t="s">
-        <v>3162</v>
+        <v>1935</v>
       </c>
       <c r="Z29" t="s">
-        <v>3503</v>
+        <v>3923</v>
       </c>
       <c r="AA29" t="s">
-        <v>3396</v>
+        <v>3906</v>
       </c>
       <c r="AB29" t="s">
-        <v>3541</v>
+        <v>2021</v>
       </c>
       <c r="AC29" t="s">
-        <v>3458</v>
+        <v>3876</v>
       </c>
       <c r="AD29" t="s">
-        <v>3256</v>
+        <v>1967</v>
       </c>
       <c r="AE29" t="s">
-        <v>2963</v>
+        <v>3914</v>
       </c>
       <c r="AF29" t="s">
-        <v>3416</v>
+        <v>3893</v>
       </c>
       <c r="AG29" t="s">
-        <v>512</v>
+        <v>3894</v>
       </c>
       <c r="AH29" t="s">
-        <v>3269</v>
+        <v>3656</v>
       </c>
       <c r="AI29" t="s">
-        <v>3615</v>
+        <v>3054</v>
       </c>
       <c r="AJ29" t="s">
-        <v>3617</v>
+        <v>3975</v>
       </c>
       <c r="AK29" t="s">
-        <v>3616</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -16493,13 +17567,13 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>3618</v>
+        <v>290</v>
       </c>
       <c r="D30" t="s">
-        <v>3620</v>
+        <v>3978</v>
       </c>
       <c r="E30" t="s">
-        <v>3619</v>
+        <v>3977</v>
       </c>
       <c r="G30" t="s">
         <v>627</v>
@@ -16511,58 +17585,58 @@
         <v>289</v>
       </c>
       <c r="T30" t="s">
-        <v>3532</v>
+        <v>3863</v>
       </c>
       <c r="U30" t="s">
-        <v>3015</v>
+        <v>3976</v>
       </c>
       <c r="V30" t="s">
-        <v>3574</v>
+        <v>3905</v>
       </c>
       <c r="W30" t="s">
-        <v>3550</v>
+        <v>3874</v>
       </c>
       <c r="X30" t="s">
-        <v>3204</v>
+        <v>3911</v>
       </c>
       <c r="Y30" t="s">
-        <v>3396</v>
+        <v>1935</v>
       </c>
       <c r="Z30" t="s">
-        <v>3545</v>
+        <v>3865</v>
       </c>
       <c r="AA30" t="s">
-        <v>3394</v>
+        <v>3934</v>
       </c>
       <c r="AB30" t="s">
-        <v>3534</v>
+        <v>1967</v>
       </c>
       <c r="AC30" t="s">
-        <v>3256</v>
+        <v>3876</v>
       </c>
       <c r="AD30" t="s">
-        <v>3410</v>
+        <v>2079</v>
       </c>
       <c r="AE30" t="s">
-        <v>2569</v>
+        <v>891</v>
       </c>
       <c r="AF30" t="s">
-        <v>3570</v>
+        <v>1700</v>
       </c>
       <c r="AG30" t="s">
-        <v>3538</v>
+        <v>3746</v>
       </c>
       <c r="AH30" t="s">
-        <v>1967</v>
+        <v>3687</v>
       </c>
       <c r="AI30" t="s">
-        <v>3618</v>
+        <v>290</v>
       </c>
       <c r="AJ30" t="s">
-        <v>3620</v>
+        <v>3978</v>
       </c>
       <c r="AK30" t="s">
-        <v>3619</v>
+        <v>3977</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -16573,13 +17647,13 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>3465</v>
+        <v>677</v>
       </c>
       <c r="D31" t="s">
-        <v>3622</v>
+        <v>3980</v>
       </c>
       <c r="E31" t="s">
-        <v>3621</v>
+        <v>3979</v>
       </c>
       <c r="G31" t="s">
         <v>627</v>
@@ -16591,58 +17665,58 @@
         <v>843</v>
       </c>
       <c r="T31" t="s">
-        <v>3532</v>
+        <v>3526</v>
       </c>
       <c r="U31" t="s">
-        <v>3533</v>
+        <v>3864</v>
       </c>
       <c r="V31" t="s">
-        <v>3574</v>
+        <v>3874</v>
       </c>
       <c r="W31" t="s">
-        <v>3015</v>
+        <v>3905</v>
       </c>
       <c r="X31" t="s">
-        <v>3564</v>
+        <v>2187</v>
       </c>
       <c r="Y31" t="s">
-        <v>3534</v>
+        <v>3906</v>
       </c>
       <c r="Z31" t="s">
-        <v>3376</v>
+        <v>3944</v>
       </c>
       <c r="AA31" t="s">
-        <v>3204</v>
+        <v>1935</v>
       </c>
       <c r="AB31" t="s">
-        <v>3394</v>
+        <v>2079</v>
       </c>
       <c r="AC31" t="s">
-        <v>3546</v>
+        <v>1967</v>
       </c>
       <c r="AD31" t="s">
-        <v>3256</v>
+        <v>3866</v>
       </c>
       <c r="AE31" t="s">
-        <v>2569</v>
+        <v>891</v>
       </c>
       <c r="AF31" t="s">
-        <v>766</v>
+        <v>3746</v>
       </c>
       <c r="AG31" t="s">
-        <v>1967</v>
+        <v>3220</v>
       </c>
       <c r="AH31" t="s">
-        <v>3396</v>
+        <v>3687</v>
       </c>
       <c r="AI31" t="s">
-        <v>3465</v>
+        <v>677</v>
       </c>
       <c r="AJ31" t="s">
-        <v>3622</v>
+        <v>3980</v>
       </c>
       <c r="AK31" t="s">
-        <v>3621</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -16653,16 +17727,16 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>3618</v>
+        <v>752</v>
       </c>
       <c r="D32" t="s">
-        <v>3624</v>
+        <v>3983</v>
       </c>
       <c r="E32" t="s">
-        <v>3623</v>
+        <v>3982</v>
       </c>
       <c r="G32" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R32" t="s">
         <v>494</v>
@@ -16671,58 +17745,58 @@
         <v>849</v>
       </c>
       <c r="T32" t="s">
-        <v>3532</v>
+        <v>3526</v>
       </c>
       <c r="U32" t="s">
-        <v>3550</v>
+        <v>3871</v>
       </c>
       <c r="V32" t="s">
-        <v>3446</v>
+        <v>3628</v>
       </c>
       <c r="W32" t="s">
-        <v>3015</v>
+        <v>3874</v>
       </c>
       <c r="X32" t="s">
-        <v>3560</v>
+        <v>3908</v>
       </c>
       <c r="Y32" t="s">
-        <v>3534</v>
+        <v>3981</v>
       </c>
       <c r="Z32" t="s">
-        <v>3525</v>
+        <v>3906</v>
       </c>
       <c r="AA32" t="s">
-        <v>3376</v>
+        <v>2174</v>
       </c>
       <c r="AB32" t="s">
-        <v>3204</v>
+        <v>3866</v>
       </c>
       <c r="AC32" t="s">
-        <v>3546</v>
+        <v>3645</v>
       </c>
       <c r="AD32" t="s">
-        <v>3256</v>
+        <v>3961</v>
       </c>
       <c r="AE32" t="s">
-        <v>3526</v>
+        <v>1927</v>
       </c>
       <c r="AF32" t="s">
-        <v>3162</v>
+        <v>3667</v>
       </c>
       <c r="AG32" t="s">
-        <v>3390</v>
+        <v>3731</v>
       </c>
       <c r="AH32" t="s">
-        <v>3420</v>
+        <v>1933</v>
       </c>
       <c r="AI32" t="s">
-        <v>3618</v>
+        <v>752</v>
       </c>
       <c r="AJ32" t="s">
-        <v>3624</v>
+        <v>3983</v>
       </c>
       <c r="AK32" t="s">
-        <v>3623</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -16733,16 +17807,16 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>3625</v>
+        <v>1485</v>
       </c>
       <c r="D33" t="s">
-        <v>3627</v>
+        <v>3985</v>
       </c>
       <c r="E33" t="s">
-        <v>3626</v>
+        <v>3984</v>
       </c>
       <c r="G33" t="s">
-        <v>880</v>
+        <v>426</v>
       </c>
       <c r="R33" t="s">
         <v>418</v>
@@ -16751,58 +17825,58 @@
         <v>241</v>
       </c>
       <c r="T33" t="s">
-        <v>3532</v>
+        <v>3914</v>
       </c>
       <c r="U33" t="s">
-        <v>766</v>
+        <v>3881</v>
       </c>
       <c r="V33" t="s">
-        <v>1162</v>
+        <v>3905</v>
       </c>
       <c r="W33" t="s">
-        <v>3015</v>
+        <v>3637</v>
       </c>
       <c r="X33" t="s">
-        <v>3545</v>
+        <v>665</v>
       </c>
       <c r="Y33" t="s">
-        <v>3551</v>
+        <v>3906</v>
       </c>
       <c r="Z33" t="s">
-        <v>3308</v>
+        <v>2187</v>
       </c>
       <c r="AA33" t="s">
-        <v>3162</v>
+        <v>3908</v>
       </c>
       <c r="AB33" t="s">
-        <v>3380</v>
+        <v>2020</v>
       </c>
       <c r="AC33" t="s">
-        <v>3256</v>
+        <v>3961</v>
       </c>
       <c r="AD33" t="s">
-        <v>2584</v>
+        <v>3866</v>
       </c>
       <c r="AE33" t="s">
-        <v>2569</v>
+        <v>1927</v>
       </c>
       <c r="AF33" t="s">
-        <v>3489</v>
+        <v>2927</v>
       </c>
       <c r="AG33" t="s">
-        <v>3540</v>
+        <v>1937</v>
       </c>
       <c r="AH33" t="s">
-        <v>3382</v>
+        <v>3628</v>
       </c>
       <c r="AI33" t="s">
-        <v>3625</v>
+        <v>1485</v>
       </c>
       <c r="AJ33" t="s">
-        <v>3627</v>
+        <v>3985</v>
       </c>
       <c r="AK33" t="s">
-        <v>3626</v>
+        <v>3984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GW 28th b4 bonus
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20314" uniqueCount="3986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21114" uniqueCount="4108">
   <si>
     <t>Places</t>
   </si>
@@ -11992,6 +11992,372 @@
   </si>
   <si>
     <t>1738</t>
+  </si>
+  <si>
+    <t>Ramsdale 2</t>
+  </si>
+  <si>
+    <t>James 18</t>
+  </si>
+  <si>
+    <t>Dennis 4</t>
+  </si>
+  <si>
+    <t>White 1</t>
+  </si>
+  <si>
+    <t>2,228,873</t>
+  </si>
+  <si>
+    <t>Guaita 8</t>
+  </si>
+  <si>
+    <t>Coady 7</t>
+  </si>
+  <si>
+    <t>Smith Rowe 0</t>
+  </si>
+  <si>
+    <t>Mané 8</t>
+  </si>
+  <si>
+    <t>Adams 4</t>
+  </si>
+  <si>
+    <t>2,802,713</t>
+  </si>
+  <si>
+    <t>James 36$ captain</t>
+  </si>
+  <si>
+    <t>Ramsey 6</t>
+  </si>
+  <si>
+    <t>Broja 4</t>
+  </si>
+  <si>
+    <t>Saka 12</t>
+  </si>
+  <si>
+    <t>Lacazette 8</t>
+  </si>
+  <si>
+    <t>468,630</t>
+  </si>
+  <si>
+    <t>1698</t>
+  </si>
+  <si>
+    <t>Sá 9</t>
+  </si>
+  <si>
+    <t>Thiago Silva 8</t>
+  </si>
+  <si>
+    <t>Coutinho 42$ captain</t>
+  </si>
+  <si>
+    <t>Willock 4</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>300,257</t>
+  </si>
+  <si>
+    <t>Forster View player information</t>
+  </si>
+  <si>
+    <t>Ait Nouri 8</t>
+  </si>
+  <si>
+    <t>Mings 14</t>
+  </si>
+  <si>
+    <t>Ziyech 0</t>
+  </si>
+  <si>
+    <t>Hwang 7</t>
+  </si>
+  <si>
+    <t>Kane 13</t>
+  </si>
+  <si>
+    <t>Davies 6</t>
+  </si>
+  <si>
+    <t>Rodriguez 2</t>
+  </si>
+  <si>
+    <t>Winks 0</t>
+  </si>
+  <si>
+    <t>835,247</t>
+  </si>
+  <si>
+    <t>Reguilón 7</t>
+  </si>
+  <si>
+    <t>Ronaldo 0</t>
+  </si>
+  <si>
+    <t>3,770,903</t>
+  </si>
+  <si>
+    <t>Coutinho 21</t>
+  </si>
+  <si>
+    <t>Havertz 48$ captain</t>
+  </si>
+  <si>
+    <t>Jiménez 7</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>506,477</t>
+  </si>
+  <si>
+    <t>1691</t>
+  </si>
+  <si>
+    <t>Ødegaard 8</t>
+  </si>
+  <si>
+    <t>1,588,548</t>
+  </si>
+  <si>
+    <t>1551</t>
+  </si>
+  <si>
+    <t>Gabriel 1</t>
+  </si>
+  <si>
+    <t>Martinelli 7</t>
+  </si>
+  <si>
+    <t>Roberts 0</t>
+  </si>
+  <si>
+    <t>Jansson 4</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>723,562</t>
+  </si>
+  <si>
+    <t>Raya View player information</t>
+  </si>
+  <si>
+    <t>Cancelo 75% chance of playing</t>
+  </si>
+  <si>
+    <t>Sissoko 9</t>
+  </si>
+  <si>
+    <t>Dennis 8$ captain</t>
+  </si>
+  <si>
+    <t>McNeil 2</t>
+  </si>
+  <si>
+    <t>Mee 0</t>
+  </si>
+  <si>
+    <t>723,070</t>
+  </si>
+  <si>
+    <t>Kulusevski 10</t>
+  </si>
+  <si>
+    <t>450,681</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>Tierney 1</t>
+  </si>
+  <si>
+    <t>871,125</t>
+  </si>
+  <si>
+    <t>1632</t>
+  </si>
+  <si>
+    <t>Ward-Prowse 8$ captain</t>
+  </si>
+  <si>
+    <t>1,249,087</t>
+  </si>
+  <si>
+    <t>1586</t>
+  </si>
+  <si>
+    <t>Mendy 7</t>
+  </si>
+  <si>
+    <t>Marçal 1</t>
+  </si>
+  <si>
+    <t>876,264</t>
+  </si>
+  <si>
+    <t>1,794,265</t>
+  </si>
+  <si>
+    <t>887,173</t>
+  </si>
+  <si>
+    <t>1630</t>
+  </si>
+  <si>
+    <t>Bednarek 0</t>
+  </si>
+  <si>
+    <t>Coady 14$ captain</t>
+  </si>
+  <si>
+    <t>1,058,317</t>
+  </si>
+  <si>
+    <t>1608</t>
+  </si>
+  <si>
+    <t>Mount 13</t>
+  </si>
+  <si>
+    <t>Richarlison 2</t>
+  </si>
+  <si>
+    <t>42,901</t>
+  </si>
+  <si>
+    <t>1854</t>
+  </si>
+  <si>
+    <t>Forster 2</t>
+  </si>
+  <si>
+    <t>Schär 12</t>
+  </si>
+  <si>
+    <t>Dubravka 6</t>
+  </si>
+  <si>
+    <t>410,081</t>
+  </si>
+  <si>
+    <t>54,138</t>
+  </si>
+  <si>
+    <t>1844</t>
+  </si>
+  <si>
+    <t>Cash 26</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>71,702</t>
+  </si>
+  <si>
+    <t>1831</t>
+  </si>
+  <si>
+    <t>Alisson 9</t>
+  </si>
+  <si>
+    <t>De Bruyne 18</t>
+  </si>
+  <si>
+    <t>614,351</t>
+  </si>
+  <si>
+    <t>1671</t>
+  </si>
+  <si>
+    <t>Wood 8</t>
+  </si>
+  <si>
+    <t>Lukaku 2$ captain</t>
+  </si>
+  <si>
+    <t>Emerson Royal 0</t>
+  </si>
+  <si>
+    <t>260,715</t>
+  </si>
+  <si>
+    <t>1750</t>
+  </si>
+  <si>
+    <t>6,661,323</t>
+  </si>
+  <si>
+    <t>1144</t>
+  </si>
+  <si>
+    <t>199,275</t>
+  </si>
+  <si>
+    <t>1770</t>
+  </si>
+  <si>
+    <t>Fraser 15</t>
+  </si>
+  <si>
+    <t>35,358</t>
+  </si>
+  <si>
+    <t>1862</t>
+  </si>
+  <si>
+    <t>359,666</t>
+  </si>
+  <si>
+    <t>1723</t>
+  </si>
+  <si>
+    <t>Watkins 12$ captain</t>
+  </si>
+  <si>
+    <t>56,863</t>
+  </si>
+  <si>
+    <t>1842</t>
+  </si>
+  <si>
+    <t>28,702</t>
+  </si>
+  <si>
+    <t>1870</t>
+  </si>
+  <si>
+    <t>Rüdiger 12$ captain</t>
+  </si>
+  <si>
+    <t>104,840</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>73,254</t>
+  </si>
+  <si>
+    <t>1830</t>
+  </si>
+  <si>
+    <t>137,870</t>
+  </si>
+  <si>
+    <t>1795</t>
   </si>
 </sst>
 </file>
@@ -15186,22 +15552,22 @@
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="19.41015625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="20.203125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="28.4609375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="38.89453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.171875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="20.171875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="23.05078125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="20.171875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="19.23828125" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="26.421875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="13.375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.94921875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="21.50390625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.92578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="19.5078125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.3828125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
   </cols>
@@ -15327,13 +15693,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>1964</v>
+        <v>290</v>
       </c>
       <c r="D2" t="s">
-        <v>2260</v>
+        <v>1986</v>
       </c>
       <c r="E2" t="s">
-        <v>3907</v>
+        <v>3990</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -15345,58 +15711,58 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="U2" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="V2" t="s">
-        <v>2837</v>
+        <v>3987</v>
       </c>
       <c r="W2" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="X2" t="s">
-        <v>3906</v>
+        <v>3017</v>
       </c>
       <c r="Y2" t="s">
-        <v>2001</v>
+        <v>2840</v>
       </c>
       <c r="Z2" t="s">
-        <v>1929</v>
+        <v>2050</v>
       </c>
       <c r="AA2" t="s">
-        <v>3633</v>
+        <v>3154</v>
       </c>
       <c r="AB2" t="s">
-        <v>2843</v>
+        <v>3379</v>
       </c>
       <c r="AC2" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AD2" t="s">
-        <v>3381</v>
+        <v>673</v>
       </c>
       <c r="AE2" t="s">
         <v>2266</v>
       </c>
       <c r="AF2" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="AG2" t="s">
         <v>914</v>
       </c>
       <c r="AH2" t="s">
-        <v>1930</v>
+        <v>3989</v>
       </c>
       <c r="AI2" t="s">
-        <v>1964</v>
+        <v>290</v>
       </c>
       <c r="AJ2" t="s">
-        <v>2260</v>
+        <v>1986</v>
       </c>
       <c r="AK2" t="s">
-        <v>3907</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -15407,13 +15773,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>1297</v>
+        <v>2004</v>
       </c>
       <c r="D3" t="s">
-        <v>3910</v>
+        <v>2121</v>
       </c>
       <c r="E3" t="s">
-        <v>3909</v>
+        <v>3996</v>
       </c>
       <c r="G3" t="s">
         <v>627</v>
@@ -15425,43 +15791,43 @@
         <v>687</v>
       </c>
       <c r="T3" t="s">
-        <v>1917</v>
+        <v>3991</v>
       </c>
       <c r="U3" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="V3" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="W3" t="s">
-        <v>765</v>
+        <v>3992</v>
       </c>
       <c r="X3" t="s">
-        <v>3633</v>
+        <v>3157</v>
       </c>
       <c r="Y3" t="s">
-        <v>1932</v>
+        <v>3154</v>
       </c>
       <c r="Z3" t="s">
-        <v>3908</v>
+        <v>3993</v>
       </c>
       <c r="AA3" t="s">
         <v>665</v>
       </c>
       <c r="AB3" t="s">
-        <v>3644</v>
+        <v>3994</v>
       </c>
       <c r="AC3" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AD3" t="s">
-        <v>3645</v>
+        <v>3995</v>
       </c>
       <c r="AE3" t="s">
         <v>2266</v>
       </c>
       <c r="AF3" t="s">
-        <v>3637</v>
+        <v>3162</v>
       </c>
       <c r="AG3" t="s">
         <v>684</v>
@@ -15470,13 +15836,13 @@
         <v>914</v>
       </c>
       <c r="AI3" t="s">
-        <v>1297</v>
+        <v>2004</v>
       </c>
       <c r="AJ3" t="s">
-        <v>3910</v>
+        <v>2121</v>
       </c>
       <c r="AK3" t="s">
-        <v>3909</v>
+        <v>3996</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -15487,16 +15853,16 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>2004</v>
+        <v>1197</v>
       </c>
       <c r="D4" t="s">
-        <v>3913</v>
+        <v>4003</v>
       </c>
       <c r="E4" t="s">
-        <v>3912</v>
+        <v>4002</v>
       </c>
       <c r="G4" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R4" t="s">
         <v>697</v>
@@ -15505,58 +15871,58 @@
         <v>696</v>
       </c>
       <c r="T4" t="s">
-        <v>3863</v>
+        <v>911</v>
       </c>
       <c r="U4" t="s">
-        <v>3648</v>
+        <v>3992</v>
       </c>
       <c r="V4" t="s">
-        <v>3905</v>
+        <v>3046</v>
       </c>
       <c r="W4" t="s">
-        <v>3864</v>
+        <v>3997</v>
       </c>
       <c r="X4" t="s">
-        <v>1935</v>
+        <v>1414</v>
       </c>
       <c r="Y4" t="s">
-        <v>3911</v>
+        <v>654</v>
       </c>
       <c r="Z4" t="s">
-        <v>3906</v>
+        <v>3169</v>
       </c>
       <c r="AA4" t="s">
-        <v>3865</v>
+        <v>3017</v>
       </c>
       <c r="AB4" t="s">
-        <v>3866</v>
+        <v>3998</v>
       </c>
       <c r="AC4" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AD4" t="s">
-        <v>2079</v>
+        <v>3988</v>
       </c>
       <c r="AE4" t="s">
-        <v>3469</v>
+        <v>2266</v>
       </c>
       <c r="AF4" t="s">
-        <v>3656</v>
+        <v>4000</v>
       </c>
       <c r="AG4" t="s">
-        <v>780</v>
+        <v>4001</v>
       </c>
       <c r="AH4" t="s">
-        <v>3657</v>
+        <v>3989</v>
       </c>
       <c r="AI4" t="s">
-        <v>2004</v>
+        <v>1197</v>
       </c>
       <c r="AJ4" t="s">
-        <v>3913</v>
+        <v>4003</v>
       </c>
       <c r="AK4" t="s">
-        <v>3912</v>
+        <v>4002</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -15567,16 +15933,16 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>1886</v>
+        <v>4008</v>
       </c>
       <c r="D5" t="s">
-        <v>3916</v>
+        <v>3985</v>
       </c>
       <c r="E5" t="s">
-        <v>3915</v>
+        <v>4009</v>
       </c>
       <c r="G5" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R5" t="s">
         <v>557</v>
@@ -15585,58 +15951,58 @@
         <v>705</v>
       </c>
       <c r="T5" t="s">
-        <v>3813</v>
+        <v>4004</v>
       </c>
       <c r="U5" t="s">
-        <v>1933</v>
+        <v>3200</v>
       </c>
       <c r="V5" t="s">
-        <v>3628</v>
+        <v>3438</v>
       </c>
       <c r="W5" t="s">
-        <v>1930</v>
+        <v>4005</v>
       </c>
       <c r="X5" t="s">
-        <v>3905</v>
+        <v>3992</v>
       </c>
       <c r="Y5" t="s">
-        <v>3662</v>
+        <v>4006</v>
       </c>
       <c r="Z5" t="s">
-        <v>3908</v>
+        <v>3169</v>
       </c>
       <c r="AA5" t="s">
-        <v>3867</v>
+        <v>4007</v>
       </c>
       <c r="AB5" t="s">
-        <v>1967</v>
+        <v>654</v>
       </c>
       <c r="AC5" t="s">
-        <v>3645</v>
+        <v>3999</v>
       </c>
       <c r="AD5" t="s">
-        <v>3444</v>
+        <v>3995</v>
       </c>
       <c r="AE5" t="s">
-        <v>3914</v>
+        <v>911</v>
       </c>
       <c r="AF5" t="s">
-        <v>1937</v>
+        <v>3881</v>
       </c>
       <c r="AG5" t="s">
-        <v>3666</v>
+        <v>4000</v>
       </c>
       <c r="AH5" t="s">
-        <v>3667</v>
+        <v>455</v>
       </c>
       <c r="AI5" t="s">
-        <v>1886</v>
+        <v>4008</v>
       </c>
       <c r="AJ5" t="s">
-        <v>3916</v>
+        <v>3985</v>
       </c>
       <c r="AK5" t="s">
-        <v>3915</v>
+        <v>4009</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -15647,13 +16013,13 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>677</v>
+        <v>627</v>
       </c>
       <c r="D6" t="s">
-        <v>3749</v>
+        <v>3951</v>
       </c>
       <c r="E6" t="s">
-        <v>3919</v>
+        <v>4019</v>
       </c>
       <c r="G6" t="s">
         <v>426</v>
@@ -15665,58 +16031,58 @@
         <v>717</v>
       </c>
       <c r="T6" t="s">
-        <v>3526</v>
+        <v>4010</v>
       </c>
       <c r="U6" t="s">
-        <v>3917</v>
+        <v>4011</v>
       </c>
       <c r="V6" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="W6" t="s">
-        <v>3816</v>
+        <v>4012</v>
       </c>
       <c r="X6" t="s">
-        <v>3918</v>
+        <v>1414</v>
       </c>
       <c r="Y6" t="s">
-        <v>3869</v>
+        <v>4006</v>
       </c>
       <c r="Z6" t="s">
-        <v>3817</v>
+        <v>3169</v>
       </c>
       <c r="AA6" t="s">
-        <v>2193</v>
+        <v>4013</v>
       </c>
       <c r="AB6" t="s">
-        <v>1343</v>
+        <v>4000</v>
       </c>
       <c r="AC6" t="s">
-        <v>2079</v>
+        <v>4014</v>
       </c>
       <c r="AD6" t="s">
-        <v>3870</v>
+        <v>4015</v>
       </c>
       <c r="AE6" t="s">
         <v>1128</v>
       </c>
       <c r="AF6" t="s">
-        <v>1937</v>
+        <v>4016</v>
       </c>
       <c r="AG6" t="s">
-        <v>3628</v>
+        <v>4017</v>
       </c>
       <c r="AH6" t="s">
-        <v>3667</v>
+        <v>4018</v>
       </c>
       <c r="AI6" t="s">
-        <v>677</v>
+        <v>627</v>
       </c>
       <c r="AJ6" t="s">
-        <v>3749</v>
+        <v>3951</v>
       </c>
       <c r="AK6" t="s">
-        <v>3919</v>
+        <v>4019</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -15727,13 +16093,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>3086</v>
+        <v>1297</v>
       </c>
       <c r="D7" t="s">
-        <v>2586</v>
+        <v>3123</v>
       </c>
       <c r="E7" t="s">
-        <v>3921</v>
+        <v>4022</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -15745,58 +16111,58 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="U7" t="s">
-        <v>3920</v>
+        <v>661</v>
       </c>
       <c r="V7" t="s">
-        <v>528</v>
+        <v>4020</v>
       </c>
       <c r="W7" t="s">
         <v>1164</v>
       </c>
       <c r="X7" t="s">
-        <v>3683</v>
+        <v>3417</v>
       </c>
       <c r="Y7" t="s">
-        <v>3908</v>
+        <v>3162</v>
       </c>
       <c r="Z7" t="s">
         <v>665</v>
       </c>
       <c r="AA7" t="s">
-        <v>3633</v>
+        <v>3154</v>
       </c>
       <c r="AB7" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AC7" t="s">
-        <v>2007</v>
+        <v>656</v>
       </c>
       <c r="AD7" t="s">
-        <v>913</v>
+        <v>4021</v>
       </c>
       <c r="AE7" t="s">
         <v>778</v>
       </c>
       <c r="AF7" t="s">
-        <v>3687</v>
+        <v>724</v>
       </c>
       <c r="AG7" t="s">
-        <v>1154</v>
+        <v>779</v>
       </c>
       <c r="AH7" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="AI7" t="s">
-        <v>3086</v>
+        <v>1297</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2586</v>
+        <v>3123</v>
       </c>
       <c r="AK7" t="s">
-        <v>3921</v>
+        <v>4022</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -15807,16 +16173,16 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>686</v>
+        <v>4026</v>
       </c>
       <c r="D8" t="s">
-        <v>3925</v>
+        <v>4028</v>
       </c>
       <c r="E8" t="s">
-        <v>3924</v>
+        <v>4027</v>
       </c>
       <c r="G8" t="s">
-        <v>880</v>
+        <v>627</v>
       </c>
       <c r="R8" t="s">
         <v>547</v>
@@ -15825,58 +16191,58 @@
         <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>3914</v>
+        <v>4004</v>
       </c>
       <c r="U8" t="s">
-        <v>3871</v>
+        <v>3881</v>
       </c>
       <c r="V8" t="s">
-        <v>2173</v>
+        <v>681</v>
       </c>
       <c r="W8" t="s">
-        <v>3922</v>
+        <v>3438</v>
       </c>
       <c r="X8" t="s">
-        <v>3872</v>
+        <v>4023</v>
       </c>
       <c r="Y8" t="s">
-        <v>3873</v>
+        <v>654</v>
       </c>
       <c r="Z8" t="s">
-        <v>3923</v>
+        <v>4007</v>
       </c>
       <c r="AA8" t="s">
-        <v>3908</v>
+        <v>4024</v>
       </c>
       <c r="AB8" t="s">
-        <v>3866</v>
+        <v>3999</v>
       </c>
       <c r="AC8" t="s">
-        <v>1967</v>
+        <v>340</v>
       </c>
       <c r="AD8" t="s">
-        <v>2079</v>
+        <v>4025</v>
       </c>
       <c r="AE8" t="s">
-        <v>1806</v>
+        <v>911</v>
       </c>
       <c r="AF8" t="s">
-        <v>1933</v>
+        <v>3169</v>
       </c>
       <c r="AG8" t="s">
-        <v>3628</v>
+        <v>3200</v>
       </c>
       <c r="AH8" t="s">
-        <v>3196</v>
+        <v>3157</v>
       </c>
       <c r="AI8" t="s">
-        <v>686</v>
+        <v>4026</v>
       </c>
       <c r="AJ8" t="s">
-        <v>3925</v>
+        <v>4028</v>
       </c>
       <c r="AK8" t="s">
-        <v>3924</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -15887,13 +16253,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>1963</v>
+        <v>704</v>
       </c>
       <c r="D9" t="s">
-        <v>2049</v>
+        <v>4031</v>
       </c>
       <c r="E9" t="s">
-        <v>3927</v>
+        <v>4030</v>
       </c>
       <c r="G9" t="s">
         <v>627</v>
@@ -15908,55 +16274,55 @@
         <v>3813</v>
       </c>
       <c r="U9" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="V9" t="s">
-        <v>3687</v>
+        <v>724</v>
       </c>
       <c r="W9" t="s">
-        <v>3926</v>
+        <v>3200</v>
       </c>
       <c r="X9" t="s">
-        <v>3633</v>
+        <v>3154</v>
       </c>
       <c r="Y9" t="s">
-        <v>3196</v>
+        <v>4029</v>
       </c>
       <c r="Z9" t="s">
-        <v>3908</v>
+        <v>3162</v>
       </c>
       <c r="AA9" t="s">
-        <v>3825</v>
+        <v>3428</v>
       </c>
       <c r="AB9" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AC9" t="s">
-        <v>913</v>
+        <v>4021</v>
       </c>
       <c r="AD9" t="s">
-        <v>3645</v>
+        <v>3995</v>
       </c>
       <c r="AE9" t="s">
         <v>2266</v>
       </c>
       <c r="AF9" t="s">
-        <v>3920</v>
+        <v>661</v>
       </c>
       <c r="AG9" t="s">
-        <v>1929</v>
+        <v>2050</v>
       </c>
       <c r="AH9" t="s">
-        <v>1354</v>
+        <v>2905</v>
       </c>
       <c r="AI9" t="s">
-        <v>1963</v>
+        <v>704</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2049</v>
+        <v>4031</v>
       </c>
       <c r="AK9" t="s">
-        <v>3927</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -15967,16 +16333,16 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>1884</v>
+        <v>4036</v>
       </c>
       <c r="D10" t="s">
-        <v>3714</v>
+        <v>3605</v>
       </c>
       <c r="E10" t="s">
-        <v>3928</v>
+        <v>4037</v>
       </c>
       <c r="G10" t="s">
-        <v>426</v>
+        <v>680</v>
       </c>
       <c r="R10" t="s">
         <v>742</v>
@@ -15985,58 +16351,58 @@
         <v>259</v>
       </c>
       <c r="T10" t="s">
-        <v>3813</v>
+        <v>4004</v>
       </c>
       <c r="U10" t="s">
-        <v>1181</v>
+        <v>4032</v>
       </c>
       <c r="V10" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="W10" t="s">
-        <v>3864</v>
+        <v>1414</v>
       </c>
       <c r="X10" t="s">
-        <v>3908</v>
+        <v>3162</v>
       </c>
       <c r="Y10" t="s">
-        <v>2174</v>
+        <v>4006</v>
       </c>
       <c r="Z10" t="s">
         <v>665</v>
       </c>
       <c r="AA10" t="s">
-        <v>3667</v>
+        <v>3169</v>
       </c>
       <c r="AB10" t="s">
-        <v>1967</v>
+        <v>4033</v>
       </c>
       <c r="AC10" t="s">
-        <v>3866</v>
+        <v>3999</v>
       </c>
       <c r="AD10" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AE10" t="s">
-        <v>3705</v>
+        <v>740</v>
       </c>
       <c r="AF10" t="s">
-        <v>3628</v>
+        <v>3252</v>
       </c>
       <c r="AG10" t="s">
-        <v>1941</v>
+        <v>4034</v>
       </c>
       <c r="AH10" t="s">
-        <v>3205</v>
+        <v>4035</v>
       </c>
       <c r="AI10" t="s">
-        <v>1884</v>
+        <v>4036</v>
       </c>
       <c r="AJ10" t="s">
-        <v>3714</v>
+        <v>3605</v>
       </c>
       <c r="AK10" t="s">
-        <v>3928</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -16047,16 +16413,16 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="D11" t="s">
-        <v>3930</v>
+        <v>3605</v>
       </c>
       <c r="E11" t="s">
-        <v>3929</v>
+        <v>4044</v>
       </c>
       <c r="G11" t="s">
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="R11" t="s">
         <v>747</v>
@@ -16065,58 +16431,58 @@
         <v>746</v>
       </c>
       <c r="T11" t="s">
+        <v>4038</v>
+      </c>
+      <c r="U11" t="s">
+        <v>4039</v>
+      </c>
+      <c r="V11" t="s">
+        <v>3191</v>
+      </c>
+      <c r="W11" t="s">
+        <v>3438</v>
+      </c>
+      <c r="X11" t="s">
+        <v>3169</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>4040</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>2883</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>3993</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>3252</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>3832</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>4041</v>
+      </c>
+      <c r="AE11" t="s">
         <v>2266</v>
       </c>
-      <c r="U11" t="s">
-        <v>3905</v>
-      </c>
-      <c r="V11" t="s">
-        <v>3874</v>
-      </c>
-      <c r="W11" t="s">
-        <v>3920</v>
-      </c>
-      <c r="X11" t="s">
-        <v>2173</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>3875</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>3869</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>2193</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>3876</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1899</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>3877</v>
-      </c>
       <c r="AF11" t="s">
-        <v>3667</v>
+        <v>661</v>
       </c>
       <c r="AG11" t="s">
-        <v>1932</v>
+        <v>4042</v>
       </c>
       <c r="AH11" t="s">
-        <v>3628</v>
+        <v>4043</v>
       </c>
       <c r="AI11" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="AJ11" t="s">
-        <v>3930</v>
+        <v>3605</v>
       </c>
       <c r="AK11" t="s">
-        <v>3929</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -16127,16 +16493,16 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>848</v>
+        <v>1192</v>
       </c>
       <c r="D12" t="s">
-        <v>3933</v>
+        <v>4047</v>
       </c>
       <c r="E12" t="s">
-        <v>3932</v>
+        <v>4046</v>
       </c>
       <c r="G12" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R12" t="s">
         <v>392</v>
@@ -16145,58 +16511,58 @@
         <v>263</v>
       </c>
       <c r="T12" t="s">
-        <v>397</v>
+        <v>4004</v>
       </c>
       <c r="U12" t="s">
-        <v>3920</v>
+        <v>3438</v>
       </c>
       <c r="V12" t="s">
-        <v>3666</v>
+        <v>3987</v>
       </c>
       <c r="W12" t="s">
-        <v>3716</v>
+        <v>3989</v>
       </c>
       <c r="X12" t="s">
-        <v>3834</v>
+        <v>3881</v>
       </c>
       <c r="Y12" t="s">
-        <v>3878</v>
+        <v>879</v>
       </c>
       <c r="Z12" t="s">
-        <v>1929</v>
+        <v>3998</v>
       </c>
       <c r="AA12" t="s">
-        <v>3835</v>
+        <v>3169</v>
       </c>
       <c r="AB12" t="s">
-        <v>3931</v>
+        <v>4015</v>
       </c>
       <c r="AC12" t="s">
-        <v>3381</v>
+        <v>3999</v>
       </c>
       <c r="AD12" t="s">
-        <v>2020</v>
+        <v>4014</v>
       </c>
       <c r="AE12" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="AF12" t="s">
-        <v>1932</v>
+        <v>4029</v>
       </c>
       <c r="AG12" t="s">
-        <v>3667</v>
+        <v>4045</v>
       </c>
       <c r="AH12" t="s">
-        <v>3876</v>
+        <v>3046</v>
       </c>
       <c r="AI12" t="s">
-        <v>848</v>
+        <v>1192</v>
       </c>
       <c r="AJ12" t="s">
-        <v>3933</v>
+        <v>4047</v>
       </c>
       <c r="AK12" t="s">
-        <v>3932</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -16207,16 +16573,16 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
-        <v>3345</v>
+        <v>4050</v>
       </c>
       <c r="E13" t="s">
-        <v>3935</v>
+        <v>4049</v>
       </c>
       <c r="G13" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R13" t="s">
         <v>486</v>
@@ -16225,58 +16591,58 @@
         <v>265</v>
       </c>
       <c r="T13" t="s">
-        <v>3914</v>
+        <v>3986</v>
       </c>
       <c r="U13" t="s">
-        <v>3666</v>
+        <v>3046</v>
       </c>
       <c r="V13" t="s">
-        <v>1953</v>
+        <v>916</v>
       </c>
       <c r="W13" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="X13" t="s">
-        <v>1933</v>
+        <v>4048</v>
       </c>
       <c r="Y13" t="s">
-        <v>3934</v>
+        <v>3017</v>
       </c>
       <c r="Z13" t="s">
-        <v>2174</v>
+        <v>4006</v>
       </c>
       <c r="AA13" t="s">
-        <v>3908</v>
+        <v>3169</v>
       </c>
       <c r="AB13" t="s">
-        <v>3444</v>
+        <v>455</v>
       </c>
       <c r="AC13" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AD13" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AE13" t="s">
-        <v>1927</v>
+        <v>911</v>
       </c>
       <c r="AF13" t="s">
-        <v>1937</v>
+        <v>4000</v>
       </c>
       <c r="AG13" t="s">
-        <v>3716</v>
+        <v>3162</v>
       </c>
       <c r="AH13" t="s">
-        <v>3667</v>
+        <v>1171</v>
       </c>
       <c r="AI13" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="AJ13" t="s">
-        <v>3345</v>
+        <v>4050</v>
       </c>
       <c r="AK13" t="s">
-        <v>3935</v>
+        <v>4049</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -16287,16 +16653,16 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>3938</v>
+        <v>4053</v>
       </c>
       <c r="E14" t="s">
-        <v>3937</v>
+        <v>4052</v>
       </c>
       <c r="G14" t="s">
-        <v>880</v>
+        <v>680</v>
       </c>
       <c r="R14" t="s">
         <v>433</v>
@@ -16305,58 +16671,58 @@
         <v>770</v>
       </c>
       <c r="T14" t="s">
-        <v>555</v>
+        <v>911</v>
       </c>
       <c r="U14" t="s">
-        <v>1953</v>
+        <v>4048</v>
       </c>
       <c r="V14" t="s">
-        <v>3879</v>
+        <v>1195</v>
       </c>
       <c r="W14" t="s">
-        <v>3936</v>
+        <v>390</v>
       </c>
       <c r="X14" t="s">
+        <v>1171</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>3994</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>654</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>4051</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>4023</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>4015</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>673</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>2963</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>3252</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>4043</v>
+      </c>
+      <c r="AH14" t="s">
         <v>3220</v>
       </c>
-      <c r="Y14" t="s">
-        <v>2186</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>3730</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>1935</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>2079</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>3381</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>3876</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>3914</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>3644</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>3731</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>1933</v>
-      </c>
       <c r="AI14" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="AJ14" t="s">
-        <v>3938</v>
+        <v>4053</v>
       </c>
       <c r="AK14" t="s">
-        <v>3937</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -16367,16 +16733,16 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>759</v>
+        <v>262</v>
       </c>
       <c r="D15" t="s">
-        <v>3940</v>
+        <v>3783</v>
       </c>
       <c r="E15" t="s">
-        <v>3939</v>
+        <v>4056</v>
       </c>
       <c r="G15" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R15" t="s">
         <v>775</v>
@@ -16385,58 +16751,58 @@
         <v>774</v>
       </c>
       <c r="T15" t="s">
-        <v>555</v>
+        <v>4054</v>
       </c>
       <c r="U15" t="s">
-        <v>3062</v>
+        <v>4055</v>
       </c>
       <c r="V15" t="s">
-        <v>3905</v>
+        <v>3438</v>
       </c>
       <c r="W15" t="s">
-        <v>2228</v>
+        <v>3046</v>
       </c>
       <c r="X15" t="s">
-        <v>3908</v>
+        <v>1414</v>
       </c>
       <c r="Y15" t="s">
-        <v>2186</v>
+        <v>1897</v>
       </c>
       <c r="Z15" t="s">
+        <v>879</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>2883</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>722</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>3832</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>3988</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>3986</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>656</v>
+      </c>
+      <c r="AG15" t="s">
         <v>3835</v>
       </c>
-      <c r="AA15" t="s">
-        <v>2193</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>3730</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>2007</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>1899</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>3628</v>
-      </c>
       <c r="AH15" t="s">
-        <v>3666</v>
+        <v>3162</v>
       </c>
       <c r="AI15" t="s">
-        <v>759</v>
+        <v>262</v>
       </c>
       <c r="AJ15" t="s">
-        <v>3940</v>
+        <v>3783</v>
       </c>
       <c r="AK15" t="s">
-        <v>3939</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -16447,13 +16813,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>881</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
-        <v>3943</v>
+        <v>2136</v>
       </c>
       <c r="E16" t="s">
-        <v>3942</v>
+        <v>4057</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -16465,58 +16831,58 @@
         <v>270</v>
       </c>
       <c r="T16" t="s">
-        <v>1173</v>
+        <v>4004</v>
       </c>
       <c r="U16" t="s">
-        <v>3205</v>
+        <v>4032</v>
       </c>
       <c r="V16" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="W16" t="s">
-        <v>1936</v>
+        <v>2229</v>
       </c>
       <c r="X16" t="s">
-        <v>1929</v>
+        <v>2050</v>
       </c>
       <c r="Y16" t="s">
-        <v>3737</v>
+        <v>3457</v>
       </c>
       <c r="Z16" t="s">
-        <v>2187</v>
+        <v>2883</v>
       </c>
       <c r="AA16" t="s">
-        <v>3941</v>
+        <v>1281</v>
       </c>
       <c r="AB16" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AC16" t="s">
-        <v>2007</v>
+        <v>656</v>
       </c>
       <c r="AD16" t="s">
-        <v>3880</v>
+        <v>340</v>
       </c>
       <c r="AE16" t="s">
         <v>2266</v>
       </c>
       <c r="AF16" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="AG16" t="s">
         <v>665</v>
       </c>
       <c r="AH16" t="s">
-        <v>3920</v>
+        <v>661</v>
       </c>
       <c r="AI16" t="s">
-        <v>881</v>
+        <v>256</v>
       </c>
       <c r="AJ16" t="s">
-        <v>3943</v>
+        <v>2136</v>
       </c>
       <c r="AK16" t="s">
-        <v>3942</v>
+        <v>4057</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -16527,16 +16893,16 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>1197</v>
       </c>
       <c r="D17" t="s">
-        <v>3946</v>
+        <v>4059</v>
       </c>
       <c r="E17" t="s">
-        <v>3945</v>
+        <v>4058</v>
       </c>
       <c r="G17" t="s">
-        <v>426</v>
+        <v>880</v>
       </c>
       <c r="R17" t="s">
         <v>322</v>
@@ -16545,58 +16911,58 @@
         <v>272</v>
       </c>
       <c r="T17" t="s">
+        <v>3986</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1414</v>
+      </c>
+      <c r="V17" t="s">
+        <v>3881</v>
+      </c>
+      <c r="W17" t="s">
+        <v>1897</v>
+      </c>
+      <c r="X17" t="s">
+        <v>3157</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>4000</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>4006</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>3169</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>4007</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>3832</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>3988</v>
+      </c>
+      <c r="AE17" t="s">
         <v>2266</v>
       </c>
-      <c r="U17" t="s">
-        <v>3834</v>
-      </c>
-      <c r="V17" t="s">
-        <v>3920</v>
-      </c>
-      <c r="W17" t="s">
-        <v>3881</v>
-      </c>
-      <c r="X17" t="s">
-        <v>3905</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>2174</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>3908</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>3944</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>3381</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>1899</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>2035</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>1927</v>
-      </c>
       <c r="AF17" t="s">
-        <v>1932</v>
+        <v>661</v>
       </c>
       <c r="AG17" t="s">
-        <v>3667</v>
+        <v>3162</v>
       </c>
       <c r="AH17" t="s">
-        <v>3628</v>
+        <v>673</v>
       </c>
       <c r="AI17" t="s">
-        <v>246</v>
+        <v>1197</v>
       </c>
       <c r="AJ17" t="s">
-        <v>3946</v>
+        <v>4059</v>
       </c>
       <c r="AK17" t="s">
-        <v>3945</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -16607,16 +16973,16 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>745</v>
+        <v>1805</v>
       </c>
       <c r="D18" t="s">
-        <v>3366</v>
+        <v>4063</v>
       </c>
       <c r="E18" t="s">
-        <v>3947</v>
+        <v>4062</v>
       </c>
       <c r="G18" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R18" t="s">
         <v>501</v>
@@ -16625,58 +16991,58 @@
         <v>787</v>
       </c>
       <c r="T18" t="s">
-        <v>3914</v>
+        <v>3986</v>
       </c>
       <c r="U18" t="s">
-        <v>3746</v>
+        <v>4060</v>
       </c>
       <c r="V18" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="W18" t="s">
-        <v>3847</v>
+        <v>4048</v>
       </c>
       <c r="X18" t="s">
-        <v>1933</v>
+        <v>1414</v>
       </c>
       <c r="Y18" t="s">
-        <v>3867</v>
+        <v>4061</v>
       </c>
       <c r="Z18" t="s">
-        <v>2187</v>
+        <v>3169</v>
       </c>
       <c r="AA18" t="s">
-        <v>2186</v>
+        <v>2883</v>
       </c>
       <c r="AB18" t="s">
-        <v>3662</v>
+        <v>654</v>
       </c>
       <c r="AC18" t="s">
-        <v>2020</v>
+        <v>722</v>
       </c>
       <c r="AD18" t="s">
-        <v>2007</v>
+        <v>3988</v>
       </c>
       <c r="AE18" t="s">
-        <v>1927</v>
+        <v>911</v>
       </c>
       <c r="AF18" t="s">
-        <v>3667</v>
+        <v>665</v>
       </c>
       <c r="AG18" t="s">
-        <v>3628</v>
+        <v>656</v>
       </c>
       <c r="AH18" t="s">
         <v>786</v>
       </c>
       <c r="AI18" t="s">
-        <v>745</v>
+        <v>1805</v>
       </c>
       <c r="AJ18" t="s">
-        <v>3366</v>
+        <v>4063</v>
       </c>
       <c r="AK18" t="s">
-        <v>3947</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -16687,16 +17053,16 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>645</v>
+        <v>4008</v>
       </c>
       <c r="D19" t="s">
-        <v>3949</v>
+        <v>4067</v>
       </c>
       <c r="E19" t="s">
-        <v>3948</v>
+        <v>4066</v>
       </c>
       <c r="G19" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R19" t="s">
         <v>347</v>
@@ -16705,58 +17071,58 @@
         <v>792</v>
       </c>
       <c r="T19" t="s">
-        <v>555</v>
+        <v>4004</v>
       </c>
       <c r="U19" t="s">
-        <v>3905</v>
+        <v>390</v>
       </c>
       <c r="V19" t="s">
-        <v>1953</v>
+        <v>3438</v>
       </c>
       <c r="W19" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="X19" t="s">
-        <v>2174</v>
+        <v>3603</v>
       </c>
       <c r="Y19" t="s">
-        <v>2186</v>
+        <v>654</v>
       </c>
       <c r="Z19" t="s">
-        <v>2187</v>
+        <v>3169</v>
       </c>
       <c r="AA19" t="s">
-        <v>3908</v>
+        <v>4064</v>
       </c>
       <c r="AB19" t="s">
-        <v>3381</v>
+        <v>4006</v>
       </c>
       <c r="AC19" t="s">
-        <v>2020</v>
+        <v>3995</v>
       </c>
       <c r="AD19" t="s">
-        <v>3866</v>
+        <v>3999</v>
       </c>
       <c r="AE19" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="AF19" t="s">
-        <v>3442</v>
+        <v>4065</v>
       </c>
       <c r="AG19" t="s">
-        <v>3667</v>
+        <v>3989</v>
       </c>
       <c r="AH19" t="s">
-        <v>1936</v>
+        <v>3046</v>
       </c>
       <c r="AI19" t="s">
-        <v>645</v>
+        <v>4008</v>
       </c>
       <c r="AJ19" t="s">
-        <v>3949</v>
+        <v>4067</v>
       </c>
       <c r="AK19" t="s">
-        <v>3948</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -16767,16 +17133,16 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D20" t="s">
-        <v>3951</v>
+        <v>3592</v>
       </c>
       <c r="E20" t="s">
-        <v>3950</v>
+        <v>4071</v>
       </c>
       <c r="G20" t="s">
-        <v>426</v>
+        <v>627</v>
       </c>
       <c r="R20" t="s">
         <v>516</v>
@@ -16785,58 +17151,58 @@
         <v>796</v>
       </c>
       <c r="T20" t="s">
-        <v>555</v>
+        <v>4068</v>
       </c>
       <c r="U20" t="s">
-        <v>3656</v>
+        <v>4069</v>
       </c>
       <c r="V20" t="s">
-        <v>3816</v>
+        <v>3157</v>
       </c>
       <c r="W20" t="s">
-        <v>3905</v>
+        <v>3046</v>
       </c>
       <c r="X20" t="s">
-        <v>3934</v>
+        <v>3154</v>
       </c>
       <c r="Y20" t="s">
-        <v>2187</v>
+        <v>3017</v>
       </c>
       <c r="Z20" t="s">
-        <v>3908</v>
+        <v>654</v>
       </c>
       <c r="AA20" t="s">
-        <v>2174</v>
+        <v>4007</v>
       </c>
       <c r="AB20" t="s">
-        <v>3381</v>
+        <v>4014</v>
       </c>
       <c r="AC20" t="s">
-        <v>3876</v>
+        <v>4015</v>
       </c>
       <c r="AD20" t="s">
-        <v>2020</v>
+        <v>3995</v>
       </c>
       <c r="AE20" t="s">
-        <v>1806</v>
+        <v>4070</v>
       </c>
       <c r="AF20" t="s">
-        <v>1933</v>
+        <v>4048</v>
       </c>
       <c r="AG20" t="s">
-        <v>1937</v>
+        <v>4000</v>
       </c>
       <c r="AH20" t="s">
-        <v>3628</v>
+        <v>1164</v>
       </c>
       <c r="AI20" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="AJ20" t="s">
-        <v>3951</v>
+        <v>3592</v>
       </c>
       <c r="AK20" t="s">
-        <v>3950</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -16847,16 +17213,16 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>2004</v>
+        <v>1198</v>
       </c>
       <c r="D21" t="s">
-        <v>3953</v>
+        <v>4073</v>
       </c>
       <c r="E21" t="s">
-        <v>3952</v>
+        <v>4072</v>
       </c>
       <c r="G21" t="s">
-        <v>680</v>
+        <v>426</v>
       </c>
       <c r="R21" t="s">
         <v>375</v>
@@ -16865,58 +17231,58 @@
         <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>555</v>
+        <v>911</v>
       </c>
       <c r="U21" t="s">
-        <v>3905</v>
+        <v>1414</v>
       </c>
       <c r="V21" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="W21" t="s">
         <v>3881</v>
       </c>
       <c r="X21" t="s">
-        <v>2186</v>
+        <v>4048</v>
       </c>
       <c r="Y21" t="s">
-        <v>3908</v>
+        <v>654</v>
       </c>
       <c r="Z21" t="s">
-        <v>3906</v>
+        <v>3169</v>
       </c>
       <c r="AA21" t="s">
-        <v>2187</v>
+        <v>4006</v>
       </c>
       <c r="AB21" t="s">
-        <v>665</v>
+        <v>3017</v>
       </c>
       <c r="AC21" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AD21" t="s">
-        <v>3866</v>
+        <v>4001</v>
       </c>
       <c r="AE21" t="s">
-        <v>3914</v>
+        <v>2963</v>
       </c>
       <c r="AF21" t="s">
-        <v>3628</v>
+        <v>1897</v>
       </c>
       <c r="AG21" t="s">
-        <v>1933</v>
+        <v>3162</v>
       </c>
       <c r="AH21" t="s">
-        <v>3277</v>
+        <v>3252</v>
       </c>
       <c r="AI21" t="s">
-        <v>2004</v>
+        <v>1198</v>
       </c>
       <c r="AJ21" t="s">
-        <v>3953</v>
+        <v>4073</v>
       </c>
       <c r="AK21" t="s">
-        <v>3952</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -16927,13 +17293,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>252</v>
+        <v>4075</v>
       </c>
       <c r="D22" t="s">
-        <v>3956</v>
+        <v>4077</v>
       </c>
       <c r="E22" t="s">
-        <v>3955</v>
+        <v>4076</v>
       </c>
       <c r="G22" t="s">
         <v>627</v>
@@ -16945,58 +17311,58 @@
         <v>804</v>
       </c>
       <c r="T22" t="s">
-        <v>3863</v>
+        <v>4070</v>
       </c>
       <c r="U22" t="s">
-        <v>3874</v>
+        <v>1414</v>
       </c>
       <c r="V22" t="s">
-        <v>3905</v>
+        <v>3997</v>
       </c>
       <c r="W22" t="s">
-        <v>3746</v>
+        <v>4074</v>
       </c>
       <c r="X22" t="s">
-        <v>3730</v>
+        <v>3438</v>
       </c>
       <c r="Y22" t="s">
-        <v>2187</v>
+        <v>654</v>
       </c>
       <c r="Z22" t="s">
-        <v>3865</v>
+        <v>3169</v>
       </c>
       <c r="AA22" t="s">
-        <v>3906</v>
+        <v>4007</v>
       </c>
       <c r="AB22" t="s">
-        <v>2079</v>
+        <v>3998</v>
       </c>
       <c r="AC22" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AD22" t="s">
-        <v>3866</v>
+        <v>4015</v>
       </c>
       <c r="AE22" t="s">
-        <v>3914</v>
+        <v>3986</v>
       </c>
       <c r="AF22" t="s">
-        <v>3954</v>
+        <v>4032</v>
       </c>
       <c r="AG22" t="s">
-        <v>3855</v>
+        <v>4000</v>
       </c>
       <c r="AH22" t="s">
-        <v>2184</v>
+        <v>802</v>
       </c>
       <c r="AI22" t="s">
-        <v>252</v>
+        <v>4075</v>
       </c>
       <c r="AJ22" t="s">
-        <v>3956</v>
+        <v>4077</v>
       </c>
       <c r="AK22" t="s">
-        <v>3955</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -17007,16 +17373,16 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>818</v>
+        <v>244</v>
       </c>
       <c r="D23" t="s">
-        <v>3958</v>
+        <v>4081</v>
       </c>
       <c r="E23" t="s">
-        <v>3957</v>
+        <v>4080</v>
       </c>
       <c r="G23" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="R23" t="s">
         <v>809</v>
@@ -17025,58 +17391,58 @@
         <v>281</v>
       </c>
       <c r="T23" t="s">
-        <v>3762</v>
+        <v>4078</v>
       </c>
       <c r="U23" t="s">
-        <v>1953</v>
+        <v>1171</v>
       </c>
       <c r="V23" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="W23" t="s">
-        <v>1348</v>
+        <v>2140</v>
       </c>
       <c r="X23" t="s">
-        <v>3908</v>
+        <v>3162</v>
       </c>
       <c r="Y23" t="s">
-        <v>2187</v>
+        <v>2883</v>
       </c>
       <c r="Z23" t="s">
-        <v>3923</v>
+        <v>4079</v>
       </c>
       <c r="AA23" t="s">
-        <v>3882</v>
+        <v>3354</v>
       </c>
       <c r="AB23" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AC23" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AD23" t="s">
-        <v>3765</v>
+        <v>1719</v>
       </c>
       <c r="AE23" t="s">
         <v>3877</v>
       </c>
       <c r="AF23" t="s">
-        <v>1930</v>
+        <v>3989</v>
       </c>
       <c r="AG23" t="s">
-        <v>1937</v>
+        <v>4000</v>
       </c>
       <c r="AH23" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="AI23" t="s">
-        <v>818</v>
+        <v>244</v>
       </c>
       <c r="AJ23" t="s">
-        <v>3958</v>
+        <v>4081</v>
       </c>
       <c r="AK23" t="s">
-        <v>3957</v>
+        <v>4080</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -17087,13 +17453,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="D24" t="s">
-        <v>3611</v>
+        <v>4086</v>
       </c>
       <c r="E24" t="s">
-        <v>3960</v>
+        <v>4085</v>
       </c>
       <c r="G24" t="s">
         <v>426</v>
@@ -17105,58 +17471,58 @@
         <v>283</v>
       </c>
       <c r="T24" t="s">
-        <v>3914</v>
+        <v>3519</v>
       </c>
       <c r="U24" t="s">
-        <v>2016</v>
+        <v>1414</v>
       </c>
       <c r="V24" t="s">
-        <v>3883</v>
+        <v>3881</v>
       </c>
       <c r="W24" t="s">
-        <v>3881</v>
+        <v>3200</v>
       </c>
       <c r="X24" t="s">
-        <v>3926</v>
+        <v>711</v>
       </c>
       <c r="Y24" t="s">
-        <v>3959</v>
+        <v>3603</v>
       </c>
       <c r="Z24" t="s">
-        <v>3872</v>
+        <v>3169</v>
       </c>
       <c r="AA24" t="s">
-        <v>3730</v>
+        <v>722</v>
       </c>
       <c r="AB24" t="s">
-        <v>3866</v>
+        <v>4082</v>
       </c>
       <c r="AC24" t="s">
-        <v>2079</v>
+        <v>4083</v>
       </c>
       <c r="AD24" t="s">
-        <v>2020</v>
+        <v>3988</v>
       </c>
       <c r="AE24" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="AF24" t="s">
-        <v>3860</v>
+        <v>4084</v>
       </c>
       <c r="AG24" t="s">
-        <v>3667</v>
+        <v>1342</v>
       </c>
       <c r="AH24" t="s">
-        <v>3628</v>
+        <v>3483</v>
       </c>
       <c r="AI24" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="AJ24" t="s">
-        <v>3611</v>
+        <v>4086</v>
       </c>
       <c r="AK24" t="s">
-        <v>3960</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -17167,13 +17533,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>2933</v>
+        <v>1886</v>
       </c>
       <c r="D25" t="s">
-        <v>3963</v>
+        <v>4088</v>
       </c>
       <c r="E25" t="s">
-        <v>3962</v>
+        <v>4087</v>
       </c>
       <c r="G25" t="s">
         <v>627</v>
@@ -17185,19 +17551,19 @@
         <v>461</v>
       </c>
       <c r="T25" t="s">
-        <v>2986</v>
+        <v>4054</v>
       </c>
       <c r="U25" t="s">
-        <v>2928</v>
+        <v>3438</v>
       </c>
       <c r="V25" t="s">
-        <v>2927</v>
+        <v>681</v>
       </c>
       <c r="W25" t="s">
-        <v>3920</v>
+        <v>661</v>
       </c>
       <c r="X25" t="s">
-        <v>2001</v>
+        <v>2840</v>
       </c>
       <c r="Y25" t="s">
         <v>1138</v>
@@ -17206,37 +17572,37 @@
         <v>1940</v>
       </c>
       <c r="AA25" t="s">
-        <v>3906</v>
+        <v>3017</v>
       </c>
       <c r="AB25" t="s">
-        <v>3961</v>
+        <v>4025</v>
       </c>
       <c r="AC25" t="s">
-        <v>2007</v>
+        <v>656</v>
       </c>
       <c r="AD25" t="s">
-        <v>3257</v>
+        <v>2234</v>
       </c>
       <c r="AE25" t="s">
-        <v>3914</v>
+        <v>911</v>
       </c>
       <c r="AF25" t="s">
-        <v>1348</v>
+        <v>2140</v>
       </c>
       <c r="AG25" t="s">
-        <v>3687</v>
+        <v>724</v>
       </c>
       <c r="AH25" t="s">
-        <v>1336</v>
+        <v>725</v>
       </c>
       <c r="AI25" t="s">
-        <v>2933</v>
+        <v>1886</v>
       </c>
       <c r="AJ25" t="s">
-        <v>3963</v>
+        <v>4088</v>
       </c>
       <c r="AK25" t="s">
-        <v>3962</v>
+        <v>4087</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -17247,16 +17613,16 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>2004</v>
+        <v>4036</v>
       </c>
       <c r="D26" t="s">
-        <v>3968</v>
+        <v>4090</v>
       </c>
       <c r="E26" t="s">
-        <v>3967</v>
+        <v>4089</v>
       </c>
       <c r="G26" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R26" t="s">
         <v>569</v>
@@ -17265,58 +17631,58 @@
         <v>572</v>
       </c>
       <c r="T26" t="s">
-        <v>3863</v>
+        <v>3986</v>
       </c>
       <c r="U26" t="s">
-        <v>3864</v>
+        <v>1414</v>
       </c>
       <c r="V26" t="s">
-        <v>3964</v>
+        <v>4005</v>
       </c>
       <c r="W26" t="s">
-        <v>3905</v>
+        <v>4074</v>
       </c>
       <c r="X26" t="s">
-        <v>3911</v>
+        <v>3998</v>
       </c>
       <c r="Y26" t="s">
-        <v>2187</v>
+        <v>654</v>
       </c>
       <c r="Z26" t="s">
-        <v>3965</v>
+        <v>3154</v>
       </c>
       <c r="AA26" t="s">
-        <v>3906</v>
+        <v>4000</v>
       </c>
       <c r="AB26" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AC26" t="s">
-        <v>3876</v>
+        <v>4025</v>
       </c>
       <c r="AD26" t="s">
-        <v>2079</v>
+        <v>3832</v>
       </c>
       <c r="AE26" t="s">
-        <v>3780</v>
+        <v>3991</v>
       </c>
       <c r="AF26" t="s">
-        <v>3687</v>
+        <v>916</v>
       </c>
       <c r="AG26" t="s">
-        <v>3656</v>
+        <v>3989</v>
       </c>
       <c r="AH26" t="s">
-        <v>3966</v>
+        <v>3162</v>
       </c>
       <c r="AI26" t="s">
-        <v>2004</v>
+        <v>4036</v>
       </c>
       <c r="AJ26" t="s">
-        <v>3968</v>
+        <v>4090</v>
       </c>
       <c r="AK26" t="s">
-        <v>3967</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -17327,13 +17693,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>262</v>
+        <v>4026</v>
       </c>
       <c r="D27" t="s">
-        <v>3971</v>
+        <v>4093</v>
       </c>
       <c r="E27" t="s">
-        <v>3970</v>
+        <v>4092</v>
       </c>
       <c r="G27" t="s">
         <v>627</v>
@@ -17345,58 +17711,58 @@
         <v>827</v>
       </c>
       <c r="T27" t="s">
-        <v>3526</v>
+        <v>4004</v>
       </c>
       <c r="U27" t="s">
-        <v>3905</v>
+        <v>3438</v>
       </c>
       <c r="V27" t="s">
-        <v>3874</v>
+        <v>3881</v>
       </c>
       <c r="W27" t="s">
-        <v>3834</v>
+        <v>3992</v>
       </c>
       <c r="X27" t="s">
-        <v>3911</v>
+        <v>4069</v>
       </c>
       <c r="Y27" t="s">
-        <v>1935</v>
+        <v>4006</v>
       </c>
       <c r="Z27" t="s">
-        <v>2187</v>
+        <v>4091</v>
       </c>
       <c r="AA27" t="s">
-        <v>3906</v>
+        <v>3169</v>
       </c>
       <c r="AB27" t="s">
-        <v>1967</v>
+        <v>654</v>
       </c>
       <c r="AC27" t="s">
-        <v>3866</v>
+        <v>4025</v>
       </c>
       <c r="AD27" t="s">
-        <v>2079</v>
+        <v>3999</v>
       </c>
       <c r="AE27" t="s">
-        <v>3784</v>
+        <v>4070</v>
       </c>
       <c r="AF27" t="s">
-        <v>3969</v>
+        <v>3017</v>
       </c>
       <c r="AG27" t="s">
-        <v>3637</v>
+        <v>1414</v>
       </c>
       <c r="AH27" t="s">
-        <v>3687</v>
+        <v>4001</v>
       </c>
       <c r="AI27" t="s">
-        <v>262</v>
+        <v>4026</v>
       </c>
       <c r="AJ27" t="s">
-        <v>3971</v>
+        <v>4093</v>
       </c>
       <c r="AK27" t="s">
-        <v>3970</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -17407,16 +17773,16 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>745</v>
+        <v>3571</v>
       </c>
       <c r="D28" t="s">
-        <v>3933</v>
+        <v>4095</v>
       </c>
       <c r="E28" t="s">
-        <v>3972</v>
+        <v>4094</v>
       </c>
       <c r="G28" t="s">
-        <v>627</v>
+        <v>3415</v>
       </c>
       <c r="R28" t="s">
         <v>832</v>
@@ -17425,58 +17791,58 @@
         <v>831</v>
       </c>
       <c r="T28" t="s">
-        <v>2266</v>
+        <v>4070</v>
       </c>
       <c r="U28" t="s">
-        <v>3905</v>
+        <v>1897</v>
       </c>
       <c r="V28" t="s">
         <v>3881</v>
       </c>
       <c r="W28" t="s">
-        <v>3917</v>
+        <v>3987</v>
       </c>
       <c r="X28" t="s">
-        <v>2184</v>
+        <v>3998</v>
       </c>
       <c r="Y28" t="s">
-        <v>3906</v>
+        <v>3017</v>
       </c>
       <c r="Z28" t="s">
-        <v>2186</v>
+        <v>879</v>
       </c>
       <c r="AA28" t="s">
-        <v>3908</v>
+        <v>3169</v>
       </c>
       <c r="AB28" t="s">
-        <v>3961</v>
+        <v>4025</v>
       </c>
       <c r="AC28" t="s">
-        <v>3866</v>
+        <v>4001</v>
       </c>
       <c r="AD28" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AE28" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="AF28" t="s">
-        <v>3666</v>
+        <v>3046</v>
       </c>
       <c r="AG28" t="s">
-        <v>3628</v>
+        <v>4011</v>
       </c>
       <c r="AH28" t="s">
-        <v>3667</v>
+        <v>4023</v>
       </c>
       <c r="AI28" t="s">
-        <v>745</v>
+        <v>3571</v>
       </c>
       <c r="AJ28" t="s">
-        <v>3933</v>
+        <v>4095</v>
       </c>
       <c r="AK28" t="s">
-        <v>3972</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -17487,16 +17853,16 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>3054</v>
+        <v>1183</v>
       </c>
       <c r="D29" t="s">
-        <v>3975</v>
+        <v>4098</v>
       </c>
       <c r="E29" t="s">
-        <v>3974</v>
+        <v>4097</v>
       </c>
       <c r="G29" t="s">
-        <v>627</v>
+        <v>426</v>
       </c>
       <c r="R29" t="s">
         <v>837</v>
@@ -17505,58 +17871,58 @@
         <v>836</v>
       </c>
       <c r="T29" t="s">
-        <v>3863</v>
+        <v>911</v>
       </c>
       <c r="U29" t="s">
-        <v>3637</v>
+        <v>4048</v>
       </c>
       <c r="V29" t="s">
-        <v>3905</v>
+        <v>3987</v>
       </c>
       <c r="W29" t="s">
-        <v>3973</v>
+        <v>1414</v>
       </c>
       <c r="X29" t="s">
-        <v>3874</v>
+        <v>3169</v>
       </c>
       <c r="Y29" t="s">
-        <v>1935</v>
+        <v>3503</v>
       </c>
       <c r="Z29" t="s">
-        <v>3923</v>
+        <v>3998</v>
       </c>
       <c r="AA29" t="s">
-        <v>3906</v>
+        <v>3994</v>
       </c>
       <c r="AB29" t="s">
-        <v>2021</v>
+        <v>3999</v>
       </c>
       <c r="AC29" t="s">
-        <v>3876</v>
+        <v>4096</v>
       </c>
       <c r="AD29" t="s">
-        <v>1967</v>
+        <v>4025</v>
       </c>
       <c r="AE29" t="s">
-        <v>3914</v>
+        <v>2963</v>
       </c>
       <c r="AF29" t="s">
-        <v>3893</v>
+        <v>1897</v>
       </c>
       <c r="AG29" t="s">
-        <v>3894</v>
+        <v>3162</v>
       </c>
       <c r="AH29" t="s">
-        <v>3656</v>
+        <v>1960</v>
       </c>
       <c r="AI29" t="s">
-        <v>3054</v>
+        <v>1183</v>
       </c>
       <c r="AJ29" t="s">
-        <v>3975</v>
+        <v>4098</v>
       </c>
       <c r="AK29" t="s">
-        <v>3974</v>
+        <v>4097</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -17567,16 +17933,16 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>290</v>
+        <v>3568</v>
       </c>
       <c r="D30" t="s">
-        <v>3978</v>
+        <v>4100</v>
       </c>
       <c r="E30" t="s">
-        <v>3977</v>
+        <v>4099</v>
       </c>
       <c r="G30" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R30" t="s">
         <v>840</v>
@@ -17585,58 +17951,58 @@
         <v>289</v>
       </c>
       <c r="T30" t="s">
-        <v>3863</v>
+        <v>911</v>
       </c>
       <c r="U30" t="s">
-        <v>3976</v>
+        <v>3992</v>
       </c>
       <c r="V30" t="s">
-        <v>3905</v>
+        <v>3438</v>
       </c>
       <c r="W30" t="s">
-        <v>3874</v>
+        <v>1414</v>
       </c>
       <c r="X30" t="s">
-        <v>3911</v>
+        <v>4048</v>
       </c>
       <c r="Y30" t="s">
-        <v>1935</v>
+        <v>4000</v>
       </c>
       <c r="Z30" t="s">
-        <v>3865</v>
+        <v>4006</v>
       </c>
       <c r="AA30" t="s">
-        <v>3934</v>
+        <v>654</v>
       </c>
       <c r="AB30" t="s">
-        <v>1967</v>
+        <v>3169</v>
       </c>
       <c r="AC30" t="s">
-        <v>3876</v>
+        <v>4025</v>
       </c>
       <c r="AD30" t="s">
-        <v>2079</v>
+        <v>4015</v>
       </c>
       <c r="AE30" t="s">
-        <v>891</v>
+        <v>3986</v>
       </c>
       <c r="AF30" t="s">
-        <v>1700</v>
+        <v>3998</v>
       </c>
       <c r="AG30" t="s">
-        <v>3746</v>
+        <v>3999</v>
       </c>
       <c r="AH30" t="s">
-        <v>3687</v>
+        <v>390</v>
       </c>
       <c r="AI30" t="s">
-        <v>290</v>
+        <v>3568</v>
       </c>
       <c r="AJ30" t="s">
-        <v>3978</v>
+        <v>4100</v>
       </c>
       <c r="AK30" t="s">
-        <v>3977</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -17647,16 +18013,16 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>677</v>
+        <v>1285</v>
       </c>
       <c r="D31" t="s">
-        <v>3980</v>
+        <v>4103</v>
       </c>
       <c r="E31" t="s">
-        <v>3979</v>
+        <v>4102</v>
       </c>
       <c r="G31" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="R31" t="s">
         <v>844</v>
@@ -17665,58 +18031,58 @@
         <v>843</v>
       </c>
       <c r="T31" t="s">
-        <v>3526</v>
+        <v>911</v>
       </c>
       <c r="U31" t="s">
-        <v>3864</v>
+        <v>3881</v>
       </c>
       <c r="V31" t="s">
-        <v>3874</v>
+        <v>4101</v>
       </c>
       <c r="W31" t="s">
-        <v>3905</v>
+        <v>1414</v>
       </c>
       <c r="X31" t="s">
-        <v>2187</v>
+        <v>3200</v>
       </c>
       <c r="Y31" t="s">
-        <v>3906</v>
+        <v>3169</v>
       </c>
       <c r="Z31" t="s">
-        <v>3944</v>
+        <v>3017</v>
       </c>
       <c r="AA31" t="s">
-        <v>1935</v>
+        <v>4023</v>
       </c>
       <c r="AB31" t="s">
-        <v>2079</v>
+        <v>654</v>
       </c>
       <c r="AC31" t="s">
-        <v>1967</v>
+        <v>3999</v>
       </c>
       <c r="AD31" t="s">
-        <v>3866</v>
+        <v>4025</v>
       </c>
       <c r="AE31" t="s">
-        <v>891</v>
+        <v>3986</v>
       </c>
       <c r="AF31" t="s">
-        <v>3746</v>
+        <v>4001</v>
       </c>
       <c r="AG31" t="s">
-        <v>3220</v>
+        <v>3998</v>
       </c>
       <c r="AH31" t="s">
-        <v>3687</v>
+        <v>3989</v>
       </c>
       <c r="AI31" t="s">
-        <v>677</v>
+        <v>1285</v>
       </c>
       <c r="AJ31" t="s">
-        <v>3980</v>
+        <v>4103</v>
       </c>
       <c r="AK31" t="s">
-        <v>3979</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -17727,16 +18093,16 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>752</v>
+        <v>1318</v>
       </c>
       <c r="D32" t="s">
-        <v>3983</v>
+        <v>4105</v>
       </c>
       <c r="E32" t="s">
-        <v>3982</v>
+        <v>4104</v>
       </c>
       <c r="G32" t="s">
-        <v>426</v>
+        <v>880</v>
       </c>
       <c r="R32" t="s">
         <v>494</v>
@@ -17745,58 +18111,58 @@
         <v>849</v>
       </c>
       <c r="T32" t="s">
-        <v>3526</v>
+        <v>4068</v>
       </c>
       <c r="U32" t="s">
-        <v>3871</v>
+        <v>4005</v>
       </c>
       <c r="V32" t="s">
-        <v>3628</v>
+        <v>1414</v>
       </c>
       <c r="W32" t="s">
-        <v>3874</v>
+        <v>4048</v>
       </c>
       <c r="X32" t="s">
-        <v>3908</v>
+        <v>4000</v>
       </c>
       <c r="Y32" t="s">
-        <v>3981</v>
+        <v>654</v>
       </c>
       <c r="Z32" t="s">
-        <v>3906</v>
+        <v>3169</v>
       </c>
       <c r="AA32" t="s">
-        <v>2174</v>
+        <v>3017</v>
       </c>
       <c r="AB32" t="s">
-        <v>3866</v>
+        <v>4006</v>
       </c>
       <c r="AC32" t="s">
-        <v>3645</v>
+        <v>3995</v>
       </c>
       <c r="AD32" t="s">
-        <v>3961</v>
+        <v>4025</v>
       </c>
       <c r="AE32" t="s">
-        <v>1927</v>
+        <v>3986</v>
       </c>
       <c r="AF32" t="s">
-        <v>3667</v>
+        <v>3420</v>
       </c>
       <c r="AG32" t="s">
-        <v>3731</v>
+        <v>3252</v>
       </c>
       <c r="AH32" t="s">
-        <v>1933</v>
+        <v>1195</v>
       </c>
       <c r="AI32" t="s">
-        <v>752</v>
+        <v>1318</v>
       </c>
       <c r="AJ32" t="s">
-        <v>3983</v>
+        <v>4105</v>
       </c>
       <c r="AK32" t="s">
-        <v>3982</v>
+        <v>4104</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -17807,13 +18173,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>1485</v>
+        <v>290</v>
       </c>
       <c r="D33" t="s">
-        <v>3985</v>
+        <v>4107</v>
       </c>
       <c r="E33" t="s">
-        <v>3984</v>
+        <v>4106</v>
       </c>
       <c r="G33" t="s">
         <v>426</v>
@@ -17825,58 +18191,58 @@
         <v>241</v>
       </c>
       <c r="T33" t="s">
-        <v>3914</v>
+        <v>911</v>
       </c>
       <c r="U33" t="s">
         <v>3881</v>
       </c>
       <c r="V33" t="s">
-        <v>3905</v>
+        <v>1414</v>
       </c>
       <c r="W33" t="s">
-        <v>3637</v>
+        <v>3157</v>
       </c>
       <c r="X33" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>3169</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>879</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>3017</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>4000</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>3988</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>4025</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>3986</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>1897</v>
+      </c>
+      <c r="AG33" t="s">
         <v>665</v>
       </c>
-      <c r="Y33" t="s">
-        <v>3906</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>2187</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>3908</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>3961</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>3866</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>1927</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>2927</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>1937</v>
-      </c>
       <c r="AH33" t="s">
-        <v>3628</v>
+        <v>3252</v>
       </c>
       <c r="AI33" t="s">
-        <v>1485</v>
+        <v>290</v>
       </c>
       <c r="AJ33" t="s">
-        <v>3985</v>
+        <v>4107</v>
       </c>
       <c r="AK33" t="s">
-        <v>3984</v>
+        <v>4106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gw 35 done fpl
</commit_message>
<xml_diff>
--- a/EdisonLogs/weather.xlsx
+++ b/EdisonLogs/weather.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12189" uniqueCount="3141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13789" uniqueCount="3291">
   <si>
     <t>Places</t>
   </si>
@@ -9457,6 +9457,456 @@
   </si>
   <si>
     <t>2266</t>
+  </si>
+  <si>
+    <t>Ramsdale 2</t>
+  </si>
+  <si>
+    <t>James 2</t>
+  </si>
+  <si>
+    <t>Son 19</t>
+  </si>
+  <si>
+    <t>White 0</t>
+  </si>
+  <si>
+    <t>2,589,841</t>
+  </si>
+  <si>
+    <t>1839</t>
+  </si>
+  <si>
+    <t>Son 38$ captain</t>
+  </si>
+  <si>
+    <t>Saka 4</t>
+  </si>
+  <si>
+    <t>Kane 6</t>
+  </si>
+  <si>
+    <t>2,806,176</t>
+  </si>
+  <si>
+    <t>1819</t>
+  </si>
+  <si>
+    <t>Kane 12$ captain</t>
+  </si>
+  <si>
+    <t>278,882</t>
+  </si>
+  <si>
+    <t>2169</t>
+  </si>
+  <si>
+    <t>393,160</t>
+  </si>
+  <si>
+    <t>Elanga 6</t>
+  </si>
+  <si>
+    <t>582,621</t>
+  </si>
+  <si>
+    <t>2089</t>
+  </si>
+  <si>
+    <t>Bowen 6</t>
+  </si>
+  <si>
+    <t>Ronaldo 7</t>
+  </si>
+  <si>
+    <t>4,270,412</t>
+  </si>
+  <si>
+    <t>1690</t>
+  </si>
+  <si>
+    <t>Martinelli 6</t>
+  </si>
+  <si>
+    <t>Richarlison 8</t>
+  </si>
+  <si>
+    <t>Pinnock 0</t>
+  </si>
+  <si>
+    <t>218,791</t>
+  </si>
+  <si>
+    <t>2192</t>
+  </si>
+  <si>
+    <t>Ajer 1</t>
+  </si>
+  <si>
+    <t>Rüdiger 1</t>
+  </si>
+  <si>
+    <t>Kulusevski 8</t>
+  </si>
+  <si>
+    <t>Nketiah 1</t>
+  </si>
+  <si>
+    <t>1,673,239</t>
+  </si>
+  <si>
+    <t>1932</t>
+  </si>
+  <si>
+    <t>Gabriel 11</t>
+  </si>
+  <si>
+    <t>Werner 2</t>
+  </si>
+  <si>
+    <t>1,253,990</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>Gray 14$ captain</t>
+  </si>
+  <si>
+    <t>776,468</t>
+  </si>
+  <si>
+    <t>2052</t>
+  </si>
+  <si>
+    <t>Ronaldo 14$ captain</t>
+  </si>
+  <si>
+    <t>Dalot 6</t>
+  </si>
+  <si>
+    <t>450,880</t>
+  </si>
+  <si>
+    <t>2119</t>
+  </si>
+  <si>
+    <t>361,665</t>
+  </si>
+  <si>
+    <t>2143</t>
+  </si>
+  <si>
+    <t>de Gea 7</t>
+  </si>
+  <si>
+    <t>Fernandes 16$ captain</t>
+  </si>
+  <si>
+    <t>1,011,753</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>518,671</t>
+  </si>
+  <si>
+    <t>2103</t>
+  </si>
+  <si>
+    <t>Tomiyasu 2</t>
+  </si>
+  <si>
+    <t>Soucek 1</t>
+  </si>
+  <si>
+    <t>Fernandes 8</t>
+  </si>
+  <si>
+    <t>2,612,718</t>
+  </si>
+  <si>
+    <t>1837</t>
+  </si>
+  <si>
+    <t>1,173,696</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>998,523</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>59,799</t>
+  </si>
+  <si>
+    <t>2284</t>
+  </si>
+  <si>
+    <t>Son 38</t>
+  </si>
+  <si>
+    <t>188,478</t>
+  </si>
+  <si>
+    <t>31,603</t>
+  </si>
+  <si>
+    <t>2317</t>
+  </si>
+  <si>
+    <t>111,172</t>
+  </si>
+  <si>
+    <t>2245</t>
+  </si>
+  <si>
+    <t>Cancelo 10</t>
+  </si>
+  <si>
+    <t>760,556</t>
+  </si>
+  <si>
+    <t>2055</t>
+  </si>
+  <si>
+    <t>307,735</t>
+  </si>
+  <si>
+    <t>Mendy 3</t>
+  </si>
+  <si>
+    <t>7,289,583</t>
+  </si>
+  <si>
+    <t>1377</t>
+  </si>
+  <si>
+    <t>279,220</t>
+  </si>
+  <si>
+    <t>31,347</t>
+  </si>
+  <si>
+    <t>2318</t>
+  </si>
+  <si>
+    <t>Ramsdale View player information</t>
+  </si>
+  <si>
+    <t>James View player information</t>
+  </si>
+  <si>
+    <t>292,522</t>
+  </si>
+  <si>
+    <t>2165</t>
+  </si>
+  <si>
+    <t>137,266</t>
+  </si>
+  <si>
+    <t>2230</t>
+  </si>
+  <si>
+    <t>11,626</t>
+  </si>
+  <si>
+    <t>2360</t>
+  </si>
+  <si>
+    <t>114,620</t>
+  </si>
+  <si>
+    <t>2243</t>
+  </si>
+  <si>
+    <t>135,609</t>
+  </si>
+  <si>
+    <t>2231</t>
+  </si>
+  <si>
+    <t>72,234</t>
+  </si>
+  <si>
+    <t>2,624,422</t>
+  </si>
+  <si>
+    <t>1842</t>
+  </si>
+  <si>
+    <t>2,777,375</t>
+  </si>
+  <si>
+    <t>1828</t>
+  </si>
+  <si>
+    <t>295,953</t>
+  </si>
+  <si>
+    <t>2167</t>
+  </si>
+  <si>
+    <t>357,664</t>
+  </si>
+  <si>
+    <t>2148</t>
+  </si>
+  <si>
+    <t>603,750</t>
+  </si>
+  <si>
+    <t>4,293,673</t>
+  </si>
+  <si>
+    <t>1695</t>
+  </si>
+  <si>
+    <t>237,691</t>
+  </si>
+  <si>
+    <t>2188</t>
+  </si>
+  <si>
+    <t>1,678,009</t>
+  </si>
+  <si>
+    <t>1937</t>
+  </si>
+  <si>
+    <t>1,216,757</t>
+  </si>
+  <si>
+    <t>767,915</t>
+  </si>
+  <si>
+    <t>2059</t>
+  </si>
+  <si>
+    <t>492,465</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>329,946</t>
+  </si>
+  <si>
+    <t>2157</t>
+  </si>
+  <si>
+    <t>1,053,889</t>
+  </si>
+  <si>
+    <t>584,492</t>
+  </si>
+  <si>
+    <t>2094</t>
+  </si>
+  <si>
+    <t>2,577,490</t>
+  </si>
+  <si>
+    <t>1848</t>
+  </si>
+  <si>
+    <t>1,189,859</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1,005,223</t>
+  </si>
+  <si>
+    <t>65,238</t>
+  </si>
+  <si>
+    <t>2282</t>
+  </si>
+  <si>
+    <t>190,141</t>
+  </si>
+  <si>
+    <t>2208</t>
+  </si>
+  <si>
+    <t>31,430</t>
+  </si>
+  <si>
+    <t>2320</t>
+  </si>
+  <si>
+    <t>119,984</t>
+  </si>
+  <si>
+    <t>763,712</t>
+  </si>
+  <si>
+    <t>2060</t>
+  </si>
+  <si>
+    <t>305,490</t>
+  </si>
+  <si>
+    <t>7,328,562</t>
+  </si>
+  <si>
+    <t>1382</t>
+  </si>
+  <si>
+    <t>301,099</t>
+  </si>
+  <si>
+    <t>2166</t>
+  </si>
+  <si>
+    <t>33,259</t>
+  </si>
+  <si>
+    <t>305,689</t>
+  </si>
+  <si>
+    <t>134,342</t>
+  </si>
+  <si>
+    <t>2235</t>
+  </si>
+  <si>
+    <t>13,334</t>
+  </si>
+  <si>
+    <t>2357</t>
+  </si>
+  <si>
+    <t>107,103</t>
+  </si>
+  <si>
+    <t>2251</t>
+  </si>
+  <si>
+    <t>145,991</t>
+  </si>
+  <si>
+    <t>2229</t>
+  </si>
+  <si>
+    <t>Foster View player information</t>
+  </si>
+  <si>
+    <t>Cancelo View player information</t>
+  </si>
+  <si>
+    <t>64,199</t>
+  </si>
+  <si>
+    <t>2283</t>
   </si>
 </sst>
 </file>
@@ -12651,21 +13101,21 @@
     <col min="8" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.015625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="21.43359375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="27.69921875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.04296875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="25.75390625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="17.55078125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.0546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="29.3125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="18.0546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.9375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.04296875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="16.171875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="21.31640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="19.0546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="22.5859375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.35546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="18.39453125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="23.96484375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="4.11328125" collapsed="true"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.94140625" collapsed="true"/>
@@ -12792,13 +13242,13 @@
         <v>2438499</v>
       </c>
       <c r="C2" t="s">
-        <v>1933</v>
+        <v>886</v>
       </c>
       <c r="D2" t="s">
-        <v>3009</v>
+        <v>3234</v>
       </c>
       <c r="E2" t="s">
-        <v>3008</v>
+        <v>3233</v>
       </c>
       <c r="G2" t="s">
         <v>627</v>
@@ -12810,22 +13260,22 @@
         <v>243</v>
       </c>
       <c r="T2" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U2" t="s">
         <v>658</v>
       </c>
       <c r="V2" t="s">
-        <v>2863</v>
+        <v>3142</v>
       </c>
       <c r="W2" t="s">
         <v>2862</v>
       </c>
       <c r="X2" t="s">
-        <v>3004</v>
+        <v>3143</v>
       </c>
       <c r="Y2" t="s">
-        <v>3005</v>
+        <v>712</v>
       </c>
       <c r="Z2" t="s">
         <v>2941</v>
@@ -12852,16 +13302,16 @@
         <v>914</v>
       </c>
       <c r="AH2" t="s">
-        <v>3007</v>
+        <v>3144</v>
       </c>
       <c r="AI2" t="s">
-        <v>1933</v>
+        <v>886</v>
       </c>
       <c r="AJ2" t="s">
-        <v>3009</v>
+        <v>3234</v>
       </c>
       <c r="AK2" t="s">
-        <v>3008</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -12872,13 +13322,13 @@
         <v>1293900</v>
       </c>
       <c r="C3" t="s">
-        <v>1885</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>3015</v>
+        <v>3236</v>
       </c>
       <c r="E3" t="s">
-        <v>3014</v>
+        <v>3235</v>
       </c>
       <c r="G3" t="s">
         <v>627</v>
@@ -12893,55 +13343,55 @@
         <v>683</v>
       </c>
       <c r="U3" t="s">
+        <v>2787</v>
+      </c>
+      <c r="V3" t="s">
         <v>2862</v>
       </c>
-      <c r="V3" t="s">
-        <v>658</v>
-      </c>
       <c r="W3" t="s">
-        <v>2787</v>
+        <v>659</v>
       </c>
       <c r="X3" t="s">
-        <v>915</v>
+        <v>1140</v>
       </c>
       <c r="Y3" t="s">
+        <v>665</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>3147</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>3148</v>
+      </c>
+      <c r="AB3" t="s">
         <v>3010</v>
       </c>
-      <c r="Z3" t="s">
-        <v>3011</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>665</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>3012</v>
-      </c>
       <c r="AC3" t="s">
-        <v>2713</v>
+        <v>3149</v>
       </c>
       <c r="AD3" t="s">
-        <v>3013</v>
+        <v>2948</v>
       </c>
       <c r="AE3" t="s">
         <v>648</v>
       </c>
       <c r="AF3" t="s">
-        <v>1140</v>
+        <v>658</v>
       </c>
       <c r="AG3" t="s">
         <v>724</v>
       </c>
       <c r="AH3" t="s">
-        <v>2948</v>
+        <v>2713</v>
       </c>
       <c r="AI3" t="s">
-        <v>1885</v>
+        <v>271</v>
       </c>
       <c r="AJ3" t="s">
-        <v>3015</v>
+        <v>3236</v>
       </c>
       <c r="AK3" t="s">
-        <v>3014</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -12952,13 +13402,13 @@
         <v>4115919</v>
       </c>
       <c r="C4" t="s">
-        <v>795</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
-        <v>3021</v>
+        <v>3238</v>
       </c>
       <c r="E4" t="s">
-        <v>3020</v>
+        <v>3237</v>
       </c>
       <c r="G4" t="s">
         <v>552</v>
@@ -12973,55 +13423,55 @@
         <v>648</v>
       </c>
       <c r="U4" t="s">
-        <v>2863</v>
+        <v>2691</v>
       </c>
       <c r="V4" t="s">
-        <v>2691</v>
+        <v>3142</v>
       </c>
       <c r="W4" t="s">
-        <v>658</v>
+        <v>3018</v>
       </c>
       <c r="X4" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>3143</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>3016</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>2157</v>
+      </c>
+      <c r="AB4" t="s">
         <v>2881</v>
       </c>
-      <c r="Y4" t="s">
-        <v>3016</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>3004</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>3012</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>2157</v>
-      </c>
       <c r="AC4" t="s">
-        <v>3017</v>
+        <v>2879</v>
       </c>
       <c r="AD4" t="s">
-        <v>2879</v>
+        <v>3152</v>
       </c>
       <c r="AE4" t="s">
         <v>667</v>
       </c>
       <c r="AF4" t="s">
-        <v>3018</v>
+        <v>658</v>
       </c>
       <c r="AG4" t="s">
-        <v>3007</v>
+        <v>3144</v>
       </c>
       <c r="AH4" t="s">
-        <v>3019</v>
+        <v>2741</v>
       </c>
       <c r="AI4" t="s">
-        <v>795</v>
+        <v>260</v>
       </c>
       <c r="AJ4" t="s">
-        <v>3021</v>
+        <v>3238</v>
       </c>
       <c r="AK4" t="s">
-        <v>3020</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -13032,13 +13482,13 @@
         <v>2324952</v>
       </c>
       <c r="C5" t="s">
-        <v>3024</v>
+        <v>647</v>
       </c>
       <c r="D5" t="s">
-        <v>3026</v>
+        <v>3240</v>
       </c>
       <c r="E5" t="s">
-        <v>3025</v>
+        <v>3239</v>
       </c>
       <c r="G5" t="s">
         <v>680</v>
@@ -13050,58 +13500,58 @@
         <v>705</v>
       </c>
       <c r="T5" t="s">
-        <v>691</v>
+        <v>2009</v>
       </c>
       <c r="U5" t="s">
-        <v>2863</v>
+        <v>3142</v>
       </c>
       <c r="V5" t="s">
-        <v>658</v>
+        <v>2691</v>
       </c>
       <c r="W5" t="s">
         <v>2862</v>
       </c>
       <c r="X5" t="s">
-        <v>2691</v>
+        <v>3006</v>
       </c>
       <c r="Y5" t="s">
-        <v>3012</v>
+        <v>2707</v>
       </c>
       <c r="Z5" t="s">
-        <v>3006</v>
+        <v>3022</v>
       </c>
       <c r="AA5" t="s">
-        <v>3016</v>
+        <v>3148</v>
       </c>
       <c r="AB5" t="s">
-        <v>3022</v>
+        <v>1345</v>
       </c>
       <c r="AC5" t="s">
+        <v>400</v>
+      </c>
+      <c r="AD5" t="s">
         <v>2985</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>400</v>
       </c>
       <c r="AE5" t="s">
         <v>667</v>
       </c>
       <c r="AF5" t="s">
-        <v>3007</v>
+        <v>3144</v>
       </c>
       <c r="AG5" t="s">
-        <v>1345</v>
+        <v>658</v>
       </c>
       <c r="AH5" t="s">
-        <v>3023</v>
+        <v>3016</v>
       </c>
       <c r="AI5" t="s">
-        <v>3024</v>
+        <v>647</v>
       </c>
       <c r="AJ5" t="s">
-        <v>3026</v>
+        <v>3240</v>
       </c>
       <c r="AK5" t="s">
-        <v>3025</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -13112,13 +13562,13 @@
         <v>2522621</v>
       </c>
       <c r="C6" t="s">
-        <v>1297</v>
+        <v>686</v>
       </c>
       <c r="D6" t="s">
-        <v>3034</v>
+        <v>3158</v>
       </c>
       <c r="E6" t="s">
-        <v>3033</v>
+        <v>3241</v>
       </c>
       <c r="G6" t="s">
         <v>627</v>
@@ -13130,58 +13580,58 @@
         <v>717</v>
       </c>
       <c r="T6" t="s">
-        <v>1128</v>
+        <v>2009</v>
       </c>
       <c r="U6" t="s">
         <v>2862</v>
       </c>
       <c r="V6" t="s">
+        <v>2202</v>
+      </c>
+      <c r="W6" t="s">
         <v>3027</v>
       </c>
-      <c r="W6" t="s">
-        <v>2202</v>
-      </c>
       <c r="X6" t="s">
+        <v>2051</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>3156</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>3010</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>3148</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3029</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>3031</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>3149</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>1128</v>
+      </c>
+      <c r="AF6" t="s">
         <v>658</v>
       </c>
-      <c r="Y6" t="s">
-        <v>3028</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AG6" t="s">
         <v>3016</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>3010</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>3012</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>3029</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>3013</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>691</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>3030</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>3031</v>
       </c>
       <c r="AH6" t="s">
         <v>3032</v>
       </c>
       <c r="AI6" t="s">
-        <v>1297</v>
+        <v>686</v>
       </c>
       <c r="AJ6" t="s">
-        <v>3034</v>
+        <v>3158</v>
       </c>
       <c r="AK6" t="s">
-        <v>3033</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -13192,13 +13642,13 @@
         <v>488734</v>
       </c>
       <c r="C7" t="s">
-        <v>1922</v>
+        <v>686</v>
       </c>
       <c r="D7" t="s">
-        <v>3040</v>
+        <v>3243</v>
       </c>
       <c r="E7" t="s">
-        <v>3039</v>
+        <v>3242</v>
       </c>
       <c r="G7" t="s">
         <v>627</v>
@@ -13210,7 +13660,7 @@
         <v>409</v>
       </c>
       <c r="T7" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U7" t="s">
         <v>3035</v>
@@ -13225,7 +13675,7 @@
         <v>1898</v>
       </c>
       <c r="Y7" t="s">
-        <v>3036</v>
+        <v>3159</v>
       </c>
       <c r="Z7" t="s">
         <v>665</v>
@@ -13237,10 +13687,10 @@
         <v>2007</v>
       </c>
       <c r="AC7" t="s">
-        <v>3037</v>
+        <v>2894</v>
       </c>
       <c r="AD7" t="s">
-        <v>3038</v>
+        <v>3160</v>
       </c>
       <c r="AE7" t="s">
         <v>778</v>
@@ -13249,19 +13699,19 @@
         <v>724</v>
       </c>
       <c r="AG7" t="s">
-        <v>1946</v>
+        <v>1154</v>
       </c>
       <c r="AH7" t="s">
         <v>1905</v>
       </c>
       <c r="AI7" t="s">
-        <v>1922</v>
+        <v>686</v>
       </c>
       <c r="AJ7" t="s">
-        <v>3040</v>
+        <v>3243</v>
       </c>
       <c r="AK7" t="s">
-        <v>3039</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -13272,13 +13722,13 @@
         <v>1069199</v>
       </c>
       <c r="C8" t="s">
-        <v>627</v>
+        <v>293</v>
       </c>
       <c r="D8" t="s">
-        <v>3046</v>
+        <v>3245</v>
       </c>
       <c r="E8" t="s">
-        <v>3045</v>
+        <v>3244</v>
       </c>
       <c r="G8" t="s">
         <v>627</v>
@@ -13293,7 +13743,7 @@
         <v>2895</v>
       </c>
       <c r="U8" t="s">
-        <v>3007</v>
+        <v>3144</v>
       </c>
       <c r="V8" t="s">
         <v>3041</v>
@@ -13302,10 +13752,10 @@
         <v>2691</v>
       </c>
       <c r="X8" t="s">
-        <v>3042</v>
+        <v>3163</v>
       </c>
       <c r="Y8" t="s">
-        <v>3004</v>
+        <v>3143</v>
       </c>
       <c r="Z8" t="s">
         <v>3022</v>
@@ -13317,10 +13767,10 @@
         <v>2881</v>
       </c>
       <c r="AC8" t="s">
-        <v>3017</v>
+        <v>3152</v>
       </c>
       <c r="AD8" t="s">
-        <v>3043</v>
+        <v>3164</v>
       </c>
       <c r="AE8" t="s">
         <v>1806</v>
@@ -13329,19 +13779,19 @@
         <v>2716</v>
       </c>
       <c r="AG8" t="s">
-        <v>3044</v>
+        <v>3165</v>
       </c>
       <c r="AH8" t="s">
         <v>2948</v>
       </c>
       <c r="AI8" t="s">
-        <v>627</v>
+        <v>293</v>
       </c>
       <c r="AJ8" t="s">
-        <v>3046</v>
+        <v>3245</v>
       </c>
       <c r="AK8" t="s">
-        <v>3045</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -13352,13 +13802,13 @@
         <v>1327409</v>
       </c>
       <c r="C9" t="s">
-        <v>1933</v>
+        <v>848</v>
       </c>
       <c r="D9" t="s">
-        <v>3054</v>
+        <v>3247</v>
       </c>
       <c r="E9" t="s">
-        <v>3053</v>
+        <v>3246</v>
       </c>
       <c r="G9" t="s">
         <v>627</v>
@@ -13370,37 +13820,37 @@
         <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>2027</v>
+        <v>410</v>
       </c>
       <c r="U9" t="s">
-        <v>658</v>
+        <v>3168</v>
       </c>
       <c r="V9" t="s">
-        <v>1354</v>
+        <v>3169</v>
       </c>
       <c r="W9" t="s">
         <v>2696</v>
       </c>
       <c r="X9" t="s">
+        <v>2967</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>2941</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>3170</v>
+      </c>
+      <c r="AA9" t="s">
         <v>3006</v>
       </c>
-      <c r="Y9" t="s">
-        <v>3047</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>3048</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>2941</v>
-      </c>
       <c r="AB9" t="s">
-        <v>3049</v>
+        <v>3171</v>
       </c>
       <c r="AC9" t="s">
-        <v>3013</v>
+        <v>773</v>
       </c>
       <c r="AD9" t="s">
-        <v>3050</v>
+        <v>3149</v>
       </c>
       <c r="AE9" t="s">
         <v>648</v>
@@ -13409,19 +13859,19 @@
         <v>3051</v>
       </c>
       <c r="AG9" t="s">
-        <v>3052</v>
+        <v>1354</v>
       </c>
       <c r="AH9" t="s">
-        <v>2819</v>
+        <v>658</v>
       </c>
       <c r="AI9" t="s">
-        <v>1933</v>
+        <v>848</v>
       </c>
       <c r="AJ9" t="s">
-        <v>3054</v>
+        <v>3247</v>
       </c>
       <c r="AK9" t="s">
-        <v>3053</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -13432,13 +13882,13 @@
         <v>2203632</v>
       </c>
       <c r="C10" t="s">
-        <v>1892</v>
+        <v>803</v>
       </c>
       <c r="D10" t="s">
-        <v>3061</v>
+        <v>3199</v>
       </c>
       <c r="E10" t="s">
-        <v>3060</v>
+        <v>3248</v>
       </c>
       <c r="G10" t="s">
         <v>627</v>
@@ -13450,37 +13900,37 @@
         <v>259</v>
       </c>
       <c r="T10" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U10" t="s">
-        <v>3055</v>
+        <v>2862</v>
       </c>
       <c r="V10" t="s">
+        <v>3174</v>
+      </c>
+      <c r="W10" t="s">
         <v>3056</v>
       </c>
-      <c r="W10" t="s">
-        <v>658</v>
-      </c>
       <c r="X10" t="s">
-        <v>2862</v>
+        <v>2881</v>
       </c>
       <c r="Y10" t="s">
-        <v>3048</v>
+        <v>3016</v>
       </c>
       <c r="Z10" t="s">
-        <v>3016</v>
+        <v>3022</v>
       </c>
       <c r="AA10" t="s">
+        <v>3170</v>
+      </c>
+      <c r="AB10" t="s">
         <v>3006</v>
       </c>
-      <c r="AB10" t="s">
-        <v>3022</v>
-      </c>
       <c r="AC10" t="s">
+        <v>3175</v>
+      </c>
+      <c r="AD10" t="s">
         <v>2007</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>3057</v>
       </c>
       <c r="AE10" t="s">
         <v>342</v>
@@ -13492,16 +13942,16 @@
         <v>3059</v>
       </c>
       <c r="AH10" t="s">
-        <v>2881</v>
+        <v>658</v>
       </c>
       <c r="AI10" t="s">
-        <v>1892</v>
+        <v>803</v>
       </c>
       <c r="AJ10" t="s">
-        <v>3061</v>
+        <v>3199</v>
       </c>
       <c r="AK10" t="s">
-        <v>3060</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -13512,13 +13962,13 @@
         <v>3998490</v>
       </c>
       <c r="C11" t="s">
-        <v>627</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
-        <v>3066</v>
+        <v>3250</v>
       </c>
       <c r="E11" t="s">
-        <v>3065</v>
+        <v>3249</v>
       </c>
       <c r="G11" t="s">
         <v>627</v>
@@ -13536,13 +13986,13 @@
         <v>2862</v>
       </c>
       <c r="V11" t="s">
-        <v>2819</v>
+        <v>3169</v>
       </c>
       <c r="W11" t="s">
         <v>916</v>
       </c>
       <c r="X11" t="s">
-        <v>2911</v>
+        <v>3178</v>
       </c>
       <c r="Y11" t="s">
         <v>3010</v>
@@ -13551,7 +14001,7 @@
         <v>1206</v>
       </c>
       <c r="AA11" t="s">
-        <v>3004</v>
+        <v>3143</v>
       </c>
       <c r="AB11" t="s">
         <v>3062</v>
@@ -13563,7 +14013,7 @@
         <v>2007</v>
       </c>
       <c r="AE11" t="s">
-        <v>3063</v>
+        <v>918</v>
       </c>
       <c r="AF11" t="s">
         <v>3064</v>
@@ -13575,13 +14025,13 @@
         <v>2708</v>
       </c>
       <c r="AI11" t="s">
-        <v>627</v>
+        <v>273</v>
       </c>
       <c r="AJ11" t="s">
-        <v>3066</v>
+        <v>3250</v>
       </c>
       <c r="AK11" t="s">
-        <v>3065</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -13592,13 +14042,13 @@
         <v>440807</v>
       </c>
       <c r="C12" t="s">
-        <v>1892</v>
+        <v>759</v>
       </c>
       <c r="D12" t="s">
-        <v>3071</v>
+        <v>3252</v>
       </c>
       <c r="E12" t="s">
-        <v>3070</v>
+        <v>3251</v>
       </c>
       <c r="G12" t="s">
         <v>627</v>
@@ -13610,58 +14060,58 @@
         <v>263</v>
       </c>
       <c r="T12" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U12" t="s">
         <v>2691</v>
       </c>
       <c r="V12" t="s">
-        <v>2185</v>
+        <v>483</v>
       </c>
       <c r="W12" t="s">
-        <v>2863</v>
+        <v>3142</v>
       </c>
       <c r="X12" t="s">
-        <v>3007</v>
+        <v>1898</v>
       </c>
       <c r="Y12" t="s">
-        <v>3047</v>
+        <v>3010</v>
       </c>
       <c r="Z12" t="s">
-        <v>1898</v>
+        <v>2967</v>
       </c>
       <c r="AA12" t="s">
-        <v>3010</v>
+        <v>2881</v>
       </c>
       <c r="AB12" t="s">
-        <v>2881</v>
+        <v>2961</v>
       </c>
       <c r="AC12" t="s">
         <v>1345</v>
       </c>
       <c r="AD12" t="s">
-        <v>3067</v>
+        <v>3181</v>
       </c>
       <c r="AE12" t="s">
         <v>1173</v>
       </c>
       <c r="AF12" t="s">
-        <v>2961</v>
+        <v>3144</v>
       </c>
       <c r="AG12" t="s">
-        <v>3068</v>
+        <v>3182</v>
       </c>
       <c r="AH12" t="s">
-        <v>3069</v>
+        <v>1359</v>
       </c>
       <c r="AI12" t="s">
-        <v>1892</v>
+        <v>759</v>
       </c>
       <c r="AJ12" t="s">
-        <v>3071</v>
+        <v>3252</v>
       </c>
       <c r="AK12" t="s">
-        <v>3070</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -13672,13 +14122,13 @@
         <v>2184142</v>
       </c>
       <c r="C13" t="s">
-        <v>1297</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>3073</v>
+        <v>3254</v>
       </c>
       <c r="E13" t="s">
-        <v>3072</v>
+        <v>3253</v>
       </c>
       <c r="G13" t="s">
         <v>646</v>
@@ -13690,10 +14140,10 @@
         <v>265</v>
       </c>
       <c r="T13" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U13" t="s">
-        <v>3055</v>
+        <v>3174</v>
       </c>
       <c r="V13" t="s">
         <v>916</v>
@@ -13705,16 +14155,16 @@
         <v>2202</v>
       </c>
       <c r="Y13" t="s">
-        <v>3004</v>
+        <v>3143</v>
       </c>
       <c r="Z13" t="s">
         <v>3006</v>
       </c>
       <c r="AA13" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="AB13" t="s">
-        <v>3048</v>
+        <v>3170</v>
       </c>
       <c r="AC13" t="s">
         <v>2157</v>
@@ -13729,19 +14179,19 @@
         <v>2879</v>
       </c>
       <c r="AG13" t="s">
-        <v>3049</v>
+        <v>773</v>
       </c>
       <c r="AH13" t="s">
         <v>1905</v>
       </c>
       <c r="AI13" t="s">
-        <v>1297</v>
+        <v>254</v>
       </c>
       <c r="AJ13" t="s">
-        <v>3073</v>
+        <v>3254</v>
       </c>
       <c r="AK13" t="s">
-        <v>3072</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -13752,13 +14202,13 @@
         <v>2795791</v>
       </c>
       <c r="C14" t="s">
-        <v>627</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
-        <v>3080</v>
+        <v>3111</v>
       </c>
       <c r="E14" t="s">
-        <v>3079</v>
+        <v>3255</v>
       </c>
       <c r="G14" t="s">
         <v>627</v>
@@ -13770,58 +14220,58 @@
         <v>770</v>
       </c>
       <c r="T14" t="s">
-        <v>3074</v>
+        <v>3187</v>
       </c>
       <c r="U14" t="s">
+        <v>3075</v>
+      </c>
+      <c r="V14" t="s">
+        <v>2692</v>
+      </c>
+      <c r="W14" t="s">
         <v>2696</v>
       </c>
-      <c r="V14" t="s">
-        <v>3075</v>
-      </c>
-      <c r="W14" t="s">
-        <v>2692</v>
-      </c>
       <c r="X14" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Y14" t="s">
         <v>2812</v>
       </c>
-      <c r="Y14" t="s">
-        <v>3076</v>
-      </c>
       <c r="Z14" t="s">
-        <v>3012</v>
+        <v>3188</v>
       </c>
       <c r="AA14" t="s">
-        <v>3016</v>
+        <v>3078</v>
       </c>
       <c r="AB14" t="s">
+        <v>3149</v>
+      </c>
+      <c r="AC14" t="s">
         <v>2985</v>
       </c>
-      <c r="AC14" t="s">
-        <v>3013</v>
-      </c>
       <c r="AD14" t="s">
-        <v>3043</v>
+        <v>3164</v>
       </c>
       <c r="AE14" t="s">
         <v>667</v>
       </c>
       <c r="AF14" t="s">
-        <v>3077</v>
+        <v>539</v>
       </c>
       <c r="AG14" t="s">
         <v>2708</v>
       </c>
       <c r="AH14" t="s">
-        <v>3078</v>
+        <v>3016</v>
       </c>
       <c r="AI14" t="s">
-        <v>627</v>
+        <v>258</v>
       </c>
       <c r="AJ14" t="s">
-        <v>3080</v>
+        <v>3111</v>
       </c>
       <c r="AK14" t="s">
-        <v>3079</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -13832,13 +14282,13 @@
         <v>228724</v>
       </c>
       <c r="C15" t="s">
-        <v>759</v>
+        <v>2133</v>
       </c>
       <c r="D15" t="s">
-        <v>2723</v>
+        <v>3257</v>
       </c>
       <c r="E15" t="s">
-        <v>3084</v>
+        <v>3256</v>
       </c>
       <c r="G15" t="s">
         <v>627</v>
@@ -13853,55 +14303,55 @@
         <v>3081</v>
       </c>
       <c r="U15" t="s">
+        <v>2691</v>
+      </c>
+      <c r="V15" t="s">
+        <v>3082</v>
+      </c>
+      <c r="W15" t="s">
         <v>2862</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>2202</v>
       </c>
-      <c r="W15" t="s">
-        <v>2691</v>
-      </c>
-      <c r="X15" t="s">
-        <v>3082</v>
-      </c>
       <c r="Y15" t="s">
+        <v>3147</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>3062</v>
+      </c>
+      <c r="AB15" t="s">
         <v>1898</v>
       </c>
-      <c r="Z15" t="s">
-        <v>3011</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>3083</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>3069</v>
-      </c>
       <c r="AC15" t="s">
-        <v>3050</v>
+        <v>3171</v>
       </c>
       <c r="AD15" t="s">
-        <v>3057</v>
+        <v>3175</v>
       </c>
       <c r="AE15" t="s">
         <v>667</v>
       </c>
       <c r="AF15" t="s">
-        <v>3062</v>
+        <v>3083</v>
       </c>
       <c r="AG15" t="s">
         <v>724</v>
       </c>
       <c r="AH15" t="s">
-        <v>3019</v>
+        <v>2741</v>
       </c>
       <c r="AI15" t="s">
-        <v>759</v>
+        <v>2133</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2723</v>
+        <v>3257</v>
       </c>
       <c r="AK15" t="s">
-        <v>3084</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -13912,13 +14362,13 @@
         <v>2185186</v>
       </c>
       <c r="C16" t="s">
-        <v>2999</v>
+        <v>268</v>
       </c>
       <c r="D16" t="s">
-        <v>3089</v>
+        <v>3259</v>
       </c>
       <c r="E16" t="s">
-        <v>3088</v>
+        <v>3258</v>
       </c>
       <c r="G16" t="s">
         <v>627</v>
@@ -13933,34 +14383,34 @@
         <v>1173</v>
       </c>
       <c r="U16" t="s">
-        <v>3055</v>
+        <v>3193</v>
       </c>
       <c r="V16" t="s">
-        <v>658</v>
+        <v>3174</v>
       </c>
       <c r="W16" t="s">
-        <v>3085</v>
+        <v>3035</v>
       </c>
       <c r="X16" t="s">
-        <v>2941</v>
+        <v>3194</v>
       </c>
       <c r="Y16" t="s">
         <v>2189</v>
       </c>
       <c r="Z16" t="s">
-        <v>3086</v>
+        <v>2941</v>
       </c>
       <c r="AA16" t="s">
-        <v>3087</v>
+        <v>3195</v>
       </c>
       <c r="AB16" t="s">
         <v>2007</v>
       </c>
       <c r="AC16" t="s">
-        <v>3037</v>
+        <v>2985</v>
       </c>
       <c r="AD16" t="s">
-        <v>2985</v>
+        <v>2894</v>
       </c>
       <c r="AE16" t="s">
         <v>648</v>
@@ -13972,16 +14422,16 @@
         <v>665</v>
       </c>
       <c r="AH16" t="s">
-        <v>3035</v>
+        <v>658</v>
       </c>
       <c r="AI16" t="s">
-        <v>2999</v>
+        <v>268</v>
       </c>
       <c r="AJ16" t="s">
-        <v>3089</v>
+        <v>3259</v>
       </c>
       <c r="AK16" t="s">
-        <v>3088</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -13992,13 +14442,13 @@
         <v>2317783</v>
       </c>
       <c r="C17" t="s">
-        <v>1927</v>
+        <v>647</v>
       </c>
       <c r="D17" t="s">
-        <v>3092</v>
+        <v>3261</v>
       </c>
       <c r="E17" t="s">
-        <v>3091</v>
+        <v>3260</v>
       </c>
       <c r="G17" t="s">
         <v>426</v>
@@ -14010,34 +14460,34 @@
         <v>272</v>
       </c>
       <c r="T17" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U17" t="s">
-        <v>658</v>
+        <v>3142</v>
       </c>
       <c r="V17" t="s">
+        <v>3090</v>
+      </c>
+      <c r="W17" t="s">
         <v>3056</v>
       </c>
-      <c r="W17" t="s">
-        <v>3090</v>
-      </c>
       <c r="X17" t="s">
-        <v>2863</v>
+        <v>3170</v>
       </c>
       <c r="Y17" t="s">
         <v>3010</v>
       </c>
       <c r="Z17" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="AA17" t="s">
-        <v>3048</v>
+        <v>1359</v>
       </c>
       <c r="AB17" t="s">
-        <v>3016</v>
+        <v>2879</v>
       </c>
       <c r="AC17" t="s">
-        <v>3069</v>
+        <v>674</v>
       </c>
       <c r="AD17" t="s">
         <v>1335</v>
@@ -14046,22 +14496,22 @@
         <v>648</v>
       </c>
       <c r="AF17" t="s">
-        <v>2879</v>
+        <v>658</v>
       </c>
       <c r="AG17" t="s">
-        <v>674</v>
+        <v>3016</v>
       </c>
       <c r="AH17" t="s">
         <v>724</v>
       </c>
       <c r="AI17" t="s">
-        <v>1927</v>
+        <v>647</v>
       </c>
       <c r="AJ17" t="s">
-        <v>3092</v>
+        <v>3261</v>
       </c>
       <c r="AK17" t="s">
-        <v>3091</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -14072,13 +14522,13 @@
         <v>364277</v>
       </c>
       <c r="C18" t="s">
-        <v>1933</v>
+        <v>759</v>
       </c>
       <c r="D18" t="s">
-        <v>3094</v>
+        <v>2743</v>
       </c>
       <c r="E18" t="s">
-        <v>3093</v>
+        <v>3262</v>
       </c>
       <c r="G18" t="s">
         <v>627</v>
@@ -14093,40 +14543,40 @@
         <v>667</v>
       </c>
       <c r="U18" t="s">
+        <v>3193</v>
+      </c>
+      <c r="V18" t="s">
+        <v>2862</v>
+      </c>
+      <c r="W18" t="s">
+        <v>483</v>
+      </c>
+      <c r="X18" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>3006</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>3170</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>3022</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>2157</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>3164</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>3171</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>2009</v>
+      </c>
+      <c r="AF18" t="s">
         <v>658</v>
-      </c>
-      <c r="V18" t="s">
-        <v>2185</v>
-      </c>
-      <c r="W18" t="s">
-        <v>2862</v>
-      </c>
-      <c r="X18" t="s">
-        <v>2157</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>3022</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>3006</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>3012</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>3048</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>3043</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>3050</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>691</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>3085</v>
       </c>
       <c r="AG18" t="s">
         <v>3056</v>
@@ -14135,13 +14585,13 @@
         <v>2007</v>
       </c>
       <c r="AI18" t="s">
-        <v>1933</v>
+        <v>759</v>
       </c>
       <c r="AJ18" t="s">
-        <v>3094</v>
+        <v>2743</v>
       </c>
       <c r="AK18" t="s">
-        <v>3093</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -14152,13 +14602,13 @@
         <v>1396639</v>
       </c>
       <c r="C19" t="s">
-        <v>1936</v>
+        <v>1886</v>
       </c>
       <c r="D19" t="s">
-        <v>3097</v>
+        <v>3264</v>
       </c>
       <c r="E19" t="s">
-        <v>3096</v>
+        <v>3263</v>
       </c>
       <c r="G19" t="s">
         <v>426</v>
@@ -14173,55 +14623,55 @@
         <v>1173</v>
       </c>
       <c r="U19" t="s">
-        <v>3028</v>
+        <v>2691</v>
       </c>
       <c r="V19" t="s">
-        <v>2691</v>
+        <v>2202</v>
       </c>
       <c r="W19" t="s">
-        <v>2202</v>
+        <v>2051</v>
       </c>
       <c r="X19" t="s">
-        <v>3016</v>
+        <v>3148</v>
       </c>
       <c r="Y19" t="s">
         <v>3006</v>
       </c>
       <c r="Z19" t="s">
-        <v>3012</v>
+        <v>2157</v>
       </c>
       <c r="AA19" t="s">
-        <v>3069</v>
+        <v>1359</v>
       </c>
       <c r="AB19" t="s">
-        <v>2157</v>
+        <v>1345</v>
       </c>
       <c r="AC19" t="s">
+        <v>3149</v>
+      </c>
+      <c r="AD19" t="s">
         <v>2007</v>
       </c>
-      <c r="AD19" t="s">
-        <v>3013</v>
-      </c>
       <c r="AE19" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="AF19" t="s">
-        <v>1345</v>
+        <v>3016</v>
       </c>
       <c r="AG19" t="s">
-        <v>3007</v>
+        <v>3144</v>
       </c>
       <c r="AH19" t="s">
         <v>3095</v>
       </c>
       <c r="AI19" t="s">
-        <v>1936</v>
+        <v>1886</v>
       </c>
       <c r="AJ19" t="s">
-        <v>3097</v>
+        <v>3264</v>
       </c>
       <c r="AK19" t="s">
-        <v>3096</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -14232,13 +14682,13 @@
         <v>1339989</v>
       </c>
       <c r="C20" t="s">
-        <v>1936</v>
+        <v>293</v>
       </c>
       <c r="D20" t="s">
-        <v>3101</v>
+        <v>3266</v>
       </c>
       <c r="E20" t="s">
-        <v>3100</v>
+        <v>3265</v>
       </c>
       <c r="G20" t="s">
         <v>627</v>
@@ -14256,37 +14706,37 @@
         <v>2202</v>
       </c>
       <c r="V20" t="s">
+        <v>2692</v>
+      </c>
+      <c r="W20" t="s">
         <v>2691</v>
       </c>
-      <c r="W20" t="s">
-        <v>2692</v>
-      </c>
       <c r="X20" t="s">
-        <v>3069</v>
+        <v>3041</v>
       </c>
       <c r="Y20" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>3204</v>
+      </c>
+      <c r="AB20" t="s">
         <v>3010</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>3004</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>3012</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>3098</v>
       </c>
       <c r="AC20" t="s">
         <v>674</v>
       </c>
       <c r="AD20" t="s">
-        <v>3050</v>
+        <v>3171</v>
       </c>
       <c r="AE20" t="s">
-        <v>3063</v>
+        <v>918</v>
       </c>
       <c r="AF20" t="s">
-        <v>3041</v>
+        <v>3098</v>
       </c>
       <c r="AG20" t="s">
         <v>3099</v>
@@ -14295,13 +14745,13 @@
         <v>724</v>
       </c>
       <c r="AI20" t="s">
-        <v>1936</v>
+        <v>293</v>
       </c>
       <c r="AJ20" t="s">
-        <v>3101</v>
+        <v>3266</v>
       </c>
       <c r="AK20" t="s">
-        <v>3100</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -14312,13 +14762,13 @@
         <v>474028</v>
       </c>
       <c r="C21" t="s">
-        <v>1885</v>
+        <v>815</v>
       </c>
       <c r="D21" t="s">
-        <v>3104</v>
+        <v>3268</v>
       </c>
       <c r="E21" t="s">
-        <v>3103</v>
+        <v>3267</v>
       </c>
       <c r="G21" t="s">
         <v>627</v>
@@ -14330,58 +14780,58 @@
         <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U21" t="s">
-        <v>658</v>
+        <v>2691</v>
       </c>
       <c r="V21" t="s">
+        <v>2202</v>
+      </c>
+      <c r="W21" t="s">
         <v>2692</v>
       </c>
-      <c r="W21" t="s">
-        <v>2202</v>
-      </c>
       <c r="X21" t="s">
-        <v>2691</v>
+        <v>3022</v>
       </c>
       <c r="Y21" t="s">
+        <v>3170</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>3148</v>
+      </c>
+      <c r="AA21" t="s">
         <v>3010</v>
       </c>
-      <c r="Z21" t="s">
-        <v>3012</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>3048</v>
-      </c>
       <c r="AB21" t="s">
-        <v>3022</v>
+        <v>1345</v>
       </c>
       <c r="AC21" t="s">
-        <v>3017</v>
+        <v>2879</v>
       </c>
       <c r="AD21" t="s">
-        <v>2879</v>
+        <v>3152</v>
       </c>
       <c r="AE21" t="s">
         <v>667</v>
       </c>
       <c r="AF21" t="s">
-        <v>1345</v>
+        <v>658</v>
       </c>
       <c r="AG21" t="s">
         <v>3102</v>
       </c>
       <c r="AH21" t="s">
-        <v>915</v>
+        <v>659</v>
       </c>
       <c r="AI21" t="s">
-        <v>1885</v>
+        <v>815</v>
       </c>
       <c r="AJ21" t="s">
-        <v>3104</v>
+        <v>3268</v>
       </c>
       <c r="AK21" t="s">
-        <v>3103</v>
+        <v>3267</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -14392,13 +14842,13 @@
         <v>1229286</v>
       </c>
       <c r="C22" t="s">
-        <v>1886</v>
+        <v>645</v>
       </c>
       <c r="D22" t="s">
-        <v>3106</v>
+        <v>3229</v>
       </c>
       <c r="E22" t="s">
-        <v>3105</v>
+        <v>3269</v>
       </c>
       <c r="G22" t="s">
         <v>552</v>
@@ -14410,16 +14860,16 @@
         <v>804</v>
       </c>
       <c r="T22" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U22" t="s">
         <v>2691</v>
       </c>
       <c r="V22" t="s">
-        <v>2863</v>
+        <v>3142</v>
       </c>
       <c r="W22" t="s">
-        <v>3055</v>
+        <v>3174</v>
       </c>
       <c r="X22" t="s">
         <v>2862</v>
@@ -14434,19 +14884,19 @@
         <v>3006</v>
       </c>
       <c r="AB22" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="AC22" t="s">
         <v>2881</v>
       </c>
       <c r="AD22" t="s">
-        <v>3013</v>
+        <v>3149</v>
       </c>
       <c r="AE22" t="s">
         <v>667</v>
       </c>
       <c r="AF22" t="s">
-        <v>3048</v>
+        <v>3170</v>
       </c>
       <c r="AG22" t="s">
         <v>1345</v>
@@ -14455,13 +14905,13 @@
         <v>2713</v>
       </c>
       <c r="AI22" t="s">
-        <v>1886</v>
+        <v>645</v>
       </c>
       <c r="AJ22" t="s">
-        <v>3106</v>
+        <v>3229</v>
       </c>
       <c r="AK22" t="s">
-        <v>3105</v>
+        <v>3269</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -14472,13 +14922,13 @@
         <v>2340261</v>
       </c>
       <c r="C23" t="s">
-        <v>3109</v>
+        <v>1485</v>
       </c>
       <c r="D23" t="s">
-        <v>3111</v>
+        <v>3271</v>
       </c>
       <c r="E23" t="s">
-        <v>3110</v>
+        <v>3270</v>
       </c>
       <c r="G23" t="s">
         <v>627</v>
@@ -14490,58 +14940,58 @@
         <v>281</v>
       </c>
       <c r="T23" t="s">
-        <v>3063</v>
+        <v>918</v>
       </c>
       <c r="U23" t="s">
-        <v>3007</v>
+        <v>3210</v>
       </c>
       <c r="V23" t="s">
-        <v>2862</v>
+        <v>2692</v>
       </c>
       <c r="W23" t="s">
-        <v>2692</v>
+        <v>658</v>
       </c>
       <c r="X23" t="s">
-        <v>658</v>
+        <v>1898</v>
       </c>
       <c r="Y23" t="s">
-        <v>3036</v>
+        <v>3148</v>
       </c>
       <c r="Z23" t="s">
-        <v>1898</v>
+        <v>3159</v>
       </c>
       <c r="AA23" t="s">
-        <v>3098</v>
+        <v>3143</v>
       </c>
       <c r="AB23" t="s">
-        <v>3004</v>
+        <v>2007</v>
       </c>
       <c r="AC23" t="s">
-        <v>3012</v>
+        <v>1345</v>
       </c>
       <c r="AD23" t="s">
-        <v>3049</v>
+        <v>773</v>
       </c>
       <c r="AE23" t="s">
         <v>3107</v>
       </c>
       <c r="AF23" t="s">
-        <v>2007</v>
+        <v>3144</v>
       </c>
       <c r="AG23" t="s">
-        <v>3108</v>
+        <v>2126</v>
       </c>
       <c r="AH23" t="s">
-        <v>1345</v>
+        <v>3098</v>
       </c>
       <c r="AI23" t="s">
-        <v>3109</v>
+        <v>1485</v>
       </c>
       <c r="AJ23" t="s">
-        <v>3111</v>
+        <v>3271</v>
       </c>
       <c r="AK23" t="s">
-        <v>3110</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -14552,13 +15002,13 @@
         <v>1708392</v>
       </c>
       <c r="C24" t="s">
-        <v>848</v>
+        <v>1805</v>
       </c>
       <c r="D24" t="s">
-        <v>3114</v>
+        <v>3223</v>
       </c>
       <c r="E24" t="s">
-        <v>3113</v>
+        <v>3272</v>
       </c>
       <c r="G24" t="s">
         <v>680</v>
@@ -14570,37 +15020,37 @@
         <v>283</v>
       </c>
       <c r="T24" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U24" t="s">
+        <v>3056</v>
+      </c>
+      <c r="V24" t="s">
         <v>916</v>
-      </c>
-      <c r="V24" t="s">
-        <v>3056</v>
       </c>
       <c r="W24" t="s">
         <v>2202</v>
       </c>
       <c r="X24" t="s">
+        <v>3027</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>3148</v>
+      </c>
+      <c r="Z24" t="s">
         <v>3112</v>
       </c>
-      <c r="Y24" t="s">
-        <v>3012</v>
-      </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AB24" t="s">
         <v>3010</v>
       </c>
-      <c r="AA24" t="s">
-        <v>3069</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>3016</v>
-      </c>
       <c r="AC24" t="s">
+        <v>3152</v>
+      </c>
+      <c r="AD24" t="s">
         <v>2007</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>3017</v>
       </c>
       <c r="AE24" t="s">
         <v>667</v>
@@ -14609,19 +15059,19 @@
         <v>360</v>
       </c>
       <c r="AG24" t="s">
-        <v>3027</v>
+        <v>3016</v>
       </c>
       <c r="AH24" t="s">
         <v>529</v>
       </c>
       <c r="AI24" t="s">
-        <v>848</v>
+        <v>1805</v>
       </c>
       <c r="AJ24" t="s">
-        <v>3114</v>
+        <v>3223</v>
       </c>
       <c r="AK24" t="s">
-        <v>3113</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -14632,13 +15082,13 @@
         <v>2719892</v>
       </c>
       <c r="C25" t="s">
-        <v>3120</v>
+        <v>262</v>
       </c>
       <c r="D25" t="s">
-        <v>3122</v>
+        <v>3274</v>
       </c>
       <c r="E25" t="s">
-        <v>3121</v>
+        <v>3273</v>
       </c>
       <c r="G25" t="s">
         <v>627</v>
@@ -14650,58 +15100,58 @@
         <v>461</v>
       </c>
       <c r="T25" t="s">
-        <v>3115</v>
+        <v>3214</v>
       </c>
       <c r="U25" t="s">
-        <v>2819</v>
+        <v>3035</v>
       </c>
       <c r="V25" t="s">
         <v>2202</v>
       </c>
       <c r="W25" t="s">
-        <v>3035</v>
+        <v>3169</v>
       </c>
       <c r="X25" t="s">
-        <v>3005</v>
+        <v>3119</v>
       </c>
       <c r="Y25" t="s">
-        <v>3116</v>
+        <v>712</v>
       </c>
       <c r="Z25" t="s">
-        <v>1934</v>
+        <v>3143</v>
       </c>
       <c r="AA25" t="s">
-        <v>3004</v>
+        <v>1138</v>
       </c>
       <c r="AB25" t="s">
+        <v>2894</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>2196</v>
+      </c>
+      <c r="AD25" t="s">
         <v>3117</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>3037</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>3118</v>
       </c>
       <c r="AE25" t="s">
         <v>667</v>
       </c>
       <c r="AF25" t="s">
-        <v>3108</v>
+        <v>2126</v>
       </c>
       <c r="AG25" t="s">
         <v>724</v>
       </c>
       <c r="AH25" t="s">
-        <v>3119</v>
+        <v>1934</v>
       </c>
       <c r="AI25" t="s">
-        <v>3120</v>
+        <v>262</v>
       </c>
       <c r="AJ25" t="s">
-        <v>3122</v>
+        <v>3274</v>
       </c>
       <c r="AK25" t="s">
-        <v>3121</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -14712,13 +15162,13 @@
         <v>122847</v>
       </c>
       <c r="C26" t="s">
-        <v>1936</v>
+        <v>1958</v>
       </c>
       <c r="D26" t="s">
-        <v>3124</v>
+        <v>3276</v>
       </c>
       <c r="E26" t="s">
-        <v>3123</v>
+        <v>3275</v>
       </c>
       <c r="G26" t="s">
         <v>627</v>
@@ -14733,28 +15183,28 @@
         <v>667</v>
       </c>
       <c r="U26" t="s">
-        <v>658</v>
+        <v>3142</v>
       </c>
       <c r="V26" t="s">
-        <v>2863</v>
+        <v>2692</v>
       </c>
       <c r="W26" t="s">
         <v>2862</v>
       </c>
       <c r="X26" t="s">
-        <v>2692</v>
+        <v>2051</v>
       </c>
       <c r="Y26" t="s">
+        <v>3022</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>3148</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AB26" t="s">
         <v>1930</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>3022</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>3069</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>3012</v>
       </c>
       <c r="AC26" t="s">
         <v>3006</v>
@@ -14763,10 +15213,10 @@
         <v>674</v>
       </c>
       <c r="AE26" t="s">
-        <v>691</v>
+        <v>2009</v>
       </c>
       <c r="AF26" t="s">
-        <v>3028</v>
+        <v>658</v>
       </c>
       <c r="AG26" t="s">
         <v>802</v>
@@ -14775,13 +15225,13 @@
         <v>3099</v>
       </c>
       <c r="AI26" t="s">
-        <v>1936</v>
+        <v>1958</v>
       </c>
       <c r="AJ26" t="s">
-        <v>3124</v>
+        <v>3276</v>
       </c>
       <c r="AK26" t="s">
-        <v>3123</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -14792,13 +15242,13 @@
         <v>362369</v>
       </c>
       <c r="C27" t="s">
-        <v>3120</v>
+        <v>260</v>
       </c>
       <c r="D27" t="s">
-        <v>3126</v>
+        <v>3219</v>
       </c>
       <c r="E27" t="s">
-        <v>3125</v>
+        <v>3277</v>
       </c>
       <c r="G27" t="s">
         <v>627</v>
@@ -14813,28 +15263,28 @@
         <v>342</v>
       </c>
       <c r="U27" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="V27" t="s">
+        <v>2862</v>
+      </c>
+      <c r="W27" t="s">
         <v>2202</v>
       </c>
-      <c r="W27" t="s">
-        <v>2862</v>
-      </c>
       <c r="X27" t="s">
-        <v>3007</v>
+        <v>3148</v>
       </c>
       <c r="Y27" t="s">
         <v>3010</v>
       </c>
       <c r="Z27" t="s">
-        <v>3011</v>
+        <v>3147</v>
       </c>
       <c r="AA27" t="s">
-        <v>3069</v>
+        <v>1359</v>
       </c>
       <c r="AB27" t="s">
-        <v>1228</v>
+        <v>3031</v>
       </c>
       <c r="AC27" t="s">
         <v>1345</v>
@@ -14846,22 +15296,22 @@
         <v>2895</v>
       </c>
       <c r="AF27" t="s">
-        <v>3012</v>
+        <v>658</v>
       </c>
       <c r="AG27" t="s">
-        <v>915</v>
+        <v>3144</v>
       </c>
       <c r="AH27" t="s">
-        <v>3031</v>
+        <v>1228</v>
       </c>
       <c r="AI27" t="s">
-        <v>3120</v>
+        <v>260</v>
       </c>
       <c r="AJ27" t="s">
-        <v>3126</v>
+        <v>3219</v>
       </c>
       <c r="AK27" t="s">
-        <v>3125</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -14872,13 +15322,13 @@
         <v>290784</v>
       </c>
       <c r="C28" t="s">
-        <v>1936</v>
+        <v>745</v>
       </c>
       <c r="D28" t="s">
-        <v>3128</v>
+        <v>3223</v>
       </c>
       <c r="E28" t="s">
-        <v>3127</v>
+        <v>3278</v>
       </c>
       <c r="G28" t="s">
         <v>627</v>
@@ -14890,10 +15340,10 @@
         <v>831</v>
       </c>
       <c r="T28" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U28" t="s">
-        <v>2863</v>
+        <v>3142</v>
       </c>
       <c r="V28" t="s">
         <v>2202</v>
@@ -14902,13 +15352,13 @@
         <v>2691</v>
       </c>
       <c r="X28" t="s">
-        <v>3048</v>
+        <v>3170</v>
       </c>
       <c r="Y28" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="Z28" t="s">
-        <v>3069</v>
+        <v>1359</v>
       </c>
       <c r="AA28" t="s">
         <v>3010</v>
@@ -14917,7 +15367,7 @@
         <v>2165</v>
       </c>
       <c r="AC28" t="s">
-        <v>3017</v>
+        <v>3152</v>
       </c>
       <c r="AD28" t="s">
         <v>2879</v>
@@ -14935,13 +15385,13 @@
         <v>2891</v>
       </c>
       <c r="AI28" t="s">
-        <v>1936</v>
+        <v>745</v>
       </c>
       <c r="AJ28" t="s">
-        <v>3128</v>
+        <v>3223</v>
       </c>
       <c r="AK28" t="s">
-        <v>3127</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -14952,13 +15402,13 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>3024</v>
+        <v>881</v>
       </c>
       <c r="D29" t="s">
-        <v>3131</v>
+        <v>3280</v>
       </c>
       <c r="E29" t="s">
-        <v>3130</v>
+        <v>3279</v>
       </c>
       <c r="G29" t="s">
         <v>680</v>
@@ -14973,55 +15423,55 @@
         <v>667</v>
       </c>
       <c r="U29" t="s">
+        <v>2692</v>
+      </c>
+      <c r="V29" t="s">
+        <v>2202</v>
+      </c>
+      <c r="W29" t="s">
         <v>2862</v>
       </c>
-      <c r="V29" t="s">
-        <v>658</v>
-      </c>
-      <c r="W29" t="s">
-        <v>2692</v>
-      </c>
       <c r="X29" t="s">
-        <v>2202</v>
+        <v>3056</v>
       </c>
       <c r="Y29" t="s">
-        <v>3056</v>
+        <v>3006</v>
       </c>
       <c r="Z29" t="s">
-        <v>3069</v>
+        <v>2941</v>
       </c>
       <c r="AA29" t="s">
-        <v>2941</v>
+        <v>1359</v>
       </c>
       <c r="AB29" t="s">
         <v>3129</v>
       </c>
       <c r="AC29" t="s">
-        <v>3006</v>
+        <v>2007</v>
       </c>
       <c r="AD29" t="s">
-        <v>3057</v>
+        <v>3175</v>
       </c>
       <c r="AE29" t="s">
-        <v>691</v>
+        <v>2009</v>
       </c>
       <c r="AF29" t="s">
-        <v>2007</v>
+        <v>658</v>
       </c>
       <c r="AG29" t="s">
-        <v>3050</v>
+        <v>3171</v>
       </c>
       <c r="AH29" t="s">
-        <v>3023</v>
+        <v>2707</v>
       </c>
       <c r="AI29" t="s">
-        <v>3024</v>
+        <v>881</v>
       </c>
       <c r="AJ29" t="s">
-        <v>3131</v>
+        <v>3280</v>
       </c>
       <c r="AK29" t="s">
-        <v>3130</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -15032,13 +15482,13 @@
         <v>23487</v>
       </c>
       <c r="C30" t="s">
-        <v>3024</v>
+        <v>1723</v>
       </c>
       <c r="D30" t="s">
-        <v>3133</v>
+        <v>3282</v>
       </c>
       <c r="E30" t="s">
-        <v>3132</v>
+        <v>3281</v>
       </c>
       <c r="G30" t="s">
         <v>426</v>
@@ -15050,34 +15500,34 @@
         <v>289</v>
       </c>
       <c r="T30" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U30" t="s">
+        <v>2862</v>
+      </c>
+      <c r="V30" t="s">
+        <v>3056</v>
+      </c>
+      <c r="W30" t="s">
         <v>2691</v>
       </c>
-      <c r="V30" t="s">
-        <v>2862</v>
-      </c>
-      <c r="W30" t="s">
-        <v>658</v>
-      </c>
       <c r="X30" t="s">
-        <v>2819</v>
+        <v>3169</v>
       </c>
       <c r="Y30" t="s">
-        <v>3056</v>
+        <v>2881</v>
       </c>
       <c r="Z30" t="s">
-        <v>3011</v>
+        <v>3147</v>
       </c>
       <c r="AA30" t="s">
-        <v>3048</v>
+        <v>3010</v>
       </c>
       <c r="AB30" t="s">
-        <v>3012</v>
+        <v>3170</v>
       </c>
       <c r="AC30" t="s">
-        <v>3010</v>
+        <v>3148</v>
       </c>
       <c r="AD30" t="s">
         <v>2879</v>
@@ -15086,7 +15536,7 @@
         <v>667</v>
       </c>
       <c r="AF30" t="s">
-        <v>2881</v>
+        <v>658</v>
       </c>
       <c r="AG30" t="s">
         <v>3031</v>
@@ -15095,13 +15545,13 @@
         <v>1345</v>
       </c>
       <c r="AI30" t="s">
-        <v>3024</v>
+        <v>1723</v>
       </c>
       <c r="AJ30" t="s">
-        <v>3133</v>
+        <v>3282</v>
       </c>
       <c r="AK30" t="s">
-        <v>3132</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -15112,13 +15562,13 @@
         <v>360554</v>
       </c>
       <c r="C31" t="s">
-        <v>1927</v>
+        <v>1993</v>
       </c>
       <c r="D31" t="s">
-        <v>3136</v>
+        <v>3284</v>
       </c>
       <c r="E31" t="s">
-        <v>3135</v>
+        <v>3283</v>
       </c>
       <c r="G31" t="s">
         <v>627</v>
@@ -15130,58 +15580,58 @@
         <v>843</v>
       </c>
       <c r="T31" t="s">
-        <v>3134</v>
+        <v>342</v>
       </c>
       <c r="U31" t="s">
-        <v>658</v>
+        <v>2202</v>
       </c>
       <c r="V31" t="s">
-        <v>2202</v>
+        <v>3075</v>
       </c>
       <c r="W31" t="s">
-        <v>2819</v>
+        <v>3169</v>
       </c>
       <c r="X31" t="s">
-        <v>3007</v>
+        <v>2165</v>
       </c>
       <c r="Y31" t="s">
-        <v>3016</v>
+        <v>3148</v>
       </c>
       <c r="Z31" t="s">
-        <v>3004</v>
+        <v>3143</v>
       </c>
       <c r="AA31" t="s">
-        <v>3048</v>
+        <v>3170</v>
       </c>
       <c r="AB31" t="s">
-        <v>3012</v>
+        <v>1345</v>
       </c>
       <c r="AC31" t="s">
-        <v>3057</v>
+        <v>3175</v>
       </c>
       <c r="AD31" t="s">
-        <v>3017</v>
+        <v>3152</v>
       </c>
       <c r="AE31" t="s">
         <v>667</v>
       </c>
       <c r="AF31" t="s">
-        <v>1345</v>
+        <v>3144</v>
       </c>
       <c r="AG31" t="s">
-        <v>3075</v>
+        <v>658</v>
       </c>
       <c r="AH31" t="s">
-        <v>2165</v>
+        <v>3016</v>
       </c>
       <c r="AI31" t="s">
-        <v>1927</v>
+        <v>1993</v>
       </c>
       <c r="AJ31" t="s">
-        <v>3136</v>
+        <v>3284</v>
       </c>
       <c r="AK31" t="s">
-        <v>3135</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -15192,13 +15642,13 @@
         <v>2090014</v>
       </c>
       <c r="C32" t="s">
-        <v>1892</v>
+        <v>1884</v>
       </c>
       <c r="D32" t="s">
-        <v>3138</v>
+        <v>3286</v>
       </c>
       <c r="E32" t="s">
-        <v>3137</v>
+        <v>3285</v>
       </c>
       <c r="G32" t="s">
         <v>880</v>
@@ -15210,58 +15660,58 @@
         <v>849</v>
       </c>
       <c r="T32" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
       <c r="U32" t="s">
+        <v>2862</v>
+      </c>
+      <c r="V32" t="s">
+        <v>1350</v>
+      </c>
+      <c r="W32" t="s">
         <v>2696</v>
       </c>
-      <c r="V32" t="s">
-        <v>2862</v>
-      </c>
-      <c r="W32" t="s">
-        <v>708</v>
-      </c>
       <c r="X32" t="s">
-        <v>3048</v>
+        <v>3170</v>
       </c>
       <c r="Y32" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="Z32" t="s">
-        <v>3083</v>
+        <v>1359</v>
       </c>
       <c r="AA32" t="s">
         <v>3006</v>
       </c>
       <c r="AB32" t="s">
-        <v>3069</v>
+        <v>3031</v>
       </c>
       <c r="AC32" t="s">
+        <v>674</v>
+      </c>
+      <c r="AD32" t="s">
         <v>2879</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>674</v>
       </c>
       <c r="AE32" t="s">
         <v>2990</v>
       </c>
       <c r="AF32" t="s">
-        <v>3031</v>
+        <v>3083</v>
       </c>
       <c r="AG32" t="s">
-        <v>915</v>
+        <v>659</v>
       </c>
       <c r="AH32" t="s">
-        <v>3077</v>
+        <v>539</v>
       </c>
       <c r="AI32" t="s">
-        <v>1892</v>
+        <v>1884</v>
       </c>
       <c r="AJ32" t="s">
-        <v>3138</v>
+        <v>3286</v>
       </c>
       <c r="AK32" t="s">
-        <v>3137</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -15272,13 +15722,13 @@
         <v>158870</v>
       </c>
       <c r="C33" t="s">
-        <v>1884</v>
+        <v>745</v>
       </c>
       <c r="D33" t="s">
-        <v>3140</v>
+        <v>3290</v>
       </c>
       <c r="E33" t="s">
-        <v>3139</v>
+        <v>3289</v>
       </c>
       <c r="G33" t="s">
         <v>680</v>
@@ -15290,10 +15740,10 @@
         <v>241</v>
       </c>
       <c r="T33" t="s">
-        <v>667</v>
+        <v>3287</v>
       </c>
       <c r="U33" t="s">
-        <v>2862</v>
+        <v>3288</v>
       </c>
       <c r="V33" t="s">
         <v>2202</v>
@@ -15305,28 +15755,28 @@
         <v>2692</v>
       </c>
       <c r="Y33" t="s">
-        <v>658</v>
+        <v>2157</v>
       </c>
       <c r="Z33" t="s">
-        <v>3012</v>
+        <v>3148</v>
       </c>
       <c r="AA33" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AB33" t="s">
         <v>3006</v>
       </c>
-      <c r="AB33" t="s">
-        <v>2157</v>
-      </c>
       <c r="AC33" t="s">
-        <v>3069</v>
+        <v>3171</v>
       </c>
       <c r="AD33" t="s">
         <v>2985</v>
       </c>
       <c r="AE33" t="s">
-        <v>691</v>
+        <v>2009</v>
       </c>
       <c r="AF33" t="s">
-        <v>3050</v>
+        <v>658</v>
       </c>
       <c r="AG33" t="s">
         <v>674</v>
@@ -15335,13 +15785,13 @@
         <v>3102</v>
       </c>
       <c r="AI33" t="s">
-        <v>1884</v>
+        <v>745</v>
       </c>
       <c r="AJ33" t="s">
-        <v>3140</v>
+        <v>3290</v>
       </c>
       <c r="AK33" t="s">
-        <v>3139</v>
+        <v>3289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>